<commit_message>
updating dates for weighing and respirometry for apple maggots 2018
</commit_message>
<xml_diff>
--- a/Data/2018-08-14_master_datac_2018_collection_year.xlsx
+++ b/Data/2018-08-14_master_datac_2018_collection_year.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tatianagerena\Documents\GitHub\Circadian_rhythm_runs_seasonal_timing\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anbe642/zScience/Circadian_rhythm_runs_seasonal_timing/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F7EA99C-A5BF-4D37-9478-CC6EEEAD9C05}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58CFB3D5-BC38-424D-98E6-BA84D36866A3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="52800" yWindow="1080" windowWidth="35820" windowHeight="18720" xr2:uid="{C7477166-8A7C-B04A-9643-C277FEDCDAAB}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="84">
   <si>
     <t>Ind_ID</t>
   </si>
@@ -212,6 +212,72 @@
   </si>
   <si>
     <t>Apple</t>
+  </si>
+  <si>
+    <t>Day19_weight</t>
+  </si>
+  <si>
+    <t>Day20_respirometry</t>
+  </si>
+  <si>
+    <t>2018-09-01</t>
+  </si>
+  <si>
+    <t>2018-09-02</t>
+  </si>
+  <si>
+    <t>2018-09-03</t>
+  </si>
+  <si>
+    <t>2018-09-04</t>
+  </si>
+  <si>
+    <t>2018-09-05</t>
+  </si>
+  <si>
+    <t>2018-09-06</t>
+  </si>
+  <si>
+    <t>2018-09-07</t>
+  </si>
+  <si>
+    <t>2018-09-08</t>
+  </si>
+  <si>
+    <t>2018-09-09</t>
+  </si>
+  <si>
+    <t>2018-09-10</t>
+  </si>
+  <si>
+    <t>2018-09-11</t>
+  </si>
+  <si>
+    <t>2018-09-12</t>
+  </si>
+  <si>
+    <t>2018-09-13</t>
+  </si>
+  <si>
+    <t>2018-09-14</t>
+  </si>
+  <si>
+    <t>2018-09-15</t>
+  </si>
+  <si>
+    <t>2018-09-16</t>
+  </si>
+  <si>
+    <t>2018-09-17</t>
+  </si>
+  <si>
+    <t>2018-09-18</t>
+  </si>
+  <si>
+    <t>2018-09-19</t>
+  </si>
+  <si>
+    <t>2018-09-20</t>
   </si>
 </sst>
 </file>
@@ -231,7 +297,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -241,6 +307,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -257,7 +329,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -283,6 +355,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -597,15 +673,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D3F78F5-4EA8-6A42-B216-41A8EC7A5E8D}">
-  <dimension ref="A1:M34"/>
+  <dimension ref="A1:Z100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="Q6" sqref="Q6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="6" max="6" width="14.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>45</v>
       </c>
@@ -645,8 +724,14 @@
       <c r="M1" s="6" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N1" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>58</v>
       </c>
@@ -674,8 +759,19 @@
       <c r="I2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
+      <c r="T2" s="1"/>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>58</v>
       </c>
@@ -703,8 +799,19 @@
       <c r="I3" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+      <c r="T3" s="1"/>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>58</v>
       </c>
@@ -729,8 +836,19 @@
       <c r="I4">
         <v>241</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
+      <c r="S4" s="1"/>
+      <c r="T4" s="1"/>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>58</v>
       </c>
@@ -755,8 +873,19 @@
       <c r="I5">
         <v>60</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="1"/>
+      <c r="S5" s="1"/>
+      <c r="T5" s="1"/>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>58</v>
       </c>
@@ -781,8 +910,19 @@
       <c r="I6">
         <v>232</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="1"/>
+      <c r="S6" s="1"/>
+      <c r="T6" s="1"/>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>58</v>
       </c>
@@ -807,8 +947,19 @@
       <c r="I7">
         <v>123</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="1"/>
+      <c r="S7" s="1"/>
+      <c r="T7" s="1"/>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>58</v>
       </c>
@@ -833,8 +984,31 @@
       <c r="I8">
         <v>298</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J8" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1"/>
+      <c r="S8" s="1"/>
+      <c r="T8" s="1"/>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>58</v>
       </c>
@@ -859,60 +1033,129 @@
       <c r="I9">
         <v>153</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="J9" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="1"/>
+      <c r="S9" s="1"/>
+      <c r="T9" s="1"/>
+    </row>
+    <row r="10" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="D10" s="9">
+      <c r="D10" s="12">
         <v>43328</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="11">
         <v>8</v>
       </c>
-      <c r="F10" s="10">
+      <c r="F10" s="13">
         <v>43335</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="11">
         <v>1</v>
       </c>
-      <c r="I10">
+      <c r="I10" s="11">
         <v>316</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="J10" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="K10" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="L10" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="M10" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="N10" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="O10" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="P10" s="14"/>
+      <c r="Q10" s="14"/>
+      <c r="R10" s="14"/>
+      <c r="S10" s="14"/>
+      <c r="T10" s="14"/>
+    </row>
+    <row r="11" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="D11" s="9">
+      <c r="D11" s="12">
         <v>43328</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="11">
         <v>8</v>
       </c>
-      <c r="F11" s="10">
+      <c r="F11" s="13">
         <v>43335</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="11">
         <v>1</v>
       </c>
-      <c r="I11">
+      <c r="I11" s="11">
         <v>152</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J11" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="K11" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="L11" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="M11" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="N11" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="O11" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="P11" s="14"/>
+      <c r="Q11" s="14"/>
+      <c r="R11" s="14"/>
+      <c r="S11" s="14"/>
+      <c r="T11" s="14"/>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>58</v>
       </c>
@@ -937,8 +1180,31 @@
       <c r="I12">
         <v>302</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J12" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="O12" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1"/>
+      <c r="R12" s="1"/>
+      <c r="S12" s="1"/>
+      <c r="T12" s="1"/>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>58</v>
       </c>
@@ -963,86 +1229,178 @@
       <c r="I13">
         <v>142</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="J13" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="N13" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="O13" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="P13" s="1"/>
+      <c r="Q13" s="1"/>
+      <c r="R13" s="1"/>
+      <c r="S13" s="1"/>
+      <c r="T13" s="1"/>
+    </row>
+    <row r="14" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="D14" s="9">
+      <c r="D14" s="12">
         <v>43328</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="11">
         <v>10</v>
       </c>
-      <c r="F14" s="10">
+      <c r="F14" s="13">
         <v>43337</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="11">
         <v>1</v>
       </c>
-      <c r="I14">
+      <c r="I14" s="11">
         <v>357</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="J14" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="K14" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="L14" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="M14" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="N14" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="O14" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="P14" s="14"/>
+      <c r="Q14" s="14"/>
+      <c r="R14" s="14"/>
+      <c r="S14" s="14"/>
+      <c r="T14" s="14"/>
+    </row>
+    <row r="15" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="D15" s="9">
+      <c r="D15" s="12">
         <v>43328</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="11">
         <v>10</v>
       </c>
-      <c r="F15" s="10">
+      <c r="F15" s="13">
         <v>43337</v>
       </c>
-      <c r="G15">
+      <c r="G15" s="11">
         <v>2</v>
       </c>
-      <c r="I15">
+      <c r="I15" s="11">
         <v>42</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="J15" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="K15" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="L15" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="M15" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="N15" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="O15" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="P15" s="14"/>
+      <c r="Q15" s="14"/>
+      <c r="R15" s="14"/>
+      <c r="S15" s="14"/>
+      <c r="T15" s="14"/>
+    </row>
+    <row r="16" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="D16" s="9">
+      <c r="D16" s="12">
         <v>43328</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="11">
         <v>10</v>
       </c>
-      <c r="F16" s="10">
+      <c r="F16" s="13">
         <v>43337</v>
       </c>
-      <c r="G16">
+      <c r="G16" s="11">
         <v>1</v>
       </c>
-      <c r="I16">
+      <c r="I16" s="11">
         <v>177</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J16" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="K16" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="L16" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="M16" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="N16" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="O16" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="P16" s="14"/>
+      <c r="Q16" s="14"/>
+      <c r="R16" s="14"/>
+      <c r="S16" s="14"/>
+      <c r="T16" s="14"/>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>58</v>
       </c>
@@ -1067,8 +1425,31 @@
       <c r="I17">
         <v>313</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J17" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="N17" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="O17" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="P17" s="1"/>
+      <c r="Q17" s="1"/>
+      <c r="R17" s="1"/>
+      <c r="S17" s="1"/>
+      <c r="T17" s="1"/>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>58</v>
       </c>
@@ -1093,8 +1474,31 @@
       <c r="I18">
         <v>129</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J18" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="M18" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="N18" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="O18" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="P18" s="1"/>
+      <c r="Q18" s="1"/>
+      <c r="R18" s="1"/>
+      <c r="S18" s="1"/>
+      <c r="T18" s="1"/>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>58</v>
       </c>
@@ -1119,86 +1523,178 @@
       <c r="I19">
         <v>165</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="J19" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="M19" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="N19" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="O19" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="P19" s="1"/>
+      <c r="Q19" s="1"/>
+      <c r="R19" s="1"/>
+      <c r="S19" s="1"/>
+      <c r="T19" s="1"/>
+    </row>
+    <row r="20" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="D20" s="9">
+      <c r="D20" s="12">
         <v>43328</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="11">
         <v>12</v>
       </c>
-      <c r="F20" s="10">
+      <c r="F20" s="13">
         <v>43339</v>
       </c>
-      <c r="G20">
+      <c r="G20" s="11">
         <v>1</v>
       </c>
-      <c r="I20">
+      <c r="I20" s="11">
         <v>220</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="J20" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="K20" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="L20" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="M20" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="N20" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="O20" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="P20" s="14"/>
+      <c r="Q20" s="14"/>
+      <c r="R20" s="14"/>
+      <c r="S20" s="14"/>
+      <c r="T20" s="14"/>
+    </row>
+    <row r="21" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="D21" s="9">
+      <c r="D21" s="12">
         <v>43328</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="11">
         <v>12</v>
       </c>
-      <c r="F21" s="10">
+      <c r="F21" s="13">
         <v>43339</v>
       </c>
-      <c r="G21">
+      <c r="G21" s="11">
         <v>2</v>
       </c>
-      <c r="I21">
+      <c r="I21" s="11">
         <v>180</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="J21" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="K21" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="L21" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="M21" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="N21" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="O21" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="P21" s="14"/>
+      <c r="Q21" s="14"/>
+      <c r="R21" s="14"/>
+      <c r="S21" s="14"/>
+      <c r="T21" s="14"/>
+    </row>
+    <row r="22" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="D22" s="9">
+      <c r="D22" s="12">
         <v>43328</v>
       </c>
-      <c r="E22">
+      <c r="E22" s="11">
         <v>12</v>
       </c>
-      <c r="F22" s="10">
+      <c r="F22" s="13">
         <v>43339</v>
       </c>
-      <c r="G22">
+      <c r="G22" s="11">
         <v>1</v>
       </c>
-      <c r="I22">
+      <c r="I22" s="11">
         <v>138</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J22" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="K22" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="L22" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="M22" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="N22" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="O22" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="P22" s="14"/>
+      <c r="Q22" s="14"/>
+      <c r="R22" s="14"/>
+      <c r="S22" s="14"/>
+      <c r="T22" s="14"/>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>58</v>
       </c>
@@ -1223,8 +1719,31 @@
       <c r="I23">
         <v>210</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J23" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="M23" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="N23" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="O23" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="P23" s="1"/>
+      <c r="Q23" s="1"/>
+      <c r="R23" s="1"/>
+      <c r="S23" s="1"/>
+      <c r="T23" s="1"/>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>58</v>
       </c>
@@ -1249,8 +1768,31 @@
       <c r="I24">
         <v>149</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J24" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="L24" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="M24" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="N24" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="O24" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="P24" s="1"/>
+      <c r="Q24" s="1"/>
+      <c r="R24" s="1"/>
+      <c r="S24" s="1"/>
+      <c r="T24" s="1"/>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>58</v>
       </c>
@@ -1275,86 +1817,178 @@
       <c r="I25">
         <v>121</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="J25" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="L25" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="M25" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="N25" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="O25" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="P25" s="1"/>
+      <c r="Q25" s="1"/>
+      <c r="R25" s="1"/>
+      <c r="S25" s="1"/>
+      <c r="T25" s="1"/>
+    </row>
+    <row r="26" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="D26" s="9">
+      <c r="D26" s="12">
         <v>43328</v>
       </c>
-      <c r="E26">
+      <c r="E26" s="11">
         <v>14</v>
       </c>
-      <c r="F26" s="10">
+      <c r="F26" s="13">
         <v>43341</v>
       </c>
-      <c r="G26">
+      <c r="G26" s="11">
         <v>1</v>
       </c>
-      <c r="I26">
+      <c r="I26" s="11">
         <v>264</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="J26" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="K26" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="L26" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="M26" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="N26" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="O26" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="P26" s="14"/>
+      <c r="Q26" s="14"/>
+      <c r="R26" s="14"/>
+      <c r="S26" s="14"/>
+      <c r="T26" s="14"/>
+    </row>
+    <row r="27" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="D27" s="9">
+      <c r="D27" s="12">
         <v>43328</v>
       </c>
-      <c r="E27">
+      <c r="E27" s="11">
         <v>14</v>
       </c>
-      <c r="F27" s="10">
+      <c r="F27" s="13">
         <v>43341</v>
       </c>
-      <c r="G27">
+      <c r="G27" s="11">
         <v>2</v>
       </c>
-      <c r="I27">
+      <c r="I27" s="11">
         <v>101</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="J27" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="K27" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="L27" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="M27" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="N27" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="O27" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="P27" s="14"/>
+      <c r="Q27" s="14"/>
+      <c r="R27" s="14"/>
+      <c r="S27" s="14"/>
+      <c r="T27" s="14"/>
+    </row>
+    <row r="28" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="D28" s="9">
+      <c r="D28" s="12">
         <v>43328</v>
       </c>
-      <c r="E28">
+      <c r="E28" s="11">
         <v>14</v>
       </c>
-      <c r="F28" s="10">
+      <c r="F28" s="13">
         <v>43341</v>
       </c>
-      <c r="G28">
+      <c r="G28" s="11">
         <v>1</v>
       </c>
-      <c r="I28">
+      <c r="I28" s="11">
         <v>119</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J28" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="K28" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="L28" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="M28" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="N28" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="O28" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="P28" s="14"/>
+      <c r="Q28" s="14"/>
+      <c r="R28" s="14"/>
+      <c r="S28" s="14"/>
+      <c r="T28" s="14"/>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>58</v>
       </c>
@@ -1379,8 +2013,31 @@
       <c r="I29">
         <v>208</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J29" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="K29" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="L29" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="M29" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="N29" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="O29" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="P29" s="1"/>
+      <c r="Q29" s="1"/>
+      <c r="R29" s="1"/>
+      <c r="S29" s="1"/>
+      <c r="T29" s="1"/>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>58</v>
       </c>
@@ -1405,8 +2062,31 @@
       <c r="I30">
         <v>152</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J30" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="K30" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="L30" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="M30" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="N30" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="O30" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="P30" s="1"/>
+      <c r="Q30" s="1"/>
+      <c r="R30" s="1"/>
+      <c r="S30" s="1"/>
+      <c r="T30" s="1"/>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>58</v>
       </c>
@@ -1431,61 +2111,2005 @@
       <c r="I31">
         <v>105</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+      <c r="J31" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="K31" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="L31" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="M31" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="N31" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="O31" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="P31" s="1"/>
+      <c r="Q31" s="1"/>
+      <c r="R31" s="1"/>
+      <c r="S31" s="1"/>
+      <c r="T31" s="1"/>
+    </row>
+    <row r="32" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="D32" s="9">
+      <c r="D32" s="12">
         <v>43328</v>
       </c>
-      <c r="E32">
+      <c r="E32" s="11">
         <v>16</v>
       </c>
-      <c r="F32" s="10">
+      <c r="F32" s="13">
         <v>43343</v>
       </c>
-      <c r="G32">
+      <c r="G32" s="11">
         <v>1</v>
       </c>
-      <c r="I32">
+      <c r="I32" s="11">
         <v>43</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+      <c r="J32" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="K32" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="L32" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="M32" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="N32" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="O32" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="P32" s="14"/>
+      <c r="Q32" s="14"/>
+      <c r="R32" s="14"/>
+      <c r="S32" s="14"/>
+      <c r="T32" s="14"/>
+    </row>
+    <row r="33" spans="1:26" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="D33" s="9">
+      <c r="D33" s="12">
         <v>43328</v>
       </c>
-      <c r="E33">
+      <c r="E33" s="11">
         <v>16</v>
       </c>
-      <c r="F33" s="10">
+      <c r="F33" s="13">
         <v>43343</v>
       </c>
-      <c r="G33">
+      <c r="G33" s="11">
         <v>1</v>
       </c>
-      <c r="I33">
+      <c r="I33" s="11">
         <v>34</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F34" s="10"/>
+      <c r="J33" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="K33" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="L33" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="M33" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="N33" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="O33" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="P33" s="14"/>
+      <c r="Q33" s="14"/>
+      <c r="R33" s="14"/>
+      <c r="S33" s="14"/>
+      <c r="T33" s="14"/>
+    </row>
+    <row r="34" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A34" s="1"/>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G34" s="1"/>
+      <c r="H34" s="1"/>
+      <c r="I34" s="1"/>
+      <c r="J34" s="1"/>
+      <c r="K34" s="1"/>
+      <c r="L34" s="1"/>
+      <c r="M34" s="1"/>
+      <c r="N34" s="1"/>
+      <c r="O34" s="1"/>
+      <c r="P34" s="1"/>
+      <c r="Q34" s="1"/>
+      <c r="R34" s="1"/>
+      <c r="S34" s="1"/>
+      <c r="T34" s="1"/>
+      <c r="U34" s="1"/>
+      <c r="V34" s="1"/>
+      <c r="W34" s="1"/>
+      <c r="X34" s="1"/>
+      <c r="Y34" s="1"/>
+      <c r="Z34" s="1"/>
+    </row>
+    <row r="35" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A35" s="1"/>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1"/>
+      <c r="I35" s="1"/>
+      <c r="J35" s="1"/>
+      <c r="K35" s="1"/>
+      <c r="L35" s="1"/>
+      <c r="M35" s="1"/>
+      <c r="N35" s="1"/>
+      <c r="O35" s="1"/>
+      <c r="P35" s="1"/>
+      <c r="Q35" s="1"/>
+      <c r="R35" s="1"/>
+      <c r="S35" s="1"/>
+      <c r="T35" s="1"/>
+      <c r="U35" s="1"/>
+      <c r="V35" s="1"/>
+      <c r="W35" s="1"/>
+      <c r="X35" s="1"/>
+      <c r="Y35" s="1"/>
+      <c r="Z35" s="1"/>
+    </row>
+    <row r="36" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A36" s="1"/>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1"/>
+      <c r="I36" s="1"/>
+      <c r="J36" s="1"/>
+      <c r="K36" s="1"/>
+      <c r="L36" s="1"/>
+      <c r="M36" s="1"/>
+      <c r="N36" s="1"/>
+      <c r="O36" s="1"/>
+      <c r="P36" s="1"/>
+      <c r="Q36" s="1"/>
+      <c r="R36" s="1"/>
+      <c r="S36" s="1"/>
+      <c r="T36" s="1"/>
+      <c r="U36" s="1"/>
+      <c r="V36" s="1"/>
+      <c r="W36" s="1"/>
+      <c r="X36" s="1"/>
+      <c r="Y36" s="1"/>
+      <c r="Z36" s="1"/>
+    </row>
+    <row r="37" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A37" s="1"/>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
+      <c r="H37" s="1"/>
+      <c r="I37" s="1"/>
+      <c r="J37" s="1"/>
+      <c r="K37" s="1"/>
+      <c r="L37" s="1"/>
+      <c r="M37" s="1"/>
+      <c r="N37" s="1"/>
+      <c r="O37" s="1"/>
+      <c r="P37" s="1"/>
+      <c r="Q37" s="1"/>
+      <c r="R37" s="1"/>
+      <c r="S37" s="1"/>
+      <c r="T37" s="1"/>
+      <c r="U37" s="1"/>
+      <c r="V37" s="1"/>
+      <c r="W37" s="1"/>
+      <c r="X37" s="1"/>
+      <c r="Y37" s="1"/>
+      <c r="Z37" s="1"/>
+    </row>
+    <row r="38" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A38" s="1"/>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+      <c r="H38" s="1"/>
+      <c r="I38" s="1"/>
+      <c r="J38" s="1"/>
+      <c r="K38" s="1"/>
+      <c r="L38" s="1"/>
+      <c r="M38" s="1"/>
+      <c r="N38" s="1"/>
+      <c r="O38" s="1"/>
+      <c r="P38" s="1"/>
+      <c r="Q38" s="1"/>
+      <c r="R38" s="1"/>
+      <c r="S38" s="1"/>
+      <c r="T38" s="1"/>
+      <c r="U38" s="1"/>
+      <c r="V38" s="1"/>
+      <c r="W38" s="1"/>
+      <c r="X38" s="1"/>
+      <c r="Y38" s="1"/>
+      <c r="Z38" s="1"/>
+    </row>
+    <row r="39" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A39" s="1"/>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1"/>
+      <c r="H39" s="1"/>
+      <c r="I39" s="1"/>
+      <c r="J39" s="1"/>
+      <c r="K39" s="1"/>
+      <c r="L39" s="1"/>
+      <c r="M39" s="1"/>
+      <c r="N39" s="1"/>
+      <c r="O39" s="1"/>
+      <c r="P39" s="1"/>
+      <c r="Q39" s="1"/>
+      <c r="R39" s="1"/>
+      <c r="S39" s="1"/>
+      <c r="T39" s="1"/>
+      <c r="U39" s="1"/>
+      <c r="V39" s="1"/>
+      <c r="W39" s="1"/>
+      <c r="X39" s="1"/>
+      <c r="Y39" s="1"/>
+      <c r="Z39" s="1"/>
+    </row>
+    <row r="40" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A40" s="1"/>
+      <c r="B40" s="1"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+      <c r="F40" s="1"/>
+      <c r="G40" s="1"/>
+      <c r="H40" s="1"/>
+      <c r="I40" s="1"/>
+      <c r="J40" s="1"/>
+      <c r="K40" s="1"/>
+      <c r="L40" s="1"/>
+      <c r="M40" s="1"/>
+      <c r="N40" s="1"/>
+      <c r="O40" s="1"/>
+      <c r="P40" s="1"/>
+      <c r="Q40" s="1"/>
+      <c r="R40" s="1"/>
+      <c r="S40" s="1"/>
+      <c r="T40" s="1"/>
+      <c r="U40" s="1"/>
+      <c r="V40" s="1"/>
+      <c r="W40" s="1"/>
+      <c r="X40" s="1"/>
+      <c r="Y40" s="1"/>
+      <c r="Z40" s="1"/>
+    </row>
+    <row r="41" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A41" s="1"/>
+      <c r="B41" s="1"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
+      <c r="F41" s="1"/>
+      <c r="G41" s="1"/>
+      <c r="H41" s="1"/>
+      <c r="I41" s="1"/>
+      <c r="J41" s="1"/>
+      <c r="K41" s="1"/>
+      <c r="L41" s="1"/>
+      <c r="M41" s="1"/>
+      <c r="N41" s="1"/>
+      <c r="O41" s="1"/>
+      <c r="P41" s="1"/>
+      <c r="Q41" s="1"/>
+      <c r="R41" s="1"/>
+      <c r="S41" s="1"/>
+      <c r="T41" s="1"/>
+      <c r="U41" s="1"/>
+      <c r="V41" s="1"/>
+      <c r="W41" s="1"/>
+      <c r="X41" s="1"/>
+      <c r="Y41" s="1"/>
+      <c r="Z41" s="1"/>
+    </row>
+    <row r="42" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A42" s="1"/>
+      <c r="B42" s="1"/>
+      <c r="C42" s="1"/>
+      <c r="D42" s="1"/>
+      <c r="E42" s="1"/>
+      <c r="F42" s="1"/>
+      <c r="G42" s="1"/>
+      <c r="H42" s="1"/>
+      <c r="I42" s="1"/>
+      <c r="J42" s="1"/>
+      <c r="K42" s="1"/>
+      <c r="L42" s="1"/>
+      <c r="M42" s="1"/>
+      <c r="N42" s="1"/>
+      <c r="O42" s="1"/>
+      <c r="P42" s="1"/>
+      <c r="Q42" s="1"/>
+      <c r="R42" s="1"/>
+      <c r="S42" s="1"/>
+      <c r="T42" s="1"/>
+      <c r="U42" s="1"/>
+      <c r="V42" s="1"/>
+      <c r="W42" s="1"/>
+      <c r="X42" s="1"/>
+      <c r="Y42" s="1"/>
+      <c r="Z42" s="1"/>
+    </row>
+    <row r="43" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A43" s="1"/>
+      <c r="B43" s="1"/>
+      <c r="C43" s="1"/>
+      <c r="D43" s="1"/>
+      <c r="E43" s="1"/>
+      <c r="F43" s="1"/>
+      <c r="G43" s="1"/>
+      <c r="H43" s="1"/>
+      <c r="I43" s="1"/>
+      <c r="J43" s="1"/>
+      <c r="K43" s="1"/>
+      <c r="L43" s="1"/>
+      <c r="M43" s="1"/>
+      <c r="N43" s="1"/>
+      <c r="O43" s="1"/>
+      <c r="P43" s="1"/>
+      <c r="Q43" s="1"/>
+      <c r="R43" s="1"/>
+      <c r="S43" s="1"/>
+      <c r="T43" s="1"/>
+      <c r="U43" s="1"/>
+      <c r="V43" s="1"/>
+      <c r="W43" s="1"/>
+      <c r="X43" s="1"/>
+      <c r="Y43" s="1"/>
+      <c r="Z43" s="1"/>
+    </row>
+    <row r="44" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A44" s="1"/>
+      <c r="B44" s="1"/>
+      <c r="C44" s="1"/>
+      <c r="D44" s="1"/>
+      <c r="E44" s="1"/>
+      <c r="F44" s="1"/>
+      <c r="G44" s="1"/>
+      <c r="H44" s="1"/>
+      <c r="I44" s="1"/>
+      <c r="J44" s="1"/>
+      <c r="K44" s="1"/>
+      <c r="L44" s="1"/>
+      <c r="M44" s="1"/>
+      <c r="N44" s="1"/>
+      <c r="O44" s="1"/>
+      <c r="P44" s="1"/>
+      <c r="Q44" s="1"/>
+      <c r="R44" s="1"/>
+      <c r="S44" s="1"/>
+      <c r="T44" s="1"/>
+      <c r="U44" s="1"/>
+      <c r="V44" s="1"/>
+      <c r="W44" s="1"/>
+      <c r="X44" s="1"/>
+      <c r="Y44" s="1"/>
+      <c r="Z44" s="1"/>
+    </row>
+    <row r="45" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A45" s="1"/>
+      <c r="B45" s="1"/>
+      <c r="C45" s="1"/>
+      <c r="D45" s="1"/>
+      <c r="E45" s="1"/>
+      <c r="F45" s="1"/>
+      <c r="G45" s="1"/>
+      <c r="H45" s="1"/>
+      <c r="I45" s="1"/>
+      <c r="J45" s="1"/>
+      <c r="K45" s="1"/>
+      <c r="L45" s="1"/>
+      <c r="M45" s="1"/>
+      <c r="N45" s="1"/>
+      <c r="O45" s="1"/>
+      <c r="P45" s="1"/>
+      <c r="Q45" s="1"/>
+      <c r="R45" s="1"/>
+      <c r="S45" s="1"/>
+      <c r="T45" s="1"/>
+      <c r="U45" s="1"/>
+      <c r="V45" s="1"/>
+      <c r="W45" s="1"/>
+      <c r="X45" s="1"/>
+      <c r="Y45" s="1"/>
+      <c r="Z45" s="1"/>
+    </row>
+    <row r="46" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A46" s="1"/>
+      <c r="B46" s="1"/>
+      <c r="C46" s="1"/>
+      <c r="D46" s="1"/>
+      <c r="E46" s="1"/>
+      <c r="F46" s="1"/>
+      <c r="G46" s="1"/>
+      <c r="H46" s="1"/>
+      <c r="I46" s="1"/>
+      <c r="J46" s="1"/>
+      <c r="K46" s="1"/>
+      <c r="L46" s="1"/>
+      <c r="M46" s="1"/>
+      <c r="N46" s="1"/>
+      <c r="O46" s="1"/>
+      <c r="P46" s="1"/>
+      <c r="Q46" s="1"/>
+      <c r="R46" s="1"/>
+      <c r="S46" s="1"/>
+      <c r="T46" s="1"/>
+      <c r="U46" s="1"/>
+      <c r="V46" s="1"/>
+      <c r="W46" s="1"/>
+      <c r="X46" s="1"/>
+      <c r="Y46" s="1"/>
+      <c r="Z46" s="1"/>
+    </row>
+    <row r="47" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A47" s="1"/>
+      <c r="B47" s="1"/>
+      <c r="C47" s="1"/>
+      <c r="D47" s="1"/>
+      <c r="E47" s="1"/>
+      <c r="F47" s="1"/>
+      <c r="G47" s="1"/>
+      <c r="H47" s="1"/>
+      <c r="I47" s="1"/>
+      <c r="J47" s="1"/>
+      <c r="K47" s="1"/>
+      <c r="L47" s="1"/>
+      <c r="M47" s="1"/>
+      <c r="N47" s="1"/>
+      <c r="O47" s="1"/>
+      <c r="P47" s="1"/>
+      <c r="Q47" s="1"/>
+      <c r="R47" s="1"/>
+      <c r="S47" s="1"/>
+      <c r="T47" s="1"/>
+      <c r="U47" s="1"/>
+      <c r="V47" s="1"/>
+      <c r="W47" s="1"/>
+      <c r="X47" s="1"/>
+      <c r="Y47" s="1"/>
+      <c r="Z47" s="1"/>
+    </row>
+    <row r="48" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A48" s="1"/>
+      <c r="B48" s="1"/>
+      <c r="C48" s="1"/>
+      <c r="D48" s="1"/>
+      <c r="E48" s="1"/>
+      <c r="F48" s="1"/>
+      <c r="G48" s="1"/>
+      <c r="H48" s="1"/>
+      <c r="I48" s="1"/>
+      <c r="J48" s="1"/>
+      <c r="K48" s="1"/>
+      <c r="L48" s="1"/>
+      <c r="M48" s="1"/>
+      <c r="N48" s="1"/>
+      <c r="O48" s="1"/>
+      <c r="P48" s="1"/>
+      <c r="Q48" s="1"/>
+      <c r="R48" s="1"/>
+      <c r="S48" s="1"/>
+      <c r="T48" s="1"/>
+      <c r="U48" s="1"/>
+      <c r="V48" s="1"/>
+      <c r="W48" s="1"/>
+      <c r="X48" s="1"/>
+      <c r="Y48" s="1"/>
+      <c r="Z48" s="1"/>
+    </row>
+    <row r="49" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A49" s="1"/>
+      <c r="B49" s="1"/>
+      <c r="C49" s="1"/>
+      <c r="D49" s="1"/>
+      <c r="E49" s="1"/>
+      <c r="F49" s="1"/>
+      <c r="G49" s="1"/>
+      <c r="H49" s="1"/>
+      <c r="I49" s="1"/>
+      <c r="J49" s="1"/>
+      <c r="K49" s="1"/>
+      <c r="L49" s="1"/>
+      <c r="M49" s="1"/>
+      <c r="N49" s="1"/>
+      <c r="O49" s="1"/>
+      <c r="P49" s="1"/>
+      <c r="Q49" s="1"/>
+      <c r="R49" s="1"/>
+      <c r="S49" s="1"/>
+      <c r="T49" s="1"/>
+      <c r="U49" s="1"/>
+      <c r="V49" s="1"/>
+      <c r="W49" s="1"/>
+      <c r="X49" s="1"/>
+      <c r="Y49" s="1"/>
+      <c r="Z49" s="1"/>
+    </row>
+    <row r="50" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A50" s="1"/>
+      <c r="B50" s="1"/>
+      <c r="C50" s="1"/>
+      <c r="D50" s="1"/>
+      <c r="E50" s="1"/>
+      <c r="F50" s="1"/>
+      <c r="G50" s="1"/>
+      <c r="H50" s="1"/>
+      <c r="I50" s="1"/>
+      <c r="J50" s="1"/>
+      <c r="K50" s="1"/>
+      <c r="L50" s="1"/>
+      <c r="M50" s="1"/>
+      <c r="N50" s="1"/>
+      <c r="O50" s="1"/>
+      <c r="P50" s="1"/>
+      <c r="Q50" s="1"/>
+      <c r="R50" s="1"/>
+      <c r="S50" s="1"/>
+      <c r="T50" s="1"/>
+      <c r="U50" s="1"/>
+      <c r="V50" s="1"/>
+      <c r="W50" s="1"/>
+      <c r="X50" s="1"/>
+      <c r="Y50" s="1"/>
+      <c r="Z50" s="1"/>
+    </row>
+    <row r="51" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A51" s="1"/>
+      <c r="B51" s="1"/>
+      <c r="C51" s="1"/>
+      <c r="D51" s="1"/>
+      <c r="E51" s="1"/>
+      <c r="F51" s="1"/>
+      <c r="G51" s="1"/>
+      <c r="H51" s="1"/>
+      <c r="I51" s="1"/>
+      <c r="J51" s="1"/>
+      <c r="K51" s="1"/>
+      <c r="L51" s="1"/>
+      <c r="M51" s="1"/>
+      <c r="N51" s="1"/>
+      <c r="O51" s="1"/>
+      <c r="P51" s="1"/>
+      <c r="Q51" s="1"/>
+      <c r="R51" s="1"/>
+      <c r="S51" s="1"/>
+      <c r="T51" s="1"/>
+      <c r="U51" s="1"/>
+      <c r="V51" s="1"/>
+      <c r="W51" s="1"/>
+      <c r="X51" s="1"/>
+      <c r="Y51" s="1"/>
+      <c r="Z51" s="1"/>
+    </row>
+    <row r="52" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A52" s="1"/>
+      <c r="B52" s="1"/>
+      <c r="C52" s="1"/>
+      <c r="D52" s="1"/>
+      <c r="E52" s="1"/>
+      <c r="F52" s="1"/>
+      <c r="G52" s="1"/>
+      <c r="H52" s="1"/>
+      <c r="I52" s="1"/>
+      <c r="J52" s="1"/>
+      <c r="K52" s="1"/>
+      <c r="L52" s="1"/>
+      <c r="M52" s="1"/>
+      <c r="N52" s="1"/>
+      <c r="O52" s="1"/>
+      <c r="P52" s="1"/>
+      <c r="Q52" s="1"/>
+      <c r="R52" s="1"/>
+      <c r="S52" s="1"/>
+      <c r="T52" s="1"/>
+      <c r="U52" s="1"/>
+      <c r="V52" s="1"/>
+      <c r="W52" s="1"/>
+      <c r="X52" s="1"/>
+      <c r="Y52" s="1"/>
+      <c r="Z52" s="1"/>
+    </row>
+    <row r="53" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A53" s="1"/>
+      <c r="B53" s="1"/>
+      <c r="C53" s="1"/>
+      <c r="D53" s="1"/>
+      <c r="E53" s="1"/>
+      <c r="F53" s="1"/>
+      <c r="G53" s="1"/>
+      <c r="H53" s="1"/>
+      <c r="I53" s="1"/>
+      <c r="J53" s="1"/>
+      <c r="K53" s="1"/>
+      <c r="L53" s="1"/>
+      <c r="M53" s="1"/>
+      <c r="N53" s="1"/>
+      <c r="O53" s="1"/>
+      <c r="P53" s="1"/>
+      <c r="Q53" s="1"/>
+      <c r="R53" s="1"/>
+      <c r="S53" s="1"/>
+      <c r="T53" s="1"/>
+      <c r="U53" s="1"/>
+      <c r="V53" s="1"/>
+      <c r="W53" s="1"/>
+      <c r="X53" s="1"/>
+      <c r="Y53" s="1"/>
+      <c r="Z53" s="1"/>
+    </row>
+    <row r="54" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A54" s="1"/>
+      <c r="B54" s="1"/>
+      <c r="C54" s="1"/>
+      <c r="D54" s="1"/>
+      <c r="E54" s="1"/>
+      <c r="F54" s="1"/>
+      <c r="G54" s="1"/>
+      <c r="H54" s="1"/>
+      <c r="I54" s="1"/>
+      <c r="J54" s="1"/>
+      <c r="K54" s="1"/>
+      <c r="L54" s="1"/>
+      <c r="M54" s="1"/>
+      <c r="N54" s="1"/>
+      <c r="O54" s="1"/>
+      <c r="P54" s="1"/>
+      <c r="Q54" s="1"/>
+      <c r="R54" s="1"/>
+      <c r="S54" s="1"/>
+      <c r="T54" s="1"/>
+      <c r="U54" s="1"/>
+      <c r="V54" s="1"/>
+      <c r="W54" s="1"/>
+      <c r="X54" s="1"/>
+      <c r="Y54" s="1"/>
+      <c r="Z54" s="1"/>
+    </row>
+    <row r="55" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A55" s="1"/>
+      <c r="B55" s="1"/>
+      <c r="C55" s="1"/>
+      <c r="D55" s="1"/>
+      <c r="E55" s="1"/>
+      <c r="F55" s="1"/>
+      <c r="G55" s="1"/>
+      <c r="H55" s="1"/>
+      <c r="I55" s="1"/>
+      <c r="J55" s="1"/>
+      <c r="K55" s="1"/>
+      <c r="L55" s="1"/>
+      <c r="M55" s="1"/>
+      <c r="N55" s="1"/>
+      <c r="O55" s="1"/>
+      <c r="P55" s="1"/>
+      <c r="Q55" s="1"/>
+      <c r="R55" s="1"/>
+      <c r="S55" s="1"/>
+      <c r="T55" s="1"/>
+      <c r="U55" s="1"/>
+      <c r="V55" s="1"/>
+      <c r="W55" s="1"/>
+      <c r="X55" s="1"/>
+      <c r="Y55" s="1"/>
+      <c r="Z55" s="1"/>
+    </row>
+    <row r="56" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A56" s="1"/>
+      <c r="B56" s="1"/>
+      <c r="C56" s="1"/>
+      <c r="D56" s="1"/>
+      <c r="E56" s="1"/>
+      <c r="F56" s="1"/>
+      <c r="G56" s="1"/>
+      <c r="H56" s="1"/>
+      <c r="I56" s="1"/>
+      <c r="J56" s="1"/>
+      <c r="K56" s="1"/>
+      <c r="L56" s="1"/>
+      <c r="M56" s="1"/>
+      <c r="N56" s="1"/>
+      <c r="O56" s="1"/>
+      <c r="P56" s="1"/>
+      <c r="Q56" s="1"/>
+      <c r="R56" s="1"/>
+      <c r="S56" s="1"/>
+      <c r="T56" s="1"/>
+      <c r="U56" s="1"/>
+      <c r="V56" s="1"/>
+      <c r="W56" s="1"/>
+      <c r="X56" s="1"/>
+      <c r="Y56" s="1"/>
+      <c r="Z56" s="1"/>
+    </row>
+    <row r="57" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A57" s="1"/>
+      <c r="B57" s="1"/>
+      <c r="C57" s="1"/>
+      <c r="D57" s="1"/>
+      <c r="E57" s="1"/>
+      <c r="F57" s="1"/>
+      <c r="G57" s="1"/>
+      <c r="H57" s="1"/>
+      <c r="I57" s="1"/>
+      <c r="J57" s="1"/>
+      <c r="K57" s="1"/>
+      <c r="L57" s="1"/>
+      <c r="M57" s="1"/>
+      <c r="N57" s="1"/>
+      <c r="O57" s="1"/>
+      <c r="P57" s="1"/>
+      <c r="Q57" s="1"/>
+      <c r="R57" s="1"/>
+      <c r="S57" s="1"/>
+      <c r="T57" s="1"/>
+      <c r="U57" s="1"/>
+      <c r="V57" s="1"/>
+      <c r="W57" s="1"/>
+      <c r="X57" s="1"/>
+      <c r="Y57" s="1"/>
+      <c r="Z57" s="1"/>
+    </row>
+    <row r="58" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A58" s="1"/>
+      <c r="B58" s="1"/>
+      <c r="C58" s="1"/>
+      <c r="D58" s="1"/>
+      <c r="E58" s="1"/>
+      <c r="F58" s="1"/>
+      <c r="G58" s="1"/>
+      <c r="H58" s="1"/>
+      <c r="I58" s="1"/>
+      <c r="J58" s="1"/>
+      <c r="K58" s="1"/>
+      <c r="L58" s="1"/>
+      <c r="M58" s="1"/>
+      <c r="N58" s="1"/>
+      <c r="O58" s="1"/>
+      <c r="P58" s="1"/>
+      <c r="Q58" s="1"/>
+      <c r="R58" s="1"/>
+      <c r="S58" s="1"/>
+      <c r="T58" s="1"/>
+      <c r="U58" s="1"/>
+      <c r="V58" s="1"/>
+      <c r="W58" s="1"/>
+      <c r="X58" s="1"/>
+      <c r="Y58" s="1"/>
+      <c r="Z58" s="1"/>
+    </row>
+    <row r="59" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A59" s="1"/>
+      <c r="B59" s="1"/>
+      <c r="C59" s="1"/>
+      <c r="D59" s="1"/>
+      <c r="E59" s="1"/>
+      <c r="F59" s="1"/>
+      <c r="G59" s="1"/>
+      <c r="H59" s="1"/>
+      <c r="I59" s="1"/>
+      <c r="J59" s="1"/>
+      <c r="K59" s="1"/>
+      <c r="L59" s="1"/>
+      <c r="M59" s="1"/>
+      <c r="N59" s="1"/>
+      <c r="O59" s="1"/>
+      <c r="P59" s="1"/>
+      <c r="Q59" s="1"/>
+      <c r="R59" s="1"/>
+      <c r="S59" s="1"/>
+      <c r="T59" s="1"/>
+      <c r="U59" s="1"/>
+      <c r="V59" s="1"/>
+      <c r="W59" s="1"/>
+      <c r="X59" s="1"/>
+      <c r="Y59" s="1"/>
+      <c r="Z59" s="1"/>
+    </row>
+    <row r="60" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A60" s="1"/>
+      <c r="B60" s="1"/>
+      <c r="C60" s="1"/>
+      <c r="D60" s="1"/>
+      <c r="E60" s="1"/>
+      <c r="F60" s="1"/>
+      <c r="G60" s="1"/>
+      <c r="H60" s="1"/>
+      <c r="I60" s="1"/>
+      <c r="J60" s="1"/>
+      <c r="K60" s="1"/>
+      <c r="L60" s="1"/>
+      <c r="M60" s="1"/>
+      <c r="N60" s="1"/>
+      <c r="O60" s="1"/>
+      <c r="P60" s="1"/>
+      <c r="Q60" s="1"/>
+      <c r="R60" s="1"/>
+      <c r="S60" s="1"/>
+      <c r="T60" s="1"/>
+      <c r="U60" s="1"/>
+      <c r="V60" s="1"/>
+      <c r="W60" s="1"/>
+      <c r="X60" s="1"/>
+      <c r="Y60" s="1"/>
+      <c r="Z60" s="1"/>
+    </row>
+    <row r="61" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A61" s="1"/>
+      <c r="B61" s="1"/>
+      <c r="C61" s="1"/>
+      <c r="D61" s="1"/>
+      <c r="E61" s="1"/>
+      <c r="F61" s="1"/>
+      <c r="G61" s="1"/>
+      <c r="H61" s="1"/>
+      <c r="I61" s="1"/>
+      <c r="J61" s="1"/>
+      <c r="K61" s="1"/>
+      <c r="L61" s="1"/>
+      <c r="M61" s="1"/>
+      <c r="N61" s="1"/>
+      <c r="O61" s="1"/>
+      <c r="P61" s="1"/>
+      <c r="Q61" s="1"/>
+      <c r="R61" s="1"/>
+      <c r="S61" s="1"/>
+      <c r="T61" s="1"/>
+      <c r="U61" s="1"/>
+      <c r="V61" s="1"/>
+      <c r="W61" s="1"/>
+      <c r="X61" s="1"/>
+      <c r="Y61" s="1"/>
+      <c r="Z61" s="1"/>
+    </row>
+    <row r="62" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A62" s="1"/>
+      <c r="B62" s="1"/>
+      <c r="C62" s="1"/>
+      <c r="D62" s="1"/>
+      <c r="E62" s="1"/>
+      <c r="F62" s="1"/>
+      <c r="G62" s="1"/>
+      <c r="H62" s="1"/>
+      <c r="I62" s="1"/>
+      <c r="J62" s="1"/>
+      <c r="K62" s="1"/>
+      <c r="L62" s="1"/>
+      <c r="M62" s="1"/>
+      <c r="N62" s="1"/>
+      <c r="O62" s="1"/>
+      <c r="P62" s="1"/>
+      <c r="Q62" s="1"/>
+      <c r="R62" s="1"/>
+      <c r="S62" s="1"/>
+      <c r="T62" s="1"/>
+      <c r="U62" s="1"/>
+      <c r="V62" s="1"/>
+      <c r="W62" s="1"/>
+      <c r="X62" s="1"/>
+      <c r="Y62" s="1"/>
+      <c r="Z62" s="1"/>
+    </row>
+    <row r="63" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A63" s="1"/>
+      <c r="B63" s="1"/>
+      <c r="C63" s="1"/>
+      <c r="D63" s="1"/>
+      <c r="E63" s="1"/>
+      <c r="F63" s="1"/>
+      <c r="G63" s="1"/>
+      <c r="H63" s="1"/>
+      <c r="I63" s="1"/>
+      <c r="J63" s="1"/>
+      <c r="K63" s="1"/>
+      <c r="L63" s="1"/>
+      <c r="M63" s="1"/>
+      <c r="N63" s="1"/>
+      <c r="O63" s="1"/>
+      <c r="P63" s="1"/>
+      <c r="Q63" s="1"/>
+      <c r="R63" s="1"/>
+      <c r="S63" s="1"/>
+      <c r="T63" s="1"/>
+      <c r="U63" s="1"/>
+      <c r="V63" s="1"/>
+      <c r="W63" s="1"/>
+      <c r="X63" s="1"/>
+      <c r="Y63" s="1"/>
+      <c r="Z63" s="1"/>
+    </row>
+    <row r="64" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A64" s="1"/>
+      <c r="B64" s="1"/>
+      <c r="C64" s="1"/>
+      <c r="D64" s="1"/>
+      <c r="E64" s="1"/>
+      <c r="F64" s="1"/>
+      <c r="G64" s="1"/>
+      <c r="H64" s="1"/>
+      <c r="I64" s="1"/>
+      <c r="J64" s="1"/>
+      <c r="K64" s="1"/>
+      <c r="L64" s="1"/>
+      <c r="M64" s="1"/>
+      <c r="N64" s="1"/>
+      <c r="O64" s="1"/>
+      <c r="P64" s="1"/>
+      <c r="Q64" s="1"/>
+      <c r="R64" s="1"/>
+      <c r="S64" s="1"/>
+      <c r="T64" s="1"/>
+      <c r="U64" s="1"/>
+      <c r="V64" s="1"/>
+      <c r="W64" s="1"/>
+      <c r="X64" s="1"/>
+      <c r="Y64" s="1"/>
+      <c r="Z64" s="1"/>
+    </row>
+    <row r="65" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A65" s="1"/>
+      <c r="B65" s="1"/>
+      <c r="C65" s="1"/>
+      <c r="D65" s="1"/>
+      <c r="E65" s="1"/>
+      <c r="F65" s="1"/>
+      <c r="G65" s="1"/>
+      <c r="H65" s="1"/>
+      <c r="I65" s="1"/>
+      <c r="J65" s="1"/>
+      <c r="K65" s="1"/>
+      <c r="L65" s="1"/>
+      <c r="M65" s="1"/>
+      <c r="N65" s="1"/>
+      <c r="O65" s="1"/>
+      <c r="P65" s="1"/>
+      <c r="Q65" s="1"/>
+      <c r="R65" s="1"/>
+      <c r="S65" s="1"/>
+      <c r="T65" s="1"/>
+      <c r="U65" s="1"/>
+      <c r="V65" s="1"/>
+      <c r="W65" s="1"/>
+      <c r="X65" s="1"/>
+      <c r="Y65" s="1"/>
+      <c r="Z65" s="1"/>
+    </row>
+    <row r="66" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A66" s="1"/>
+      <c r="B66" s="1"/>
+      <c r="C66" s="1"/>
+      <c r="D66" s="1"/>
+      <c r="E66" s="1"/>
+      <c r="F66" s="1"/>
+      <c r="G66" s="1"/>
+      <c r="H66" s="1"/>
+      <c r="I66" s="1"/>
+      <c r="J66" s="1"/>
+      <c r="K66" s="1"/>
+      <c r="L66" s="1"/>
+      <c r="M66" s="1"/>
+      <c r="N66" s="1"/>
+      <c r="O66" s="1"/>
+      <c r="P66" s="1"/>
+      <c r="Q66" s="1"/>
+      <c r="R66" s="1"/>
+      <c r="S66" s="1"/>
+      <c r="T66" s="1"/>
+      <c r="U66" s="1"/>
+      <c r="V66" s="1"/>
+      <c r="W66" s="1"/>
+      <c r="X66" s="1"/>
+      <c r="Y66" s="1"/>
+      <c r="Z66" s="1"/>
+    </row>
+    <row r="67" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A67" s="1"/>
+      <c r="B67" s="1"/>
+      <c r="C67" s="1"/>
+      <c r="D67" s="1"/>
+      <c r="E67" s="1"/>
+      <c r="F67" s="1"/>
+      <c r="G67" s="1"/>
+      <c r="H67" s="1"/>
+      <c r="I67" s="1"/>
+      <c r="J67" s="1"/>
+      <c r="K67" s="1"/>
+      <c r="L67" s="1"/>
+      <c r="M67" s="1"/>
+      <c r="N67" s="1"/>
+      <c r="O67" s="1"/>
+      <c r="P67" s="1"/>
+      <c r="Q67" s="1"/>
+      <c r="R67" s="1"/>
+      <c r="S67" s="1"/>
+      <c r="T67" s="1"/>
+      <c r="U67" s="1"/>
+      <c r="V67" s="1"/>
+      <c r="W67" s="1"/>
+      <c r="X67" s="1"/>
+      <c r="Y67" s="1"/>
+      <c r="Z67" s="1"/>
+    </row>
+    <row r="68" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A68" s="1"/>
+      <c r="B68" s="1"/>
+      <c r="C68" s="1"/>
+      <c r="D68" s="1"/>
+      <c r="E68" s="1"/>
+      <c r="F68" s="1"/>
+      <c r="G68" s="1"/>
+      <c r="H68" s="1"/>
+      <c r="I68" s="1"/>
+      <c r="J68" s="1"/>
+      <c r="K68" s="1"/>
+      <c r="L68" s="1"/>
+      <c r="M68" s="1"/>
+      <c r="N68" s="1"/>
+      <c r="O68" s="1"/>
+      <c r="P68" s="1"/>
+      <c r="Q68" s="1"/>
+      <c r="R68" s="1"/>
+      <c r="S68" s="1"/>
+      <c r="T68" s="1"/>
+      <c r="U68" s="1"/>
+      <c r="V68" s="1"/>
+      <c r="W68" s="1"/>
+      <c r="X68" s="1"/>
+      <c r="Y68" s="1"/>
+      <c r="Z68" s="1"/>
+    </row>
+    <row r="69" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A69" s="1"/>
+      <c r="B69" s="1"/>
+      <c r="C69" s="1"/>
+      <c r="D69" s="1"/>
+      <c r="E69" s="1"/>
+      <c r="F69" s="1"/>
+      <c r="G69" s="1"/>
+      <c r="H69" s="1"/>
+      <c r="I69" s="1"/>
+      <c r="J69" s="1"/>
+      <c r="K69" s="1"/>
+      <c r="L69" s="1"/>
+      <c r="M69" s="1"/>
+      <c r="N69" s="1"/>
+      <c r="O69" s="1"/>
+      <c r="P69" s="1"/>
+      <c r="Q69" s="1"/>
+      <c r="R69" s="1"/>
+      <c r="S69" s="1"/>
+      <c r="T69" s="1"/>
+      <c r="U69" s="1"/>
+      <c r="V69" s="1"/>
+      <c r="W69" s="1"/>
+      <c r="X69" s="1"/>
+      <c r="Y69" s="1"/>
+      <c r="Z69" s="1"/>
+    </row>
+    <row r="70" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A70" s="1"/>
+      <c r="B70" s="1"/>
+      <c r="C70" s="1"/>
+      <c r="D70" s="1"/>
+      <c r="E70" s="1"/>
+      <c r="F70" s="1"/>
+      <c r="G70" s="1"/>
+      <c r="H70" s="1"/>
+      <c r="I70" s="1"/>
+      <c r="J70" s="1"/>
+      <c r="K70" s="1"/>
+      <c r="L70" s="1"/>
+      <c r="M70" s="1"/>
+      <c r="N70" s="1"/>
+      <c r="O70" s="1"/>
+      <c r="P70" s="1"/>
+      <c r="Q70" s="1"/>
+      <c r="R70" s="1"/>
+      <c r="S70" s="1"/>
+      <c r="T70" s="1"/>
+      <c r="U70" s="1"/>
+      <c r="V70" s="1"/>
+      <c r="W70" s="1"/>
+      <c r="X70" s="1"/>
+      <c r="Y70" s="1"/>
+      <c r="Z70" s="1"/>
+    </row>
+    <row r="71" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A71" s="1"/>
+      <c r="B71" s="1"/>
+      <c r="C71" s="1"/>
+      <c r="D71" s="1"/>
+      <c r="E71" s="1"/>
+      <c r="F71" s="1"/>
+      <c r="G71" s="1"/>
+      <c r="H71" s="1"/>
+      <c r="I71" s="1"/>
+      <c r="J71" s="1"/>
+      <c r="K71" s="1"/>
+      <c r="L71" s="1"/>
+      <c r="M71" s="1"/>
+      <c r="N71" s="1"/>
+      <c r="O71" s="1"/>
+      <c r="P71" s="1"/>
+      <c r="Q71" s="1"/>
+      <c r="R71" s="1"/>
+      <c r="S71" s="1"/>
+      <c r="T71" s="1"/>
+      <c r="U71" s="1"/>
+      <c r="V71" s="1"/>
+      <c r="W71" s="1"/>
+      <c r="X71" s="1"/>
+      <c r="Y71" s="1"/>
+      <c r="Z71" s="1"/>
+    </row>
+    <row r="72" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A72" s="1"/>
+      <c r="B72" s="1"/>
+      <c r="C72" s="1"/>
+      <c r="D72" s="1"/>
+      <c r="E72" s="1"/>
+      <c r="F72" s="1"/>
+      <c r="G72" s="1"/>
+      <c r="H72" s="1"/>
+      <c r="I72" s="1"/>
+      <c r="J72" s="1"/>
+      <c r="K72" s="1"/>
+      <c r="L72" s="1"/>
+      <c r="M72" s="1"/>
+      <c r="N72" s="1"/>
+      <c r="O72" s="1"/>
+      <c r="P72" s="1"/>
+      <c r="Q72" s="1"/>
+      <c r="R72" s="1"/>
+      <c r="S72" s="1"/>
+      <c r="T72" s="1"/>
+      <c r="U72" s="1"/>
+      <c r="V72" s="1"/>
+      <c r="W72" s="1"/>
+      <c r="X72" s="1"/>
+      <c r="Y72" s="1"/>
+      <c r="Z72" s="1"/>
+    </row>
+    <row r="73" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A73" s="1"/>
+      <c r="B73" s="1"/>
+      <c r="C73" s="1"/>
+      <c r="D73" s="1"/>
+      <c r="E73" s="1"/>
+      <c r="F73" s="1"/>
+      <c r="G73" s="1"/>
+      <c r="H73" s="1"/>
+      <c r="I73" s="1"/>
+      <c r="J73" s="1"/>
+      <c r="K73" s="1"/>
+      <c r="L73" s="1"/>
+      <c r="M73" s="1"/>
+      <c r="N73" s="1"/>
+      <c r="O73" s="1"/>
+      <c r="P73" s="1"/>
+      <c r="Q73" s="1"/>
+      <c r="R73" s="1"/>
+      <c r="S73" s="1"/>
+      <c r="T73" s="1"/>
+      <c r="U73" s="1"/>
+      <c r="V73" s="1"/>
+      <c r="W73" s="1"/>
+      <c r="X73" s="1"/>
+      <c r="Y73" s="1"/>
+      <c r="Z73" s="1"/>
+    </row>
+    <row r="74" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A74" s="1"/>
+      <c r="B74" s="1"/>
+      <c r="C74" s="1"/>
+      <c r="D74" s="1"/>
+      <c r="E74" s="1"/>
+      <c r="F74" s="1"/>
+      <c r="G74" s="1"/>
+      <c r="H74" s="1"/>
+      <c r="I74" s="1"/>
+      <c r="J74" s="1"/>
+      <c r="K74" s="1"/>
+      <c r="L74" s="1"/>
+      <c r="M74" s="1"/>
+      <c r="N74" s="1"/>
+      <c r="O74" s="1"/>
+      <c r="P74" s="1"/>
+      <c r="Q74" s="1"/>
+      <c r="R74" s="1"/>
+      <c r="S74" s="1"/>
+      <c r="T74" s="1"/>
+      <c r="U74" s="1"/>
+      <c r="V74" s="1"/>
+      <c r="W74" s="1"/>
+      <c r="X74" s="1"/>
+      <c r="Y74" s="1"/>
+      <c r="Z74" s="1"/>
+    </row>
+    <row r="75" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A75" s="1"/>
+      <c r="B75" s="1"/>
+      <c r="C75" s="1"/>
+      <c r="D75" s="1"/>
+      <c r="E75" s="1"/>
+      <c r="F75" s="1"/>
+      <c r="G75" s="1"/>
+      <c r="H75" s="1"/>
+      <c r="I75" s="1"/>
+      <c r="J75" s="1"/>
+      <c r="K75" s="1"/>
+      <c r="L75" s="1"/>
+      <c r="M75" s="1"/>
+      <c r="N75" s="1"/>
+      <c r="O75" s="1"/>
+      <c r="P75" s="1"/>
+      <c r="Q75" s="1"/>
+      <c r="R75" s="1"/>
+      <c r="S75" s="1"/>
+      <c r="T75" s="1"/>
+      <c r="U75" s="1"/>
+      <c r="V75" s="1"/>
+      <c r="W75" s="1"/>
+      <c r="X75" s="1"/>
+      <c r="Y75" s="1"/>
+      <c r="Z75" s="1"/>
+    </row>
+    <row r="76" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A76" s="1"/>
+      <c r="B76" s="1"/>
+      <c r="C76" s="1"/>
+      <c r="D76" s="1"/>
+      <c r="E76" s="1"/>
+      <c r="F76" s="1"/>
+      <c r="G76" s="1"/>
+      <c r="H76" s="1"/>
+      <c r="I76" s="1"/>
+      <c r="J76" s="1"/>
+      <c r="K76" s="1"/>
+      <c r="L76" s="1"/>
+      <c r="M76" s="1"/>
+      <c r="N76" s="1"/>
+      <c r="O76" s="1"/>
+      <c r="P76" s="1"/>
+      <c r="Q76" s="1"/>
+      <c r="R76" s="1"/>
+      <c r="S76" s="1"/>
+      <c r="T76" s="1"/>
+      <c r="U76" s="1"/>
+      <c r="V76" s="1"/>
+      <c r="W76" s="1"/>
+      <c r="X76" s="1"/>
+      <c r="Y76" s="1"/>
+      <c r="Z76" s="1"/>
+    </row>
+    <row r="77" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A77" s="1"/>
+      <c r="B77" s="1"/>
+      <c r="C77" s="1"/>
+      <c r="D77" s="1"/>
+      <c r="E77" s="1"/>
+      <c r="F77" s="1"/>
+      <c r="G77" s="1"/>
+      <c r="H77" s="1"/>
+      <c r="I77" s="1"/>
+      <c r="J77" s="1"/>
+      <c r="K77" s="1"/>
+      <c r="L77" s="1"/>
+      <c r="M77" s="1"/>
+      <c r="N77" s="1"/>
+      <c r="O77" s="1"/>
+      <c r="P77" s="1"/>
+      <c r="Q77" s="1"/>
+      <c r="R77" s="1"/>
+      <c r="S77" s="1"/>
+      <c r="T77" s="1"/>
+      <c r="U77" s="1"/>
+      <c r="V77" s="1"/>
+      <c r="W77" s="1"/>
+      <c r="X77" s="1"/>
+      <c r="Y77" s="1"/>
+      <c r="Z77" s="1"/>
+    </row>
+    <row r="78" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A78" s="1"/>
+      <c r="B78" s="1"/>
+      <c r="C78" s="1"/>
+      <c r="D78" s="1"/>
+      <c r="E78" s="1"/>
+      <c r="F78" s="1"/>
+      <c r="G78" s="1"/>
+      <c r="H78" s="1"/>
+      <c r="I78" s="1"/>
+      <c r="J78" s="1"/>
+      <c r="K78" s="1"/>
+      <c r="L78" s="1"/>
+      <c r="M78" s="1"/>
+      <c r="N78" s="1"/>
+      <c r="O78" s="1"/>
+      <c r="P78" s="1"/>
+      <c r="Q78" s="1"/>
+      <c r="R78" s="1"/>
+      <c r="S78" s="1"/>
+      <c r="T78" s="1"/>
+      <c r="U78" s="1"/>
+      <c r="V78" s="1"/>
+      <c r="W78" s="1"/>
+      <c r="X78" s="1"/>
+      <c r="Y78" s="1"/>
+      <c r="Z78" s="1"/>
+    </row>
+    <row r="79" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A79" s="1"/>
+      <c r="B79" s="1"/>
+      <c r="C79" s="1"/>
+      <c r="D79" s="1"/>
+      <c r="E79" s="1"/>
+      <c r="F79" s="1"/>
+      <c r="G79" s="1"/>
+      <c r="H79" s="1"/>
+      <c r="I79" s="1"/>
+      <c r="J79" s="1"/>
+      <c r="K79" s="1"/>
+      <c r="L79" s="1"/>
+      <c r="M79" s="1"/>
+      <c r="N79" s="1"/>
+      <c r="O79" s="1"/>
+      <c r="P79" s="1"/>
+      <c r="Q79" s="1"/>
+      <c r="R79" s="1"/>
+      <c r="S79" s="1"/>
+      <c r="T79" s="1"/>
+      <c r="U79" s="1"/>
+      <c r="V79" s="1"/>
+      <c r="W79" s="1"/>
+      <c r="X79" s="1"/>
+      <c r="Y79" s="1"/>
+      <c r="Z79" s="1"/>
+    </row>
+    <row r="80" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A80" s="1"/>
+      <c r="B80" s="1"/>
+      <c r="C80" s="1"/>
+      <c r="D80" s="1"/>
+      <c r="E80" s="1"/>
+      <c r="F80" s="1"/>
+      <c r="G80" s="1"/>
+      <c r="H80" s="1"/>
+      <c r="I80" s="1"/>
+      <c r="J80" s="1"/>
+      <c r="K80" s="1"/>
+      <c r="L80" s="1"/>
+      <c r="M80" s="1"/>
+      <c r="N80" s="1"/>
+      <c r="O80" s="1"/>
+      <c r="P80" s="1"/>
+      <c r="Q80" s="1"/>
+      <c r="R80" s="1"/>
+      <c r="S80" s="1"/>
+      <c r="T80" s="1"/>
+      <c r="U80" s="1"/>
+      <c r="V80" s="1"/>
+      <c r="W80" s="1"/>
+      <c r="X80" s="1"/>
+      <c r="Y80" s="1"/>
+      <c r="Z80" s="1"/>
+    </row>
+    <row r="81" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A81" s="1"/>
+      <c r="B81" s="1"/>
+      <c r="C81" s="1"/>
+      <c r="D81" s="1"/>
+      <c r="E81" s="1"/>
+      <c r="F81" s="1"/>
+      <c r="G81" s="1"/>
+      <c r="H81" s="1"/>
+      <c r="I81" s="1"/>
+      <c r="J81" s="1"/>
+      <c r="K81" s="1"/>
+      <c r="L81" s="1"/>
+      <c r="M81" s="1"/>
+      <c r="N81" s="1"/>
+      <c r="O81" s="1"/>
+      <c r="P81" s="1"/>
+      <c r="Q81" s="1"/>
+      <c r="R81" s="1"/>
+      <c r="S81" s="1"/>
+      <c r="T81" s="1"/>
+      <c r="U81" s="1"/>
+      <c r="V81" s="1"/>
+      <c r="W81" s="1"/>
+      <c r="X81" s="1"/>
+      <c r="Y81" s="1"/>
+      <c r="Z81" s="1"/>
+    </row>
+    <row r="82" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A82" s="1"/>
+      <c r="B82" s="1"/>
+      <c r="C82" s="1"/>
+      <c r="D82" s="1"/>
+      <c r="E82" s="1"/>
+      <c r="F82" s="1"/>
+      <c r="G82" s="1"/>
+      <c r="H82" s="1"/>
+      <c r="I82" s="1"/>
+      <c r="J82" s="1"/>
+      <c r="K82" s="1"/>
+      <c r="L82" s="1"/>
+      <c r="M82" s="1"/>
+      <c r="N82" s="1"/>
+      <c r="O82" s="1"/>
+      <c r="P82" s="1"/>
+      <c r="Q82" s="1"/>
+      <c r="R82" s="1"/>
+      <c r="S82" s="1"/>
+      <c r="T82" s="1"/>
+      <c r="U82" s="1"/>
+      <c r="V82" s="1"/>
+      <c r="W82" s="1"/>
+      <c r="X82" s="1"/>
+      <c r="Y82" s="1"/>
+      <c r="Z82" s="1"/>
+    </row>
+    <row r="83" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A83" s="1"/>
+      <c r="B83" s="1"/>
+      <c r="C83" s="1"/>
+      <c r="D83" s="1"/>
+      <c r="E83" s="1"/>
+      <c r="F83" s="1"/>
+      <c r="G83" s="1"/>
+      <c r="H83" s="1"/>
+      <c r="I83" s="1"/>
+      <c r="J83" s="1"/>
+      <c r="K83" s="1"/>
+      <c r="L83" s="1"/>
+      <c r="M83" s="1"/>
+      <c r="N83" s="1"/>
+      <c r="O83" s="1"/>
+      <c r="P83" s="1"/>
+      <c r="Q83" s="1"/>
+      <c r="R83" s="1"/>
+      <c r="S83" s="1"/>
+      <c r="T83" s="1"/>
+      <c r="U83" s="1"/>
+      <c r="V83" s="1"/>
+      <c r="W83" s="1"/>
+      <c r="X83" s="1"/>
+      <c r="Y83" s="1"/>
+      <c r="Z83" s="1"/>
+    </row>
+    <row r="84" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A84" s="1"/>
+      <c r="B84" s="1"/>
+      <c r="C84" s="1"/>
+      <c r="D84" s="1"/>
+      <c r="E84" s="1"/>
+      <c r="F84" s="1"/>
+      <c r="G84" s="1"/>
+      <c r="H84" s="1"/>
+      <c r="I84" s="1"/>
+      <c r="J84" s="1"/>
+      <c r="K84" s="1"/>
+      <c r="L84" s="1"/>
+      <c r="M84" s="1"/>
+      <c r="N84" s="1"/>
+      <c r="O84" s="1"/>
+      <c r="P84" s="1"/>
+      <c r="Q84" s="1"/>
+      <c r="R84" s="1"/>
+      <c r="S84" s="1"/>
+      <c r="T84" s="1"/>
+      <c r="U84" s="1"/>
+      <c r="V84" s="1"/>
+      <c r="W84" s="1"/>
+      <c r="X84" s="1"/>
+      <c r="Y84" s="1"/>
+      <c r="Z84" s="1"/>
+    </row>
+    <row r="85" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A85" s="1"/>
+      <c r="B85" s="1"/>
+      <c r="C85" s="1"/>
+      <c r="D85" s="1"/>
+      <c r="E85" s="1"/>
+      <c r="F85" s="1"/>
+      <c r="G85" s="1"/>
+      <c r="H85" s="1"/>
+      <c r="I85" s="1"/>
+      <c r="J85" s="1"/>
+      <c r="K85" s="1"/>
+      <c r="L85" s="1"/>
+      <c r="M85" s="1"/>
+      <c r="N85" s="1"/>
+      <c r="O85" s="1"/>
+      <c r="P85" s="1"/>
+      <c r="Q85" s="1"/>
+      <c r="R85" s="1"/>
+      <c r="S85" s="1"/>
+      <c r="T85" s="1"/>
+      <c r="U85" s="1"/>
+      <c r="V85" s="1"/>
+      <c r="W85" s="1"/>
+      <c r="X85" s="1"/>
+      <c r="Y85" s="1"/>
+      <c r="Z85" s="1"/>
+    </row>
+    <row r="86" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A86" s="1"/>
+      <c r="B86" s="1"/>
+      <c r="C86" s="1"/>
+      <c r="D86" s="1"/>
+      <c r="E86" s="1"/>
+      <c r="F86" s="1"/>
+      <c r="G86" s="1"/>
+      <c r="H86" s="1"/>
+      <c r="I86" s="1"/>
+      <c r="J86" s="1"/>
+      <c r="K86" s="1"/>
+      <c r="L86" s="1"/>
+      <c r="M86" s="1"/>
+      <c r="N86" s="1"/>
+      <c r="O86" s="1"/>
+      <c r="P86" s="1"/>
+      <c r="Q86" s="1"/>
+      <c r="R86" s="1"/>
+      <c r="S86" s="1"/>
+      <c r="T86" s="1"/>
+      <c r="U86" s="1"/>
+      <c r="V86" s="1"/>
+      <c r="W86" s="1"/>
+      <c r="X86" s="1"/>
+      <c r="Y86" s="1"/>
+      <c r="Z86" s="1"/>
+    </row>
+    <row r="87" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A87" s="1"/>
+      <c r="B87" s="1"/>
+      <c r="C87" s="1"/>
+      <c r="D87" s="1"/>
+      <c r="E87" s="1"/>
+      <c r="F87" s="1"/>
+      <c r="G87" s="1"/>
+      <c r="H87" s="1"/>
+      <c r="I87" s="1"/>
+      <c r="J87" s="1"/>
+      <c r="K87" s="1"/>
+      <c r="L87" s="1"/>
+      <c r="M87" s="1"/>
+      <c r="N87" s="1"/>
+      <c r="O87" s="1"/>
+      <c r="P87" s="1"/>
+      <c r="Q87" s="1"/>
+      <c r="R87" s="1"/>
+      <c r="S87" s="1"/>
+      <c r="T87" s="1"/>
+      <c r="U87" s="1"/>
+      <c r="V87" s="1"/>
+      <c r="W87" s="1"/>
+      <c r="X87" s="1"/>
+      <c r="Y87" s="1"/>
+      <c r="Z87" s="1"/>
+    </row>
+    <row r="88" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A88" s="1"/>
+      <c r="B88" s="1"/>
+      <c r="C88" s="1"/>
+      <c r="D88" s="1"/>
+      <c r="E88" s="1"/>
+      <c r="F88" s="1"/>
+      <c r="G88" s="1"/>
+      <c r="H88" s="1"/>
+      <c r="I88" s="1"/>
+      <c r="J88" s="1"/>
+      <c r="K88" s="1"/>
+      <c r="L88" s="1"/>
+      <c r="M88" s="1"/>
+      <c r="N88" s="1"/>
+      <c r="O88" s="1"/>
+      <c r="P88" s="1"/>
+      <c r="Q88" s="1"/>
+      <c r="R88" s="1"/>
+      <c r="S88" s="1"/>
+      <c r="T88" s="1"/>
+      <c r="U88" s="1"/>
+      <c r="V88" s="1"/>
+      <c r="W88" s="1"/>
+      <c r="X88" s="1"/>
+      <c r="Y88" s="1"/>
+      <c r="Z88" s="1"/>
+    </row>
+    <row r="89" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A89" s="1"/>
+      <c r="B89" s="1"/>
+      <c r="C89" s="1"/>
+      <c r="D89" s="1"/>
+      <c r="E89" s="1"/>
+      <c r="F89" s="1"/>
+      <c r="G89" s="1"/>
+      <c r="H89" s="1"/>
+      <c r="I89" s="1"/>
+      <c r="J89" s="1"/>
+      <c r="K89" s="1"/>
+      <c r="L89" s="1"/>
+      <c r="M89" s="1"/>
+      <c r="N89" s="1"/>
+      <c r="O89" s="1"/>
+      <c r="P89" s="1"/>
+      <c r="Q89" s="1"/>
+      <c r="R89" s="1"/>
+      <c r="S89" s="1"/>
+      <c r="T89" s="1"/>
+      <c r="U89" s="1"/>
+      <c r="V89" s="1"/>
+      <c r="W89" s="1"/>
+      <c r="X89" s="1"/>
+      <c r="Y89" s="1"/>
+      <c r="Z89" s="1"/>
+    </row>
+    <row r="90" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A90" s="1"/>
+      <c r="B90" s="1"/>
+      <c r="C90" s="1"/>
+      <c r="D90" s="1"/>
+      <c r="E90" s="1"/>
+      <c r="F90" s="1"/>
+      <c r="G90" s="1"/>
+      <c r="H90" s="1"/>
+      <c r="I90" s="1"/>
+      <c r="J90" s="1"/>
+      <c r="K90" s="1"/>
+      <c r="L90" s="1"/>
+      <c r="M90" s="1"/>
+      <c r="N90" s="1"/>
+      <c r="O90" s="1"/>
+      <c r="P90" s="1"/>
+      <c r="Q90" s="1"/>
+      <c r="R90" s="1"/>
+      <c r="S90" s="1"/>
+      <c r="T90" s="1"/>
+      <c r="U90" s="1"/>
+      <c r="V90" s="1"/>
+      <c r="W90" s="1"/>
+      <c r="X90" s="1"/>
+      <c r="Y90" s="1"/>
+      <c r="Z90" s="1"/>
+    </row>
+    <row r="91" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A91" s="1"/>
+      <c r="B91" s="1"/>
+      <c r="C91" s="1"/>
+      <c r="D91" s="1"/>
+      <c r="E91" s="1"/>
+      <c r="F91" s="1"/>
+      <c r="G91" s="1"/>
+      <c r="H91" s="1"/>
+      <c r="I91" s="1"/>
+      <c r="J91" s="1"/>
+      <c r="K91" s="1"/>
+      <c r="L91" s="1"/>
+      <c r="M91" s="1"/>
+      <c r="N91" s="1"/>
+      <c r="O91" s="1"/>
+      <c r="P91" s="1"/>
+      <c r="Q91" s="1"/>
+      <c r="R91" s="1"/>
+      <c r="S91" s="1"/>
+      <c r="T91" s="1"/>
+      <c r="U91" s="1"/>
+      <c r="V91" s="1"/>
+      <c r="W91" s="1"/>
+      <c r="X91" s="1"/>
+      <c r="Y91" s="1"/>
+      <c r="Z91" s="1"/>
+    </row>
+    <row r="92" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A92" s="1"/>
+      <c r="B92" s="1"/>
+      <c r="C92" s="1"/>
+      <c r="D92" s="1"/>
+      <c r="E92" s="1"/>
+      <c r="F92" s="1"/>
+      <c r="G92" s="1"/>
+      <c r="H92" s="1"/>
+      <c r="I92" s="1"/>
+      <c r="J92" s="1"/>
+      <c r="K92" s="1"/>
+      <c r="L92" s="1"/>
+      <c r="M92" s="1"/>
+      <c r="N92" s="1"/>
+      <c r="O92" s="1"/>
+      <c r="P92" s="1"/>
+      <c r="Q92" s="1"/>
+      <c r="R92" s="1"/>
+      <c r="S92" s="1"/>
+      <c r="T92" s="1"/>
+      <c r="U92" s="1"/>
+      <c r="V92" s="1"/>
+      <c r="W92" s="1"/>
+      <c r="X92" s="1"/>
+      <c r="Y92" s="1"/>
+      <c r="Z92" s="1"/>
+    </row>
+    <row r="93" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A93" s="1"/>
+      <c r="B93" s="1"/>
+      <c r="C93" s="1"/>
+      <c r="D93" s="1"/>
+      <c r="E93" s="1"/>
+      <c r="F93" s="1"/>
+      <c r="G93" s="1"/>
+      <c r="H93" s="1"/>
+      <c r="I93" s="1"/>
+      <c r="J93" s="1"/>
+      <c r="K93" s="1"/>
+      <c r="L93" s="1"/>
+      <c r="M93" s="1"/>
+      <c r="N93" s="1"/>
+      <c r="O93" s="1"/>
+      <c r="P93" s="1"/>
+      <c r="Q93" s="1"/>
+      <c r="R93" s="1"/>
+      <c r="S93" s="1"/>
+      <c r="T93" s="1"/>
+      <c r="U93" s="1"/>
+      <c r="V93" s="1"/>
+      <c r="W93" s="1"/>
+      <c r="X93" s="1"/>
+      <c r="Y93" s="1"/>
+      <c r="Z93" s="1"/>
+    </row>
+    <row r="94" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A94" s="1"/>
+      <c r="B94" s="1"/>
+      <c r="C94" s="1"/>
+      <c r="D94" s="1"/>
+      <c r="E94" s="1"/>
+      <c r="F94" s="1"/>
+      <c r="G94" s="1"/>
+      <c r="H94" s="1"/>
+      <c r="I94" s="1"/>
+      <c r="J94" s="1"/>
+      <c r="K94" s="1"/>
+      <c r="L94" s="1"/>
+      <c r="M94" s="1"/>
+      <c r="N94" s="1"/>
+      <c r="O94" s="1"/>
+      <c r="P94" s="1"/>
+      <c r="Q94" s="1"/>
+      <c r="R94" s="1"/>
+      <c r="S94" s="1"/>
+      <c r="T94" s="1"/>
+      <c r="U94" s="1"/>
+      <c r="V94" s="1"/>
+      <c r="W94" s="1"/>
+      <c r="X94" s="1"/>
+      <c r="Y94" s="1"/>
+      <c r="Z94" s="1"/>
+    </row>
+    <row r="95" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A95" s="1"/>
+      <c r="B95" s="1"/>
+      <c r="C95" s="1"/>
+      <c r="D95" s="1"/>
+      <c r="E95" s="1"/>
+      <c r="F95" s="1"/>
+      <c r="G95" s="1"/>
+      <c r="H95" s="1"/>
+      <c r="I95" s="1"/>
+      <c r="J95" s="1"/>
+      <c r="K95" s="1"/>
+      <c r="L95" s="1"/>
+      <c r="M95" s="1"/>
+      <c r="N95" s="1"/>
+      <c r="O95" s="1"/>
+      <c r="P95" s="1"/>
+      <c r="Q95" s="1"/>
+      <c r="R95" s="1"/>
+      <c r="S95" s="1"/>
+      <c r="T95" s="1"/>
+      <c r="U95" s="1"/>
+      <c r="V95" s="1"/>
+      <c r="W95" s="1"/>
+      <c r="X95" s="1"/>
+      <c r="Y95" s="1"/>
+      <c r="Z95" s="1"/>
+    </row>
+    <row r="96" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A96" s="1"/>
+      <c r="B96" s="1"/>
+      <c r="C96" s="1"/>
+      <c r="D96" s="1"/>
+      <c r="E96" s="1"/>
+      <c r="F96" s="1"/>
+      <c r="G96" s="1"/>
+      <c r="H96" s="1"/>
+      <c r="I96" s="1"/>
+      <c r="J96" s="1"/>
+      <c r="K96" s="1"/>
+      <c r="L96" s="1"/>
+      <c r="M96" s="1"/>
+      <c r="N96" s="1"/>
+      <c r="O96" s="1"/>
+      <c r="P96" s="1"/>
+      <c r="Q96" s="1"/>
+      <c r="R96" s="1"/>
+      <c r="S96" s="1"/>
+      <c r="T96" s="1"/>
+      <c r="U96" s="1"/>
+      <c r="V96" s="1"/>
+      <c r="W96" s="1"/>
+      <c r="X96" s="1"/>
+      <c r="Y96" s="1"/>
+      <c r="Z96" s="1"/>
+    </row>
+    <row r="97" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A97" s="1"/>
+      <c r="B97" s="1"/>
+      <c r="C97" s="1"/>
+      <c r="D97" s="1"/>
+      <c r="E97" s="1"/>
+      <c r="F97" s="1"/>
+      <c r="G97" s="1"/>
+      <c r="H97" s="1"/>
+      <c r="I97" s="1"/>
+      <c r="J97" s="1"/>
+      <c r="K97" s="1"/>
+      <c r="L97" s="1"/>
+      <c r="M97" s="1"/>
+      <c r="N97" s="1"/>
+      <c r="O97" s="1"/>
+      <c r="P97" s="1"/>
+      <c r="Q97" s="1"/>
+      <c r="R97" s="1"/>
+      <c r="S97" s="1"/>
+      <c r="T97" s="1"/>
+      <c r="U97" s="1"/>
+      <c r="V97" s="1"/>
+      <c r="W97" s="1"/>
+      <c r="X97" s="1"/>
+      <c r="Y97" s="1"/>
+      <c r="Z97" s="1"/>
+    </row>
+    <row r="98" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A98" s="1"/>
+      <c r="B98" s="1"/>
+      <c r="C98" s="1"/>
+      <c r="D98" s="1"/>
+      <c r="E98" s="1"/>
+      <c r="F98" s="1"/>
+      <c r="G98" s="1"/>
+      <c r="H98" s="1"/>
+      <c r="I98" s="1"/>
+      <c r="J98" s="1"/>
+      <c r="K98" s="1"/>
+      <c r="L98" s="1"/>
+      <c r="M98" s="1"/>
+      <c r="N98" s="1"/>
+      <c r="O98" s="1"/>
+      <c r="P98" s="1"/>
+      <c r="Q98" s="1"/>
+      <c r="R98" s="1"/>
+      <c r="S98" s="1"/>
+      <c r="T98" s="1"/>
+      <c r="U98" s="1"/>
+      <c r="V98" s="1"/>
+      <c r="W98" s="1"/>
+      <c r="X98" s="1"/>
+      <c r="Y98" s="1"/>
+      <c r="Z98" s="1"/>
+    </row>
+    <row r="99" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A99" s="1"/>
+      <c r="B99" s="1"/>
+      <c r="C99" s="1"/>
+      <c r="D99" s="1"/>
+      <c r="E99" s="1"/>
+      <c r="F99" s="1"/>
+      <c r="G99" s="1"/>
+      <c r="H99" s="1"/>
+      <c r="I99" s="1"/>
+      <c r="J99" s="1"/>
+      <c r="K99" s="1"/>
+      <c r="L99" s="1"/>
+      <c r="M99" s="1"/>
+      <c r="N99" s="1"/>
+      <c r="O99" s="1"/>
+      <c r="P99" s="1"/>
+      <c r="Q99" s="1"/>
+      <c r="R99" s="1"/>
+      <c r="S99" s="1"/>
+      <c r="T99" s="1"/>
+      <c r="U99" s="1"/>
+      <c r="V99" s="1"/>
+      <c r="W99" s="1"/>
+      <c r="X99" s="1"/>
+      <c r="Y99" s="1"/>
+      <c r="Z99" s="1"/>
+    </row>
+    <row r="100" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A100" s="1"/>
+      <c r="B100" s="1"/>
+      <c r="C100" s="1"/>
+      <c r="D100" s="1"/>
+      <c r="E100" s="1"/>
+      <c r="F100" s="1"/>
+      <c r="G100" s="1"/>
+      <c r="H100" s="1"/>
+      <c r="I100" s="1"/>
+      <c r="J100" s="1"/>
+      <c r="K100" s="1"/>
+      <c r="L100" s="1"/>
+      <c r="M100" s="1"/>
+      <c r="N100" s="1"/>
+      <c r="O100" s="1"/>
+      <c r="P100" s="1"/>
+      <c r="Q100" s="1"/>
+      <c r="R100" s="1"/>
+      <c r="S100" s="1"/>
+      <c r="T100" s="1"/>
+      <c r="U100" s="1"/>
+      <c r="V100" s="1"/>
+      <c r="W100" s="1"/>
+      <c r="X100" s="1"/>
+      <c r="Y100" s="1"/>
+      <c r="Z100" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1501,12 +4125,12 @@
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="7" max="7" width="13.625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
moving files around for randomization 2017; creating 2018 randomization folder
randomizing wells for 2018 collection year for RT and SO treatments
</commit_message>
<xml_diff>
--- a/Data/2018-08-14_master_datac_2018_collection_year.xlsx
+++ b/Data/2018-08-14_master_datac_2018_collection_year.xlsx
@@ -1,32 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anbe642/zScience/Circadian_rhythm_runs_seasonal_timing/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andrew.nguyen\Desktop\Circadian_rhythm_runs_seasonal_timing\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{213DFDFB-3F16-7C40-B808-99605E9BAA3D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAA62708-4984-404C-B283-B1FF762D48E8}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1800" yWindow="1940" windowWidth="35820" windowHeight="18720" xr2:uid="{C7477166-8A7C-B04A-9643-C277FEDCDAAB}"/>
+    <workbookView xWindow="1800" yWindow="1935" windowWidth="35820" windowHeight="18720" activeTab="1" xr2:uid="{C7477166-8A7C-B04A-9643-C277FEDCDAAB}"/>
   </bookViews>
   <sheets>
     <sheet name="Maggot_Collections" sheetId="2" r:id="rId1"/>
     <sheet name="Data_collect" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="839" uniqueCount="181">
   <si>
     <t>Ind_ID</t>
   </si>
@@ -281,6 +286,294 @@
   </si>
   <si>
     <t>2018-08-31</t>
+  </si>
+  <si>
+    <t>GC</t>
+  </si>
+  <si>
+    <t>RT</t>
+  </si>
+  <si>
+    <t>SO</t>
+  </si>
+  <si>
+    <t>2018-08-16</t>
+  </si>
+  <si>
+    <t>green</t>
+  </si>
+  <si>
+    <t>red</t>
+  </si>
+  <si>
+    <t>A6-1</t>
+  </si>
+  <si>
+    <t>A6-2</t>
+  </si>
+  <si>
+    <t>A6-3</t>
+  </si>
+  <si>
+    <t>A6-4</t>
+  </si>
+  <si>
+    <t>A6-5</t>
+  </si>
+  <si>
+    <t>A6-6</t>
+  </si>
+  <si>
+    <t>A6-7</t>
+  </si>
+  <si>
+    <t>A6-8</t>
+  </si>
+  <si>
+    <t>A6-9</t>
+  </si>
+  <si>
+    <t>A6-10</t>
+  </si>
+  <si>
+    <t>A6-11</t>
+  </si>
+  <si>
+    <t>A6-12</t>
+  </si>
+  <si>
+    <t>A6-13</t>
+  </si>
+  <si>
+    <t>A6-14</t>
+  </si>
+  <si>
+    <t>A6-15</t>
+  </si>
+  <si>
+    <t>A6-16</t>
+  </si>
+  <si>
+    <t>A6-17</t>
+  </si>
+  <si>
+    <t>A6-18</t>
+  </si>
+  <si>
+    <t>A6-19</t>
+  </si>
+  <si>
+    <t>A6-20</t>
+  </si>
+  <si>
+    <t>A6-21</t>
+  </si>
+  <si>
+    <t>A6-22</t>
+  </si>
+  <si>
+    <t>A6-23</t>
+  </si>
+  <si>
+    <t>A6-24</t>
+  </si>
+  <si>
+    <t>A6-25</t>
+  </si>
+  <si>
+    <t>A6-26</t>
+  </si>
+  <si>
+    <t>A6-27</t>
+  </si>
+  <si>
+    <t>A6-28</t>
+  </si>
+  <si>
+    <t>A6-29</t>
+  </si>
+  <si>
+    <t>A6-30</t>
+  </si>
+  <si>
+    <t>A2</t>
+  </si>
+  <si>
+    <t>F12</t>
+  </si>
+  <si>
+    <t>H2</t>
+  </si>
+  <si>
+    <t>C5</t>
+  </si>
+  <si>
+    <t>B4</t>
+  </si>
+  <si>
+    <t>B9</t>
+  </si>
+  <si>
+    <t>C10</t>
+  </si>
+  <si>
+    <t>G2</t>
+  </si>
+  <si>
+    <t>D11</t>
+  </si>
+  <si>
+    <t>B11</t>
+  </si>
+  <si>
+    <t>B6</t>
+  </si>
+  <si>
+    <t>E7</t>
+  </si>
+  <si>
+    <t>B12</t>
+  </si>
+  <si>
+    <t>A9</t>
+  </si>
+  <si>
+    <t>F8</t>
+  </si>
+  <si>
+    <t>C7</t>
+  </si>
+  <si>
+    <t>G7</t>
+  </si>
+  <si>
+    <t>E1</t>
+  </si>
+  <si>
+    <t>A10</t>
+  </si>
+  <si>
+    <t>G3</t>
+  </si>
+  <si>
+    <t>H4</t>
+  </si>
+  <si>
+    <t>H11</t>
+  </si>
+  <si>
+    <t>B2</t>
+  </si>
+  <si>
+    <t>H6</t>
+  </si>
+  <si>
+    <t>C11</t>
+  </si>
+  <si>
+    <t>H5</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>G12</t>
+  </si>
+  <si>
+    <t>G8</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>F4</t>
+  </si>
+  <si>
+    <t>D9</t>
+  </si>
+  <si>
+    <t>H8</t>
+  </si>
+  <si>
+    <t>H12</t>
+  </si>
+  <si>
+    <t>B10</t>
+  </si>
+  <si>
+    <t>D3</t>
+  </si>
+  <si>
+    <t>E6</t>
+  </si>
+  <si>
+    <t>F1</t>
+  </si>
+  <si>
+    <t>F11</t>
+  </si>
+  <si>
+    <t>G9</t>
+  </si>
+  <si>
+    <t>D6</t>
+  </si>
+  <si>
+    <t>C4</t>
+  </si>
+  <si>
+    <t>D12</t>
+  </si>
+  <si>
+    <t>B5</t>
+  </si>
+  <si>
+    <t>A7</t>
+  </si>
+  <si>
+    <t>H3</t>
+  </si>
+  <si>
+    <t>A8</t>
+  </si>
+  <si>
+    <t>E9</t>
+  </si>
+  <si>
+    <t>C6</t>
+  </si>
+  <si>
+    <t>B1</t>
+  </si>
+  <si>
+    <t>D8</t>
+  </si>
+  <si>
+    <t>F7</t>
+  </si>
+  <si>
+    <t>D2</t>
+  </si>
+  <si>
+    <t>B8</t>
+  </si>
+  <si>
+    <t>H10</t>
+  </si>
+  <si>
+    <t>E12</t>
+  </si>
+  <si>
+    <t>C9</t>
+  </si>
+  <si>
+    <t>B7</t>
+  </si>
+  <si>
+    <t>E2</t>
+  </si>
+  <si>
+    <t>E3</t>
   </si>
 </sst>
 </file>
@@ -678,16 +971,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D3F78F5-4EA8-6A42-B216-41A8EC7A5E8D}">
   <dimension ref="A1:Z100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S25" sqref="S25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:XFD7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="6" max="6" width="14.1640625" customWidth="1"/>
+    <col min="6" max="6" width="14.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>45</v>
       </c>
@@ -734,7 +1027,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>58</v>
       </c>
@@ -774,7 +1067,7 @@
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>58</v>
       </c>
@@ -814,7 +1107,7 @@
       <c r="S3" s="1"/>
       <c r="T3" s="1"/>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>58</v>
       </c>
@@ -851,7 +1144,7 @@
       <c r="S4" s="1"/>
       <c r="T4" s="1"/>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>58</v>
       </c>
@@ -888,7 +1181,7 @@
       <c r="S5" s="1"/>
       <c r="T5" s="1"/>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>58</v>
       </c>
@@ -937,7 +1230,7 @@
       <c r="S6" s="1"/>
       <c r="T6" s="1"/>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>58</v>
       </c>
@@ -986,7 +1279,7 @@
       <c r="S7" s="1"/>
       <c r="T7" s="1"/>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>58</v>
       </c>
@@ -1035,7 +1328,7 @@
       <c r="S8" s="1"/>
       <c r="T8" s="1"/>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>58</v>
       </c>
@@ -1084,7 +1377,7 @@
       <c r="S9" s="1"/>
       <c r="T9" s="1"/>
     </row>
-    <row r="10" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>58</v>
       </c>
@@ -1133,7 +1426,7 @@
       <c r="S10" s="14"/>
       <c r="T10" s="14"/>
     </row>
-    <row r="11" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
         <v>58</v>
       </c>
@@ -1182,7 +1475,7 @@
       <c r="S11" s="14"/>
       <c r="T11" s="14"/>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>58</v>
       </c>
@@ -1231,7 +1524,7 @@
       <c r="S12" s="1"/>
       <c r="T12" s="1"/>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>58</v>
       </c>
@@ -1280,7 +1573,7 @@
       <c r="S13" s="1"/>
       <c r="T13" s="1"/>
     </row>
-    <row r="14" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
         <v>58</v>
       </c>
@@ -1329,7 +1622,7 @@
       <c r="S14" s="14"/>
       <c r="T14" s="14"/>
     </row>
-    <row r="15" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
         <v>58</v>
       </c>
@@ -1378,7 +1671,7 @@
       <c r="S15" s="14"/>
       <c r="T15" s="14"/>
     </row>
-    <row r="16" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
         <v>58</v>
       </c>
@@ -1427,7 +1720,7 @@
       <c r="S16" s="14"/>
       <c r="T16" s="14"/>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>58</v>
       </c>
@@ -1476,7 +1769,7 @@
       <c r="S17" s="1"/>
       <c r="T17" s="1"/>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>58</v>
       </c>
@@ -1525,7 +1818,7 @@
       <c r="S18" s="1"/>
       <c r="T18" s="1"/>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>58</v>
       </c>
@@ -1574,7 +1867,7 @@
       <c r="S19" s="1"/>
       <c r="T19" s="1"/>
     </row>
-    <row r="20" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>58</v>
       </c>
@@ -1623,7 +1916,7 @@
       <c r="S20" s="14"/>
       <c r="T20" s="14"/>
     </row>
-    <row r="21" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
         <v>58</v>
       </c>
@@ -1672,7 +1965,7 @@
       <c r="S21" s="14"/>
       <c r="T21" s="14"/>
     </row>
-    <row r="22" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
         <v>58</v>
       </c>
@@ -1721,7 +2014,7 @@
       <c r="S22" s="14"/>
       <c r="T22" s="14"/>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>58</v>
       </c>
@@ -1770,7 +2063,7 @@
       <c r="S23" s="1"/>
       <c r="T23" s="1"/>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>58</v>
       </c>
@@ -1819,7 +2112,7 @@
       <c r="S24" s="1"/>
       <c r="T24" s="1"/>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>58</v>
       </c>
@@ -1868,7 +2161,7 @@
       <c r="S25" s="1"/>
       <c r="T25" s="1"/>
     </row>
-    <row r="26" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="s">
         <v>58</v>
       </c>
@@ -1917,7 +2210,7 @@
       <c r="S26" s="14"/>
       <c r="T26" s="14"/>
     </row>
-    <row r="27" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="11" t="s">
         <v>58</v>
       </c>
@@ -1966,7 +2259,7 @@
       <c r="S27" s="14"/>
       <c r="T27" s="14"/>
     </row>
-    <row r="28" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="s">
         <v>58</v>
       </c>
@@ -2015,7 +2308,7 @@
       <c r="S28" s="14"/>
       <c r="T28" s="14"/>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>58</v>
       </c>
@@ -2064,7 +2357,7 @@
       <c r="S29" s="1"/>
       <c r="T29" s="1"/>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>58</v>
       </c>
@@ -2113,7 +2406,7 @@
       <c r="S30" s="1"/>
       <c r="T30" s="1"/>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>58</v>
       </c>
@@ -2162,7 +2455,7 @@
       <c r="S31" s="1"/>
       <c r="T31" s="1"/>
     </row>
-    <row r="32" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="11" t="s">
         <v>58</v>
       </c>
@@ -2211,7 +2504,7 @@
       <c r="S32" s="14"/>
       <c r="T32" s="14"/>
     </row>
-    <row r="33" spans="1:26" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:26" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="11" t="s">
         <v>58</v>
       </c>
@@ -2260,7 +2553,7 @@
       <c r="S33" s="14"/>
       <c r="T33" s="14"/>
     </row>
-    <row r="34" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -2290,7 +2583,7 @@
       <c r="Y34" s="1"/>
       <c r="Z34" s="1"/>
     </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -2318,7 +2611,7 @@
       <c r="Y35" s="1"/>
       <c r="Z35" s="1"/>
     </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -2346,7 +2639,7 @@
       <c r="Y36" s="1"/>
       <c r="Z36" s="1"/>
     </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -2374,7 +2667,7 @@
       <c r="Y37" s="1"/>
       <c r="Z37" s="1"/>
     </row>
-    <row r="38" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -2402,7 +2695,7 @@
       <c r="Y38" s="1"/>
       <c r="Z38" s="1"/>
     </row>
-    <row r="39" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -2430,7 +2723,7 @@
       <c r="Y39" s="1"/>
       <c r="Z39" s="1"/>
     </row>
-    <row r="40" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -2458,7 +2751,7 @@
       <c r="Y40" s="1"/>
       <c r="Z40" s="1"/>
     </row>
-    <row r="41" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -2486,7 +2779,7 @@
       <c r="Y41" s="1"/>
       <c r="Z41" s="1"/>
     </row>
-    <row r="42" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -2514,7 +2807,7 @@
       <c r="Y42" s="1"/>
       <c r="Z42" s="1"/>
     </row>
-    <row r="43" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -2542,7 +2835,7 @@
       <c r="Y43" s="1"/>
       <c r="Z43" s="1"/>
     </row>
-    <row r="44" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -2570,7 +2863,7 @@
       <c r="Y44" s="1"/>
       <c r="Z44" s="1"/>
     </row>
-    <row r="45" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -2598,7 +2891,7 @@
       <c r="Y45" s="1"/>
       <c r="Z45" s="1"/>
     </row>
-    <row r="46" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
@@ -2626,7 +2919,7 @@
       <c r="Y46" s="1"/>
       <c r="Z46" s="1"/>
     </row>
-    <row r="47" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -2654,7 +2947,7 @@
       <c r="Y47" s="1"/>
       <c r="Z47" s="1"/>
     </row>
-    <row r="48" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -2682,7 +2975,7 @@
       <c r="Y48" s="1"/>
       <c r="Z48" s="1"/>
     </row>
-    <row r="49" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -2710,7 +3003,7 @@
       <c r="Y49" s="1"/>
       <c r="Z49" s="1"/>
     </row>
-    <row r="50" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -2738,7 +3031,7 @@
       <c r="Y50" s="1"/>
       <c r="Z50" s="1"/>
     </row>
-    <row r="51" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -2766,7 +3059,7 @@
       <c r="Y51" s="1"/>
       <c r="Z51" s="1"/>
     </row>
-    <row r="52" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -2794,7 +3087,7 @@
       <c r="Y52" s="1"/>
       <c r="Z52" s="1"/>
     </row>
-    <row r="53" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -2822,7 +3115,7 @@
       <c r="Y53" s="1"/>
       <c r="Z53" s="1"/>
     </row>
-    <row r="54" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
@@ -2850,7 +3143,7 @@
       <c r="Y54" s="1"/>
       <c r="Z54" s="1"/>
     </row>
-    <row r="55" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
@@ -2878,7 +3171,7 @@
       <c r="Y55" s="1"/>
       <c r="Z55" s="1"/>
     </row>
-    <row r="56" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
@@ -2906,7 +3199,7 @@
       <c r="Y56" s="1"/>
       <c r="Z56" s="1"/>
     </row>
-    <row r="57" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
@@ -2934,7 +3227,7 @@
       <c r="Y57" s="1"/>
       <c r="Z57" s="1"/>
     </row>
-    <row r="58" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -2962,7 +3255,7 @@
       <c r="Y58" s="1"/>
       <c r="Z58" s="1"/>
     </row>
-    <row r="59" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
@@ -2990,7 +3283,7 @@
       <c r="Y59" s="1"/>
       <c r="Z59" s="1"/>
     </row>
-    <row r="60" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -3018,7 +3311,7 @@
       <c r="Y60" s="1"/>
       <c r="Z60" s="1"/>
     </row>
-    <row r="61" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
@@ -3046,7 +3339,7 @@
       <c r="Y61" s="1"/>
       <c r="Z61" s="1"/>
     </row>
-    <row r="62" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
@@ -3074,7 +3367,7 @@
       <c r="Y62" s="1"/>
       <c r="Z62" s="1"/>
     </row>
-    <row r="63" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
@@ -3102,7 +3395,7 @@
       <c r="Y63" s="1"/>
       <c r="Z63" s="1"/>
     </row>
-    <row r="64" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
@@ -3130,7 +3423,7 @@
       <c r="Y64" s="1"/>
       <c r="Z64" s="1"/>
     </row>
-    <row r="65" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
@@ -3158,7 +3451,7 @@
       <c r="Y65" s="1"/>
       <c r="Z65" s="1"/>
     </row>
-    <row r="66" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
@@ -3186,7 +3479,7 @@
       <c r="Y66" s="1"/>
       <c r="Z66" s="1"/>
     </row>
-    <row r="67" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
@@ -3214,7 +3507,7 @@
       <c r="Y67" s="1"/>
       <c r="Z67" s="1"/>
     </row>
-    <row r="68" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
@@ -3242,7 +3535,7 @@
       <c r="Y68" s="1"/>
       <c r="Z68" s="1"/>
     </row>
-    <row r="69" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
@@ -3270,7 +3563,7 @@
       <c r="Y69" s="1"/>
       <c r="Z69" s="1"/>
     </row>
-    <row r="70" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
@@ -3298,7 +3591,7 @@
       <c r="Y70" s="1"/>
       <c r="Z70" s="1"/>
     </row>
-    <row r="71" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
@@ -3326,7 +3619,7 @@
       <c r="Y71" s="1"/>
       <c r="Z71" s="1"/>
     </row>
-    <row r="72" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A72" s="1"/>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
@@ -3354,7 +3647,7 @@
       <c r="Y72" s="1"/>
       <c r="Z72" s="1"/>
     </row>
-    <row r="73" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
@@ -3382,7 +3675,7 @@
       <c r="Y73" s="1"/>
       <c r="Z73" s="1"/>
     </row>
-    <row r="74" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
@@ -3410,7 +3703,7 @@
       <c r="Y74" s="1"/>
       <c r="Z74" s="1"/>
     </row>
-    <row r="75" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
@@ -3438,7 +3731,7 @@
       <c r="Y75" s="1"/>
       <c r="Z75" s="1"/>
     </row>
-    <row r="76" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A76" s="1"/>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
@@ -3466,7 +3759,7 @@
       <c r="Y76" s="1"/>
       <c r="Z76" s="1"/>
     </row>
-    <row r="77" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
@@ -3494,7 +3787,7 @@
       <c r="Y77" s="1"/>
       <c r="Z77" s="1"/>
     </row>
-    <row r="78" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
@@ -3522,7 +3815,7 @@
       <c r="Y78" s="1"/>
       <c r="Z78" s="1"/>
     </row>
-    <row r="79" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
@@ -3550,7 +3843,7 @@
       <c r="Y79" s="1"/>
       <c r="Z79" s="1"/>
     </row>
-    <row r="80" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
@@ -3578,7 +3871,7 @@
       <c r="Y80" s="1"/>
       <c r="Z80" s="1"/>
     </row>
-    <row r="81" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A81" s="1"/>
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
@@ -3606,7 +3899,7 @@
       <c r="Y81" s="1"/>
       <c r="Z81" s="1"/>
     </row>
-    <row r="82" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A82" s="1"/>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
@@ -3634,7 +3927,7 @@
       <c r="Y82" s="1"/>
       <c r="Z82" s="1"/>
     </row>
-    <row r="83" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A83" s="1"/>
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
@@ -3662,7 +3955,7 @@
       <c r="Y83" s="1"/>
       <c r="Z83" s="1"/>
     </row>
-    <row r="84" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A84" s="1"/>
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
@@ -3690,7 +3983,7 @@
       <c r="Y84" s="1"/>
       <c r="Z84" s="1"/>
     </row>
-    <row r="85" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A85" s="1"/>
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
@@ -3718,7 +4011,7 @@
       <c r="Y85" s="1"/>
       <c r="Z85" s="1"/>
     </row>
-    <row r="86" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A86" s="1"/>
       <c r="B86" s="1"/>
       <c r="C86" s="1"/>
@@ -3746,7 +4039,7 @@
       <c r="Y86" s="1"/>
       <c r="Z86" s="1"/>
     </row>
-    <row r="87" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A87" s="1"/>
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
@@ -3774,7 +4067,7 @@
       <c r="Y87" s="1"/>
       <c r="Z87" s="1"/>
     </row>
-    <row r="88" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A88" s="1"/>
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
@@ -3802,7 +4095,7 @@
       <c r="Y88" s="1"/>
       <c r="Z88" s="1"/>
     </row>
-    <row r="89" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A89" s="1"/>
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
@@ -3830,7 +4123,7 @@
       <c r="Y89" s="1"/>
       <c r="Z89" s="1"/>
     </row>
-    <row r="90" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A90" s="1"/>
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
@@ -3858,7 +4151,7 @@
       <c r="Y90" s="1"/>
       <c r="Z90" s="1"/>
     </row>
-    <row r="91" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A91" s="1"/>
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
@@ -3886,7 +4179,7 @@
       <c r="Y91" s="1"/>
       <c r="Z91" s="1"/>
     </row>
-    <row r="92" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A92" s="1"/>
       <c r="B92" s="1"/>
       <c r="C92" s="1"/>
@@ -3914,7 +4207,7 @@
       <c r="Y92" s="1"/>
       <c r="Z92" s="1"/>
     </row>
-    <row r="93" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A93" s="1"/>
       <c r="B93" s="1"/>
       <c r="C93" s="1"/>
@@ -3942,7 +4235,7 @@
       <c r="Y93" s="1"/>
       <c r="Z93" s="1"/>
     </row>
-    <row r="94" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A94" s="1"/>
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
@@ -3970,7 +4263,7 @@
       <c r="Y94" s="1"/>
       <c r="Z94" s="1"/>
     </row>
-    <row r="95" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A95" s="1"/>
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
@@ -3998,7 +4291,7 @@
       <c r="Y95" s="1"/>
       <c r="Z95" s="1"/>
     </row>
-    <row r="96" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A96" s="1"/>
       <c r="B96" s="1"/>
       <c r="C96" s="1"/>
@@ -4026,7 +4319,7 @@
       <c r="Y96" s="1"/>
       <c r="Z96" s="1"/>
     </row>
-    <row r="97" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A97" s="1"/>
       <c r="B97" s="1"/>
       <c r="C97" s="1"/>
@@ -4054,7 +4347,7 @@
       <c r="Y97" s="1"/>
       <c r="Z97" s="1"/>
     </row>
-    <row r="98" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A98" s="1"/>
       <c r="B98" s="1"/>
       <c r="C98" s="1"/>
@@ -4082,7 +4375,7 @@
       <c r="Y98" s="1"/>
       <c r="Z98" s="1"/>
     </row>
-    <row r="99" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A99" s="1"/>
       <c r="B99" s="1"/>
       <c r="C99" s="1"/>
@@ -4110,7 +4403,7 @@
       <c r="Y99" s="1"/>
       <c r="Z99" s="1"/>
     </row>
-    <row r="100" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A100" s="1"/>
       <c r="B100" s="1"/>
       <c r="C100" s="1"/>
@@ -4146,18 +4439,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92725FB9-1A17-2546-9DFA-6C0D39437891}">
-  <dimension ref="A1:AS1"/>
+  <dimension ref="A1:AS91"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" topLeftCell="Q18" workbookViewId="0">
+      <selection activeCell="AB32" sqref="AB32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="7" max="7" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.375" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4176,7 +4470,7 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
@@ -4294,7 +4588,2228 @@
         <v>44</v>
       </c>
     </row>
+    <row r="2" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K2" t="s">
+        <v>61</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="3" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K3" t="s">
+        <v>61</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K4" t="s">
+        <v>61</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K5" t="s">
+        <v>61</v>
+      </c>
+      <c r="T5" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="6" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K6" t="s">
+        <v>61</v>
+      </c>
+      <c r="T6" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="7" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K7" t="s">
+        <v>61</v>
+      </c>
+      <c r="T7" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="8" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K8" t="s">
+        <v>61</v>
+      </c>
+      <c r="T8" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="9" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K9" t="s">
+        <v>61</v>
+      </c>
+      <c r="T9" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="10" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K10" t="s">
+        <v>61</v>
+      </c>
+      <c r="T10" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y10" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z10" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="11" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K11" t="s">
+        <v>61</v>
+      </c>
+      <c r="T11" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K12" t="s">
+        <v>61</v>
+      </c>
+      <c r="T12" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z12" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="13" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K13" t="s">
+        <v>61</v>
+      </c>
+      <c r="T13" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y13" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z13" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="14" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K14" t="s">
+        <v>61</v>
+      </c>
+      <c r="T14" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y14" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z14" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="15" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K15" t="s">
+        <v>61</v>
+      </c>
+      <c r="T15" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y15" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z15" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="16" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K16" t="s">
+        <v>61</v>
+      </c>
+      <c r="T16" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y16" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z16" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="17" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K17" t="s">
+        <v>61</v>
+      </c>
+      <c r="T17" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y17" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z17" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="18" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K18" t="s">
+        <v>61</v>
+      </c>
+      <c r="T18" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y18" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z18" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="19" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K19" t="s">
+        <v>61</v>
+      </c>
+      <c r="T19" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y19" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z19" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="20" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K20" t="s">
+        <v>61</v>
+      </c>
+      <c r="T20" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y20" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z20" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="21" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K21" t="s">
+        <v>61</v>
+      </c>
+      <c r="T21" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y21" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z21" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="22" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K22" t="s">
+        <v>61</v>
+      </c>
+      <c r="T22" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y22" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z22" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="23" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K23" t="s">
+        <v>61</v>
+      </c>
+      <c r="T23" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y23" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z23" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="24" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K24" t="s">
+        <v>61</v>
+      </c>
+      <c r="T24" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y24" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z24" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="25" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K25" t="s">
+        <v>61</v>
+      </c>
+      <c r="T25" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y25" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z25" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="26" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K26" t="s">
+        <v>61</v>
+      </c>
+      <c r="T26" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y26" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z26" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="27" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K27" t="s">
+        <v>61</v>
+      </c>
+      <c r="T27" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y27" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z27" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="28" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K28" t="s">
+        <v>61</v>
+      </c>
+      <c r="T28" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y28" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z28" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="29" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K29" t="s">
+        <v>61</v>
+      </c>
+      <c r="T29" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y29" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z29" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="30" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K30" t="s">
+        <v>61</v>
+      </c>
+      <c r="T30" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y30" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z30" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="31" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K31" t="s">
+        <v>61</v>
+      </c>
+      <c r="T31" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y31" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z31" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="32" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>1</v>
+      </c>
+      <c r="B32" t="s">
+        <v>89</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K32" t="s">
+        <v>61</v>
+      </c>
+      <c r="T32" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y32" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z32" t="str">
+        <f>"A6"&amp;Y32&amp;"-"&amp;AC32</f>
+        <v>A6RT-A2</v>
+      </c>
+      <c r="AC32" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="33" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>2</v>
+      </c>
+      <c r="B33" t="s">
+        <v>89</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K33" t="s">
+        <v>61</v>
+      </c>
+      <c r="T33" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y33" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z33" t="str">
+        <f t="shared" ref="Z33:Z91" si="0">"A6"&amp;Y33&amp;"-"&amp;AC33</f>
+        <v>A6RT-F12</v>
+      </c>
+      <c r="AC33" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="34" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>3</v>
+      </c>
+      <c r="B34" t="s">
+        <v>89</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K34" t="s">
+        <v>61</v>
+      </c>
+      <c r="T34" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y34" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z34" t="str">
+        <f t="shared" si="0"/>
+        <v>A6RT-H2</v>
+      </c>
+      <c r="AC34" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="35" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>4</v>
+      </c>
+      <c r="B35" t="s">
+        <v>89</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K35" t="s">
+        <v>61</v>
+      </c>
+      <c r="T35" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y35" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z35" t="str">
+        <f t="shared" si="0"/>
+        <v>A6RT-C5</v>
+      </c>
+      <c r="AC35" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="36" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>5</v>
+      </c>
+      <c r="B36" t="s">
+        <v>89</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K36" t="s">
+        <v>61</v>
+      </c>
+      <c r="T36" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y36" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z36" t="str">
+        <f t="shared" si="0"/>
+        <v>A6RT-B4</v>
+      </c>
+      <c r="AC36" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="37" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>6</v>
+      </c>
+      <c r="B37" t="s">
+        <v>89</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K37" t="s">
+        <v>61</v>
+      </c>
+      <c r="T37" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y37" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z37" t="str">
+        <f t="shared" si="0"/>
+        <v>A6RT-B9</v>
+      </c>
+      <c r="AC37" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="38" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>7</v>
+      </c>
+      <c r="B38" t="s">
+        <v>89</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K38" t="s">
+        <v>61</v>
+      </c>
+      <c r="T38" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y38" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z38" t="str">
+        <f t="shared" si="0"/>
+        <v>A6RT-C10</v>
+      </c>
+      <c r="AC38" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="39" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>8</v>
+      </c>
+      <c r="B39" t="s">
+        <v>89</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K39" t="s">
+        <v>61</v>
+      </c>
+      <c r="T39" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y39" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z39" t="str">
+        <f t="shared" si="0"/>
+        <v>A6RT-G2</v>
+      </c>
+      <c r="AC39" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="40" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>9</v>
+      </c>
+      <c r="B40" t="s">
+        <v>89</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K40" t="s">
+        <v>61</v>
+      </c>
+      <c r="T40" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y40" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z40" t="str">
+        <f t="shared" si="0"/>
+        <v>A6RT-D11</v>
+      </c>
+      <c r="AC40" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="41" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>10</v>
+      </c>
+      <c r="B41" t="s">
+        <v>89</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K41" t="s">
+        <v>61</v>
+      </c>
+      <c r="T41" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y41" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z41" t="str">
+        <f t="shared" si="0"/>
+        <v>A6RT-B11</v>
+      </c>
+      <c r="AC41" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="42" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>11</v>
+      </c>
+      <c r="B42" t="s">
+        <v>89</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K42" t="s">
+        <v>61</v>
+      </c>
+      <c r="T42" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y42" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z42" t="str">
+        <f t="shared" si="0"/>
+        <v>A6RT-B6</v>
+      </c>
+      <c r="AC42" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="43" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>12</v>
+      </c>
+      <c r="B43" t="s">
+        <v>89</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K43" t="s">
+        <v>61</v>
+      </c>
+      <c r="T43" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y43" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z43" t="str">
+        <f t="shared" si="0"/>
+        <v>A6RT-E7</v>
+      </c>
+      <c r="AC43" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="44" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>13</v>
+      </c>
+      <c r="B44" t="s">
+        <v>89</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K44" t="s">
+        <v>61</v>
+      </c>
+      <c r="T44" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y44" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z44" t="str">
+        <f t="shared" si="0"/>
+        <v>A6RT-B12</v>
+      </c>
+      <c r="AC44" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="45" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>14</v>
+      </c>
+      <c r="B45" t="s">
+        <v>89</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K45" t="s">
+        <v>61</v>
+      </c>
+      <c r="T45" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y45" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z45" t="str">
+        <f t="shared" si="0"/>
+        <v>A6RT-A9</v>
+      </c>
+      <c r="AC45" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="46" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>15</v>
+      </c>
+      <c r="B46" t="s">
+        <v>89</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K46" t="s">
+        <v>61</v>
+      </c>
+      <c r="T46" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y46" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z46" t="str">
+        <f t="shared" si="0"/>
+        <v>A6RT-F8</v>
+      </c>
+      <c r="AC46" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="47" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>16</v>
+      </c>
+      <c r="B47" t="s">
+        <v>89</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K47" t="s">
+        <v>61</v>
+      </c>
+      <c r="T47" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y47" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z47" t="str">
+        <f t="shared" si="0"/>
+        <v>A6RT-C7</v>
+      </c>
+      <c r="AC47" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="48" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>17</v>
+      </c>
+      <c r="B48" t="s">
+        <v>89</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K48" t="s">
+        <v>61</v>
+      </c>
+      <c r="T48" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y48" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z48" t="str">
+        <f t="shared" si="0"/>
+        <v>A6RT-G7</v>
+      </c>
+      <c r="AC48" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="49" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>18</v>
+      </c>
+      <c r="B49" t="s">
+        <v>89</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K49" t="s">
+        <v>61</v>
+      </c>
+      <c r="T49" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y49" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z49" t="str">
+        <f t="shared" si="0"/>
+        <v>A6RT-E1</v>
+      </c>
+      <c r="AC49" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="50" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>19</v>
+      </c>
+      <c r="B50" t="s">
+        <v>89</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K50" t="s">
+        <v>61</v>
+      </c>
+      <c r="T50" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y50" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z50" t="str">
+        <f t="shared" si="0"/>
+        <v>A6RT-A10</v>
+      </c>
+      <c r="AC50" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="51" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>20</v>
+      </c>
+      <c r="B51" t="s">
+        <v>89</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K51" t="s">
+        <v>61</v>
+      </c>
+      <c r="T51" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y51" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z51" t="str">
+        <f t="shared" si="0"/>
+        <v>A6RT-G3</v>
+      </c>
+      <c r="AC51" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="52" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>21</v>
+      </c>
+      <c r="B52" t="s">
+        <v>89</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K52" t="s">
+        <v>61</v>
+      </c>
+      <c r="T52" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y52" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z52" t="str">
+        <f t="shared" si="0"/>
+        <v>A6RT-H4</v>
+      </c>
+      <c r="AC52" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="53" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>22</v>
+      </c>
+      <c r="B53" t="s">
+        <v>89</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K53" t="s">
+        <v>61</v>
+      </c>
+      <c r="T53" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y53" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z53" t="str">
+        <f t="shared" si="0"/>
+        <v>A6RT-H11</v>
+      </c>
+      <c r="AC53" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="54" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>23</v>
+      </c>
+      <c r="B54" t="s">
+        <v>89</v>
+      </c>
+      <c r="G54" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K54" t="s">
+        <v>61</v>
+      </c>
+      <c r="T54" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y54" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z54" t="str">
+        <f t="shared" si="0"/>
+        <v>A6RT-B2</v>
+      </c>
+      <c r="AC54" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="55" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>24</v>
+      </c>
+      <c r="B55" t="s">
+        <v>89</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K55" t="s">
+        <v>61</v>
+      </c>
+      <c r="T55" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y55" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z55" t="str">
+        <f t="shared" si="0"/>
+        <v>A6RT-H6</v>
+      </c>
+      <c r="AC55" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="56" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>25</v>
+      </c>
+      <c r="B56" t="s">
+        <v>89</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K56" t="s">
+        <v>61</v>
+      </c>
+      <c r="T56" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y56" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z56" t="str">
+        <f t="shared" si="0"/>
+        <v>A6RT-C11</v>
+      </c>
+      <c r="AC56" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="57" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>26</v>
+      </c>
+      <c r="B57" t="s">
+        <v>89</v>
+      </c>
+      <c r="G57" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K57" t="s">
+        <v>61</v>
+      </c>
+      <c r="T57" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y57" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z57" t="str">
+        <f t="shared" si="0"/>
+        <v>A6RT-H5</v>
+      </c>
+      <c r="AC57" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="58" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>27</v>
+      </c>
+      <c r="B58" t="s">
+        <v>89</v>
+      </c>
+      <c r="G58" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K58" t="s">
+        <v>61</v>
+      </c>
+      <c r="T58" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y58" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z58" t="str">
+        <f t="shared" si="0"/>
+        <v>A6RT-C1</v>
+      </c>
+      <c r="AC58" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="59" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>28</v>
+      </c>
+      <c r="B59" t="s">
+        <v>89</v>
+      </c>
+      <c r="G59" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K59" t="s">
+        <v>61</v>
+      </c>
+      <c r="T59" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y59" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z59" t="str">
+        <f t="shared" si="0"/>
+        <v>A6RT-G12</v>
+      </c>
+      <c r="AC59" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="60" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>29</v>
+      </c>
+      <c r="B60" t="s">
+        <v>89</v>
+      </c>
+      <c r="G60" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K60" t="s">
+        <v>61</v>
+      </c>
+      <c r="T60" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y60" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z60" t="str">
+        <f t="shared" si="0"/>
+        <v>A6RT-G8</v>
+      </c>
+      <c r="AC60" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="61" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>30</v>
+      </c>
+      <c r="B61" t="s">
+        <v>89</v>
+      </c>
+      <c r="G61" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K61" t="s">
+        <v>61</v>
+      </c>
+      <c r="T61" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y61" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z61" t="str">
+        <f t="shared" si="0"/>
+        <v>A6RT-C2</v>
+      </c>
+      <c r="AC61" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="62" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>1</v>
+      </c>
+      <c r="B62" t="s">
+        <v>90</v>
+      </c>
+      <c r="G62" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K62" t="s">
+        <v>61</v>
+      </c>
+      <c r="T62" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y62" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z62" t="str">
+        <f t="shared" si="0"/>
+        <v>A6SO-F4</v>
+      </c>
+      <c r="AC62" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="63" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>2</v>
+      </c>
+      <c r="B63" t="s">
+        <v>90</v>
+      </c>
+      <c r="G63" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K63" t="s">
+        <v>61</v>
+      </c>
+      <c r="T63" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y63" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z63" t="str">
+        <f t="shared" si="0"/>
+        <v>A6SO-D9</v>
+      </c>
+      <c r="AC63" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="64" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>3</v>
+      </c>
+      <c r="B64" t="s">
+        <v>90</v>
+      </c>
+      <c r="G64" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K64" t="s">
+        <v>61</v>
+      </c>
+      <c r="T64" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y64" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z64" t="str">
+        <f t="shared" si="0"/>
+        <v>A6SO-H8</v>
+      </c>
+      <c r="AC64" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="65" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>4</v>
+      </c>
+      <c r="B65" t="s">
+        <v>90</v>
+      </c>
+      <c r="G65" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K65" t="s">
+        <v>61</v>
+      </c>
+      <c r="T65" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y65" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z65" t="str">
+        <f t="shared" si="0"/>
+        <v>A6SO-H12</v>
+      </c>
+      <c r="AC65" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="66" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>5</v>
+      </c>
+      <c r="B66" t="s">
+        <v>90</v>
+      </c>
+      <c r="G66" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K66" t="s">
+        <v>61</v>
+      </c>
+      <c r="T66" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y66" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z66" t="str">
+        <f t="shared" si="0"/>
+        <v>A6SO-B10</v>
+      </c>
+      <c r="AC66" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="67" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>6</v>
+      </c>
+      <c r="B67" t="s">
+        <v>90</v>
+      </c>
+      <c r="G67" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K67" t="s">
+        <v>61</v>
+      </c>
+      <c r="T67" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y67" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z67" t="str">
+        <f t="shared" si="0"/>
+        <v>A6SO-D3</v>
+      </c>
+      <c r="AC67" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="68" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>7</v>
+      </c>
+      <c r="B68" t="s">
+        <v>90</v>
+      </c>
+      <c r="G68" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K68" t="s">
+        <v>61</v>
+      </c>
+      <c r="T68" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y68" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z68" t="str">
+        <f t="shared" si="0"/>
+        <v>A6SO-E6</v>
+      </c>
+      <c r="AC68" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="69" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>8</v>
+      </c>
+      <c r="B69" t="s">
+        <v>90</v>
+      </c>
+      <c r="G69" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K69" t="s">
+        <v>61</v>
+      </c>
+      <c r="T69" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y69" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z69" t="str">
+        <f t="shared" si="0"/>
+        <v>A6SO-F1</v>
+      </c>
+      <c r="AC69" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="70" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>9</v>
+      </c>
+      <c r="B70" t="s">
+        <v>90</v>
+      </c>
+      <c r="G70" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K70" t="s">
+        <v>61</v>
+      </c>
+      <c r="T70" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y70" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z70" t="str">
+        <f t="shared" si="0"/>
+        <v>A6SO-F11</v>
+      </c>
+      <c r="AC70" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="71" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>10</v>
+      </c>
+      <c r="B71" t="s">
+        <v>90</v>
+      </c>
+      <c r="G71" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K71" t="s">
+        <v>61</v>
+      </c>
+      <c r="T71" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y71" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z71" t="str">
+        <f t="shared" si="0"/>
+        <v>A6SO-G9</v>
+      </c>
+      <c r="AC71" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="72" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>11</v>
+      </c>
+      <c r="B72" t="s">
+        <v>90</v>
+      </c>
+      <c r="G72" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K72" t="s">
+        <v>61</v>
+      </c>
+      <c r="T72" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y72" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z72" t="str">
+        <f t="shared" si="0"/>
+        <v>A6SO-D6</v>
+      </c>
+      <c r="AC72" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="73" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>12</v>
+      </c>
+      <c r="B73" t="s">
+        <v>90</v>
+      </c>
+      <c r="G73" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K73" t="s">
+        <v>61</v>
+      </c>
+      <c r="T73" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y73" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z73" t="str">
+        <f t="shared" si="0"/>
+        <v>A6SO-C4</v>
+      </c>
+      <c r="AC73" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="74" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>13</v>
+      </c>
+      <c r="B74" t="s">
+        <v>90</v>
+      </c>
+      <c r="G74" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K74" t="s">
+        <v>61</v>
+      </c>
+      <c r="T74" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y74" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z74" t="str">
+        <f t="shared" si="0"/>
+        <v>A6SO-D12</v>
+      </c>
+      <c r="AC74" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="75" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>14</v>
+      </c>
+      <c r="B75" t="s">
+        <v>90</v>
+      </c>
+      <c r="G75" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K75" t="s">
+        <v>61</v>
+      </c>
+      <c r="T75" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y75" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z75" t="str">
+        <f t="shared" si="0"/>
+        <v>A6SO-B5</v>
+      </c>
+      <c r="AC75" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="76" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>15</v>
+      </c>
+      <c r="B76" t="s">
+        <v>90</v>
+      </c>
+      <c r="G76" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K76" t="s">
+        <v>61</v>
+      </c>
+      <c r="T76" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y76" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z76" t="str">
+        <f t="shared" si="0"/>
+        <v>A6SO-A7</v>
+      </c>
+      <c r="AC76" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="77" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>16</v>
+      </c>
+      <c r="B77" t="s">
+        <v>90</v>
+      </c>
+      <c r="G77" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K77" t="s">
+        <v>61</v>
+      </c>
+      <c r="T77" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y77" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z77" t="str">
+        <f t="shared" si="0"/>
+        <v>A6SO-H3</v>
+      </c>
+      <c r="AC77" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="78" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>17</v>
+      </c>
+      <c r="B78" t="s">
+        <v>90</v>
+      </c>
+      <c r="G78" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K78" t="s">
+        <v>61</v>
+      </c>
+      <c r="T78" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y78" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z78" t="str">
+        <f t="shared" si="0"/>
+        <v>A6SO-A8</v>
+      </c>
+      <c r="AC78" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="79" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>18</v>
+      </c>
+      <c r="B79" t="s">
+        <v>90</v>
+      </c>
+      <c r="G79" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K79" t="s">
+        <v>61</v>
+      </c>
+      <c r="T79" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y79" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z79" t="str">
+        <f t="shared" si="0"/>
+        <v>A6SO-E9</v>
+      </c>
+      <c r="AC79" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="80" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>19</v>
+      </c>
+      <c r="B80" t="s">
+        <v>90</v>
+      </c>
+      <c r="G80" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K80" t="s">
+        <v>61</v>
+      </c>
+      <c r="T80" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y80" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z80" t="str">
+        <f t="shared" si="0"/>
+        <v>A6SO-C6</v>
+      </c>
+      <c r="AC80" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="81" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>20</v>
+      </c>
+      <c r="B81" t="s">
+        <v>90</v>
+      </c>
+      <c r="G81" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K81" t="s">
+        <v>61</v>
+      </c>
+      <c r="T81" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y81" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z81" t="str">
+        <f t="shared" si="0"/>
+        <v>A6SO-B1</v>
+      </c>
+      <c r="AC81" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="82" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>21</v>
+      </c>
+      <c r="B82" t="s">
+        <v>90</v>
+      </c>
+      <c r="G82" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K82" t="s">
+        <v>61</v>
+      </c>
+      <c r="T82" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y82" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z82" t="str">
+        <f t="shared" si="0"/>
+        <v>A6SO-D8</v>
+      </c>
+      <c r="AC82" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="83" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>22</v>
+      </c>
+      <c r="B83" t="s">
+        <v>90</v>
+      </c>
+      <c r="G83" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K83" t="s">
+        <v>61</v>
+      </c>
+      <c r="T83" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y83" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z83" t="str">
+        <f t="shared" si="0"/>
+        <v>A6SO-F7</v>
+      </c>
+      <c r="AC83" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="84" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>23</v>
+      </c>
+      <c r="B84" t="s">
+        <v>90</v>
+      </c>
+      <c r="G84" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K84" t="s">
+        <v>61</v>
+      </c>
+      <c r="T84" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y84" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z84" t="str">
+        <f t="shared" si="0"/>
+        <v>A6SO-D2</v>
+      </c>
+      <c r="AC84" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="85" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>24</v>
+      </c>
+      <c r="B85" t="s">
+        <v>90</v>
+      </c>
+      <c r="G85" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K85" t="s">
+        <v>61</v>
+      </c>
+      <c r="T85" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y85" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z85" t="str">
+        <f t="shared" si="0"/>
+        <v>A6SO-B8</v>
+      </c>
+      <c r="AC85" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="86" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>25</v>
+      </c>
+      <c r="B86" t="s">
+        <v>90</v>
+      </c>
+      <c r="G86" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K86" t="s">
+        <v>61</v>
+      </c>
+      <c r="T86" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y86" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z86" t="str">
+        <f t="shared" si="0"/>
+        <v>A6SO-H10</v>
+      </c>
+      <c r="AC86" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="87" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>26</v>
+      </c>
+      <c r="B87" t="s">
+        <v>90</v>
+      </c>
+      <c r="G87" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K87" t="s">
+        <v>61</v>
+      </c>
+      <c r="T87" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y87" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z87" t="str">
+        <f t="shared" si="0"/>
+        <v>A6SO-E12</v>
+      </c>
+      <c r="AC87" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="88" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>27</v>
+      </c>
+      <c r="B88" t="s">
+        <v>90</v>
+      </c>
+      <c r="G88" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K88" t="s">
+        <v>61</v>
+      </c>
+      <c r="T88" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y88" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z88" t="str">
+        <f t="shared" si="0"/>
+        <v>A6SO-C9</v>
+      </c>
+      <c r="AC88" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="89" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>28</v>
+      </c>
+      <c r="B89" t="s">
+        <v>90</v>
+      </c>
+      <c r="G89" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K89" t="s">
+        <v>61</v>
+      </c>
+      <c r="T89" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y89" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z89" t="str">
+        <f t="shared" si="0"/>
+        <v>A6SO-B7</v>
+      </c>
+      <c r="AC89" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="90" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>29</v>
+      </c>
+      <c r="B90" t="s">
+        <v>90</v>
+      </c>
+      <c r="G90" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K90" t="s">
+        <v>61</v>
+      </c>
+      <c r="T90" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y90" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z90" t="str">
+        <f t="shared" si="0"/>
+        <v>A6SO-E2</v>
+      </c>
+      <c r="AC90" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="91" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>30</v>
+      </c>
+      <c r="B91" t="s">
+        <v>90</v>
+      </c>
+      <c r="G91" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K91" t="s">
+        <v>61</v>
+      </c>
+      <c r="T91" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y91" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z91" t="str">
+        <f t="shared" si="0"/>
+        <v>A6SO-E3</v>
+      </c>
+      <c r="AC91" t="s">
+        <v>180</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
adding maggot sampling information
</commit_message>
<xml_diff>
--- a/Data/2018-08-14_master_datac_2018_collection_year.xlsx
+++ b/Data/2018-08-14_master_datac_2018_collection_year.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andrew.nguyen\Desktop\Circadian_rhythm_runs_seasonal_timing\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAA62708-4984-404C-B283-B1FF762D48E8}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9706075-21F3-4D47-8A63-61AB58FF8FDF}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1800" yWindow="1935" windowWidth="35820" windowHeight="18720" activeTab="1" xr2:uid="{C7477166-8A7C-B04A-9643-C277FEDCDAAB}"/>
+    <workbookView xWindow="1800" yWindow="1935" windowWidth="35820" windowHeight="18720" xr2:uid="{C7477166-8A7C-B04A-9643-C277FEDCDAAB}"/>
   </bookViews>
   <sheets>
     <sheet name="Maggot_Collections" sheetId="2" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="839" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1200" uniqueCount="208">
   <si>
     <t>Ind_ID</t>
   </si>
@@ -574,6 +574,87 @@
   </si>
   <si>
     <t>E3</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>257</t>
+  </si>
+  <si>
+    <t>2018-08-29</t>
+  </si>
+  <si>
+    <t>TG</t>
+  </si>
+  <si>
+    <t>44</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>2018-09-22</t>
+  </si>
+  <si>
+    <t>Lansing</t>
+  </si>
+  <si>
+    <t>MSU F+W</t>
+  </si>
+  <si>
+    <t>MSU clinical</t>
+  </si>
+  <si>
+    <t>2018-09-21</t>
+  </si>
+  <si>
+    <t>147</t>
+  </si>
+  <si>
+    <t>TG + Hinal</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>MSU</t>
+  </si>
+  <si>
+    <t>Crab</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>Leonard Ferris road</t>
+  </si>
+  <si>
+    <t>5</t>
   </si>
 </sst>
 </file>
@@ -625,7 +706,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -652,7 +733,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
@@ -969,14 +1049,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D3F78F5-4EA8-6A42-B216-41A8EC7A5E8D}">
-  <dimension ref="A1:Z100"/>
+  <dimension ref="A1:Z102"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD7"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="4" max="4" width="11" style="1"/>
     <col min="6" max="6" width="14.125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1037,8 +1118,8 @@
       <c r="C2" t="s">
         <v>61</v>
       </c>
-      <c r="D2" s="9">
-        <v>43328</v>
+      <c r="D2" s="1" t="s">
+        <v>88</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -1077,8 +1158,8 @@
       <c r="C3" t="s">
         <v>61</v>
       </c>
-      <c r="D3" s="9">
-        <v>43328</v>
+      <c r="D3" s="1" t="s">
+        <v>88</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -1117,8 +1198,8 @@
       <c r="C4" t="s">
         <v>61</v>
       </c>
-      <c r="D4" s="9">
-        <v>43328</v>
+      <c r="D4" s="1" t="s">
+        <v>88</v>
       </c>
       <c r="E4">
         <v>5</v>
@@ -1128,6 +1209,9 @@
       </c>
       <c r="G4">
         <v>1</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>189</v>
       </c>
       <c r="I4">
         <v>241</v>
@@ -1154,8 +1238,8 @@
       <c r="C5" t="s">
         <v>61</v>
       </c>
-      <c r="D5" s="9">
-        <v>43328</v>
+      <c r="D5" s="1" t="s">
+        <v>88</v>
       </c>
       <c r="E5">
         <v>5</v>
@@ -1165,6 +1249,9 @@
       </c>
       <c r="G5">
         <v>1</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>189</v>
       </c>
       <c r="I5">
         <v>60</v>
@@ -1191,8 +1278,8 @@
       <c r="C6" t="s">
         <v>61</v>
       </c>
-      <c r="D6" s="9">
-        <v>43328</v>
+      <c r="D6" s="1" t="s">
+        <v>88</v>
       </c>
       <c r="E6">
         <v>6</v>
@@ -1202,6 +1289,9 @@
       </c>
       <c r="G6">
         <v>1</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>189</v>
       </c>
       <c r="I6">
         <v>232</v>
@@ -1240,8 +1330,8 @@
       <c r="C7" t="s">
         <v>61</v>
       </c>
-      <c r="D7" s="9">
-        <v>43328</v>
+      <c r="D7" s="1" t="s">
+        <v>88</v>
       </c>
       <c r="E7">
         <v>6</v>
@@ -1251,6 +1341,9 @@
       </c>
       <c r="G7">
         <v>1</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>189</v>
       </c>
       <c r="I7">
         <v>123</v>
@@ -1289,8 +1382,8 @@
       <c r="C8" t="s">
         <v>61</v>
       </c>
-      <c r="D8" s="9">
-        <v>43328</v>
+      <c r="D8" s="1" t="s">
+        <v>88</v>
       </c>
       <c r="E8">
         <v>7</v>
@@ -1300,6 +1393,9 @@
       </c>
       <c r="G8">
         <v>1</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>189</v>
       </c>
       <c r="I8">
         <v>298</v>
@@ -1338,8 +1434,8 @@
       <c r="C9" t="s">
         <v>61</v>
       </c>
-      <c r="D9" s="9">
-        <v>43328</v>
+      <c r="D9" s="1" t="s">
+        <v>88</v>
       </c>
       <c r="E9">
         <v>7</v>
@@ -1349,6 +1445,9 @@
       </c>
       <c r="G9">
         <v>1</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>189</v>
       </c>
       <c r="I9">
         <v>153</v>
@@ -1387,44 +1486,47 @@
       <c r="C10" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="D10" s="12">
-        <v>43328</v>
+      <c r="D10" s="1" t="s">
+        <v>88</v>
       </c>
       <c r="E10" s="11">
         <v>8</v>
       </c>
-      <c r="F10" s="13">
+      <c r="F10" s="12">
         <v>43335</v>
       </c>
       <c r="G10" s="11">
         <v>1</v>
       </c>
+      <c r="H10" s="1" t="s">
+        <v>189</v>
+      </c>
       <c r="I10" s="11">
         <v>316</v>
       </c>
-      <c r="J10" s="14" t="s">
+      <c r="J10" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="K10" s="14" t="s">
+      <c r="K10" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="L10" s="14" t="s">
+      <c r="L10" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="M10" s="14" t="s">
+      <c r="M10" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="N10" s="14" t="s">
+      <c r="N10" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="O10" s="14" t="s">
+      <c r="O10" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="P10" s="14"/>
-      <c r="Q10" s="14"/>
-      <c r="R10" s="14"/>
-      <c r="S10" s="14"/>
-      <c r="T10" s="14"/>
+      <c r="P10" s="13"/>
+      <c r="Q10" s="13"/>
+      <c r="R10" s="13"/>
+      <c r="S10" s="13"/>
+      <c r="T10" s="13"/>
     </row>
     <row r="11" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
@@ -1436,44 +1538,47 @@
       <c r="C11" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="D11" s="12">
-        <v>43328</v>
+      <c r="D11" s="1" t="s">
+        <v>88</v>
       </c>
       <c r="E11" s="11">
         <v>8</v>
       </c>
-      <c r="F11" s="13">
+      <c r="F11" s="12">
         <v>43335</v>
       </c>
       <c r="G11" s="11">
         <v>1</v>
       </c>
+      <c r="H11" s="1" t="s">
+        <v>189</v>
+      </c>
       <c r="I11" s="11">
         <v>152</v>
       </c>
-      <c r="J11" s="14" t="s">
+      <c r="J11" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="K11" s="14" t="s">
+      <c r="K11" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="L11" s="14" t="s">
+      <c r="L11" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="M11" s="14" t="s">
+      <c r="M11" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="N11" s="14" t="s">
+      <c r="N11" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="O11" s="14" t="s">
+      <c r="O11" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="P11" s="14"/>
-      <c r="Q11" s="14"/>
-      <c r="R11" s="14"/>
-      <c r="S11" s="14"/>
-      <c r="T11" s="14"/>
+      <c r="P11" s="13"/>
+      <c r="Q11" s="13"/>
+      <c r="R11" s="13"/>
+      <c r="S11" s="13"/>
+      <c r="T11" s="13"/>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -1485,8 +1590,8 @@
       <c r="C12" t="s">
         <v>61</v>
       </c>
-      <c r="D12" s="9">
-        <v>43328</v>
+      <c r="D12" s="1" t="s">
+        <v>88</v>
       </c>
       <c r="E12">
         <v>9</v>
@@ -1496,6 +1601,9 @@
       </c>
       <c r="G12">
         <v>1</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>189</v>
       </c>
       <c r="I12">
         <v>302</v>
@@ -1534,8 +1642,8 @@
       <c r="C13" t="s">
         <v>61</v>
       </c>
-      <c r="D13" s="9">
-        <v>43328</v>
+      <c r="D13" s="1" t="s">
+        <v>88</v>
       </c>
       <c r="E13">
         <v>9</v>
@@ -1545,6 +1653,9 @@
       </c>
       <c r="G13">
         <v>1</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>189</v>
       </c>
       <c r="I13">
         <v>142</v>
@@ -1583,44 +1694,47 @@
       <c r="C14" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="D14" s="12">
-        <v>43328</v>
+      <c r="D14" s="1" t="s">
+        <v>88</v>
       </c>
       <c r="E14" s="11">
         <v>10</v>
       </c>
-      <c r="F14" s="13">
+      <c r="F14" s="12">
         <v>43337</v>
       </c>
       <c r="G14" s="11">
         <v>1</v>
       </c>
+      <c r="H14" s="1" t="s">
+        <v>189</v>
+      </c>
       <c r="I14" s="11">
         <v>357</v>
       </c>
-      <c r="J14" s="14" t="s">
+      <c r="J14" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="K14" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="L14" s="14" t="s">
+      <c r="K14" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="L14" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="M14" s="14" t="s">
+      <c r="M14" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="N14" s="14" t="s">
+      <c r="N14" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="O14" s="14" t="s">
+      <c r="O14" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="P14" s="14"/>
-      <c r="Q14" s="14"/>
-      <c r="R14" s="14"/>
-      <c r="S14" s="14"/>
-      <c r="T14" s="14"/>
+      <c r="P14" s="13"/>
+      <c r="Q14" s="13"/>
+      <c r="R14" s="13"/>
+      <c r="S14" s="13"/>
+      <c r="T14" s="13"/>
     </row>
     <row r="15" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
@@ -1632,44 +1746,47 @@
       <c r="C15" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="D15" s="12">
-        <v>43328</v>
+      <c r="D15" s="1" t="s">
+        <v>88</v>
       </c>
       <c r="E15" s="11">
         <v>10</v>
       </c>
-      <c r="F15" s="13">
+      <c r="F15" s="12">
         <v>43337</v>
       </c>
       <c r="G15" s="11">
         <v>2</v>
       </c>
+      <c r="H15" s="1" t="s">
+        <v>189</v>
+      </c>
       <c r="I15" s="11">
         <v>42</v>
       </c>
-      <c r="J15" s="14" t="s">
+      <c r="J15" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="K15" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="L15" s="14" t="s">
+      <c r="K15" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="L15" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="M15" s="14" t="s">
+      <c r="M15" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="N15" s="14" t="s">
+      <c r="N15" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="O15" s="14" t="s">
+      <c r="O15" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="P15" s="14"/>
-      <c r="Q15" s="14"/>
-      <c r="R15" s="14"/>
-      <c r="S15" s="14"/>
-      <c r="T15" s="14"/>
+      <c r="P15" s="13"/>
+      <c r="Q15" s="13"/>
+      <c r="R15" s="13"/>
+      <c r="S15" s="13"/>
+      <c r="T15" s="13"/>
     </row>
     <row r="16" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
@@ -1681,44 +1798,47 @@
       <c r="C16" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="D16" s="12">
-        <v>43328</v>
+      <c r="D16" s="1" t="s">
+        <v>88</v>
       </c>
       <c r="E16" s="11">
         <v>10</v>
       </c>
-      <c r="F16" s="13">
+      <c r="F16" s="12">
         <v>43337</v>
       </c>
       <c r="G16" s="11">
         <v>1</v>
       </c>
+      <c r="H16" s="1" t="s">
+        <v>189</v>
+      </c>
       <c r="I16" s="11">
         <v>177</v>
       </c>
-      <c r="J16" s="14" t="s">
+      <c r="J16" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="K16" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="L16" s="14" t="s">
+      <c r="K16" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="L16" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="M16" s="14" t="s">
+      <c r="M16" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="N16" s="14" t="s">
+      <c r="N16" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="O16" s="14" t="s">
+      <c r="O16" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="P16" s="14"/>
-      <c r="Q16" s="14"/>
-      <c r="R16" s="14"/>
-      <c r="S16" s="14"/>
-      <c r="T16" s="14"/>
+      <c r="P16" s="13"/>
+      <c r="Q16" s="13"/>
+      <c r="R16" s="13"/>
+      <c r="S16" s="13"/>
+      <c r="T16" s="13"/>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
@@ -1730,8 +1850,8 @@
       <c r="C17" t="s">
         <v>61</v>
       </c>
-      <c r="D17" s="9">
-        <v>43328</v>
+      <c r="D17" s="1" t="s">
+        <v>88</v>
       </c>
       <c r="E17">
         <v>11</v>
@@ -1741,6 +1861,9 @@
       </c>
       <c r="G17">
         <v>1</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>189</v>
       </c>
       <c r="I17">
         <v>313</v>
@@ -1779,8 +1902,8 @@
       <c r="C18" t="s">
         <v>61</v>
       </c>
-      <c r="D18" s="9">
-        <v>43328</v>
+      <c r="D18" s="1" t="s">
+        <v>88</v>
       </c>
       <c r="E18">
         <v>11</v>
@@ -1790,6 +1913,9 @@
       </c>
       <c r="G18">
         <v>2</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>189</v>
       </c>
       <c r="I18">
         <v>129</v>
@@ -1828,8 +1954,8 @@
       <c r="C19" t="s">
         <v>61</v>
       </c>
-      <c r="D19" s="9">
-        <v>43328</v>
+      <c r="D19" s="1" t="s">
+        <v>88</v>
       </c>
       <c r="E19">
         <v>11</v>
@@ -1839,6 +1965,9 @@
       </c>
       <c r="G19">
         <v>1</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>189</v>
       </c>
       <c r="I19">
         <v>165</v>
@@ -1877,44 +2006,47 @@
       <c r="C20" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="D20" s="12">
-        <v>43328</v>
+      <c r="D20" s="1" t="s">
+        <v>88</v>
       </c>
       <c r="E20" s="11">
         <v>12</v>
       </c>
-      <c r="F20" s="13">
+      <c r="F20" s="12">
         <v>43339</v>
       </c>
       <c r="G20" s="11">
         <v>1</v>
       </c>
+      <c r="H20" s="1" t="s">
+        <v>189</v>
+      </c>
       <c r="I20" s="11">
         <v>220</v>
       </c>
-      <c r="J20" s="14" t="s">
+      <c r="J20" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="K20" s="14" t="s">
+      <c r="K20" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="L20" s="14" t="s">
+      <c r="L20" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="M20" s="14" t="s">
+      <c r="M20" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="N20" s="14" t="s">
+      <c r="N20" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="O20" s="14" t="s">
+      <c r="O20" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="P20" s="14"/>
-      <c r="Q20" s="14"/>
-      <c r="R20" s="14"/>
-      <c r="S20" s="14"/>
-      <c r="T20" s="14"/>
+      <c r="P20" s="13"/>
+      <c r="Q20" s="13"/>
+      <c r="R20" s="13"/>
+      <c r="S20" s="13"/>
+      <c r="T20" s="13"/>
     </row>
     <row r="21" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
@@ -1926,44 +2058,47 @@
       <c r="C21" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="D21" s="12">
-        <v>43328</v>
+      <c r="D21" s="1" t="s">
+        <v>88</v>
       </c>
       <c r="E21" s="11">
         <v>12</v>
       </c>
-      <c r="F21" s="13">
+      <c r="F21" s="12">
         <v>43339</v>
       </c>
       <c r="G21" s="11">
         <v>2</v>
       </c>
+      <c r="H21" s="1" t="s">
+        <v>189</v>
+      </c>
       <c r="I21" s="11">
         <v>180</v>
       </c>
-      <c r="J21" s="14" t="s">
+      <c r="J21" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="K21" s="14" t="s">
+      <c r="K21" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="L21" s="14" t="s">
+      <c r="L21" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="M21" s="14" t="s">
+      <c r="M21" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="N21" s="14" t="s">
+      <c r="N21" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="O21" s="14" t="s">
+      <c r="O21" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="P21" s="14"/>
-      <c r="Q21" s="14"/>
-      <c r="R21" s="14"/>
-      <c r="S21" s="14"/>
-      <c r="T21" s="14"/>
+      <c r="P21" s="13"/>
+      <c r="Q21" s="13"/>
+      <c r="R21" s="13"/>
+      <c r="S21" s="13"/>
+      <c r="T21" s="13"/>
     </row>
     <row r="22" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
@@ -1975,44 +2110,47 @@
       <c r="C22" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="D22" s="12">
-        <v>43328</v>
+      <c r="D22" s="1" t="s">
+        <v>88</v>
       </c>
       <c r="E22" s="11">
         <v>12</v>
       </c>
-      <c r="F22" s="13">
+      <c r="F22" s="12">
         <v>43339</v>
       </c>
       <c r="G22" s="11">
         <v>1</v>
       </c>
+      <c r="H22" s="1" t="s">
+        <v>189</v>
+      </c>
       <c r="I22" s="11">
         <v>138</v>
       </c>
-      <c r="J22" s="14" t="s">
+      <c r="J22" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="K22" s="14" t="s">
+      <c r="K22" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="L22" s="14" t="s">
+      <c r="L22" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="M22" s="14" t="s">
+      <c r="M22" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="N22" s="14" t="s">
+      <c r="N22" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="O22" s="14" t="s">
+      <c r="O22" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="P22" s="14"/>
-      <c r="Q22" s="14"/>
-      <c r="R22" s="14"/>
-      <c r="S22" s="14"/>
-      <c r="T22" s="14"/>
+      <c r="P22" s="13"/>
+      <c r="Q22" s="13"/>
+      <c r="R22" s="13"/>
+      <c r="S22" s="13"/>
+      <c r="T22" s="13"/>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
@@ -2024,8 +2162,8 @@
       <c r="C23" t="s">
         <v>61</v>
       </c>
-      <c r="D23" s="9">
-        <v>43328</v>
+      <c r="D23" s="1" t="s">
+        <v>88</v>
       </c>
       <c r="E23">
         <v>13</v>
@@ -2035,6 +2173,9 @@
       </c>
       <c r="G23">
         <v>1</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>189</v>
       </c>
       <c r="I23">
         <v>210</v>
@@ -2073,8 +2214,8 @@
       <c r="C24" t="s">
         <v>61</v>
       </c>
-      <c r="D24" s="9">
-        <v>43328</v>
+      <c r="D24" s="1" t="s">
+        <v>88</v>
       </c>
       <c r="E24">
         <v>13</v>
@@ -2084,6 +2225,9 @@
       </c>
       <c r="G24">
         <v>2</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>189</v>
       </c>
       <c r="I24">
         <v>149</v>
@@ -2122,8 +2266,8 @@
       <c r="C25" t="s">
         <v>61</v>
       </c>
-      <c r="D25" s="9">
-        <v>43328</v>
+      <c r="D25" s="1" t="s">
+        <v>88</v>
       </c>
       <c r="E25">
         <v>13</v>
@@ -2133,6 +2277,9 @@
       </c>
       <c r="G25">
         <v>1</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>189</v>
       </c>
       <c r="I25">
         <v>121</v>
@@ -2171,44 +2318,47 @@
       <c r="C26" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="D26" s="12">
-        <v>43328</v>
+      <c r="D26" s="1" t="s">
+        <v>88</v>
       </c>
       <c r="E26" s="11">
         <v>14</v>
       </c>
-      <c r="F26" s="13">
+      <c r="F26" s="12">
         <v>43341</v>
       </c>
       <c r="G26" s="11">
         <v>1</v>
       </c>
+      <c r="H26" s="1" t="s">
+        <v>189</v>
+      </c>
       <c r="I26" s="11">
         <v>264</v>
       </c>
-      <c r="J26" s="14" t="s">
+      <c r="J26" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="K26" s="14" t="s">
+      <c r="K26" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="L26" s="14" t="s">
+      <c r="L26" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="M26" s="14" t="s">
+      <c r="M26" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="N26" s="14" t="s">
+      <c r="N26" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="O26" s="14" t="s">
+      <c r="O26" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="P26" s="14"/>
-      <c r="Q26" s="14"/>
-      <c r="R26" s="14"/>
-      <c r="S26" s="14"/>
-      <c r="T26" s="14"/>
+      <c r="P26" s="13"/>
+      <c r="Q26" s="13"/>
+      <c r="R26" s="13"/>
+      <c r="S26" s="13"/>
+      <c r="T26" s="13"/>
     </row>
     <row r="27" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="11" t="s">
@@ -2220,44 +2370,47 @@
       <c r="C27" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="D27" s="12">
-        <v>43328</v>
+      <c r="D27" s="1" t="s">
+        <v>88</v>
       </c>
       <c r="E27" s="11">
         <v>14</v>
       </c>
-      <c r="F27" s="13">
+      <c r="F27" s="12">
         <v>43341</v>
       </c>
       <c r="G27" s="11">
         <v>2</v>
       </c>
+      <c r="H27" s="1" t="s">
+        <v>189</v>
+      </c>
       <c r="I27" s="11">
         <v>101</v>
       </c>
-      <c r="J27" s="14" t="s">
+      <c r="J27" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="K27" s="14" t="s">
+      <c r="K27" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="L27" s="14" t="s">
+      <c r="L27" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="M27" s="14" t="s">
+      <c r="M27" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="N27" s="14" t="s">
+      <c r="N27" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="O27" s="14" t="s">
+      <c r="O27" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="P27" s="14"/>
-      <c r="Q27" s="14"/>
-      <c r="R27" s="14"/>
-      <c r="S27" s="14"/>
-      <c r="T27" s="14"/>
+      <c r="P27" s="13"/>
+      <c r="Q27" s="13"/>
+      <c r="R27" s="13"/>
+      <c r="S27" s="13"/>
+      <c r="T27" s="13"/>
     </row>
     <row r="28" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="s">
@@ -2269,44 +2422,47 @@
       <c r="C28" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="D28" s="12">
-        <v>43328</v>
+      <c r="D28" s="1" t="s">
+        <v>88</v>
       </c>
       <c r="E28" s="11">
         <v>14</v>
       </c>
-      <c r="F28" s="13">
+      <c r="F28" s="12">
         <v>43341</v>
       </c>
       <c r="G28" s="11">
         <v>1</v>
       </c>
+      <c r="H28" s="1" t="s">
+        <v>189</v>
+      </c>
       <c r="I28" s="11">
         <v>119</v>
       </c>
-      <c r="J28" s="14" t="s">
+      <c r="J28" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="K28" s="14" t="s">
+      <c r="K28" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="L28" s="14" t="s">
+      <c r="L28" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="M28" s="14" t="s">
+      <c r="M28" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="N28" s="14" t="s">
+      <c r="N28" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="O28" s="14" t="s">
+      <c r="O28" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="P28" s="14"/>
-      <c r="Q28" s="14"/>
-      <c r="R28" s="14"/>
-      <c r="S28" s="14"/>
-      <c r="T28" s="14"/>
+      <c r="P28" s="13"/>
+      <c r="Q28" s="13"/>
+      <c r="R28" s="13"/>
+      <c r="S28" s="13"/>
+      <c r="T28" s="13"/>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
@@ -2318,8 +2474,8 @@
       <c r="C29" t="s">
         <v>61</v>
       </c>
-      <c r="D29" s="9">
-        <v>43328</v>
+      <c r="D29" s="1" t="s">
+        <v>88</v>
       </c>
       <c r="E29">
         <v>15</v>
@@ -2329,6 +2485,9 @@
       </c>
       <c r="G29">
         <v>1</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>189</v>
       </c>
       <c r="I29">
         <v>208</v>
@@ -2367,8 +2526,8 @@
       <c r="C30" t="s">
         <v>61</v>
       </c>
-      <c r="D30" s="9">
-        <v>43328</v>
+      <c r="D30" s="1" t="s">
+        <v>88</v>
       </c>
       <c r="E30">
         <v>15</v>
@@ -2378,6 +2537,9 @@
       </c>
       <c r="G30">
         <v>2</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>189</v>
       </c>
       <c r="I30">
         <v>152</v>
@@ -2416,8 +2578,8 @@
       <c r="C31" t="s">
         <v>61</v>
       </c>
-      <c r="D31" s="9">
-        <v>43328</v>
+      <c r="D31" s="1" t="s">
+        <v>88</v>
       </c>
       <c r="E31">
         <v>15</v>
@@ -2427,6 +2589,9 @@
       </c>
       <c r="G31">
         <v>1</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>189</v>
       </c>
       <c r="I31">
         <v>105</v>
@@ -2465,44 +2630,47 @@
       <c r="C32" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="D32" s="12">
-        <v>43328</v>
+      <c r="D32" s="1" t="s">
+        <v>88</v>
       </c>
       <c r="E32" s="11">
         <v>16</v>
       </c>
-      <c r="F32" s="13">
+      <c r="F32" s="12">
         <v>43343</v>
       </c>
       <c r="G32" s="11">
         <v>1</v>
       </c>
+      <c r="H32" s="1" t="s">
+        <v>189</v>
+      </c>
       <c r="I32" s="11">
         <v>43</v>
       </c>
-      <c r="J32" s="14" t="s">
+      <c r="J32" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="K32" s="14" t="s">
+      <c r="K32" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="L32" s="14" t="s">
+      <c r="L32" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="M32" s="14" t="s">
+      <c r="M32" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="N32" s="14" t="s">
+      <c r="N32" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="O32" s="14" t="s">
+      <c r="O32" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="P32" s="14"/>
-      <c r="Q32" s="14"/>
-      <c r="R32" s="14"/>
-      <c r="S32" s="14"/>
-      <c r="T32" s="14"/>
+      <c r="P32" s="13"/>
+      <c r="Q32" s="13"/>
+      <c r="R32" s="13"/>
+      <c r="S32" s="13"/>
+      <c r="T32" s="13"/>
     </row>
     <row r="33" spans="1:26" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="11" t="s">
@@ -2514,63 +2682,94 @@
       <c r="C33" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="D33" s="12">
-        <v>43328</v>
+      <c r="D33" s="1" t="s">
+        <v>88</v>
       </c>
       <c r="E33" s="11">
         <v>16</v>
       </c>
-      <c r="F33" s="13">
+      <c r="F33" s="12">
         <v>43343</v>
       </c>
       <c r="G33" s="11">
         <v>1</v>
       </c>
+      <c r="H33" s="1" t="s">
+        <v>189</v>
+      </c>
       <c r="I33" s="11">
         <v>34</v>
       </c>
-      <c r="J33" s="14" t="s">
+      <c r="J33" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="K33" s="14" t="s">
+      <c r="K33" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="L33" s="14" t="s">
+      <c r="L33" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="M33" s="14" t="s">
+      <c r="M33" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="N33" s="14" t="s">
+      <c r="N33" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="O33" s="14" t="s">
+      <c r="O33" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="P33" s="14"/>
-      <c r="Q33" s="14"/>
-      <c r="R33" s="14"/>
-      <c r="S33" s="14"/>
-      <c r="T33" s="14"/>
+      <c r="P33" s="13"/>
+      <c r="Q33" s="13"/>
+      <c r="R33" s="13"/>
+      <c r="S33" s="13"/>
+      <c r="T33" s="13"/>
     </row>
     <row r="34" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A34" s="1"/>
-      <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
+      <c r="A34" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C34" t="s">
+        <v>61</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>185</v>
+      </c>
       <c r="F34" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="G34" s="1"/>
-      <c r="H34" s="1"/>
-      <c r="I34" s="1"/>
-      <c r="J34" s="1"/>
-      <c r="K34" s="1"/>
-      <c r="L34" s="1"/>
-      <c r="M34" s="1"/>
-      <c r="N34" s="1"/>
-      <c r="O34" s="1"/>
+      <c r="G34" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="J34" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="K34" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="L34" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="M34" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="N34" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="O34" s="1" t="s">
+        <v>198</v>
+      </c>
       <c r="P34" s="1"/>
       <c r="Q34" s="1"/>
       <c r="R34" s="1"/>
@@ -2584,21 +2783,51 @@
       <c r="Z34" s="1"/>
     </row>
     <row r="35" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A35" s="1"/>
-      <c r="B35" s="1"/>
-      <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
-      <c r="E35" s="1"/>
-      <c r="F35" s="1"/>
-      <c r="G35" s="1"/>
-      <c r="H35" s="1"/>
-      <c r="I35" s="1"/>
-      <c r="J35" s="1"/>
-      <c r="K35" s="1"/>
-      <c r="L35" s="1"/>
-      <c r="M35" s="1"/>
-      <c r="N35" s="1"/>
-      <c r="O35" s="1"/>
+      <c r="A35" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C35" t="s">
+        <v>61</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="J35" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="K35" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="L35" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="M35" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="N35" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="O35" s="1" t="s">
+        <v>198</v>
+      </c>
       <c r="P35" s="1"/>
       <c r="Q35" s="1"/>
       <c r="R35" s="1"/>
@@ -2612,21 +2841,51 @@
       <c r="Z35" s="1"/>
     </row>
     <row r="36" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A36" s="1"/>
-      <c r="B36" s="1"/>
-      <c r="C36" s="1"/>
-      <c r="D36" s="1"/>
-      <c r="E36" s="1"/>
-      <c r="F36" s="1"/>
-      <c r="G36" s="1"/>
-      <c r="H36" s="1"/>
-      <c r="I36" s="1"/>
-      <c r="J36" s="1"/>
-      <c r="K36" s="1"/>
-      <c r="L36" s="1"/>
-      <c r="M36" s="1"/>
-      <c r="N36" s="1"/>
-      <c r="O36" s="1"/>
+      <c r="A36" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C36" t="s">
+        <v>61</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="J36" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="K36" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="L36" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="M36" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="N36" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="O36" s="1" t="s">
+        <v>198</v>
+      </c>
       <c r="P36" s="1"/>
       <c r="Q36" s="1"/>
       <c r="R36" s="1"/>
@@ -2640,21 +2899,51 @@
       <c r="Z36" s="1"/>
     </row>
     <row r="37" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A37" s="1"/>
-      <c r="B37" s="1"/>
-      <c r="C37" s="1"/>
-      <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
-      <c r="F37" s="1"/>
-      <c r="G37" s="1"/>
-      <c r="H37" s="1"/>
-      <c r="I37" s="1"/>
-      <c r="J37" s="1"/>
-      <c r="K37" s="1"/>
-      <c r="L37" s="1"/>
-      <c r="M37" s="1"/>
-      <c r="N37" s="1"/>
-      <c r="O37" s="1"/>
+      <c r="A37" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C37" t="s">
+        <v>61</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="J37" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="K37" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="L37" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="M37" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="N37" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="O37" s="1" t="s">
+        <v>198</v>
+      </c>
       <c r="P37" s="1"/>
       <c r="Q37" s="1"/>
       <c r="R37" s="1"/>
@@ -2668,21 +2957,51 @@
       <c r="Z37" s="1"/>
     </row>
     <row r="38" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A38" s="1"/>
-      <c r="B38" s="1"/>
-      <c r="C38" s="1"/>
-      <c r="D38" s="1"/>
-      <c r="E38" s="1"/>
-      <c r="F38" s="1"/>
-      <c r="G38" s="1"/>
-      <c r="H38" s="1"/>
-      <c r="I38" s="1"/>
-      <c r="J38" s="1"/>
-      <c r="K38" s="1"/>
-      <c r="L38" s="1"/>
-      <c r="M38" s="1"/>
-      <c r="N38" s="1"/>
-      <c r="O38" s="1"/>
+      <c r="A38" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C38" t="s">
+        <v>61</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="J38" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="K38" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="L38" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="M38" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="N38" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="O38" s="1" t="s">
+        <v>198</v>
+      </c>
       <c r="P38" s="1"/>
       <c r="Q38" s="1"/>
       <c r="R38" s="1"/>
@@ -2696,21 +3015,51 @@
       <c r="Z38" s="1"/>
     </row>
     <row r="39" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A39" s="1"/>
-      <c r="B39" s="1"/>
-      <c r="C39" s="1"/>
-      <c r="D39" s="1"/>
-      <c r="E39" s="1"/>
-      <c r="F39" s="1"/>
-      <c r="G39" s="1"/>
-      <c r="H39" s="1"/>
-      <c r="I39" s="1"/>
-      <c r="J39" s="1"/>
-      <c r="K39" s="1"/>
-      <c r="L39" s="1"/>
-      <c r="M39" s="1"/>
-      <c r="N39" s="1"/>
-      <c r="O39" s="1"/>
+      <c r="A39" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C39" t="s">
+        <v>61</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="J39" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="K39" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="L39" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="M39" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="N39" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="O39" s="1" t="s">
+        <v>198</v>
+      </c>
       <c r="P39" s="1"/>
       <c r="Q39" s="1"/>
       <c r="R39" s="1"/>
@@ -2724,21 +3073,51 @@
       <c r="Z39" s="1"/>
     </row>
     <row r="40" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A40" s="1"/>
-      <c r="B40" s="1"/>
-      <c r="C40" s="1"/>
-      <c r="D40" s="1"/>
-      <c r="E40" s="1"/>
-      <c r="F40" s="1"/>
-      <c r="G40" s="1"/>
-      <c r="H40" s="1"/>
-      <c r="I40" s="1"/>
-      <c r="J40" s="1"/>
-      <c r="K40" s="1"/>
-      <c r="L40" s="1"/>
-      <c r="M40" s="1"/>
-      <c r="N40" s="1"/>
-      <c r="O40" s="1"/>
+      <c r="A40" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="J40" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="K40" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="L40" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="M40" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="N40" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="O40" s="1" t="s">
+        <v>198</v>
+      </c>
       <c r="P40" s="1"/>
       <c r="Q40" s="1"/>
       <c r="R40" s="1"/>
@@ -2752,21 +3131,51 @@
       <c r="Z40" s="1"/>
     </row>
     <row r="41" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A41" s="1"/>
-      <c r="B41" s="1"/>
-      <c r="C41" s="1"/>
-      <c r="D41" s="1"/>
-      <c r="E41" s="1"/>
-      <c r="F41" s="1"/>
-      <c r="G41" s="1"/>
-      <c r="H41" s="1"/>
-      <c r="I41" s="1"/>
-      <c r="J41" s="1"/>
-      <c r="K41" s="1"/>
-      <c r="L41" s="1"/>
-      <c r="M41" s="1"/>
-      <c r="N41" s="1"/>
-      <c r="O41" s="1"/>
+      <c r="A41" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="I41" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="J41" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="K41" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="L41" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="M41" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="N41" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="O41" s="1" t="s">
+        <v>198</v>
+      </c>
       <c r="P41" s="1"/>
       <c r="Q41" s="1"/>
       <c r="R41" s="1"/>
@@ -2780,21 +3189,51 @@
       <c r="Z41" s="1"/>
     </row>
     <row r="42" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A42" s="1"/>
-      <c r="B42" s="1"/>
-      <c r="C42" s="1"/>
-      <c r="D42" s="1"/>
-      <c r="E42" s="1"/>
-      <c r="F42" s="1"/>
-      <c r="G42" s="1"/>
-      <c r="H42" s="1"/>
-      <c r="I42" s="1"/>
-      <c r="J42" s="1"/>
-      <c r="K42" s="1"/>
-      <c r="L42" s="1"/>
-      <c r="M42" s="1"/>
-      <c r="N42" s="1"/>
-      <c r="O42" s="1"/>
+      <c r="A42" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="I42" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="J42" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="K42" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="L42" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="M42" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="N42" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="O42" s="1" t="s">
+        <v>198</v>
+      </c>
       <c r="P42" s="1"/>
       <c r="Q42" s="1"/>
       <c r="R42" s="1"/>
@@ -2808,21 +3247,51 @@
       <c r="Z42" s="1"/>
     </row>
     <row r="43" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A43" s="1"/>
-      <c r="B43" s="1"/>
-      <c r="C43" s="1"/>
-      <c r="D43" s="1"/>
-      <c r="E43" s="1"/>
-      <c r="F43" s="1"/>
-      <c r="G43" s="1"/>
-      <c r="H43" s="1"/>
-      <c r="I43" s="1"/>
-      <c r="J43" s="1"/>
-      <c r="K43" s="1"/>
-      <c r="L43" s="1"/>
-      <c r="M43" s="1"/>
-      <c r="N43" s="1"/>
-      <c r="O43" s="1"/>
+      <c r="A43" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C43" t="s">
+        <v>61</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="I43" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="J43" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="K43" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="L43" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="M43" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="N43" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="O43" s="1" t="s">
+        <v>194</v>
+      </c>
       <c r="P43" s="1"/>
       <c r="Q43" s="1"/>
       <c r="R43" s="1"/>
@@ -2836,21 +3305,51 @@
       <c r="Z43" s="1"/>
     </row>
     <row r="44" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A44" s="1"/>
-      <c r="B44" s="1"/>
-      <c r="C44" s="1"/>
-      <c r="D44" s="1"/>
-      <c r="E44" s="1"/>
-      <c r="F44" s="1"/>
-      <c r="G44" s="1"/>
-      <c r="H44" s="1"/>
-      <c r="I44" s="1"/>
-      <c r="J44" s="1"/>
-      <c r="K44" s="1"/>
-      <c r="L44" s="1"/>
-      <c r="M44" s="1"/>
-      <c r="N44" s="1"/>
-      <c r="O44" s="1"/>
+      <c r="A44" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C44" t="s">
+        <v>61</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="I44" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="J44" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="K44" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="L44" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="M44" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="N44" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="O44" s="1" t="s">
+        <v>194</v>
+      </c>
       <c r="P44" s="1"/>
       <c r="Q44" s="1"/>
       <c r="R44" s="1"/>
@@ -2864,21 +3363,51 @@
       <c r="Z44" s="1"/>
     </row>
     <row r="45" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A45" s="1"/>
-      <c r="B45" s="1"/>
-      <c r="C45" s="1"/>
-      <c r="D45" s="1"/>
-      <c r="E45" s="1"/>
-      <c r="F45" s="1"/>
-      <c r="G45" s="1"/>
-      <c r="H45" s="1"/>
-      <c r="I45" s="1"/>
-      <c r="J45" s="1"/>
-      <c r="K45" s="1"/>
-      <c r="L45" s="1"/>
-      <c r="M45" s="1"/>
-      <c r="N45" s="1"/>
-      <c r="O45" s="1"/>
+      <c r="A45" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C45" t="s">
+        <v>61</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="I45" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="J45" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="K45" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="L45" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="M45" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="N45" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="O45" s="1" t="s">
+        <v>194</v>
+      </c>
       <c r="P45" s="1"/>
       <c r="Q45" s="1"/>
       <c r="R45" s="1"/>
@@ -2892,21 +3421,51 @@
       <c r="Z45" s="1"/>
     </row>
     <row r="46" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A46" s="1"/>
-      <c r="B46" s="1"/>
-      <c r="C46" s="1"/>
-      <c r="D46" s="1"/>
-      <c r="E46" s="1"/>
-      <c r="F46" s="1"/>
-      <c r="G46" s="1"/>
-      <c r="H46" s="1"/>
-      <c r="I46" s="1"/>
-      <c r="J46" s="1"/>
-      <c r="K46" s="1"/>
-      <c r="L46" s="1"/>
-      <c r="M46" s="1"/>
-      <c r="N46" s="1"/>
-      <c r="O46" s="1"/>
+      <c r="A46" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C46" t="s">
+        <v>61</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="I46" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="J46" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="K46" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="L46" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="M46" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="N46" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="O46" s="1" t="s">
+        <v>194</v>
+      </c>
       <c r="P46" s="1"/>
       <c r="Q46" s="1"/>
       <c r="R46" s="1"/>
@@ -2920,21 +3479,51 @@
       <c r="Z46" s="1"/>
     </row>
     <row r="47" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A47" s="1"/>
-      <c r="B47" s="1"/>
-      <c r="C47" s="1"/>
-      <c r="D47" s="1"/>
-      <c r="E47" s="1"/>
-      <c r="F47" s="1"/>
-      <c r="G47" s="1"/>
-      <c r="H47" s="1"/>
-      <c r="I47" s="1"/>
-      <c r="J47" s="1"/>
-      <c r="K47" s="1"/>
-      <c r="L47" s="1"/>
-      <c r="M47" s="1"/>
-      <c r="N47" s="1"/>
-      <c r="O47" s="1"/>
+      <c r="A47" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C47" t="s">
+        <v>61</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="H47" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="I47" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="J47" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="K47" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="L47" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="M47" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="N47" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="O47" s="1" t="s">
+        <v>194</v>
+      </c>
       <c r="P47" s="1"/>
       <c r="Q47" s="1"/>
       <c r="R47" s="1"/>
@@ -2948,21 +3537,51 @@
       <c r="Z47" s="1"/>
     </row>
     <row r="48" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A48" s="1"/>
-      <c r="B48" s="1"/>
-      <c r="C48" s="1"/>
-      <c r="D48" s="1"/>
-      <c r="E48" s="1"/>
-      <c r="F48" s="1"/>
-      <c r="G48" s="1"/>
-      <c r="H48" s="1"/>
-      <c r="I48" s="1"/>
-      <c r="J48" s="1"/>
-      <c r="K48" s="1"/>
-      <c r="L48" s="1"/>
-      <c r="M48" s="1"/>
-      <c r="N48" s="1"/>
-      <c r="O48" s="1"/>
+      <c r="A48" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C48" t="s">
+        <v>61</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="H48" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="I48" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="J48" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="K48" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="L48" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="M48" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="N48" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="O48" s="1" t="s">
+        <v>194</v>
+      </c>
       <c r="P48" s="1"/>
       <c r="Q48" s="1"/>
       <c r="R48" s="1"/>
@@ -2976,21 +3595,51 @@
       <c r="Z48" s="1"/>
     </row>
     <row r="49" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A49" s="1"/>
-      <c r="B49" s="1"/>
-      <c r="C49" s="1"/>
-      <c r="D49" s="1"/>
-      <c r="E49" s="1"/>
-      <c r="F49" s="1"/>
-      <c r="G49" s="1"/>
-      <c r="H49" s="1"/>
-      <c r="I49" s="1"/>
-      <c r="J49" s="1"/>
-      <c r="K49" s="1"/>
-      <c r="L49" s="1"/>
-      <c r="M49" s="1"/>
-      <c r="N49" s="1"/>
-      <c r="O49" s="1"/>
+      <c r="A49" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="H49" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="I49" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="J49" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="K49" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="L49" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="M49" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="N49" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="O49" s="1" t="s">
+        <v>194</v>
+      </c>
       <c r="P49" s="1"/>
       <c r="Q49" s="1"/>
       <c r="R49" s="1"/>
@@ -3004,21 +3653,51 @@
       <c r="Z49" s="1"/>
     </row>
     <row r="50" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A50" s="1"/>
-      <c r="B50" s="1"/>
-      <c r="C50" s="1"/>
-      <c r="D50" s="1"/>
-      <c r="E50" s="1"/>
-      <c r="F50" s="1"/>
-      <c r="G50" s="1"/>
-      <c r="H50" s="1"/>
-      <c r="I50" s="1"/>
-      <c r="J50" s="1"/>
-      <c r="K50" s="1"/>
-      <c r="L50" s="1"/>
-      <c r="M50" s="1"/>
-      <c r="N50" s="1"/>
-      <c r="O50" s="1"/>
+      <c r="A50" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="H50" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="I50" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="J50" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="K50" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="L50" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="M50" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="N50" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="O50" s="1" t="s">
+        <v>194</v>
+      </c>
       <c r="P50" s="1"/>
       <c r="Q50" s="1"/>
       <c r="R50" s="1"/>
@@ -3032,21 +3711,51 @@
       <c r="Z50" s="1"/>
     </row>
     <row r="51" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A51" s="1"/>
-      <c r="B51" s="1"/>
-      <c r="C51" s="1"/>
-      <c r="D51" s="1"/>
-      <c r="E51" s="1"/>
-      <c r="F51" s="1"/>
-      <c r="G51" s="1"/>
-      <c r="H51" s="1"/>
-      <c r="I51" s="1"/>
-      <c r="J51" s="1"/>
-      <c r="K51" s="1"/>
-      <c r="L51" s="1"/>
-      <c r="M51" s="1"/>
-      <c r="N51" s="1"/>
-      <c r="O51" s="1"/>
+      <c r="A51" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="H51" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="I51" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="J51" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="K51" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="L51" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="M51" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="N51" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="O51" s="1" t="s">
+        <v>194</v>
+      </c>
       <c r="P51" s="1"/>
       <c r="Q51" s="1"/>
       <c r="R51" s="1"/>
@@ -3060,21 +3769,51 @@
       <c r="Z51" s="1"/>
     </row>
     <row r="52" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A52" s="1"/>
-      <c r="B52" s="1"/>
-      <c r="C52" s="1"/>
-      <c r="D52" s="1"/>
-      <c r="E52" s="1"/>
-      <c r="F52" s="1"/>
-      <c r="G52" s="1"/>
-      <c r="H52" s="1"/>
-      <c r="I52" s="1"/>
-      <c r="J52" s="1"/>
-      <c r="K52" s="1"/>
-      <c r="L52" s="1"/>
-      <c r="M52" s="1"/>
-      <c r="N52" s="1"/>
-      <c r="O52" s="1"/>
+      <c r="A52" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="H52" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="I52" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="J52" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="K52" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="L52" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="M52" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="N52" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="O52" s="1" t="s">
+        <v>194</v>
+      </c>
       <c r="P52" s="1"/>
       <c r="Q52" s="1"/>
       <c r="R52" s="1"/>
@@ -3088,21 +3827,51 @@
       <c r="Z52" s="1"/>
     </row>
     <row r="53" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A53" s="1"/>
-      <c r="B53" s="1"/>
-      <c r="C53" s="1"/>
-      <c r="D53" s="1"/>
-      <c r="E53" s="1"/>
-      <c r="F53" s="1"/>
-      <c r="G53" s="1"/>
-      <c r="H53" s="1"/>
-      <c r="I53" s="1"/>
-      <c r="J53" s="1"/>
-      <c r="K53" s="1"/>
-      <c r="L53" s="1"/>
-      <c r="M53" s="1"/>
-      <c r="N53" s="1"/>
-      <c r="O53" s="1"/>
+      <c r="A53" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="H53" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="I53" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="J53" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="K53" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="L53" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="M53" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="N53" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="O53" s="1" t="s">
+        <v>194</v>
+      </c>
       <c r="P53" s="1"/>
       <c r="Q53" s="1"/>
       <c r="R53" s="1"/>
@@ -3119,7 +3888,6 @@
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
-      <c r="D54" s="1"/>
       <c r="E54" s="1"/>
       <c r="F54" s="1"/>
       <c r="G54" s="1"/>
@@ -3147,7 +3915,6 @@
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
-      <c r="D55" s="1"/>
       <c r="E55" s="1"/>
       <c r="F55" s="1"/>
       <c r="G55" s="1"/>
@@ -3175,7 +3942,6 @@
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
-      <c r="D56" s="1"/>
       <c r="E56" s="1"/>
       <c r="F56" s="1"/>
       <c r="G56" s="1"/>
@@ -3203,7 +3969,6 @@
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
-      <c r="D57" s="1"/>
       <c r="E57" s="1"/>
       <c r="F57" s="1"/>
       <c r="G57" s="1"/>
@@ -3231,7 +3996,6 @@
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
-      <c r="D58" s="1"/>
       <c r="E58" s="1"/>
       <c r="F58" s="1"/>
       <c r="G58" s="1"/>
@@ -3259,7 +4023,6 @@
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
-      <c r="D59" s="1"/>
       <c r="E59" s="1"/>
       <c r="F59" s="1"/>
       <c r="G59" s="1"/>
@@ -3287,7 +4050,6 @@
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
-      <c r="D60" s="1"/>
       <c r="E60" s="1"/>
       <c r="F60" s="1"/>
       <c r="G60" s="1"/>
@@ -3315,7 +4077,6 @@
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
-      <c r="D61" s="1"/>
       <c r="E61" s="1"/>
       <c r="F61" s="1"/>
       <c r="G61" s="1"/>
@@ -3343,7 +4104,6 @@
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
-      <c r="D62" s="1"/>
       <c r="E62" s="1"/>
       <c r="F62" s="1"/>
       <c r="G62" s="1"/>
@@ -3371,7 +4131,6 @@
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
-      <c r="D63" s="1"/>
       <c r="E63" s="1"/>
       <c r="F63" s="1"/>
       <c r="G63" s="1"/>
@@ -3399,7 +4158,6 @@
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
-      <c r="D64" s="1"/>
       <c r="E64" s="1"/>
       <c r="F64" s="1"/>
       <c r="G64" s="1"/>
@@ -3427,7 +4185,6 @@
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
-      <c r="D65" s="1"/>
       <c r="E65" s="1"/>
       <c r="F65" s="1"/>
       <c r="G65" s="1"/>
@@ -3455,7 +4212,6 @@
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
-      <c r="D66" s="1"/>
       <c r="E66" s="1"/>
       <c r="F66" s="1"/>
       <c r="G66" s="1"/>
@@ -3483,7 +4239,6 @@
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
-      <c r="D67" s="1"/>
       <c r="E67" s="1"/>
       <c r="F67" s="1"/>
       <c r="G67" s="1"/>
@@ -3511,7 +4266,6 @@
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
-      <c r="D68" s="1"/>
       <c r="E68" s="1"/>
       <c r="F68" s="1"/>
       <c r="G68" s="1"/>
@@ -3539,7 +4293,6 @@
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
-      <c r="D69" s="1"/>
       <c r="E69" s="1"/>
       <c r="F69" s="1"/>
       <c r="G69" s="1"/>
@@ -3567,7 +4320,6 @@
       <c r="A70" s="1"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
-      <c r="D70" s="1"/>
       <c r="E70" s="1"/>
       <c r="F70" s="1"/>
       <c r="G70" s="1"/>
@@ -3595,7 +4347,6 @@
       <c r="A71" s="1"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
-      <c r="D71" s="1"/>
       <c r="E71" s="1"/>
       <c r="F71" s="1"/>
       <c r="G71" s="1"/>
@@ -3623,7 +4374,6 @@
       <c r="A72" s="1"/>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
-      <c r="D72" s="1"/>
       <c r="E72" s="1"/>
       <c r="F72" s="1"/>
       <c r="G72" s="1"/>
@@ -3651,7 +4401,6 @@
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
-      <c r="D73" s="1"/>
       <c r="E73" s="1"/>
       <c r="F73" s="1"/>
       <c r="G73" s="1"/>
@@ -3679,7 +4428,6 @@
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
-      <c r="D74" s="1"/>
       <c r="E74" s="1"/>
       <c r="F74" s="1"/>
       <c r="G74" s="1"/>
@@ -3707,7 +4455,6 @@
       <c r="A75" s="1"/>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
-      <c r="D75" s="1"/>
       <c r="E75" s="1"/>
       <c r="F75" s="1"/>
       <c r="G75" s="1"/>
@@ -3735,7 +4482,6 @@
       <c r="A76" s="1"/>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
-      <c r="D76" s="1"/>
       <c r="E76" s="1"/>
       <c r="F76" s="1"/>
       <c r="G76" s="1"/>
@@ -3763,7 +4509,6 @@
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
-      <c r="D77" s="1"/>
       <c r="E77" s="1"/>
       <c r="F77" s="1"/>
       <c r="G77" s="1"/>
@@ -3791,7 +4536,6 @@
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
-      <c r="D78" s="1"/>
       <c r="E78" s="1"/>
       <c r="F78" s="1"/>
       <c r="G78" s="1"/>
@@ -3819,7 +4563,6 @@
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
-      <c r="D79" s="1"/>
       <c r="E79" s="1"/>
       <c r="F79" s="1"/>
       <c r="G79" s="1"/>
@@ -3847,7 +4590,6 @@
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
-      <c r="D80" s="1"/>
       <c r="E80" s="1"/>
       <c r="F80" s="1"/>
       <c r="G80" s="1"/>
@@ -3875,7 +4617,6 @@
       <c r="A81" s="1"/>
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
-      <c r="D81" s="1"/>
       <c r="E81" s="1"/>
       <c r="F81" s="1"/>
       <c r="G81" s="1"/>
@@ -3903,7 +4644,6 @@
       <c r="A82" s="1"/>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
-      <c r="D82" s="1"/>
       <c r="E82" s="1"/>
       <c r="F82" s="1"/>
       <c r="G82" s="1"/>
@@ -3931,7 +4671,6 @@
       <c r="A83" s="1"/>
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
-      <c r="D83" s="1"/>
       <c r="E83" s="1"/>
       <c r="F83" s="1"/>
       <c r="G83" s="1"/>
@@ -3959,7 +4698,6 @@
       <c r="A84" s="1"/>
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
-      <c r="D84" s="1"/>
       <c r="E84" s="1"/>
       <c r="F84" s="1"/>
       <c r="G84" s="1"/>
@@ -3987,7 +4725,6 @@
       <c r="A85" s="1"/>
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
-      <c r="D85" s="1"/>
       <c r="E85" s="1"/>
       <c r="F85" s="1"/>
       <c r="G85" s="1"/>
@@ -4015,7 +4752,6 @@
       <c r="A86" s="1"/>
       <c r="B86" s="1"/>
       <c r="C86" s="1"/>
-      <c r="D86" s="1"/>
       <c r="E86" s="1"/>
       <c r="F86" s="1"/>
       <c r="G86" s="1"/>
@@ -4043,7 +4779,6 @@
       <c r="A87" s="1"/>
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
-      <c r="D87" s="1"/>
       <c r="E87" s="1"/>
       <c r="F87" s="1"/>
       <c r="G87" s="1"/>
@@ -4071,7 +4806,6 @@
       <c r="A88" s="1"/>
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
-      <c r="D88" s="1"/>
       <c r="E88" s="1"/>
       <c r="F88" s="1"/>
       <c r="G88" s="1"/>
@@ -4099,7 +4833,6 @@
       <c r="A89" s="1"/>
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
-      <c r="D89" s="1"/>
       <c r="E89" s="1"/>
       <c r="F89" s="1"/>
       <c r="G89" s="1"/>
@@ -4127,7 +4860,6 @@
       <c r="A90" s="1"/>
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
-      <c r="D90" s="1"/>
       <c r="E90" s="1"/>
       <c r="F90" s="1"/>
       <c r="G90" s="1"/>
@@ -4155,7 +4887,6 @@
       <c r="A91" s="1"/>
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
-      <c r="D91" s="1"/>
       <c r="E91" s="1"/>
       <c r="F91" s="1"/>
       <c r="G91" s="1"/>
@@ -4183,7 +4914,6 @@
       <c r="A92" s="1"/>
       <c r="B92" s="1"/>
       <c r="C92" s="1"/>
-      <c r="D92" s="1"/>
       <c r="E92" s="1"/>
       <c r="F92" s="1"/>
       <c r="G92" s="1"/>
@@ -4211,7 +4941,6 @@
       <c r="A93" s="1"/>
       <c r="B93" s="1"/>
       <c r="C93" s="1"/>
-      <c r="D93" s="1"/>
       <c r="E93" s="1"/>
       <c r="F93" s="1"/>
       <c r="G93" s="1"/>
@@ -4239,7 +4968,6 @@
       <c r="A94" s="1"/>
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
-      <c r="D94" s="1"/>
       <c r="E94" s="1"/>
       <c r="F94" s="1"/>
       <c r="G94" s="1"/>
@@ -4267,7 +4995,6 @@
       <c r="A95" s="1"/>
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
-      <c r="D95" s="1"/>
       <c r="E95" s="1"/>
       <c r="F95" s="1"/>
       <c r="G95" s="1"/>
@@ -4295,7 +5022,6 @@
       <c r="A96" s="1"/>
       <c r="B96" s="1"/>
       <c r="C96" s="1"/>
-      <c r="D96" s="1"/>
       <c r="E96" s="1"/>
       <c r="F96" s="1"/>
       <c r="G96" s="1"/>
@@ -4323,7 +5049,6 @@
       <c r="A97" s="1"/>
       <c r="B97" s="1"/>
       <c r="C97" s="1"/>
-      <c r="D97" s="1"/>
       <c r="E97" s="1"/>
       <c r="F97" s="1"/>
       <c r="G97" s="1"/>
@@ -4351,7 +5076,6 @@
       <c r="A98" s="1"/>
       <c r="B98" s="1"/>
       <c r="C98" s="1"/>
-      <c r="D98" s="1"/>
       <c r="E98" s="1"/>
       <c r="F98" s="1"/>
       <c r="G98" s="1"/>
@@ -4379,7 +5103,6 @@
       <c r="A99" s="1"/>
       <c r="B99" s="1"/>
       <c r="C99" s="1"/>
-      <c r="D99" s="1"/>
       <c r="E99" s="1"/>
       <c r="F99" s="1"/>
       <c r="G99" s="1"/>
@@ -4407,7 +5130,6 @@
       <c r="A100" s="1"/>
       <c r="B100" s="1"/>
       <c r="C100" s="1"/>
-      <c r="D100" s="1"/>
       <c r="E100" s="1"/>
       <c r="F100" s="1"/>
       <c r="G100" s="1"/>
@@ -4431,6 +5153,60 @@
       <c r="Y100" s="1"/>
       <c r="Z100" s="1"/>
     </row>
+    <row r="101" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A101" s="1"/>
+      <c r="B101" s="1"/>
+      <c r="C101" s="1"/>
+      <c r="E101" s="1"/>
+      <c r="F101" s="1"/>
+      <c r="G101" s="1"/>
+      <c r="H101" s="1"/>
+      <c r="I101" s="1"/>
+      <c r="J101" s="1"/>
+      <c r="K101" s="1"/>
+      <c r="L101" s="1"/>
+      <c r="M101" s="1"/>
+      <c r="N101" s="1"/>
+      <c r="O101" s="1"/>
+      <c r="P101" s="1"/>
+      <c r="Q101" s="1"/>
+      <c r="R101" s="1"/>
+      <c r="S101" s="1"/>
+      <c r="T101" s="1"/>
+      <c r="U101" s="1"/>
+      <c r="V101" s="1"/>
+      <c r="W101" s="1"/>
+      <c r="X101" s="1"/>
+      <c r="Y101" s="1"/>
+      <c r="Z101" s="1"/>
+    </row>
+    <row r="102" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A102" s="1"/>
+      <c r="B102" s="1"/>
+      <c r="C102" s="1"/>
+      <c r="E102" s="1"/>
+      <c r="F102" s="1"/>
+      <c r="G102" s="1"/>
+      <c r="H102" s="1"/>
+      <c r="I102" s="1"/>
+      <c r="J102" s="1"/>
+      <c r="K102" s="1"/>
+      <c r="L102" s="1"/>
+      <c r="M102" s="1"/>
+      <c r="N102" s="1"/>
+      <c r="O102" s="1"/>
+      <c r="P102" s="1"/>
+      <c r="Q102" s="1"/>
+      <c r="R102" s="1"/>
+      <c r="S102" s="1"/>
+      <c r="T102" s="1"/>
+      <c r="U102" s="1"/>
+      <c r="V102" s="1"/>
+      <c r="W102" s="1"/>
+      <c r="X102" s="1"/>
+      <c r="Y102" s="1"/>
+      <c r="Z102" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4441,7 +5217,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92725FB9-1A17-2546-9DFA-6C0D39437891}">
   <dimension ref="A1:AS91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q18" workbookViewId="0">
+    <sheetView topLeftCell="Q18" workbookViewId="0">
       <selection activeCell="AB32" sqref="AB32"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
updated collections sheets 2018
</commit_message>
<xml_diff>
--- a/Data/2018-08-14_master_datac_2018_collection_year.xlsx
+++ b/Data/2018-08-14_master_datac_2018_collection_year.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andrew.nguyen\Desktop\Circadian_rhythm_runs_seasonal_timing\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9706075-21F3-4D47-8A63-61AB58FF8FDF}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F26EAB03-E28C-40B8-A86D-25EDF99F3D1C}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1800" yWindow="1935" windowWidth="35820" windowHeight="18720" xr2:uid="{C7477166-8A7C-B04A-9643-C277FEDCDAAB}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1200" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1500" uniqueCount="222">
   <si>
     <t>Ind_ID</t>
   </si>
@@ -655,6 +655,48 @@
   </si>
   <si>
     <t>5</t>
+  </si>
+  <si>
+    <t>MSU ATC</t>
+  </si>
+  <si>
+    <t>TG + ANBE</t>
+  </si>
+  <si>
+    <t>71</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>2018-09-23</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>41</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>70</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>2018-09-24</t>
   </si>
 </sst>
 </file>
@@ -674,7 +716,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -693,6 +735,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -706,7 +754,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -735,6 +783,8 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1051,8 +1101,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D3F78F5-4EA8-6A42-B216-41A8EC7A5E8D}">
   <dimension ref="A1:Z102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="F44" sqref="F44"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="H65" sqref="H65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3246,686 +3296,748 @@
       <c r="Y42" s="1"/>
       <c r="Z42" s="1"/>
     </row>
-    <row r="43" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
+    <row r="43" spans="1:26" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="B43" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="C43" t="s">
-        <v>61</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="E43" s="1" t="s">
+      <c r="C43" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="D43" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="E43" s="14" t="s">
+        <v>217</v>
+      </c>
+      <c r="F43" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="G43" s="14" t="s">
+        <v>181</v>
+      </c>
+      <c r="H43" s="14" t="s">
+        <v>200</v>
+      </c>
+      <c r="I43" s="14" t="s">
+        <v>199</v>
+      </c>
+      <c r="J43" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="K43" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="L43" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="M43" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="N43" s="14" t="s">
+        <v>198</v>
+      </c>
+      <c r="O43" s="14" t="s">
+        <v>194</v>
+      </c>
+      <c r="P43" s="14"/>
+      <c r="Q43" s="14"/>
+      <c r="R43" s="14"/>
+      <c r="S43" s="14"/>
+      <c r="T43" s="14"/>
+      <c r="U43" s="14"/>
+      <c r="V43" s="14"/>
+      <c r="W43" s="14"/>
+      <c r="X43" s="14"/>
+      <c r="Y43" s="14"/>
+      <c r="Z43" s="14"/>
+    </row>
+    <row r="44" spans="1:26" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="B44" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="C44" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="D44" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="E44" s="14" t="s">
+        <v>217</v>
+      </c>
+      <c r="F44" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="G44" s="14" t="s">
+        <v>181</v>
+      </c>
+      <c r="H44" s="14" t="s">
+        <v>200</v>
+      </c>
+      <c r="I44" s="14" t="s">
+        <v>201</v>
+      </c>
+      <c r="J44" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="K44" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="L44" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="M44" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="N44" s="14" t="s">
+        <v>198</v>
+      </c>
+      <c r="O44" s="14" t="s">
+        <v>194</v>
+      </c>
+      <c r="P44" s="14"/>
+      <c r="Q44" s="14"/>
+      <c r="R44" s="14"/>
+      <c r="S44" s="14"/>
+      <c r="T44" s="14"/>
+      <c r="U44" s="14"/>
+      <c r="V44" s="14"/>
+      <c r="W44" s="14"/>
+      <c r="X44" s="14"/>
+      <c r="Y44" s="14"/>
+      <c r="Z44" s="14"/>
+    </row>
+    <row r="45" spans="1:26" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="B45" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="C45" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="D45" s="14" t="s">
+        <v>188</v>
+      </c>
+      <c r="E45" s="14" t="s">
         <v>182</v>
       </c>
-      <c r="F43" s="1" t="s">
+      <c r="F45" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="G43" s="1" t="s">
+      <c r="G45" s="14" t="s">
         <v>181</v>
       </c>
-      <c r="H43" s="1" t="s">
+      <c r="H45" s="14" t="s">
         <v>200</v>
       </c>
-      <c r="I43" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="J43" s="1" t="s">
+      <c r="I45" s="14" t="s">
+        <v>186</v>
+      </c>
+      <c r="J45" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="K43" s="1" t="s">
+      <c r="K45" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="L43" s="1" t="s">
+      <c r="L45" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="M43" s="1" t="s">
+      <c r="M45" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="N43" s="1" t="s">
+      <c r="N45" s="14" t="s">
         <v>198</v>
       </c>
-      <c r="O43" s="1" t="s">
+      <c r="O45" s="14" t="s">
         <v>194</v>
       </c>
-      <c r="P43" s="1"/>
-      <c r="Q43" s="1"/>
-      <c r="R43" s="1"/>
-      <c r="S43" s="1"/>
-      <c r="T43" s="1"/>
-      <c r="U43" s="1"/>
-      <c r="V43" s="1"/>
-      <c r="W43" s="1"/>
-      <c r="X43" s="1"/>
-      <c r="Y43" s="1"/>
-      <c r="Z43" s="1"/>
-    </row>
-    <row r="44" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
+      <c r="P45" s="14"/>
+      <c r="Q45" s="14"/>
+      <c r="R45" s="14"/>
+      <c r="S45" s="14"/>
+      <c r="T45" s="14"/>
+      <c r="U45" s="14"/>
+      <c r="V45" s="14"/>
+      <c r="W45" s="14"/>
+      <c r="X45" s="14"/>
+      <c r="Y45" s="14"/>
+      <c r="Z45" s="14"/>
+    </row>
+    <row r="46" spans="1:26" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="B46" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="C46" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="D46" s="14" t="s">
+        <v>188</v>
+      </c>
+      <c r="E46" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="F46" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="G46" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="H46" s="14" t="s">
+        <v>200</v>
+      </c>
+      <c r="I46" s="14" t="s">
+        <v>201</v>
+      </c>
+      <c r="J46" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="K46" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="L46" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="M46" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="N46" s="14" t="s">
+        <v>198</v>
+      </c>
+      <c r="O46" s="14" t="s">
+        <v>194</v>
+      </c>
+      <c r="P46" s="14"/>
+      <c r="Q46" s="14"/>
+      <c r="R46" s="14"/>
+      <c r="S46" s="14"/>
+      <c r="T46" s="14"/>
+      <c r="U46" s="14"/>
+      <c r="V46" s="14"/>
+      <c r="W46" s="14"/>
+      <c r="X46" s="14"/>
+      <c r="Y46" s="14"/>
+      <c r="Z46" s="14"/>
+    </row>
+    <row r="47" spans="1:26" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="B47" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="C47" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="D47" s="14" t="s">
+        <v>188</v>
+      </c>
+      <c r="E47" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="F47" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="G47" s="14" t="s">
+        <v>183</v>
+      </c>
+      <c r="H47" s="14" t="s">
+        <v>200</v>
+      </c>
+      <c r="I47" s="14" t="s">
+        <v>204</v>
+      </c>
+      <c r="J47" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="K47" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="L47" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="M47" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="N47" s="14" t="s">
+        <v>198</v>
+      </c>
+      <c r="O47" s="14" t="s">
+        <v>194</v>
+      </c>
+      <c r="P47" s="14"/>
+      <c r="Q47" s="14"/>
+      <c r="R47" s="14"/>
+      <c r="S47" s="14"/>
+      <c r="T47" s="14"/>
+      <c r="U47" s="14"/>
+      <c r="V47" s="14"/>
+      <c r="W47" s="14"/>
+      <c r="X47" s="14"/>
+      <c r="Y47" s="14"/>
+      <c r="Z47" s="14"/>
+    </row>
+    <row r="48" spans="1:26" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="B48" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="C48" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="D48" s="14" t="s">
+        <v>188</v>
+      </c>
+      <c r="E48" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="F48" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="G48" s="14" t="s">
+        <v>184</v>
+      </c>
+      <c r="H48" s="14" t="s">
+        <v>200</v>
+      </c>
+      <c r="I48" s="14" t="s">
+        <v>193</v>
+      </c>
+      <c r="J48" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="K48" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="L48" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="M48" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="N48" s="14" t="s">
+        <v>198</v>
+      </c>
+      <c r="O48" s="14" t="s">
+        <v>194</v>
+      </c>
+      <c r="P48" s="14"/>
+      <c r="Q48" s="14"/>
+      <c r="R48" s="14"/>
+      <c r="S48" s="14"/>
+      <c r="T48" s="14"/>
+      <c r="U48" s="14"/>
+      <c r="V48" s="14"/>
+      <c r="W48" s="14"/>
+      <c r="X48" s="14"/>
+      <c r="Y48" s="14"/>
+      <c r="Z48" s="14"/>
+    </row>
+    <row r="49" spans="1:26" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="B49" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="C44" t="s">
-        <v>61</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="E44" s="1" t="s">
+      <c r="C49" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="D49" s="14" t="s">
+        <v>188</v>
+      </c>
+      <c r="E49" s="14" t="s">
         <v>182</v>
       </c>
-      <c r="F44" s="1" t="s">
+      <c r="F49" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="G44" s="1" t="s">
+      <c r="G49" s="14" t="s">
         <v>181</v>
       </c>
-      <c r="H44" s="1" t="s">
+      <c r="H49" s="14" t="s">
         <v>200</v>
       </c>
-      <c r="I44" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="J44" s="1" t="s">
+      <c r="I49" s="14" t="s">
+        <v>181</v>
+      </c>
+      <c r="J49" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="K44" s="1" t="s">
+      <c r="K49" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="L44" s="1" t="s">
+      <c r="L49" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="M44" s="1" t="s">
+      <c r="M49" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="N44" s="1" t="s">
+      <c r="N49" s="14" t="s">
         <v>198</v>
       </c>
-      <c r="O44" s="1" t="s">
+      <c r="O49" s="14" t="s">
         <v>194</v>
       </c>
-      <c r="P44" s="1"/>
-      <c r="Q44" s="1"/>
-      <c r="R44" s="1"/>
-      <c r="S44" s="1"/>
-      <c r="T44" s="1"/>
-      <c r="U44" s="1"/>
-      <c r="V44" s="1"/>
-      <c r="W44" s="1"/>
-      <c r="X44" s="1"/>
-      <c r="Y44" s="1"/>
-      <c r="Z44" s="1"/>
-    </row>
-    <row r="45" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
+      <c r="P49" s="14"/>
+      <c r="Q49" s="14"/>
+      <c r="R49" s="14"/>
+      <c r="S49" s="14"/>
+      <c r="T49" s="14"/>
+      <c r="U49" s="14"/>
+      <c r="V49" s="14"/>
+      <c r="W49" s="14"/>
+      <c r="X49" s="14"/>
+      <c r="Y49" s="14"/>
+      <c r="Z49" s="14"/>
+    </row>
+    <row r="50" spans="1:26" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="14" t="s">
+        <v>195</v>
+      </c>
+      <c r="B50" s="14" t="s">
+        <v>202</v>
+      </c>
+      <c r="C50" s="14" t="s">
+        <v>203</v>
+      </c>
+      <c r="D50" s="14" t="s">
+        <v>188</v>
+      </c>
+      <c r="E50" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="F50" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="G50" s="14" t="s">
+        <v>181</v>
+      </c>
+      <c r="H50" s="14" t="s">
+        <v>200</v>
+      </c>
+      <c r="I50" s="14" t="s">
+        <v>204</v>
+      </c>
+      <c r="J50" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="K50" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="L50" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="M50" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="N50" s="14" t="s">
+        <v>198</v>
+      </c>
+      <c r="O50" s="14" t="s">
+        <v>194</v>
+      </c>
+      <c r="P50" s="14"/>
+      <c r="Q50" s="14"/>
+      <c r="R50" s="14"/>
+      <c r="S50" s="14"/>
+      <c r="T50" s="14"/>
+      <c r="U50" s="14"/>
+      <c r="V50" s="14"/>
+      <c r="W50" s="14"/>
+      <c r="X50" s="14"/>
+      <c r="Y50" s="14"/>
+      <c r="Z50" s="14"/>
+    </row>
+    <row r="51" spans="1:26" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="14" t="s">
+        <v>195</v>
+      </c>
+      <c r="B51" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="C51" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="D51" s="14" t="s">
+        <v>188</v>
+      </c>
+      <c r="E51" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="F51" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="G51" s="14" t="s">
+        <v>181</v>
+      </c>
+      <c r="H51" s="14" t="s">
+        <v>200</v>
+      </c>
+      <c r="I51" s="14" t="s">
+        <v>183</v>
+      </c>
+      <c r="J51" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="K51" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="L51" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="M51" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="N51" s="14" t="s">
+        <v>198</v>
+      </c>
+      <c r="O51" s="14" t="s">
+        <v>194</v>
+      </c>
+      <c r="P51" s="14"/>
+      <c r="Q51" s="14"/>
+      <c r="R51" s="14"/>
+      <c r="S51" s="14"/>
+      <c r="T51" s="14"/>
+      <c r="U51" s="14"/>
+      <c r="V51" s="14"/>
+      <c r="W51" s="14"/>
+      <c r="X51" s="14"/>
+      <c r="Y51" s="14"/>
+      <c r="Z51" s="14"/>
+    </row>
+    <row r="52" spans="1:26" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="14" t="s">
+        <v>195</v>
+      </c>
+      <c r="B52" s="14" t="s">
+        <v>196</v>
+      </c>
+      <c r="C52" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="D52" s="14" t="s">
+        <v>188</v>
+      </c>
+      <c r="E52" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="F52" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="G52" s="14" t="s">
+        <v>181</v>
+      </c>
+      <c r="H52" s="14" t="s">
+        <v>200</v>
+      </c>
+      <c r="I52" s="14" t="s">
+        <v>205</v>
+      </c>
+      <c r="J52" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="K52" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="L52" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="M52" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="N52" s="14" t="s">
+        <v>198</v>
+      </c>
+      <c r="O52" s="14" t="s">
+        <v>194</v>
+      </c>
+      <c r="P52" s="14"/>
+      <c r="Q52" s="14"/>
+      <c r="R52" s="14"/>
+      <c r="S52" s="14"/>
+      <c r="T52" s="14"/>
+      <c r="U52" s="14"/>
+      <c r="V52" s="14"/>
+      <c r="W52" s="14"/>
+      <c r="X52" s="14"/>
+      <c r="Y52" s="14"/>
+      <c r="Z52" s="14"/>
+    </row>
+    <row r="53" spans="1:26" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="B53" s="14" t="s">
+        <v>206</v>
+      </c>
+      <c r="C53" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="D53" s="14" t="s">
+        <v>188</v>
+      </c>
+      <c r="E53" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="F53" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="G53" s="14" t="s">
+        <v>181</v>
+      </c>
+      <c r="H53" s="14" t="s">
+        <v>200</v>
+      </c>
+      <c r="I53" s="14" t="s">
+        <v>207</v>
+      </c>
+      <c r="J53" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="K53" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="L53" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="M53" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="N53" s="14" t="s">
+        <v>198</v>
+      </c>
+      <c r="O53" s="14" t="s">
+        <v>194</v>
+      </c>
+      <c r="P53" s="14"/>
+      <c r="Q53" s="14"/>
+      <c r="R53" s="14"/>
+      <c r="S53" s="14"/>
+      <c r="T53" s="14"/>
+      <c r="U53" s="14"/>
+      <c r="V53" s="14"/>
+      <c r="W53" s="14"/>
+      <c r="X53" s="14"/>
+      <c r="Y53" s="14"/>
+      <c r="Z53" s="14"/>
+    </row>
+    <row r="54" spans="1:26" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="14" t="s">
+        <v>195</v>
+      </c>
+      <c r="B54" s="14" t="s">
+        <v>208</v>
+      </c>
+      <c r="C54" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="D54" s="14" t="s">
+        <v>188</v>
+      </c>
+      <c r="E54" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="F54" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="G54" s="14" t="s">
+        <v>181</v>
+      </c>
+      <c r="H54" s="14" t="s">
+        <v>200</v>
+      </c>
+      <c r="I54" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="J54" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="K54" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="L54" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="M54" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="N54" s="14" t="s">
+        <v>198</v>
+      </c>
+      <c r="O54" s="14" t="s">
+        <v>194</v>
+      </c>
+      <c r="P54" s="14"/>
+      <c r="Q54" s="14"/>
+      <c r="R54" s="14"/>
+      <c r="S54" s="14"/>
+      <c r="T54" s="14"/>
+      <c r="U54" s="14"/>
+      <c r="V54" s="14"/>
+      <c r="W54" s="14"/>
+      <c r="X54" s="14"/>
+      <c r="Y54" s="14"/>
+      <c r="Z54" s="14"/>
+    </row>
+    <row r="55" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B55" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C45" t="s">
-        <v>61</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="F45" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="G45" s="1" t="s">
+      <c r="C55" t="s">
+        <v>61</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G55" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="H45" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="I45" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="J45" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="K45" s="1" t="s">
+      <c r="H55" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="I55" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="J55" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="L45" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="M45" s="1" t="s">
+      <c r="K55" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="L55" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="N45" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="O45" s="1" t="s">
+      <c r="M55" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="N55" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="P45" s="1"/>
-      <c r="Q45" s="1"/>
-      <c r="R45" s="1"/>
-      <c r="S45" s="1"/>
-      <c r="T45" s="1"/>
-      <c r="U45" s="1"/>
-      <c r="V45" s="1"/>
-      <c r="W45" s="1"/>
-      <c r="X45" s="1"/>
-      <c r="Y45" s="1"/>
-      <c r="Z45" s="1"/>
-    </row>
-    <row r="46" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C46" t="s">
-        <v>61</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="F46" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="G46" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="H46" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="I46" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="J46" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="K46" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="L46" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="M46" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="N46" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="O46" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="P46" s="1"/>
-      <c r="Q46" s="1"/>
-      <c r="R46" s="1"/>
-      <c r="S46" s="1"/>
-      <c r="T46" s="1"/>
-      <c r="U46" s="1"/>
-      <c r="V46" s="1"/>
-      <c r="W46" s="1"/>
-      <c r="X46" s="1"/>
-      <c r="Y46" s="1"/>
-      <c r="Z46" s="1"/>
-    </row>
-    <row r="47" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C47" t="s">
-        <v>61</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="E47" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="F47" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="G47" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="H47" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="I47" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="J47" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="K47" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="L47" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="M47" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="N47" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="O47" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="P47" s="1"/>
-      <c r="Q47" s="1"/>
-      <c r="R47" s="1"/>
-      <c r="S47" s="1"/>
-      <c r="T47" s="1"/>
-      <c r="U47" s="1"/>
-      <c r="V47" s="1"/>
-      <c r="W47" s="1"/>
-      <c r="X47" s="1"/>
-      <c r="Y47" s="1"/>
-      <c r="Z47" s="1"/>
-    </row>
-    <row r="48" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C48" t="s">
-        <v>61</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="E48" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="F48" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="G48" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="H48" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="I48" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="J48" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="K48" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="L48" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="M48" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="N48" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="O48" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="P48" s="1"/>
-      <c r="Q48" s="1"/>
-      <c r="R48" s="1"/>
-      <c r="S48" s="1"/>
-      <c r="T48" s="1"/>
-      <c r="U48" s="1"/>
-      <c r="V48" s="1"/>
-      <c r="W48" s="1"/>
-      <c r="X48" s="1"/>
-      <c r="Y48" s="1"/>
-      <c r="Z48" s="1"/>
-    </row>
-    <row r="49" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A49" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="F49" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="G49" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="H49" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="I49" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="J49" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="K49" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="L49" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="M49" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="N49" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="O49" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="P49" s="1"/>
-      <c r="Q49" s="1"/>
-      <c r="R49" s="1"/>
-      <c r="S49" s="1"/>
-      <c r="T49" s="1"/>
-      <c r="U49" s="1"/>
-      <c r="V49" s="1"/>
-      <c r="W49" s="1"/>
-      <c r="X49" s="1"/>
-      <c r="Y49" s="1"/>
-      <c r="Z49" s="1"/>
-    </row>
-    <row r="50" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A50" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="F50" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="G50" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="H50" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="I50" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="J50" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="K50" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="L50" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="M50" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="N50" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="O50" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="P50" s="1"/>
-      <c r="Q50" s="1"/>
-      <c r="R50" s="1"/>
-      <c r="S50" s="1"/>
-      <c r="T50" s="1"/>
-      <c r="U50" s="1"/>
-      <c r="V50" s="1"/>
-      <c r="W50" s="1"/>
-      <c r="X50" s="1"/>
-      <c r="Y50" s="1"/>
-      <c r="Z50" s="1"/>
-    </row>
-    <row r="51" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A51" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="F51" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="G51" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="H51" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="I51" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="J51" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="K51" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="L51" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="M51" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="N51" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="O51" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="P51" s="1"/>
-      <c r="Q51" s="1"/>
-      <c r="R51" s="1"/>
-      <c r="S51" s="1"/>
-      <c r="T51" s="1"/>
-      <c r="U51" s="1"/>
-      <c r="V51" s="1"/>
-      <c r="W51" s="1"/>
-      <c r="X51" s="1"/>
-      <c r="Y51" s="1"/>
-      <c r="Z51" s="1"/>
-    </row>
-    <row r="52" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A52" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="E52" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="F52" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="G52" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="H52" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="I52" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="J52" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="K52" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="L52" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="M52" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="N52" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="O52" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="P52" s="1"/>
-      <c r="Q52" s="1"/>
-      <c r="R52" s="1"/>
-      <c r="S52" s="1"/>
-      <c r="T52" s="1"/>
-      <c r="U52" s="1"/>
-      <c r="V52" s="1"/>
-      <c r="W52" s="1"/>
-      <c r="X52" s="1"/>
-      <c r="Y52" s="1"/>
-      <c r="Z52" s="1"/>
-    </row>
-    <row r="53" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A53" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="E53" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="F53" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="G53" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="H53" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="I53" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="J53" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="K53" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="L53" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="M53" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="N53" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="O53" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="P53" s="1"/>
-      <c r="Q53" s="1"/>
-      <c r="R53" s="1"/>
-      <c r="S53" s="1"/>
-      <c r="T53" s="1"/>
-      <c r="U53" s="1"/>
-      <c r="V53" s="1"/>
-      <c r="W53" s="1"/>
-      <c r="X53" s="1"/>
-      <c r="Y53" s="1"/>
-      <c r="Z53" s="1"/>
-    </row>
-    <row r="54" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A54" s="1"/>
-      <c r="B54" s="1"/>
-      <c r="C54" s="1"/>
-      <c r="E54" s="1"/>
-      <c r="F54" s="1"/>
-      <c r="G54" s="1"/>
-      <c r="H54" s="1"/>
-      <c r="I54" s="1"/>
-      <c r="J54" s="1"/>
-      <c r="K54" s="1"/>
-      <c r="L54" s="1"/>
-      <c r="M54" s="1"/>
-      <c r="N54" s="1"/>
-      <c r="O54" s="1"/>
-      <c r="P54" s="1"/>
-      <c r="Q54" s="1"/>
-      <c r="R54" s="1"/>
-      <c r="S54" s="1"/>
-      <c r="T54" s="1"/>
-      <c r="U54" s="1"/>
-      <c r="V54" s="1"/>
-      <c r="W54" s="1"/>
-      <c r="X54" s="1"/>
-      <c r="Y54" s="1"/>
-      <c r="Z54" s="1"/>
-    </row>
-    <row r="55" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A55" s="1"/>
-      <c r="B55" s="1"/>
-      <c r="C55" s="1"/>
-      <c r="E55" s="1"/>
-      <c r="F55" s="1"/>
-      <c r="G55" s="1"/>
-      <c r="H55" s="1"/>
-      <c r="I55" s="1"/>
-      <c r="J55" s="1"/>
-      <c r="K55" s="1"/>
-      <c r="L55" s="1"/>
-      <c r="M55" s="1"/>
-      <c r="N55" s="1"/>
-      <c r="O55" s="1"/>
+      <c r="O55" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="P55" s="1"/>
       <c r="Q55" s="1"/>
       <c r="R55" s="1"/>
@@ -3939,20 +4051,51 @@
       <c r="Z55" s="1"/>
     </row>
     <row r="56" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A56" s="1"/>
-      <c r="B56" s="1"/>
-      <c r="C56" s="1"/>
-      <c r="E56" s="1"/>
-      <c r="F56" s="1"/>
-      <c r="G56" s="1"/>
-      <c r="H56" s="1"/>
-      <c r="I56" s="1"/>
-      <c r="J56" s="1"/>
-      <c r="K56" s="1"/>
-      <c r="L56" s="1"/>
-      <c r="M56" s="1"/>
-      <c r="N56" s="1"/>
-      <c r="O56" s="1"/>
+      <c r="A56" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C56" t="s">
+        <v>61</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="H56" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="I56" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="J56" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="K56" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="L56" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="M56" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="N56" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="O56" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="P56" s="1"/>
       <c r="Q56" s="1"/>
       <c r="R56" s="1"/>
@@ -3966,20 +4109,51 @@
       <c r="Z56" s="1"/>
     </row>
     <row r="57" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A57" s="1"/>
-      <c r="B57" s="1"/>
-      <c r="C57" s="1"/>
-      <c r="E57" s="1"/>
-      <c r="F57" s="1"/>
-      <c r="G57" s="1"/>
-      <c r="H57" s="1"/>
-      <c r="I57" s="1"/>
-      <c r="J57" s="1"/>
-      <c r="K57" s="1"/>
-      <c r="L57" s="1"/>
-      <c r="M57" s="1"/>
-      <c r="N57" s="1"/>
-      <c r="O57" s="1"/>
+      <c r="A57" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G57" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="H57" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="I57" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="J57" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="K57" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="L57" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="M57" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="N57" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="O57" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="P57" s="1"/>
       <c r="Q57" s="1"/>
       <c r="R57" s="1"/>
@@ -3993,20 +4167,51 @@
       <c r="Z57" s="1"/>
     </row>
     <row r="58" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A58" s="1"/>
-      <c r="B58" s="1"/>
-      <c r="C58" s="1"/>
-      <c r="E58" s="1"/>
-      <c r="F58" s="1"/>
-      <c r="G58" s="1"/>
-      <c r="H58" s="1"/>
-      <c r="I58" s="1"/>
-      <c r="J58" s="1"/>
-      <c r="K58" s="1"/>
-      <c r="L58" s="1"/>
-      <c r="M58" s="1"/>
-      <c r="N58" s="1"/>
-      <c r="O58" s="1"/>
+      <c r="A58" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G58" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="H58" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="I58" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="J58" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="K58" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="L58" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="M58" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="N58" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="O58" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="P58" s="1"/>
       <c r="Q58" s="1"/>
       <c r="R58" s="1"/>
@@ -4020,20 +4225,51 @@
       <c r="Z58" s="1"/>
     </row>
     <row r="59" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A59" s="1"/>
-      <c r="B59" s="1"/>
-      <c r="C59" s="1"/>
-      <c r="E59" s="1"/>
-      <c r="F59" s="1"/>
-      <c r="G59" s="1"/>
-      <c r="H59" s="1"/>
-      <c r="I59" s="1"/>
-      <c r="J59" s="1"/>
-      <c r="K59" s="1"/>
-      <c r="L59" s="1"/>
-      <c r="M59" s="1"/>
-      <c r="N59" s="1"/>
-      <c r="O59" s="1"/>
+      <c r="A59" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G59" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="H59" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="I59" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="J59" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="K59" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="L59" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="M59" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="N59" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="O59" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="P59" s="1"/>
       <c r="Q59" s="1"/>
       <c r="R59" s="1"/>
@@ -4047,20 +4283,51 @@
       <c r="Z59" s="1"/>
     </row>
     <row r="60" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A60" s="1"/>
-      <c r="B60" s="1"/>
-      <c r="C60" s="1"/>
-      <c r="E60" s="1"/>
-      <c r="F60" s="1"/>
-      <c r="G60" s="1"/>
-      <c r="H60" s="1"/>
-      <c r="I60" s="1"/>
-      <c r="J60" s="1"/>
-      <c r="K60" s="1"/>
-      <c r="L60" s="1"/>
-      <c r="M60" s="1"/>
-      <c r="N60" s="1"/>
-      <c r="O60" s="1"/>
+      <c r="A60" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G60" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="H60" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="I60" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="J60" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="K60" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="L60" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="M60" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="N60" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="O60" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="P60" s="1"/>
       <c r="Q60" s="1"/>
       <c r="R60" s="1"/>
@@ -4074,20 +4341,51 @@
       <c r="Z60" s="1"/>
     </row>
     <row r="61" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A61" s="1"/>
-      <c r="B61" s="1"/>
-      <c r="C61" s="1"/>
-      <c r="E61" s="1"/>
-      <c r="F61" s="1"/>
-      <c r="G61" s="1"/>
-      <c r="H61" s="1"/>
-      <c r="I61" s="1"/>
-      <c r="J61" s="1"/>
-      <c r="K61" s="1"/>
-      <c r="L61" s="1"/>
-      <c r="M61" s="1"/>
-      <c r="N61" s="1"/>
-      <c r="O61" s="1"/>
+      <c r="A61" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G61" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="H61" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="I61" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="J61" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="K61" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="L61" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="M61" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="N61" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="O61" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="P61" s="1"/>
       <c r="Q61" s="1"/>
       <c r="R61" s="1"/>
@@ -4101,20 +4399,51 @@
       <c r="Z61" s="1"/>
     </row>
     <row r="62" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A62" s="1"/>
-      <c r="B62" s="1"/>
-      <c r="C62" s="1"/>
-      <c r="E62" s="1"/>
-      <c r="F62" s="1"/>
-      <c r="G62" s="1"/>
-      <c r="H62" s="1"/>
-      <c r="I62" s="1"/>
-      <c r="J62" s="1"/>
-      <c r="K62" s="1"/>
-      <c r="L62" s="1"/>
-      <c r="M62" s="1"/>
-      <c r="N62" s="1"/>
-      <c r="O62" s="1"/>
+      <c r="A62" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G62" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="H62" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="I62" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="J62" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="K62" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="L62" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="M62" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="N62" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="O62" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="P62" s="1"/>
       <c r="Q62" s="1"/>
       <c r="R62" s="1"/>
@@ -4127,302 +4456,643 @@
       <c r="Y62" s="1"/>
       <c r="Z62" s="1"/>
     </row>
-    <row r="63" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A63" s="1"/>
-      <c r="B63" s="1"/>
-      <c r="C63" s="1"/>
-      <c r="E63" s="1"/>
-      <c r="F63" s="1"/>
-      <c r="G63" s="1"/>
-      <c r="H63" s="1"/>
-      <c r="I63" s="1"/>
-      <c r="J63" s="1"/>
-      <c r="K63" s="1"/>
-      <c r="L63" s="1"/>
-      <c r="M63" s="1"/>
-      <c r="N63" s="1"/>
-      <c r="O63" s="1"/>
-      <c r="P63" s="1"/>
-      <c r="Q63" s="1"/>
-      <c r="R63" s="1"/>
-      <c r="S63" s="1"/>
-      <c r="T63" s="1"/>
-      <c r="U63" s="1"/>
-      <c r="V63" s="1"/>
-      <c r="W63" s="1"/>
-      <c r="X63" s="1"/>
-      <c r="Y63" s="1"/>
-      <c r="Z63" s="1"/>
-    </row>
-    <row r="64" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A64" s="1"/>
-      <c r="B64" s="1"/>
-      <c r="C64" s="1"/>
-      <c r="E64" s="1"/>
-      <c r="F64" s="1"/>
-      <c r="G64" s="1"/>
-      <c r="H64" s="1"/>
-      <c r="I64" s="1"/>
-      <c r="J64" s="1"/>
-      <c r="K64" s="1"/>
-      <c r="L64" s="1"/>
-      <c r="M64" s="1"/>
-      <c r="N64" s="1"/>
-      <c r="O64" s="1"/>
-      <c r="P64" s="1"/>
-      <c r="Q64" s="1"/>
-      <c r="R64" s="1"/>
-      <c r="S64" s="1"/>
-      <c r="T64" s="1"/>
-      <c r="U64" s="1"/>
-      <c r="V64" s="1"/>
-      <c r="W64" s="1"/>
-      <c r="X64" s="1"/>
-      <c r="Y64" s="1"/>
-      <c r="Z64" s="1"/>
-    </row>
-    <row r="65" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A65" s="1"/>
-      <c r="B65" s="1"/>
-      <c r="C65" s="1"/>
-      <c r="E65" s="1"/>
-      <c r="F65" s="1"/>
-      <c r="G65" s="1"/>
-      <c r="H65" s="1"/>
-      <c r="I65" s="1"/>
-      <c r="J65" s="1"/>
-      <c r="K65" s="1"/>
-      <c r="L65" s="1"/>
-      <c r="M65" s="1"/>
-      <c r="N65" s="1"/>
-      <c r="O65" s="1"/>
-      <c r="P65" s="1"/>
-      <c r="Q65" s="1"/>
-      <c r="R65" s="1"/>
-      <c r="S65" s="1"/>
-      <c r="T65" s="1"/>
-      <c r="U65" s="1"/>
-      <c r="V65" s="1"/>
-      <c r="W65" s="1"/>
-      <c r="X65" s="1"/>
-      <c r="Y65" s="1"/>
-      <c r="Z65" s="1"/>
-    </row>
-    <row r="66" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A66" s="1"/>
-      <c r="B66" s="1"/>
-      <c r="C66" s="1"/>
-      <c r="E66" s="1"/>
-      <c r="F66" s="1"/>
-      <c r="G66" s="1"/>
-      <c r="H66" s="1"/>
-      <c r="I66" s="1"/>
-      <c r="J66" s="1"/>
-      <c r="K66" s="1"/>
-      <c r="L66" s="1"/>
-      <c r="M66" s="1"/>
-      <c r="N66" s="1"/>
-      <c r="O66" s="1"/>
-      <c r="P66" s="1"/>
-      <c r="Q66" s="1"/>
-      <c r="R66" s="1"/>
-      <c r="S66" s="1"/>
-      <c r="T66" s="1"/>
-      <c r="U66" s="1"/>
-      <c r="V66" s="1"/>
-      <c r="W66" s="1"/>
-      <c r="X66" s="1"/>
-      <c r="Y66" s="1"/>
-      <c r="Z66" s="1"/>
-    </row>
-    <row r="67" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A67" s="1"/>
-      <c r="B67" s="1"/>
-      <c r="C67" s="1"/>
-      <c r="E67" s="1"/>
-      <c r="F67" s="1"/>
-      <c r="G67" s="1"/>
-      <c r="H67" s="1"/>
-      <c r="I67" s="1"/>
-      <c r="J67" s="1"/>
-      <c r="K67" s="1"/>
-      <c r="L67" s="1"/>
-      <c r="M67" s="1"/>
-      <c r="N67" s="1"/>
-      <c r="O67" s="1"/>
-      <c r="P67" s="1"/>
-      <c r="Q67" s="1"/>
-      <c r="R67" s="1"/>
-      <c r="S67" s="1"/>
-      <c r="T67" s="1"/>
-      <c r="U67" s="1"/>
-      <c r="V67" s="1"/>
-      <c r="W67" s="1"/>
-      <c r="X67" s="1"/>
-      <c r="Y67" s="1"/>
-      <c r="Z67" s="1"/>
-    </row>
-    <row r="68" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A68" s="1"/>
-      <c r="B68" s="1"/>
-      <c r="C68" s="1"/>
-      <c r="E68" s="1"/>
-      <c r="F68" s="1"/>
-      <c r="G68" s="1"/>
-      <c r="H68" s="1"/>
-      <c r="I68" s="1"/>
-      <c r="J68" s="1"/>
-      <c r="K68" s="1"/>
-      <c r="L68" s="1"/>
-      <c r="M68" s="1"/>
-      <c r="N68" s="1"/>
-      <c r="O68" s="1"/>
-      <c r="P68" s="1"/>
-      <c r="Q68" s="1"/>
-      <c r="R68" s="1"/>
-      <c r="S68" s="1"/>
-      <c r="T68" s="1"/>
-      <c r="U68" s="1"/>
-      <c r="V68" s="1"/>
-      <c r="W68" s="1"/>
-      <c r="X68" s="1"/>
-      <c r="Y68" s="1"/>
-      <c r="Z68" s="1"/>
-    </row>
-    <row r="69" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A69" s="1"/>
-      <c r="B69" s="1"/>
-      <c r="C69" s="1"/>
-      <c r="E69" s="1"/>
-      <c r="F69" s="1"/>
-      <c r="G69" s="1"/>
-      <c r="H69" s="1"/>
-      <c r="I69" s="1"/>
-      <c r="J69" s="1"/>
-      <c r="K69" s="1"/>
-      <c r="L69" s="1"/>
-      <c r="M69" s="1"/>
-      <c r="N69" s="1"/>
-      <c r="O69" s="1"/>
-      <c r="P69" s="1"/>
-      <c r="Q69" s="1"/>
-      <c r="R69" s="1"/>
-      <c r="S69" s="1"/>
-      <c r="T69" s="1"/>
-      <c r="U69" s="1"/>
-      <c r="V69" s="1"/>
-      <c r="W69" s="1"/>
-      <c r="X69" s="1"/>
-      <c r="Y69" s="1"/>
-      <c r="Z69" s="1"/>
-    </row>
-    <row r="70" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A70" s="1"/>
-      <c r="B70" s="1"/>
-      <c r="C70" s="1"/>
-      <c r="E70" s="1"/>
-      <c r="F70" s="1"/>
-      <c r="G70" s="1"/>
-      <c r="H70" s="1"/>
-      <c r="I70" s="1"/>
-      <c r="J70" s="1"/>
-      <c r="K70" s="1"/>
-      <c r="L70" s="1"/>
-      <c r="M70" s="1"/>
-      <c r="N70" s="1"/>
-      <c r="O70" s="1"/>
-      <c r="P70" s="1"/>
-      <c r="Q70" s="1"/>
-      <c r="R70" s="1"/>
-      <c r="S70" s="1"/>
-      <c r="T70" s="1"/>
-      <c r="U70" s="1"/>
-      <c r="V70" s="1"/>
-      <c r="W70" s="1"/>
-      <c r="X70" s="1"/>
-      <c r="Y70" s="1"/>
-      <c r="Z70" s="1"/>
-    </row>
-    <row r="71" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A71" s="1"/>
-      <c r="B71" s="1"/>
-      <c r="C71" s="1"/>
-      <c r="E71" s="1"/>
-      <c r="F71" s="1"/>
-      <c r="G71" s="1"/>
-      <c r="H71" s="1"/>
-      <c r="I71" s="1"/>
-      <c r="J71" s="1"/>
-      <c r="K71" s="1"/>
-      <c r="L71" s="1"/>
-      <c r="M71" s="1"/>
-      <c r="N71" s="1"/>
-      <c r="O71" s="1"/>
-      <c r="P71" s="1"/>
-      <c r="Q71" s="1"/>
-      <c r="R71" s="1"/>
-      <c r="S71" s="1"/>
-      <c r="T71" s="1"/>
-      <c r="U71" s="1"/>
-      <c r="V71" s="1"/>
-      <c r="W71" s="1"/>
-      <c r="X71" s="1"/>
-      <c r="Y71" s="1"/>
-      <c r="Z71" s="1"/>
-    </row>
-    <row r="72" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A72" s="1"/>
-      <c r="B72" s="1"/>
-      <c r="C72" s="1"/>
-      <c r="E72" s="1"/>
-      <c r="F72" s="1"/>
-      <c r="G72" s="1"/>
-      <c r="H72" s="1"/>
-      <c r="I72" s="1"/>
-      <c r="J72" s="1"/>
-      <c r="K72" s="1"/>
-      <c r="L72" s="1"/>
-      <c r="M72" s="1"/>
-      <c r="N72" s="1"/>
-      <c r="O72" s="1"/>
-      <c r="P72" s="1"/>
-      <c r="Q72" s="1"/>
-      <c r="R72" s="1"/>
-      <c r="S72" s="1"/>
-      <c r="T72" s="1"/>
-      <c r="U72" s="1"/>
-      <c r="V72" s="1"/>
-      <c r="W72" s="1"/>
-      <c r="X72" s="1"/>
-      <c r="Y72" s="1"/>
-      <c r="Z72" s="1"/>
-    </row>
-    <row r="73" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A73" s="1"/>
-      <c r="B73" s="1"/>
-      <c r="C73" s="1"/>
-      <c r="E73" s="1"/>
-      <c r="F73" s="1"/>
-      <c r="G73" s="1"/>
-      <c r="H73" s="1"/>
-      <c r="I73" s="1"/>
-      <c r="J73" s="1"/>
-      <c r="K73" s="1"/>
-      <c r="L73" s="1"/>
-      <c r="M73" s="1"/>
-      <c r="N73" s="1"/>
-      <c r="O73" s="1"/>
-      <c r="P73" s="1"/>
-      <c r="Q73" s="1"/>
-      <c r="R73" s="1"/>
-      <c r="S73" s="1"/>
-      <c r="T73" s="1"/>
-      <c r="U73" s="1"/>
-      <c r="V73" s="1"/>
-      <c r="W73" s="1"/>
-      <c r="X73" s="1"/>
-      <c r="Y73" s="1"/>
-      <c r="Z73" s="1"/>
+    <row r="63" spans="1:26" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="14" t="s">
+        <v>195</v>
+      </c>
+      <c r="B63" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="C63" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="D63" s="14" t="s">
+        <v>188</v>
+      </c>
+      <c r="E63" s="14" t="s">
+        <v>184</v>
+      </c>
+      <c r="F63" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="G63" s="14" t="s">
+        <v>181</v>
+      </c>
+      <c r="H63" s="14" t="s">
+        <v>200</v>
+      </c>
+      <c r="I63" s="14" t="s">
+        <v>214</v>
+      </c>
+      <c r="J63" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="K63" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="L63" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="M63" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="N63" s="14" t="s">
+        <v>213</v>
+      </c>
+      <c r="O63" s="14" t="s">
+        <v>221</v>
+      </c>
+      <c r="P63" s="14"/>
+      <c r="Q63" s="14"/>
+      <c r="R63" s="14"/>
+      <c r="S63" s="14"/>
+      <c r="T63" s="14"/>
+      <c r="U63" s="14"/>
+      <c r="V63" s="14"/>
+      <c r="W63" s="14"/>
+      <c r="X63" s="14"/>
+      <c r="Y63" s="14"/>
+      <c r="Z63" s="14"/>
+    </row>
+    <row r="64" spans="1:26" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="14" t="s">
+        <v>195</v>
+      </c>
+      <c r="B64" s="14" t="s">
+        <v>196</v>
+      </c>
+      <c r="C64" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="D64" s="14" t="s">
+        <v>188</v>
+      </c>
+      <c r="E64" s="14" t="s">
+        <v>184</v>
+      </c>
+      <c r="F64" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="G64" s="14" t="s">
+        <v>181</v>
+      </c>
+      <c r="H64" s="14" t="s">
+        <v>200</v>
+      </c>
+      <c r="I64" s="14" t="s">
+        <v>214</v>
+      </c>
+      <c r="J64" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="K64" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="L64" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="M64" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="N64" s="14" t="s">
+        <v>213</v>
+      </c>
+      <c r="O64" s="14" t="s">
+        <v>221</v>
+      </c>
+      <c r="P64" s="14"/>
+      <c r="Q64" s="14"/>
+      <c r="R64" s="14"/>
+      <c r="S64" s="14"/>
+      <c r="T64" s="14"/>
+      <c r="U64" s="14"/>
+      <c r="V64" s="14"/>
+      <c r="W64" s="14"/>
+      <c r="X64" s="14"/>
+      <c r="Y64" s="14"/>
+      <c r="Z64" s="14"/>
+    </row>
+    <row r="65" spans="1:26" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="14" t="s">
+        <v>195</v>
+      </c>
+      <c r="B65" s="14" t="s">
+        <v>208</v>
+      </c>
+      <c r="C65" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="D65" s="14" t="s">
+        <v>188</v>
+      </c>
+      <c r="E65" s="14" t="s">
+        <v>184</v>
+      </c>
+      <c r="F65" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="G65" s="14" t="s">
+        <v>181</v>
+      </c>
+      <c r="H65" s="14" t="s">
+        <v>200</v>
+      </c>
+      <c r="I65" s="14" t="s">
+        <v>204</v>
+      </c>
+      <c r="J65" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="K65" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="L65" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="M65" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="N65" s="14" t="s">
+        <v>213</v>
+      </c>
+      <c r="O65" s="14" t="s">
+        <v>221</v>
+      </c>
+      <c r="P65" s="14"/>
+      <c r="Q65" s="14"/>
+      <c r="R65" s="14"/>
+      <c r="S65" s="14"/>
+      <c r="T65" s="14"/>
+      <c r="U65" s="14"/>
+      <c r="V65" s="14"/>
+      <c r="W65" s="14"/>
+      <c r="X65" s="14"/>
+      <c r="Y65" s="14"/>
+      <c r="Z65" s="14"/>
+    </row>
+    <row r="66" spans="1:26" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="B66" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="C66" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="D66" s="14" t="s">
+        <v>188</v>
+      </c>
+      <c r="E66" s="14" t="s">
+        <v>207</v>
+      </c>
+      <c r="F66" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="G66" s="14" t="s">
+        <v>181</v>
+      </c>
+      <c r="H66" s="14" t="s">
+        <v>200</v>
+      </c>
+      <c r="I66" s="14" t="s">
+        <v>215</v>
+      </c>
+      <c r="J66" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="K66" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="L66" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="M66" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="N66" s="14" t="s">
+        <v>213</v>
+      </c>
+      <c r="O66" s="14" t="s">
+        <v>221</v>
+      </c>
+      <c r="P66" s="14"/>
+      <c r="Q66" s="14"/>
+      <c r="R66" s="14"/>
+      <c r="S66" s="14"/>
+      <c r="T66" s="14"/>
+      <c r="U66" s="14"/>
+      <c r="V66" s="14"/>
+      <c r="W66" s="14"/>
+      <c r="X66" s="14"/>
+      <c r="Y66" s="14"/>
+      <c r="Z66" s="14"/>
+    </row>
+    <row r="67" spans="1:26" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="B67" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="C67" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="D67" s="14" t="s">
+        <v>188</v>
+      </c>
+      <c r="E67" s="14" t="s">
+        <v>207</v>
+      </c>
+      <c r="F67" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="G67" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="H67" s="14" t="s">
+        <v>200</v>
+      </c>
+      <c r="I67" s="14" t="s">
+        <v>216</v>
+      </c>
+      <c r="J67" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="K67" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="L67" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="M67" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="N67" s="14" t="s">
+        <v>213</v>
+      </c>
+      <c r="O67" s="14" t="s">
+        <v>221</v>
+      </c>
+      <c r="P67" s="14"/>
+      <c r="Q67" s="14"/>
+      <c r="R67" s="14"/>
+      <c r="S67" s="14"/>
+      <c r="T67" s="14"/>
+      <c r="U67" s="14"/>
+      <c r="V67" s="14"/>
+      <c r="W67" s="14"/>
+      <c r="X67" s="14"/>
+      <c r="Y67" s="14"/>
+      <c r="Z67" s="14"/>
+    </row>
+    <row r="68" spans="1:26" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="B68" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="C68" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="D68" s="14" t="s">
+        <v>188</v>
+      </c>
+      <c r="E68" s="14" t="s">
+        <v>207</v>
+      </c>
+      <c r="F68" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="G68" s="14" t="s">
+        <v>183</v>
+      </c>
+      <c r="H68" s="14" t="s">
+        <v>200</v>
+      </c>
+      <c r="I68" s="14" t="s">
+        <v>186</v>
+      </c>
+      <c r="J68" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="K68" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="L68" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="M68" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="N68" s="14" t="s">
+        <v>213</v>
+      </c>
+      <c r="O68" s="14" t="s">
+        <v>221</v>
+      </c>
+      <c r="P68" s="14"/>
+      <c r="Q68" s="14"/>
+      <c r="R68" s="14"/>
+      <c r="S68" s="14"/>
+      <c r="T68" s="14"/>
+      <c r="U68" s="14"/>
+      <c r="V68" s="14"/>
+      <c r="W68" s="14"/>
+      <c r="X68" s="14"/>
+      <c r="Y68" s="14"/>
+      <c r="Z68" s="14"/>
+    </row>
+    <row r="69" spans="1:26" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="B69" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="C69" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="D69" s="14" t="s">
+        <v>188</v>
+      </c>
+      <c r="E69" s="14" t="s">
+        <v>207</v>
+      </c>
+      <c r="F69" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="G69" s="14" t="s">
+        <v>184</v>
+      </c>
+      <c r="H69" s="14" t="s">
+        <v>200</v>
+      </c>
+      <c r="I69" s="14" t="s">
+        <v>216</v>
+      </c>
+      <c r="J69" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="K69" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="L69" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="M69" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="N69" s="14" t="s">
+        <v>213</v>
+      </c>
+      <c r="O69" s="14" t="s">
+        <v>221</v>
+      </c>
+      <c r="P69" s="14"/>
+      <c r="Q69" s="14"/>
+      <c r="R69" s="14"/>
+      <c r="S69" s="14"/>
+      <c r="T69" s="14"/>
+      <c r="U69" s="14"/>
+      <c r="V69" s="14"/>
+      <c r="W69" s="14"/>
+      <c r="X69" s="14"/>
+      <c r="Y69" s="14"/>
+      <c r="Z69" s="14"/>
+    </row>
+    <row r="70" spans="1:26" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="B70" s="14" t="s">
+        <v>206</v>
+      </c>
+      <c r="C70" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="D70" s="14" t="s">
+        <v>188</v>
+      </c>
+      <c r="E70" s="14" t="s">
+        <v>207</v>
+      </c>
+      <c r="F70" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="G70" s="14" t="s">
+        <v>181</v>
+      </c>
+      <c r="H70" s="14" t="s">
+        <v>200</v>
+      </c>
+      <c r="I70" s="14" t="s">
+        <v>183</v>
+      </c>
+      <c r="J70" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="K70" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="L70" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="M70" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="N70" s="14" t="s">
+        <v>213</v>
+      </c>
+      <c r="O70" s="14" t="s">
+        <v>221</v>
+      </c>
+      <c r="P70" s="14"/>
+      <c r="Q70" s="14"/>
+      <c r="R70" s="14"/>
+      <c r="S70" s="14"/>
+      <c r="T70" s="14"/>
+      <c r="U70" s="14"/>
+      <c r="V70" s="14"/>
+      <c r="W70" s="14"/>
+      <c r="X70" s="14"/>
+      <c r="Y70" s="14"/>
+      <c r="Z70" s="14"/>
+    </row>
+    <row r="71" spans="1:26" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="B71" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="C71" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="D71" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="E71" s="14" t="s">
+        <v>218</v>
+      </c>
+      <c r="F71" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="G71" s="14" t="s">
+        <v>181</v>
+      </c>
+      <c r="H71" s="14" t="s">
+        <v>200</v>
+      </c>
+      <c r="I71" s="14" t="s">
+        <v>219</v>
+      </c>
+      <c r="J71" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="K71" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="L71" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="M71" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="N71" s="14" t="s">
+        <v>213</v>
+      </c>
+      <c r="O71" s="14" t="s">
+        <v>221</v>
+      </c>
+      <c r="P71" s="14"/>
+      <c r="Q71" s="14"/>
+      <c r="R71" s="14"/>
+      <c r="S71" s="14"/>
+      <c r="T71" s="14"/>
+      <c r="U71" s="14"/>
+      <c r="V71" s="14"/>
+      <c r="W71" s="14"/>
+      <c r="X71" s="14"/>
+      <c r="Y71" s="14"/>
+      <c r="Z71" s="14"/>
+    </row>
+    <row r="72" spans="1:26" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="B72" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="C72" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="D72" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="E72" s="14" t="s">
+        <v>218</v>
+      </c>
+      <c r="F72" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="G72" s="14" t="s">
+        <v>181</v>
+      </c>
+      <c r="H72" s="14" t="s">
+        <v>200</v>
+      </c>
+      <c r="I72" s="14" t="s">
+        <v>220</v>
+      </c>
+      <c r="J72" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="K72" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="L72" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="M72" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="N72" s="14" t="s">
+        <v>213</v>
+      </c>
+      <c r="O72" s="14" t="s">
+        <v>221</v>
+      </c>
+      <c r="P72" s="14"/>
+      <c r="Q72" s="14"/>
+      <c r="R72" s="14"/>
+      <c r="S72" s="14"/>
+      <c r="T72" s="14"/>
+      <c r="U72" s="14"/>
+      <c r="V72" s="14"/>
+      <c r="W72" s="14"/>
+      <c r="X72" s="14"/>
+      <c r="Y72" s="14"/>
+      <c r="Z72" s="14"/>
+    </row>
+    <row r="73" spans="1:26" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="14" t="s">
+        <v>195</v>
+      </c>
+      <c r="B73" s="14" t="s">
+        <v>202</v>
+      </c>
+      <c r="C73" s="14" t="s">
+        <v>203</v>
+      </c>
+      <c r="D73" s="14" t="s">
+        <v>188</v>
+      </c>
+      <c r="E73" s="14" t="s">
+        <v>207</v>
+      </c>
+      <c r="F73" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="G73" s="14" t="s">
+        <v>181</v>
+      </c>
+      <c r="H73" s="14" t="s">
+        <v>200</v>
+      </c>
+      <c r="I73" s="14" t="s">
+        <v>184</v>
+      </c>
+      <c r="J73" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="K73" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="L73" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="M73" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="N73" s="14" t="s">
+        <v>213</v>
+      </c>
+      <c r="O73" s="14" t="s">
+        <v>221</v>
+      </c>
+      <c r="P73" s="14"/>
+      <c r="Q73" s="14"/>
+      <c r="R73" s="14"/>
+      <c r="S73" s="14"/>
+      <c r="T73" s="14"/>
+      <c r="U73" s="14"/>
+      <c r="V73" s="14"/>
+      <c r="W73" s="14"/>
+      <c r="X73" s="14"/>
+      <c r="Y73" s="14"/>
+      <c r="Z73" s="14"/>
     </row>
     <row r="74" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>

</xml_diff>

<commit_message>
sampling cohort 6 2018-08-21
</commit_message>
<xml_diff>
--- a/Data/2018-08-14_master_datac_2018_collection_year.xlsx
+++ b/Data/2018-08-14_master_datac_2018_collection_year.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andrew.nguyen\Desktop\Circadian_rhythm_runs_seasonal_timing\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F26EAB03-E28C-40B8-A86D-25EDF99F3D1C}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CAAA300-08CC-40DA-B88C-784CF8C3A8C4}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1800" yWindow="1935" windowWidth="35820" windowHeight="18720" xr2:uid="{C7477166-8A7C-B04A-9643-C277FEDCDAAB}"/>
+    <workbookView xWindow="1800" yWindow="1935" windowWidth="35820" windowHeight="18720" activeTab="1" xr2:uid="{C7477166-8A7C-B04A-9643-C277FEDCDAAB}"/>
   </bookViews>
   <sheets>
     <sheet name="Maggot_Collections" sheetId="2" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1500" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1590" uniqueCount="222">
   <si>
     <t>Ind_ID</t>
   </si>
@@ -1101,7 +1101,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D3F78F5-4EA8-6A42-B216-41A8EC7A5E8D}">
   <dimension ref="A1:Z102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+    <sheetView topLeftCell="A52" workbookViewId="0">
       <selection activeCell="H65" sqref="H65"/>
     </sheetView>
   </sheetViews>
@@ -5887,8 +5887,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92725FB9-1A17-2546-9DFA-6C0D39437891}">
   <dimension ref="A1:AS91"/>
   <sheetViews>
-    <sheetView topLeftCell="Q18" workbookViewId="0">
-      <selection activeCell="AB32" sqref="AB32"/>
+    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
+      <selection activeCell="C77" sqref="C77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -6038,6 +6038,9 @@
       <c r="A2">
         <v>1</v>
       </c>
+      <c r="C2" t="s">
+        <v>59</v>
+      </c>
       <c r="G2" s="1" t="s">
         <v>88</v>
       </c>
@@ -6058,6 +6061,9 @@
       <c r="A3">
         <v>2</v>
       </c>
+      <c r="C3" t="s">
+        <v>59</v>
+      </c>
       <c r="G3" s="1" t="s">
         <v>88</v>
       </c>
@@ -6078,6 +6084,9 @@
       <c r="A4">
         <v>3</v>
       </c>
+      <c r="C4" t="s">
+        <v>59</v>
+      </c>
       <c r="G4" s="1" t="s">
         <v>88</v>
       </c>
@@ -6098,6 +6107,9 @@
       <c r="A5">
         <v>4</v>
       </c>
+      <c r="C5" t="s">
+        <v>59</v>
+      </c>
       <c r="G5" s="1" t="s">
         <v>88</v>
       </c>
@@ -6118,6 +6130,9 @@
       <c r="A6">
         <v>5</v>
       </c>
+      <c r="C6" t="s">
+        <v>59</v>
+      </c>
       <c r="G6" s="1" t="s">
         <v>88</v>
       </c>
@@ -6138,6 +6153,9 @@
       <c r="A7">
         <v>6</v>
       </c>
+      <c r="C7" t="s">
+        <v>59</v>
+      </c>
       <c r="G7" s="1" t="s">
         <v>88</v>
       </c>
@@ -6158,6 +6176,9 @@
       <c r="A8">
         <v>7</v>
       </c>
+      <c r="C8" t="s">
+        <v>59</v>
+      </c>
       <c r="G8" s="1" t="s">
         <v>88</v>
       </c>
@@ -6178,6 +6199,9 @@
       <c r="A9">
         <v>8</v>
       </c>
+      <c r="C9" t="s">
+        <v>59</v>
+      </c>
       <c r="G9" s="1" t="s">
         <v>88</v>
       </c>
@@ -6198,6 +6222,9 @@
       <c r="A10">
         <v>9</v>
       </c>
+      <c r="C10" t="s">
+        <v>59</v>
+      </c>
       <c r="G10" s="1" t="s">
         <v>88</v>
       </c>
@@ -6218,6 +6245,9 @@
       <c r="A11">
         <v>10</v>
       </c>
+      <c r="C11" t="s">
+        <v>59</v>
+      </c>
       <c r="G11" s="1" t="s">
         <v>88</v>
       </c>
@@ -6238,6 +6268,9 @@
       <c r="A12">
         <v>11</v>
       </c>
+      <c r="C12" t="s">
+        <v>59</v>
+      </c>
       <c r="G12" s="1" t="s">
         <v>88</v>
       </c>
@@ -6258,6 +6291,9 @@
       <c r="A13">
         <v>12</v>
       </c>
+      <c r="C13" t="s">
+        <v>59</v>
+      </c>
       <c r="G13" s="1" t="s">
         <v>88</v>
       </c>
@@ -6278,6 +6314,9 @@
       <c r="A14">
         <v>13</v>
       </c>
+      <c r="C14" t="s">
+        <v>59</v>
+      </c>
       <c r="G14" s="1" t="s">
         <v>88</v>
       </c>
@@ -6298,6 +6337,9 @@
       <c r="A15">
         <v>14</v>
       </c>
+      <c r="C15" t="s">
+        <v>59</v>
+      </c>
       <c r="G15" s="1" t="s">
         <v>88</v>
       </c>
@@ -6318,6 +6360,9 @@
       <c r="A16">
         <v>15</v>
       </c>
+      <c r="C16" t="s">
+        <v>59</v>
+      </c>
       <c r="G16" s="1" t="s">
         <v>88</v>
       </c>
@@ -6338,6 +6383,9 @@
       <c r="A17">
         <v>16</v>
       </c>
+      <c r="C17" t="s">
+        <v>60</v>
+      </c>
       <c r="G17" s="1" t="s">
         <v>88</v>
       </c>
@@ -6358,6 +6406,9 @@
       <c r="A18">
         <v>17</v>
       </c>
+      <c r="C18" t="s">
+        <v>60</v>
+      </c>
       <c r="G18" s="1" t="s">
         <v>88</v>
       </c>
@@ -6378,6 +6429,9 @@
       <c r="A19">
         <v>18</v>
       </c>
+      <c r="C19" t="s">
+        <v>60</v>
+      </c>
       <c r="G19" s="1" t="s">
         <v>88</v>
       </c>
@@ -6398,6 +6452,9 @@
       <c r="A20">
         <v>19</v>
       </c>
+      <c r="C20" t="s">
+        <v>60</v>
+      </c>
       <c r="G20" s="1" t="s">
         <v>88</v>
       </c>
@@ -6418,6 +6475,9 @@
       <c r="A21">
         <v>20</v>
       </c>
+      <c r="C21" t="s">
+        <v>60</v>
+      </c>
       <c r="G21" s="1" t="s">
         <v>88</v>
       </c>
@@ -6438,6 +6498,9 @@
       <c r="A22">
         <v>21</v>
       </c>
+      <c r="C22" t="s">
+        <v>60</v>
+      </c>
       <c r="G22" s="1" t="s">
         <v>88</v>
       </c>
@@ -6458,6 +6521,9 @@
       <c r="A23">
         <v>22</v>
       </c>
+      <c r="C23" t="s">
+        <v>60</v>
+      </c>
       <c r="G23" s="1" t="s">
         <v>88</v>
       </c>
@@ -6478,6 +6544,9 @@
       <c r="A24">
         <v>23</v>
       </c>
+      <c r="C24" t="s">
+        <v>60</v>
+      </c>
       <c r="G24" s="1" t="s">
         <v>88</v>
       </c>
@@ -6498,6 +6567,9 @@
       <c r="A25">
         <v>24</v>
       </c>
+      <c r="C25" t="s">
+        <v>60</v>
+      </c>
       <c r="G25" s="1" t="s">
         <v>88</v>
       </c>
@@ -6518,6 +6590,9 @@
       <c r="A26">
         <v>25</v>
       </c>
+      <c r="C26" t="s">
+        <v>60</v>
+      </c>
       <c r="G26" s="1" t="s">
         <v>88</v>
       </c>
@@ -6538,6 +6613,9 @@
       <c r="A27">
         <v>26</v>
       </c>
+      <c r="C27" t="s">
+        <v>60</v>
+      </c>
       <c r="G27" s="1" t="s">
         <v>88</v>
       </c>
@@ -6558,6 +6636,9 @@
       <c r="A28">
         <v>27</v>
       </c>
+      <c r="C28" t="s">
+        <v>60</v>
+      </c>
       <c r="G28" s="1" t="s">
         <v>88</v>
       </c>
@@ -6578,6 +6659,9 @@
       <c r="A29">
         <v>28</v>
       </c>
+      <c r="C29" t="s">
+        <v>60</v>
+      </c>
       <c r="G29" s="1" t="s">
         <v>88</v>
       </c>
@@ -6598,6 +6682,9 @@
       <c r="A30">
         <v>29</v>
       </c>
+      <c r="C30" t="s">
+        <v>60</v>
+      </c>
       <c r="G30" s="1" t="s">
         <v>88</v>
       </c>
@@ -6618,6 +6705,9 @@
       <c r="A31">
         <v>30</v>
       </c>
+      <c r="C31" t="s">
+        <v>60</v>
+      </c>
       <c r="G31" s="1" t="s">
         <v>88</v>
       </c>
@@ -6641,6 +6731,9 @@
       <c r="B32" t="s">
         <v>89</v>
       </c>
+      <c r="C32" t="s">
+        <v>59</v>
+      </c>
       <c r="G32" s="1" t="s">
         <v>88</v>
       </c>
@@ -6668,6 +6761,9 @@
       <c r="B33" t="s">
         <v>89</v>
       </c>
+      <c r="C33" t="s">
+        <v>59</v>
+      </c>
       <c r="G33" s="1" t="s">
         <v>88</v>
       </c>
@@ -6695,6 +6791,9 @@
       <c r="B34" t="s">
         <v>89</v>
       </c>
+      <c r="C34" t="s">
+        <v>59</v>
+      </c>
       <c r="G34" s="1" t="s">
         <v>88</v>
       </c>
@@ -6722,6 +6821,9 @@
       <c r="B35" t="s">
         <v>89</v>
       </c>
+      <c r="C35" t="s">
+        <v>59</v>
+      </c>
       <c r="G35" s="1" t="s">
         <v>88</v>
       </c>
@@ -6749,6 +6851,9 @@
       <c r="B36" t="s">
         <v>89</v>
       </c>
+      <c r="C36" t="s">
+        <v>59</v>
+      </c>
       <c r="G36" s="1" t="s">
         <v>88</v>
       </c>
@@ -6776,6 +6881,9 @@
       <c r="B37" t="s">
         <v>89</v>
       </c>
+      <c r="C37" t="s">
+        <v>59</v>
+      </c>
       <c r="G37" s="1" t="s">
         <v>88</v>
       </c>
@@ -6803,6 +6911,9 @@
       <c r="B38" t="s">
         <v>89</v>
       </c>
+      <c r="C38" t="s">
+        <v>59</v>
+      </c>
       <c r="G38" s="1" t="s">
         <v>88</v>
       </c>
@@ -6830,6 +6941,9 @@
       <c r="B39" t="s">
         <v>89</v>
       </c>
+      <c r="C39" t="s">
+        <v>59</v>
+      </c>
       <c r="G39" s="1" t="s">
         <v>88</v>
       </c>
@@ -6857,6 +6971,9 @@
       <c r="B40" t="s">
         <v>89</v>
       </c>
+      <c r="C40" t="s">
+        <v>59</v>
+      </c>
       <c r="G40" s="1" t="s">
         <v>88</v>
       </c>
@@ -6884,6 +7001,9 @@
       <c r="B41" t="s">
         <v>89</v>
       </c>
+      <c r="C41" t="s">
+        <v>59</v>
+      </c>
       <c r="G41" s="1" t="s">
         <v>88</v>
       </c>
@@ -6911,6 +7031,9 @@
       <c r="B42" t="s">
         <v>89</v>
       </c>
+      <c r="C42" t="s">
+        <v>59</v>
+      </c>
       <c r="G42" s="1" t="s">
         <v>88</v>
       </c>
@@ -6938,6 +7061,9 @@
       <c r="B43" t="s">
         <v>89</v>
       </c>
+      <c r="C43" t="s">
+        <v>59</v>
+      </c>
       <c r="G43" s="1" t="s">
         <v>88</v>
       </c>
@@ -6965,6 +7091,9 @@
       <c r="B44" t="s">
         <v>89</v>
       </c>
+      <c r="C44" t="s">
+        <v>59</v>
+      </c>
       <c r="G44" s="1" t="s">
         <v>88</v>
       </c>
@@ -6992,6 +7121,9 @@
       <c r="B45" t="s">
         <v>89</v>
       </c>
+      <c r="C45" t="s">
+        <v>59</v>
+      </c>
       <c r="G45" s="1" t="s">
         <v>88</v>
       </c>
@@ -7019,6 +7151,9 @@
       <c r="B46" t="s">
         <v>89</v>
       </c>
+      <c r="C46" t="s">
+        <v>59</v>
+      </c>
       <c r="G46" s="1" t="s">
         <v>88</v>
       </c>
@@ -7046,6 +7181,9 @@
       <c r="B47" t="s">
         <v>89</v>
       </c>
+      <c r="C47" t="s">
+        <v>60</v>
+      </c>
       <c r="G47" s="1" t="s">
         <v>88</v>
       </c>
@@ -7073,6 +7211,9 @@
       <c r="B48" t="s">
         <v>89</v>
       </c>
+      <c r="C48" t="s">
+        <v>60</v>
+      </c>
       <c r="G48" s="1" t="s">
         <v>88</v>
       </c>
@@ -7100,6 +7241,9 @@
       <c r="B49" t="s">
         <v>89</v>
       </c>
+      <c r="C49" t="s">
+        <v>60</v>
+      </c>
       <c r="G49" s="1" t="s">
         <v>88</v>
       </c>
@@ -7127,6 +7271,9 @@
       <c r="B50" t="s">
         <v>89</v>
       </c>
+      <c r="C50" t="s">
+        <v>60</v>
+      </c>
       <c r="G50" s="1" t="s">
         <v>88</v>
       </c>
@@ -7154,6 +7301,9 @@
       <c r="B51" t="s">
         <v>89</v>
       </c>
+      <c r="C51" t="s">
+        <v>60</v>
+      </c>
       <c r="G51" s="1" t="s">
         <v>88</v>
       </c>
@@ -7181,6 +7331,9 @@
       <c r="B52" t="s">
         <v>89</v>
       </c>
+      <c r="C52" t="s">
+        <v>60</v>
+      </c>
       <c r="G52" s="1" t="s">
         <v>88</v>
       </c>
@@ -7208,6 +7361,9 @@
       <c r="B53" t="s">
         <v>89</v>
       </c>
+      <c r="C53" t="s">
+        <v>60</v>
+      </c>
       <c r="G53" s="1" t="s">
         <v>88</v>
       </c>
@@ -7235,6 +7391,9 @@
       <c r="B54" t="s">
         <v>89</v>
       </c>
+      <c r="C54" t="s">
+        <v>60</v>
+      </c>
       <c r="G54" s="1" t="s">
         <v>88</v>
       </c>
@@ -7262,6 +7421,9 @@
       <c r="B55" t="s">
         <v>89</v>
       </c>
+      <c r="C55" t="s">
+        <v>60</v>
+      </c>
       <c r="G55" s="1" t="s">
         <v>88</v>
       </c>
@@ -7289,6 +7451,9 @@
       <c r="B56" t="s">
         <v>89</v>
       </c>
+      <c r="C56" t="s">
+        <v>60</v>
+      </c>
       <c r="G56" s="1" t="s">
         <v>88</v>
       </c>
@@ -7316,6 +7481,9 @@
       <c r="B57" t="s">
         <v>89</v>
       </c>
+      <c r="C57" t="s">
+        <v>60</v>
+      </c>
       <c r="G57" s="1" t="s">
         <v>88</v>
       </c>
@@ -7343,6 +7511,9 @@
       <c r="B58" t="s">
         <v>89</v>
       </c>
+      <c r="C58" t="s">
+        <v>60</v>
+      </c>
       <c r="G58" s="1" t="s">
         <v>88</v>
       </c>
@@ -7370,6 +7541,9 @@
       <c r="B59" t="s">
         <v>89</v>
       </c>
+      <c r="C59" t="s">
+        <v>60</v>
+      </c>
       <c r="G59" s="1" t="s">
         <v>88</v>
       </c>
@@ -7397,6 +7571,9 @@
       <c r="B60" t="s">
         <v>89</v>
       </c>
+      <c r="C60" t="s">
+        <v>60</v>
+      </c>
       <c r="G60" s="1" t="s">
         <v>88</v>
       </c>
@@ -7424,6 +7601,9 @@
       <c r="B61" t="s">
         <v>89</v>
       </c>
+      <c r="C61" t="s">
+        <v>60</v>
+      </c>
       <c r="G61" s="1" t="s">
         <v>88</v>
       </c>
@@ -7451,6 +7631,9 @@
       <c r="B62" t="s">
         <v>90</v>
       </c>
+      <c r="C62" t="s">
+        <v>59</v>
+      </c>
       <c r="G62" s="1" t="s">
         <v>88</v>
       </c>
@@ -7478,6 +7661,9 @@
       <c r="B63" t="s">
         <v>90</v>
       </c>
+      <c r="C63" t="s">
+        <v>59</v>
+      </c>
       <c r="G63" s="1" t="s">
         <v>88</v>
       </c>
@@ -7505,6 +7691,9 @@
       <c r="B64" t="s">
         <v>90</v>
       </c>
+      <c r="C64" t="s">
+        <v>59</v>
+      </c>
       <c r="G64" s="1" t="s">
         <v>88</v>
       </c>
@@ -7532,6 +7721,9 @@
       <c r="B65" t="s">
         <v>90</v>
       </c>
+      <c r="C65" t="s">
+        <v>59</v>
+      </c>
       <c r="G65" s="1" t="s">
         <v>88</v>
       </c>
@@ -7559,6 +7751,9 @@
       <c r="B66" t="s">
         <v>90</v>
       </c>
+      <c r="C66" t="s">
+        <v>59</v>
+      </c>
       <c r="G66" s="1" t="s">
         <v>88</v>
       </c>
@@ -7586,6 +7781,9 @@
       <c r="B67" t="s">
         <v>90</v>
       </c>
+      <c r="C67" t="s">
+        <v>59</v>
+      </c>
       <c r="G67" s="1" t="s">
         <v>88</v>
       </c>
@@ -7613,6 +7811,9 @@
       <c r="B68" t="s">
         <v>90</v>
       </c>
+      <c r="C68" t="s">
+        <v>59</v>
+      </c>
       <c r="G68" s="1" t="s">
         <v>88</v>
       </c>
@@ -7640,6 +7841,9 @@
       <c r="B69" t="s">
         <v>90</v>
       </c>
+      <c r="C69" t="s">
+        <v>59</v>
+      </c>
       <c r="G69" s="1" t="s">
         <v>88</v>
       </c>
@@ -7667,6 +7871,9 @@
       <c r="B70" t="s">
         <v>90</v>
       </c>
+      <c r="C70" t="s">
+        <v>59</v>
+      </c>
       <c r="G70" s="1" t="s">
         <v>88</v>
       </c>
@@ -7694,6 +7901,9 @@
       <c r="B71" t="s">
         <v>90</v>
       </c>
+      <c r="C71" t="s">
+        <v>59</v>
+      </c>
       <c r="G71" s="1" t="s">
         <v>88</v>
       </c>
@@ -7721,6 +7931,9 @@
       <c r="B72" t="s">
         <v>90</v>
       </c>
+      <c r="C72" t="s">
+        <v>59</v>
+      </c>
       <c r="G72" s="1" t="s">
         <v>88</v>
       </c>
@@ -7748,6 +7961,9 @@
       <c r="B73" t="s">
         <v>90</v>
       </c>
+      <c r="C73" t="s">
+        <v>59</v>
+      </c>
       <c r="G73" s="1" t="s">
         <v>88</v>
       </c>
@@ -7775,6 +7991,9 @@
       <c r="B74" t="s">
         <v>90</v>
       </c>
+      <c r="C74" t="s">
+        <v>59</v>
+      </c>
       <c r="G74" s="1" t="s">
         <v>88</v>
       </c>
@@ -7802,6 +8021,9 @@
       <c r="B75" t="s">
         <v>90</v>
       </c>
+      <c r="C75" t="s">
+        <v>59</v>
+      </c>
       <c r="G75" s="1" t="s">
         <v>88</v>
       </c>
@@ -7829,6 +8051,9 @@
       <c r="B76" t="s">
         <v>90</v>
       </c>
+      <c r="C76" t="s">
+        <v>59</v>
+      </c>
       <c r="G76" s="1" t="s">
         <v>88</v>
       </c>
@@ -7856,6 +8081,9 @@
       <c r="B77" t="s">
         <v>90</v>
       </c>
+      <c r="C77" t="s">
+        <v>60</v>
+      </c>
       <c r="G77" s="1" t="s">
         <v>88</v>
       </c>
@@ -7883,6 +8111,9 @@
       <c r="B78" t="s">
         <v>90</v>
       </c>
+      <c r="C78" t="s">
+        <v>60</v>
+      </c>
       <c r="G78" s="1" t="s">
         <v>88</v>
       </c>
@@ -7910,6 +8141,9 @@
       <c r="B79" t="s">
         <v>90</v>
       </c>
+      <c r="C79" t="s">
+        <v>60</v>
+      </c>
       <c r="G79" s="1" t="s">
         <v>88</v>
       </c>
@@ -7937,6 +8171,9 @@
       <c r="B80" t="s">
         <v>90</v>
       </c>
+      <c r="C80" t="s">
+        <v>60</v>
+      </c>
       <c r="G80" s="1" t="s">
         <v>88</v>
       </c>
@@ -7964,6 +8201,9 @@
       <c r="B81" t="s">
         <v>90</v>
       </c>
+      <c r="C81" t="s">
+        <v>60</v>
+      </c>
       <c r="G81" s="1" t="s">
         <v>88</v>
       </c>
@@ -7991,6 +8231,9 @@
       <c r="B82" t="s">
         <v>90</v>
       </c>
+      <c r="C82" t="s">
+        <v>60</v>
+      </c>
       <c r="G82" s="1" t="s">
         <v>88</v>
       </c>
@@ -8018,6 +8261,9 @@
       <c r="B83" t="s">
         <v>90</v>
       </c>
+      <c r="C83" t="s">
+        <v>60</v>
+      </c>
       <c r="G83" s="1" t="s">
         <v>88</v>
       </c>
@@ -8045,6 +8291,9 @@
       <c r="B84" t="s">
         <v>90</v>
       </c>
+      <c r="C84" t="s">
+        <v>60</v>
+      </c>
       <c r="G84" s="1" t="s">
         <v>88</v>
       </c>
@@ -8072,6 +8321,9 @@
       <c r="B85" t="s">
         <v>90</v>
       </c>
+      <c r="C85" t="s">
+        <v>60</v>
+      </c>
       <c r="G85" s="1" t="s">
         <v>88</v>
       </c>
@@ -8099,6 +8351,9 @@
       <c r="B86" t="s">
         <v>90</v>
       </c>
+      <c r="C86" t="s">
+        <v>60</v>
+      </c>
       <c r="G86" s="1" t="s">
         <v>88</v>
       </c>
@@ -8126,6 +8381,9 @@
       <c r="B87" t="s">
         <v>90</v>
       </c>
+      <c r="C87" t="s">
+        <v>60</v>
+      </c>
       <c r="G87" s="1" t="s">
         <v>88</v>
       </c>
@@ -8153,6 +8411,9 @@
       <c r="B88" t="s">
         <v>90</v>
       </c>
+      <c r="C88" t="s">
+        <v>60</v>
+      </c>
       <c r="G88" s="1" t="s">
         <v>88</v>
       </c>
@@ -8180,6 +8441,9 @@
       <c r="B89" t="s">
         <v>90</v>
       </c>
+      <c r="C89" t="s">
+        <v>60</v>
+      </c>
       <c r="G89" s="1" t="s">
         <v>88</v>
       </c>
@@ -8207,6 +8471,9 @@
       <c r="B90" t="s">
         <v>90</v>
       </c>
+      <c r="C90" t="s">
+        <v>60</v>
+      </c>
       <c r="G90" s="1" t="s">
         <v>88</v>
       </c>
@@ -8233,6 +8500,9 @@
       </c>
       <c r="B91" t="s">
         <v>90</v>
+      </c>
+      <c r="C91" t="s">
+        <v>60</v>
       </c>
       <c r="G91" s="1" t="s">
         <v>88</v>

</xml_diff>

<commit_message>
updating data sheet cohort 11 day 10 weights
cohort 11 2018-08-26
</commit_message>
<xml_diff>
--- a/Data/2018-08-14_master_datac_2018_collection_year.xlsx
+++ b/Data/2018-08-14_master_datac_2018_collection_year.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andrew.nguyen\Desktop\Circadian_rhythm_runs_seasonal_timing\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CAAA300-08CC-40DA-B88C-784CF8C3A8C4}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2F9F750-C883-4DDD-9042-6D1A38039169}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1800" yWindow="1935" windowWidth="35820" windowHeight="18720" activeTab="1" xr2:uid="{C7477166-8A7C-B04A-9643-C277FEDCDAAB}"/>
+    <workbookView xWindow="1800" yWindow="1935" windowWidth="35820" windowHeight="18720" xr2:uid="{C7477166-8A7C-B04A-9643-C277FEDCDAAB}"/>
   </bookViews>
   <sheets>
     <sheet name="Maggot_Collections" sheetId="2" r:id="rId1"/>
     <sheet name="Data_collect" sheetId="1" r:id="rId2"/>
+    <sheet name="Pupal_Splits" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="179021"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1590" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2180" uniqueCount="237">
   <si>
     <t>Ind_ID</t>
   </si>
@@ -697,6 +698,51 @@
   </si>
   <si>
     <t>2018-09-24</t>
+  </si>
+  <si>
+    <t>Cohort_day</t>
+  </si>
+  <si>
+    <t>Collection_date</t>
+  </si>
+  <si>
+    <t>Cohort_date</t>
+  </si>
+  <si>
+    <t>Site_Name</t>
+  </si>
+  <si>
+    <t>Hinal</t>
+  </si>
+  <si>
+    <t>Andrew</t>
+  </si>
+  <si>
+    <t>2018-08-21</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>2018-08-26</t>
+  </si>
+  <si>
+    <t>white</t>
+  </si>
+  <si>
+    <t>blue</t>
+  </si>
+  <si>
+    <t>blank</t>
+  </si>
+  <si>
+    <t>16:49</t>
+  </si>
+  <si>
+    <t>17:04</t>
+  </si>
+  <si>
+    <t>16:37</t>
   </si>
 </sst>
 </file>
@@ -716,7 +762,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -741,6 +787,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -754,7 +812,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -785,6 +843,10 @@
     <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1101,8 +1163,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D3F78F5-4EA8-6A42-B216-41A8EC7A5E8D}">
   <dimension ref="A1:Z102"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="H65" sqref="H65"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1352,10 +1414,10 @@
       <c r="K6" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="L6" s="1" t="s">
+      <c r="L6" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="M6" s="1" t="s">
+      <c r="M6" s="19" t="s">
         <v>68</v>
       </c>
       <c r="N6" s="1" t="s">
@@ -1404,10 +1466,10 @@
       <c r="K7" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="L7" s="1" t="s">
+      <c r="L7" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="M7" s="1" t="s">
+      <c r="M7" s="19" t="s">
         <v>68</v>
       </c>
       <c r="N7" s="1" t="s">
@@ -1456,10 +1518,10 @@
       <c r="K8" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="L8" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="M8" s="1" t="s">
+      <c r="L8" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="M8" s="19" t="s">
         <v>69</v>
       </c>
       <c r="N8" s="1" t="s">
@@ -1508,10 +1570,10 @@
       <c r="K9" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="L9" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="M9" s="1" t="s">
+      <c r="L9" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="M9" s="19" t="s">
         <v>69</v>
       </c>
       <c r="N9" s="1" t="s">
@@ -1560,10 +1622,10 @@
       <c r="K10" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="L10" s="13" t="s">
+      <c r="L10" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="M10" s="13" t="s">
+      <c r="M10" s="19" t="s">
         <v>70</v>
       </c>
       <c r="N10" s="13" t="s">
@@ -1612,10 +1674,10 @@
       <c r="K11" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="L11" s="13" t="s">
+      <c r="L11" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="M11" s="13" t="s">
+      <c r="M11" s="19" t="s">
         <v>70</v>
       </c>
       <c r="N11" s="13" t="s">
@@ -1664,10 +1726,10 @@
       <c r="K12" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="L12" s="1" t="s">
+      <c r="L12" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="M12" s="1" t="s">
+      <c r="M12" s="19" t="s">
         <v>71</v>
       </c>
       <c r="N12" s="1" t="s">
@@ -1716,10 +1778,10 @@
       <c r="K13" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="L13" s="1" t="s">
+      <c r="L13" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="M13" s="1" t="s">
+      <c r="M13" s="19" t="s">
         <v>71</v>
       </c>
       <c r="N13" s="1" t="s">
@@ -1768,10 +1830,10 @@
       <c r="K14" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="L14" s="13" t="s">
+      <c r="L14" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="M14" s="13" t="s">
+      <c r="M14" s="19" t="s">
         <v>72</v>
       </c>
       <c r="N14" s="13" t="s">
@@ -1820,10 +1882,10 @@
       <c r="K15" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="L15" s="13" t="s">
+      <c r="L15" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="M15" s="13" t="s">
+      <c r="M15" s="19" t="s">
         <v>72</v>
       </c>
       <c r="N15" s="13" t="s">
@@ -1872,10 +1934,10 @@
       <c r="K16" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="L16" s="13" t="s">
+      <c r="L16" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="M16" s="13" t="s">
+      <c r="M16" s="19" t="s">
         <v>72</v>
       </c>
       <c r="N16" s="13" t="s">
@@ -1890,161 +1952,161 @@
       <c r="S16" s="13"/>
       <c r="T16" s="13"/>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="17" spans="1:20" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="B17" t="s">
-        <v>59</v>
-      </c>
-      <c r="C17" t="s">
-        <v>61</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="E17">
+      <c r="B17" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="D17" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="E17" s="16">
         <v>11</v>
       </c>
-      <c r="F17" s="10">
+      <c r="F17" s="18">
         <v>43338</v>
       </c>
-      <c r="G17">
+      <c r="G17" s="16">
         <v>1</v>
       </c>
-      <c r="H17" s="1" t="s">
+      <c r="H17" s="17" t="s">
         <v>189</v>
       </c>
-      <c r="I17">
+      <c r="I17" s="16">
         <v>313</v>
       </c>
-      <c r="J17" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="K17" s="1" t="s">
+      <c r="J17" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="K17" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="L17" s="1" t="s">
+      <c r="L17" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="M17" s="1" t="s">
+      <c r="M17" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="N17" s="1" t="s">
+      <c r="N17" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="O17" s="1" t="s">
+      <c r="O17" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="P17" s="1"/>
-      <c r="Q17" s="1"/>
-      <c r="R17" s="1"/>
-      <c r="S17" s="1"/>
-      <c r="T17" s="1"/>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="P17" s="17"/>
+      <c r="Q17" s="17"/>
+      <c r="R17" s="17"/>
+      <c r="S17" s="17"/>
+      <c r="T17" s="17"/>
+    </row>
+    <row r="18" spans="1:20" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="B18" t="s">
-        <v>59</v>
-      </c>
-      <c r="C18" t="s">
-        <v>61</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="E18">
+      <c r="B18" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="D18" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="E18" s="16">
         <v>11</v>
       </c>
-      <c r="F18" s="10">
+      <c r="F18" s="18">
         <v>43338</v>
       </c>
-      <c r="G18">
+      <c r="G18" s="16">
         <v>2</v>
       </c>
-      <c r="H18" s="1" t="s">
+      <c r="H18" s="17" t="s">
         <v>189</v>
       </c>
-      <c r="I18">
+      <c r="I18" s="16">
         <v>129</v>
       </c>
-      <c r="J18" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="K18" s="1" t="s">
+      <c r="J18" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="K18" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="L18" s="1" t="s">
+      <c r="L18" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="M18" s="1" t="s">
+      <c r="M18" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="N18" s="1" t="s">
+      <c r="N18" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="O18" s="1" t="s">
+      <c r="O18" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="P18" s="1"/>
-      <c r="Q18" s="1"/>
-      <c r="R18" s="1"/>
-      <c r="S18" s="1"/>
-      <c r="T18" s="1"/>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="P18" s="17"/>
+      <c r="Q18" s="17"/>
+      <c r="R18" s="17"/>
+      <c r="S18" s="17"/>
+      <c r="T18" s="17"/>
+    </row>
+    <row r="19" spans="1:20" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="C19" t="s">
-        <v>61</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="E19">
+      <c r="C19" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="D19" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="E19" s="16">
         <v>11</v>
       </c>
-      <c r="F19" s="10">
+      <c r="F19" s="18">
         <v>43338</v>
       </c>
-      <c r="G19">
+      <c r="G19" s="16">
         <v>1</v>
       </c>
-      <c r="H19" s="1" t="s">
+      <c r="H19" s="17" t="s">
         <v>189</v>
       </c>
-      <c r="I19">
+      <c r="I19" s="16">
         <v>165</v>
       </c>
-      <c r="J19" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="K19" s="1" t="s">
+      <c r="J19" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="K19" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="L19" s="1" t="s">
+      <c r="L19" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="M19" s="1" t="s">
+      <c r="M19" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="N19" s="1" t="s">
+      <c r="N19" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="O19" s="1" t="s">
+      <c r="O19" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="P19" s="1"/>
-      <c r="Q19" s="1"/>
-      <c r="R19" s="1"/>
-      <c r="S19" s="1"/>
-      <c r="T19" s="1"/>
+      <c r="P19" s="17"/>
+      <c r="Q19" s="17"/>
+      <c r="R19" s="17"/>
+      <c r="S19" s="17"/>
+      <c r="T19" s="17"/>
     </row>
     <row r="20" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
@@ -5885,15 +5947,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92725FB9-1A17-2546-9DFA-6C0D39437891}">
-  <dimension ref="A1:AS91"/>
+  <dimension ref="A1:AS185"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
-      <selection activeCell="C77" sqref="C77"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D184" sqref="D184"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="5" max="5" width="11" style="1"/>
     <col min="7" max="7" width="13.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="11" style="1"/>
     <col min="20" max="20" width="15.375" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5910,7 +5975,7 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F1" t="s">
@@ -8507,6 +8572,9 @@
       <c r="G91" s="1" t="s">
         <v>88</v>
       </c>
+      <c r="J91">
+        <v>6</v>
+      </c>
       <c r="K91" t="s">
         <v>61</v>
       </c>
@@ -8522,6 +8590,3021 @@
       </c>
       <c r="AC91" t="s">
         <v>180</v>
+      </c>
+    </row>
+    <row r="92" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>1</v>
+      </c>
+      <c r="B92" t="s">
+        <v>231</v>
+      </c>
+      <c r="C92" t="s">
+        <v>59</v>
+      </c>
+      <c r="D92">
+        <v>9.9659999999999993</v>
+      </c>
+      <c r="E92" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="G92" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H92" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I92" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="J92">
+        <v>11</v>
+      </c>
+      <c r="K92" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="93" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>2</v>
+      </c>
+      <c r="B93" t="s">
+        <v>231</v>
+      </c>
+      <c r="C93" t="s">
+        <v>59</v>
+      </c>
+      <c r="D93">
+        <v>9.9120000000000008</v>
+      </c>
+      <c r="G93" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H93" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I93" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="J93">
+        <v>11</v>
+      </c>
+      <c r="K93" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="94" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>3</v>
+      </c>
+      <c r="B94" t="s">
+        <v>231</v>
+      </c>
+      <c r="C94" t="s">
+        <v>59</v>
+      </c>
+      <c r="D94">
+        <v>6.5419999999999998</v>
+      </c>
+      <c r="G94" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H94" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I94" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="J94">
+        <v>11</v>
+      </c>
+      <c r="K94" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="95" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>4</v>
+      </c>
+      <c r="B95" t="s">
+        <v>231</v>
+      </c>
+      <c r="C95" t="s">
+        <v>60</v>
+      </c>
+      <c r="D95">
+        <v>9.1750000000000007</v>
+      </c>
+      <c r="G95" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H95" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I95" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="J95">
+        <v>11</v>
+      </c>
+      <c r="K95" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="96" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>5</v>
+      </c>
+      <c r="B96" t="s">
+        <v>231</v>
+      </c>
+      <c r="C96" t="s">
+        <v>60</v>
+      </c>
+      <c r="D96">
+        <v>6.3680000000000003</v>
+      </c>
+      <c r="G96" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H96" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I96" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="J96">
+        <v>11</v>
+      </c>
+      <c r="K96" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>6</v>
+      </c>
+      <c r="B97" t="s">
+        <v>231</v>
+      </c>
+      <c r="C97" t="s">
+        <v>59</v>
+      </c>
+      <c r="D97">
+        <v>11.004</v>
+      </c>
+      <c r="G97" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H97" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I97" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="J97">
+        <v>11</v>
+      </c>
+      <c r="K97" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>7</v>
+      </c>
+      <c r="B98" t="s">
+        <v>231</v>
+      </c>
+      <c r="C98" t="s">
+        <v>59</v>
+      </c>
+      <c r="D98">
+        <v>7.3</v>
+      </c>
+      <c r="G98" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H98" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I98" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="J98">
+        <v>11</v>
+      </c>
+      <c r="K98" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>8</v>
+      </c>
+      <c r="B99" t="s">
+        <v>231</v>
+      </c>
+      <c r="C99" t="s">
+        <v>60</v>
+      </c>
+      <c r="D99">
+        <v>10.097</v>
+      </c>
+      <c r="G99" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H99" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I99" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="J99">
+        <v>11</v>
+      </c>
+      <c r="K99" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>9</v>
+      </c>
+      <c r="B100" t="s">
+        <v>231</v>
+      </c>
+      <c r="C100" t="s">
+        <v>60</v>
+      </c>
+      <c r="D100">
+        <v>8.2029999999999994</v>
+      </c>
+      <c r="G100" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H100" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I100" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="J100">
+        <v>11</v>
+      </c>
+      <c r="K100" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>10</v>
+      </c>
+      <c r="B101" t="s">
+        <v>231</v>
+      </c>
+      <c r="C101" t="s">
+        <v>60</v>
+      </c>
+      <c r="D101">
+        <v>9.5419999999999998</v>
+      </c>
+      <c r="G101" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H101" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I101" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="J101">
+        <v>11</v>
+      </c>
+      <c r="K101" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A102">
+        <v>11</v>
+      </c>
+      <c r="B102" t="s">
+        <v>231</v>
+      </c>
+      <c r="C102" t="s">
+        <v>59</v>
+      </c>
+      <c r="D102">
+        <v>7.2389999999999999</v>
+      </c>
+      <c r="G102" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H102" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I102" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="J102">
+        <v>11</v>
+      </c>
+      <c r="K102" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A103">
+        <v>12</v>
+      </c>
+      <c r="B103" t="s">
+        <v>231</v>
+      </c>
+      <c r="C103" t="s">
+        <v>59</v>
+      </c>
+      <c r="D103">
+        <v>11.362</v>
+      </c>
+      <c r="G103" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H103" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I103" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="J103">
+        <v>11</v>
+      </c>
+      <c r="K103" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A104">
+        <v>13</v>
+      </c>
+      <c r="B104" t="s">
+        <v>231</v>
+      </c>
+      <c r="C104" t="s">
+        <v>60</v>
+      </c>
+      <c r="D104">
+        <v>6.62</v>
+      </c>
+      <c r="G104" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H104" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I104" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="J104">
+        <v>11</v>
+      </c>
+      <c r="K104" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A105">
+        <v>14</v>
+      </c>
+      <c r="B105" t="s">
+        <v>231</v>
+      </c>
+      <c r="C105" t="s">
+        <v>60</v>
+      </c>
+      <c r="D105">
+        <v>6.4130000000000003</v>
+      </c>
+      <c r="G105" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H105" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I105" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="J105">
+        <v>11</v>
+      </c>
+      <c r="K105" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A106">
+        <v>15</v>
+      </c>
+      <c r="B106" t="s">
+        <v>231</v>
+      </c>
+      <c r="C106" t="s">
+        <v>59</v>
+      </c>
+      <c r="D106">
+        <v>4.7149999999999999</v>
+      </c>
+      <c r="G106" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H106" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I106" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="J106">
+        <v>11</v>
+      </c>
+      <c r="K106" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A107">
+        <v>16</v>
+      </c>
+      <c r="B107" t="s">
+        <v>231</v>
+      </c>
+      <c r="C107" t="s">
+        <v>60</v>
+      </c>
+      <c r="D107">
+        <v>11</v>
+      </c>
+      <c r="G107" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H107" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I107" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="J107">
+        <v>11</v>
+      </c>
+      <c r="K107" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A108">
+        <v>17</v>
+      </c>
+      <c r="B108" t="s">
+        <v>231</v>
+      </c>
+      <c r="C108" t="s">
+        <v>59</v>
+      </c>
+      <c r="D108">
+        <v>12.013</v>
+      </c>
+      <c r="G108" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H108" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I108" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="J108">
+        <v>11</v>
+      </c>
+      <c r="K108" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A109">
+        <v>18</v>
+      </c>
+      <c r="B109" t="s">
+        <v>231</v>
+      </c>
+      <c r="C109" t="s">
+        <v>60</v>
+      </c>
+      <c r="D109">
+        <v>8.2040000000000006</v>
+      </c>
+      <c r="G109" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H109" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I109" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="J109">
+        <v>11</v>
+      </c>
+      <c r="K109" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A110">
+        <v>19</v>
+      </c>
+      <c r="B110" t="s">
+        <v>231</v>
+      </c>
+      <c r="C110" t="s">
+        <v>60</v>
+      </c>
+      <c r="D110">
+        <v>6.7530000000000001</v>
+      </c>
+      <c r="G110" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H110" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I110" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="J110">
+        <v>11</v>
+      </c>
+      <c r="K110" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A111">
+        <v>20</v>
+      </c>
+      <c r="B111" t="s">
+        <v>231</v>
+      </c>
+      <c r="C111" t="s">
+        <v>59</v>
+      </c>
+      <c r="D111">
+        <v>6.2270000000000003</v>
+      </c>
+      <c r="G111" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H111" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I111" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="J111">
+        <v>11</v>
+      </c>
+      <c r="K111" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A112">
+        <v>21</v>
+      </c>
+      <c r="B112" t="s">
+        <v>231</v>
+      </c>
+      <c r="C112" t="s">
+        <v>59</v>
+      </c>
+      <c r="D112">
+        <v>5.76</v>
+      </c>
+      <c r="G112" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H112" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I112" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="J112">
+        <v>11</v>
+      </c>
+      <c r="K112" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A113">
+        <v>22</v>
+      </c>
+      <c r="B113" t="s">
+        <v>231</v>
+      </c>
+      <c r="C113" t="s">
+        <v>59</v>
+      </c>
+      <c r="D113">
+        <v>5.7779999999999996</v>
+      </c>
+      <c r="G113" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H113" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I113" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="J113">
+        <v>11</v>
+      </c>
+      <c r="K113" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A114">
+        <v>23</v>
+      </c>
+      <c r="B114" t="s">
+        <v>231</v>
+      </c>
+      <c r="C114" t="s">
+        <v>60</v>
+      </c>
+      <c r="D114">
+        <v>5.8529999999999998</v>
+      </c>
+      <c r="G114" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H114" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I114" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="J114">
+        <v>11</v>
+      </c>
+      <c r="K114" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A115">
+        <v>24</v>
+      </c>
+      <c r="B115" t="s">
+        <v>231</v>
+      </c>
+      <c r="C115" t="s">
+        <v>59</v>
+      </c>
+      <c r="D115">
+        <v>9.7059999999999995</v>
+      </c>
+      <c r="G115" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H115" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I115" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="J115">
+        <v>11</v>
+      </c>
+      <c r="K115" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A116">
+        <v>25</v>
+      </c>
+      <c r="B116" t="s">
+        <v>231</v>
+      </c>
+      <c r="C116" t="s">
+        <v>60</v>
+      </c>
+      <c r="D116">
+        <v>9.57</v>
+      </c>
+      <c r="G116" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H116" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I116" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="J116">
+        <v>11</v>
+      </c>
+      <c r="K116" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A117">
+        <v>26</v>
+      </c>
+      <c r="B117" t="s">
+        <v>231</v>
+      </c>
+      <c r="C117" t="s">
+        <v>60</v>
+      </c>
+      <c r="D117">
+        <v>7.0039999999999996</v>
+      </c>
+      <c r="G117" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H117" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I117" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="J117">
+        <v>11</v>
+      </c>
+      <c r="K117" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A118">
+        <v>27</v>
+      </c>
+      <c r="B118" t="s">
+        <v>231</v>
+      </c>
+      <c r="C118" t="s">
+        <v>60</v>
+      </c>
+      <c r="D118">
+        <v>6.43</v>
+      </c>
+      <c r="G118" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H118" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I118" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="J118">
+        <v>11</v>
+      </c>
+      <c r="K118" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A119">
+        <v>28</v>
+      </c>
+      <c r="B119" t="s">
+        <v>231</v>
+      </c>
+      <c r="C119" t="s">
+        <v>59</v>
+      </c>
+      <c r="D119">
+        <v>10.427</v>
+      </c>
+      <c r="G119" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H119" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I119" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="J119">
+        <v>11</v>
+      </c>
+      <c r="K119" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A120">
+        <v>29</v>
+      </c>
+      <c r="B120" t="s">
+        <v>231</v>
+      </c>
+      <c r="C120" t="s">
+        <v>60</v>
+      </c>
+      <c r="D120">
+        <v>8.0690000000000008</v>
+      </c>
+      <c r="G120" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H120" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I120" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="J120">
+        <v>11</v>
+      </c>
+      <c r="K120" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A121">
+        <v>30</v>
+      </c>
+      <c r="B121" t="s">
+        <v>231</v>
+      </c>
+      <c r="C121" t="s">
+        <v>59</v>
+      </c>
+      <c r="D121">
+        <v>6.6520000000000001</v>
+      </c>
+      <c r="G121" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H121" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I121" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="J121">
+        <v>11</v>
+      </c>
+      <c r="K121" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A122">
+        <v>31</v>
+      </c>
+      <c r="B122" t="s">
+        <v>231</v>
+      </c>
+      <c r="C122" t="s">
+        <v>60</v>
+      </c>
+      <c r="D122">
+        <v>7.7389999999999999</v>
+      </c>
+      <c r="G122" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H122" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I122" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="J122">
+        <v>11</v>
+      </c>
+      <c r="K122" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A123">
+        <v>32</v>
+      </c>
+      <c r="B123" t="s">
+        <v>231</v>
+      </c>
+      <c r="C123" t="s">
+        <v>59</v>
+      </c>
+      <c r="D123">
+        <v>7.1740000000000004</v>
+      </c>
+      <c r="G123" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H123" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I123" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="J123">
+        <v>11</v>
+      </c>
+      <c r="K123" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A124">
+        <v>33</v>
+      </c>
+      <c r="B124" t="s">
+        <v>231</v>
+      </c>
+      <c r="C124" t="s">
+        <v>59</v>
+      </c>
+      <c r="D124">
+        <v>8.4019999999999992</v>
+      </c>
+      <c r="G124" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H124" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I124" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="J124">
+        <v>11</v>
+      </c>
+      <c r="K124" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A125">
+        <v>34</v>
+      </c>
+      <c r="B125" t="s">
+        <v>231</v>
+      </c>
+      <c r="C125" t="s">
+        <v>60</v>
+      </c>
+      <c r="D125">
+        <v>6.335</v>
+      </c>
+      <c r="G125" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H125" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I125" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="J125">
+        <v>11</v>
+      </c>
+      <c r="K125" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A126">
+        <v>35</v>
+      </c>
+      <c r="B126" t="s">
+        <v>231</v>
+      </c>
+      <c r="C126" t="s">
+        <v>59</v>
+      </c>
+      <c r="D126">
+        <v>7.6909999999999998</v>
+      </c>
+      <c r="G126" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H126" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I126" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="J126">
+        <v>11</v>
+      </c>
+      <c r="K126" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A127">
+        <v>36</v>
+      </c>
+      <c r="B127" t="s">
+        <v>231</v>
+      </c>
+      <c r="C127" t="s">
+        <v>60</v>
+      </c>
+      <c r="D127">
+        <v>6.8559999999999999</v>
+      </c>
+      <c r="G127" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H127" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I127" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="J127">
+        <v>11</v>
+      </c>
+      <c r="K127" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A128">
+        <v>37</v>
+      </c>
+      <c r="B128" t="s">
+        <v>231</v>
+      </c>
+      <c r="C128" t="s">
+        <v>59</v>
+      </c>
+      <c r="D128">
+        <v>9.6440000000000001</v>
+      </c>
+      <c r="G128" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H128" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I128" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="J128">
+        <v>11</v>
+      </c>
+      <c r="K128" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A129">
+        <v>38</v>
+      </c>
+      <c r="B129" t="s">
+        <v>231</v>
+      </c>
+      <c r="C129" t="s">
+        <v>59</v>
+      </c>
+      <c r="D129">
+        <v>10.042999999999999</v>
+      </c>
+      <c r="G129" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H129" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I129" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="J129">
+        <v>11</v>
+      </c>
+      <c r="K129" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A130">
+        <v>39</v>
+      </c>
+      <c r="B130" t="s">
+        <v>231</v>
+      </c>
+      <c r="C130" t="s">
+        <v>60</v>
+      </c>
+      <c r="D130">
+        <v>4.0110000000000001</v>
+      </c>
+      <c r="G130" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H130" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I130" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="J130">
+        <v>11</v>
+      </c>
+      <c r="K130" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A131">
+        <v>40</v>
+      </c>
+      <c r="B131" t="s">
+        <v>231</v>
+      </c>
+      <c r="C131" t="s">
+        <v>60</v>
+      </c>
+      <c r="D131">
+        <v>5.2640000000000002</v>
+      </c>
+      <c r="G131" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H131" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I131" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="J131">
+        <v>11</v>
+      </c>
+      <c r="K131" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A132">
+        <v>41</v>
+      </c>
+      <c r="B132" t="s">
+        <v>231</v>
+      </c>
+      <c r="C132" t="s">
+        <v>60</v>
+      </c>
+      <c r="D132">
+        <v>4.7290000000000001</v>
+      </c>
+      <c r="G132" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H132" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I132" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="J132">
+        <v>11</v>
+      </c>
+      <c r="K132" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A133">
+        <v>42</v>
+      </c>
+      <c r="B133" t="s">
+        <v>231</v>
+      </c>
+      <c r="C133" t="s">
+        <v>59</v>
+      </c>
+      <c r="D133">
+        <v>10.238</v>
+      </c>
+      <c r="G133" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H133" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I133" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="J133">
+        <v>11</v>
+      </c>
+      <c r="K133" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A134">
+        <v>43</v>
+      </c>
+      <c r="B134" t="s">
+        <v>231</v>
+      </c>
+      <c r="C134" t="s">
+        <v>60</v>
+      </c>
+      <c r="D134">
+        <v>10.393000000000001</v>
+      </c>
+      <c r="G134" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H134" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I134" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="J134">
+        <v>11</v>
+      </c>
+      <c r="K134" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A135">
+        <v>44</v>
+      </c>
+      <c r="B135" t="s">
+        <v>231</v>
+      </c>
+      <c r="C135" t="s">
+        <v>59</v>
+      </c>
+      <c r="D135">
+        <v>7.2569999999999997</v>
+      </c>
+      <c r="G135" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H135" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I135" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="J135">
+        <v>11</v>
+      </c>
+      <c r="K135" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="136" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A136">
+        <v>45</v>
+      </c>
+      <c r="B136" t="s">
+        <v>231</v>
+      </c>
+      <c r="C136" t="s">
+        <v>60</v>
+      </c>
+      <c r="D136">
+        <v>7.4619999999999997</v>
+      </c>
+      <c r="G136" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H136" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I136" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="J136">
+        <v>11</v>
+      </c>
+      <c r="K136" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="137" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A137">
+        <v>46</v>
+      </c>
+      <c r="B137" t="s">
+        <v>231</v>
+      </c>
+      <c r="C137" t="s">
+        <v>233</v>
+      </c>
+      <c r="G137" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H137" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I137" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="J137">
+        <v>11</v>
+      </c>
+      <c r="K137" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A138">
+        <v>47</v>
+      </c>
+      <c r="B138" t="s">
+        <v>231</v>
+      </c>
+      <c r="C138" t="s">
+        <v>233</v>
+      </c>
+      <c r="E138" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="G138" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H138" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I138" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="J138">
+        <v>11</v>
+      </c>
+      <c r="K138" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="139" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A139">
+        <v>1</v>
+      </c>
+      <c r="B139" t="s">
+        <v>232</v>
+      </c>
+      <c r="C139" t="s">
+        <v>59</v>
+      </c>
+      <c r="D139">
+        <v>6.4989999999999997</v>
+      </c>
+      <c r="E139" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="G139" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H139" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I139" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="J139">
+        <v>11</v>
+      </c>
+      <c r="K139" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="140" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A140">
+        <v>2</v>
+      </c>
+      <c r="B140" t="s">
+        <v>232</v>
+      </c>
+      <c r="C140" t="s">
+        <v>60</v>
+      </c>
+      <c r="D140">
+        <v>8.8190000000000008</v>
+      </c>
+      <c r="G140" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H140" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I140" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="J140">
+        <v>11</v>
+      </c>
+      <c r="K140" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="141" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A141">
+        <v>3</v>
+      </c>
+      <c r="B141" t="s">
+        <v>232</v>
+      </c>
+      <c r="C141" t="s">
+        <v>59</v>
+      </c>
+      <c r="D141">
+        <v>8.1460000000000008</v>
+      </c>
+      <c r="G141" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H141" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I141" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="J141">
+        <v>11</v>
+      </c>
+      <c r="K141" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="142" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A142">
+        <v>4</v>
+      </c>
+      <c r="B142" t="s">
+        <v>232</v>
+      </c>
+      <c r="C142" t="s">
+        <v>59</v>
+      </c>
+      <c r="D142">
+        <v>6.7469999999999999</v>
+      </c>
+      <c r="G142" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H142" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I142" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="J142">
+        <v>11</v>
+      </c>
+      <c r="K142" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="143" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A143">
+        <v>5</v>
+      </c>
+      <c r="B143" t="s">
+        <v>232</v>
+      </c>
+      <c r="C143" t="s">
+        <v>59</v>
+      </c>
+      <c r="D143">
+        <v>8.3829999999999991</v>
+      </c>
+      <c r="G143" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H143" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I143" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="J143">
+        <v>11</v>
+      </c>
+      <c r="K143" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="144" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A144">
+        <v>6</v>
+      </c>
+      <c r="B144" t="s">
+        <v>232</v>
+      </c>
+      <c r="C144" t="s">
+        <v>60</v>
+      </c>
+      <c r="D144">
+        <v>11.62</v>
+      </c>
+      <c r="G144" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H144" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I144" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="J144">
+        <v>11</v>
+      </c>
+      <c r="K144" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="145" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A145">
+        <v>7</v>
+      </c>
+      <c r="B145" t="s">
+        <v>232</v>
+      </c>
+      <c r="C145" t="s">
+        <v>59</v>
+      </c>
+      <c r="D145">
+        <v>7.6989999999999998</v>
+      </c>
+      <c r="G145" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H145" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I145" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="J145">
+        <v>11</v>
+      </c>
+      <c r="K145" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="146" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A146">
+        <v>8</v>
+      </c>
+      <c r="B146" t="s">
+        <v>232</v>
+      </c>
+      <c r="C146" t="s">
+        <v>60</v>
+      </c>
+      <c r="D146">
+        <v>5.2329999999999997</v>
+      </c>
+      <c r="G146" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H146" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I146" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="J146">
+        <v>11</v>
+      </c>
+      <c r="K146" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="147" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A147">
+        <v>9</v>
+      </c>
+      <c r="B147" t="s">
+        <v>232</v>
+      </c>
+      <c r="C147" t="s">
+        <v>60</v>
+      </c>
+      <c r="D147">
+        <v>8.7330000000000005</v>
+      </c>
+      <c r="G147" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H147" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I147" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="J147">
+        <v>11</v>
+      </c>
+      <c r="K147" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="148" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A148">
+        <v>10</v>
+      </c>
+      <c r="B148" t="s">
+        <v>232</v>
+      </c>
+      <c r="C148" t="s">
+        <v>59</v>
+      </c>
+      <c r="D148">
+        <v>9.7370000000000001</v>
+      </c>
+      <c r="G148" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H148" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I148" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="J148">
+        <v>11</v>
+      </c>
+      <c r="K148" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="149" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A149">
+        <v>11</v>
+      </c>
+      <c r="B149" t="s">
+        <v>232</v>
+      </c>
+      <c r="C149" t="s">
+        <v>60</v>
+      </c>
+      <c r="D149">
+        <v>15.02</v>
+      </c>
+      <c r="G149" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H149" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I149" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="J149">
+        <v>11</v>
+      </c>
+      <c r="K149" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="150" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A150">
+        <v>12</v>
+      </c>
+      <c r="B150" t="s">
+        <v>232</v>
+      </c>
+      <c r="C150" t="s">
+        <v>60</v>
+      </c>
+      <c r="D150">
+        <v>9.1539999999999999</v>
+      </c>
+      <c r="G150" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H150" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I150" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="J150">
+        <v>11</v>
+      </c>
+      <c r="K150" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="151" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A151">
+        <v>13</v>
+      </c>
+      <c r="B151" t="s">
+        <v>232</v>
+      </c>
+      <c r="C151" t="s">
+        <v>59</v>
+      </c>
+      <c r="D151">
+        <v>10.824</v>
+      </c>
+      <c r="G151" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H151" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I151" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="J151">
+        <v>11</v>
+      </c>
+      <c r="K151" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="152" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A152">
+        <v>14</v>
+      </c>
+      <c r="B152" t="s">
+        <v>232</v>
+      </c>
+      <c r="C152" t="s">
+        <v>59</v>
+      </c>
+      <c r="D152">
+        <v>7.7549999999999999</v>
+      </c>
+      <c r="G152" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H152" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I152" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="J152">
+        <v>11</v>
+      </c>
+      <c r="K152" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="153" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A153">
+        <v>15</v>
+      </c>
+      <c r="B153" t="s">
+        <v>232</v>
+      </c>
+      <c r="C153" t="s">
+        <v>60</v>
+      </c>
+      <c r="D153">
+        <v>9.1980000000000004</v>
+      </c>
+      <c r="G153" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H153" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I153" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="J153">
+        <v>11</v>
+      </c>
+      <c r="K153" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="154" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A154">
+        <v>16</v>
+      </c>
+      <c r="B154" t="s">
+        <v>232</v>
+      </c>
+      <c r="C154" t="s">
+        <v>59</v>
+      </c>
+      <c r="D154">
+        <v>8.8879999999999999</v>
+      </c>
+      <c r="G154" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H154" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I154" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="J154">
+        <v>11</v>
+      </c>
+      <c r="K154" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="155" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A155">
+        <v>17</v>
+      </c>
+      <c r="B155" t="s">
+        <v>232</v>
+      </c>
+      <c r="C155" t="s">
+        <v>60</v>
+      </c>
+      <c r="D155">
+        <v>11.337999999999999</v>
+      </c>
+      <c r="G155" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H155" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I155" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="J155">
+        <v>11</v>
+      </c>
+      <c r="K155" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="156" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A156">
+        <v>18</v>
+      </c>
+      <c r="B156" t="s">
+        <v>232</v>
+      </c>
+      <c r="C156" t="s">
+        <v>59</v>
+      </c>
+      <c r="D156">
+        <v>7.0209999999999999</v>
+      </c>
+      <c r="G156" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H156" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I156" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="J156">
+        <v>11</v>
+      </c>
+      <c r="K156" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="157" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A157">
+        <v>19</v>
+      </c>
+      <c r="B157" t="s">
+        <v>232</v>
+      </c>
+      <c r="C157" t="s">
+        <v>60</v>
+      </c>
+      <c r="D157">
+        <v>8.8230000000000004</v>
+      </c>
+      <c r="G157" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H157" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I157" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="J157">
+        <v>11</v>
+      </c>
+      <c r="K157" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="158" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A158">
+        <v>20</v>
+      </c>
+      <c r="B158" t="s">
+        <v>232</v>
+      </c>
+      <c r="C158" t="s">
+        <v>59</v>
+      </c>
+      <c r="D158">
+        <v>10.875</v>
+      </c>
+      <c r="G158" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H158" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I158" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="J158">
+        <v>11</v>
+      </c>
+      <c r="K158" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="159" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A159">
+        <v>21</v>
+      </c>
+      <c r="B159" t="s">
+        <v>232</v>
+      </c>
+      <c r="C159" t="s">
+        <v>59</v>
+      </c>
+      <c r="D159">
+        <v>8.3859999999999992</v>
+      </c>
+      <c r="G159" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H159" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I159" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="J159">
+        <v>11</v>
+      </c>
+      <c r="K159" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="160" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A160">
+        <v>22</v>
+      </c>
+      <c r="B160" t="s">
+        <v>232</v>
+      </c>
+      <c r="C160" t="s">
+        <v>60</v>
+      </c>
+      <c r="D160">
+        <v>9.9160000000000004</v>
+      </c>
+      <c r="G160" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H160" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I160" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="J160">
+        <v>11</v>
+      </c>
+      <c r="K160" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="161" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A161">
+        <v>23</v>
+      </c>
+      <c r="B161" t="s">
+        <v>232</v>
+      </c>
+      <c r="C161" t="s">
+        <v>59</v>
+      </c>
+      <c r="D161">
+        <v>9.9610000000000003</v>
+      </c>
+      <c r="G161" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H161" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I161" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="J161">
+        <v>11</v>
+      </c>
+      <c r="K161" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="162" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A162">
+        <v>24</v>
+      </c>
+      <c r="B162" t="s">
+        <v>232</v>
+      </c>
+      <c r="C162" t="s">
+        <v>60</v>
+      </c>
+      <c r="D162">
+        <v>7.0469999999999997</v>
+      </c>
+      <c r="G162" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H162" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I162" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="J162">
+        <v>11</v>
+      </c>
+      <c r="K162" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="163" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A163">
+        <v>25</v>
+      </c>
+      <c r="B163" t="s">
+        <v>232</v>
+      </c>
+      <c r="C163" t="s">
+        <v>59</v>
+      </c>
+      <c r="D163">
+        <v>9.8320000000000007</v>
+      </c>
+      <c r="G163" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H163" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I163" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="J163">
+        <v>11</v>
+      </c>
+      <c r="K163" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="164" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A164">
+        <v>26</v>
+      </c>
+      <c r="B164" t="s">
+        <v>232</v>
+      </c>
+      <c r="C164" t="s">
+        <v>60</v>
+      </c>
+      <c r="D164">
+        <v>8.1859999999999999</v>
+      </c>
+      <c r="G164" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H164" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I164" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="J164">
+        <v>11</v>
+      </c>
+      <c r="K164" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="165" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A165">
+        <v>27</v>
+      </c>
+      <c r="B165" t="s">
+        <v>232</v>
+      </c>
+      <c r="C165" t="s">
+        <v>59</v>
+      </c>
+      <c r="D165">
+        <v>8.1010000000000009</v>
+      </c>
+      <c r="G165" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H165" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I165" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="J165">
+        <v>11</v>
+      </c>
+      <c r="K165" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="166" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A166">
+        <v>28</v>
+      </c>
+      <c r="B166" t="s">
+        <v>232</v>
+      </c>
+      <c r="C166" t="s">
+        <v>59</v>
+      </c>
+      <c r="D166">
+        <v>10.337</v>
+      </c>
+      <c r="G166" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H166" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I166" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="J166">
+        <v>11</v>
+      </c>
+      <c r="K166" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="167" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A167">
+        <v>29</v>
+      </c>
+      <c r="B167" t="s">
+        <v>232</v>
+      </c>
+      <c r="C167" t="s">
+        <v>60</v>
+      </c>
+      <c r="D167">
+        <v>6.2240000000000002</v>
+      </c>
+      <c r="G167" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H167" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I167" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="J167">
+        <v>11</v>
+      </c>
+      <c r="K167" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="168" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A168">
+        <v>30</v>
+      </c>
+      <c r="B168" t="s">
+        <v>232</v>
+      </c>
+      <c r="C168" t="s">
+        <v>60</v>
+      </c>
+      <c r="D168">
+        <v>6.5</v>
+      </c>
+      <c r="G168" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H168" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I168" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="J168">
+        <v>11</v>
+      </c>
+      <c r="K168" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="169" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A169">
+        <v>31</v>
+      </c>
+      <c r="B169" t="s">
+        <v>232</v>
+      </c>
+      <c r="C169" t="s">
+        <v>60</v>
+      </c>
+      <c r="D169">
+        <v>8.1460000000000008</v>
+      </c>
+      <c r="G169" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H169" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I169" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="J169">
+        <v>11</v>
+      </c>
+      <c r="K169" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="170" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A170">
+        <v>32</v>
+      </c>
+      <c r="B170" t="s">
+        <v>232</v>
+      </c>
+      <c r="C170" t="s">
+        <v>59</v>
+      </c>
+      <c r="D170">
+        <v>10.167</v>
+      </c>
+      <c r="G170" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H170" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I170" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="J170">
+        <v>11</v>
+      </c>
+      <c r="K170" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="171" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A171">
+        <v>33</v>
+      </c>
+      <c r="B171" t="s">
+        <v>232</v>
+      </c>
+      <c r="C171" t="s">
+        <v>59</v>
+      </c>
+      <c r="D171">
+        <v>11.026999999999999</v>
+      </c>
+      <c r="G171" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H171" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I171" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="J171">
+        <v>11</v>
+      </c>
+      <c r="K171" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="172" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A172">
+        <v>34</v>
+      </c>
+      <c r="B172" t="s">
+        <v>232</v>
+      </c>
+      <c r="C172" t="s">
+        <v>60</v>
+      </c>
+      <c r="D172">
+        <v>5.7759999999999998</v>
+      </c>
+      <c r="G172" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H172" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I172" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="J172">
+        <v>11</v>
+      </c>
+      <c r="K172" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="173" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A173">
+        <v>35</v>
+      </c>
+      <c r="B173" t="s">
+        <v>232</v>
+      </c>
+      <c r="C173" t="s">
+        <v>59</v>
+      </c>
+      <c r="D173">
+        <v>5.8470000000000004</v>
+      </c>
+      <c r="G173" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H173" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I173" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="J173">
+        <v>11</v>
+      </c>
+      <c r="K173" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="174" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A174">
+        <v>36</v>
+      </c>
+      <c r="B174" t="s">
+        <v>232</v>
+      </c>
+      <c r="C174" t="s">
+        <v>60</v>
+      </c>
+      <c r="D174">
+        <v>6.3609999999999998</v>
+      </c>
+      <c r="G174" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H174" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I174" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="J174">
+        <v>11</v>
+      </c>
+      <c r="K174" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="175" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A175">
+        <v>37</v>
+      </c>
+      <c r="B175" t="s">
+        <v>232</v>
+      </c>
+      <c r="C175" t="s">
+        <v>59</v>
+      </c>
+      <c r="D175">
+        <v>5.7770000000000001</v>
+      </c>
+      <c r="G175" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H175" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I175" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="J175">
+        <v>11</v>
+      </c>
+      <c r="K175" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="176" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A176">
+        <v>38</v>
+      </c>
+      <c r="B176" t="s">
+        <v>232</v>
+      </c>
+      <c r="C176" t="s">
+        <v>60</v>
+      </c>
+      <c r="D176">
+        <v>5.282</v>
+      </c>
+      <c r="G176" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H176" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I176" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="J176">
+        <v>11</v>
+      </c>
+      <c r="K176" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="177" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A177">
+        <v>39</v>
+      </c>
+      <c r="B177" t="s">
+        <v>232</v>
+      </c>
+      <c r="C177" t="s">
+        <v>59</v>
+      </c>
+      <c r="D177">
+        <v>6.83</v>
+      </c>
+      <c r="G177" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H177" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I177" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="J177">
+        <v>11</v>
+      </c>
+      <c r="K177" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="178" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A178">
+        <v>40</v>
+      </c>
+      <c r="B178" t="s">
+        <v>232</v>
+      </c>
+      <c r="C178" t="s">
+        <v>59</v>
+      </c>
+      <c r="D178">
+        <v>7.0819999999999999</v>
+      </c>
+      <c r="G178" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H178" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I178" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="J178">
+        <v>11</v>
+      </c>
+      <c r="K178" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="179" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A179">
+        <v>41</v>
+      </c>
+      <c r="B179" t="s">
+        <v>232</v>
+      </c>
+      <c r="C179" t="s">
+        <v>60</v>
+      </c>
+      <c r="D179">
+        <v>8.8620000000000001</v>
+      </c>
+      <c r="G179" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H179" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I179" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="J179">
+        <v>11</v>
+      </c>
+      <c r="K179" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="180" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A180">
+        <v>42</v>
+      </c>
+      <c r="B180" t="s">
+        <v>232</v>
+      </c>
+      <c r="C180" t="s">
+        <v>60</v>
+      </c>
+      <c r="D180">
+        <v>3.0169999999999999</v>
+      </c>
+      <c r="G180" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H180" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I180" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="J180">
+        <v>11</v>
+      </c>
+      <c r="K180" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="181" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A181">
+        <v>43</v>
+      </c>
+      <c r="B181" t="s">
+        <v>232</v>
+      </c>
+      <c r="C181" t="s">
+        <v>59</v>
+      </c>
+      <c r="D181">
+        <v>10.318</v>
+      </c>
+      <c r="G181" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H181" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I181" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="J181">
+        <v>11</v>
+      </c>
+      <c r="K181" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="182" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A182">
+        <v>44</v>
+      </c>
+      <c r="B182" t="s">
+        <v>232</v>
+      </c>
+      <c r="C182" t="s">
+        <v>60</v>
+      </c>
+      <c r="D182">
+        <v>6.1980000000000004</v>
+      </c>
+      <c r="G182" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H182" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I182" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="J182">
+        <v>11</v>
+      </c>
+      <c r="K182" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="183" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A183">
+        <v>45</v>
+      </c>
+      <c r="B183" t="s">
+        <v>232</v>
+      </c>
+      <c r="C183" t="s">
+        <v>59</v>
+      </c>
+      <c r="D183">
+        <v>6.5460000000000003</v>
+      </c>
+      <c r="G183" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H183" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I183" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="J183">
+        <v>11</v>
+      </c>
+      <c r="K183" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="184" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A184">
+        <v>46</v>
+      </c>
+      <c r="B184" t="s">
+        <v>232</v>
+      </c>
+      <c r="C184" t="s">
+        <v>233</v>
+      </c>
+      <c r="G184" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H184" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I184" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="J184">
+        <v>11</v>
+      </c>
+      <c r="K184" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="185" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A185">
+        <v>47</v>
+      </c>
+      <c r="B185" t="s">
+        <v>232</v>
+      </c>
+      <c r="C185" t="s">
+        <v>233</v>
+      </c>
+      <c r="E185" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="G185" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H185" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I185" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="J185">
+        <v>11</v>
+      </c>
+      <c r="K185" t="s">
+        <v>61</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD836908-61FC-4C6A-BB55-EB17A2B99FDD}">
+  <dimension ref="A1:I31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="13.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.875" style="1" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" t="s">
+        <v>225</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="G1" t="s">
+        <v>226</v>
+      </c>
+      <c r="H1" t="s">
+        <v>227</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="G2">
+        <v>123</v>
+      </c>
+      <c r="H2">
+        <v>45</v>
+      </c>
+      <c r="I2">
+        <f>SUM(G2:H2)</f>
+        <v>168</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="G3">
+        <v>64</v>
+      </c>
+      <c r="H3">
+        <v>45</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ref="I3:I31" si="0">SUM(G3:H3)</f>
+        <v>109</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I23">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I24">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I29">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>229</v>
+      </c>
+      <c r="G31">
+        <f>SUM(G2:G30)</f>
+        <v>187</v>
+      </c>
+      <c r="H31">
+        <f>SUM(H2:H30)</f>
+        <v>90</v>
+      </c>
+      <c r="I31">
+        <f t="shared" si="0"/>
+        <v>277</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding weights da12 cohort apple 2018-08-27
</commit_message>
<xml_diff>
--- a/Data/2018-08-14_master_datac_2018_collection_year.xlsx
+++ b/Data/2018-08-14_master_datac_2018_collection_year.xlsx
@@ -1,33 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anbe642/zScience/Circadian_rhythm_runs_seasonal_timing/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andrew.nguyen\Desktop\Circadian_rhythm_runs_seasonal_timing\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F6D90B0-A98E-874B-A3A2-7332372C767F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38B2D309-CA2E-444E-A66E-C4F5E8AAD831}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1800" yWindow="1940" windowWidth="48500" windowHeight="26120" activeTab="1" xr2:uid="{C7477166-8A7C-B04A-9643-C277FEDCDAAB}"/>
+    <workbookView xWindow="1800" yWindow="1935" windowWidth="48495" windowHeight="26115" activeTab="1" xr2:uid="{C7477166-8A7C-B04A-9643-C277FEDCDAAB}"/>
   </bookViews>
   <sheets>
     <sheet name="Maggot_Collections" sheetId="2" r:id="rId1"/>
     <sheet name="Data_collect" sheetId="1" r:id="rId2"/>
     <sheet name="Pupal_Splits" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3292" uniqueCount="388">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3556" uniqueCount="393">
   <si>
     <t>Ind_ID</t>
   </si>
@@ -1191,6 +1196,21 @@
   </si>
   <si>
     <t>E8</t>
+  </si>
+  <si>
+    <t>orange</t>
+  </si>
+  <si>
+    <t>2018-08-27</t>
+  </si>
+  <si>
+    <t>13:44</t>
+  </si>
+  <si>
+    <t>13:49</t>
+  </si>
+  <si>
+    <t>13:38</t>
   </si>
 </sst>
 </file>
@@ -1615,13 +1635,13 @@
       <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="11" style="1"/>
-    <col min="6" max="6" width="14.1640625" customWidth="1"/>
+    <col min="6" max="6" width="14.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>45</v>
       </c>
@@ -1668,7 +1688,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>58</v>
       </c>
@@ -1708,7 +1728,7 @@
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>58</v>
       </c>
@@ -1748,7 +1768,7 @@
       <c r="S3" s="1"/>
       <c r="T3" s="1"/>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>58</v>
       </c>
@@ -1788,7 +1808,7 @@
       <c r="S4" s="1"/>
       <c r="T4" s="1"/>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>58</v>
       </c>
@@ -1828,7 +1848,7 @@
       <c r="S5" s="1"/>
       <c r="T5" s="1"/>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>58</v>
       </c>
@@ -1880,7 +1900,7 @@
       <c r="S6" s="1"/>
       <c r="T6" s="1"/>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>58</v>
       </c>
@@ -1932,7 +1952,7 @@
       <c r="S7" s="1"/>
       <c r="T7" s="1"/>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>58</v>
       </c>
@@ -1984,7 +2004,7 @@
       <c r="S8" s="1"/>
       <c r="T8" s="1"/>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>58</v>
       </c>
@@ -2036,7 +2056,7 @@
       <c r="S9" s="1"/>
       <c r="T9" s="1"/>
     </row>
-    <row r="10" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>58</v>
       </c>
@@ -2088,7 +2108,7 @@
       <c r="S10" s="13"/>
       <c r="T10" s="13"/>
     </row>
-    <row r="11" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
         <v>58</v>
       </c>
@@ -2140,7 +2160,7 @@
       <c r="S11" s="13"/>
       <c r="T11" s="13"/>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>58</v>
       </c>
@@ -2192,7 +2212,7 @@
       <c r="S12" s="1"/>
       <c r="T12" s="1"/>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>58</v>
       </c>
@@ -2244,7 +2264,7 @@
       <c r="S13" s="1"/>
       <c r="T13" s="1"/>
     </row>
-    <row r="14" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
         <v>58</v>
       </c>
@@ -2296,7 +2316,7 @@
       <c r="S14" s="13"/>
       <c r="T14" s="13"/>
     </row>
-    <row r="15" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
         <v>58</v>
       </c>
@@ -2348,7 +2368,7 @@
       <c r="S15" s="13"/>
       <c r="T15" s="13"/>
     </row>
-    <row r="16" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
         <v>58</v>
       </c>
@@ -2400,7 +2420,7 @@
       <c r="S16" s="13"/>
       <c r="T16" s="13"/>
     </row>
-    <row r="17" spans="1:20" s="16" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:20" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="16" t="s">
         <v>58</v>
       </c>
@@ -2452,7 +2472,7 @@
       <c r="S17" s="17"/>
       <c r="T17" s="17"/>
     </row>
-    <row r="18" spans="1:20" s="16" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:20" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="16" t="s">
         <v>58</v>
       </c>
@@ -2504,7 +2524,7 @@
       <c r="S18" s="17"/>
       <c r="T18" s="17"/>
     </row>
-    <row r="19" spans="1:20" s="16" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:20" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="16" t="s">
         <v>58</v>
       </c>
@@ -2556,7 +2576,7 @@
       <c r="S19" s="17"/>
       <c r="T19" s="17"/>
     </row>
-    <row r="20" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>58</v>
       </c>
@@ -2608,7 +2628,7 @@
       <c r="S20" s="13"/>
       <c r="T20" s="13"/>
     </row>
-    <row r="21" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
         <v>58</v>
       </c>
@@ -2660,7 +2680,7 @@
       <c r="S21" s="13"/>
       <c r="T21" s="13"/>
     </row>
-    <row r="22" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
         <v>58</v>
       </c>
@@ -2712,7 +2732,7 @@
       <c r="S22" s="13"/>
       <c r="T22" s="13"/>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>58</v>
       </c>
@@ -2764,7 +2784,7 @@
       <c r="S23" s="1"/>
       <c r="T23" s="1"/>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>58</v>
       </c>
@@ -2816,7 +2836,7 @@
       <c r="S24" s="1"/>
       <c r="T24" s="1"/>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>58</v>
       </c>
@@ -2868,7 +2888,7 @@
       <c r="S25" s="1"/>
       <c r="T25" s="1"/>
     </row>
-    <row r="26" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="s">
         <v>58</v>
       </c>
@@ -2920,7 +2940,7 @@
       <c r="S26" s="13"/>
       <c r="T26" s="13"/>
     </row>
-    <row r="27" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="11" t="s">
         <v>58</v>
       </c>
@@ -2972,7 +2992,7 @@
       <c r="S27" s="13"/>
       <c r="T27" s="13"/>
     </row>
-    <row r="28" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="s">
         <v>58</v>
       </c>
@@ -3024,7 +3044,7 @@
       <c r="S28" s="13"/>
       <c r="T28" s="13"/>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>58</v>
       </c>
@@ -3076,7 +3096,7 @@
       <c r="S29" s="1"/>
       <c r="T29" s="1"/>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>58</v>
       </c>
@@ -3128,7 +3148,7 @@
       <c r="S30" s="1"/>
       <c r="T30" s="1"/>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>58</v>
       </c>
@@ -3180,7 +3200,7 @@
       <c r="S31" s="1"/>
       <c r="T31" s="1"/>
     </row>
-    <row r="32" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="11" t="s">
         <v>58</v>
       </c>
@@ -3232,7 +3252,7 @@
       <c r="S32" s="13"/>
       <c r="T32" s="13"/>
     </row>
-    <row r="33" spans="1:26" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:26" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="11" t="s">
         <v>58</v>
       </c>
@@ -3284,7 +3304,7 @@
       <c r="S33" s="13"/>
       <c r="T33" s="13"/>
     </row>
-    <row r="34" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>58</v>
       </c>
@@ -3342,7 +3362,7 @@
       <c r="Y34" s="1"/>
       <c r="Z34" s="1"/>
     </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>58</v>
       </c>
@@ -3400,7 +3420,7 @@
       <c r="Y35" s="1"/>
       <c r="Z35" s="1"/>
     </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>58</v>
       </c>
@@ -3458,7 +3478,7 @@
       <c r="Y36" s="1"/>
       <c r="Z36" s="1"/>
     </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>58</v>
       </c>
@@ -3516,7 +3536,7 @@
       <c r="Y37" s="1"/>
       <c r="Z37" s="1"/>
     </row>
-    <row r="38" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>58</v>
       </c>
@@ -3574,7 +3594,7 @@
       <c r="Y38" s="1"/>
       <c r="Z38" s="1"/>
     </row>
-    <row r="39" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>58</v>
       </c>
@@ -3632,7 +3652,7 @@
       <c r="Y39" s="1"/>
       <c r="Z39" s="1"/>
     </row>
-    <row r="40" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>195</v>
       </c>
@@ -3690,7 +3710,7 @@
       <c r="Y40" s="1"/>
       <c r="Z40" s="1"/>
     </row>
-    <row r="41" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>195</v>
       </c>
@@ -3748,7 +3768,7 @@
       <c r="Y41" s="1"/>
       <c r="Z41" s="1"/>
     </row>
-    <row r="42" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>195</v>
       </c>
@@ -3806,7 +3826,7 @@
       <c r="Y42" s="1"/>
       <c r="Z42" s="1"/>
     </row>
-    <row r="43" spans="1:26" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:26" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="14" t="s">
         <v>58</v>
       </c>
@@ -3864,7 +3884,7 @@
       <c r="Y43" s="14"/>
       <c r="Z43" s="14"/>
     </row>
-    <row r="44" spans="1:26" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:26" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="14" t="s">
         <v>58</v>
       </c>
@@ -3922,7 +3942,7 @@
       <c r="Y44" s="14"/>
       <c r="Z44" s="14"/>
     </row>
-    <row r="45" spans="1:26" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:26" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="14" t="s">
         <v>58</v>
       </c>
@@ -3980,7 +4000,7 @@
       <c r="Y45" s="14"/>
       <c r="Z45" s="14"/>
     </row>
-    <row r="46" spans="1:26" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:26" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="14" t="s">
         <v>58</v>
       </c>
@@ -4038,7 +4058,7 @@
       <c r="Y46" s="14"/>
       <c r="Z46" s="14"/>
     </row>
-    <row r="47" spans="1:26" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:26" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="14" t="s">
         <v>58</v>
       </c>
@@ -4096,7 +4116,7 @@
       <c r="Y47" s="14"/>
       <c r="Z47" s="14"/>
     </row>
-    <row r="48" spans="1:26" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:26" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="14" t="s">
         <v>58</v>
       </c>
@@ -4154,7 +4174,7 @@
       <c r="Y48" s="14"/>
       <c r="Z48" s="14"/>
     </row>
-    <row r="49" spans="1:26" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:26" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="14" t="s">
         <v>58</v>
       </c>
@@ -4212,7 +4232,7 @@
       <c r="Y49" s="14"/>
       <c r="Z49" s="14"/>
     </row>
-    <row r="50" spans="1:26" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:26" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="14" t="s">
         <v>195</v>
       </c>
@@ -4270,7 +4290,7 @@
       <c r="Y50" s="14"/>
       <c r="Z50" s="14"/>
     </row>
-    <row r="51" spans="1:26" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:26" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="14" t="s">
         <v>195</v>
       </c>
@@ -4328,7 +4348,7 @@
       <c r="Y51" s="14"/>
       <c r="Z51" s="14"/>
     </row>
-    <row r="52" spans="1:26" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:26" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="14" t="s">
         <v>195</v>
       </c>
@@ -4386,7 +4406,7 @@
       <c r="Y52" s="14"/>
       <c r="Z52" s="14"/>
     </row>
-    <row r="53" spans="1:26" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:26" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="14" t="s">
         <v>58</v>
       </c>
@@ -4444,7 +4464,7 @@
       <c r="Y53" s="14"/>
       <c r="Z53" s="14"/>
     </row>
-    <row r="54" spans="1:26" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:26" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="14" t="s">
         <v>195</v>
       </c>
@@ -4502,7 +4522,7 @@
       <c r="Y54" s="14"/>
       <c r="Z54" s="14"/>
     </row>
-    <row r="55" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>58</v>
       </c>
@@ -4560,7 +4580,7 @@
       <c r="Y55" s="1"/>
       <c r="Z55" s="1"/>
     </row>
-    <row r="56" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>58</v>
       </c>
@@ -4618,7 +4638,7 @@
       <c r="Y56" s="1"/>
       <c r="Z56" s="1"/>
     </row>
-    <row r="57" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>58</v>
       </c>
@@ -4676,7 +4696,7 @@
       <c r="Y57" s="1"/>
       <c r="Z57" s="1"/>
     </row>
-    <row r="58" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>58</v>
       </c>
@@ -4734,7 +4754,7 @@
       <c r="Y58" s="1"/>
       <c r="Z58" s="1"/>
     </row>
-    <row r="59" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>58</v>
       </c>
@@ -4792,7 +4812,7 @@
       <c r="Y59" s="1"/>
       <c r="Z59" s="1"/>
     </row>
-    <row r="60" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>58</v>
       </c>
@@ -4850,7 +4870,7 @@
       <c r="Y60" s="1"/>
       <c r="Z60" s="1"/>
     </row>
-    <row r="61" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>195</v>
       </c>
@@ -4908,7 +4928,7 @@
       <c r="Y61" s="1"/>
       <c r="Z61" s="1"/>
     </row>
-    <row r="62" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>195</v>
       </c>
@@ -4966,7 +4986,7 @@
       <c r="Y62" s="1"/>
       <c r="Z62" s="1"/>
     </row>
-    <row r="63" spans="1:26" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:26" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="14" t="s">
         <v>195</v>
       </c>
@@ -5024,7 +5044,7 @@
       <c r="Y63" s="14"/>
       <c r="Z63" s="14"/>
     </row>
-    <row r="64" spans="1:26" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:26" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="14" t="s">
         <v>195</v>
       </c>
@@ -5082,7 +5102,7 @@
       <c r="Y64" s="14"/>
       <c r="Z64" s="14"/>
     </row>
-    <row r="65" spans="1:26" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:26" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="14" t="s">
         <v>195</v>
       </c>
@@ -5140,7 +5160,7 @@
       <c r="Y65" s="14"/>
       <c r="Z65" s="14"/>
     </row>
-    <row r="66" spans="1:26" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:26" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="14" t="s">
         <v>58</v>
       </c>
@@ -5198,7 +5218,7 @@
       <c r="Y66" s="14"/>
       <c r="Z66" s="14"/>
     </row>
-    <row r="67" spans="1:26" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:26" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="14" t="s">
         <v>58</v>
       </c>
@@ -5256,7 +5276,7 @@
       <c r="Y67" s="14"/>
       <c r="Z67" s="14"/>
     </row>
-    <row r="68" spans="1:26" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:26" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="14" t="s">
         <v>58</v>
       </c>
@@ -5314,7 +5334,7 @@
       <c r="Y68" s="14"/>
       <c r="Z68" s="14"/>
     </row>
-    <row r="69" spans="1:26" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:26" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="14" t="s">
         <v>58</v>
       </c>
@@ -5372,7 +5392,7 @@
       <c r="Y69" s="14"/>
       <c r="Z69" s="14"/>
     </row>
-    <row r="70" spans="1:26" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:26" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="14" t="s">
         <v>58</v>
       </c>
@@ -5430,7 +5450,7 @@
       <c r="Y70" s="14"/>
       <c r="Z70" s="14"/>
     </row>
-    <row r="71" spans="1:26" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:26" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="14" t="s">
         <v>58</v>
       </c>
@@ -5488,7 +5508,7 @@
       <c r="Y71" s="14"/>
       <c r="Z71" s="14"/>
     </row>
-    <row r="72" spans="1:26" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:26" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="14" t="s">
         <v>58</v>
       </c>
@@ -5546,7 +5566,7 @@
       <c r="Y72" s="14"/>
       <c r="Z72" s="14"/>
     </row>
-    <row r="73" spans="1:26" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:26" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="14" t="s">
         <v>195</v>
       </c>
@@ -5604,7 +5624,7 @@
       <c r="Y73" s="14"/>
       <c r="Z73" s="14"/>
     </row>
-    <row r="74" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
@@ -5631,7 +5651,7 @@
       <c r="Y74" s="1"/>
       <c r="Z74" s="1"/>
     </row>
-    <row r="75" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
@@ -5658,7 +5678,7 @@
       <c r="Y75" s="1"/>
       <c r="Z75" s="1"/>
     </row>
-    <row r="76" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A76" s="1"/>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
@@ -5685,7 +5705,7 @@
       <c r="Y76" s="1"/>
       <c r="Z76" s="1"/>
     </row>
-    <row r="77" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
@@ -5712,7 +5732,7 @@
       <c r="Y77" s="1"/>
       <c r="Z77" s="1"/>
     </row>
-    <row r="78" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
@@ -5739,7 +5759,7 @@
       <c r="Y78" s="1"/>
       <c r="Z78" s="1"/>
     </row>
-    <row r="79" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
@@ -5766,7 +5786,7 @@
       <c r="Y79" s="1"/>
       <c r="Z79" s="1"/>
     </row>
-    <row r="80" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
@@ -5793,7 +5813,7 @@
       <c r="Y80" s="1"/>
       <c r="Z80" s="1"/>
     </row>
-    <row r="81" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A81" s="1"/>
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
@@ -5820,7 +5840,7 @@
       <c r="Y81" s="1"/>
       <c r="Z81" s="1"/>
     </row>
-    <row r="82" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A82" s="1"/>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
@@ -5847,7 +5867,7 @@
       <c r="Y82" s="1"/>
       <c r="Z82" s="1"/>
     </row>
-    <row r="83" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A83" s="1"/>
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
@@ -5874,7 +5894,7 @@
       <c r="Y83" s="1"/>
       <c r="Z83" s="1"/>
     </row>
-    <row r="84" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A84" s="1"/>
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
@@ -5901,7 +5921,7 @@
       <c r="Y84" s="1"/>
       <c r="Z84" s="1"/>
     </row>
-    <row r="85" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A85" s="1"/>
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
@@ -5928,7 +5948,7 @@
       <c r="Y85" s="1"/>
       <c r="Z85" s="1"/>
     </row>
-    <row r="86" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A86" s="1"/>
       <c r="B86" s="1"/>
       <c r="C86" s="1"/>
@@ -5955,7 +5975,7 @@
       <c r="Y86" s="1"/>
       <c r="Z86" s="1"/>
     </row>
-    <row r="87" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A87" s="1"/>
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
@@ -5982,7 +6002,7 @@
       <c r="Y87" s="1"/>
       <c r="Z87" s="1"/>
     </row>
-    <row r="88" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A88" s="1"/>
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
@@ -6009,7 +6029,7 @@
       <c r="Y88" s="1"/>
       <c r="Z88" s="1"/>
     </row>
-    <row r="89" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A89" s="1"/>
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
@@ -6036,7 +6056,7 @@
       <c r="Y89" s="1"/>
       <c r="Z89" s="1"/>
     </row>
-    <row r="90" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A90" s="1"/>
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
@@ -6063,7 +6083,7 @@
       <c r="Y90" s="1"/>
       <c r="Z90" s="1"/>
     </row>
-    <row r="91" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A91" s="1"/>
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
@@ -6090,7 +6110,7 @@
       <c r="Y91" s="1"/>
       <c r="Z91" s="1"/>
     </row>
-    <row r="92" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A92" s="1"/>
       <c r="B92" s="1"/>
       <c r="C92" s="1"/>
@@ -6117,7 +6137,7 @@
       <c r="Y92" s="1"/>
       <c r="Z92" s="1"/>
     </row>
-    <row r="93" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A93" s="1"/>
       <c r="B93" s="1"/>
       <c r="C93" s="1"/>
@@ -6144,7 +6164,7 @@
       <c r="Y93" s="1"/>
       <c r="Z93" s="1"/>
     </row>
-    <row r="94" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A94" s="1"/>
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
@@ -6171,7 +6191,7 @@
       <c r="Y94" s="1"/>
       <c r="Z94" s="1"/>
     </row>
-    <row r="95" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A95" s="1"/>
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
@@ -6198,7 +6218,7 @@
       <c r="Y95" s="1"/>
       <c r="Z95" s="1"/>
     </row>
-    <row r="96" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A96" s="1"/>
       <c r="B96" s="1"/>
       <c r="C96" s="1"/>
@@ -6225,7 +6245,7 @@
       <c r="Y96" s="1"/>
       <c r="Z96" s="1"/>
     </row>
-    <row r="97" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A97" s="1"/>
       <c r="B97" s="1"/>
       <c r="C97" s="1"/>
@@ -6252,7 +6272,7 @@
       <c r="Y97" s="1"/>
       <c r="Z97" s="1"/>
     </row>
-    <row r="98" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A98" s="1"/>
       <c r="B98" s="1"/>
       <c r="C98" s="1"/>
@@ -6279,7 +6299,7 @@
       <c r="Y98" s="1"/>
       <c r="Z98" s="1"/>
     </row>
-    <row r="99" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A99" s="1"/>
       <c r="B99" s="1"/>
       <c r="C99" s="1"/>
@@ -6306,7 +6326,7 @@
       <c r="Y99" s="1"/>
       <c r="Z99" s="1"/>
     </row>
-    <row r="100" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A100" s="1"/>
       <c r="B100" s="1"/>
       <c r="C100" s="1"/>
@@ -6333,7 +6353,7 @@
       <c r="Y100" s="1"/>
       <c r="Z100" s="1"/>
     </row>
-    <row r="101" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A101" s="1"/>
       <c r="B101" s="1"/>
       <c r="C101" s="1"/>
@@ -6360,7 +6380,7 @@
       <c r="Y101" s="1"/>
       <c r="Z101" s="1"/>
     </row>
-    <row r="102" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A102" s="1"/>
       <c r="B102" s="1"/>
       <c r="C102" s="1"/>
@@ -6395,22 +6415,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92725FB9-1A17-2546-9DFA-6C0D39437891}">
-  <dimension ref="A1:AS275"/>
+  <dimension ref="A1:AS319"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A162" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AC92" sqref="AC92:AC183"/>
+      <pane ySplit="1" topLeftCell="A292" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D318" sqref="D318"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="5" max="5" width="11" style="1"/>
-    <col min="7" max="7" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="11" style="1"/>
-    <col min="20" max="20" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.375" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6547,7 +6567,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -6576,7 +6596,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -6605,7 +6625,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="4" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -6634,7 +6654,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="5" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -6663,7 +6683,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="6" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -6692,7 +6712,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="7" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -6721,7 +6741,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="8" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -6750,7 +6770,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="9" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -6779,7 +6799,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="10" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -6808,7 +6828,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="11" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -6837,7 +6857,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="12" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -6866,7 +6886,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="13" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -6895,7 +6915,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="14" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -6924,7 +6944,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="15" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -6953,7 +6973,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="16" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -6982,7 +7002,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="17" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -7011,7 +7031,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="18" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -7040,7 +7060,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="19" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -7069,7 +7089,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="20" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -7098,7 +7118,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="21" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -7127,7 +7147,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="22" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -7156,7 +7176,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="23" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -7185,7 +7205,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="24" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -7214,7 +7234,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="25" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -7243,7 +7263,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="26" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -7272,7 +7292,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="27" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -7301,7 +7321,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="28" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -7330,7 +7350,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="29" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -7359,7 +7379,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="30" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -7388,7 +7408,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="31" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -7417,7 +7437,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="32" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>1</v>
       </c>
@@ -7453,7 +7473,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="33" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>2</v>
       </c>
@@ -7489,7 +7509,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="34" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>3</v>
       </c>
@@ -7525,7 +7545,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="35" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>4</v>
       </c>
@@ -7561,7 +7581,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="36" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>5</v>
       </c>
@@ -7597,7 +7617,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="37" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>6</v>
       </c>
@@ -7633,7 +7653,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="38" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>7</v>
       </c>
@@ -7669,7 +7689,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="39" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>8</v>
       </c>
@@ -7705,7 +7725,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="40" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>9</v>
       </c>
@@ -7741,7 +7761,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="41" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>10</v>
       </c>
@@ -7777,7 +7797,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="42" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>11</v>
       </c>
@@ -7813,7 +7833,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="43" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>12</v>
       </c>
@@ -7849,7 +7869,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="44" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>13</v>
       </c>
@@ -7885,7 +7905,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="45" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>14</v>
       </c>
@@ -7921,7 +7941,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="46" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>15</v>
       </c>
@@ -7957,7 +7977,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="47" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>16</v>
       </c>
@@ -7993,7 +8013,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="48" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>17</v>
       </c>
@@ -8029,7 +8049,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="49" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>18</v>
       </c>
@@ -8065,7 +8085,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="50" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>19</v>
       </c>
@@ -8101,7 +8121,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="51" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>20</v>
       </c>
@@ -8137,7 +8157,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="52" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>21</v>
       </c>
@@ -8173,7 +8193,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="53" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>22</v>
       </c>
@@ -8209,7 +8229,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="54" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>23</v>
       </c>
@@ -8245,7 +8265,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="55" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>24</v>
       </c>
@@ -8281,7 +8301,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="56" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>25</v>
       </c>
@@ -8317,7 +8337,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="57" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>26</v>
       </c>
@@ -8353,7 +8373,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="58" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>27</v>
       </c>
@@ -8389,7 +8409,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="59" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>28</v>
       </c>
@@ -8425,7 +8445,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="60" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>29</v>
       </c>
@@ -8461,7 +8481,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="61" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>30</v>
       </c>
@@ -8497,7 +8517,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="62" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>1</v>
       </c>
@@ -8533,7 +8553,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="63" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>2</v>
       </c>
@@ -8569,7 +8589,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="64" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>3</v>
       </c>
@@ -8605,7 +8625,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="65" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>4</v>
       </c>
@@ -8641,7 +8661,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="66" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>5</v>
       </c>
@@ -8677,7 +8697,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="67" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>6</v>
       </c>
@@ -8713,7 +8733,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="68" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>7</v>
       </c>
@@ -8749,7 +8769,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="69" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>8</v>
       </c>
@@ -8785,7 +8805,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="70" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>9</v>
       </c>
@@ -8821,7 +8841,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="71" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>10</v>
       </c>
@@ -8857,7 +8877,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="72" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>11</v>
       </c>
@@ -8893,7 +8913,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="73" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>12</v>
       </c>
@@ -8929,7 +8949,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="74" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>13</v>
       </c>
@@ -8965,7 +8985,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="75" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>14</v>
       </c>
@@ -9001,7 +9021,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="76" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>15</v>
       </c>
@@ -9037,7 +9057,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="77" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>16</v>
       </c>
@@ -9073,7 +9093,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="78" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>17</v>
       </c>
@@ -9109,7 +9129,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="79" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>18</v>
       </c>
@@ -9145,7 +9165,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="80" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>19</v>
       </c>
@@ -9181,7 +9201,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="81" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>20</v>
       </c>
@@ -9217,7 +9237,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="82" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>21</v>
       </c>
@@ -9253,7 +9273,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="83" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>22</v>
       </c>
@@ -9289,7 +9309,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="84" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>23</v>
       </c>
@@ -9325,7 +9345,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="85" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>24</v>
       </c>
@@ -9361,7 +9381,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="86" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>25</v>
       </c>
@@ -9397,7 +9417,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="87" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>26</v>
       </c>
@@ -9433,7 +9453,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="88" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>27</v>
       </c>
@@ -9469,7 +9489,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="89" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>28</v>
       </c>
@@ -9505,7 +9525,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="90" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>29</v>
       </c>
@@ -9541,7 +9561,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="91" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>30</v>
       </c>
@@ -9577,7 +9597,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="92" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>1</v>
       </c>
@@ -9621,7 +9641,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="93" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>2</v>
       </c>
@@ -9659,7 +9679,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="94" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>3</v>
       </c>
@@ -9697,7 +9717,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="95" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>4</v>
       </c>
@@ -9738,7 +9758,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="96" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>5</v>
       </c>
@@ -9779,7 +9799,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="97" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>6</v>
       </c>
@@ -9817,7 +9837,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="98" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>7</v>
       </c>
@@ -9858,7 +9878,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="99" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>8</v>
       </c>
@@ -9899,7 +9919,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="100" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>9</v>
       </c>
@@ -9940,7 +9960,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="101" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>10</v>
       </c>
@@ -9981,7 +10001,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="102" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>11</v>
       </c>
@@ -10019,7 +10039,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="103" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>12</v>
       </c>
@@ -10060,7 +10080,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="104" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>13</v>
       </c>
@@ -10101,7 +10121,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="105" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>14</v>
       </c>
@@ -10142,7 +10162,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="106" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>15</v>
       </c>
@@ -10183,7 +10203,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="107" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>16</v>
       </c>
@@ -10224,7 +10244,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="108" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>17</v>
       </c>
@@ -10262,7 +10282,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="109" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>18</v>
       </c>
@@ -10303,7 +10323,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="110" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>19</v>
       </c>
@@ -10341,7 +10361,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="111" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>20</v>
       </c>
@@ -10382,7 +10402,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="112" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>21</v>
       </c>
@@ -10423,7 +10443,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="113" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>22</v>
       </c>
@@ -10461,7 +10481,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="114" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>23</v>
       </c>
@@ -10502,7 +10522,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="115" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>24</v>
       </c>
@@ -10540,7 +10560,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="116" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>25</v>
       </c>
@@ -10581,7 +10601,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="117" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>26</v>
       </c>
@@ -10619,7 +10639,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="118" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>27</v>
       </c>
@@ -10657,7 +10677,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="119" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>28</v>
       </c>
@@ -10698,7 +10718,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="120" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>29</v>
       </c>
@@ -10739,7 +10759,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="121" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>30</v>
       </c>
@@ -10777,7 +10797,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="122" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>31</v>
       </c>
@@ -10818,7 +10838,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="123" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>32</v>
       </c>
@@ -10856,7 +10876,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="124" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>33</v>
       </c>
@@ -10894,7 +10914,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="125" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>34</v>
       </c>
@@ -10935,7 +10955,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="126" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>35</v>
       </c>
@@ -10976,7 +10996,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="127" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>36</v>
       </c>
@@ -11014,7 +11034,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="128" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>37</v>
       </c>
@@ -11055,7 +11075,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="129" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>38</v>
       </c>
@@ -11096,7 +11116,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="130" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>39</v>
       </c>
@@ -11137,7 +11157,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="131" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>40</v>
       </c>
@@ -11175,7 +11195,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="132" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>41</v>
       </c>
@@ -11216,7 +11236,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="133" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>42</v>
       </c>
@@ -11257,7 +11277,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="134" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>43</v>
       </c>
@@ -11295,7 +11315,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="135" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>44</v>
       </c>
@@ -11336,7 +11356,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="136" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>45</v>
       </c>
@@ -11374,7 +11394,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="137" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>46</v>
       </c>
@@ -11403,7 +11423,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="138" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>47</v>
       </c>
@@ -11435,7 +11455,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="139" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>1</v>
       </c>
@@ -11476,7 +11496,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="140" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>2</v>
       </c>
@@ -11517,7 +11537,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="141" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>3</v>
       </c>
@@ -11558,7 +11578,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="142" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>4</v>
       </c>
@@ -11599,7 +11619,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="143" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>5</v>
       </c>
@@ -11640,7 +11660,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="144" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>6</v>
       </c>
@@ -11681,7 +11701,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="145" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>7</v>
       </c>
@@ -11722,7 +11742,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="146" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>8</v>
       </c>
@@ -11763,7 +11783,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="147" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>9</v>
       </c>
@@ -11801,7 +11821,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="148" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>10</v>
       </c>
@@ -11842,7 +11862,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="149" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>11</v>
       </c>
@@ -11880,7 +11900,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="150" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>12</v>
       </c>
@@ -11918,7 +11938,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="151" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>13</v>
       </c>
@@ -11959,7 +11979,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="152" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>14</v>
       </c>
@@ -12000,7 +12020,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="153" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>15</v>
       </c>
@@ -12041,7 +12061,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="154" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>16</v>
       </c>
@@ -12079,7 +12099,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="155" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>17</v>
       </c>
@@ -12120,7 +12140,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="156" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>18</v>
       </c>
@@ -12161,7 +12181,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="157" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>19</v>
       </c>
@@ -12202,7 +12222,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="158" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>20</v>
       </c>
@@ -12240,7 +12260,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="159" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>21</v>
       </c>
@@ -12281,7 +12301,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="160" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>22</v>
       </c>
@@ -12319,7 +12339,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="161" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>23</v>
       </c>
@@ -12360,7 +12380,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="162" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>24</v>
       </c>
@@ -12398,7 +12418,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="163" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>25</v>
       </c>
@@ -12436,7 +12456,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="164" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>26</v>
       </c>
@@ -12477,7 +12497,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="165" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>27</v>
       </c>
@@ -12515,7 +12535,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="166" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A166">
         <v>28</v>
       </c>
@@ -12553,7 +12573,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="167" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A167">
         <v>29</v>
       </c>
@@ -12594,7 +12614,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="168" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A168">
         <v>30</v>
       </c>
@@ -12635,7 +12655,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="169" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A169">
         <v>31</v>
       </c>
@@ -12676,7 +12696,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="170" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A170">
         <v>32</v>
       </c>
@@ -12717,7 +12737,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="171" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A171">
         <v>33</v>
       </c>
@@ -12758,7 +12778,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="172" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A172">
         <v>34</v>
       </c>
@@ -12799,7 +12819,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="173" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A173">
         <v>35</v>
       </c>
@@ -12840,7 +12860,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="174" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A174">
         <v>36</v>
       </c>
@@ -12881,7 +12901,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="175" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A175">
         <v>37</v>
       </c>
@@ -12922,7 +12942,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="176" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A176">
         <v>38</v>
       </c>
@@ -12960,7 +12980,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="177" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A177">
         <v>39</v>
       </c>
@@ -13001,7 +13021,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="178" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A178">
         <v>40</v>
       </c>
@@ -13042,7 +13062,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="179" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A179">
         <v>41</v>
       </c>
@@ -13083,7 +13103,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="180" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A180">
         <v>42</v>
       </c>
@@ -13121,7 +13141,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="181" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A181">
         <v>43</v>
       </c>
@@ -13159,7 +13179,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="182" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A182">
         <v>44</v>
       </c>
@@ -13200,7 +13220,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="183" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A183">
         <v>45</v>
       </c>
@@ -13238,7 +13258,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="184" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A184">
         <v>46</v>
       </c>
@@ -13267,7 +13287,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="185" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A185">
         <v>47</v>
       </c>
@@ -13299,7 +13319,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="186" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A186">
         <v>1</v>
       </c>
@@ -13328,7 +13348,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="187" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A187">
         <v>2</v>
       </c>
@@ -13357,7 +13377,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="188" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A188">
         <v>3</v>
       </c>
@@ -13386,7 +13406,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="189" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A189">
         <v>4</v>
       </c>
@@ -13415,7 +13435,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="190" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A190">
         <v>5</v>
       </c>
@@ -13444,7 +13464,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="191" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A191">
         <v>6</v>
       </c>
@@ -13473,7 +13493,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="192" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A192">
         <v>7</v>
       </c>
@@ -13502,7 +13522,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="193" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A193">
         <v>8</v>
       </c>
@@ -13531,7 +13551,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="194" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A194">
         <v>9</v>
       </c>
@@ -13560,7 +13580,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="195" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A195">
         <v>10</v>
       </c>
@@ -13589,7 +13609,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="196" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A196">
         <v>11</v>
       </c>
@@ -13618,7 +13638,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="197" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A197">
         <v>12</v>
       </c>
@@ -13647,7 +13667,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="198" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A198">
         <v>13</v>
       </c>
@@ -13676,7 +13696,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="199" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A199">
         <v>14</v>
       </c>
@@ -13705,7 +13725,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="200" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A200">
         <v>15</v>
       </c>
@@ -13734,7 +13754,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="201" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A201">
         <v>16</v>
       </c>
@@ -13763,7 +13783,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="202" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A202">
         <v>17</v>
       </c>
@@ -13792,7 +13812,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="203" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A203">
         <v>18</v>
       </c>
@@ -13821,7 +13841,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="204" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A204">
         <v>19</v>
       </c>
@@ -13850,7 +13870,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="205" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A205">
         <v>20</v>
       </c>
@@ -13879,7 +13899,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="206" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A206">
         <v>21</v>
       </c>
@@ -13908,7 +13928,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="207" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A207">
         <v>22</v>
       </c>
@@ -13937,7 +13957,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="208" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A208">
         <v>23</v>
       </c>
@@ -13966,7 +13986,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="209" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A209">
         <v>24</v>
       </c>
@@ -13995,7 +14015,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="210" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A210">
         <v>25</v>
       </c>
@@ -14024,7 +14044,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="211" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A211">
         <v>26</v>
       </c>
@@ -14053,7 +14073,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="212" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A212">
         <v>27</v>
       </c>
@@ -14082,7 +14102,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="213" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A213">
         <v>28</v>
       </c>
@@ -14111,7 +14131,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="214" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A214">
         <v>29</v>
       </c>
@@ -14140,7 +14160,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="215" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A215">
         <v>30</v>
       </c>
@@ -14169,7 +14189,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="216" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A216">
         <v>1</v>
       </c>
@@ -14205,7 +14225,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="217" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A217">
         <v>2</v>
       </c>
@@ -14241,7 +14261,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="218" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A218">
         <v>3</v>
       </c>
@@ -14277,7 +14297,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="219" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A219">
         <v>4</v>
       </c>
@@ -14313,7 +14333,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="220" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A220">
         <v>5</v>
       </c>
@@ -14349,7 +14369,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="221" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A221">
         <v>6</v>
       </c>
@@ -14385,7 +14405,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="222" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A222">
         <v>7</v>
       </c>
@@ -14421,7 +14441,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="223" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A223">
         <v>8</v>
       </c>
@@ -14457,7 +14477,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="224" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A224">
         <v>9</v>
       </c>
@@ -14493,7 +14513,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="225" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A225">
         <v>10</v>
       </c>
@@ -14529,7 +14549,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="226" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A226">
         <v>11</v>
       </c>
@@ -14565,7 +14585,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="227" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A227">
         <v>12</v>
       </c>
@@ -14601,7 +14621,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="228" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A228">
         <v>13</v>
       </c>
@@ -14637,7 +14657,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="229" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A229">
         <v>14</v>
       </c>
@@ -14673,7 +14693,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="230" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A230">
         <v>15</v>
       </c>
@@ -14709,7 +14729,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="231" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A231">
         <v>16</v>
       </c>
@@ -14745,7 +14765,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="232" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A232">
         <v>17</v>
       </c>
@@ -14781,7 +14801,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="233" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A233">
         <v>18</v>
       </c>
@@ -14817,7 +14837,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="234" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A234">
         <v>19</v>
       </c>
@@ -14853,7 +14873,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="235" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A235">
         <v>20</v>
       </c>
@@ -14889,7 +14909,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="236" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A236">
         <v>21</v>
       </c>
@@ -14925,7 +14945,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="237" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A237">
         <v>22</v>
       </c>
@@ -14961,7 +14981,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="238" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A238">
         <v>23</v>
       </c>
@@ -14997,7 +15017,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="239" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A239">
         <v>24</v>
       </c>
@@ -15033,7 +15053,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="240" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A240">
         <v>25</v>
       </c>
@@ -15069,7 +15089,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="241" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A241">
         <v>26</v>
       </c>
@@ -15105,7 +15125,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="242" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A242">
         <v>27</v>
       </c>
@@ -15141,7 +15161,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="243" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A243">
         <v>28</v>
       </c>
@@ -15177,7 +15197,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="244" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A244">
         <v>29</v>
       </c>
@@ -15213,7 +15233,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="245" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A245">
         <v>30</v>
       </c>
@@ -15249,7 +15269,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="246" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A246">
         <v>1</v>
       </c>
@@ -15285,7 +15305,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="247" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A247">
         <v>2</v>
       </c>
@@ -15321,7 +15341,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="248" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A248">
         <v>3</v>
       </c>
@@ -15357,7 +15377,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="249" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A249">
         <v>4</v>
       </c>
@@ -15393,7 +15413,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="250" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A250">
         <v>5</v>
       </c>
@@ -15429,7 +15449,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="251" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A251">
         <v>6</v>
       </c>
@@ -15465,7 +15485,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="252" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A252">
         <v>7</v>
       </c>
@@ -15501,7 +15521,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="253" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A253">
         <v>8</v>
       </c>
@@ -15537,7 +15557,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="254" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A254">
         <v>9</v>
       </c>
@@ -15573,7 +15593,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="255" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A255">
         <v>10</v>
       </c>
@@ -15609,7 +15629,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="256" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A256">
         <v>11</v>
       </c>
@@ -15645,7 +15665,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="257" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A257">
         <v>12</v>
       </c>
@@ -15681,7 +15701,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="258" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A258">
         <v>13</v>
       </c>
@@ -15717,7 +15737,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="259" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A259">
         <v>14</v>
       </c>
@@ -15753,7 +15773,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="260" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A260">
         <v>15</v>
       </c>
@@ -15789,7 +15809,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="261" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A261">
         <v>16</v>
       </c>
@@ -15825,7 +15845,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="262" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A262">
         <v>17</v>
       </c>
@@ -15861,7 +15881,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="263" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A263">
         <v>18</v>
       </c>
@@ -15897,7 +15917,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="264" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A264">
         <v>19</v>
       </c>
@@ -15933,7 +15953,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="265" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A265">
         <v>20</v>
       </c>
@@ -15969,7 +15989,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="266" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A266">
         <v>21</v>
       </c>
@@ -16005,7 +16025,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="267" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A267">
         <v>22</v>
       </c>
@@ -16041,7 +16061,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="268" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A268">
         <v>23</v>
       </c>
@@ -16077,7 +16097,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="269" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A269">
         <v>24</v>
       </c>
@@ -16113,7 +16133,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="270" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A270">
         <v>25</v>
       </c>
@@ -16149,7 +16169,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="271" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A271">
         <v>26</v>
       </c>
@@ -16185,7 +16205,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="272" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A272">
         <v>27</v>
       </c>
@@ -16221,7 +16241,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="273" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A273">
         <v>28</v>
       </c>
@@ -16257,7 +16277,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="274" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A274">
         <v>29</v>
       </c>
@@ -16293,7 +16313,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="275" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A275">
         <v>30</v>
       </c>
@@ -16327,6 +16347,1270 @@
       </c>
       <c r="AC275" t="s">
         <v>254</v>
+      </c>
+    </row>
+    <row r="276" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A276">
+        <v>1</v>
+      </c>
+      <c r="B276" t="s">
+        <v>90</v>
+      </c>
+      <c r="C276" t="s">
+        <v>60</v>
+      </c>
+      <c r="D276">
+        <v>10.505000000000001</v>
+      </c>
+      <c r="E276" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="G276" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H276" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I276" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="J276">
+        <v>12</v>
+      </c>
+      <c r="K276" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="277" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A277">
+        <v>2</v>
+      </c>
+      <c r="B277" t="s">
+        <v>90</v>
+      </c>
+      <c r="C277" t="s">
+        <v>60</v>
+      </c>
+      <c r="D277">
+        <v>7.7539999999999996</v>
+      </c>
+      <c r="G277" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H277" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I277" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="J277">
+        <v>12</v>
+      </c>
+      <c r="K277" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="278" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A278">
+        <v>3</v>
+      </c>
+      <c r="B278" t="s">
+        <v>90</v>
+      </c>
+      <c r="C278" t="s">
+        <v>59</v>
+      </c>
+      <c r="D278">
+        <v>8.0920000000000005</v>
+      </c>
+      <c r="G278" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H278" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I278" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="J278">
+        <v>12</v>
+      </c>
+      <c r="K278" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="279" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A279">
+        <v>4</v>
+      </c>
+      <c r="B279" t="s">
+        <v>90</v>
+      </c>
+      <c r="C279" t="s">
+        <v>60</v>
+      </c>
+      <c r="D279">
+        <v>6.2539999999999996</v>
+      </c>
+      <c r="G279" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H279" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I279" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="J279">
+        <v>12</v>
+      </c>
+      <c r="K279" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="280" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A280">
+        <v>5</v>
+      </c>
+      <c r="B280" t="s">
+        <v>90</v>
+      </c>
+      <c r="C280" t="s">
+        <v>59</v>
+      </c>
+      <c r="D280">
+        <v>8.7449999999999992</v>
+      </c>
+      <c r="G280" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H280" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I280" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="J280">
+        <v>12</v>
+      </c>
+      <c r="K280" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="281" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A281">
+        <v>6</v>
+      </c>
+      <c r="B281" t="s">
+        <v>90</v>
+      </c>
+      <c r="C281" t="s">
+        <v>60</v>
+      </c>
+      <c r="D281">
+        <v>6.0759999999999996</v>
+      </c>
+      <c r="G281" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H281" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I281" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="J281">
+        <v>12</v>
+      </c>
+      <c r="K281" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="282" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A282">
+        <v>7</v>
+      </c>
+      <c r="B282" t="s">
+        <v>90</v>
+      </c>
+      <c r="C282" t="s">
+        <v>59</v>
+      </c>
+      <c r="D282">
+        <v>6.4139999999999997</v>
+      </c>
+      <c r="G282" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H282" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I282" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="J282">
+        <v>12</v>
+      </c>
+      <c r="K282" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="283" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A283">
+        <v>8</v>
+      </c>
+      <c r="B283" t="s">
+        <v>90</v>
+      </c>
+      <c r="C283" t="s">
+        <v>60</v>
+      </c>
+      <c r="D283">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="G283" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H283" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I283" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="J283">
+        <v>12</v>
+      </c>
+      <c r="K283" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="284" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A284">
+        <v>9</v>
+      </c>
+      <c r="B284" t="s">
+        <v>90</v>
+      </c>
+      <c r="C284" t="s">
+        <v>59</v>
+      </c>
+      <c r="D284">
+        <v>8.1159999999999997</v>
+      </c>
+      <c r="G284" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H284" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I284" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="J284">
+        <v>12</v>
+      </c>
+      <c r="K284" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="285" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A285">
+        <v>10</v>
+      </c>
+      <c r="B285" t="s">
+        <v>90</v>
+      </c>
+      <c r="C285" t="s">
+        <v>60</v>
+      </c>
+      <c r="D285">
+        <v>8.8789999999999996</v>
+      </c>
+      <c r="G285" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H285" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I285" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="J285">
+        <v>12</v>
+      </c>
+      <c r="K285" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="286" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A286">
+        <v>11</v>
+      </c>
+      <c r="B286" t="s">
+        <v>90</v>
+      </c>
+      <c r="C286" t="s">
+        <v>60</v>
+      </c>
+      <c r="D286">
+        <v>7.4950000000000001</v>
+      </c>
+      <c r="G286" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H286" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I286" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="J286">
+        <v>12</v>
+      </c>
+      <c r="K286" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="287" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A287">
+        <v>12</v>
+      </c>
+      <c r="B287" t="s">
+        <v>90</v>
+      </c>
+      <c r="C287" t="s">
+        <v>60</v>
+      </c>
+      <c r="D287">
+        <v>10.103</v>
+      </c>
+      <c r="G287" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H287" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I287" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="J287">
+        <v>12</v>
+      </c>
+      <c r="K287" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="288" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A288">
+        <v>13</v>
+      </c>
+      <c r="B288" t="s">
+        <v>90</v>
+      </c>
+      <c r="C288" t="s">
+        <v>59</v>
+      </c>
+      <c r="D288">
+        <v>9.6980000000000004</v>
+      </c>
+      <c r="G288" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H288" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I288" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="J288">
+        <v>12</v>
+      </c>
+      <c r="K288" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="289" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A289">
+        <v>14</v>
+      </c>
+      <c r="B289" t="s">
+        <v>90</v>
+      </c>
+      <c r="C289" t="s">
+        <v>60</v>
+      </c>
+      <c r="D289">
+        <v>9.5640000000000001</v>
+      </c>
+      <c r="G289" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H289" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I289" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="J289">
+        <v>12</v>
+      </c>
+      <c r="K289" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="290" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A290">
+        <v>15</v>
+      </c>
+      <c r="B290" t="s">
+        <v>90</v>
+      </c>
+      <c r="C290" t="s">
+        <v>59</v>
+      </c>
+      <c r="D290">
+        <v>8.6340000000000003</v>
+      </c>
+      <c r="G290" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H290" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I290" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="J290">
+        <v>12</v>
+      </c>
+      <c r="K290" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="291" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A291">
+        <v>16</v>
+      </c>
+      <c r="B291" t="s">
+        <v>90</v>
+      </c>
+      <c r="C291" t="s">
+        <v>60</v>
+      </c>
+      <c r="D291">
+        <v>6.4130000000000003</v>
+      </c>
+      <c r="G291" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H291" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I291" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="J291">
+        <v>12</v>
+      </c>
+      <c r="K291" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="292" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A292">
+        <v>17</v>
+      </c>
+      <c r="B292" t="s">
+        <v>90</v>
+      </c>
+      <c r="C292" t="s">
+        <v>59</v>
+      </c>
+      <c r="D292">
+        <v>6.6890000000000001</v>
+      </c>
+      <c r="G292" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H292" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I292" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="J292">
+        <v>12</v>
+      </c>
+      <c r="K292" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="293" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A293">
+        <v>18</v>
+      </c>
+      <c r="B293" t="s">
+        <v>90</v>
+      </c>
+      <c r="C293" t="s">
+        <v>59</v>
+      </c>
+      <c r="D293">
+        <v>6.4089999999999998</v>
+      </c>
+      <c r="G293" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H293" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I293" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="J293">
+        <v>12</v>
+      </c>
+      <c r="K293" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="294" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A294">
+        <v>19</v>
+      </c>
+      <c r="B294" t="s">
+        <v>90</v>
+      </c>
+      <c r="C294" t="s">
+        <v>59</v>
+      </c>
+      <c r="D294">
+        <v>8.5830000000000002</v>
+      </c>
+      <c r="G294" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H294" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I294" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="J294">
+        <v>12</v>
+      </c>
+      <c r="K294" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="295" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A295">
+        <v>20</v>
+      </c>
+      <c r="B295" t="s">
+        <v>90</v>
+      </c>
+      <c r="C295" t="s">
+        <v>59</v>
+      </c>
+      <c r="D295">
+        <v>7.5229999999999997</v>
+      </c>
+      <c r="E295" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="G295" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H295" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I295" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="J295">
+        <v>12</v>
+      </c>
+      <c r="K295" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="296" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A296">
+        <v>21</v>
+      </c>
+      <c r="B296" t="s">
+        <v>90</v>
+      </c>
+      <c r="C296" t="s">
+        <v>233</v>
+      </c>
+      <c r="G296" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H296" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I296" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="J296">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="297" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A297">
+        <v>22</v>
+      </c>
+      <c r="B297" t="s">
+        <v>90</v>
+      </c>
+      <c r="C297" t="s">
+        <v>233</v>
+      </c>
+      <c r="G297" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H297" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I297" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="J297">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="298" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A298">
+        <v>1</v>
+      </c>
+      <c r="B298" t="s">
+        <v>388</v>
+      </c>
+      <c r="C298" t="s">
+        <v>59</v>
+      </c>
+      <c r="D298">
+        <v>10.206</v>
+      </c>
+      <c r="E298" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="G298" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H298" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I298" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="J298">
+        <v>12</v>
+      </c>
+      <c r="K298" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="299" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A299">
+        <v>2</v>
+      </c>
+      <c r="B299" t="s">
+        <v>388</v>
+      </c>
+      <c r="C299" t="s">
+        <v>59</v>
+      </c>
+      <c r="D299">
+        <v>11.188000000000001</v>
+      </c>
+      <c r="G299" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H299" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I299" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="J299">
+        <v>12</v>
+      </c>
+      <c r="K299" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="300" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A300">
+        <v>3</v>
+      </c>
+      <c r="B300" t="s">
+        <v>388</v>
+      </c>
+      <c r="C300" t="s">
+        <v>60</v>
+      </c>
+      <c r="D300">
+        <v>8.84</v>
+      </c>
+      <c r="G300" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H300" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I300" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="J300">
+        <v>12</v>
+      </c>
+      <c r="K300" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="301" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A301">
+        <v>4</v>
+      </c>
+      <c r="B301" t="s">
+        <v>388</v>
+      </c>
+      <c r="C301" t="s">
+        <v>59</v>
+      </c>
+      <c r="D301">
+        <v>10.257999999999999</v>
+      </c>
+      <c r="G301" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H301" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I301" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="J301">
+        <v>12</v>
+      </c>
+      <c r="K301" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="302" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A302">
+        <v>5</v>
+      </c>
+      <c r="B302" t="s">
+        <v>388</v>
+      </c>
+      <c r="C302" t="s">
+        <v>60</v>
+      </c>
+      <c r="D302">
+        <v>9.7279999999999998</v>
+      </c>
+      <c r="G302" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H302" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I302" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="J302">
+        <v>12</v>
+      </c>
+      <c r="K302" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="303" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A303">
+        <v>6</v>
+      </c>
+      <c r="B303" t="s">
+        <v>388</v>
+      </c>
+      <c r="C303" t="s">
+        <v>59</v>
+      </c>
+      <c r="D303">
+        <v>7.4139999999999997</v>
+      </c>
+      <c r="G303" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H303" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I303" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="J303">
+        <v>12</v>
+      </c>
+      <c r="K303" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="304" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A304">
+        <v>7</v>
+      </c>
+      <c r="B304" t="s">
+        <v>388</v>
+      </c>
+      <c r="C304" t="s">
+        <v>60</v>
+      </c>
+      <c r="D304">
+        <v>6.7629999999999999</v>
+      </c>
+      <c r="G304" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H304" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I304" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="J304">
+        <v>12</v>
+      </c>
+      <c r="K304" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="305" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A305">
+        <v>8</v>
+      </c>
+      <c r="B305" t="s">
+        <v>388</v>
+      </c>
+      <c r="C305" t="s">
+        <v>59</v>
+      </c>
+      <c r="D305">
+        <v>8.6720000000000006</v>
+      </c>
+      <c r="G305" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H305" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I305" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="J305">
+        <v>12</v>
+      </c>
+      <c r="K305" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="306" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A306">
+        <v>9</v>
+      </c>
+      <c r="B306" t="s">
+        <v>388</v>
+      </c>
+      <c r="C306" t="s">
+        <v>60</v>
+      </c>
+      <c r="D306">
+        <v>7.6029999999999998</v>
+      </c>
+      <c r="G306" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H306" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I306" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="J306">
+        <v>12</v>
+      </c>
+      <c r="K306" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="307" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A307">
+        <v>10</v>
+      </c>
+      <c r="B307" t="s">
+        <v>388</v>
+      </c>
+      <c r="C307" t="s">
+        <v>60</v>
+      </c>
+      <c r="D307">
+        <v>6.6710000000000003</v>
+      </c>
+      <c r="G307" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H307" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I307" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="J307">
+        <v>12</v>
+      </c>
+      <c r="K307" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="308" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A308">
+        <v>11</v>
+      </c>
+      <c r="B308" t="s">
+        <v>388</v>
+      </c>
+      <c r="C308" t="s">
+        <v>59</v>
+      </c>
+      <c r="D308">
+        <v>9.8219999999999992</v>
+      </c>
+      <c r="G308" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H308" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I308" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="J308">
+        <v>12</v>
+      </c>
+      <c r="K308" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="309" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A309">
+        <v>12</v>
+      </c>
+      <c r="B309" t="s">
+        <v>388</v>
+      </c>
+      <c r="C309" t="s">
+        <v>60</v>
+      </c>
+      <c r="D309">
+        <v>7.8040000000000003</v>
+      </c>
+      <c r="G309" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H309" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I309" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="J309">
+        <v>12</v>
+      </c>
+      <c r="K309" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="310" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A310">
+        <v>13</v>
+      </c>
+      <c r="B310" t="s">
+        <v>388</v>
+      </c>
+      <c r="C310" t="s">
+        <v>60</v>
+      </c>
+      <c r="D310">
+        <v>3.76</v>
+      </c>
+      <c r="G310" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H310" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I310" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="J310">
+        <v>12</v>
+      </c>
+      <c r="K310" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="311" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A311">
+        <v>14</v>
+      </c>
+      <c r="B311" t="s">
+        <v>388</v>
+      </c>
+      <c r="C311" t="s">
+        <v>59</v>
+      </c>
+      <c r="D311">
+        <v>7.6929999999999996</v>
+      </c>
+      <c r="G311" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H311" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I311" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="J311">
+        <v>12</v>
+      </c>
+      <c r="K311" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="312" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A312">
+        <v>15</v>
+      </c>
+      <c r="B312" t="s">
+        <v>388</v>
+      </c>
+      <c r="C312" t="s">
+        <v>60</v>
+      </c>
+      <c r="D312">
+        <v>5.6</v>
+      </c>
+      <c r="G312" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H312" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I312" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="J312">
+        <v>12</v>
+      </c>
+      <c r="K312" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="313" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A313">
+        <v>16</v>
+      </c>
+      <c r="B313" t="s">
+        <v>388</v>
+      </c>
+      <c r="C313" t="s">
+        <v>60</v>
+      </c>
+      <c r="D313">
+        <v>8.48</v>
+      </c>
+      <c r="G313" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H313" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I313" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="J313">
+        <v>12</v>
+      </c>
+      <c r="K313" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="314" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A314">
+        <v>17</v>
+      </c>
+      <c r="B314" t="s">
+        <v>388</v>
+      </c>
+      <c r="C314" t="s">
+        <v>59</v>
+      </c>
+      <c r="D314">
+        <v>9.8160000000000007</v>
+      </c>
+      <c r="G314" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H314" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I314" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="J314">
+        <v>12</v>
+      </c>
+      <c r="K314" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="315" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A315">
+        <v>18</v>
+      </c>
+      <c r="B315" t="s">
+        <v>388</v>
+      </c>
+      <c r="C315" t="s">
+        <v>59</v>
+      </c>
+      <c r="D315">
+        <v>6.5</v>
+      </c>
+      <c r="G315" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H315" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I315" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="J315">
+        <v>12</v>
+      </c>
+      <c r="K315" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="316" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A316">
+        <v>19</v>
+      </c>
+      <c r="B316" t="s">
+        <v>388</v>
+      </c>
+      <c r="C316" t="s">
+        <v>60</v>
+      </c>
+      <c r="D316">
+        <v>5.49</v>
+      </c>
+      <c r="G316" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H316" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I316" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="J316">
+        <v>12</v>
+      </c>
+      <c r="K316" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="317" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A317">
+        <v>20</v>
+      </c>
+      <c r="B317" t="s">
+        <v>388</v>
+      </c>
+      <c r="C317" t="s">
+        <v>59</v>
+      </c>
+      <c r="D317">
+        <v>8.3529999999999998</v>
+      </c>
+      <c r="G317" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H317" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I317" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="J317">
+        <v>12</v>
+      </c>
+      <c r="K317" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="318" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A318">
+        <v>21</v>
+      </c>
+      <c r="B318" t="s">
+        <v>90</v>
+      </c>
+      <c r="C318" t="s">
+        <v>233</v>
+      </c>
+      <c r="G318" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H318" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I318" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="J318">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="319" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A319">
+        <v>22</v>
+      </c>
+      <c r="B319" t="s">
+        <v>90</v>
+      </c>
+      <c r="C319" t="s">
+        <v>233</v>
+      </c>
+      <c r="E319" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="G319" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H319" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I319" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="J319">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -16343,14 +17627,14 @@
       <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>45</v>
       </c>
@@ -16379,7 +17663,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>58</v>
       </c>
@@ -16409,7 +17693,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>58</v>
       </c>
@@ -16439,169 +17723,169 @@
         <v>109</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I11">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I17">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I19">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I20">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I21">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I22">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I23">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I24">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I25">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I26">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I27">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I30">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>229</v>
       </c>

</xml_diff>

<commit_message>
adding collection information of pupae
</commit_message>
<xml_diff>
--- a/Data/2018-08-14_master_datac_2018_collection_year.xlsx
+++ b/Data/2018-08-14_master_datac_2018_collection_year.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andrew.nguyen\Desktop\Circadian_rhythm_runs_seasonal_timing\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38B2D309-CA2E-444E-A66E-C4F5E8AAD831}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9A0C79D-E770-4DBB-9409-72BD73262540}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1800" yWindow="1935" windowWidth="48495" windowHeight="26115" activeTab="1" xr2:uid="{C7477166-8A7C-B04A-9643-C277FEDCDAAB}"/>
+    <workbookView xWindow="1800" yWindow="1935" windowWidth="48495" windowHeight="26115" xr2:uid="{C7477166-8A7C-B04A-9643-C277FEDCDAAB}"/>
   </bookViews>
   <sheets>
     <sheet name="Maggot_Collections" sheetId="2" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3556" uniqueCount="393">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3566" uniqueCount="395">
   <si>
     <t>Ind_ID</t>
   </si>
@@ -1211,6 +1211,12 @@
   </si>
   <si>
     <t>13:38</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>36</t>
   </si>
 </sst>
 </file>
@@ -1631,8 +1637,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D3F78F5-4EA8-6A42-B216-41A8EC7A5E8D}">
   <dimension ref="A1:Z102"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1:J1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5625,15 +5631,36 @@
       <c r="Z73" s="14"/>
     </row>
     <row r="74" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A74" s="1"/>
-      <c r="B74" s="1"/>
-      <c r="C74" s="1"/>
-      <c r="E74" s="1"/>
-      <c r="F74" s="1"/>
-      <c r="G74" s="1"/>
-      <c r="H74" s="1"/>
-      <c r="I74" s="1"/>
-      <c r="J74" s="1"/>
+      <c r="A74" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="F74" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="G74" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="H74" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="I74" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="J74" s="1" t="s">
+        <v>78</v>
+      </c>
       <c r="K74" s="1"/>
       <c r="L74" s="1"/>
       <c r="M74" s="1"/>
@@ -6417,7 +6444,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92725FB9-1A17-2546-9DFA-6C0D39437891}">
   <dimension ref="A1:AS319"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A292" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D318" sqref="D318"/>
     </sheetView>

</xml_diff>

<commit_message>
making new folder for respirometry raw data to distringuish between years
processing 2018 respo data so far
</commit_message>
<xml_diff>
--- a/Data/2018-08-14_master_datac_2018_collection_year.xlsx
+++ b/Data/2018-08-14_master_datac_2018_collection_year.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andrew.nguyen\Desktop\Circadian_rhythm_runs_seasonal_timing\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9A0C79D-E770-4DBB-9409-72BD73262540}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1C61B09-CEF1-43CC-8642-1A18198F3EDD}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1800" yWindow="1935" windowWidth="48495" windowHeight="26115" xr2:uid="{C7477166-8A7C-B04A-9643-C277FEDCDAAB}"/>
+    <workbookView xWindow="1800" yWindow="1935" windowWidth="48495" windowHeight="26115" activeTab="1" xr2:uid="{C7477166-8A7C-B04A-9643-C277FEDCDAAB}"/>
   </bookViews>
   <sheets>
     <sheet name="Maggot_Collections" sheetId="2" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3566" uniqueCount="395">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3568" uniqueCount="395">
   <si>
     <t>Ind_ID</t>
   </si>
@@ -1286,7 +1286,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -1321,6 +1321,8 @@
     <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1637,8 +1639,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D3F78F5-4EA8-6A42-B216-41A8EC7A5E8D}">
   <dimension ref="A1:Z102"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:J1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -6444,9 +6446,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92725FB9-1A17-2546-9DFA-6C0D39437891}">
   <dimension ref="A1:AS319"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A292" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D318" sqref="D318"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A285" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L276" sqref="L276:L297"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -9655,6 +9657,15 @@
       <c r="K92" t="s">
         <v>61</v>
       </c>
+      <c r="L92">
+        <v>6262</v>
+      </c>
+      <c r="M92" s="20">
+        <v>0.47093750000000001</v>
+      </c>
+      <c r="N92">
+        <v>0.1970401</v>
+      </c>
       <c r="T92" s="1" t="s">
         <v>73</v>
       </c>
@@ -9696,6 +9707,15 @@
       <c r="K93" t="s">
         <v>61</v>
       </c>
+      <c r="L93">
+        <v>6262</v>
+      </c>
+      <c r="M93" s="20">
+        <v>0.47167824074074072</v>
+      </c>
+      <c r="N93">
+        <v>0.13336590000000001</v>
+      </c>
       <c r="T93" s="1" t="s">
         <v>73</v>
       </c>
@@ -9734,6 +9754,15 @@
       <c r="K94" t="s">
         <v>61</v>
       </c>
+      <c r="L94">
+        <v>6262</v>
+      </c>
+      <c r="M94" s="20">
+        <v>0.4725462962962963</v>
+      </c>
+      <c r="N94">
+        <v>0.74489930000000004</v>
+      </c>
       <c r="T94" s="1" t="s">
         <v>73</v>
       </c>
@@ -9772,6 +9801,15 @@
       <c r="K95" t="s">
         <v>61</v>
       </c>
+      <c r="L95">
+        <v>6262</v>
+      </c>
+      <c r="M95" s="20">
+        <v>0.47342592592592592</v>
+      </c>
+      <c r="N95">
+        <v>0.85287159999999995</v>
+      </c>
       <c r="T95" s="1" t="s">
         <v>73</v>
       </c>
@@ -9813,6 +9851,15 @@
       <c r="K96" t="s">
         <v>61</v>
       </c>
+      <c r="L96">
+        <v>6262</v>
+      </c>
+      <c r="M96" s="20">
+        <v>0.47438657407407409</v>
+      </c>
+      <c r="N96">
+        <v>0.13788710000000001</v>
+      </c>
       <c r="T96" s="1" t="s">
         <v>73</v>
       </c>
@@ -9854,6 +9901,15 @@
       <c r="K97" t="s">
         <v>61</v>
       </c>
+      <c r="L97">
+        <v>6262</v>
+      </c>
+      <c r="M97" s="20">
+        <v>0.47538194444444448</v>
+      </c>
+      <c r="N97">
+        <v>0.2489103</v>
+      </c>
       <c r="T97" s="1" t="s">
         <v>73</v>
       </c>
@@ -9892,6 +9948,15 @@
       <c r="K98" t="s">
         <v>61</v>
       </c>
+      <c r="L98">
+        <v>6262</v>
+      </c>
+      <c r="M98" s="20">
+        <v>0.47619212962962965</v>
+      </c>
+      <c r="N98">
+        <v>0.3853647</v>
+      </c>
       <c r="T98" s="1" t="s">
         <v>73</v>
       </c>
@@ -9933,6 +9998,15 @@
       <c r="K99" t="s">
         <v>61</v>
       </c>
+      <c r="L99">
+        <v>6262</v>
+      </c>
+      <c r="M99" s="20">
+        <v>0.47695601851851849</v>
+      </c>
+      <c r="N99">
+        <v>1.2578400000000001</v>
+      </c>
       <c r="T99" s="1" t="s">
         <v>73</v>
       </c>
@@ -9974,6 +10048,15 @@
       <c r="K100" t="s">
         <v>61</v>
       </c>
+      <c r="L100">
+        <v>6262</v>
+      </c>
+      <c r="M100" s="20">
+        <v>0.47784722222222226</v>
+      </c>
+      <c r="N100">
+        <v>0.1002569</v>
+      </c>
       <c r="T100" s="1" t="s">
         <v>73</v>
       </c>
@@ -10015,6 +10098,15 @@
       <c r="K101" t="s">
         <v>61</v>
       </c>
+      <c r="L101">
+        <v>6262</v>
+      </c>
+      <c r="M101" s="20">
+        <v>0.47856481481481478</v>
+      </c>
+      <c r="N101">
+        <v>1.1946300000000001</v>
+      </c>
       <c r="T101" s="1" t="s">
         <v>73</v>
       </c>
@@ -10056,6 +10148,15 @@
       <c r="K102" t="s">
         <v>61</v>
       </c>
+      <c r="L102">
+        <v>6262</v>
+      </c>
+      <c r="M102" s="20">
+        <v>0.47949074074074072</v>
+      </c>
+      <c r="N102">
+        <v>1.2690429999999999</v>
+      </c>
       <c r="T102" s="1" t="s">
         <v>73</v>
       </c>
@@ -10094,6 +10195,15 @@
       <c r="K103" t="s">
         <v>61</v>
       </c>
+      <c r="L103">
+        <v>6262</v>
+      </c>
+      <c r="M103" s="20">
+        <v>0.48037037037037034</v>
+      </c>
+      <c r="N103">
+        <v>1.4929490000000001</v>
+      </c>
       <c r="T103" s="1" t="s">
         <v>73</v>
       </c>
@@ -10135,6 +10245,15 @@
       <c r="K104" t="s">
         <v>61</v>
       </c>
+      <c r="L104">
+        <v>6262</v>
+      </c>
+      <c r="M104" s="20">
+        <v>0.48130787037037037</v>
+      </c>
+      <c r="N104">
+        <v>0.14917730000000001</v>
+      </c>
       <c r="T104" s="1" t="s">
         <v>73</v>
       </c>
@@ -10176,6 +10295,15 @@
       <c r="K105" t="s">
         <v>61</v>
       </c>
+      <c r="L105">
+        <v>6262</v>
+      </c>
+      <c r="M105" s="20">
+        <v>0.48201388888888891</v>
+      </c>
+      <c r="N105">
+        <v>0.1464047</v>
+      </c>
       <c r="T105" s="1" t="s">
         <v>73</v>
       </c>
@@ -10217,6 +10345,15 @@
       <c r="K106" t="s">
         <v>61</v>
       </c>
+      <c r="L106">
+        <v>6262</v>
+      </c>
+      <c r="M106" s="20">
+        <v>0.48284722222222221</v>
+      </c>
+      <c r="N106">
+        <v>0.61558199999999996</v>
+      </c>
       <c r="T106" s="1" t="s">
         <v>73</v>
       </c>
@@ -10258,6 +10395,15 @@
       <c r="K107" t="s">
         <v>61</v>
       </c>
+      <c r="L107">
+        <v>6262</v>
+      </c>
+      <c r="M107" s="20">
+        <v>0.48363425925925929</v>
+      </c>
+      <c r="N107">
+        <v>0.2616211</v>
+      </c>
       <c r="T107" s="1" t="s">
         <v>73</v>
       </c>
@@ -10299,6 +10445,15 @@
       <c r="K108" t="s">
         <v>61</v>
       </c>
+      <c r="L108">
+        <v>6262</v>
+      </c>
+      <c r="M108" s="20">
+        <v>0.48434027777777783</v>
+      </c>
+      <c r="N108">
+        <v>0.2566137</v>
+      </c>
       <c r="T108" s="1" t="s">
         <v>73</v>
       </c>
@@ -10337,6 +10492,15 @@
       <c r="K109" t="s">
         <v>61</v>
       </c>
+      <c r="L109">
+        <v>6262</v>
+      </c>
+      <c r="M109" s="20">
+        <v>0.48504629629629631</v>
+      </c>
+      <c r="N109">
+        <v>0.1296766</v>
+      </c>
       <c r="T109" s="1" t="s">
         <v>73</v>
       </c>
@@ -10378,6 +10542,15 @@
       <c r="K110" t="s">
         <v>61</v>
       </c>
+      <c r="L110">
+        <v>6262</v>
+      </c>
+      <c r="M110" s="20">
+        <v>0.48574074074074075</v>
+      </c>
+      <c r="N110">
+        <v>0.89022429999999997</v>
+      </c>
       <c r="T110" s="1" t="s">
         <v>73</v>
       </c>
@@ -10416,6 +10589,15 @@
       <c r="K111" t="s">
         <v>61</v>
       </c>
+      <c r="L111">
+        <v>6262</v>
+      </c>
+      <c r="M111" s="20">
+        <v>0.48659722222222218</v>
+      </c>
+      <c r="N111">
+        <v>0.70833469999999998</v>
+      </c>
       <c r="T111" s="1" t="s">
         <v>73</v>
       </c>
@@ -10457,6 +10639,15 @@
       <c r="K112" t="s">
         <v>61</v>
       </c>
+      <c r="L112">
+        <v>6262</v>
+      </c>
+      <c r="M112" s="20">
+        <v>0.48748842592592595</v>
+      </c>
+      <c r="N112">
+        <v>0.1138883</v>
+      </c>
       <c r="T112" s="1" t="s">
         <v>73</v>
       </c>
@@ -10498,6 +10689,15 @@
       <c r="K113" t="s">
         <v>61</v>
       </c>
+      <c r="L113">
+        <v>6262</v>
+      </c>
+      <c r="M113" s="20">
+        <v>0.48832175925925925</v>
+      </c>
+      <c r="N113">
+        <v>0.6530359</v>
+      </c>
       <c r="T113" s="1" t="s">
         <v>73</v>
       </c>
@@ -10536,6 +10736,15 @@
       <c r="K114" t="s">
         <v>61</v>
       </c>
+      <c r="L114">
+        <v>6262</v>
+      </c>
+      <c r="M114" s="20">
+        <v>0.48907407407407405</v>
+      </c>
+      <c r="N114">
+        <v>0.15391759999999999</v>
+      </c>
       <c r="T114" s="1" t="s">
         <v>73</v>
       </c>
@@ -10577,6 +10786,15 @@
       <c r="K115" t="s">
         <v>61</v>
       </c>
+      <c r="L115">
+        <v>6262</v>
+      </c>
+      <c r="M115" s="20">
+        <v>0.4899074074074074</v>
+      </c>
+      <c r="N115">
+        <v>0.1257113</v>
+      </c>
       <c r="T115" s="1" t="s">
         <v>73</v>
       </c>
@@ -10615,6 +10833,15 @@
       <c r="K116" t="s">
         <v>61</v>
       </c>
+      <c r="L116">
+        <v>6262</v>
+      </c>
+      <c r="M116" s="20">
+        <v>0.49062500000000003</v>
+      </c>
+      <c r="N116">
+        <v>0.3096526</v>
+      </c>
       <c r="T116" s="1" t="s">
         <v>73</v>
       </c>
@@ -10656,6 +10883,15 @@
       <c r="K117" t="s">
         <v>61</v>
       </c>
+      <c r="L117">
+        <v>6262</v>
+      </c>
+      <c r="M117" s="20">
+        <v>0.49136574074074074</v>
+      </c>
+      <c r="N117">
+        <v>0.17303840000000001</v>
+      </c>
       <c r="T117" s="1" t="s">
         <v>73</v>
       </c>
@@ -10694,6 +10930,15 @@
       <c r="K118" t="s">
         <v>61</v>
       </c>
+      <c r="L118">
+        <v>6262</v>
+      </c>
+      <c r="M118" s="20">
+        <v>0.49208333333333337</v>
+      </c>
+      <c r="N118">
+        <v>0.81787480000000001</v>
+      </c>
       <c r="T118" s="1" t="s">
         <v>73</v>
       </c>
@@ -10732,6 +10977,15 @@
       <c r="K119" t="s">
         <v>61</v>
       </c>
+      <c r="L119">
+        <v>6262</v>
+      </c>
+      <c r="M119" s="20">
+        <v>0.49296296296296299</v>
+      </c>
+      <c r="N119">
+        <v>1.1387959999999999</v>
+      </c>
       <c r="T119" s="1" t="s">
         <v>73</v>
       </c>
@@ -10773,6 +11027,15 @@
       <c r="K120" t="s">
         <v>61</v>
       </c>
+      <c r="L120">
+        <v>6262</v>
+      </c>
+      <c r="M120" s="20">
+        <v>0.49381944444444442</v>
+      </c>
+      <c r="N120">
+        <v>0.30968760000000001</v>
+      </c>
       <c r="T120" s="1" t="s">
         <v>73</v>
       </c>
@@ -10814,6 +11077,15 @@
       <c r="K121" t="s">
         <v>61</v>
       </c>
+      <c r="L121">
+        <v>6262</v>
+      </c>
+      <c r="M121" s="20">
+        <v>0.49454861111111109</v>
+      </c>
+      <c r="N121">
+        <v>1.482758</v>
+      </c>
       <c r="T121" s="1" t="s">
         <v>73</v>
       </c>
@@ -10852,6 +11124,15 @@
       <c r="K122" t="s">
         <v>61</v>
       </c>
+      <c r="L122">
+        <v>6262</v>
+      </c>
+      <c r="M122" s="20">
+        <v>0.49539351851851854</v>
+      </c>
+      <c r="N122">
+        <v>0.92802739999999995</v>
+      </c>
       <c r="T122" s="1" t="s">
         <v>73</v>
       </c>
@@ -10893,6 +11174,15 @@
       <c r="K123" t="s">
         <v>61</v>
       </c>
+      <c r="L123">
+        <v>6262</v>
+      </c>
+      <c r="M123" s="20">
+        <v>0.49625000000000002</v>
+      </c>
+      <c r="N123" s="21">
+        <v>7.1121240000000002E-2</v>
+      </c>
       <c r="T123" s="1" t="s">
         <v>73</v>
       </c>
@@ -10931,6 +11221,15 @@
       <c r="K124" t="s">
         <v>61</v>
       </c>
+      <c r="L124">
+        <v>6262</v>
+      </c>
+      <c r="M124" s="20">
+        <v>0.49715277777777778</v>
+      </c>
+      <c r="N124">
+        <v>0.12740109999999999</v>
+      </c>
       <c r="T124" s="1" t="s">
         <v>73</v>
       </c>
@@ -10969,6 +11268,15 @@
       <c r="K125" t="s">
         <v>61</v>
       </c>
+      <c r="L125">
+        <v>6262</v>
+      </c>
+      <c r="M125" s="20">
+        <v>0.49784722222222227</v>
+      </c>
+      <c r="N125">
+        <v>0.98314860000000004</v>
+      </c>
       <c r="T125" s="1" t="s">
         <v>73</v>
       </c>
@@ -11010,6 +11318,15 @@
       <c r="K126" t="s">
         <v>61</v>
       </c>
+      <c r="L126">
+        <v>6262</v>
+      </c>
+      <c r="M126" s="20">
+        <v>0.49873842592592593</v>
+      </c>
+      <c r="N126">
+        <v>1.0477609999999999</v>
+      </c>
       <c r="T126" s="1" t="s">
         <v>73</v>
       </c>
@@ -11051,6 +11368,15 @@
       <c r="K127" t="s">
         <v>61</v>
       </c>
+      <c r="L127">
+        <v>6262</v>
+      </c>
+      <c r="M127" s="20">
+        <v>0.51457175925925924</v>
+      </c>
+      <c r="N127">
+        <v>0.109638</v>
+      </c>
       <c r="T127" s="1" t="s">
         <v>73</v>
       </c>
@@ -11089,6 +11415,15 @@
       <c r="K128" t="s">
         <v>61</v>
       </c>
+      <c r="L128">
+        <v>6262</v>
+      </c>
+      <c r="M128" s="20">
+        <v>0.51545138888888886</v>
+      </c>
+      <c r="N128">
+        <v>1.4345509999999999</v>
+      </c>
       <c r="T128" s="1" t="s">
         <v>73</v>
       </c>
@@ -11130,6 +11465,15 @@
       <c r="K129" t="s">
         <v>61</v>
       </c>
+      <c r="L129">
+        <v>6262</v>
+      </c>
+      <c r="M129" s="20">
+        <v>0.51640046296296294</v>
+      </c>
+      <c r="N129">
+        <v>1.2323409999999999</v>
+      </c>
       <c r="T129" s="1" t="s">
         <v>73</v>
       </c>
@@ -11171,6 +11515,15 @@
       <c r="K130" t="s">
         <v>61</v>
       </c>
+      <c r="L130">
+        <v>6262</v>
+      </c>
+      <c r="M130" s="20">
+        <v>0.51728009259259256</v>
+      </c>
+      <c r="N130">
+        <v>3.2334070000000001</v>
+      </c>
       <c r="T130" s="1" t="s">
         <v>73</v>
       </c>
@@ -11212,6 +11565,15 @@
       <c r="K131" t="s">
         <v>61</v>
       </c>
+      <c r="L131">
+        <v>6262</v>
+      </c>
+      <c r="M131" s="20">
+        <v>0.51832175925925927</v>
+      </c>
+      <c r="N131">
+        <v>0.13739380000000001</v>
+      </c>
       <c r="T131" s="1" t="s">
         <v>73</v>
       </c>
@@ -11250,6 +11612,15 @@
       <c r="K132" t="s">
         <v>61</v>
       </c>
+      <c r="L132">
+        <v>6262</v>
+      </c>
+      <c r="M132" s="20">
+        <v>0.51903935185185179</v>
+      </c>
+      <c r="N132">
+        <v>0.1400179</v>
+      </c>
       <c r="T132" s="1" t="s">
         <v>73</v>
       </c>
@@ -11291,6 +11662,15 @@
       <c r="K133" t="s">
         <v>61</v>
       </c>
+      <c r="L133">
+        <v>6262</v>
+      </c>
+      <c r="M133" s="20">
+        <v>0.51986111111111111</v>
+      </c>
+      <c r="N133">
+        <v>1.369402</v>
+      </c>
       <c r="T133" s="1" t="s">
         <v>73</v>
       </c>
@@ -11332,6 +11712,15 @@
       <c r="K134" t="s">
         <v>61</v>
       </c>
+      <c r="L134">
+        <v>6262</v>
+      </c>
+      <c r="M134" s="20">
+        <v>0.52076388888888892</v>
+      </c>
+      <c r="N134">
+        <v>0.1629767</v>
+      </c>
       <c r="T134" s="1" t="s">
         <v>73</v>
       </c>
@@ -11370,6 +11759,15 @@
       <c r="K135" t="s">
         <v>61</v>
       </c>
+      <c r="L135">
+        <v>6262</v>
+      </c>
+      <c r="M135" s="20">
+        <v>0.52152777777777781</v>
+      </c>
+      <c r="N135">
+        <v>0.165682</v>
+      </c>
       <c r="T135" s="1" t="s">
         <v>73</v>
       </c>
@@ -11411,6 +11809,15 @@
       <c r="K136" t="s">
         <v>61</v>
       </c>
+      <c r="L136">
+        <v>6262</v>
+      </c>
+      <c r="M136" s="20">
+        <v>0.52258101851851857</v>
+      </c>
+      <c r="N136">
+        <v>0.1706609</v>
+      </c>
       <c r="T136" s="1" t="s">
         <v>73</v>
       </c>
@@ -11446,6 +11853,15 @@
       <c r="K137" t="s">
         <v>61</v>
       </c>
+      <c r="L137">
+        <v>6262</v>
+      </c>
+      <c r="M137" s="20">
+        <v>0.52347222222222223</v>
+      </c>
+      <c r="N137" s="21">
+        <v>1.517576E-2</v>
+      </c>
       <c r="T137" s="1" t="s">
         <v>73</v>
       </c>
@@ -11478,6 +11894,15 @@
       <c r="K138" t="s">
         <v>61</v>
       </c>
+      <c r="L138">
+        <v>6262</v>
+      </c>
+      <c r="M138" s="20">
+        <v>0.52417824074074071</v>
+      </c>
+      <c r="N138" s="21">
+        <v>1.5057539999999999E-2</v>
+      </c>
       <c r="T138" s="1" t="s">
         <v>73</v>
       </c>
@@ -11513,6 +11938,15 @@
       <c r="K139" t="s">
         <v>61</v>
       </c>
+      <c r="L139">
+        <v>7000</v>
+      </c>
+      <c r="M139" s="20">
+        <v>0.47093750000000001</v>
+      </c>
+      <c r="N139" s="21">
+        <v>5.1285450000000003E-2</v>
+      </c>
       <c r="T139" s="1" t="s">
         <v>73</v>
       </c>
@@ -11551,6 +11985,15 @@
       <c r="K140" t="s">
         <v>61</v>
       </c>
+      <c r="L140">
+        <v>7000</v>
+      </c>
+      <c r="M140" s="20">
+        <v>0.47167824074074072</v>
+      </c>
+      <c r="N140">
+        <v>0.58465710000000004</v>
+      </c>
       <c r="T140" s="1" t="s">
         <v>73</v>
       </c>
@@ -11592,6 +12035,15 @@
       <c r="K141" t="s">
         <v>61</v>
       </c>
+      <c r="L141">
+        <v>7000</v>
+      </c>
+      <c r="M141" s="20">
+        <v>0.4725462962962963</v>
+      </c>
+      <c r="N141" s="21">
+        <v>9.7062759999999998E-2</v>
+      </c>
       <c r="T141" s="1" t="s">
         <v>73</v>
       </c>
@@ -11633,6 +12085,15 @@
       <c r="K142" t="s">
         <v>61</v>
       </c>
+      <c r="L142">
+        <v>7000</v>
+      </c>
+      <c r="M142" s="20">
+        <v>0.47342592592592592</v>
+      </c>
+      <c r="N142">
+        <v>0.64936369999999999</v>
+      </c>
       <c r="T142" s="1" t="s">
         <v>73</v>
       </c>
@@ -11674,6 +12135,15 @@
       <c r="K143" t="s">
         <v>61</v>
       </c>
+      <c r="L143">
+        <v>7000</v>
+      </c>
+      <c r="M143" s="20">
+        <v>0.47438657407407409</v>
+      </c>
+      <c r="N143">
+        <v>1.50685</v>
+      </c>
       <c r="T143" s="1" t="s">
         <v>73</v>
       </c>
@@ -11715,6 +12185,15 @@
       <c r="K144" t="s">
         <v>61</v>
       </c>
+      <c r="L144">
+        <v>7000</v>
+      </c>
+      <c r="M144" s="20">
+        <v>0.47538194444444448</v>
+      </c>
+      <c r="N144">
+        <v>0.17113790000000001</v>
+      </c>
       <c r="T144" s="1" t="s">
         <v>73</v>
       </c>
@@ -11756,6 +12235,15 @@
       <c r="K145" t="s">
         <v>61</v>
       </c>
+      <c r="L145">
+        <v>7000</v>
+      </c>
+      <c r="M145" s="20">
+        <v>0.47619212962962965</v>
+      </c>
+      <c r="N145">
+        <v>9.6943799999999997E-2</v>
+      </c>
       <c r="T145" s="1" t="s">
         <v>73</v>
       </c>
@@ -11797,6 +12285,15 @@
       <c r="K146" t="s">
         <v>61</v>
       </c>
+      <c r="L146">
+        <v>7000</v>
+      </c>
+      <c r="M146" s="20">
+        <v>0.47695601851851849</v>
+      </c>
+      <c r="N146">
+        <v>0.4973764</v>
+      </c>
       <c r="T146" s="1" t="s">
         <v>73</v>
       </c>
@@ -11838,6 +12335,15 @@
       <c r="K147" t="s">
         <v>61</v>
       </c>
+      <c r="L147">
+        <v>7000</v>
+      </c>
+      <c r="M147" s="20">
+        <v>0.47784722222222226</v>
+      </c>
+      <c r="N147" s="21">
+        <v>7.759228E-2</v>
+      </c>
       <c r="T147" s="1" t="s">
         <v>73</v>
       </c>
@@ -11876,6 +12382,15 @@
       <c r="K148" t="s">
         <v>61</v>
       </c>
+      <c r="L148">
+        <v>7000</v>
+      </c>
+      <c r="M148" s="20">
+        <v>0.47856481481481478</v>
+      </c>
+      <c r="N148" s="21">
+        <v>7.1666450000000007E-2</v>
+      </c>
       <c r="T148" s="1" t="s">
         <v>73</v>
       </c>
@@ -11917,6 +12432,15 @@
       <c r="K149" t="s">
         <v>61</v>
       </c>
+      <c r="L149">
+        <v>7000</v>
+      </c>
+      <c r="M149" s="20">
+        <v>0.47949074074074072</v>
+      </c>
+      <c r="N149">
+        <v>0.46812979999999998</v>
+      </c>
       <c r="T149" s="1" t="s">
         <v>73</v>
       </c>
@@ -11955,6 +12479,15 @@
       <c r="K150" t="s">
         <v>61</v>
       </c>
+      <c r="L150">
+        <v>7000</v>
+      </c>
+      <c r="M150" s="20">
+        <v>0.48037037037037034</v>
+      </c>
+      <c r="N150">
+        <v>0.13641529999999999</v>
+      </c>
       <c r="T150" s="1" t="s">
         <v>73</v>
       </c>
@@ -11993,6 +12526,15 @@
       <c r="K151" t="s">
         <v>61</v>
       </c>
+      <c r="L151">
+        <v>7000</v>
+      </c>
+      <c r="M151" s="20">
+        <v>0.48130787037037037</v>
+      </c>
+      <c r="N151">
+        <v>0.1132746</v>
+      </c>
       <c r="T151" s="1" t="s">
         <v>73</v>
       </c>
@@ -12034,6 +12576,15 @@
       <c r="K152" t="s">
         <v>61</v>
       </c>
+      <c r="L152">
+        <v>7000</v>
+      </c>
+      <c r="M152" s="20">
+        <v>0.48201388888888891</v>
+      </c>
+      <c r="N152">
+        <v>0.85572360000000003</v>
+      </c>
       <c r="T152" s="1" t="s">
         <v>73</v>
       </c>
@@ -12075,6 +12626,15 @@
       <c r="K153" t="s">
         <v>61</v>
       </c>
+      <c r="L153">
+        <v>7000</v>
+      </c>
+      <c r="M153" s="20">
+        <v>0.48284722222222221</v>
+      </c>
+      <c r="N153">
+        <v>0.15050740000000001</v>
+      </c>
       <c r="T153" s="1" t="s">
         <v>73</v>
       </c>
@@ -12116,6 +12676,15 @@
       <c r="K154" t="s">
         <v>61</v>
       </c>
+      <c r="L154">
+        <v>7000</v>
+      </c>
+      <c r="M154" s="20">
+        <v>0.48363425925925929</v>
+      </c>
+      <c r="N154" s="21">
+        <v>5.9912069999999998E-2</v>
+      </c>
       <c r="T154" s="1" t="s">
         <v>73</v>
       </c>
@@ -12154,6 +12723,15 @@
       <c r="K155" t="s">
         <v>61</v>
       </c>
+      <c r="L155">
+        <v>7000</v>
+      </c>
+      <c r="M155" s="20">
+        <v>0.48434027777777783</v>
+      </c>
+      <c r="N155">
+        <v>0.12034</v>
+      </c>
       <c r="T155" s="1" t="s">
         <v>73</v>
       </c>
@@ -12195,6 +12773,15 @@
       <c r="K156" t="s">
         <v>61</v>
       </c>
+      <c r="L156">
+        <v>7000</v>
+      </c>
+      <c r="M156" s="20">
+        <v>0.48504629629629631</v>
+      </c>
+      <c r="N156" s="21">
+        <v>8.0263559999999998E-2</v>
+      </c>
       <c r="T156" s="1" t="s">
         <v>73</v>
       </c>
@@ -12236,6 +12823,15 @@
       <c r="K157" t="s">
         <v>61</v>
       </c>
+      <c r="L157">
+        <v>7000</v>
+      </c>
+      <c r="M157" s="20">
+        <v>0.48574074074074075</v>
+      </c>
+      <c r="N157">
+        <v>0.70180109999999996</v>
+      </c>
       <c r="T157" s="1" t="s">
         <v>73</v>
       </c>
@@ -12277,6 +12873,15 @@
       <c r="K158" t="s">
         <v>61</v>
       </c>
+      <c r="L158">
+        <v>7000</v>
+      </c>
+      <c r="M158" s="20">
+        <v>0.48659722222222218</v>
+      </c>
+      <c r="N158">
+        <v>0.92372509999999997</v>
+      </c>
       <c r="T158" s="1" t="s">
         <v>73</v>
       </c>
@@ -12315,6 +12920,15 @@
       <c r="K159" t="s">
         <v>61</v>
       </c>
+      <c r="L159">
+        <v>7000</v>
+      </c>
+      <c r="M159" s="20">
+        <v>0.48748842592592595</v>
+      </c>
+      <c r="N159">
+        <v>0.77597720000000003</v>
+      </c>
       <c r="T159" s="1" t="s">
         <v>73</v>
       </c>
@@ -12356,6 +12970,15 @@
       <c r="K160" t="s">
         <v>61</v>
       </c>
+      <c r="L160">
+        <v>7000</v>
+      </c>
+      <c r="M160" s="20">
+        <v>0.48832175925925925</v>
+      </c>
+      <c r="N160">
+        <v>0.1450272</v>
+      </c>
       <c r="T160" s="1" t="s">
         <v>73</v>
       </c>
@@ -12394,6 +13017,15 @@
       <c r="K161" t="s">
         <v>61</v>
       </c>
+      <c r="L161">
+        <v>7000</v>
+      </c>
+      <c r="M161" s="20">
+        <v>0.48907407407407405</v>
+      </c>
+      <c r="N161">
+        <v>0.73810480000000001</v>
+      </c>
       <c r="T161" s="1" t="s">
         <v>73</v>
       </c>
@@ -12435,6 +13067,15 @@
       <c r="K162" t="s">
         <v>61</v>
       </c>
+      <c r="L162">
+        <v>7000</v>
+      </c>
+      <c r="M162" s="20">
+        <v>0.4899074074074074</v>
+      </c>
+      <c r="N162">
+        <v>0.1215401</v>
+      </c>
       <c r="T162" s="1" t="s">
         <v>73</v>
       </c>
@@ -12473,6 +13114,15 @@
       <c r="K163" t="s">
         <v>61</v>
       </c>
+      <c r="L163">
+        <v>7000</v>
+      </c>
+      <c r="M163" s="20">
+        <v>0.49062500000000003</v>
+      </c>
+      <c r="N163" s="21">
+        <v>7.7478649999999996E-2</v>
+      </c>
       <c r="T163" s="1" t="s">
         <v>73</v>
       </c>
@@ -12511,6 +13161,15 @@
       <c r="K164" t="s">
         <v>61</v>
       </c>
+      <c r="L164">
+        <v>7000</v>
+      </c>
+      <c r="M164" s="20">
+        <v>0.49136574074074074</v>
+      </c>
+      <c r="N164" s="21">
+        <v>8.7185029999999997E-2</v>
+      </c>
       <c r="T164" s="1" t="s">
         <v>73</v>
       </c>
@@ -12552,6 +13211,15 @@
       <c r="K165" t="s">
         <v>61</v>
       </c>
+      <c r="L165">
+        <v>7000</v>
+      </c>
+      <c r="M165" s="20">
+        <v>0.49208333333333337</v>
+      </c>
+      <c r="N165">
+        <v>0.1196178</v>
+      </c>
       <c r="T165" s="1" t="s">
         <v>73</v>
       </c>
@@ -12590,6 +13258,15 @@
       <c r="K166" t="s">
         <v>61</v>
       </c>
+      <c r="L166">
+        <v>7000</v>
+      </c>
+      <c r="M166" s="20">
+        <v>0.49296296296296299</v>
+      </c>
+      <c r="N166">
+        <v>0.17530589999999999</v>
+      </c>
       <c r="T166" s="1" t="s">
         <v>73</v>
       </c>
@@ -12628,6 +13305,15 @@
       <c r="K167" t="s">
         <v>61</v>
       </c>
+      <c r="L167">
+        <v>7000</v>
+      </c>
+      <c r="M167" s="20">
+        <v>0.49381944444444442</v>
+      </c>
+      <c r="N167">
+        <v>9.7768999999999995E-2</v>
+      </c>
       <c r="T167" s="1" t="s">
         <v>73</v>
       </c>
@@ -12669,6 +13355,15 @@
       <c r="K168" t="s">
         <v>61</v>
       </c>
+      <c r="L168">
+        <v>7000</v>
+      </c>
+      <c r="M168" s="20">
+        <v>0.49454861111111109</v>
+      </c>
+      <c r="N168">
+        <v>0.44250270000000003</v>
+      </c>
       <c r="T168" s="1" t="s">
         <v>73</v>
       </c>
@@ -12710,6 +13405,15 @@
       <c r="K169" t="s">
         <v>61</v>
       </c>
+      <c r="L169">
+        <v>7000</v>
+      </c>
+      <c r="M169" s="20">
+        <v>0.49539351851851854</v>
+      </c>
+      <c r="N169">
+        <v>7.2012400000000004E-2</v>
+      </c>
       <c r="T169" s="1" t="s">
         <v>73</v>
       </c>
@@ -12751,6 +13455,15 @@
       <c r="K170" t="s">
         <v>61</v>
       </c>
+      <c r="L170">
+        <v>7000</v>
+      </c>
+      <c r="M170" s="20">
+        <v>0.49625000000000002</v>
+      </c>
+      <c r="N170">
+        <v>0.94064519999999996</v>
+      </c>
       <c r="T170" s="1" t="s">
         <v>73</v>
       </c>
@@ -12792,6 +13505,15 @@
       <c r="K171" t="s">
         <v>61</v>
       </c>
+      <c r="L171">
+        <v>7000</v>
+      </c>
+      <c r="M171" s="20">
+        <v>0.49715277777777778</v>
+      </c>
+      <c r="N171" s="21">
+        <v>8.9814859999999996E-2</v>
+      </c>
       <c r="T171" s="1" t="s">
         <v>73</v>
       </c>
@@ -12833,6 +13555,15 @@
       <c r="K172" t="s">
         <v>61</v>
       </c>
+      <c r="L172">
+        <v>7000</v>
+      </c>
+      <c r="M172" s="20">
+        <v>0.49784722222222227</v>
+      </c>
+      <c r="N172" s="21">
+        <v>9.6213660000000006E-2</v>
+      </c>
       <c r="T172" s="1" t="s">
         <v>73</v>
       </c>
@@ -12874,6 +13605,15 @@
       <c r="K173" t="s">
         <v>61</v>
       </c>
+      <c r="L173">
+        <v>7000</v>
+      </c>
+      <c r="M173" s="20">
+        <v>0.49873842592592593</v>
+      </c>
+      <c r="N173" s="21">
+        <v>9.322076E-2</v>
+      </c>
       <c r="T173" s="1" t="s">
         <v>73</v>
       </c>
@@ -12915,6 +13655,15 @@
       <c r="K174" t="s">
         <v>61</v>
       </c>
+      <c r="L174">
+        <v>7000</v>
+      </c>
+      <c r="M174" s="20">
+        <v>0.51457175925925924</v>
+      </c>
+      <c r="N174" s="21">
+        <v>9.0419239999999998E-2</v>
+      </c>
       <c r="T174" s="1" t="s">
         <v>73</v>
       </c>
@@ -12956,6 +13705,15 @@
       <c r="K175" t="s">
         <v>61</v>
       </c>
+      <c r="L175">
+        <v>7000</v>
+      </c>
+      <c r="M175" s="20">
+        <v>0.51545138888888886</v>
+      </c>
+      <c r="N175">
+        <v>0.11817270000000001</v>
+      </c>
       <c r="T175" s="1" t="s">
         <v>73</v>
       </c>
@@ -12997,6 +13755,15 @@
       <c r="K176" t="s">
         <v>61</v>
       </c>
+      <c r="L176">
+        <v>7000</v>
+      </c>
+      <c r="M176" s="20">
+        <v>0.51640046296296294</v>
+      </c>
+      <c r="N176">
+        <v>0.68029110000000004</v>
+      </c>
       <c r="T176" s="1" t="s">
         <v>73</v>
       </c>
@@ -13035,6 +13802,15 @@
       <c r="K177" t="s">
         <v>61</v>
       </c>
+      <c r="L177">
+        <v>7000</v>
+      </c>
+      <c r="M177" s="20">
+        <v>0.51728009259259256</v>
+      </c>
+      <c r="N177" s="21">
+        <v>9.4185749999999999E-2</v>
+      </c>
       <c r="T177" s="1" t="s">
         <v>73</v>
       </c>
@@ -13076,6 +13852,15 @@
       <c r="K178" t="s">
         <v>61</v>
       </c>
+      <c r="L178">
+        <v>7000</v>
+      </c>
+      <c r="M178" s="20">
+        <v>0.51832175925925927</v>
+      </c>
+      <c r="N178" s="21">
+        <v>9.1616569999999994E-2</v>
+      </c>
       <c r="T178" s="1" t="s">
         <v>73</v>
       </c>
@@ -13117,6 +13902,15 @@
       <c r="K179" t="s">
         <v>61</v>
       </c>
+      <c r="L179">
+        <v>7000</v>
+      </c>
+      <c r="M179" s="20">
+        <v>0.51903935185185179</v>
+      </c>
+      <c r="N179">
+        <v>0.93948520000000002</v>
+      </c>
       <c r="T179" s="1" t="s">
         <v>73</v>
       </c>
@@ -13158,6 +13952,15 @@
       <c r="K180" t="s">
         <v>61</v>
       </c>
+      <c r="L180">
+        <v>7000</v>
+      </c>
+      <c r="M180" s="20">
+        <v>0.51986111111111111</v>
+      </c>
+      <c r="N180">
+        <v>0.1224875</v>
+      </c>
       <c r="T180" s="1" t="s">
         <v>73</v>
       </c>
@@ -13196,6 +13999,15 @@
       <c r="K181" t="s">
         <v>61</v>
       </c>
+      <c r="L181">
+        <v>7000</v>
+      </c>
+      <c r="M181" s="20">
+        <v>0.52076388888888892</v>
+      </c>
+      <c r="N181">
+        <v>0.1082694</v>
+      </c>
       <c r="T181" s="1" t="s">
         <v>73</v>
       </c>
@@ -13234,6 +14046,15 @@
       <c r="K182" t="s">
         <v>61</v>
       </c>
+      <c r="L182">
+        <v>7000</v>
+      </c>
+      <c r="M182" s="20">
+        <v>0.52152777777777781</v>
+      </c>
+      <c r="N182" s="21">
+        <v>7.8673350000000003E-2</v>
+      </c>
       <c r="T182" s="1" t="s">
         <v>73</v>
       </c>
@@ -13275,6 +14096,15 @@
       <c r="K183" t="s">
         <v>61</v>
       </c>
+      <c r="L183">
+        <v>7000</v>
+      </c>
+      <c r="M183" s="20">
+        <v>0.52258101851851857</v>
+      </c>
+      <c r="N183" s="21">
+        <v>2.6454790000000001E-3</v>
+      </c>
       <c r="T183" s="1" t="s">
         <v>73</v>
       </c>
@@ -13310,6 +14140,15 @@
       <c r="K184" t="s">
         <v>61</v>
       </c>
+      <c r="L184">
+        <v>7000</v>
+      </c>
+      <c r="M184" s="20">
+        <v>0.52347222222222223</v>
+      </c>
+      <c r="N184" s="21">
+        <v>9.3572949999999998E-3</v>
+      </c>
       <c r="T184" s="1" t="s">
         <v>73</v>
       </c>
@@ -13342,6 +14181,15 @@
       <c r="K185" t="s">
         <v>61</v>
       </c>
+      <c r="L185">
+        <v>7000</v>
+      </c>
+      <c r="M185" s="20">
+        <v>0.52417824074074071</v>
+      </c>
+      <c r="N185" s="21">
+        <v>1.1425980000000001E-2</v>
+      </c>
       <c r="T185" s="1" t="s">
         <v>73</v>
       </c>
@@ -16407,6 +17255,15 @@
       <c r="K276" t="s">
         <v>61</v>
       </c>
+      <c r="L276">
+        <v>7000</v>
+      </c>
+      <c r="M276" s="20">
+        <v>0.41784722222222226</v>
+      </c>
+      <c r="N276">
+        <v>0.12277009999999999</v>
+      </c>
     </row>
     <row r="277" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A277">
@@ -16436,6 +17293,15 @@
       <c r="K277" t="s">
         <v>61</v>
       </c>
+      <c r="L277">
+        <v>7000</v>
+      </c>
+      <c r="M277" s="20">
+        <v>0.41900462962962964</v>
+      </c>
+      <c r="N277">
+        <v>0.70028290000000004</v>
+      </c>
     </row>
     <row r="278" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A278">
@@ -16465,6 +17331,15 @@
       <c r="K278" t="s">
         <v>61</v>
       </c>
+      <c r="L278">
+        <v>7000</v>
+      </c>
+      <c r="M278" s="20">
+        <v>0.42020833333333335</v>
+      </c>
+      <c r="N278" s="21">
+        <v>6.7837389999999997E-2</v>
+      </c>
     </row>
     <row r="279" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A279">
@@ -16494,6 +17369,15 @@
       <c r="K279" t="s">
         <v>61</v>
       </c>
+      <c r="L279">
+        <v>7000</v>
+      </c>
+      <c r="M279" s="20">
+        <v>0.42140046296296302</v>
+      </c>
+      <c r="N279">
+        <v>0.46603889999999998</v>
+      </c>
     </row>
     <row r="280" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A280">
@@ -16523,6 +17407,15 @@
       <c r="K280" t="s">
         <v>61</v>
       </c>
+      <c r="L280">
+        <v>7000</v>
+      </c>
+      <c r="M280" s="20">
+        <v>0.42251157407407408</v>
+      </c>
+      <c r="N280" s="21">
+        <v>9.7149630000000001E-2</v>
+      </c>
     </row>
     <row r="281" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A281">
@@ -16552,6 +17445,15 @@
       <c r="K281" t="s">
         <v>61</v>
       </c>
+      <c r="L281">
+        <v>7000</v>
+      </c>
+      <c r="M281" s="20">
+        <v>0.42379629629629628</v>
+      </c>
+      <c r="N281">
+        <v>0.59092040000000001</v>
+      </c>
     </row>
     <row r="282" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A282">
@@ -16581,6 +17483,15 @@
       <c r="K282" t="s">
         <v>61</v>
       </c>
+      <c r="L282">
+        <v>7000</v>
+      </c>
+      <c r="M282" s="20">
+        <v>0.424837962962963</v>
+      </c>
+      <c r="N282">
+        <v>0.1025996</v>
+      </c>
     </row>
     <row r="283" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A283">
@@ -16610,6 +17521,15 @@
       <c r="K283" t="s">
         <v>61</v>
       </c>
+      <c r="L283">
+        <v>7000</v>
+      </c>
+      <c r="M283" s="20">
+        <v>0.42625000000000002</v>
+      </c>
+      <c r="N283">
+        <v>0.1445264</v>
+      </c>
     </row>
     <row r="284" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A284">
@@ -16639,6 +17559,15 @@
       <c r="K284" t="s">
         <v>61</v>
       </c>
+      <c r="L284">
+        <v>7000</v>
+      </c>
+      <c r="M284" s="20">
+        <v>0.42733796296296295</v>
+      </c>
+      <c r="N284">
+        <v>0.7662523</v>
+      </c>
     </row>
     <row r="285" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A285">
@@ -16668,6 +17597,15 @@
       <c r="K285" t="s">
         <v>61</v>
       </c>
+      <c r="L285">
+        <v>7000</v>
+      </c>
+      <c r="M285" s="20">
+        <v>0.42842592592592593</v>
+      </c>
+      <c r="N285">
+        <v>0.79609700000000005</v>
+      </c>
     </row>
     <row r="286" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A286">
@@ -16697,6 +17635,15 @@
       <c r="K286" t="s">
         <v>61</v>
       </c>
+      <c r="L286">
+        <v>7000</v>
+      </c>
+      <c r="M286" s="20">
+        <v>0.42939814814814814</v>
+      </c>
+      <c r="N286">
+        <v>0.11193790000000001</v>
+      </c>
     </row>
     <row r="287" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A287">
@@ -16726,6 +17673,15 @@
       <c r="K287" t="s">
         <v>61</v>
       </c>
+      <c r="L287">
+        <v>7000</v>
+      </c>
+      <c r="M287" s="20">
+        <v>0.43023148148148144</v>
+      </c>
+      <c r="N287">
+        <v>0.80031540000000001</v>
+      </c>
     </row>
     <row r="288" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A288">
@@ -16755,8 +17711,17 @@
       <c r="K288" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="289" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L288">
+        <v>7000</v>
+      </c>
+      <c r="M288" s="20">
+        <v>0.43116898148148147</v>
+      </c>
+      <c r="N288">
+        <v>0.1230512</v>
+      </c>
+    </row>
+    <row r="289" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A289">
         <v>14</v>
       </c>
@@ -16784,8 +17749,17 @@
       <c r="K289" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="290" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L289">
+        <v>7000</v>
+      </c>
+      <c r="M289" s="20">
+        <v>0.43210648148148145</v>
+      </c>
+      <c r="N289">
+        <v>0.10142959999999999</v>
+      </c>
+    </row>
+    <row r="290" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A290">
         <v>15</v>
       </c>
@@ -16813,8 +17787,17 @@
       <c r="K290" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="291" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L290">
+        <v>7000</v>
+      </c>
+      <c r="M290" s="20">
+        <v>0.43312499999999998</v>
+      </c>
+      <c r="N290" s="21">
+        <v>8.0545110000000003E-2</v>
+      </c>
+    </row>
+    <row r="291" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A291">
         <v>16</v>
       </c>
@@ -16842,8 +17825,17 @@
       <c r="K291" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="292" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L291">
+        <v>7000</v>
+      </c>
+      <c r="M291" s="20">
+        <v>0.43394675925925924</v>
+      </c>
+      <c r="N291">
+        <v>0.5833024</v>
+      </c>
+    </row>
+    <row r="292" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A292">
         <v>17</v>
       </c>
@@ -16871,8 +17863,17 @@
       <c r="K292" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="293" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L292">
+        <v>7000</v>
+      </c>
+      <c r="M292" s="20">
+        <v>0.4349189814814815</v>
+      </c>
+      <c r="N292">
+        <v>0.52003160000000004</v>
+      </c>
+    </row>
+    <row r="293" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A293">
         <v>18</v>
       </c>
@@ -16900,8 +17901,17 @@
       <c r="K293" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="294" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L293">
+        <v>7000</v>
+      </c>
+      <c r="M293" s="20">
+        <v>0.43596064814814817</v>
+      </c>
+      <c r="N293" s="21">
+        <v>8.6169090000000004E-2</v>
+      </c>
+    </row>
+    <row r="294" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A294">
         <v>19</v>
       </c>
@@ -16929,8 +17939,17 @@
       <c r="K294" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="295" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L294">
+        <v>7000</v>
+      </c>
+      <c r="M294" s="20">
+        <v>0.43678240740740737</v>
+      </c>
+      <c r="N294" s="21">
+        <v>7.3894829999999995E-2</v>
+      </c>
+    </row>
+    <row r="295" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A295">
         <v>20</v>
       </c>
@@ -16961,8 +17980,17 @@
       <c r="K295" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="296" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L295">
+        <v>7000</v>
+      </c>
+      <c r="M295" s="20">
+        <v>0.43760416666666663</v>
+      </c>
+      <c r="N295">
+        <v>0.68196570000000001</v>
+      </c>
+    </row>
+    <row r="296" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A296">
         <v>21</v>
       </c>
@@ -16984,8 +18012,20 @@
       <c r="J296">
         <v>12</v>
       </c>
-    </row>
-    <row r="297" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K296" t="s">
+        <v>61</v>
+      </c>
+      <c r="L296">
+        <v>7000</v>
+      </c>
+      <c r="M296" s="20">
+        <v>0.43853009259259257</v>
+      </c>
+      <c r="N296" s="21">
+        <v>8.2836980000000008E-3</v>
+      </c>
+    </row>
+    <row r="297" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A297">
         <v>22</v>
       </c>
@@ -17007,8 +18047,20 @@
       <c r="J297">
         <v>12</v>
       </c>
-    </row>
-    <row r="298" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K297" t="s">
+        <v>61</v>
+      </c>
+      <c r="L297">
+        <v>7000</v>
+      </c>
+      <c r="M297" s="20">
+        <v>0.4392361111111111</v>
+      </c>
+      <c r="N297" s="21">
+        <v>7.9548310000000007E-3</v>
+      </c>
+    </row>
+    <row r="298" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A298">
         <v>1</v>
       </c>
@@ -17039,8 +18091,17 @@
       <c r="K298" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="299" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L298">
+        <v>6262</v>
+      </c>
+      <c r="M298" s="20">
+        <v>0.41784722222222226</v>
+      </c>
+      <c r="N298">
+        <v>0.21415609999999999</v>
+      </c>
+    </row>
+    <row r="299" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A299">
         <v>2</v>
       </c>
@@ -17068,8 +18129,17 @@
       <c r="K299" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="300" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L299">
+        <v>6262</v>
+      </c>
+      <c r="M299" s="20">
+        <v>0.41900462962962964</v>
+      </c>
+      <c r="N299">
+        <v>1.54416</v>
+      </c>
+    </row>
+    <row r="300" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A300">
         <v>3</v>
       </c>
@@ -17097,8 +18167,17 @@
       <c r="K300" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="301" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L300">
+        <v>6262</v>
+      </c>
+      <c r="M300" s="20">
+        <v>0.42020833333333335</v>
+      </c>
+      <c r="N300">
+        <v>1.456161</v>
+      </c>
+    </row>
+    <row r="301" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A301">
         <v>4</v>
       </c>
@@ -17126,8 +18205,17 @@
       <c r="K301" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="302" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L301">
+        <v>6262</v>
+      </c>
+      <c r="M301" s="20">
+        <v>0.42140046296296302</v>
+      </c>
+      <c r="N301">
+        <v>0.15702050000000001</v>
+      </c>
+    </row>
+    <row r="302" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A302">
         <v>5</v>
       </c>
@@ -17155,8 +18243,17 @@
       <c r="K302" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="303" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L302">
+        <v>6262</v>
+      </c>
+      <c r="M302" s="20">
+        <v>0.42251157407407408</v>
+      </c>
+      <c r="N302">
+        <v>1.242848</v>
+      </c>
+    </row>
+    <row r="303" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A303">
         <v>6</v>
       </c>
@@ -17184,8 +18281,17 @@
       <c r="K303" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="304" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L303">
+        <v>6262</v>
+      </c>
+      <c r="M303" s="20">
+        <v>0.42379629629629628</v>
+      </c>
+      <c r="N303" s="21">
+        <v>8.9593690000000004E-2</v>
+      </c>
+    </row>
+    <row r="304" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A304">
         <v>7</v>
       </c>
@@ -17213,8 +18319,17 @@
       <c r="K304" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="305" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L304">
+        <v>6262</v>
+      </c>
+      <c r="M304" s="20">
+        <v>0.424837962962963</v>
+      </c>
+      <c r="N304">
+        <v>0.88852350000000002</v>
+      </c>
+    </row>
+    <row r="305" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A305">
         <v>8</v>
       </c>
@@ -17242,8 +18357,17 @@
       <c r="K305" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="306" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L305">
+        <v>6262</v>
+      </c>
+      <c r="M305" s="20">
+        <v>0.42625000000000002</v>
+      </c>
+      <c r="N305">
+        <v>1.329091</v>
+      </c>
+    </row>
+    <row r="306" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A306">
         <v>9</v>
       </c>
@@ -17271,8 +18395,17 @@
       <c r="K306" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="307" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L306">
+        <v>6262</v>
+      </c>
+      <c r="M306" s="20">
+        <v>0.42733796296296295</v>
+      </c>
+      <c r="N306">
+        <v>1.511344</v>
+      </c>
+    </row>
+    <row r="307" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A307">
         <v>10</v>
       </c>
@@ -17300,8 +18433,17 @@
       <c r="K307" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="308" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L307">
+        <v>6262</v>
+      </c>
+      <c r="M307" s="20">
+        <v>0.42842592592592593</v>
+      </c>
+      <c r="N307">
+        <v>0.16845199999999999</v>
+      </c>
+    </row>
+    <row r="308" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A308">
         <v>11</v>
       </c>
@@ -17329,8 +18471,17 @@
       <c r="K308" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="309" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L308">
+        <v>6262</v>
+      </c>
+      <c r="M308" s="20">
+        <v>0.42939814814814814</v>
+      </c>
+      <c r="N308">
+        <v>0.1916591</v>
+      </c>
+    </row>
+    <row r="309" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A309">
         <v>12</v>
       </c>
@@ -17358,8 +18509,17 @@
       <c r="K309" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="310" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L309">
+        <v>6262</v>
+      </c>
+      <c r="M309" s="20">
+        <v>0.43023148148148144</v>
+      </c>
+      <c r="N309">
+        <v>0.22653429999999999</v>
+      </c>
+    </row>
+    <row r="310" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A310">
         <v>13</v>
       </c>
@@ -17387,8 +18547,17 @@
       <c r="K310" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="311" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L310">
+        <v>6262</v>
+      </c>
+      <c r="M310" s="20">
+        <v>0.43116898148148147</v>
+      </c>
+      <c r="N310">
+        <v>0.46903630000000002</v>
+      </c>
+    </row>
+    <row r="311" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A311">
         <v>14</v>
       </c>
@@ -17416,8 +18585,17 @@
       <c r="K311" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="312" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L311">
+        <v>6262</v>
+      </c>
+      <c r="M311" s="20">
+        <v>0.43210648148148145</v>
+      </c>
+      <c r="N311">
+        <v>0.98061030000000005</v>
+      </c>
+    </row>
+    <row r="312" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A312">
         <v>15</v>
       </c>
@@ -17445,8 +18623,17 @@
       <c r="K312" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="313" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L312">
+        <v>6262</v>
+      </c>
+      <c r="M312" s="20">
+        <v>0.43312499999999998</v>
+      </c>
+      <c r="N312">
+        <v>0.133075</v>
+      </c>
+    </row>
+    <row r="313" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A313">
         <v>16</v>
       </c>
@@ -17474,8 +18661,17 @@
       <c r="K313" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="314" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L313">
+        <v>6262</v>
+      </c>
+      <c r="M313" s="20">
+        <v>0.43394675925925924</v>
+      </c>
+      <c r="N313">
+        <v>1.2619419999999999</v>
+      </c>
+    </row>
+    <row r="314" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A314">
         <v>17</v>
       </c>
@@ -17503,8 +18699,17 @@
       <c r="K314" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="315" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L314">
+        <v>6262</v>
+      </c>
+      <c r="M314" s="20">
+        <v>0.4349189814814815</v>
+      </c>
+      <c r="N314">
+        <v>1.1777489999999999</v>
+      </c>
+    </row>
+    <row r="315" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A315">
         <v>18</v>
       </c>
@@ -17532,8 +18737,17 @@
       <c r="K315" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="316" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L315">
+        <v>6262</v>
+      </c>
+      <c r="M315" s="20">
+        <v>0.43596064814814817</v>
+      </c>
+      <c r="N315">
+        <v>0.16995160000000001</v>
+      </c>
+    </row>
+    <row r="316" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A316">
         <v>19</v>
       </c>
@@ -17561,8 +18775,17 @@
       <c r="K316" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="317" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L316">
+        <v>6262</v>
+      </c>
+      <c r="M316" s="20">
+        <v>0.43678240740740737</v>
+      </c>
+      <c r="N316">
+        <v>0.1100877</v>
+      </c>
+    </row>
+    <row r="317" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A317">
         <v>20</v>
       </c>
@@ -17590,8 +18813,17 @@
       <c r="K317" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="318" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L317">
+        <v>6262</v>
+      </c>
+      <c r="M317" s="20">
+        <v>0.43760416666666663</v>
+      </c>
+      <c r="N317">
+        <v>0.14432429999999999</v>
+      </c>
+    </row>
+    <row r="318" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A318">
         <v>21</v>
       </c>
@@ -17613,8 +18845,17 @@
       <c r="J318">
         <v>12</v>
       </c>
-    </row>
-    <row r="319" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L318">
+        <v>6262</v>
+      </c>
+      <c r="M318" s="20">
+        <v>0.43853009259259257</v>
+      </c>
+      <c r="N318" s="21">
+        <v>1.377661E-2</v>
+      </c>
+    </row>
+    <row r="319" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A319">
         <v>22</v>
       </c>
@@ -17638,6 +18879,15 @@
       </c>
       <c r="J319">
         <v>12</v>
+      </c>
+      <c r="L319">
+        <v>6262</v>
+      </c>
+      <c r="M319" s="20">
+        <v>0.4392361111111111</v>
+      </c>
+      <c r="N319" s="21">
+        <v>1.357036E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding scripts to help hinal
</commit_message>
<xml_diff>
--- a/Data/2018-08-14_master_datac_2018_collection_year.xlsx
+++ b/Data/2018-08-14_master_datac_2018_collection_year.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andrew.nguyen\Desktop\Circadian_rhythm_runs_seasonal_timing\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6133F54-EA1B-4402-AF9A-6000F53608F1}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{313EC8B3-708F-4557-94BD-04BFB496F539}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1800" yWindow="1935" windowWidth="48495" windowHeight="26115" xr2:uid="{C7477166-8A7C-B04A-9643-C277FEDCDAAB}"/>
+    <workbookView xWindow="1800" yWindow="1935" windowWidth="48495" windowHeight="26115" activeTab="1" xr2:uid="{C7477166-8A7C-B04A-9643-C277FEDCDAAB}"/>
   </bookViews>
   <sheets>
     <sheet name="Maggot_Collections" sheetId="2" r:id="rId1"/>
@@ -1966,8 +1966,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D3F78F5-4EA8-6A42-B216-41A8EC7A5E8D}">
   <dimension ref="A1:AD102"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="J59" sqref="J59"/>
     </sheetView>
   </sheetViews>
@@ -7224,9 +7224,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92725FB9-1A17-2546-9DFA-6C0D39437891}">
   <dimension ref="A1:AS589"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A526" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O567" sqref="O567"/>
+      <selection pane="bottomLeft" activeCell="M537" sqref="M537"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
randomizing cohort day 12 apple; 2018-08-27
</commit_message>
<xml_diff>
--- a/Data/2018-08-14_master_datac_2018_collection_year.xlsx
+++ b/Data/2018-08-14_master_datac_2018_collection_year.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andrew.nguyen\Desktop\Circadian_rhythm_runs_seasonal_timing\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{068BD75B-6C68-4C71-B0AF-74E27898F60C}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE6F2ABB-7D69-4288-90A3-2FF53629D65B}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1800" yWindow="1935" windowWidth="48495" windowHeight="26115" activeTab="1" xr2:uid="{C7477166-8A7C-B04A-9643-C277FEDCDAAB}"/>
+    <workbookView xWindow="1800" yWindow="1935" windowWidth="48495" windowHeight="26115" xr2:uid="{C7477166-8A7C-B04A-9643-C277FEDCDAAB}"/>
   </bookViews>
   <sheets>
     <sheet name="Maggot_Collections" sheetId="2" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5587" uniqueCount="501">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5704" uniqueCount="543">
   <si>
     <t>Ind_ID</t>
   </si>
@@ -1535,6 +1535,132 @@
   </si>
   <si>
     <t>Day7weight</t>
+  </si>
+  <si>
+    <t>a12r1_18</t>
+  </si>
+  <si>
+    <t>a12r2_18</t>
+  </si>
+  <si>
+    <t>a12r3_18</t>
+  </si>
+  <si>
+    <t>a12r4_18</t>
+  </si>
+  <si>
+    <t>a12r5_18</t>
+  </si>
+  <si>
+    <t>a12r6_18</t>
+  </si>
+  <si>
+    <t>a12r7_18</t>
+  </si>
+  <si>
+    <t>a12r8_18</t>
+  </si>
+  <si>
+    <t>a12r9_18</t>
+  </si>
+  <si>
+    <t>a12r10_18</t>
+  </si>
+  <si>
+    <t>a12r11_18</t>
+  </si>
+  <si>
+    <t>a12r12_18</t>
+  </si>
+  <si>
+    <t>a12r13_18</t>
+  </si>
+  <si>
+    <t>a12r14_18</t>
+  </si>
+  <si>
+    <t>a12r15_18</t>
+  </si>
+  <si>
+    <t>a12r16_18</t>
+  </si>
+  <si>
+    <t>a12r17_18</t>
+  </si>
+  <si>
+    <t>a12r18_18</t>
+  </si>
+  <si>
+    <t>a12r19_18</t>
+  </si>
+  <si>
+    <t>a12r20_18</t>
+  </si>
+  <si>
+    <t>a12r21_18</t>
+  </si>
+  <si>
+    <t>a12r22_18</t>
+  </si>
+  <si>
+    <t>a12o1_18</t>
+  </si>
+  <si>
+    <t>a12o2_18</t>
+  </si>
+  <si>
+    <t>a12o3_18</t>
+  </si>
+  <si>
+    <t>a12o4_18</t>
+  </si>
+  <si>
+    <t>a12o5_18</t>
+  </si>
+  <si>
+    <t>a12o6_18</t>
+  </si>
+  <si>
+    <t>a12o7_18</t>
+  </si>
+  <si>
+    <t>a12o8_18</t>
+  </si>
+  <si>
+    <t>a12o9_18</t>
+  </si>
+  <si>
+    <t>a12o10_18</t>
+  </si>
+  <si>
+    <t>a12o11_18</t>
+  </si>
+  <si>
+    <t>a12o12_18</t>
+  </si>
+  <si>
+    <t>a12o13_18</t>
+  </si>
+  <si>
+    <t>a12o14_18</t>
+  </si>
+  <si>
+    <t>a12o15_18</t>
+  </si>
+  <si>
+    <t>a12o16_18</t>
+  </si>
+  <si>
+    <t>a12o17_18</t>
+  </si>
+  <si>
+    <t>a12o18_18</t>
+  </si>
+  <si>
+    <t>a12o19_18</t>
+  </si>
+  <si>
+    <t>a12o20_18</t>
   </si>
 </sst>
 </file>
@@ -1966,9 +2092,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D3F78F5-4EA8-6A42-B216-41A8EC7A5E8D}">
   <dimension ref="A1:AD102"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J59" sqref="J59"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N34" sqref="N34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -7224,9 +7350,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92725FB9-1A17-2546-9DFA-6C0D39437891}">
   <dimension ref="A1:AS589"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A582" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Z530" sqref="Z530:Z589"/>
+    <sheetView topLeftCell="T1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A267" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="U297" sqref="U297"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -18045,6 +18171,15 @@
       <c r="T276" s="1" t="s">
         <v>74</v>
       </c>
+      <c r="Y276" t="s">
+        <v>376</v>
+      </c>
+      <c r="Z276" t="s">
+        <v>501</v>
+      </c>
+      <c r="AC276" t="s">
+        <v>248</v>
+      </c>
     </row>
     <row r="277" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A277">
@@ -18086,6 +18221,15 @@
       <c r="T277" s="1" t="s">
         <v>74</v>
       </c>
+      <c r="Y277" t="s">
+        <v>376</v>
+      </c>
+      <c r="Z277" t="s">
+        <v>502</v>
+      </c>
+      <c r="AC277" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="278" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A278">
@@ -18127,6 +18271,12 @@
       <c r="T278" s="1" t="s">
         <v>74</v>
       </c>
+      <c r="Y278" t="s">
+        <v>377</v>
+      </c>
+      <c r="Z278" t="s">
+        <v>503</v>
+      </c>
     </row>
     <row r="279" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A279">
@@ -18168,6 +18318,15 @@
       <c r="T279" s="1" t="s">
         <v>74</v>
       </c>
+      <c r="Y279" t="s">
+        <v>376</v>
+      </c>
+      <c r="Z279" t="s">
+        <v>504</v>
+      </c>
+      <c r="AC279" t="s">
+        <v>245</v>
+      </c>
     </row>
     <row r="280" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A280">
@@ -18209,6 +18368,15 @@
       <c r="T280" s="1" t="s">
         <v>74</v>
       </c>
+      <c r="Y280" t="s">
+        <v>378</v>
+      </c>
+      <c r="Z280" t="s">
+        <v>505</v>
+      </c>
+      <c r="AC280" t="s">
+        <v>174</v>
+      </c>
     </row>
     <row r="281" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A281">
@@ -18250,6 +18418,12 @@
       <c r="T281" s="1" t="s">
         <v>74</v>
       </c>
+      <c r="Y281" t="s">
+        <v>377</v>
+      </c>
+      <c r="Z281" t="s">
+        <v>506</v>
+      </c>
     </row>
     <row r="282" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A282">
@@ -18291,6 +18465,12 @@
       <c r="T282" s="1" t="s">
         <v>74</v>
       </c>
+      <c r="Y282" t="s">
+        <v>377</v>
+      </c>
+      <c r="Z282" t="s">
+        <v>507</v>
+      </c>
     </row>
     <row r="283" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A283">
@@ -18332,6 +18512,15 @@
       <c r="T283" s="1" t="s">
         <v>74</v>
       </c>
+      <c r="Y283" t="s">
+        <v>376</v>
+      </c>
+      <c r="Z283" t="s">
+        <v>508</v>
+      </c>
+      <c r="AC283" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="284" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A284">
@@ -18373,6 +18562,15 @@
       <c r="T284" s="1" t="s">
         <v>74</v>
       </c>
+      <c r="Y284" t="s">
+        <v>378</v>
+      </c>
+      <c r="Z284" t="s">
+        <v>509</v>
+      </c>
+      <c r="AC284" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="285" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A285">
@@ -18414,6 +18612,15 @@
       <c r="T285" s="1" t="s">
         <v>74</v>
       </c>
+      <c r="Y285" t="s">
+        <v>378</v>
+      </c>
+      <c r="Z285" t="s">
+        <v>510</v>
+      </c>
+      <c r="AC285" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="286" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A286">
@@ -18455,6 +18662,12 @@
       <c r="T286" s="1" t="s">
         <v>74</v>
       </c>
+      <c r="Y286" t="s">
+        <v>377</v>
+      </c>
+      <c r="Z286" t="s">
+        <v>511</v>
+      </c>
     </row>
     <row r="287" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A287">
@@ -18496,6 +18709,15 @@
       <c r="T287" s="1" t="s">
         <v>74</v>
       </c>
+      <c r="Y287" t="s">
+        <v>378</v>
+      </c>
+      <c r="Z287" t="s">
+        <v>512</v>
+      </c>
+      <c r="AC287" t="s">
+        <v>396</v>
+      </c>
     </row>
     <row r="288" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A288">
@@ -18537,8 +18759,17 @@
       <c r="T288" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="289" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="Y288" t="s">
+        <v>376</v>
+      </c>
+      <c r="Z288" t="s">
+        <v>513</v>
+      </c>
+      <c r="AC288" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="289" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A289">
         <v>14</v>
       </c>
@@ -18578,8 +18809,17 @@
       <c r="T289" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="290" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="Y289" t="s">
+        <v>376</v>
+      </c>
+      <c r="Z289" t="s">
+        <v>514</v>
+      </c>
+      <c r="AC289" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="290" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A290">
         <v>15</v>
       </c>
@@ -18619,8 +18859,14 @@
       <c r="T290" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="291" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="Y290" t="s">
+        <v>377</v>
+      </c>
+      <c r="Z290" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="291" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A291">
         <v>16</v>
       </c>
@@ -18660,8 +18906,17 @@
       <c r="T291" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="292" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="Y291" t="s">
+        <v>378</v>
+      </c>
+      <c r="Z291" t="s">
+        <v>516</v>
+      </c>
+      <c r="AC291" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="292" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A292">
         <v>17</v>
       </c>
@@ -18701,8 +18956,14 @@
       <c r="T292" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="293" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="Y292" t="s">
+        <v>377</v>
+      </c>
+      <c r="Z292" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="293" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A293">
         <v>18</v>
       </c>
@@ -18742,8 +19003,17 @@
       <c r="T293" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="294" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="Y293" t="s">
+        <v>378</v>
+      </c>
+      <c r="Z293" t="s">
+        <v>518</v>
+      </c>
+      <c r="AC293" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="294" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A294">
         <v>19</v>
       </c>
@@ -18783,8 +19053,14 @@
       <c r="T294" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="295" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="Y294" t="s">
+        <v>377</v>
+      </c>
+      <c r="Z294" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="295" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A295">
         <v>20</v>
       </c>
@@ -18827,8 +19103,14 @@
       <c r="T295" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="296" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="Y295" t="s">
+        <v>377</v>
+      </c>
+      <c r="Z295" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="296" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A296">
         <v>21</v>
       </c>
@@ -18865,8 +19147,14 @@
       <c r="T296" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="297" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="Y296" t="s">
+        <v>377</v>
+      </c>
+      <c r="Z296" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="297" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A297">
         <v>22</v>
       </c>
@@ -18903,8 +19191,17 @@
       <c r="T297" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="298" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="Y297" t="s">
+        <v>378</v>
+      </c>
+      <c r="Z297" t="s">
+        <v>522</v>
+      </c>
+      <c r="AC297" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="298" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A298">
         <v>1</v>
       </c>
@@ -18947,8 +19244,14 @@
       <c r="T298" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="299" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="Y298" t="s">
+        <v>377</v>
+      </c>
+      <c r="Z298" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="299" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A299">
         <v>2</v>
       </c>
@@ -18988,8 +19291,14 @@
       <c r="T299" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="300" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="Y299" t="s">
+        <v>377</v>
+      </c>
+      <c r="Z299" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="300" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A300">
         <v>3</v>
       </c>
@@ -19029,8 +19338,17 @@
       <c r="T300" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="301" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="Y300" t="s">
+        <v>376</v>
+      </c>
+      <c r="Z300" t="s">
+        <v>525</v>
+      </c>
+      <c r="AC300" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="301" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A301">
         <v>4</v>
       </c>
@@ -19070,8 +19388,14 @@
       <c r="T301" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="302" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="Y301" t="s">
+        <v>377</v>
+      </c>
+      <c r="Z301" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="302" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A302">
         <v>5</v>
       </c>
@@ -19111,8 +19435,17 @@
       <c r="T302" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="303" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="Y302" t="s">
+        <v>376</v>
+      </c>
+      <c r="Z302" t="s">
+        <v>527</v>
+      </c>
+      <c r="AC302" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="303" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A303">
         <v>6</v>
       </c>
@@ -19152,8 +19485,17 @@
       <c r="T303" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="304" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="Y303" t="s">
+        <v>376</v>
+      </c>
+      <c r="Z303" t="s">
+        <v>528</v>
+      </c>
+      <c r="AC303" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="304" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A304">
         <v>7</v>
       </c>
@@ -19193,8 +19535,17 @@
       <c r="T304" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="305" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="Y304" t="s">
+        <v>378</v>
+      </c>
+      <c r="Z304" t="s">
+        <v>529</v>
+      </c>
+      <c r="AC304" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="305" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A305">
         <v>8</v>
       </c>
@@ -19234,8 +19585,14 @@
       <c r="T305" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="306" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="Y305" t="s">
+        <v>377</v>
+      </c>
+      <c r="Z305" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="306" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A306">
         <v>9</v>
       </c>
@@ -19275,8 +19632,14 @@
       <c r="T306" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="307" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="Y306" t="s">
+        <v>377</v>
+      </c>
+      <c r="Z306" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="307" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A307">
         <v>10</v>
       </c>
@@ -19316,8 +19679,17 @@
       <c r="T307" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="308" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="Y307" t="s">
+        <v>376</v>
+      </c>
+      <c r="Z307" t="s">
+        <v>532</v>
+      </c>
+      <c r="AC307" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="308" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A308">
         <v>11</v>
       </c>
@@ -19357,8 +19729,17 @@
       <c r="T308" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="309" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="Y308" t="s">
+        <v>376</v>
+      </c>
+      <c r="Z308" t="s">
+        <v>533</v>
+      </c>
+      <c r="AC308" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="309" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A309">
         <v>12</v>
       </c>
@@ -19398,8 +19779,17 @@
       <c r="T309" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="310" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="Y309" t="s">
+        <v>376</v>
+      </c>
+      <c r="Z309" t="s">
+        <v>534</v>
+      </c>
+      <c r="AC309" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="310" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A310">
         <v>13</v>
       </c>
@@ -19439,8 +19829,17 @@
       <c r="T310" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="311" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="Y310" t="s">
+        <v>378</v>
+      </c>
+      <c r="Z310" t="s">
+        <v>535</v>
+      </c>
+      <c r="AC310" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="311" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A311">
         <v>14</v>
       </c>
@@ -19480,8 +19879,14 @@
       <c r="T311" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="312" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="Y311" t="s">
+        <v>377</v>
+      </c>
+      <c r="Z311" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="312" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A312">
         <v>15</v>
       </c>
@@ -19521,8 +19926,17 @@
       <c r="T312" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="313" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="Y312" t="s">
+        <v>376</v>
+      </c>
+      <c r="Z312" t="s">
+        <v>537</v>
+      </c>
+      <c r="AC312" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="313" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A313">
         <v>16</v>
       </c>
@@ -19562,8 +19976,14 @@
       <c r="T313" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="314" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="Y313" t="s">
+        <v>377</v>
+      </c>
+      <c r="Z313" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="314" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A314">
         <v>17</v>
       </c>
@@ -19603,8 +20023,17 @@
       <c r="T314" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="315" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="Y314" t="s">
+        <v>378</v>
+      </c>
+      <c r="Z314" t="s">
+        <v>539</v>
+      </c>
+      <c r="AC314" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="315" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A315">
         <v>18</v>
       </c>
@@ -19644,8 +20073,17 @@
       <c r="T315" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="316" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="Y315" t="s">
+        <v>378</v>
+      </c>
+      <c r="Z315" t="s">
+        <v>540</v>
+      </c>
+      <c r="AC315" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="316" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A316">
         <v>19</v>
       </c>
@@ -19685,8 +20123,17 @@
       <c r="T316" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="317" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="Y316" t="s">
+        <v>378</v>
+      </c>
+      <c r="Z316" t="s">
+        <v>541</v>
+      </c>
+      <c r="AC316" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="317" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A317">
         <v>20</v>
       </c>
@@ -19726,8 +20173,17 @@
       <c r="T317" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="318" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="Y317" t="s">
+        <v>378</v>
+      </c>
+      <c r="Z317" t="s">
+        <v>542</v>
+      </c>
+      <c r="AC317" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="318" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A318">
         <v>21</v>
       </c>
@@ -19749,6 +20205,9 @@
       <c r="J318">
         <v>12</v>
       </c>
+      <c r="K318" t="s">
+        <v>61</v>
+      </c>
       <c r="L318">
         <v>6262</v>
       </c>
@@ -19761,8 +20220,14 @@
       <c r="T318" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="319" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="Y318" t="s">
+        <v>377</v>
+      </c>
+      <c r="Z318" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="319" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A319">
         <v>22</v>
       </c>
@@ -19787,6 +20252,9 @@
       <c r="J319">
         <v>12</v>
       </c>
+      <c r="K319" t="s">
+        <v>61</v>
+      </c>
       <c r="L319">
         <v>6262</v>
       </c>
@@ -19799,8 +20267,17 @@
       <c r="T319" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="320" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="Y319" t="s">
+        <v>378</v>
+      </c>
+      <c r="Z319" t="s">
+        <v>522</v>
+      </c>
+      <c r="AC319" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="320" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A320">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
entering apple cohort 12 2018-08-27
</commit_message>
<xml_diff>
--- a/Data/2018-08-14_master_datac_2018_collection_year.xlsx
+++ b/Data/2018-08-14_master_datac_2018_collection_year.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hinalkharva\Desktop\Circadian_rhythm_runs_seasonal_timing\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andrew.nguyen\Desktop\Circadian_rhythm_runs_seasonal_timing\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38CD9EE7-A1C8-453A-8634-5DF668C1A24A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{456FEF1B-CDA0-46FD-BB8E-EAF639FABE80}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1800" yWindow="1935" windowWidth="48495" windowHeight="26115" activeTab="1" xr2:uid="{C7477166-8A7C-B04A-9643-C277FEDCDAAB}"/>
   </bookViews>
@@ -21,6 +21,11 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -8412,8 +8417,8 @@
   <dimension ref="A1:AS589"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A564" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O582" sqref="O582"/>
+      <pane ySplit="1" topLeftCell="A298" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O318" sqref="O318"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -19229,6 +19234,9 @@
       <c r="N276">
         <v>0.12277009999999999</v>
       </c>
+      <c r="O276">
+        <v>9.9290000000000003</v>
+      </c>
       <c r="T276" s="1" t="s">
         <v>74</v>
       </c>
@@ -19279,6 +19287,9 @@
       <c r="N277">
         <v>0.70028290000000004</v>
       </c>
+      <c r="O277">
+        <v>7.0609999999999999</v>
+      </c>
       <c r="T277" s="1" t="s">
         <v>74</v>
       </c>
@@ -19329,6 +19340,9 @@
       <c r="N278" s="21">
         <v>6.7837389999999997E-2</v>
       </c>
+      <c r="O278">
+        <v>7.3390000000000004</v>
+      </c>
       <c r="T278" s="1" t="s">
         <v>74</v>
       </c>
@@ -19376,6 +19390,9 @@
       <c r="N279">
         <v>0.46603889999999998</v>
       </c>
+      <c r="O279">
+        <v>5.7560000000000002</v>
+      </c>
       <c r="T279" s="1" t="s">
         <v>74</v>
       </c>
@@ -19426,6 +19443,9 @@
       <c r="N280" s="21">
         <v>9.7149630000000001E-2</v>
       </c>
+      <c r="O280">
+        <v>8.1379999999999999</v>
+      </c>
       <c r="T280" s="1" t="s">
         <v>74</v>
       </c>
@@ -19476,6 +19496,9 @@
       <c r="N281">
         <v>0.59092040000000001</v>
       </c>
+      <c r="O281">
+        <v>5.7530000000000001</v>
+      </c>
       <c r="T281" s="1" t="s">
         <v>74</v>
       </c>
@@ -19523,6 +19546,9 @@
       <c r="N282">
         <v>0.1025996</v>
       </c>
+      <c r="O282">
+        <v>5.835</v>
+      </c>
       <c r="T282" s="1" t="s">
         <v>74</v>
       </c>
@@ -19570,6 +19596,9 @@
       <c r="N283">
         <v>0.1445264</v>
       </c>
+      <c r="O283">
+        <v>8.5</v>
+      </c>
       <c r="T283" s="1" t="s">
         <v>74</v>
       </c>
@@ -19620,6 +19649,9 @@
       <c r="N284">
         <v>0.7662523</v>
       </c>
+      <c r="O284">
+        <v>7.8810000000000002</v>
+      </c>
       <c r="T284" s="1" t="s">
         <v>74</v>
       </c>
@@ -19670,6 +19702,9 @@
       <c r="N285">
         <v>0.79609700000000005</v>
       </c>
+      <c r="O285">
+        <v>8.093</v>
+      </c>
       <c r="T285" s="1" t="s">
         <v>74</v>
       </c>
@@ -19720,6 +19755,9 @@
       <c r="N286">
         <v>0.11193790000000001</v>
       </c>
+      <c r="O286">
+        <v>6.8730000000000002</v>
+      </c>
       <c r="T286" s="1" t="s">
         <v>74</v>
       </c>
@@ -19767,6 +19805,9 @@
       <c r="N287">
         <v>0.80031540000000001</v>
       </c>
+      <c r="O287">
+        <v>9.1649999999999991</v>
+      </c>
       <c r="T287" s="1" t="s">
         <v>74</v>
       </c>
@@ -19817,6 +19858,9 @@
       <c r="N288">
         <v>0.1230512</v>
       </c>
+      <c r="O288">
+        <v>9.0359999999999996</v>
+      </c>
       <c r="T288" s="1" t="s">
         <v>74</v>
       </c>
@@ -19867,6 +19911,9 @@
       <c r="N289">
         <v>0.10142959999999999</v>
       </c>
+      <c r="O289">
+        <v>8.7129999999999992</v>
+      </c>
       <c r="T289" s="1" t="s">
         <v>74</v>
       </c>
@@ -19917,6 +19964,9 @@
       <c r="N290" s="21">
         <v>8.0545110000000003E-2</v>
       </c>
+      <c r="O290">
+        <v>8.1890000000000001</v>
+      </c>
       <c r="T290" s="1" t="s">
         <v>74</v>
       </c>
@@ -19964,6 +20014,9 @@
       <c r="N291">
         <v>0.5833024</v>
       </c>
+      <c r="O291">
+        <v>2.5009999999999999</v>
+      </c>
       <c r="T291" s="1" t="s">
         <v>74</v>
       </c>
@@ -20014,6 +20067,9 @@
       <c r="N292">
         <v>0.52003160000000004</v>
       </c>
+      <c r="O292">
+        <v>6.3010000000000002</v>
+      </c>
       <c r="T292" s="1" t="s">
         <v>74</v>
       </c>
@@ -20061,6 +20117,9 @@
       <c r="N293" s="21">
         <v>8.6169090000000004E-2</v>
       </c>
+      <c r="O293">
+        <v>6.0869999999999997</v>
+      </c>
       <c r="T293" s="1" t="s">
         <v>74</v>
       </c>
@@ -20111,6 +20170,9 @@
       <c r="N294" s="21">
         <v>7.3894829999999995E-2</v>
       </c>
+      <c r="O294">
+        <v>8.4649999999999999</v>
+      </c>
       <c r="T294" s="1" t="s">
         <v>74</v>
       </c>
@@ -20161,6 +20223,9 @@
       <c r="N295">
         <v>0.68196570000000001</v>
       </c>
+      <c r="O295">
+        <v>7.319</v>
+      </c>
       <c r="T295" s="1" t="s">
         <v>74</v>
       </c>
@@ -20302,6 +20367,9 @@
       <c r="N298">
         <v>0.21415609999999999</v>
       </c>
+      <c r="O298">
+        <v>9.6630000000000003</v>
+      </c>
       <c r="T298" s="1" t="s">
         <v>74</v>
       </c>
@@ -20349,6 +20417,9 @@
       <c r="N299">
         <v>1.54416</v>
       </c>
+      <c r="O299">
+        <v>10.476000000000001</v>
+      </c>
       <c r="T299" s="1" t="s">
         <v>74</v>
       </c>
@@ -20396,6 +20467,9 @@
       <c r="N300">
         <v>1.456161</v>
       </c>
+      <c r="O300">
+        <v>8.2170000000000005</v>
+      </c>
       <c r="T300" s="1" t="s">
         <v>74</v>
       </c>
@@ -20446,6 +20520,9 @@
       <c r="N301">
         <v>0.15702050000000001</v>
       </c>
+      <c r="O301">
+        <v>9.5839999999999996</v>
+      </c>
       <c r="T301" s="1" t="s">
         <v>74</v>
       </c>
@@ -20493,6 +20570,9 @@
       <c r="N302">
         <v>1.242848</v>
       </c>
+      <c r="O302">
+        <v>8.7010000000000005</v>
+      </c>
       <c r="T302" s="1" t="s">
         <v>74</v>
       </c>
@@ -20543,6 +20623,9 @@
       <c r="N303" s="21">
         <v>8.9593690000000004E-2</v>
       </c>
+      <c r="O303">
+        <v>6.6660000000000004</v>
+      </c>
       <c r="T303" s="1" t="s">
         <v>74</v>
       </c>
@@ -20593,6 +20676,9 @@
       <c r="N304">
         <v>0.88852350000000002</v>
       </c>
+      <c r="O304">
+        <v>6.25</v>
+      </c>
       <c r="T304" s="1" t="s">
         <v>74</v>
       </c>
@@ -20643,6 +20729,9 @@
       <c r="N305">
         <v>1.329091</v>
       </c>
+      <c r="O305">
+        <v>7.6050000000000004</v>
+      </c>
       <c r="T305" s="1" t="s">
         <v>74</v>
       </c>
@@ -20690,6 +20779,9 @@
       <c r="N306">
         <v>1.511344</v>
       </c>
+      <c r="O306">
+        <v>7.0229999999999997</v>
+      </c>
       <c r="T306" s="1" t="s">
         <v>74</v>
       </c>
@@ -20737,6 +20829,9 @@
       <c r="N307">
         <v>0.16845199999999999</v>
       </c>
+      <c r="O307">
+        <v>6.1989999999999998</v>
+      </c>
       <c r="T307" s="1" t="s">
         <v>74</v>
       </c>
@@ -20787,6 +20882,9 @@
       <c r="N308">
         <v>0.1916591</v>
       </c>
+      <c r="O308">
+        <v>9.1940000000000008</v>
+      </c>
       <c r="T308" s="1" t="s">
         <v>74</v>
       </c>
@@ -20837,6 +20935,9 @@
       <c r="N309">
         <v>0.22653429999999999</v>
       </c>
+      <c r="O309">
+        <v>7.2949999999999999</v>
+      </c>
       <c r="T309" s="1" t="s">
         <v>74</v>
       </c>
@@ -20887,6 +20988,9 @@
       <c r="N310">
         <v>0.46903630000000002</v>
       </c>
+      <c r="O310">
+        <v>3.5070000000000001</v>
+      </c>
       <c r="T310" s="1" t="s">
         <v>74</v>
       </c>
@@ -20937,6 +21041,9 @@
       <c r="N311">
         <v>0.98061030000000005</v>
       </c>
+      <c r="O311">
+        <v>7.0060000000000002</v>
+      </c>
       <c r="T311" s="1" t="s">
         <v>74</v>
       </c>
@@ -20984,6 +21091,9 @@
       <c r="N312">
         <v>0.133075</v>
       </c>
+      <c r="O312">
+        <v>5.2249999999999996</v>
+      </c>
       <c r="T312" s="1" t="s">
         <v>74</v>
       </c>
@@ -21034,6 +21144,9 @@
       <c r="N313">
         <v>1.2619419999999999</v>
       </c>
+      <c r="O313">
+        <v>7.7329999999999997</v>
+      </c>
       <c r="T313" s="1" t="s">
         <v>74</v>
       </c>
@@ -21081,6 +21194,9 @@
       <c r="N314">
         <v>1.1777489999999999</v>
       </c>
+      <c r="O314">
+        <v>8.9610000000000003</v>
+      </c>
       <c r="T314" s="1" t="s">
         <v>74</v>
       </c>
@@ -21131,6 +21247,9 @@
       <c r="N315">
         <v>0.16995160000000001</v>
       </c>
+      <c r="O315">
+        <v>6.0350000000000001</v>
+      </c>
       <c r="T315" s="1" t="s">
         <v>74</v>
       </c>
@@ -21181,6 +21300,9 @@
       <c r="N316">
         <v>0.1100877</v>
       </c>
+      <c r="O316">
+        <v>5.415</v>
+      </c>
       <c r="T316" s="1" t="s">
         <v>74</v>
       </c>
@@ -21230,6 +21352,9 @@
       </c>
       <c r="N317">
         <v>0.14432429999999999</v>
+      </c>
+      <c r="O317">
+        <v>7.7619999999999996</v>
       </c>
       <c r="T317" s="1" t="s">
         <v>74</v>

</xml_diff>

<commit_message>
randomizing for day 13 apple cohort 2018-08-28
</commit_message>
<xml_diff>
--- a/Data/2018-08-14_master_datac_2018_collection_year.xlsx
+++ b/Data/2018-08-14_master_datac_2018_collection_year.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andrew.nguyen\Desktop\Circadian_rhythm_runs_seasonal_timing\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8893BF16-9FFC-43D5-8189-F008FE1C5E30}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43C61F2F-4D52-488E-BE4F-6D24DB6E23EF}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1800" yWindow="1935" windowWidth="48495" windowHeight="26115" activeTab="1" xr2:uid="{C7477166-8A7C-B04A-9643-C277FEDCDAAB}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6539" uniqueCount="557">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7169" uniqueCount="588">
   <si>
     <t>Ind_ID</t>
   </si>
@@ -1703,6 +1703,99 @@
   </si>
   <si>
     <t>a12-1</t>
+  </si>
+  <si>
+    <t>2018-08-28</t>
+  </si>
+  <si>
+    <t>A12-1</t>
+  </si>
+  <si>
+    <t>A12-2</t>
+  </si>
+  <si>
+    <t>A12-3</t>
+  </si>
+  <si>
+    <t>A12-4</t>
+  </si>
+  <si>
+    <t>A12-5</t>
+  </si>
+  <si>
+    <t>A12-6</t>
+  </si>
+  <si>
+    <t>A12-7</t>
+  </si>
+  <si>
+    <t>A12-8</t>
+  </si>
+  <si>
+    <t>A12-9</t>
+  </si>
+  <si>
+    <t>A12-10</t>
+  </si>
+  <si>
+    <t>A12-11</t>
+  </si>
+  <si>
+    <t>A12-12</t>
+  </si>
+  <si>
+    <t>A12-13</t>
+  </si>
+  <si>
+    <t>A12-14</t>
+  </si>
+  <si>
+    <t>A12-15</t>
+  </si>
+  <si>
+    <t>A12-16</t>
+  </si>
+  <si>
+    <t>A12-17</t>
+  </si>
+  <si>
+    <t>A12-18</t>
+  </si>
+  <si>
+    <t>A12-19</t>
+  </si>
+  <si>
+    <t>A12-20</t>
+  </si>
+  <si>
+    <t>A12-21</t>
+  </si>
+  <si>
+    <t>A12-22</t>
+  </si>
+  <si>
+    <t>A12-23</t>
+  </si>
+  <si>
+    <t>A12-24</t>
+  </si>
+  <si>
+    <t>A12-25</t>
+  </si>
+  <si>
+    <t>A12-26</t>
+  </si>
+  <si>
+    <t>A12-27</t>
+  </si>
+  <si>
+    <t>A12-28</t>
+  </si>
+  <si>
+    <t>A12-29</t>
+  </si>
+  <si>
+    <t>A12-30</t>
   </si>
 </sst>
 </file>
@@ -2154,7 +2247,7 @@
   <dimension ref="A1:AC113"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A92" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A85" sqref="A85:XFD85"/>
     </sheetView>
   </sheetViews>
@@ -8418,11 +8511,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92725FB9-1A17-2546-9DFA-6C0D39437891}">
-  <dimension ref="A1:AS629"/>
+  <dimension ref="A1:AS719"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H360" sqref="H360"/>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A704" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AC660" sqref="AC660:AC719"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -31950,6 +32043,2856 @@
       </c>
       <c r="AC629" t="s">
         <v>138</v>
+      </c>
+    </row>
+    <row r="630" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A630">
+        <v>1</v>
+      </c>
+      <c r="C630" t="s">
+        <v>59</v>
+      </c>
+      <c r="G630" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I630" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="J630">
+        <v>13</v>
+      </c>
+      <c r="K630" t="s">
+        <v>61</v>
+      </c>
+      <c r="T630" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y630" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z630" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="631" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A631">
+        <v>2</v>
+      </c>
+      <c r="C631" t="s">
+        <v>59</v>
+      </c>
+      <c r="G631" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I631" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="J631">
+        <v>13</v>
+      </c>
+      <c r="K631" t="s">
+        <v>61</v>
+      </c>
+      <c r="T631" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y631" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z631" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="632" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A632">
+        <v>3</v>
+      </c>
+      <c r="C632" t="s">
+        <v>59</v>
+      </c>
+      <c r="G632" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I632" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="J632">
+        <v>13</v>
+      </c>
+      <c r="K632" t="s">
+        <v>61</v>
+      </c>
+      <c r="T632" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y632" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z632" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="633" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A633">
+        <v>4</v>
+      </c>
+      <c r="C633" t="s">
+        <v>59</v>
+      </c>
+      <c r="G633" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I633" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="J633">
+        <v>13</v>
+      </c>
+      <c r="K633" t="s">
+        <v>61</v>
+      </c>
+      <c r="T633" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y633" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z633" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="634" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A634">
+        <v>5</v>
+      </c>
+      <c r="C634" t="s">
+        <v>59</v>
+      </c>
+      <c r="G634" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I634" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="J634">
+        <v>13</v>
+      </c>
+      <c r="K634" t="s">
+        <v>61</v>
+      </c>
+      <c r="T634" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y634" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z634" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="635" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A635">
+        <v>6</v>
+      </c>
+      <c r="C635" t="s">
+        <v>59</v>
+      </c>
+      <c r="G635" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I635" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="J635">
+        <v>13</v>
+      </c>
+      <c r="K635" t="s">
+        <v>61</v>
+      </c>
+      <c r="T635" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y635" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z635" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="636" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A636">
+        <v>7</v>
+      </c>
+      <c r="C636" t="s">
+        <v>59</v>
+      </c>
+      <c r="G636" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I636" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="J636">
+        <v>13</v>
+      </c>
+      <c r="K636" t="s">
+        <v>61</v>
+      </c>
+      <c r="T636" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y636" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z636" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="637" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A637">
+        <v>8</v>
+      </c>
+      <c r="C637" t="s">
+        <v>59</v>
+      </c>
+      <c r="G637" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I637" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="J637">
+        <v>13</v>
+      </c>
+      <c r="K637" t="s">
+        <v>61</v>
+      </c>
+      <c r="T637" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y637" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z637" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="638" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A638">
+        <v>9</v>
+      </c>
+      <c r="C638" t="s">
+        <v>59</v>
+      </c>
+      <c r="G638" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I638" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="J638">
+        <v>13</v>
+      </c>
+      <c r="K638" t="s">
+        <v>61</v>
+      </c>
+      <c r="T638" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y638" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z638" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="639" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A639">
+        <v>10</v>
+      </c>
+      <c r="C639" t="s">
+        <v>59</v>
+      </c>
+      <c r="G639" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I639" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="J639">
+        <v>13</v>
+      </c>
+      <c r="K639" t="s">
+        <v>61</v>
+      </c>
+      <c r="T639" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y639" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z639" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="640" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A640">
+        <v>11</v>
+      </c>
+      <c r="C640" t="s">
+        <v>59</v>
+      </c>
+      <c r="G640" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I640" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="J640">
+        <v>13</v>
+      </c>
+      <c r="K640" t="s">
+        <v>61</v>
+      </c>
+      <c r="T640" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y640" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z640" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="641" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A641">
+        <v>12</v>
+      </c>
+      <c r="C641" t="s">
+        <v>59</v>
+      </c>
+      <c r="G641" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I641" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="J641">
+        <v>13</v>
+      </c>
+      <c r="K641" t="s">
+        <v>61</v>
+      </c>
+      <c r="T641" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y641" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z641" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="642" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A642">
+        <v>13</v>
+      </c>
+      <c r="C642" t="s">
+        <v>59</v>
+      </c>
+      <c r="G642" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I642" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="J642">
+        <v>13</v>
+      </c>
+      <c r="K642" t="s">
+        <v>61</v>
+      </c>
+      <c r="T642" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y642" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z642" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="643" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A643">
+        <v>14</v>
+      </c>
+      <c r="C643" t="s">
+        <v>59</v>
+      </c>
+      <c r="G643" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I643" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="J643">
+        <v>13</v>
+      </c>
+      <c r="K643" t="s">
+        <v>61</v>
+      </c>
+      <c r="T643" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y643" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z643" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="644" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A644">
+        <v>15</v>
+      </c>
+      <c r="C644" t="s">
+        <v>59</v>
+      </c>
+      <c r="G644" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I644" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="J644">
+        <v>13</v>
+      </c>
+      <c r="K644" t="s">
+        <v>61</v>
+      </c>
+      <c r="T644" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y644" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z644" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="645" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A645">
+        <v>16</v>
+      </c>
+      <c r="C645" t="s">
+        <v>60</v>
+      </c>
+      <c r="G645" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I645" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="J645">
+        <v>13</v>
+      </c>
+      <c r="K645" t="s">
+        <v>61</v>
+      </c>
+      <c r="T645" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y645" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z645" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="646" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A646">
+        <v>17</v>
+      </c>
+      <c r="C646" t="s">
+        <v>60</v>
+      </c>
+      <c r="G646" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I646" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="J646">
+        <v>13</v>
+      </c>
+      <c r="K646" t="s">
+        <v>61</v>
+      </c>
+      <c r="T646" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y646" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z646" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="647" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A647">
+        <v>18</v>
+      </c>
+      <c r="C647" t="s">
+        <v>60</v>
+      </c>
+      <c r="G647" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I647" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="J647">
+        <v>13</v>
+      </c>
+      <c r="K647" t="s">
+        <v>61</v>
+      </c>
+      <c r="T647" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y647" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z647" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="648" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A648">
+        <v>19</v>
+      </c>
+      <c r="C648" t="s">
+        <v>60</v>
+      </c>
+      <c r="G648" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I648" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="J648">
+        <v>13</v>
+      </c>
+      <c r="K648" t="s">
+        <v>61</v>
+      </c>
+      <c r="T648" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y648" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z648" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="649" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A649">
+        <v>20</v>
+      </c>
+      <c r="C649" t="s">
+        <v>60</v>
+      </c>
+      <c r="G649" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I649" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="J649">
+        <v>13</v>
+      </c>
+      <c r="K649" t="s">
+        <v>61</v>
+      </c>
+      <c r="T649" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y649" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z649" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="650" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A650">
+        <v>21</v>
+      </c>
+      <c r="C650" t="s">
+        <v>60</v>
+      </c>
+      <c r="G650" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I650" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="J650">
+        <v>13</v>
+      </c>
+      <c r="K650" t="s">
+        <v>61</v>
+      </c>
+      <c r="T650" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y650" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z650" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="651" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A651">
+        <v>22</v>
+      </c>
+      <c r="C651" t="s">
+        <v>60</v>
+      </c>
+      <c r="G651" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I651" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="J651">
+        <v>13</v>
+      </c>
+      <c r="K651" t="s">
+        <v>61</v>
+      </c>
+      <c r="T651" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y651" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z651" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="652" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A652">
+        <v>23</v>
+      </c>
+      <c r="C652" t="s">
+        <v>60</v>
+      </c>
+      <c r="G652" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I652" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="J652">
+        <v>13</v>
+      </c>
+      <c r="K652" t="s">
+        <v>61</v>
+      </c>
+      <c r="T652" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y652" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z652" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="653" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A653">
+        <v>24</v>
+      </c>
+      <c r="C653" t="s">
+        <v>60</v>
+      </c>
+      <c r="G653" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I653" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="J653">
+        <v>13</v>
+      </c>
+      <c r="K653" t="s">
+        <v>61</v>
+      </c>
+      <c r="T653" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y653" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z653" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="654" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A654">
+        <v>25</v>
+      </c>
+      <c r="C654" t="s">
+        <v>60</v>
+      </c>
+      <c r="G654" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I654" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="J654">
+        <v>13</v>
+      </c>
+      <c r="K654" t="s">
+        <v>61</v>
+      </c>
+      <c r="T654" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y654" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z654" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="655" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A655">
+        <v>26</v>
+      </c>
+      <c r="C655" t="s">
+        <v>60</v>
+      </c>
+      <c r="G655" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I655" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="J655">
+        <v>13</v>
+      </c>
+      <c r="K655" t="s">
+        <v>61</v>
+      </c>
+      <c r="T655" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y655" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z655" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="656" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A656">
+        <v>27</v>
+      </c>
+      <c r="C656" t="s">
+        <v>60</v>
+      </c>
+      <c r="G656" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I656" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="J656">
+        <v>13</v>
+      </c>
+      <c r="K656" t="s">
+        <v>61</v>
+      </c>
+      <c r="T656" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y656" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z656" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="657" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A657">
+        <v>28</v>
+      </c>
+      <c r="C657" t="s">
+        <v>60</v>
+      </c>
+      <c r="G657" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I657" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="J657">
+        <v>13</v>
+      </c>
+      <c r="K657" t="s">
+        <v>61</v>
+      </c>
+      <c r="T657" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y657" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z657" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="658" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A658">
+        <v>29</v>
+      </c>
+      <c r="C658" t="s">
+        <v>60</v>
+      </c>
+      <c r="G658" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I658" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="J658">
+        <v>13</v>
+      </c>
+      <c r="K658" t="s">
+        <v>61</v>
+      </c>
+      <c r="T658" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y658" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z658" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="659" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A659">
+        <v>30</v>
+      </c>
+      <c r="C659" t="s">
+        <v>60</v>
+      </c>
+      <c r="G659" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I659" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="J659">
+        <v>13</v>
+      </c>
+      <c r="K659" t="s">
+        <v>61</v>
+      </c>
+      <c r="T659" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y659" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z659" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="660" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A660">
+        <v>1</v>
+      </c>
+      <c r="C660" t="s">
+        <v>59</v>
+      </c>
+      <c r="G660" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I660" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="J660">
+        <v>13</v>
+      </c>
+      <c r="K660" t="s">
+        <v>61</v>
+      </c>
+      <c r="T660" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y660" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z660" t="str">
+        <f>"A12"&amp;Y660&amp;"-"&amp;AC660</f>
+        <v>A12RT-G6</v>
+      </c>
+      <c r="AC660" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="661" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A661">
+        <v>2</v>
+      </c>
+      <c r="C661" t="s">
+        <v>59</v>
+      </c>
+      <c r="G661" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I661" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="J661">
+        <v>13</v>
+      </c>
+      <c r="K661" t="s">
+        <v>61</v>
+      </c>
+      <c r="T661" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y661" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z661" t="str">
+        <f t="shared" ref="Z661:Z719" si="6">"A12"&amp;Y661&amp;"-"&amp;AC661</f>
+        <v>A12RT-G10</v>
+      </c>
+      <c r="AC661" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="662" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A662">
+        <v>3</v>
+      </c>
+      <c r="C662" t="s">
+        <v>59</v>
+      </c>
+      <c r="G662" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I662" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="J662">
+        <v>13</v>
+      </c>
+      <c r="K662" t="s">
+        <v>61</v>
+      </c>
+      <c r="T662" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y662" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z662" t="str">
+        <f t="shared" si="6"/>
+        <v>A12RT-A11</v>
+      </c>
+      <c r="AC662" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="663" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A663">
+        <v>4</v>
+      </c>
+      <c r="C663" t="s">
+        <v>59</v>
+      </c>
+      <c r="G663" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I663" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="J663">
+        <v>13</v>
+      </c>
+      <c r="K663" t="s">
+        <v>61</v>
+      </c>
+      <c r="T663" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y663" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z663" t="str">
+        <f t="shared" si="6"/>
+        <v>A12RT-B11</v>
+      </c>
+      <c r="AC663" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="664" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A664">
+        <v>5</v>
+      </c>
+      <c r="C664" t="s">
+        <v>59</v>
+      </c>
+      <c r="G664" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I664" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="J664">
+        <v>13</v>
+      </c>
+      <c r="K664" t="s">
+        <v>61</v>
+      </c>
+      <c r="T664" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y664" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z664" t="str">
+        <f t="shared" si="6"/>
+        <v>A12RT-F12</v>
+      </c>
+      <c r="AC664" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="665" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A665">
+        <v>6</v>
+      </c>
+      <c r="C665" t="s">
+        <v>59</v>
+      </c>
+      <c r="G665" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I665" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="J665">
+        <v>13</v>
+      </c>
+      <c r="K665" t="s">
+        <v>61</v>
+      </c>
+      <c r="T665" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y665" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z665" t="str">
+        <f t="shared" si="6"/>
+        <v>A12RT-H7</v>
+      </c>
+      <c r="AC665" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="666" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A666">
+        <v>7</v>
+      </c>
+      <c r="C666" t="s">
+        <v>59</v>
+      </c>
+      <c r="G666" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I666" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="J666">
+        <v>13</v>
+      </c>
+      <c r="K666" t="s">
+        <v>61</v>
+      </c>
+      <c r="T666" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y666" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z666" t="str">
+        <f t="shared" si="6"/>
+        <v>A12RT-D9</v>
+      </c>
+      <c r="AC666" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="667" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A667">
+        <v>8</v>
+      </c>
+      <c r="C667" t="s">
+        <v>59</v>
+      </c>
+      <c r="G667" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I667" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="J667">
+        <v>13</v>
+      </c>
+      <c r="K667" t="s">
+        <v>61</v>
+      </c>
+      <c r="T667" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y667" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z667" t="str">
+        <f t="shared" si="6"/>
+        <v>A12RT-F6</v>
+      </c>
+      <c r="AC667" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="668" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A668">
+        <v>9</v>
+      </c>
+      <c r="C668" t="s">
+        <v>59</v>
+      </c>
+      <c r="G668" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I668" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="J668">
+        <v>13</v>
+      </c>
+      <c r="K668" t="s">
+        <v>61</v>
+      </c>
+      <c r="T668" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y668" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z668" t="str">
+        <f t="shared" si="6"/>
+        <v>A12RT-E5</v>
+      </c>
+      <c r="AC668" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="669" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A669">
+        <v>10</v>
+      </c>
+      <c r="C669" t="s">
+        <v>59</v>
+      </c>
+      <c r="G669" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I669" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="J669">
+        <v>13</v>
+      </c>
+      <c r="K669" t="s">
+        <v>61</v>
+      </c>
+      <c r="T669" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y669" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z669" t="str">
+        <f t="shared" si="6"/>
+        <v>A12RT-D2</v>
+      </c>
+      <c r="AC669" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="670" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A670">
+        <v>11</v>
+      </c>
+      <c r="C670" t="s">
+        <v>59</v>
+      </c>
+      <c r="G670" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I670" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="J670">
+        <v>13</v>
+      </c>
+      <c r="K670" t="s">
+        <v>61</v>
+      </c>
+      <c r="T670" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y670" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z670" t="str">
+        <f t="shared" si="6"/>
+        <v>A12RT-F10</v>
+      </c>
+      <c r="AC670" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="671" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A671">
+        <v>12</v>
+      </c>
+      <c r="C671" t="s">
+        <v>59</v>
+      </c>
+      <c r="G671" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I671" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="J671">
+        <v>13</v>
+      </c>
+      <c r="K671" t="s">
+        <v>61</v>
+      </c>
+      <c r="T671" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y671" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z671" t="str">
+        <f t="shared" si="6"/>
+        <v>A12RT-C12</v>
+      </c>
+      <c r="AC671" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="672" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A672">
+        <v>13</v>
+      </c>
+      <c r="C672" t="s">
+        <v>59</v>
+      </c>
+      <c r="G672" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I672" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="J672">
+        <v>13</v>
+      </c>
+      <c r="K672" t="s">
+        <v>61</v>
+      </c>
+      <c r="T672" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y672" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z672" t="str">
+        <f t="shared" si="6"/>
+        <v>A12RT-A8</v>
+      </c>
+      <c r="AC672" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="673" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A673">
+        <v>14</v>
+      </c>
+      <c r="C673" t="s">
+        <v>59</v>
+      </c>
+      <c r="G673" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I673" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="J673">
+        <v>13</v>
+      </c>
+      <c r="K673" t="s">
+        <v>61</v>
+      </c>
+      <c r="T673" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y673" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z673" t="str">
+        <f t="shared" si="6"/>
+        <v>A12RT-D6</v>
+      </c>
+      <c r="AC673" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="674" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A674">
+        <v>15</v>
+      </c>
+      <c r="C674" t="s">
+        <v>59</v>
+      </c>
+      <c r="G674" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I674" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="J674">
+        <v>13</v>
+      </c>
+      <c r="K674" t="s">
+        <v>61</v>
+      </c>
+      <c r="T674" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y674" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z674" t="str">
+        <f t="shared" si="6"/>
+        <v>A12RT-C4</v>
+      </c>
+      <c r="AC674" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="675" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A675">
+        <v>16</v>
+      </c>
+      <c r="C675" t="s">
+        <v>60</v>
+      </c>
+      <c r="G675" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I675" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="J675">
+        <v>13</v>
+      </c>
+      <c r="K675" t="s">
+        <v>61</v>
+      </c>
+      <c r="T675" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y675" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z675" t="str">
+        <f t="shared" si="6"/>
+        <v>A12RT-H1</v>
+      </c>
+      <c r="AC675" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="676" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A676">
+        <v>17</v>
+      </c>
+      <c r="C676" t="s">
+        <v>60</v>
+      </c>
+      <c r="G676" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I676" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="J676">
+        <v>13</v>
+      </c>
+      <c r="K676" t="s">
+        <v>61</v>
+      </c>
+      <c r="T676" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y676" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z676" t="str">
+        <f t="shared" si="6"/>
+        <v>A12RT-A9</v>
+      </c>
+      <c r="AC676" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="677" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A677">
+        <v>18</v>
+      </c>
+      <c r="C677" t="s">
+        <v>60</v>
+      </c>
+      <c r="G677" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I677" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="J677">
+        <v>13</v>
+      </c>
+      <c r="K677" t="s">
+        <v>61</v>
+      </c>
+      <c r="T677" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y677" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z677" t="str">
+        <f t="shared" si="6"/>
+        <v>A12RT-E10</v>
+      </c>
+      <c r="AC677" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="678" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A678">
+        <v>19</v>
+      </c>
+      <c r="C678" t="s">
+        <v>60</v>
+      </c>
+      <c r="G678" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I678" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="J678">
+        <v>13</v>
+      </c>
+      <c r="K678" t="s">
+        <v>61</v>
+      </c>
+      <c r="T678" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y678" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z678" t="str">
+        <f t="shared" si="6"/>
+        <v>A12RT-G3</v>
+      </c>
+      <c r="AC678" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="679" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A679">
+        <v>20</v>
+      </c>
+      <c r="C679" t="s">
+        <v>60</v>
+      </c>
+      <c r="G679" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I679" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="J679">
+        <v>13</v>
+      </c>
+      <c r="K679" t="s">
+        <v>61</v>
+      </c>
+      <c r="T679" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y679" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z679" t="str">
+        <f t="shared" si="6"/>
+        <v>A12RT-H9</v>
+      </c>
+      <c r="AC679" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="680" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A680">
+        <v>21</v>
+      </c>
+      <c r="C680" t="s">
+        <v>60</v>
+      </c>
+      <c r="G680" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I680" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="J680">
+        <v>13</v>
+      </c>
+      <c r="K680" t="s">
+        <v>61</v>
+      </c>
+      <c r="T680" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y680" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z680" t="str">
+        <f t="shared" si="6"/>
+        <v>A12RT-B5</v>
+      </c>
+      <c r="AC680" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="681" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A681">
+        <v>22</v>
+      </c>
+      <c r="C681" t="s">
+        <v>60</v>
+      </c>
+      <c r="G681" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I681" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="J681">
+        <v>13</v>
+      </c>
+      <c r="K681" t="s">
+        <v>61</v>
+      </c>
+      <c r="T681" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y681" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z681" t="str">
+        <f t="shared" si="6"/>
+        <v>A12RT-E12</v>
+      </c>
+      <c r="AC681" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="682" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A682">
+        <v>23</v>
+      </c>
+      <c r="C682" t="s">
+        <v>60</v>
+      </c>
+      <c r="G682" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I682" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="J682">
+        <v>13</v>
+      </c>
+      <c r="K682" t="s">
+        <v>61</v>
+      </c>
+      <c r="T682" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y682" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z682" t="str">
+        <f t="shared" si="6"/>
+        <v>A12RT-A4</v>
+      </c>
+      <c r="AC682" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="683" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A683">
+        <v>24</v>
+      </c>
+      <c r="C683" t="s">
+        <v>60</v>
+      </c>
+      <c r="G683" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I683" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="J683">
+        <v>13</v>
+      </c>
+      <c r="K683" t="s">
+        <v>61</v>
+      </c>
+      <c r="T683" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y683" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z683" t="str">
+        <f t="shared" si="6"/>
+        <v>A12RT-A2</v>
+      </c>
+      <c r="AC683" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="684" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A684">
+        <v>25</v>
+      </c>
+      <c r="C684" t="s">
+        <v>60</v>
+      </c>
+      <c r="G684" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I684" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="J684">
+        <v>13</v>
+      </c>
+      <c r="K684" t="s">
+        <v>61</v>
+      </c>
+      <c r="T684" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y684" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z684" t="str">
+        <f t="shared" si="6"/>
+        <v>A12RT-H4</v>
+      </c>
+      <c r="AC684" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="685" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A685">
+        <v>26</v>
+      </c>
+      <c r="C685" t="s">
+        <v>60</v>
+      </c>
+      <c r="G685" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I685" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="J685">
+        <v>13</v>
+      </c>
+      <c r="K685" t="s">
+        <v>61</v>
+      </c>
+      <c r="T685" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y685" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z685" t="str">
+        <f t="shared" si="6"/>
+        <v>A12RT-B3</v>
+      </c>
+      <c r="AC685" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="686" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A686">
+        <v>27</v>
+      </c>
+      <c r="C686" t="s">
+        <v>60</v>
+      </c>
+      <c r="G686" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I686" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="J686">
+        <v>13</v>
+      </c>
+      <c r="K686" t="s">
+        <v>61</v>
+      </c>
+      <c r="T686" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y686" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z686" t="str">
+        <f t="shared" si="6"/>
+        <v>A12RT-C11</v>
+      </c>
+      <c r="AC686" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="687" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A687">
+        <v>28</v>
+      </c>
+      <c r="C687" t="s">
+        <v>60</v>
+      </c>
+      <c r="G687" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I687" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="J687">
+        <v>13</v>
+      </c>
+      <c r="K687" t="s">
+        <v>61</v>
+      </c>
+      <c r="T687" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y687" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z687" t="str">
+        <f t="shared" si="6"/>
+        <v>A12RT-G5</v>
+      </c>
+      <c r="AC687" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="688" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A688">
+        <v>29</v>
+      </c>
+      <c r="C688" t="s">
+        <v>60</v>
+      </c>
+      <c r="G688" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I688" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="J688">
+        <v>13</v>
+      </c>
+      <c r="K688" t="s">
+        <v>61</v>
+      </c>
+      <c r="T688" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y688" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z688" t="str">
+        <f t="shared" si="6"/>
+        <v>A12RT-G11</v>
+      </c>
+      <c r="AC688" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="689" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A689">
+        <v>30</v>
+      </c>
+      <c r="C689" t="s">
+        <v>60</v>
+      </c>
+      <c r="G689" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I689" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="J689">
+        <v>13</v>
+      </c>
+      <c r="K689" t="s">
+        <v>61</v>
+      </c>
+      <c r="T689" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y689" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z689" t="str">
+        <f t="shared" si="6"/>
+        <v>A12RT-H6</v>
+      </c>
+      <c r="AC689" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="690" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A690">
+        <v>1</v>
+      </c>
+      <c r="C690" t="s">
+        <v>59</v>
+      </c>
+      <c r="G690" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I690" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="J690">
+        <v>13</v>
+      </c>
+      <c r="K690" t="s">
+        <v>61</v>
+      </c>
+      <c r="T690" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y690" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z690" t="str">
+        <f t="shared" si="6"/>
+        <v>A12SO-A6</v>
+      </c>
+      <c r="AC690" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="691" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A691">
+        <v>2</v>
+      </c>
+      <c r="C691" t="s">
+        <v>59</v>
+      </c>
+      <c r="G691" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I691" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="J691">
+        <v>13</v>
+      </c>
+      <c r="K691" t="s">
+        <v>61</v>
+      </c>
+      <c r="T691" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y691" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z691" t="str">
+        <f t="shared" si="6"/>
+        <v>A12SO-F2</v>
+      </c>
+      <c r="AC691" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="692" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A692">
+        <v>3</v>
+      </c>
+      <c r="C692" t="s">
+        <v>59</v>
+      </c>
+      <c r="G692" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I692" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="J692">
+        <v>13</v>
+      </c>
+      <c r="K692" t="s">
+        <v>61</v>
+      </c>
+      <c r="T692" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y692" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z692" t="str">
+        <f t="shared" si="6"/>
+        <v>A12SO-D12</v>
+      </c>
+      <c r="AC692" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="693" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A693">
+        <v>4</v>
+      </c>
+      <c r="C693" t="s">
+        <v>59</v>
+      </c>
+      <c r="G693" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I693" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="J693">
+        <v>13</v>
+      </c>
+      <c r="K693" t="s">
+        <v>61</v>
+      </c>
+      <c r="T693" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y693" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z693" t="str">
+        <f t="shared" si="6"/>
+        <v>A12SO-E4</v>
+      </c>
+      <c r="AC693" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="694" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A694">
+        <v>5</v>
+      </c>
+      <c r="C694" t="s">
+        <v>59</v>
+      </c>
+      <c r="G694" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I694" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="J694">
+        <v>13</v>
+      </c>
+      <c r="K694" t="s">
+        <v>61</v>
+      </c>
+      <c r="T694" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y694" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z694" t="str">
+        <f t="shared" si="6"/>
+        <v>A12SO-E1</v>
+      </c>
+      <c r="AC694" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="695" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A695">
+        <v>6</v>
+      </c>
+      <c r="C695" t="s">
+        <v>59</v>
+      </c>
+      <c r="G695" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I695" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="J695">
+        <v>13</v>
+      </c>
+      <c r="K695" t="s">
+        <v>61</v>
+      </c>
+      <c r="T695" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y695" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z695" t="str">
+        <f t="shared" si="6"/>
+        <v>A12SO-E6</v>
+      </c>
+      <c r="AC695" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="696" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A696">
+        <v>7</v>
+      </c>
+      <c r="C696" t="s">
+        <v>59</v>
+      </c>
+      <c r="G696" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I696" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="J696">
+        <v>13</v>
+      </c>
+      <c r="K696" t="s">
+        <v>61</v>
+      </c>
+      <c r="T696" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y696" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z696" t="str">
+        <f t="shared" si="6"/>
+        <v>A12SO-F9</v>
+      </c>
+      <c r="AC696" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="697" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A697">
+        <v>8</v>
+      </c>
+      <c r="C697" t="s">
+        <v>59</v>
+      </c>
+      <c r="G697" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I697" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="J697">
+        <v>13</v>
+      </c>
+      <c r="K697" t="s">
+        <v>61</v>
+      </c>
+      <c r="T697" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y697" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z697" t="str">
+        <f t="shared" si="6"/>
+        <v>A12SO-F3</v>
+      </c>
+      <c r="AC697" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="698" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A698">
+        <v>9</v>
+      </c>
+      <c r="C698" t="s">
+        <v>59</v>
+      </c>
+      <c r="G698" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I698" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="J698">
+        <v>13</v>
+      </c>
+      <c r="K698" t="s">
+        <v>61</v>
+      </c>
+      <c r="T698" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y698" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z698" t="str">
+        <f t="shared" si="6"/>
+        <v>A12SO-A1</v>
+      </c>
+      <c r="AC698" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="699" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A699">
+        <v>10</v>
+      </c>
+      <c r="C699" t="s">
+        <v>59</v>
+      </c>
+      <c r="G699" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I699" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="J699">
+        <v>13</v>
+      </c>
+      <c r="K699" t="s">
+        <v>61</v>
+      </c>
+      <c r="T699" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y699" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z699" t="str">
+        <f t="shared" si="6"/>
+        <v>A12SO-C7</v>
+      </c>
+      <c r="AC699" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="700" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A700">
+        <v>11</v>
+      </c>
+      <c r="C700" t="s">
+        <v>59</v>
+      </c>
+      <c r="G700" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I700" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="J700">
+        <v>13</v>
+      </c>
+      <c r="K700" t="s">
+        <v>61</v>
+      </c>
+      <c r="T700" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y700" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z700" t="str">
+        <f t="shared" si="6"/>
+        <v>A12SO-D4</v>
+      </c>
+      <c r="AC700" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="701" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A701">
+        <v>12</v>
+      </c>
+      <c r="C701" t="s">
+        <v>59</v>
+      </c>
+      <c r="G701" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I701" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="J701">
+        <v>13</v>
+      </c>
+      <c r="K701" t="s">
+        <v>61</v>
+      </c>
+      <c r="T701" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y701" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z701" t="str">
+        <f t="shared" si="6"/>
+        <v>A12SO-F11</v>
+      </c>
+      <c r="AC701" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="702" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A702">
+        <v>13</v>
+      </c>
+      <c r="C702" t="s">
+        <v>59</v>
+      </c>
+      <c r="G702" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I702" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="J702">
+        <v>13</v>
+      </c>
+      <c r="K702" t="s">
+        <v>61</v>
+      </c>
+      <c r="T702" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y702" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z702" t="str">
+        <f t="shared" si="6"/>
+        <v>A12SO-D8</v>
+      </c>
+      <c r="AC702" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="703" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A703">
+        <v>14</v>
+      </c>
+      <c r="C703" t="s">
+        <v>59</v>
+      </c>
+      <c r="G703" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I703" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="J703">
+        <v>13</v>
+      </c>
+      <c r="K703" t="s">
+        <v>61</v>
+      </c>
+      <c r="T703" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y703" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z703" t="str">
+        <f t="shared" si="6"/>
+        <v>A12SO-A7</v>
+      </c>
+      <c r="AC703" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="704" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A704">
+        <v>15</v>
+      </c>
+      <c r="C704" t="s">
+        <v>59</v>
+      </c>
+      <c r="G704" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I704" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="J704">
+        <v>13</v>
+      </c>
+      <c r="K704" t="s">
+        <v>61</v>
+      </c>
+      <c r="T704" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y704" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z704" t="str">
+        <f t="shared" si="6"/>
+        <v>A12SO-G9</v>
+      </c>
+      <c r="AC704" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="705" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A705">
+        <v>16</v>
+      </c>
+      <c r="C705" t="s">
+        <v>60</v>
+      </c>
+      <c r="G705" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I705" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="J705">
+        <v>13</v>
+      </c>
+      <c r="K705" t="s">
+        <v>61</v>
+      </c>
+      <c r="T705" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y705" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z705" t="str">
+        <f t="shared" si="6"/>
+        <v>A12SO-B6</v>
+      </c>
+      <c r="AC705" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="706" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A706">
+        <v>17</v>
+      </c>
+      <c r="C706" t="s">
+        <v>60</v>
+      </c>
+      <c r="G706" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I706" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="J706">
+        <v>13</v>
+      </c>
+      <c r="K706" t="s">
+        <v>61</v>
+      </c>
+      <c r="T706" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y706" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z706" t="str">
+        <f t="shared" si="6"/>
+        <v>A12SO-H10</v>
+      </c>
+      <c r="AC706" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="707" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A707">
+        <v>18</v>
+      </c>
+      <c r="C707" t="s">
+        <v>60</v>
+      </c>
+      <c r="G707" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I707" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="J707">
+        <v>13</v>
+      </c>
+      <c r="K707" t="s">
+        <v>61</v>
+      </c>
+      <c r="T707" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y707" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z707" t="str">
+        <f t="shared" si="6"/>
+        <v>A12SO-C1</v>
+      </c>
+      <c r="AC707" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="708" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A708">
+        <v>19</v>
+      </c>
+      <c r="C708" t="s">
+        <v>60</v>
+      </c>
+      <c r="G708" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I708" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="J708">
+        <v>13</v>
+      </c>
+      <c r="K708" t="s">
+        <v>61</v>
+      </c>
+      <c r="T708" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y708" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z708" t="str">
+        <f t="shared" si="6"/>
+        <v>A12SO-D5</v>
+      </c>
+      <c r="AC708" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="709" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A709">
+        <v>20</v>
+      </c>
+      <c r="C709" t="s">
+        <v>60</v>
+      </c>
+      <c r="G709" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I709" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="J709">
+        <v>13</v>
+      </c>
+      <c r="K709" t="s">
+        <v>61</v>
+      </c>
+      <c r="T709" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y709" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z709" t="str">
+        <f t="shared" si="6"/>
+        <v>A12SO-E2</v>
+      </c>
+      <c r="AC709" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="710" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A710">
+        <v>21</v>
+      </c>
+      <c r="C710" t="s">
+        <v>60</v>
+      </c>
+      <c r="G710" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I710" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="J710">
+        <v>13</v>
+      </c>
+      <c r="K710" t="s">
+        <v>61</v>
+      </c>
+      <c r="T710" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y710" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z710" t="str">
+        <f t="shared" si="6"/>
+        <v>A12SO-G4</v>
+      </c>
+      <c r="AC710" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="711" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A711">
+        <v>22</v>
+      </c>
+      <c r="C711" t="s">
+        <v>60</v>
+      </c>
+      <c r="G711" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I711" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="J711">
+        <v>13</v>
+      </c>
+      <c r="K711" t="s">
+        <v>61</v>
+      </c>
+      <c r="T711" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y711" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z711" t="str">
+        <f t="shared" si="6"/>
+        <v>A12SO-D1</v>
+      </c>
+      <c r="AC711" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="712" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A712">
+        <v>23</v>
+      </c>
+      <c r="C712" t="s">
+        <v>60</v>
+      </c>
+      <c r="G712" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I712" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="J712">
+        <v>13</v>
+      </c>
+      <c r="K712" t="s">
+        <v>61</v>
+      </c>
+      <c r="T712" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y712" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z712" t="str">
+        <f t="shared" si="6"/>
+        <v>A12SO-C5</v>
+      </c>
+      <c r="AC712" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="713" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A713">
+        <v>24</v>
+      </c>
+      <c r="C713" t="s">
+        <v>60</v>
+      </c>
+      <c r="G713" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I713" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="J713">
+        <v>13</v>
+      </c>
+      <c r="K713" t="s">
+        <v>61</v>
+      </c>
+      <c r="T713" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y713" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z713" t="str">
+        <f t="shared" si="6"/>
+        <v>A12SO-A5</v>
+      </c>
+      <c r="AC713" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="714" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A714">
+        <v>25</v>
+      </c>
+      <c r="C714" t="s">
+        <v>60</v>
+      </c>
+      <c r="G714" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I714" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="J714">
+        <v>13</v>
+      </c>
+      <c r="K714" t="s">
+        <v>61</v>
+      </c>
+      <c r="T714" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y714" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z714" t="str">
+        <f t="shared" si="6"/>
+        <v>A12SO-E8</v>
+      </c>
+      <c r="AC714" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="715" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A715">
+        <v>26</v>
+      </c>
+      <c r="C715" t="s">
+        <v>60</v>
+      </c>
+      <c r="G715" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I715" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="J715">
+        <v>13</v>
+      </c>
+      <c r="K715" t="s">
+        <v>61</v>
+      </c>
+      <c r="T715" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y715" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z715" t="str">
+        <f t="shared" si="6"/>
+        <v>A12SO-B10</v>
+      </c>
+      <c r="AC715" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="716" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A716">
+        <v>27</v>
+      </c>
+      <c r="C716" t="s">
+        <v>60</v>
+      </c>
+      <c r="G716" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I716" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="J716">
+        <v>13</v>
+      </c>
+      <c r="K716" t="s">
+        <v>61</v>
+      </c>
+      <c r="T716" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y716" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z716" t="str">
+        <f t="shared" si="6"/>
+        <v>A12SO-H11</v>
+      </c>
+      <c r="AC716" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="717" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A717">
+        <v>28</v>
+      </c>
+      <c r="C717" t="s">
+        <v>60</v>
+      </c>
+      <c r="G717" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I717" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="J717">
+        <v>13</v>
+      </c>
+      <c r="K717" t="s">
+        <v>61</v>
+      </c>
+      <c r="T717" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y717" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z717" t="str">
+        <f t="shared" si="6"/>
+        <v>A12SO-D3</v>
+      </c>
+      <c r="AC717" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="718" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A718">
+        <v>29</v>
+      </c>
+      <c r="C718" t="s">
+        <v>60</v>
+      </c>
+      <c r="G718" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I718" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="J718">
+        <v>13</v>
+      </c>
+      <c r="K718" t="s">
+        <v>61</v>
+      </c>
+      <c r="T718" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y718" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z718" t="str">
+        <f t="shared" si="6"/>
+        <v>A12SO-B12</v>
+      </c>
+      <c r="AC718" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="719" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A719">
+        <v>30</v>
+      </c>
+      <c r="C719" t="s">
+        <v>60</v>
+      </c>
+      <c r="G719" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I719" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="J719">
+        <v>13</v>
+      </c>
+      <c r="K719" t="s">
+        <v>61</v>
+      </c>
+      <c r="T719" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y719" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z719" t="str">
+        <f t="shared" si="6"/>
+        <v>A12SO-E9</v>
+      </c>
+      <c r="AC719" t="s">
+        <v>168</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
entering storage info and day 13 cohort 2018-08-28 treatments
</commit_message>
<xml_diff>
--- a/Data/2018-08-14_master_datac_2018_collection_year.xlsx
+++ b/Data/2018-08-14_master_datac_2018_collection_year.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andrew.nguyen\Desktop\Circadian_rhythm_runs_seasonal_timing\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43C61F2F-4D52-488E-BE4F-6D24DB6E23EF}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DF8CBD2-C6D2-4BA2-A608-7D3AE2AAC030}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1800" yWindow="1935" windowWidth="48495" windowHeight="26115" activeTab="1" xr2:uid="{C7477166-8A7C-B04A-9643-C277FEDCDAAB}"/>
   </bookViews>
@@ -1708,94 +1708,94 @@
     <t>2018-08-28</t>
   </si>
   <si>
-    <t>A12-1</t>
-  </si>
-  <si>
-    <t>A12-2</t>
-  </si>
-  <si>
-    <t>A12-3</t>
-  </si>
-  <si>
-    <t>A12-4</t>
-  </si>
-  <si>
-    <t>A12-5</t>
-  </si>
-  <si>
-    <t>A12-6</t>
-  </si>
-  <si>
-    <t>A12-7</t>
-  </si>
-  <si>
-    <t>A12-8</t>
-  </si>
-  <si>
-    <t>A12-9</t>
-  </si>
-  <si>
-    <t>A12-10</t>
-  </si>
-  <si>
-    <t>A12-11</t>
-  </si>
-  <si>
-    <t>A12-12</t>
-  </si>
-  <si>
-    <t>A12-13</t>
-  </si>
-  <si>
-    <t>A12-14</t>
-  </si>
-  <si>
-    <t>A12-15</t>
-  </si>
-  <si>
-    <t>A12-16</t>
-  </si>
-  <si>
-    <t>A12-17</t>
-  </si>
-  <si>
-    <t>A12-18</t>
-  </si>
-  <si>
-    <t>A12-19</t>
-  </si>
-  <si>
-    <t>A12-20</t>
-  </si>
-  <si>
-    <t>A12-21</t>
-  </si>
-  <si>
-    <t>A12-22</t>
-  </si>
-  <si>
-    <t>A12-23</t>
-  </si>
-  <si>
-    <t>A12-24</t>
-  </si>
-  <si>
-    <t>A12-25</t>
-  </si>
-  <si>
-    <t>A12-26</t>
-  </si>
-  <si>
-    <t>A12-27</t>
-  </si>
-  <si>
-    <t>A12-28</t>
-  </si>
-  <si>
-    <t>A12-29</t>
-  </si>
-  <si>
-    <t>A12-30</t>
+    <t>A13-1</t>
+  </si>
+  <si>
+    <t>A13-2</t>
+  </si>
+  <si>
+    <t>A13-3</t>
+  </si>
+  <si>
+    <t>A13-4</t>
+  </si>
+  <si>
+    <t>A13-5</t>
+  </si>
+  <si>
+    <t>A13-6</t>
+  </si>
+  <si>
+    <t>A13-7</t>
+  </si>
+  <si>
+    <t>A13-8</t>
+  </si>
+  <si>
+    <t>A13-9</t>
+  </si>
+  <si>
+    <t>A13-10</t>
+  </si>
+  <si>
+    <t>A13-11</t>
+  </si>
+  <si>
+    <t>A13-12</t>
+  </si>
+  <si>
+    <t>A13-13</t>
+  </si>
+  <si>
+    <t>A13-14</t>
+  </si>
+  <si>
+    <t>A13-15</t>
+  </si>
+  <si>
+    <t>A13-16</t>
+  </si>
+  <si>
+    <t>A13-17</t>
+  </si>
+  <si>
+    <t>A13-18</t>
+  </si>
+  <si>
+    <t>A13-19</t>
+  </si>
+  <si>
+    <t>A13-20</t>
+  </si>
+  <si>
+    <t>A13-21</t>
+  </si>
+  <si>
+    <t>A13-22</t>
+  </si>
+  <si>
+    <t>A13-23</t>
+  </si>
+  <si>
+    <t>A13-24</t>
+  </si>
+  <si>
+    <t>A13-25</t>
+  </si>
+  <si>
+    <t>A13-26</t>
+  </si>
+  <si>
+    <t>A13-27</t>
+  </si>
+  <si>
+    <t>A13-28</t>
+  </si>
+  <si>
+    <t>A13-29</t>
+  </si>
+  <si>
+    <t>A13-30</t>
   </si>
 </sst>
 </file>
@@ -8513,9 +8513,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92725FB9-1A17-2546-9DFA-6C0D39437891}">
   <dimension ref="A1:AS719"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A704" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AC660" sqref="AC660:AC719"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A695" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AD710" sqref="AD710"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -32941,8 +32941,8 @@
         <v>86</v>
       </c>
       <c r="Z660" t="str">
-        <f>"A12"&amp;Y660&amp;"-"&amp;AC660</f>
-        <v>A12RT-G6</v>
+        <f>"A13"&amp;Y660&amp;"-"&amp;AC660</f>
+        <v>A13RT-G6</v>
       </c>
       <c r="AC660" t="s">
         <v>236</v>
@@ -32974,8 +32974,8 @@
         <v>86</v>
       </c>
       <c r="Z661" t="str">
-        <f t="shared" ref="Z661:Z719" si="6">"A12"&amp;Y661&amp;"-"&amp;AC661</f>
-        <v>A12RT-G10</v>
+        <f t="shared" ref="Z661:Z719" si="6">"A13"&amp;Y661&amp;"-"&amp;AC661</f>
+        <v>A13RT-G10</v>
       </c>
       <c r="AC661" t="s">
         <v>396</v>
@@ -33008,7 +33008,7 @@
       </c>
       <c r="Z662" t="str">
         <f t="shared" si="6"/>
-        <v>A12RT-A11</v>
+        <v>A13RT-A11</v>
       </c>
       <c r="AC662" t="s">
         <v>238</v>
@@ -33041,7 +33041,7 @@
       </c>
       <c r="Z663" t="str">
         <f t="shared" si="6"/>
-        <v>A12RT-B11</v>
+        <v>A13RT-B11</v>
       </c>
       <c r="AC663" t="s">
         <v>130</v>
@@ -33074,7 +33074,7 @@
       </c>
       <c r="Z664" t="str">
         <f t="shared" si="6"/>
-        <v>A12RT-F12</v>
+        <v>A13RT-F12</v>
       </c>
       <c r="AC664" t="s">
         <v>122</v>
@@ -33107,7 +33107,7 @@
       </c>
       <c r="Z665" t="str">
         <f t="shared" si="6"/>
-        <v>A12RT-H7</v>
+        <v>A13RT-H7</v>
       </c>
       <c r="AC665" t="s">
         <v>380</v>
@@ -33140,7 +33140,7 @@
       </c>
       <c r="Z666" t="str">
         <f t="shared" si="6"/>
-        <v>A12RT-D9</v>
+        <v>A13RT-D9</v>
       </c>
       <c r="AC666" t="s">
         <v>152</v>
@@ -33173,7 +33173,7 @@
       </c>
       <c r="Z667" t="str">
         <f t="shared" si="6"/>
-        <v>A12RT-F6</v>
+        <v>A13RT-F6</v>
       </c>
       <c r="AC667" t="s">
         <v>385</v>
@@ -33206,7 +33206,7 @@
       </c>
       <c r="Z668" t="str">
         <f t="shared" si="6"/>
-        <v>A12RT-E5</v>
+        <v>A13RT-E5</v>
       </c>
       <c r="AC668" t="s">
         <v>399</v>
@@ -33239,7 +33239,7 @@
       </c>
       <c r="Z669" t="str">
         <f t="shared" si="6"/>
-        <v>A12RT-D2</v>
+        <v>A13RT-D2</v>
       </c>
       <c r="AC669" t="s">
         <v>173</v>
@@ -33272,7 +33272,7 @@
       </c>
       <c r="Z670" t="str">
         <f t="shared" si="6"/>
-        <v>A12RT-F10</v>
+        <v>A13RT-F10</v>
       </c>
       <c r="AC670" t="s">
         <v>383</v>
@@ -33305,7 +33305,7 @@
       </c>
       <c r="Z671" t="str">
         <f t="shared" si="6"/>
-        <v>A12RT-C12</v>
+        <v>A13RT-C12</v>
       </c>
       <c r="AC671" t="s">
         <v>397</v>
@@ -33338,7 +33338,7 @@
       </c>
       <c r="Z672" t="str">
         <f t="shared" si="6"/>
-        <v>A12RT-A8</v>
+        <v>A13RT-A8</v>
       </c>
       <c r="AC672" t="s">
         <v>167</v>
@@ -33371,7 +33371,7 @@
       </c>
       <c r="Z673" t="str">
         <f t="shared" si="6"/>
-        <v>A12RT-D6</v>
+        <v>A13RT-D6</v>
       </c>
       <c r="AC673" t="s">
         <v>161</v>
@@ -33404,7 +33404,7 @@
       </c>
       <c r="Z674" t="str">
         <f t="shared" si="6"/>
-        <v>A12RT-C4</v>
+        <v>A13RT-C4</v>
       </c>
       <c r="AC674" t="s">
         <v>162</v>
@@ -33437,7 +33437,7 @@
       </c>
       <c r="Z675" t="str">
         <f t="shared" si="6"/>
-        <v>A12RT-H1</v>
+        <v>A13RT-H1</v>
       </c>
       <c r="AC675" t="s">
         <v>240</v>
@@ -33470,7 +33470,7 @@
       </c>
       <c r="Z676" t="str">
         <f t="shared" si="6"/>
-        <v>A12RT-A9</v>
+        <v>A13RT-A9</v>
       </c>
       <c r="AC676" t="s">
         <v>134</v>
@@ -33503,7 +33503,7 @@
       </c>
       <c r="Z677" t="str">
         <f t="shared" si="6"/>
-        <v>A12RT-E10</v>
+        <v>A13RT-E10</v>
       </c>
       <c r="AC677" t="s">
         <v>249</v>
@@ -33536,7 +33536,7 @@
       </c>
       <c r="Z678" t="str">
         <f t="shared" si="6"/>
-        <v>A12RT-G3</v>
+        <v>A13RT-G3</v>
       </c>
       <c r="AC678" t="s">
         <v>140</v>
@@ -33569,7 +33569,7 @@
       </c>
       <c r="Z679" t="str">
         <f t="shared" si="6"/>
-        <v>A12RT-H9</v>
+        <v>A13RT-H9</v>
       </c>
       <c r="AC679" t="s">
         <v>381</v>
@@ -33602,7 +33602,7 @@
       </c>
       <c r="Z680" t="str">
         <f t="shared" si="6"/>
-        <v>A12RT-B5</v>
+        <v>A13RT-B5</v>
       </c>
       <c r="AC680" t="s">
         <v>164</v>
@@ -33635,7 +33635,7 @@
       </c>
       <c r="Z681" t="str">
         <f t="shared" si="6"/>
-        <v>A12RT-E12</v>
+        <v>A13RT-E12</v>
       </c>
       <c r="AC681" t="s">
         <v>176</v>
@@ -33668,7 +33668,7 @@
       </c>
       <c r="Z682" t="str">
         <f t="shared" si="6"/>
-        <v>A12RT-A4</v>
+        <v>A13RT-A4</v>
       </c>
       <c r="AC682" t="s">
         <v>253</v>
@@ -33701,7 +33701,7 @@
       </c>
       <c r="Z683" t="str">
         <f t="shared" si="6"/>
-        <v>A12RT-A2</v>
+        <v>A13RT-A2</v>
       </c>
       <c r="AC683" t="s">
         <v>121</v>
@@ -33734,7 +33734,7 @@
       </c>
       <c r="Z684" t="str">
         <f t="shared" si="6"/>
-        <v>A12RT-H4</v>
+        <v>A13RT-H4</v>
       </c>
       <c r="AC684" t="s">
         <v>141</v>
@@ -33767,7 +33767,7 @@
       </c>
       <c r="Z685" t="str">
         <f t="shared" si="6"/>
-        <v>A12RT-B3</v>
+        <v>A13RT-B3</v>
       </c>
       <c r="AC685" t="s">
         <v>243</v>
@@ -33800,7 +33800,7 @@
       </c>
       <c r="Z686" t="str">
         <f t="shared" si="6"/>
-        <v>A12RT-C11</v>
+        <v>A13RT-C11</v>
       </c>
       <c r="AC686" t="s">
         <v>145</v>
@@ -33833,7 +33833,7 @@
       </c>
       <c r="Z687" t="str">
         <f t="shared" si="6"/>
-        <v>A12RT-G5</v>
+        <v>A13RT-G5</v>
       </c>
       <c r="AC687" t="s">
         <v>431</v>
@@ -33866,7 +33866,7 @@
       </c>
       <c r="Z688" t="str">
         <f t="shared" si="6"/>
-        <v>A12RT-G11</v>
+        <v>A13RT-G11</v>
       </c>
       <c r="AC688" t="s">
         <v>250</v>
@@ -33899,7 +33899,7 @@
       </c>
       <c r="Z689" t="str">
         <f t="shared" si="6"/>
-        <v>A12RT-H6</v>
+        <v>A13RT-H6</v>
       </c>
       <c r="AC689" t="s">
         <v>144</v>
@@ -33932,7 +33932,7 @@
       </c>
       <c r="Z690" t="str">
         <f t="shared" si="6"/>
-        <v>A12SO-A6</v>
+        <v>A13SO-A6</v>
       </c>
       <c r="AC690" t="s">
         <v>245</v>
@@ -33965,7 +33965,7 @@
       </c>
       <c r="Z691" t="str">
         <f t="shared" si="6"/>
-        <v>A12SO-F2</v>
+        <v>A13SO-F2</v>
       </c>
       <c r="AC691" t="s">
         <v>464</v>
@@ -33998,7 +33998,7 @@
       </c>
       <c r="Z692" t="str">
         <f t="shared" si="6"/>
-        <v>A12SO-D12</v>
+        <v>A13SO-D12</v>
       </c>
       <c r="AC692" t="s">
         <v>163</v>
@@ -34031,7 +34031,7 @@
       </c>
       <c r="Z693" t="str">
         <f t="shared" si="6"/>
-        <v>A12SO-E4</v>
+        <v>A13SO-E4</v>
       </c>
       <c r="AC693" t="s">
         <v>398</v>
@@ -34064,7 +34064,7 @@
       </c>
       <c r="Z694" t="str">
         <f t="shared" si="6"/>
-        <v>A12SO-E1</v>
+        <v>A13SO-E1</v>
       </c>
       <c r="AC694" t="s">
         <v>138</v>
@@ -34097,7 +34097,7 @@
       </c>
       <c r="Z695" t="str">
         <f t="shared" si="6"/>
-        <v>A12SO-E6</v>
+        <v>A13SO-E6</v>
       </c>
       <c r="AC695" t="s">
         <v>157</v>
@@ -34130,7 +34130,7 @@
       </c>
       <c r="Z696" t="str">
         <f t="shared" si="6"/>
-        <v>A12SO-F9</v>
+        <v>A13SO-F9</v>
       </c>
       <c r="AC696" t="s">
         <v>241</v>
@@ -34163,7 +34163,7 @@
       </c>
       <c r="Z697" t="str">
         <f t="shared" si="6"/>
-        <v>A12SO-F3</v>
+        <v>A13SO-F3</v>
       </c>
       <c r="AC697" t="s">
         <v>242</v>
@@ -34196,7 +34196,7 @@
       </c>
       <c r="Z698" t="str">
         <f t="shared" si="6"/>
-        <v>A12SO-A1</v>
+        <v>A13SO-A1</v>
       </c>
       <c r="AC698" t="s">
         <v>248</v>
@@ -34229,7 +34229,7 @@
       </c>
       <c r="Z699" t="str">
         <f t="shared" si="6"/>
-        <v>A12SO-C7</v>
+        <v>A13SO-C7</v>
       </c>
       <c r="AC699" t="s">
         <v>136</v>
@@ -34262,7 +34262,7 @@
       </c>
       <c r="Z700" t="str">
         <f t="shared" si="6"/>
-        <v>A12SO-D4</v>
+        <v>A13SO-D4</v>
       </c>
       <c r="AC700" t="s">
         <v>237</v>
@@ -34295,7 +34295,7 @@
       </c>
       <c r="Z701" t="str">
         <f t="shared" si="6"/>
-        <v>A12SO-F11</v>
+        <v>A13SO-F11</v>
       </c>
       <c r="AC701" t="s">
         <v>159</v>
@@ -34328,7 +34328,7 @@
       </c>
       <c r="Z702" t="str">
         <f t="shared" si="6"/>
-        <v>A12SO-D8</v>
+        <v>A13SO-D8</v>
       </c>
       <c r="AC702" t="s">
         <v>171</v>
@@ -34361,7 +34361,7 @@
       </c>
       <c r="Z703" t="str">
         <f t="shared" si="6"/>
-        <v>A12SO-A7</v>
+        <v>A13SO-A7</v>
       </c>
       <c r="AC703" t="s">
         <v>165</v>
@@ -34394,7 +34394,7 @@
       </c>
       <c r="Z704" t="str">
         <f t="shared" si="6"/>
-        <v>A12SO-G9</v>
+        <v>A13SO-G9</v>
       </c>
       <c r="AC704" t="s">
         <v>160</v>
@@ -34427,7 +34427,7 @@
       </c>
       <c r="Z705" t="str">
         <f t="shared" si="6"/>
-        <v>A12SO-B6</v>
+        <v>A13SO-B6</v>
       </c>
       <c r="AC705" t="s">
         <v>131</v>
@@ -34460,7 +34460,7 @@
       </c>
       <c r="Z706" t="str">
         <f t="shared" si="6"/>
-        <v>A12SO-H10</v>
+        <v>A13SO-H10</v>
       </c>
       <c r="AC706" t="s">
         <v>175</v>
@@ -34493,7 +34493,7 @@
       </c>
       <c r="Z707" t="str">
         <f t="shared" si="6"/>
-        <v>A12SO-C1</v>
+        <v>A13SO-C1</v>
       </c>
       <c r="AC707" t="s">
         <v>147</v>
@@ -34526,7 +34526,7 @@
       </c>
       <c r="Z708" t="str">
         <f t="shared" si="6"/>
-        <v>A12SO-D5</v>
+        <v>A13SO-D5</v>
       </c>
       <c r="AC708" t="s">
         <v>252</v>
@@ -34559,7 +34559,7 @@
       </c>
       <c r="Z709" t="str">
         <f t="shared" si="6"/>
-        <v>A12SO-E2</v>
+        <v>A13SO-E2</v>
       </c>
       <c r="AC709" t="s">
         <v>179</v>
@@ -34592,7 +34592,7 @@
       </c>
       <c r="Z710" t="str">
         <f t="shared" si="6"/>
-        <v>A12SO-G4</v>
+        <v>A13SO-G4</v>
       </c>
       <c r="AC710" t="s">
         <v>244</v>
@@ -34625,7 +34625,7 @@
       </c>
       <c r="Z711" t="str">
         <f t="shared" si="6"/>
-        <v>A12SO-D1</v>
+        <v>A13SO-D1</v>
       </c>
       <c r="AC711" t="s">
         <v>382</v>
@@ -34658,7 +34658,7 @@
       </c>
       <c r="Z712" t="str">
         <f t="shared" si="6"/>
-        <v>A12SO-C5</v>
+        <v>A13SO-C5</v>
       </c>
       <c r="AC712" t="s">
         <v>124</v>
@@ -34691,7 +34691,7 @@
       </c>
       <c r="Z713" t="str">
         <f t="shared" si="6"/>
-        <v>A12SO-A5</v>
+        <v>A13SO-A5</v>
       </c>
       <c r="AC713" t="s">
         <v>247</v>
@@ -34724,7 +34724,7 @@
       </c>
       <c r="Z714" t="str">
         <f t="shared" si="6"/>
-        <v>A12SO-E8</v>
+        <v>A13SO-E8</v>
       </c>
       <c r="AC714" t="s">
         <v>386</v>
@@ -34757,7 +34757,7 @@
       </c>
       <c r="Z715" t="str">
         <f t="shared" si="6"/>
-        <v>A12SO-B10</v>
+        <v>A13SO-B10</v>
       </c>
       <c r="AC715" t="s">
         <v>155</v>
@@ -34790,7 +34790,7 @@
       </c>
       <c r="Z716" t="str">
         <f t="shared" si="6"/>
-        <v>A12SO-H11</v>
+        <v>A13SO-H11</v>
       </c>
       <c r="AC716" t="s">
         <v>142</v>
@@ -34823,7 +34823,7 @@
       </c>
       <c r="Z717" t="str">
         <f t="shared" si="6"/>
-        <v>A12SO-D3</v>
+        <v>A13SO-D3</v>
       </c>
       <c r="AC717" t="s">
         <v>156</v>
@@ -34856,7 +34856,7 @@
       </c>
       <c r="Z718" t="str">
         <f t="shared" si="6"/>
-        <v>A12SO-B12</v>
+        <v>A13SO-B12</v>
       </c>
       <c r="AC718" t="s">
         <v>133</v>
@@ -34889,7 +34889,7 @@
       </c>
       <c r="Z719" t="str">
         <f t="shared" si="6"/>
-        <v>A12SO-E9</v>
+        <v>A13SO-E9</v>
       </c>
       <c r="AC719" t="s">
         <v>168</v>

</xml_diff>

<commit_message>
updating data, storage, and resp raw data
</commit_message>
<xml_diff>
--- a/Data/2018-08-14_master_datac_2018_collection_year.xlsx
+++ b/Data/2018-08-14_master_datac_2018_collection_year.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andrew.nguyen\Desktop\Circadian_rhythm_runs_seasonal_timing\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A33B9B85-1FD3-4331-8EA7-19B9B1EE6DFE}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4076C75A-040A-4120-BD91-3722920AB626}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="53055" yWindow="465" windowWidth="36360" windowHeight="21135" activeTab="1" xr2:uid="{C7477166-8A7C-B04A-9643-C277FEDCDAAB}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9997" uniqueCount="694">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10244" uniqueCount="704">
   <si>
     <t>Ind_ID</t>
   </si>
@@ -2114,6 +2114,36 @@
   </si>
   <si>
     <t>15:17</t>
+  </si>
+  <si>
+    <t>A20-1</t>
+  </si>
+  <si>
+    <t>A20-2</t>
+  </si>
+  <si>
+    <t>A20-3</t>
+  </si>
+  <si>
+    <t>A20-4</t>
+  </si>
+  <si>
+    <t>A2-5-1</t>
+  </si>
+  <si>
+    <t>A2-5-2</t>
+  </si>
+  <si>
+    <t>A2-5-3</t>
+  </si>
+  <si>
+    <t>A2-5-4</t>
+  </si>
+  <si>
+    <t>A2-5-5</t>
+  </si>
+  <si>
+    <t>A2-5-6</t>
   </si>
 </sst>
 </file>
@@ -2697,8 +2727,8 @@
   <dimension ref="A1:AC306"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O103" sqref="O103"/>
+      <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A106" sqref="A106:XFD112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -6298,7 +6328,7 @@
         <v>188</v>
       </c>
       <c r="E63" s="14" t="s">
-        <v>184</v>
+        <v>207</v>
       </c>
       <c r="F63" s="14" t="s">
         <v>67</v>
@@ -6365,7 +6395,7 @@
         <v>188</v>
       </c>
       <c r="E64" s="14" t="s">
-        <v>184</v>
+        <v>207</v>
       </c>
       <c r="F64" s="14" t="s">
         <v>67</v>
@@ -6432,7 +6462,7 @@
         <v>188</v>
       </c>
       <c r="E65" s="14" t="s">
-        <v>184</v>
+        <v>207</v>
       </c>
       <c r="F65" s="14" t="s">
         <v>67</v>
@@ -12006,11 +12036,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92725FB9-1A17-2546-9DFA-6C0D39437891}">
-  <dimension ref="A1:AS1083"/>
+  <dimension ref="A1:AS1118"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A885" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A900" sqref="A900:XFD989"/>
+      <pane ySplit="1" topLeftCell="A981" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J996" sqref="J996"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -46719,6 +46749,15 @@
       <c r="K990" t="s">
         <v>61</v>
       </c>
+      <c r="L990">
+        <v>7000</v>
+      </c>
+      <c r="M990" s="20">
+        <v>0.38622685185185185</v>
+      </c>
+      <c r="N990">
+        <v>0.1599476</v>
+      </c>
       <c r="T990" s="1" t="s">
         <v>213</v>
       </c>
@@ -46751,6 +46790,15 @@
       <c r="K991" t="s">
         <v>61</v>
       </c>
+      <c r="L991">
+        <v>7000</v>
+      </c>
+      <c r="M991" s="20">
+        <v>0.38715277777777773</v>
+      </c>
+      <c r="N991">
+        <v>0.45276509999999998</v>
+      </c>
       <c r="T991" s="1" t="s">
         <v>213</v>
       </c>
@@ -46783,6 +46831,15 @@
       <c r="K992" t="s">
         <v>61</v>
       </c>
+      <c r="L992">
+        <v>7000</v>
+      </c>
+      <c r="M992" s="20">
+        <v>0.3880439814814815</v>
+      </c>
+      <c r="N992" s="21">
+        <v>4.0381090000000001E-2</v>
+      </c>
       <c r="T992" s="1" t="s">
         <v>213</v>
       </c>
@@ -46815,6 +46872,15 @@
       <c r="K993" t="s">
         <v>61</v>
       </c>
+      <c r="L993">
+        <v>7000</v>
+      </c>
+      <c r="M993" s="20">
+        <v>0.38880787037037035</v>
+      </c>
+      <c r="N993">
+        <v>0.35760560000000002</v>
+      </c>
       <c r="T993" s="1" t="s">
         <v>213</v>
       </c>
@@ -46847,6 +46913,15 @@
       <c r="K994" t="s">
         <v>61</v>
       </c>
+      <c r="L994">
+        <v>7000</v>
+      </c>
+      <c r="M994" s="20">
+        <v>0.38966435185185189</v>
+      </c>
+      <c r="N994" s="21">
+        <v>6.4647609999999994E-2</v>
+      </c>
       <c r="T994" s="1" t="s">
         <v>213</v>
       </c>
@@ -46879,6 +46954,15 @@
       <c r="K995" t="s">
         <v>61</v>
       </c>
+      <c r="L995">
+        <v>7000</v>
+      </c>
+      <c r="M995" s="20">
+        <v>0.39041666666666663</v>
+      </c>
+      <c r="N995">
+        <v>0.1237704</v>
+      </c>
       <c r="T995" s="1" t="s">
         <v>213</v>
       </c>
@@ -46911,6 +46995,15 @@
       <c r="K996" t="s">
         <v>61</v>
       </c>
+      <c r="L996">
+        <v>7000</v>
+      </c>
+      <c r="M996" s="20">
+        <v>0.39143518518518516</v>
+      </c>
+      <c r="N996" s="21">
+        <v>6.7688979999999996E-2</v>
+      </c>
       <c r="T996" s="1" t="s">
         <v>213</v>
       </c>
@@ -46943,6 +47036,15 @@
       <c r="K997" t="s">
         <v>61</v>
       </c>
+      <c r="L997">
+        <v>7000</v>
+      </c>
+      <c r="M997" s="20">
+        <v>0.39217592592592593</v>
+      </c>
+      <c r="N997" s="21">
+        <v>6.9644049999999999E-2</v>
+      </c>
       <c r="T997" s="1" t="s">
         <v>213</v>
       </c>
@@ -46975,6 +47077,15 @@
       <c r="K998" t="s">
         <v>61</v>
       </c>
+      <c r="L998">
+        <v>7000</v>
+      </c>
+      <c r="M998" s="20">
+        <v>0.39293981481481483</v>
+      </c>
+      <c r="N998">
+        <v>0.37370199999999998</v>
+      </c>
       <c r="T998" s="1" t="s">
         <v>213</v>
       </c>
@@ -47007,6 +47118,15 @@
       <c r="K999" t="s">
         <v>61</v>
       </c>
+      <c r="L999">
+        <v>7000</v>
+      </c>
+      <c r="M999" s="20">
+        <v>0.39376157407407408</v>
+      </c>
+      <c r="N999">
+        <v>0.39185619999999999</v>
+      </c>
       <c r="T999" s="1" t="s">
         <v>213</v>
       </c>
@@ -47039,6 +47159,15 @@
       <c r="K1000" t="s">
         <v>61</v>
       </c>
+      <c r="L1000">
+        <v>7000</v>
+      </c>
+      <c r="M1000" s="20">
+        <v>0.39461805555555557</v>
+      </c>
+      <c r="N1000">
+        <v>0.1216961</v>
+      </c>
       <c r="T1000" s="1" t="s">
         <v>213</v>
       </c>
@@ -47071,6 +47200,15 @@
       <c r="K1001" t="s">
         <v>61</v>
       </c>
+      <c r="L1001">
+        <v>7000</v>
+      </c>
+      <c r="M1001" s="20">
+        <v>0.395474537037037</v>
+      </c>
+      <c r="N1001" s="21">
+        <v>5.6496449999999997E-2</v>
+      </c>
       <c r="T1001" s="1" t="s">
         <v>213</v>
       </c>
@@ -47103,6 +47241,15 @@
       <c r="K1002" t="s">
         <v>61</v>
       </c>
+      <c r="L1002">
+        <v>7000</v>
+      </c>
+      <c r="M1002" s="20">
+        <v>0.39643518518518522</v>
+      </c>
+      <c r="N1002" s="21">
+        <v>5.0329440000000003E-2</v>
+      </c>
       <c r="T1002" s="1" t="s">
         <v>213</v>
       </c>
@@ -47135,6 +47282,15 @@
       <c r="K1003" t="s">
         <v>61</v>
       </c>
+      <c r="L1003">
+        <v>7000</v>
+      </c>
+      <c r="M1003" s="20">
+        <v>0.39717592592592593</v>
+      </c>
+      <c r="N1003" s="21">
+        <v>7.7695219999999995E-2</v>
+      </c>
       <c r="T1003" s="1" t="s">
         <v>213</v>
       </c>
@@ -47167,6 +47323,15 @@
       <c r="K1004" t="s">
         <v>61</v>
       </c>
+      <c r="L1004">
+        <v>7000</v>
+      </c>
+      <c r="M1004" s="20">
+        <v>0.39806712962962965</v>
+      </c>
+      <c r="N1004" s="21">
+        <v>8.1830490000000006E-2</v>
+      </c>
       <c r="T1004" s="1" t="s">
         <v>213</v>
       </c>
@@ -47199,6 +47364,15 @@
       <c r="K1005" t="s">
         <v>61</v>
       </c>
+      <c r="L1005">
+        <v>7000</v>
+      </c>
+      <c r="M1005" s="20">
+        <v>0.39872685185185186</v>
+      </c>
+      <c r="N1005" s="21">
+        <v>7.4962589999999996E-2</v>
+      </c>
       <c r="T1005" s="1" t="s">
         <v>213</v>
       </c>
@@ -47231,6 +47405,15 @@
       <c r="K1006" t="s">
         <v>61</v>
       </c>
+      <c r="L1006">
+        <v>7000</v>
+      </c>
+      <c r="M1006" s="20">
+        <v>0.39951388888888889</v>
+      </c>
+      <c r="N1006" s="21">
+        <v>6.2480430000000003E-2</v>
+      </c>
       <c r="T1006" s="1" t="s">
         <v>213</v>
       </c>
@@ -47263,6 +47446,15 @@
       <c r="K1007" t="s">
         <v>61</v>
       </c>
+      <c r="L1007">
+        <v>7000</v>
+      </c>
+      <c r="M1007" s="20">
+        <v>0.40034722222222219</v>
+      </c>
+      <c r="N1007" s="21">
+        <v>5.5404040000000002E-2</v>
+      </c>
       <c r="T1007" s="1" t="s">
         <v>213</v>
       </c>
@@ -47295,6 +47487,15 @@
       <c r="K1008" t="s">
         <v>61</v>
       </c>
+      <c r="L1008">
+        <v>7000</v>
+      </c>
+      <c r="M1008" s="20">
+        <v>0.40111111111111114</v>
+      </c>
+      <c r="N1008" s="21">
+        <v>4.8383839999999997E-2</v>
+      </c>
       <c r="T1008" s="1" t="s">
         <v>213</v>
       </c>
@@ -47327,6 +47528,15 @@
       <c r="K1009" t="s">
         <v>61</v>
       </c>
+      <c r="L1009">
+        <v>7000</v>
+      </c>
+      <c r="M1009" s="20">
+        <v>0.40180555555555553</v>
+      </c>
+      <c r="N1009">
+        <v>0.48377959999999998</v>
+      </c>
       <c r="T1009" s="1" t="s">
         <v>213</v>
       </c>
@@ -47359,6 +47569,15 @@
       <c r="K1010" t="s">
         <v>61</v>
       </c>
+      <c r="L1010">
+        <v>7000</v>
+      </c>
+      <c r="M1010" s="20">
+        <v>0.40263888888888894</v>
+      </c>
+      <c r="N1010" s="21">
+        <v>5.4492539999999999E-2</v>
+      </c>
       <c r="T1010" s="1" t="s">
         <v>213</v>
       </c>
@@ -47391,6 +47610,15 @@
       <c r="K1011" t="s">
         <v>61</v>
       </c>
+      <c r="L1011">
+        <v>7000</v>
+      </c>
+      <c r="M1011" s="20">
+        <v>0.40342592592592591</v>
+      </c>
+      <c r="N1011" s="21">
+        <v>7.0734630000000007E-2</v>
+      </c>
       <c r="T1011" s="1" t="s">
         <v>213</v>
       </c>
@@ -47423,6 +47651,15 @@
       <c r="K1012" t="s">
         <v>61</v>
       </c>
+      <c r="L1012">
+        <v>7000</v>
+      </c>
+      <c r="M1012" s="20">
+        <v>0.40421296296296294</v>
+      </c>
+      <c r="N1012">
+        <v>0.32921420000000001</v>
+      </c>
       <c r="T1012" s="1" t="s">
         <v>213</v>
       </c>
@@ -47455,6 +47692,15 @@
       <c r="K1013" t="s">
         <v>61</v>
       </c>
+      <c r="L1013">
+        <v>7000</v>
+      </c>
+      <c r="M1013" s="20">
+        <v>0.40501157407407407</v>
+      </c>
+      <c r="N1013" s="21">
+        <v>9.3297779999999997E-2</v>
+      </c>
       <c r="T1013" s="1" t="s">
         <v>213</v>
       </c>
@@ -47487,6 +47733,15 @@
       <c r="K1014" t="s">
         <v>61</v>
       </c>
+      <c r="L1014">
+        <v>7000</v>
+      </c>
+      <c r="M1014" s="20">
+        <v>0.40596064814814814</v>
+      </c>
+      <c r="N1014" s="21">
+        <v>5.9871340000000002E-2</v>
+      </c>
       <c r="T1014" s="1" t="s">
         <v>213</v>
       </c>
@@ -47519,6 +47774,15 @@
       <c r="K1015" t="s">
         <v>61</v>
       </c>
+      <c r="L1015">
+        <v>7000</v>
+      </c>
+      <c r="M1015" s="20">
+        <v>0.40673611111111113</v>
+      </c>
+      <c r="N1015" s="21">
+        <v>9.1106820000000005E-2</v>
+      </c>
       <c r="T1015" s="1" t="s">
         <v>213</v>
       </c>
@@ -47551,6 +47815,15 @@
       <c r="K1016" t="s">
         <v>61</v>
       </c>
+      <c r="L1016">
+        <v>7000</v>
+      </c>
+      <c r="M1016" s="20">
+        <v>0.40747685185185184</v>
+      </c>
+      <c r="N1016" s="21">
+        <v>7.4969049999999995E-2</v>
+      </c>
       <c r="T1016" s="1" t="s">
         <v>213</v>
       </c>
@@ -47583,6 +47856,15 @@
       <c r="K1017" t="s">
         <v>61</v>
       </c>
+      <c r="L1017">
+        <v>7000</v>
+      </c>
+      <c r="M1017" s="20">
+        <v>0.40841435185185188</v>
+      </c>
+      <c r="N1017">
+        <v>0.2690111</v>
+      </c>
       <c r="T1017" s="1" t="s">
         <v>213</v>
       </c>
@@ -47615,6 +47897,15 @@
       <c r="K1018" t="s">
         <v>61</v>
       </c>
+      <c r="L1018">
+        <v>7000</v>
+      </c>
+      <c r="M1018" s="20">
+        <v>0.40920138888888885</v>
+      </c>
+      <c r="N1018" s="21">
+        <v>7.4936610000000001E-2</v>
+      </c>
       <c r="T1018" s="1" t="s">
         <v>213</v>
       </c>
@@ -47647,6 +47938,15 @@
       <c r="K1019" t="s">
         <v>61</v>
       </c>
+      <c r="L1019">
+        <v>7000</v>
+      </c>
+      <c r="M1019" s="20">
+        <v>0.40993055555555552</v>
+      </c>
+      <c r="N1019" s="21">
+        <v>9.009578E-2</v>
+      </c>
       <c r="T1019" s="1" t="s">
         <v>213</v>
       </c>
@@ -47679,6 +47979,15 @@
       <c r="K1020" t="s">
         <v>61</v>
       </c>
+      <c r="L1020">
+        <v>7000</v>
+      </c>
+      <c r="M1020" s="20">
+        <v>0.41104166666666669</v>
+      </c>
+      <c r="N1020" s="21">
+        <v>7.5274859999999999E-2</v>
+      </c>
       <c r="T1020" s="1" t="s">
         <v>213</v>
       </c>
@@ -47711,6 +48020,15 @@
       <c r="K1021" t="s">
         <v>61</v>
       </c>
+      <c r="L1021">
+        <v>7000</v>
+      </c>
+      <c r="M1021" s="20">
+        <v>0.41177083333333336</v>
+      </c>
+      <c r="N1021" s="21">
+        <v>8.6463960000000006E-2</v>
+      </c>
       <c r="T1021" s="1" t="s">
         <v>213</v>
       </c>
@@ -47743,6 +48061,15 @@
       <c r="K1022" t="s">
         <v>61</v>
       </c>
+      <c r="L1022">
+        <v>7000</v>
+      </c>
+      <c r="M1022" s="20">
+        <v>0.41273148148148148</v>
+      </c>
+      <c r="N1022" s="21">
+        <v>7.8758170000000002E-2</v>
+      </c>
       <c r="T1022" s="1" t="s">
         <v>213</v>
       </c>
@@ -47775,6 +48102,15 @@
       <c r="K1023" t="s">
         <v>61</v>
       </c>
+      <c r="L1023">
+        <v>7000</v>
+      </c>
+      <c r="M1023" s="20">
+        <v>0.41363425925925923</v>
+      </c>
+      <c r="N1023" s="21">
+        <v>9.1868320000000003E-2</v>
+      </c>
       <c r="T1023" s="1" t="s">
         <v>213</v>
       </c>
@@ -47807,6 +48143,15 @@
       <c r="K1024" t="s">
         <v>61</v>
       </c>
+      <c r="L1024">
+        <v>7000</v>
+      </c>
+      <c r="M1024" s="20">
+        <v>0.41439814814814818</v>
+      </c>
+      <c r="N1024">
+        <v>0.30310769999999998</v>
+      </c>
       <c r="T1024" s="1" t="s">
         <v>213</v>
       </c>
@@ -47839,6 +48184,15 @@
       <c r="K1025" t="s">
         <v>61</v>
       </c>
+      <c r="L1025">
+        <v>7000</v>
+      </c>
+      <c r="M1025" s="20">
+        <v>0.4152777777777778</v>
+      </c>
+      <c r="N1025" s="21">
+        <v>6.4114069999999995E-2</v>
+      </c>
       <c r="T1025" s="1" t="s">
         <v>213</v>
       </c>
@@ -47871,6 +48225,15 @@
       <c r="K1026" t="s">
         <v>61</v>
       </c>
+      <c r="L1026">
+        <v>7000</v>
+      </c>
+      <c r="M1026" s="20">
+        <v>0.41600694444444447</v>
+      </c>
+      <c r="N1026">
+        <v>0.1605722</v>
+      </c>
       <c r="T1026" s="1" t="s">
         <v>213</v>
       </c>
@@ -47903,6 +48266,15 @@
       <c r="K1027" t="s">
         <v>61</v>
       </c>
+      <c r="L1027">
+        <v>7000</v>
+      </c>
+      <c r="M1027" s="20">
+        <v>0.41677083333333331</v>
+      </c>
+      <c r="N1027">
+        <v>0.52054400000000001</v>
+      </c>
       <c r="T1027" s="1" t="s">
         <v>213</v>
       </c>
@@ -47935,6 +48307,15 @@
       <c r="K1028" t="s">
         <v>61</v>
       </c>
+      <c r="L1028">
+        <v>7000</v>
+      </c>
+      <c r="M1028" s="20">
+        <v>0.41783564814814816</v>
+      </c>
+      <c r="N1028" s="21">
+        <v>7.247344E-2</v>
+      </c>
       <c r="T1028" s="1" t="s">
         <v>213</v>
       </c>
@@ -47967,6 +48348,15 @@
       <c r="K1029" t="s">
         <v>61</v>
       </c>
+      <c r="L1029">
+        <v>7000</v>
+      </c>
+      <c r="M1029" s="20">
+        <v>0.41862268518518514</v>
+      </c>
+      <c r="N1029">
+        <v>0.43283549999999998</v>
+      </c>
       <c r="T1029" s="1" t="s">
         <v>213</v>
       </c>
@@ -47999,6 +48389,15 @@
       <c r="K1030" t="s">
         <v>61</v>
       </c>
+      <c r="L1030">
+        <v>7000</v>
+      </c>
+      <c r="M1030" s="20">
+        <v>0.41934027777777777</v>
+      </c>
+      <c r="N1030">
+        <v>0.5201945</v>
+      </c>
       <c r="T1030" s="1" t="s">
         <v>213</v>
       </c>
@@ -48031,6 +48430,15 @@
       <c r="K1031" t="s">
         <v>61</v>
       </c>
+      <c r="L1031">
+        <v>7000</v>
+      </c>
+      <c r="M1031" s="20">
+        <v>0.42026620370370371</v>
+      </c>
+      <c r="N1031" s="21">
+        <v>6.5045919999999993E-2</v>
+      </c>
       <c r="T1031" s="1" t="s">
         <v>213</v>
       </c>
@@ -48063,6 +48471,15 @@
       <c r="K1032" t="s">
         <v>61</v>
       </c>
+      <c r="L1032">
+        <v>7000</v>
+      </c>
+      <c r="M1032" s="20">
+        <v>0.42106481481481484</v>
+      </c>
+      <c r="N1032" s="21">
+        <v>5.0732770000000003E-2</v>
+      </c>
       <c r="T1032" s="1" t="s">
         <v>213</v>
       </c>
@@ -48095,6 +48512,15 @@
       <c r="K1033" t="s">
         <v>61</v>
       </c>
+      <c r="L1033">
+        <v>7000</v>
+      </c>
+      <c r="M1033" s="20">
+        <v>0.42192129629629632</v>
+      </c>
+      <c r="N1033" s="21">
+        <v>4.7503950000000003E-2</v>
+      </c>
       <c r="T1033" s="1" t="s">
         <v>213</v>
       </c>
@@ -48127,6 +48553,15 @@
       <c r="K1034" t="s">
         <v>61</v>
       </c>
+      <c r="L1034">
+        <v>7000</v>
+      </c>
+      <c r="M1034" s="20">
+        <v>0.4227083333333333</v>
+      </c>
+      <c r="N1034">
+        <v>0.13220019999999999</v>
+      </c>
       <c r="T1034" s="1" t="s">
         <v>213</v>
       </c>
@@ -48156,6 +48591,15 @@
       <c r="K1035" t="s">
         <v>61</v>
       </c>
+      <c r="L1035">
+        <v>7000</v>
+      </c>
+      <c r="M1035" s="20">
+        <v>0.42347222222222225</v>
+      </c>
+      <c r="N1035" s="21">
+        <v>9.6734969999999997E-3</v>
+      </c>
       <c r="T1035" s="1" t="s">
         <v>213</v>
       </c>
@@ -48188,6 +48632,15 @@
       <c r="K1036" t="s">
         <v>61</v>
       </c>
+      <c r="L1036">
+        <v>7000</v>
+      </c>
+      <c r="M1036" s="20">
+        <v>0.42451388888888886</v>
+      </c>
+      <c r="N1036" s="21">
+        <v>9.6405880000000003E-3</v>
+      </c>
       <c r="T1036" s="1" t="s">
         <v>213</v>
       </c>
@@ -48223,6 +48676,15 @@
       <c r="K1037" t="s">
         <v>61</v>
       </c>
+      <c r="L1037">
+        <v>6262</v>
+      </c>
+      <c r="M1037" s="20">
+        <v>0.38622685185185185</v>
+      </c>
+      <c r="N1037">
+        <v>0.53582229999999997</v>
+      </c>
       <c r="T1037" s="1" t="s">
         <v>213</v>
       </c>
@@ -48255,6 +48717,15 @@
       <c r="K1038" t="s">
         <v>61</v>
       </c>
+      <c r="L1038">
+        <v>6262</v>
+      </c>
+      <c r="M1038" s="20">
+        <v>0.38715277777777773</v>
+      </c>
+      <c r="N1038">
+        <v>0.1563206</v>
+      </c>
       <c r="T1038" s="1" t="s">
         <v>213</v>
       </c>
@@ -48287,6 +48758,15 @@
       <c r="K1039" t="s">
         <v>61</v>
       </c>
+      <c r="L1039">
+        <v>6262</v>
+      </c>
+      <c r="M1039" s="20">
+        <v>0.3880439814814815</v>
+      </c>
+      <c r="N1039">
+        <v>0.1032771</v>
+      </c>
       <c r="T1039" s="1" t="s">
         <v>213</v>
       </c>
@@ -48319,6 +48799,15 @@
       <c r="K1040" t="s">
         <v>61</v>
       </c>
+      <c r="L1040">
+        <v>6262</v>
+      </c>
+      <c r="M1040" s="20">
+        <v>0.38880787037037035</v>
+      </c>
+      <c r="N1040">
+        <v>0.12387380000000001</v>
+      </c>
       <c r="T1040" s="1" t="s">
         <v>213</v>
       </c>
@@ -48351,6 +48840,15 @@
       <c r="K1041" t="s">
         <v>61</v>
       </c>
+      <c r="L1041">
+        <v>6262</v>
+      </c>
+      <c r="M1041" s="20">
+        <v>0.38966435185185189</v>
+      </c>
+      <c r="N1041">
+        <v>0.17735790000000001</v>
+      </c>
       <c r="T1041" s="1" t="s">
         <v>213</v>
       </c>
@@ -48383,6 +48881,15 @@
       <c r="K1042" t="s">
         <v>61</v>
       </c>
+      <c r="L1042">
+        <v>6262</v>
+      </c>
+      <c r="M1042" s="20">
+        <v>0.39041666666666663</v>
+      </c>
+      <c r="N1042">
+        <v>1.2198629999999999</v>
+      </c>
       <c r="T1042" s="1" t="s">
         <v>213</v>
       </c>
@@ -48415,6 +48922,15 @@
       <c r="K1043" t="s">
         <v>61</v>
       </c>
+      <c r="L1043">
+        <v>6262</v>
+      </c>
+      <c r="M1043" s="20">
+        <v>0.39143518518518516</v>
+      </c>
+      <c r="N1043">
+        <v>0.1508727</v>
+      </c>
       <c r="T1043" s="1" t="s">
         <v>213</v>
       </c>
@@ -48447,6 +48963,15 @@
       <c r="K1044" t="s">
         <v>61</v>
       </c>
+      <c r="L1044">
+        <v>6262</v>
+      </c>
+      <c r="M1044" s="20">
+        <v>0.39217592592592593</v>
+      </c>
+      <c r="N1044" s="21">
+        <v>7.9226580000000005E-2</v>
+      </c>
       <c r="T1044" s="1" t="s">
         <v>213</v>
       </c>
@@ -48479,6 +49004,15 @@
       <c r="K1045" t="s">
         <v>61</v>
       </c>
+      <c r="L1045">
+        <v>6262</v>
+      </c>
+      <c r="M1045" s="20">
+        <v>0.39293981481481483</v>
+      </c>
+      <c r="N1045" s="21">
+        <v>7.9388280000000006E-2</v>
+      </c>
       <c r="T1045" s="1" t="s">
         <v>213</v>
       </c>
@@ -48511,6 +49045,15 @@
       <c r="K1046" t="s">
         <v>61</v>
       </c>
+      <c r="L1046">
+        <v>6262</v>
+      </c>
+      <c r="M1046" s="20">
+        <v>0.39376157407407408</v>
+      </c>
+      <c r="N1046">
+        <v>0.14393410000000001</v>
+      </c>
       <c r="T1046" s="1" t="s">
         <v>213</v>
       </c>
@@ -48543,6 +49086,15 @@
       <c r="K1047" t="s">
         <v>61</v>
       </c>
+      <c r="L1047">
+        <v>6262</v>
+      </c>
+      <c r="M1047" s="20">
+        <v>0.39461805555555557</v>
+      </c>
+      <c r="N1047">
+        <v>0.117183</v>
+      </c>
       <c r="T1047" s="1" t="s">
         <v>213</v>
       </c>
@@ -48575,6 +49127,15 @@
       <c r="K1048" t="s">
         <v>61</v>
       </c>
+      <c r="L1048">
+        <v>6262</v>
+      </c>
+      <c r="M1048" s="20">
+        <v>0.395474537037037</v>
+      </c>
+      <c r="N1048">
+        <v>0.82421829999999996</v>
+      </c>
       <c r="T1048" s="1" t="s">
         <v>213</v>
       </c>
@@ -48607,6 +49168,15 @@
       <c r="K1049" t="s">
         <v>61</v>
       </c>
+      <c r="L1049">
+        <v>6262</v>
+      </c>
+      <c r="M1049" s="20">
+        <v>0.39643518518518522</v>
+      </c>
+      <c r="N1049">
+        <v>0.1126433</v>
+      </c>
       <c r="T1049" s="1" t="s">
         <v>213</v>
       </c>
@@ -48639,6 +49209,15 @@
       <c r="K1050" t="s">
         <v>61</v>
       </c>
+      <c r="L1050">
+        <v>6262</v>
+      </c>
+      <c r="M1050" s="20">
+        <v>0.39717592592592593</v>
+      </c>
+      <c r="N1050">
+        <v>0.66805639999999999</v>
+      </c>
       <c r="T1050" s="1" t="s">
         <v>213</v>
       </c>
@@ -48671,6 +49250,15 @@
       <c r="K1051" t="s">
         <v>61</v>
       </c>
+      <c r="L1051">
+        <v>6262</v>
+      </c>
+      <c r="M1051" s="20">
+        <v>0.39806712962962965</v>
+      </c>
+      <c r="N1051" s="21">
+        <v>6.4429570000000005E-2</v>
+      </c>
       <c r="T1051" s="1" t="s">
         <v>213</v>
       </c>
@@ -48703,6 +49291,15 @@
       <c r="K1052" t="s">
         <v>61</v>
       </c>
+      <c r="L1052">
+        <v>6262</v>
+      </c>
+      <c r="M1052" s="20">
+        <v>0.39872685185185186</v>
+      </c>
+      <c r="N1052">
+        <v>7.8821500000000003E-2</v>
+      </c>
       <c r="T1052" s="1" t="s">
         <v>213</v>
       </c>
@@ -48735,6 +49332,15 @@
       <c r="K1053" t="s">
         <v>61</v>
       </c>
+      <c r="L1053">
+        <v>6262</v>
+      </c>
+      <c r="M1053" s="20">
+        <v>0.39951388888888889</v>
+      </c>
+      <c r="N1053">
+        <v>8.7887499999999993E-2</v>
+      </c>
       <c r="T1053" s="1" t="s">
         <v>213</v>
       </c>
@@ -48767,6 +49373,15 @@
       <c r="K1054" t="s">
         <v>61</v>
       </c>
+      <c r="L1054">
+        <v>6262</v>
+      </c>
+      <c r="M1054" s="20">
+        <v>0.40034722222222219</v>
+      </c>
+      <c r="N1054" s="21">
+        <v>9.0903639999999994E-2</v>
+      </c>
       <c r="T1054" s="1" t="s">
         <v>213</v>
       </c>
@@ -48799,6 +49414,15 @@
       <c r="K1055" t="s">
         <v>61</v>
       </c>
+      <c r="L1055">
+        <v>6262</v>
+      </c>
+      <c r="M1055" s="20">
+        <v>0.40111111111111114</v>
+      </c>
+      <c r="N1055" s="21">
+        <v>5.9986780000000003E-2</v>
+      </c>
       <c r="T1055" s="1" t="s">
         <v>213</v>
       </c>
@@ -48831,6 +49455,15 @@
       <c r="K1056" t="s">
         <v>61</v>
       </c>
+      <c r="L1056">
+        <v>6262</v>
+      </c>
+      <c r="M1056" s="20">
+        <v>0.40180555555555553</v>
+      </c>
+      <c r="N1056">
+        <v>0.1607354</v>
+      </c>
       <c r="T1056" s="1" t="s">
         <v>213</v>
       </c>
@@ -48863,6 +49496,15 @@
       <c r="K1057" t="s">
         <v>61</v>
       </c>
+      <c r="L1057">
+        <v>6262</v>
+      </c>
+      <c r="M1057" s="20">
+        <v>0.40263888888888894</v>
+      </c>
+      <c r="N1057">
+        <v>0.1230528</v>
+      </c>
       <c r="T1057" s="1" t="s">
         <v>213</v>
       </c>
@@ -48895,6 +49537,15 @@
       <c r="K1058" t="s">
         <v>61</v>
       </c>
+      <c r="L1058">
+        <v>6262</v>
+      </c>
+      <c r="M1058" s="20">
+        <v>0.40342592592592591</v>
+      </c>
+      <c r="N1058">
+        <v>0.12855800000000001</v>
+      </c>
       <c r="T1058" s="1" t="s">
         <v>213</v>
       </c>
@@ -48927,6 +49578,15 @@
       <c r="K1059" t="s">
         <v>61</v>
       </c>
+      <c r="L1059">
+        <v>6262</v>
+      </c>
+      <c r="M1059" s="20">
+        <v>0.40421296296296294</v>
+      </c>
+      <c r="N1059" s="21">
+        <v>7.2165549999999995E-2</v>
+      </c>
       <c r="T1059" s="1" t="s">
         <v>213</v>
       </c>
@@ -48959,6 +49619,15 @@
       <c r="K1060" t="s">
         <v>61</v>
       </c>
+      <c r="L1060">
+        <v>6262</v>
+      </c>
+      <c r="M1060" s="20">
+        <v>0.40501157407407407</v>
+      </c>
+      <c r="N1060">
+        <v>0.79508699999999999</v>
+      </c>
       <c r="T1060" s="1" t="s">
         <v>213</v>
       </c>
@@ -48991,6 +49660,15 @@
       <c r="K1061" t="s">
         <v>61</v>
       </c>
+      <c r="L1061">
+        <v>6262</v>
+      </c>
+      <c r="M1061" s="20">
+        <v>0.40596064814814814</v>
+      </c>
+      <c r="N1061">
+        <v>0.1354204</v>
+      </c>
       <c r="T1061" s="1" t="s">
         <v>213</v>
       </c>
@@ -49023,6 +49701,15 @@
       <c r="K1062" t="s">
         <v>61</v>
       </c>
+      <c r="L1062">
+        <v>6262</v>
+      </c>
+      <c r="M1062" s="20">
+        <v>0.40673611111111113</v>
+      </c>
+      <c r="N1062" s="21">
+        <v>8.4525180000000005E-2</v>
+      </c>
       <c r="T1062" s="1" t="s">
         <v>213</v>
       </c>
@@ -49055,6 +49742,15 @@
       <c r="K1063" t="s">
         <v>61</v>
       </c>
+      <c r="L1063">
+        <v>6262</v>
+      </c>
+      <c r="M1063" s="20">
+        <v>0.40747685185185184</v>
+      </c>
+      <c r="N1063">
+        <v>1.0307489999999999</v>
+      </c>
       <c r="T1063" s="1" t="s">
         <v>213</v>
       </c>
@@ -49087,6 +49783,15 @@
       <c r="K1064" t="s">
         <v>61</v>
       </c>
+      <c r="L1064">
+        <v>6262</v>
+      </c>
+      <c r="M1064" s="20">
+        <v>0.40841435185185188</v>
+      </c>
+      <c r="N1064" s="21">
+        <v>9.0086669999999994E-2</v>
+      </c>
       <c r="T1064" s="1" t="s">
         <v>213</v>
       </c>
@@ -49119,6 +49824,15 @@
       <c r="K1065" t="s">
         <v>61</v>
       </c>
+      <c r="L1065">
+        <v>6262</v>
+      </c>
+      <c r="M1065" s="20">
+        <v>0.40920138888888885</v>
+      </c>
+      <c r="N1065">
+        <v>0.101032</v>
+      </c>
       <c r="T1065" s="1" t="s">
         <v>213</v>
       </c>
@@ -49151,6 +49865,15 @@
       <c r="K1066" t="s">
         <v>61</v>
       </c>
+      <c r="L1066">
+        <v>6262</v>
+      </c>
+      <c r="M1066" s="20">
+        <v>0.40993055555555552</v>
+      </c>
+      <c r="N1066">
+        <v>1.315436</v>
+      </c>
       <c r="T1066" s="1" t="s">
         <v>213</v>
       </c>
@@ -49183,6 +49906,15 @@
       <c r="K1067" t="s">
         <v>61</v>
       </c>
+      <c r="L1067">
+        <v>6262</v>
+      </c>
+      <c r="M1067" s="20">
+        <v>0.41104166666666669</v>
+      </c>
+      <c r="N1067" s="21">
+        <v>6.2707470000000001E-2</v>
+      </c>
       <c r="T1067" s="1" t="s">
         <v>213</v>
       </c>
@@ -49215,6 +49947,15 @@
       <c r="K1068" t="s">
         <v>61</v>
       </c>
+      <c r="L1068">
+        <v>6262</v>
+      </c>
+      <c r="M1068" s="20">
+        <v>0.41177083333333336</v>
+      </c>
+      <c r="N1068">
+        <v>0.86417460000000001</v>
+      </c>
       <c r="T1068" s="1" t="s">
         <v>213</v>
       </c>
@@ -49247,6 +49988,15 @@
       <c r="K1069" t="s">
         <v>61</v>
       </c>
+      <c r="L1069">
+        <v>6262</v>
+      </c>
+      <c r="M1069" s="20">
+        <v>0.41273148148148148</v>
+      </c>
+      <c r="N1069" s="21">
+        <v>8.6048449999999999E-2</v>
+      </c>
       <c r="T1069" s="1" t="s">
         <v>213</v>
       </c>
@@ -49279,6 +50029,15 @@
       <c r="K1070" t="s">
         <v>61</v>
       </c>
+      <c r="L1070">
+        <v>6262</v>
+      </c>
+      <c r="M1070" s="20">
+        <v>0.41363425925925923</v>
+      </c>
+      <c r="N1070">
+        <v>0.1086746</v>
+      </c>
       <c r="T1070" s="1" t="s">
         <v>213</v>
       </c>
@@ -49311,6 +50070,15 @@
       <c r="K1071" t="s">
         <v>61</v>
       </c>
+      <c r="L1071">
+        <v>6262</v>
+      </c>
+      <c r="M1071" s="20">
+        <v>0.41439814814814818</v>
+      </c>
+      <c r="N1071" s="21">
+        <v>9.0717629999999994E-2</v>
+      </c>
       <c r="T1071" s="1" t="s">
         <v>213</v>
       </c>
@@ -49343,11 +50111,20 @@
       <c r="K1072" t="s">
         <v>61</v>
       </c>
+      <c r="L1072">
+        <v>6262</v>
+      </c>
+      <c r="M1072" s="20">
+        <v>0.4152777777777778</v>
+      </c>
+      <c r="N1072" s="21">
+        <v>8.322562E-2</v>
+      </c>
       <c r="T1072" s="1" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="1073" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1073" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1073">
         <v>37</v>
       </c>
@@ -49375,11 +50152,20 @@
       <c r="K1073" t="s">
         <v>61</v>
       </c>
+      <c r="L1073">
+        <v>6262</v>
+      </c>
+      <c r="M1073" s="20">
+        <v>0.41600694444444447</v>
+      </c>
+      <c r="N1073">
+        <v>0.1316833</v>
+      </c>
       <c r="T1073" s="1" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="1074" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1074" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1074">
         <v>38</v>
       </c>
@@ -49407,11 +50193,20 @@
       <c r="K1074" t="s">
         <v>61</v>
       </c>
+      <c r="L1074">
+        <v>6262</v>
+      </c>
+      <c r="M1074" s="20">
+        <v>0.41677083333333331</v>
+      </c>
+      <c r="N1074">
+        <v>1.022467</v>
+      </c>
       <c r="T1074" s="1" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="1075" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1075" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1075">
         <v>39</v>
       </c>
@@ -49439,11 +50234,20 @@
       <c r="K1075" t="s">
         <v>61</v>
       </c>
+      <c r="L1075">
+        <v>6262</v>
+      </c>
+      <c r="M1075" s="20">
+        <v>0.41783564814814816</v>
+      </c>
+      <c r="N1075">
+        <v>0.10568180000000001</v>
+      </c>
       <c r="T1075" s="1" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="1076" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1076" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1076">
         <v>40</v>
       </c>
@@ -49471,11 +50275,20 @@
       <c r="K1076" t="s">
         <v>61</v>
       </c>
+      <c r="L1076">
+        <v>6262</v>
+      </c>
+      <c r="M1076" s="20">
+        <v>0.41862268518518514</v>
+      </c>
+      <c r="N1076" s="21">
+        <v>5.720592E-2</v>
+      </c>
       <c r="T1076" s="1" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="1077" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1077" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1077">
         <v>41</v>
       </c>
@@ -49503,11 +50316,20 @@
       <c r="K1077" t="s">
         <v>61</v>
       </c>
+      <c r="L1077">
+        <v>6262</v>
+      </c>
+      <c r="M1077" s="20">
+        <v>0.41934027777777777</v>
+      </c>
+      <c r="N1077">
+        <v>0.80207340000000005</v>
+      </c>
       <c r="T1077" s="1" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="1078" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1078" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1078">
         <v>42</v>
       </c>
@@ -49535,11 +50357,20 @@
       <c r="K1078" t="s">
         <v>61</v>
       </c>
+      <c r="L1078">
+        <v>6262</v>
+      </c>
+      <c r="M1078" s="20">
+        <v>0.42026620370370371</v>
+      </c>
+      <c r="N1078">
+        <v>0.17547650000000001</v>
+      </c>
       <c r="T1078" s="1" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="1079" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1079" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1079">
         <v>43</v>
       </c>
@@ -49567,11 +50398,20 @@
       <c r="K1079" t="s">
         <v>61</v>
       </c>
+      <c r="L1079">
+        <v>6262</v>
+      </c>
+      <c r="M1079" s="20">
+        <v>0.42106481481481484</v>
+      </c>
+      <c r="N1079">
+        <v>0.17211609999999999</v>
+      </c>
       <c r="T1079" s="1" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="1080" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1080" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1080">
         <v>44</v>
       </c>
@@ -49599,11 +50439,20 @@
       <c r="K1080" t="s">
         <v>61</v>
       </c>
+      <c r="L1080">
+        <v>6262</v>
+      </c>
+      <c r="M1080" s="20">
+        <v>0.42192129629629632</v>
+      </c>
+      <c r="N1080">
+        <v>0.1636775</v>
+      </c>
       <c r="T1080" s="1" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="1081" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1081" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1081">
         <v>45</v>
       </c>
@@ -49631,11 +50480,20 @@
       <c r="K1081" t="s">
         <v>61</v>
       </c>
+      <c r="L1081">
+        <v>6262</v>
+      </c>
+      <c r="M1081" s="20">
+        <v>0.4227083333333333</v>
+      </c>
+      <c r="N1081" s="21">
+        <v>7.8189869999999995E-2</v>
+      </c>
       <c r="T1081" s="1" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="1082" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1082" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1082">
         <v>46</v>
       </c>
@@ -49660,8 +50518,20 @@
       <c r="K1082" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="1083" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="L1082">
+        <v>6262</v>
+      </c>
+      <c r="M1082" s="20">
+        <v>0.42347222222222225</v>
+      </c>
+      <c r="N1082" s="21">
+        <v>1.467134E-2</v>
+      </c>
+      <c r="T1082" s="1" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="1083" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1083">
         <v>47</v>
       </c>
@@ -49688,6 +50558,1133 @@
       </c>
       <c r="K1083" t="s">
         <v>61</v>
+      </c>
+      <c r="L1083">
+        <v>6262</v>
+      </c>
+      <c r="M1083" s="20">
+        <v>0.42451388888888886</v>
+      </c>
+      <c r="N1083" s="21">
+        <v>1.234064E-2</v>
+      </c>
+      <c r="T1083" s="1" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="1084" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1084">
+        <v>1</v>
+      </c>
+      <c r="C1084" t="s">
+        <v>60</v>
+      </c>
+      <c r="G1084" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I1084" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="J1084">
+        <v>20</v>
+      </c>
+      <c r="K1084" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1084" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="Y1084" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z1084" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="1085" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1085">
+        <v>2</v>
+      </c>
+      <c r="C1085" t="s">
+        <v>60</v>
+      </c>
+      <c r="G1085" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I1085" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="J1085">
+        <v>20</v>
+      </c>
+      <c r="K1085" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1085" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="Y1085" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z1085" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="1086" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1086">
+        <v>3</v>
+      </c>
+      <c r="C1086" t="s">
+        <v>60</v>
+      </c>
+      <c r="G1086" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I1086" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="J1086">
+        <v>20</v>
+      </c>
+      <c r="K1086" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1086" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="Y1086" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z1086" t="s">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="1087" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1087">
+        <v>4</v>
+      </c>
+      <c r="C1087" t="s">
+        <v>60</v>
+      </c>
+      <c r="G1087" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I1087" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="J1087">
+        <v>20</v>
+      </c>
+      <c r="K1087" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1087" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="Y1087" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z1087" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="1088" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1088">
+        <v>1</v>
+      </c>
+      <c r="C1088" t="s">
+        <v>60</v>
+      </c>
+      <c r="G1088" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I1088" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="J1088">
+        <v>20</v>
+      </c>
+      <c r="K1088" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1088" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="Y1088" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z1088" t="str">
+        <f>"A20"&amp;Y1088&amp;"-"&amp;AC1088</f>
+        <v>A20RT-A1</v>
+      </c>
+      <c r="AC1088" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="1089" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1089">
+        <v>2</v>
+      </c>
+      <c r="C1089" t="s">
+        <v>60</v>
+      </c>
+      <c r="G1089" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I1089" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="J1089">
+        <v>20</v>
+      </c>
+      <c r="K1089" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1089" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="Y1089" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z1089" t="str">
+        <f t="shared" ref="Z1089:Z1097" si="10">"A20"&amp;Y1089&amp;"-"&amp;AC1089</f>
+        <v>A20RT-A2</v>
+      </c>
+      <c r="AC1089" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="1090" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1090">
+        <v>3</v>
+      </c>
+      <c r="C1090" t="s">
+        <v>60</v>
+      </c>
+      <c r="G1090" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I1090" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="J1090">
+        <v>20</v>
+      </c>
+      <c r="K1090" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1090" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="Y1090" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z1090" t="str">
+        <f t="shared" si="10"/>
+        <v>A20RT-A3</v>
+      </c>
+      <c r="AC1090" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="1091" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1091">
+        <v>4</v>
+      </c>
+      <c r="C1091" t="s">
+        <v>60</v>
+      </c>
+      <c r="G1091" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I1091" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="J1091">
+        <v>20</v>
+      </c>
+      <c r="K1091" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1091" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="Y1091" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z1091" t="str">
+        <f t="shared" si="10"/>
+        <v>A20RT-A4</v>
+      </c>
+      <c r="AC1091" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="1092" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1092">
+        <v>1</v>
+      </c>
+      <c r="C1092" t="s">
+        <v>60</v>
+      </c>
+      <c r="G1092" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I1092" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="J1092">
+        <v>20</v>
+      </c>
+      <c r="K1092" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1092" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="Y1092" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z1092" t="str">
+        <f t="shared" si="10"/>
+        <v>A20SO-A1</v>
+      </c>
+      <c r="AC1092" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="1093" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1093">
+        <v>2</v>
+      </c>
+      <c r="C1093" t="s">
+        <v>60</v>
+      </c>
+      <c r="G1093" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I1093" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="J1093">
+        <v>20</v>
+      </c>
+      <c r="K1093" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1093" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="Y1093" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z1093" t="str">
+        <f t="shared" si="10"/>
+        <v>A20SO-A2</v>
+      </c>
+      <c r="AC1093" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="1094" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1094">
+        <v>3</v>
+      </c>
+      <c r="C1094" t="s">
+        <v>60</v>
+      </c>
+      <c r="G1094" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I1094" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="J1094">
+        <v>20</v>
+      </c>
+      <c r="K1094" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1094" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="Y1094" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z1094" t="str">
+        <f t="shared" si="10"/>
+        <v>A20SO-A3</v>
+      </c>
+      <c r="AC1094" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="1095" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1095">
+        <v>4</v>
+      </c>
+      <c r="C1095" t="s">
+        <v>60</v>
+      </c>
+      <c r="G1095" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I1095" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="J1095">
+        <v>20</v>
+      </c>
+      <c r="K1095" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1095" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="Y1095" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z1095" t="str">
+        <f t="shared" si="10"/>
+        <v>A20SO-A4</v>
+      </c>
+      <c r="AC1095" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="1096" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1096">
+        <v>5</v>
+      </c>
+      <c r="C1096" t="s">
+        <v>202</v>
+      </c>
+      <c r="G1096" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1096" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="J1096">
+        <v>5</v>
+      </c>
+      <c r="K1096" t="s">
+        <v>203</v>
+      </c>
+      <c r="T1096" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="Y1096" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z1096" t="str">
+        <f t="shared" si="10"/>
+        <v>A20RT-A5</v>
+      </c>
+      <c r="AC1096" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="1097" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1097">
+        <v>5</v>
+      </c>
+      <c r="C1097" t="s">
+        <v>202</v>
+      </c>
+      <c r="G1097" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1097" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="J1097">
+        <v>5</v>
+      </c>
+      <c r="K1097" t="s">
+        <v>203</v>
+      </c>
+      <c r="T1097" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="Y1097" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z1097" t="str">
+        <f t="shared" si="10"/>
+        <v>A20SO-A5</v>
+      </c>
+      <c r="AC1097" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="1098" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1098">
+        <v>5</v>
+      </c>
+      <c r="C1098" t="s">
+        <v>60</v>
+      </c>
+      <c r="G1098" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1098" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="J1098">
+        <v>5</v>
+      </c>
+      <c r="K1098" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1098" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="Y1098" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z1098" t="s">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="1099" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1099">
+        <v>6</v>
+      </c>
+      <c r="C1099" t="s">
+        <v>60</v>
+      </c>
+      <c r="G1099" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1099" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="J1099">
+        <v>5</v>
+      </c>
+      <c r="K1099" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1099" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="Y1099" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z1099" t="str">
+        <f>"A2-5"&amp;Y1099&amp;"-"&amp;AC1099</f>
+        <v>A2-5RT-A6</v>
+      </c>
+      <c r="AC1099" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="1100" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1100">
+        <v>6</v>
+      </c>
+      <c r="C1100" t="s">
+        <v>60</v>
+      </c>
+      <c r="G1100" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1100" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="J1100">
+        <v>5</v>
+      </c>
+      <c r="K1100" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1100" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="Y1100" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z1100" t="str">
+        <f>"A2-5"&amp;Y1100&amp;"-"&amp;AC1100</f>
+        <v>A2-5SO-A6</v>
+      </c>
+      <c r="AC1100" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="1101" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1101">
+        <v>6</v>
+      </c>
+      <c r="C1101" t="s">
+        <v>202</v>
+      </c>
+      <c r="G1101" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1101" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="J1101">
+        <v>5</v>
+      </c>
+      <c r="K1101" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1101" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="Y1101" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z1101" t="s">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="1102" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1102">
+        <v>7</v>
+      </c>
+      <c r="C1102" t="s">
+        <v>202</v>
+      </c>
+      <c r="G1102" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1102" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="J1102">
+        <v>5</v>
+      </c>
+      <c r="K1102" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1102" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="Y1102" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z1102" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="1103" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1103">
+        <v>8</v>
+      </c>
+      <c r="C1103" t="s">
+        <v>202</v>
+      </c>
+      <c r="G1103" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1103" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="J1103">
+        <v>5</v>
+      </c>
+      <c r="K1103" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1103" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="Y1103" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z1103" t="s">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="1104" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1104">
+        <v>9</v>
+      </c>
+      <c r="C1104" t="s">
+        <v>202</v>
+      </c>
+      <c r="G1104" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1104" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="J1104">
+        <v>5</v>
+      </c>
+      <c r="K1104" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1104" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="Y1104" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z1104" t="s">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="1105" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1105">
+        <v>7</v>
+      </c>
+      <c r="C1105" t="s">
+        <v>202</v>
+      </c>
+      <c r="G1105" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1105" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="J1105">
+        <v>5</v>
+      </c>
+      <c r="K1105" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1105" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="Y1105" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z1105" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="1106" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1106">
+        <v>7</v>
+      </c>
+      <c r="C1106" t="s">
+        <v>202</v>
+      </c>
+      <c r="G1106" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1106" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="J1106">
+        <v>5</v>
+      </c>
+      <c r="K1106" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1106" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="Y1106" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z1106" t="str">
+        <f>"A2-5"&amp;Y1106&amp;"-"&amp;AC1106</f>
+        <v>A2-5RT-A7</v>
+      </c>
+      <c r="AC1106" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="1107" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1107">
+        <v>8</v>
+      </c>
+      <c r="C1107" t="s">
+        <v>202</v>
+      </c>
+      <c r="G1107" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1107" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="J1107">
+        <v>5</v>
+      </c>
+      <c r="K1107" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1107" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="Y1107" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z1107" t="str">
+        <f t="shared" ref="Z1107:Z1118" si="11">"A2-5"&amp;Y1107&amp;"-"&amp;AC1107</f>
+        <v>A2-5RT-A8</v>
+      </c>
+      <c r="AC1107" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="1108" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1108">
+        <v>9</v>
+      </c>
+      <c r="C1108" t="s">
+        <v>202</v>
+      </c>
+      <c r="G1108" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1108" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="J1108">
+        <v>5</v>
+      </c>
+      <c r="K1108" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1108" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="Y1108" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z1108" t="str">
+        <f t="shared" si="11"/>
+        <v>A2-5RT-A9</v>
+      </c>
+      <c r="AC1108" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1109" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1109">
+        <v>10</v>
+      </c>
+      <c r="C1109" t="s">
+        <v>202</v>
+      </c>
+      <c r="G1109" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1109" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="J1109">
+        <v>5</v>
+      </c>
+      <c r="K1109" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1109" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="Y1109" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z1109" t="str">
+        <f t="shared" si="11"/>
+        <v>A2-5RT-A10</v>
+      </c>
+      <c r="AC1109" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="1110" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1110">
+        <v>11</v>
+      </c>
+      <c r="C1110" t="s">
+        <v>202</v>
+      </c>
+      <c r="G1110" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1110" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="J1110">
+        <v>5</v>
+      </c>
+      <c r="K1110" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1110" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="Y1110" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z1110" t="str">
+        <f t="shared" si="11"/>
+        <v>A2-5RT-A11</v>
+      </c>
+      <c r="AC1110" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="1111" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1111">
+        <v>12</v>
+      </c>
+      <c r="C1111" t="s">
+        <v>202</v>
+      </c>
+      <c r="G1111" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1111" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="J1111">
+        <v>5</v>
+      </c>
+      <c r="K1111" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1111" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="Y1111" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z1111" t="str">
+        <f t="shared" si="11"/>
+        <v>A2-5RT-A12</v>
+      </c>
+      <c r="AC1111" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="1112" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1112">
+        <v>8</v>
+      </c>
+      <c r="C1112" t="s">
+        <v>202</v>
+      </c>
+      <c r="G1112" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1112" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="J1112">
+        <v>5</v>
+      </c>
+      <c r="K1112" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1112" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="Y1112" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z1112" t="str">
+        <f t="shared" si="11"/>
+        <v>A2-5SO-A7</v>
+      </c>
+      <c r="AC1112" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="1113" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1113">
+        <v>9</v>
+      </c>
+      <c r="C1113" t="s">
+        <v>202</v>
+      </c>
+      <c r="G1113" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1113" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="J1113">
+        <v>5</v>
+      </c>
+      <c r="K1113" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1113" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="Y1113" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z1113" t="str">
+        <f t="shared" si="11"/>
+        <v>A2-5SO-A8</v>
+      </c>
+      <c r="AC1113" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="1114" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1114">
+        <v>10</v>
+      </c>
+      <c r="C1114" t="s">
+        <v>202</v>
+      </c>
+      <c r="G1114" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1114" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="J1114">
+        <v>5</v>
+      </c>
+      <c r="K1114" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1114" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="Y1114" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z1114" t="str">
+        <f t="shared" si="11"/>
+        <v>A2-5SO-A9</v>
+      </c>
+      <c r="AC1114" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1115" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1115">
+        <v>11</v>
+      </c>
+      <c r="C1115" t="s">
+        <v>202</v>
+      </c>
+      <c r="G1115" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1115" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="J1115">
+        <v>5</v>
+      </c>
+      <c r="K1115" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1115" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="Y1115" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z1115" t="str">
+        <f t="shared" si="11"/>
+        <v>A2-5SO-A10</v>
+      </c>
+      <c r="AC1115" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="1116" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1116">
+        <v>12</v>
+      </c>
+      <c r="C1116" t="s">
+        <v>202</v>
+      </c>
+      <c r="G1116" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1116" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="J1116">
+        <v>5</v>
+      </c>
+      <c r="K1116" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1116" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="Y1116" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z1116" t="str">
+        <f t="shared" si="11"/>
+        <v>A2-5SO-A11</v>
+      </c>
+      <c r="AC1116" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="1117" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1117">
+        <v>13</v>
+      </c>
+      <c r="C1117" t="s">
+        <v>202</v>
+      </c>
+      <c r="G1117" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1117" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="J1117">
+        <v>5</v>
+      </c>
+      <c r="K1117" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1117" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="Y1117" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z1117" t="str">
+        <f t="shared" si="11"/>
+        <v>A2-5SO-A12</v>
+      </c>
+      <c r="AC1117" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="1118" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1118">
+        <v>14</v>
+      </c>
+      <c r="C1118" t="s">
+        <v>202</v>
+      </c>
+      <c r="G1118" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1118" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="J1118">
+        <v>5</v>
+      </c>
+      <c r="K1118" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1118" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="Y1118" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z1118" t="str">
+        <f t="shared" si="11"/>
+        <v>A2-5SO-B1</v>
+      </c>
+      <c r="AC1118" t="s">
+        <v>170</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
entering weight data for adys 10 and 25 cohort 2018-09-09
</commit_message>
<xml_diff>
--- a/Data/2018-08-14_master_datac_2018_collection_year.xlsx
+++ b/Data/2018-08-14_master_datac_2018_collection_year.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andrew.nguyen\Desktop\Circadian_rhythm_runs_seasonal_timing\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4076C75A-040A-4120-BD91-3722920AB626}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31FDAF47-20A0-4530-BC32-8EA9AEB8D1BB}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="53055" yWindow="465" windowWidth="36360" windowHeight="21135" activeTab="1" xr2:uid="{C7477166-8A7C-B04A-9643-C277FEDCDAAB}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10244" uniqueCount="704">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10687" uniqueCount="709">
   <si>
     <t>Ind_ID</t>
   </si>
@@ -2144,6 +2144,21 @@
   </si>
   <si>
     <t>A2-5-6</t>
+  </si>
+  <si>
+    <t>Blank</t>
+  </si>
+  <si>
+    <t>14:45</t>
+  </si>
+  <si>
+    <t>14:37</t>
+  </si>
+  <si>
+    <t>14:36</t>
+  </si>
+  <si>
+    <t>14:25</t>
   </si>
 </sst>
 </file>
@@ -12036,11 +12051,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92725FB9-1A17-2546-9DFA-6C0D39437891}">
-  <dimension ref="A1:AS1118"/>
+  <dimension ref="A1:AS1206"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A981" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J996" sqref="J996"/>
+      <pane ySplit="1" topLeftCell="A1062" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M1206" sqref="M1206"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -51685,6 +51700,2291 @@
       </c>
       <c r="AC1118" t="s">
         <v>170</v>
+      </c>
+    </row>
+    <row r="1119" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1119">
+        <v>1</v>
+      </c>
+      <c r="B1119" t="s">
+        <v>90</v>
+      </c>
+      <c r="C1119" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1119">
+        <v>6.4470000000000001</v>
+      </c>
+      <c r="E1119" s="1" t="s">
+        <v>706</v>
+      </c>
+      <c r="G1119" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1119" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1119">
+        <v>10</v>
+      </c>
+      <c r="K1119" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="1120" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1120">
+        <v>2</v>
+      </c>
+      <c r="B1120" t="s">
+        <v>90</v>
+      </c>
+      <c r="C1120" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1120">
+        <v>4.375</v>
+      </c>
+      <c r="G1120" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1120" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1120">
+        <v>10</v>
+      </c>
+      <c r="K1120" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="1121" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1121">
+        <v>3</v>
+      </c>
+      <c r="B1121" t="s">
+        <v>90</v>
+      </c>
+      <c r="C1121" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1121">
+        <v>6.56</v>
+      </c>
+      <c r="G1121" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1121" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1121">
+        <v>10</v>
+      </c>
+      <c r="K1121" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="1122" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1122">
+        <v>4</v>
+      </c>
+      <c r="B1122" t="s">
+        <v>90</v>
+      </c>
+      <c r="C1122" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1122">
+        <v>3.3359999999999999</v>
+      </c>
+      <c r="G1122" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1122" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1122">
+        <v>10</v>
+      </c>
+      <c r="K1122" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="1123" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1123">
+        <v>5</v>
+      </c>
+      <c r="B1123" t="s">
+        <v>90</v>
+      </c>
+      <c r="C1123" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1123">
+        <v>7.077</v>
+      </c>
+      <c r="G1123" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1123" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1123">
+        <v>10</v>
+      </c>
+      <c r="K1123" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="1124" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1124">
+        <v>6</v>
+      </c>
+      <c r="B1124" t="s">
+        <v>90</v>
+      </c>
+      <c r="C1124" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1124">
+        <v>4.3949999999999996</v>
+      </c>
+      <c r="G1124" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1124" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1124">
+        <v>10</v>
+      </c>
+      <c r="K1124" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="1125" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1125">
+        <v>7</v>
+      </c>
+      <c r="B1125" t="s">
+        <v>90</v>
+      </c>
+      <c r="C1125" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1125">
+        <v>4.1820000000000004</v>
+      </c>
+      <c r="G1125" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1125" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1125">
+        <v>10</v>
+      </c>
+      <c r="K1125" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="1126" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1126">
+        <v>8</v>
+      </c>
+      <c r="B1126" t="s">
+        <v>90</v>
+      </c>
+      <c r="C1126" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1126">
+        <v>5.44</v>
+      </c>
+      <c r="G1126" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1126" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1126">
+        <v>10</v>
+      </c>
+      <c r="K1126" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="1127" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1127">
+        <v>9</v>
+      </c>
+      <c r="B1127" t="s">
+        <v>90</v>
+      </c>
+      <c r="C1127" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1127">
+        <v>4.1440000000000001</v>
+      </c>
+      <c r="G1127" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1127" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1127">
+        <v>10</v>
+      </c>
+      <c r="K1127" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="1128" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1128">
+        <v>10</v>
+      </c>
+      <c r="B1128" t="s">
+        <v>90</v>
+      </c>
+      <c r="C1128" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1128">
+        <v>6.1029999999999998</v>
+      </c>
+      <c r="G1128" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1128" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1128">
+        <v>10</v>
+      </c>
+      <c r="K1128" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="1129" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1129">
+        <v>11</v>
+      </c>
+      <c r="B1129" t="s">
+        <v>90</v>
+      </c>
+      <c r="C1129" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1129">
+        <v>6.8970000000000002</v>
+      </c>
+      <c r="G1129" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1129" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1129">
+        <v>10</v>
+      </c>
+      <c r="K1129" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="1130" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1130">
+        <v>12</v>
+      </c>
+      <c r="B1130" t="s">
+        <v>90</v>
+      </c>
+      <c r="C1130" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1130">
+        <v>3.6070000000000002</v>
+      </c>
+      <c r="G1130" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1130" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1130">
+        <v>10</v>
+      </c>
+      <c r="K1130" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="1131" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1131">
+        <v>13</v>
+      </c>
+      <c r="B1131" t="s">
+        <v>90</v>
+      </c>
+      <c r="C1131" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1131">
+        <v>7.3780000000000001</v>
+      </c>
+      <c r="G1131" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1131" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1131">
+        <v>10</v>
+      </c>
+      <c r="K1131" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="1132" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1132">
+        <v>14</v>
+      </c>
+      <c r="B1132" t="s">
+        <v>90</v>
+      </c>
+      <c r="C1132" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1132">
+        <v>8.093</v>
+      </c>
+      <c r="G1132" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1132" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1132">
+        <v>10</v>
+      </c>
+      <c r="K1132" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="1133" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1133">
+        <v>15</v>
+      </c>
+      <c r="B1133" t="s">
+        <v>90</v>
+      </c>
+      <c r="C1133" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1133">
+        <v>5.7960000000000003</v>
+      </c>
+      <c r="G1133" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1133" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1133">
+        <v>10</v>
+      </c>
+      <c r="K1133" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="1134" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1134">
+        <v>16</v>
+      </c>
+      <c r="B1134" t="s">
+        <v>90</v>
+      </c>
+      <c r="C1134" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1134">
+        <v>3.4780000000000002</v>
+      </c>
+      <c r="G1134" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1134" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1134">
+        <v>10</v>
+      </c>
+      <c r="K1134" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="1135" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1135">
+        <v>17</v>
+      </c>
+      <c r="B1135" t="s">
+        <v>90</v>
+      </c>
+      <c r="C1135" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1135">
+        <v>5.1360000000000001</v>
+      </c>
+      <c r="G1135" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1135" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1135">
+        <v>10</v>
+      </c>
+      <c r="K1135" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="1136" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1136">
+        <v>18</v>
+      </c>
+      <c r="B1136" t="s">
+        <v>90</v>
+      </c>
+      <c r="C1136" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1136">
+        <v>4.4279999999999999</v>
+      </c>
+      <c r="G1136" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1136" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1136">
+        <v>10</v>
+      </c>
+      <c r="K1136" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="1137" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1137">
+        <v>19</v>
+      </c>
+      <c r="B1137" t="s">
+        <v>90</v>
+      </c>
+      <c r="C1137" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1137">
+        <v>4.2709999999999999</v>
+      </c>
+      <c r="G1137" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1137" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1137">
+        <v>10</v>
+      </c>
+      <c r="K1137" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="1138" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1138">
+        <v>20</v>
+      </c>
+      <c r="B1138" t="s">
+        <v>90</v>
+      </c>
+      <c r="C1138" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1138">
+        <v>2.8250000000000002</v>
+      </c>
+      <c r="G1138" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1138" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1138">
+        <v>10</v>
+      </c>
+      <c r="K1138" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="1139" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1139">
+        <v>21</v>
+      </c>
+      <c r="B1139" t="s">
+        <v>90</v>
+      </c>
+      <c r="C1139" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1139">
+        <v>6.3109999999999999</v>
+      </c>
+      <c r="G1139" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1139" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1139">
+        <v>10</v>
+      </c>
+      <c r="K1139" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="1140" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1140">
+        <v>22</v>
+      </c>
+      <c r="B1140" t="s">
+        <v>90</v>
+      </c>
+      <c r="C1140" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1140">
+        <v>4.5469999999999997</v>
+      </c>
+      <c r="G1140" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1140" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1140">
+        <v>10</v>
+      </c>
+      <c r="K1140" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="1141" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1141">
+        <v>23</v>
+      </c>
+      <c r="B1141" t="s">
+        <v>90</v>
+      </c>
+      <c r="C1141" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1141">
+        <v>4.3170000000000002</v>
+      </c>
+      <c r="G1141" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1141" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1141">
+        <v>10</v>
+      </c>
+      <c r="K1141" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="1142" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1142">
+        <v>24</v>
+      </c>
+      <c r="B1142" t="s">
+        <v>90</v>
+      </c>
+      <c r="C1142" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1142">
+        <v>6.5590000000000002</v>
+      </c>
+      <c r="G1142" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1142" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1142">
+        <v>10</v>
+      </c>
+      <c r="K1142" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="1143" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1143">
+        <v>25</v>
+      </c>
+      <c r="B1143" t="s">
+        <v>90</v>
+      </c>
+      <c r="C1143" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1143">
+        <v>4.633</v>
+      </c>
+      <c r="G1143" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1143" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1143">
+        <v>10</v>
+      </c>
+      <c r="K1143" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="1144" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1144">
+        <v>26</v>
+      </c>
+      <c r="B1144" t="s">
+        <v>90</v>
+      </c>
+      <c r="C1144" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1144">
+        <v>4.915</v>
+      </c>
+      <c r="G1144" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1144" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1144">
+        <v>10</v>
+      </c>
+      <c r="K1144" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="1145" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1145">
+        <v>27</v>
+      </c>
+      <c r="B1145" t="s">
+        <v>90</v>
+      </c>
+      <c r="C1145" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1145">
+        <v>6.5410000000000004</v>
+      </c>
+      <c r="G1145" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1145" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1145">
+        <v>10</v>
+      </c>
+      <c r="K1145" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="1146" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1146">
+        <v>28</v>
+      </c>
+      <c r="B1146" t="s">
+        <v>90</v>
+      </c>
+      <c r="C1146" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1146">
+        <v>2.3140000000000001</v>
+      </c>
+      <c r="G1146" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1146" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1146">
+        <v>10</v>
+      </c>
+      <c r="K1146" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="1147" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1147">
+        <v>29</v>
+      </c>
+      <c r="B1147" t="s">
+        <v>90</v>
+      </c>
+      <c r="C1147" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1147">
+        <v>3.2989999999999999</v>
+      </c>
+      <c r="G1147" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1147" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1147">
+        <v>10</v>
+      </c>
+      <c r="K1147" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="1148" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1148">
+        <v>30</v>
+      </c>
+      <c r="B1148" t="s">
+        <v>90</v>
+      </c>
+      <c r="C1148" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1148">
+        <v>4.5869999999999997</v>
+      </c>
+      <c r="G1148" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1148" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1148">
+        <v>10</v>
+      </c>
+      <c r="K1148" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="1149" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1149">
+        <v>31</v>
+      </c>
+      <c r="B1149" t="s">
+        <v>90</v>
+      </c>
+      <c r="C1149" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1149">
+        <v>3.984</v>
+      </c>
+      <c r="G1149" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1149" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1149">
+        <v>10</v>
+      </c>
+      <c r="K1149" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="1150" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1150">
+        <v>32</v>
+      </c>
+      <c r="B1150" t="s">
+        <v>90</v>
+      </c>
+      <c r="C1150" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1150">
+        <v>5.3410000000000002</v>
+      </c>
+      <c r="G1150" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1150" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1150">
+        <v>10</v>
+      </c>
+      <c r="K1150" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="1151" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1151">
+        <v>33</v>
+      </c>
+      <c r="C1151" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1151">
+        <v>2.52</v>
+      </c>
+      <c r="G1151" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1151" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1151">
+        <v>10</v>
+      </c>
+      <c r="K1151" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="1152" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1152">
+        <v>34</v>
+      </c>
+      <c r="B1152" t="s">
+        <v>90</v>
+      </c>
+      <c r="C1152" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1152">
+        <v>5.5590000000000002</v>
+      </c>
+      <c r="G1152" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1152" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1152">
+        <v>10</v>
+      </c>
+      <c r="K1152" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="1153" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1153">
+        <v>35</v>
+      </c>
+      <c r="B1153" t="s">
+        <v>90</v>
+      </c>
+      <c r="C1153" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1153">
+        <v>4.34</v>
+      </c>
+      <c r="G1153" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1153" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1153">
+        <v>10</v>
+      </c>
+      <c r="K1153" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="1154" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1154">
+        <v>36</v>
+      </c>
+      <c r="B1154" t="s">
+        <v>90</v>
+      </c>
+      <c r="C1154" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1154">
+        <v>4.3680000000000003</v>
+      </c>
+      <c r="G1154" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1154" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1154">
+        <v>10</v>
+      </c>
+      <c r="K1154" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="1155" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1155">
+        <v>37</v>
+      </c>
+      <c r="B1155" t="s">
+        <v>90</v>
+      </c>
+      <c r="C1155" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1155">
+        <v>4.5209999999999999</v>
+      </c>
+      <c r="G1155" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1155" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1155">
+        <v>10</v>
+      </c>
+      <c r="K1155" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="1156" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1156">
+        <v>38</v>
+      </c>
+      <c r="B1156" t="s">
+        <v>90</v>
+      </c>
+      <c r="C1156" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1156">
+        <v>2.6160000000000001</v>
+      </c>
+      <c r="G1156" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1156" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1156">
+        <v>10</v>
+      </c>
+      <c r="K1156" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="1157" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1157">
+        <v>39</v>
+      </c>
+      <c r="B1157" t="s">
+        <v>90</v>
+      </c>
+      <c r="C1157" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1157">
+        <v>5.0830000000000002</v>
+      </c>
+      <c r="G1157" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1157" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1157">
+        <v>10</v>
+      </c>
+      <c r="K1157" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="1158" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1158">
+        <v>46</v>
+      </c>
+      <c r="B1158" t="s">
+        <v>90</v>
+      </c>
+      <c r="C1158" t="s">
+        <v>704</v>
+      </c>
+      <c r="G1158" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1158" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1158">
+        <v>10</v>
+      </c>
+      <c r="K1158" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="1159" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1159">
+        <v>47</v>
+      </c>
+      <c r="B1159" t="s">
+        <v>90</v>
+      </c>
+      <c r="C1159" t="s">
+        <v>704</v>
+      </c>
+      <c r="E1159" s="1" t="s">
+        <v>705</v>
+      </c>
+      <c r="G1159" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1159" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1159">
+        <v>10</v>
+      </c>
+      <c r="K1159" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="1160" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1160">
+        <v>1</v>
+      </c>
+      <c r="B1160" t="s">
+        <v>387</v>
+      </c>
+      <c r="C1160" t="s">
+        <v>202</v>
+      </c>
+      <c r="D1160">
+        <v>6.1239999999999997</v>
+      </c>
+      <c r="E1160" s="1" t="s">
+        <v>708</v>
+      </c>
+      <c r="G1160" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1160" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1160">
+        <v>10</v>
+      </c>
+      <c r="K1160" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="1161" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1161">
+        <v>2</v>
+      </c>
+      <c r="B1161" t="s">
+        <v>387</v>
+      </c>
+      <c r="C1161" t="s">
+        <v>202</v>
+      </c>
+      <c r="D1161">
+        <v>8.3450000000000006</v>
+      </c>
+      <c r="G1161" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1161" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1161">
+        <v>10</v>
+      </c>
+      <c r="K1161" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="1162" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1162">
+        <v>3</v>
+      </c>
+      <c r="B1162" t="s">
+        <v>387</v>
+      </c>
+      <c r="C1162" t="s">
+        <v>202</v>
+      </c>
+      <c r="D1162">
+        <v>6.5529999999999999</v>
+      </c>
+      <c r="G1162" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1162" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1162">
+        <v>10</v>
+      </c>
+      <c r="K1162" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="1163" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1163">
+        <v>4</v>
+      </c>
+      <c r="B1163" t="s">
+        <v>387</v>
+      </c>
+      <c r="C1163" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1163">
+        <v>3.8679999999999999</v>
+      </c>
+      <c r="G1163" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I1163" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1163">
+        <v>25</v>
+      </c>
+      <c r="K1163" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="1164" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1164">
+        <v>5</v>
+      </c>
+      <c r="B1164" t="s">
+        <v>387</v>
+      </c>
+      <c r="C1164" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1164">
+        <v>4.2279999999999998</v>
+      </c>
+      <c r="G1164" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1164" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1164">
+        <v>10</v>
+      </c>
+      <c r="K1164" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="1165" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1165">
+        <v>6</v>
+      </c>
+      <c r="B1165" t="s">
+        <v>387</v>
+      </c>
+      <c r="C1165" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1165">
+        <v>7.64</v>
+      </c>
+      <c r="G1165" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1165" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1165">
+        <v>10</v>
+      </c>
+      <c r="K1165" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="1166" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1166">
+        <v>7</v>
+      </c>
+      <c r="B1166" t="s">
+        <v>387</v>
+      </c>
+      <c r="C1166" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1166">
+        <v>8.8940000000000001</v>
+      </c>
+      <c r="G1166" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1166" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1166">
+        <v>10</v>
+      </c>
+      <c r="K1166" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="1167" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1167">
+        <v>8</v>
+      </c>
+      <c r="B1167" t="s">
+        <v>387</v>
+      </c>
+      <c r="C1167" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1167">
+        <v>7.1079999999999997</v>
+      </c>
+      <c r="G1167" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1167" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1167">
+        <v>10</v>
+      </c>
+      <c r="K1167" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="1168" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1168">
+        <v>9</v>
+      </c>
+      <c r="B1168" t="s">
+        <v>387</v>
+      </c>
+      <c r="C1168" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1168">
+        <v>7.2130000000000001</v>
+      </c>
+      <c r="G1168" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1168" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1168">
+        <v>10</v>
+      </c>
+      <c r="K1168" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="1169" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1169">
+        <v>10</v>
+      </c>
+      <c r="B1169" t="s">
+        <v>387</v>
+      </c>
+      <c r="C1169" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1169">
+        <v>8.82</v>
+      </c>
+      <c r="G1169" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1169" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1169">
+        <v>10</v>
+      </c>
+      <c r="K1169" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="1170" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1170">
+        <v>11</v>
+      </c>
+      <c r="B1170" t="s">
+        <v>387</v>
+      </c>
+      <c r="C1170" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1170">
+        <v>6.8890000000000002</v>
+      </c>
+      <c r="G1170" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1170" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1170">
+        <v>10</v>
+      </c>
+      <c r="K1170" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="1171" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1171">
+        <v>12</v>
+      </c>
+      <c r="B1171" t="s">
+        <v>387</v>
+      </c>
+      <c r="C1171" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1171">
+        <v>10.754</v>
+      </c>
+      <c r="G1171" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1171" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1171">
+        <v>10</v>
+      </c>
+      <c r="K1171" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="1172" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1172">
+        <v>13</v>
+      </c>
+      <c r="B1172" t="s">
+        <v>387</v>
+      </c>
+      <c r="C1172" t="s">
+        <v>202</v>
+      </c>
+      <c r="D1172">
+        <v>9.2189999999999994</v>
+      </c>
+      <c r="G1172" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1172" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1172">
+        <v>10</v>
+      </c>
+      <c r="K1172" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="1173" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1173">
+        <v>14</v>
+      </c>
+      <c r="B1173" t="s">
+        <v>387</v>
+      </c>
+      <c r="C1173" t="s">
+        <v>202</v>
+      </c>
+      <c r="D1173">
+        <v>9.3559999999999999</v>
+      </c>
+      <c r="G1173" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1173" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1173">
+        <v>10</v>
+      </c>
+      <c r="K1173" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="1174" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1174">
+        <v>15</v>
+      </c>
+      <c r="B1174" t="s">
+        <v>387</v>
+      </c>
+      <c r="C1174" t="s">
+        <v>202</v>
+      </c>
+      <c r="D1174">
+        <v>6.0519999999999996</v>
+      </c>
+      <c r="G1174" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1174" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1174">
+        <v>10</v>
+      </c>
+      <c r="K1174" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="1175" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1175">
+        <v>16</v>
+      </c>
+      <c r="B1175" t="s">
+        <v>387</v>
+      </c>
+      <c r="C1175" t="s">
+        <v>202</v>
+      </c>
+      <c r="D1175">
+        <v>8.5690000000000008</v>
+      </c>
+      <c r="G1175" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1175" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1175">
+        <v>10</v>
+      </c>
+      <c r="K1175" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="1176" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1176">
+        <v>17</v>
+      </c>
+      <c r="B1176" t="s">
+        <v>387</v>
+      </c>
+      <c r="C1176" t="s">
+        <v>202</v>
+      </c>
+      <c r="D1176">
+        <v>8.5559999999999992</v>
+      </c>
+      <c r="G1176" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1176" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1176">
+        <v>10</v>
+      </c>
+      <c r="K1176" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="1177" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1177">
+        <v>18</v>
+      </c>
+      <c r="B1177" t="s">
+        <v>387</v>
+      </c>
+      <c r="C1177" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1177">
+        <v>5.0149999999999997</v>
+      </c>
+      <c r="G1177" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I1177" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1177">
+        <v>25</v>
+      </c>
+      <c r="K1177" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="1178" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1178">
+        <v>19</v>
+      </c>
+      <c r="B1178" t="s">
+        <v>387</v>
+      </c>
+      <c r="C1178" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1178">
+        <v>4.9059999999999997</v>
+      </c>
+      <c r="G1178" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1178" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1178">
+        <v>10</v>
+      </c>
+      <c r="K1178" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="1179" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1179">
+        <v>20</v>
+      </c>
+      <c r="B1179" t="s">
+        <v>387</v>
+      </c>
+      <c r="C1179" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1179">
+        <v>7.444</v>
+      </c>
+      <c r="G1179" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1179" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1179">
+        <v>10</v>
+      </c>
+      <c r="K1179" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="1180" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1180">
+        <v>21</v>
+      </c>
+      <c r="B1180" t="s">
+        <v>387</v>
+      </c>
+      <c r="C1180" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1180">
+        <v>5.8129999999999997</v>
+      </c>
+      <c r="G1180" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1180" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1180">
+        <v>10</v>
+      </c>
+      <c r="K1180" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="1181" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1181">
+        <v>22</v>
+      </c>
+      <c r="B1181" t="s">
+        <v>387</v>
+      </c>
+      <c r="C1181" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1181">
+        <v>2.7360000000000002</v>
+      </c>
+      <c r="G1181" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1181" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1181">
+        <v>10</v>
+      </c>
+      <c r="K1181" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="1182" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1182">
+        <v>23</v>
+      </c>
+      <c r="B1182" t="s">
+        <v>387</v>
+      </c>
+      <c r="C1182" t="s">
+        <v>202</v>
+      </c>
+      <c r="D1182">
+        <v>5.6470000000000002</v>
+      </c>
+      <c r="G1182" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1182" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1182">
+        <v>10</v>
+      </c>
+      <c r="K1182" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="1183" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1183">
+        <v>24</v>
+      </c>
+      <c r="B1183" t="s">
+        <v>387</v>
+      </c>
+      <c r="C1183" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1183">
+        <v>6.9020000000000001</v>
+      </c>
+      <c r="G1183" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1183" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1183">
+        <v>10</v>
+      </c>
+      <c r="K1183" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="1184" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1184">
+        <v>25</v>
+      </c>
+      <c r="B1184" t="s">
+        <v>387</v>
+      </c>
+      <c r="C1184" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1184">
+        <v>4.9969999999999999</v>
+      </c>
+      <c r="G1184" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1184" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1184">
+        <v>10</v>
+      </c>
+      <c r="K1184" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="1185" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1185">
+        <v>26</v>
+      </c>
+      <c r="B1185" t="s">
+        <v>387</v>
+      </c>
+      <c r="C1185" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1185">
+        <v>3.8620000000000001</v>
+      </c>
+      <c r="G1185" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1185" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1185">
+        <v>10</v>
+      </c>
+      <c r="K1185" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="1186" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1186">
+        <v>27</v>
+      </c>
+      <c r="B1186" t="s">
+        <v>387</v>
+      </c>
+      <c r="C1186" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1186">
+        <v>7.4770000000000003</v>
+      </c>
+      <c r="G1186" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1186" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1186">
+        <v>10</v>
+      </c>
+      <c r="K1186" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="1187" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1187">
+        <v>28</v>
+      </c>
+      <c r="B1187" t="s">
+        <v>387</v>
+      </c>
+      <c r="C1187" t="s">
+        <v>202</v>
+      </c>
+      <c r="D1187">
+        <v>7.1159999999999997</v>
+      </c>
+      <c r="G1187" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1187" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1187">
+        <v>10</v>
+      </c>
+      <c r="K1187" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="1188" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1188">
+        <v>29</v>
+      </c>
+      <c r="B1188" t="s">
+        <v>387</v>
+      </c>
+      <c r="C1188" t="s">
+        <v>202</v>
+      </c>
+      <c r="D1188">
+        <v>7.492</v>
+      </c>
+      <c r="G1188" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1188" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1188">
+        <v>10</v>
+      </c>
+      <c r="K1188" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="1189" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1189">
+        <v>30</v>
+      </c>
+      <c r="B1189" t="s">
+        <v>387</v>
+      </c>
+      <c r="C1189" t="s">
+        <v>202</v>
+      </c>
+      <c r="D1189">
+        <v>6.4539999999999997</v>
+      </c>
+      <c r="G1189" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1189" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1189">
+        <v>10</v>
+      </c>
+      <c r="K1189" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="1190" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1190">
+        <v>31</v>
+      </c>
+      <c r="B1190" t="s">
+        <v>387</v>
+      </c>
+      <c r="C1190" t="s">
+        <v>202</v>
+      </c>
+      <c r="D1190">
+        <v>7</v>
+      </c>
+      <c r="G1190" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1190" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1190">
+        <v>10</v>
+      </c>
+      <c r="K1190" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="1191" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1191">
+        <v>32</v>
+      </c>
+      <c r="B1191" t="s">
+        <v>387</v>
+      </c>
+      <c r="C1191" t="s">
+        <v>202</v>
+      </c>
+      <c r="D1191">
+        <v>6.8929999999999998</v>
+      </c>
+      <c r="G1191" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1191" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1191">
+        <v>10</v>
+      </c>
+      <c r="K1191" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="1192" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1192">
+        <v>33</v>
+      </c>
+      <c r="B1192" t="s">
+        <v>387</v>
+      </c>
+      <c r="C1192" t="s">
+        <v>202</v>
+      </c>
+      <c r="D1192">
+        <v>6.8259999999999996</v>
+      </c>
+      <c r="G1192" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1192" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1192">
+        <v>10</v>
+      </c>
+      <c r="K1192" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="1193" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1193">
+        <v>34</v>
+      </c>
+      <c r="B1193" t="s">
+        <v>387</v>
+      </c>
+      <c r="C1193" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1193">
+        <v>4.7149999999999999</v>
+      </c>
+      <c r="G1193" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1193" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1193">
+        <v>10</v>
+      </c>
+      <c r="K1193" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="1194" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1194">
+        <v>35</v>
+      </c>
+      <c r="B1194" t="s">
+        <v>387</v>
+      </c>
+      <c r="C1194" t="s">
+        <v>202</v>
+      </c>
+      <c r="D1194">
+        <v>5.8330000000000002</v>
+      </c>
+      <c r="G1194" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1194" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1194">
+        <v>10</v>
+      </c>
+      <c r="K1194" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="1195" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1195">
+        <v>36</v>
+      </c>
+      <c r="B1195" t="s">
+        <v>387</v>
+      </c>
+      <c r="C1195" t="s">
+        <v>202</v>
+      </c>
+      <c r="D1195">
+        <v>6.71</v>
+      </c>
+      <c r="G1195" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1195" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1195">
+        <v>10</v>
+      </c>
+      <c r="K1195" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="1196" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1196">
+        <v>37</v>
+      </c>
+      <c r="B1196" t="s">
+        <v>387</v>
+      </c>
+      <c r="C1196" t="s">
+        <v>202</v>
+      </c>
+      <c r="D1196">
+        <v>2.6339999999999999</v>
+      </c>
+      <c r="G1196" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1196" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1196">
+        <v>10</v>
+      </c>
+      <c r="K1196" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="1197" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1197">
+        <v>38</v>
+      </c>
+      <c r="B1197" t="s">
+        <v>387</v>
+      </c>
+      <c r="C1197" t="s">
+        <v>202</v>
+      </c>
+      <c r="D1197">
+        <v>8.7520000000000007</v>
+      </c>
+      <c r="G1197" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1197" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1197">
+        <v>10</v>
+      </c>
+      <c r="K1197" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="1198" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1198">
+        <v>39</v>
+      </c>
+      <c r="B1198" t="s">
+        <v>387</v>
+      </c>
+      <c r="C1198" t="s">
+        <v>202</v>
+      </c>
+      <c r="D1198">
+        <v>8.0559999999999992</v>
+      </c>
+      <c r="G1198" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1198" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1198">
+        <v>10</v>
+      </c>
+      <c r="K1198" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="1199" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1199">
+        <v>40</v>
+      </c>
+      <c r="B1199" t="s">
+        <v>387</v>
+      </c>
+      <c r="C1199" t="s">
+        <v>202</v>
+      </c>
+      <c r="D1199">
+        <v>6.5819999999999999</v>
+      </c>
+      <c r="G1199" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1199" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1199">
+        <v>10</v>
+      </c>
+      <c r="K1199" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="1200" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1200">
+        <v>41</v>
+      </c>
+      <c r="B1200" t="s">
+        <v>387</v>
+      </c>
+      <c r="C1200" t="s">
+        <v>202</v>
+      </c>
+      <c r="D1200">
+        <v>6.742</v>
+      </c>
+      <c r="G1200" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1200" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1200">
+        <v>10</v>
+      </c>
+      <c r="K1200" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="1201" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1201">
+        <v>42</v>
+      </c>
+      <c r="B1201" t="s">
+        <v>387</v>
+      </c>
+      <c r="C1201" t="s">
+        <v>202</v>
+      </c>
+      <c r="D1201">
+        <v>4.5199999999999996</v>
+      </c>
+      <c r="G1201" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1201" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1201">
+        <v>10</v>
+      </c>
+      <c r="K1201" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="1202" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1202">
+        <v>43</v>
+      </c>
+      <c r="B1202" t="s">
+        <v>387</v>
+      </c>
+      <c r="C1202" t="s">
+        <v>202</v>
+      </c>
+      <c r="D1202">
+        <v>3.6259999999999999</v>
+      </c>
+      <c r="G1202" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1202" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1202">
+        <v>10</v>
+      </c>
+      <c r="K1202" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="1203" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1203">
+        <v>44</v>
+      </c>
+      <c r="B1203" t="s">
+        <v>387</v>
+      </c>
+      <c r="C1203" t="s">
+        <v>202</v>
+      </c>
+      <c r="D1203">
+        <v>6.6740000000000004</v>
+      </c>
+      <c r="G1203" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1203" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1203">
+        <v>10</v>
+      </c>
+      <c r="K1203" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="1204" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1204">
+        <v>45</v>
+      </c>
+      <c r="B1204" t="s">
+        <v>387</v>
+      </c>
+      <c r="C1204" t="s">
+        <v>202</v>
+      </c>
+      <c r="D1204">
+        <v>7.2270000000000003</v>
+      </c>
+      <c r="G1204" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1204" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1204">
+        <v>10</v>
+      </c>
+      <c r="K1204" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="1205" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1205">
+        <v>46</v>
+      </c>
+      <c r="B1205" t="s">
+        <v>387</v>
+      </c>
+      <c r="C1205" t="s">
+        <v>704</v>
+      </c>
+      <c r="G1205" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1205" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1205">
+        <v>10</v>
+      </c>
+      <c r="K1205" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="1206" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1206">
+        <v>47</v>
+      </c>
+      <c r="B1206" t="s">
+        <v>387</v>
+      </c>
+      <c r="C1206" t="s">
+        <v>704</v>
+      </c>
+      <c r="E1206" s="1" t="s">
+        <v>707</v>
+      </c>
+      <c r="G1206" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1206" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1206">
+        <v>10</v>
+      </c>
+      <c r="K1206" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding dates to master data sheet 2018
</commit_message>
<xml_diff>
--- a/Data/2018-08-14_master_datac_2018_collection_year.xlsx
+++ b/Data/2018-08-14_master_datac_2018_collection_year.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hinalkharva\Desktop\Circadian_rhythm_runs_seasonal_timing\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A8C41CF-86DB-43B9-866D-CB674BDAE40B}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B948F67A-7AFF-467F-A85B-3F964EEBB21A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="53055" yWindow="465" windowWidth="36360" windowHeight="21135" xr2:uid="{C7477166-8A7C-B04A-9643-C277FEDCDAAB}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10911" uniqueCount="715">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10941" uniqueCount="715">
   <si>
     <t>Ind_ID</t>
   </si>
@@ -2767,8 +2767,8 @@
   <dimension ref="A1:AC306"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A122" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N143" sqref="N143"/>
+      <pane ySplit="1" topLeftCell="A124" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N133" sqref="N133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -10141,8 +10141,12 @@
       <c r="J129" s="1"/>
       <c r="K129" s="1"/>
       <c r="L129" s="1"/>
-      <c r="M129" s="1"/>
-      <c r="N129" s="1"/>
+      <c r="M129" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="N129" s="1" t="s">
+        <v>221</v>
+      </c>
       <c r="O129" s="1"/>
       <c r="P129" s="1"/>
       <c r="Q129" s="1"/>
@@ -10179,8 +10183,12 @@
       <c r="J130" s="1"/>
       <c r="K130" s="1"/>
       <c r="L130" s="1"/>
-      <c r="M130" s="1"/>
-      <c r="N130" s="1"/>
+      <c r="M130" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="N130" s="1" t="s">
+        <v>221</v>
+      </c>
       <c r="O130" s="1"/>
       <c r="P130" s="1"/>
       <c r="Q130" s="1"/>
@@ -10217,8 +10225,12 @@
       <c r="J131" s="1"/>
       <c r="K131" s="1"/>
       <c r="L131" s="1"/>
-      <c r="M131" s="1"/>
-      <c r="N131" s="1"/>
+      <c r="M131" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="N131" s="1" t="s">
+        <v>221</v>
+      </c>
       <c r="O131" s="1"/>
       <c r="P131" s="1"/>
       <c r="Q131" s="1"/>
@@ -10255,8 +10267,12 @@
       <c r="J132" s="1"/>
       <c r="K132" s="1"/>
       <c r="L132" s="1"/>
-      <c r="M132" s="1"/>
-      <c r="N132" s="1"/>
+      <c r="M132" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="N132" s="1" t="s">
+        <v>221</v>
+      </c>
       <c r="O132" s="1"/>
       <c r="P132" s="1"/>
       <c r="Q132" s="1"/>
@@ -10293,8 +10309,12 @@
       <c r="J133" s="1"/>
       <c r="K133" s="1"/>
       <c r="L133" s="1"/>
-      <c r="M133" s="1"/>
-      <c r="N133" s="1"/>
+      <c r="M133" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="N133" s="1" t="s">
+        <v>221</v>
+      </c>
       <c r="O133" s="1"/>
       <c r="P133" s="1"/>
       <c r="Q133" s="1"/>
@@ -10331,7 +10351,9 @@
       <c r="J134" s="1"/>
       <c r="K134" s="1"/>
       <c r="L134" s="1"/>
-      <c r="M134" s="1"/>
+      <c r="M134" s="1" t="s">
+        <v>221</v>
+      </c>
       <c r="N134" s="1"/>
       <c r="O134" s="1"/>
       <c r="P134" s="1"/>
@@ -10369,7 +10391,9 @@
       <c r="J135" s="1"/>
       <c r="K135" s="1"/>
       <c r="L135" s="1"/>
-      <c r="M135" s="1"/>
+      <c r="M135" s="1" t="s">
+        <v>221</v>
+      </c>
       <c r="N135" s="1"/>
       <c r="O135" s="1"/>
       <c r="P135" s="1"/>
@@ -10407,7 +10431,9 @@
       <c r="J136" s="1"/>
       <c r="K136" s="1"/>
       <c r="L136" s="1"/>
-      <c r="M136" s="1"/>
+      <c r="M136" s="1" t="s">
+        <v>221</v>
+      </c>
       <c r="N136" s="1"/>
       <c r="O136" s="1"/>
       <c r="P136" s="1"/>
@@ -10445,7 +10471,9 @@
       <c r="J137" s="1"/>
       <c r="K137" s="1"/>
       <c r="L137" s="1"/>
-      <c r="M137" s="1"/>
+      <c r="M137" s="1" t="s">
+        <v>221</v>
+      </c>
       <c r="N137" s="1"/>
       <c r="O137" s="1"/>
       <c r="P137" s="1"/>
@@ -10483,7 +10511,9 @@
       <c r="J138" s="1"/>
       <c r="K138" s="1"/>
       <c r="L138" s="1"/>
-      <c r="M138" s="1"/>
+      <c r="M138" s="1" t="s">
+        <v>542</v>
+      </c>
       <c r="N138" s="1"/>
       <c r="O138" s="1"/>
       <c r="P138" s="1"/>
@@ -10521,7 +10551,9 @@
       <c r="J139" s="1"/>
       <c r="K139" s="1"/>
       <c r="L139" s="1"/>
-      <c r="M139" s="1"/>
+      <c r="M139" s="1" t="s">
+        <v>542</v>
+      </c>
       <c r="N139" s="1"/>
       <c r="O139" s="1"/>
       <c r="P139" s="1"/>
@@ -10559,7 +10591,9 @@
       <c r="J140" s="1"/>
       <c r="K140" s="1"/>
       <c r="L140" s="1"/>
-      <c r="M140" s="1"/>
+      <c r="M140" s="1" t="s">
+        <v>542</v>
+      </c>
       <c r="N140" s="1"/>
       <c r="O140" s="1"/>
       <c r="P140" s="1"/>
@@ -10597,7 +10631,9 @@
       <c r="J141" s="1"/>
       <c r="K141" s="1"/>
       <c r="L141" s="1"/>
-      <c r="M141" s="1"/>
+      <c r="M141" s="1" t="s">
+        <v>542</v>
+      </c>
       <c r="N141" s="1"/>
       <c r="O141" s="1"/>
       <c r="P141" s="1"/>
@@ -10635,7 +10671,9 @@
       <c r="J142" s="1"/>
       <c r="K142" s="1"/>
       <c r="L142" s="1"/>
-      <c r="M142" s="1"/>
+      <c r="M142" s="1" t="s">
+        <v>543</v>
+      </c>
       <c r="N142" s="1"/>
       <c r="O142" s="1"/>
       <c r="P142" s="1"/>
@@ -10673,7 +10711,9 @@
       <c r="J143" s="1"/>
       <c r="K143" s="1"/>
       <c r="L143" s="1"/>
-      <c r="M143" s="1"/>
+      <c r="M143" s="1" t="s">
+        <v>543</v>
+      </c>
       <c r="N143" s="1"/>
       <c r="O143" s="1"/>
       <c r="P143" s="1"/>
@@ -10711,7 +10751,9 @@
       <c r="J144" s="1"/>
       <c r="K144" s="1"/>
       <c r="L144" s="1"/>
-      <c r="M144" s="1"/>
+      <c r="M144" s="1" t="s">
+        <v>543</v>
+      </c>
       <c r="N144" s="1"/>
       <c r="O144" s="1"/>
       <c r="P144" s="1"/>
@@ -10749,7 +10791,9 @@
       <c r="J145" s="1"/>
       <c r="K145" s="1"/>
       <c r="L145" s="1"/>
-      <c r="M145" s="1"/>
+      <c r="M145" s="1" t="s">
+        <v>544</v>
+      </c>
       <c r="N145" s="1"/>
       <c r="O145" s="1"/>
       <c r="P145" s="1"/>
@@ -10787,7 +10831,9 @@
       <c r="J146" s="1"/>
       <c r="K146" s="1"/>
       <c r="L146" s="1"/>
-      <c r="M146" s="1"/>
+      <c r="M146" s="1" t="s">
+        <v>544</v>
+      </c>
       <c r="N146" s="1"/>
       <c r="O146" s="1"/>
       <c r="P146" s="1"/>
@@ -10825,7 +10871,9 @@
       <c r="J147" s="1"/>
       <c r="K147" s="1"/>
       <c r="L147" s="1"/>
-      <c r="M147" s="1"/>
+      <c r="M147" s="1" t="s">
+        <v>544</v>
+      </c>
       <c r="N147" s="1"/>
       <c r="O147" s="1"/>
       <c r="P147" s="1"/>
@@ -10863,7 +10911,9 @@
       <c r="J148" s="1"/>
       <c r="K148" s="1"/>
       <c r="L148" s="1"/>
-      <c r="M148" s="1"/>
+      <c r="M148" s="1" t="s">
+        <v>678</v>
+      </c>
       <c r="N148" s="1"/>
       <c r="O148" s="1"/>
       <c r="P148" s="1"/>
@@ -10901,7 +10951,9 @@
       <c r="J149" s="1"/>
       <c r="K149" s="1"/>
       <c r="L149" s="1"/>
-      <c r="M149" s="1"/>
+      <c r="M149" s="1" t="s">
+        <v>678</v>
+      </c>
       <c r="N149" s="1"/>
       <c r="O149" s="1"/>
       <c r="P149" s="1"/>
@@ -10939,7 +10991,9 @@
       <c r="J150" s="1"/>
       <c r="K150" s="1"/>
       <c r="L150" s="1"/>
-      <c r="M150" s="1"/>
+      <c r="M150" s="1" t="s">
+        <v>678</v>
+      </c>
       <c r="N150" s="1"/>
       <c r="O150" s="1"/>
       <c r="P150" s="1"/>
@@ -10977,7 +11031,9 @@
       <c r="J151" s="1"/>
       <c r="K151" s="1"/>
       <c r="L151" s="1"/>
-      <c r="M151" s="1"/>
+      <c r="M151" s="1" t="s">
+        <v>679</v>
+      </c>
       <c r="N151" s="1"/>
       <c r="O151" s="1"/>
       <c r="P151" s="1"/>
@@ -11015,7 +11071,9 @@
       <c r="J152" s="1"/>
       <c r="K152" s="1"/>
       <c r="L152" s="1"/>
-      <c r="M152" s="1"/>
+      <c r="M152" s="1" t="s">
+        <v>679</v>
+      </c>
       <c r="N152" s="1"/>
       <c r="O152" s="1"/>
       <c r="P152" s="1"/>
@@ -11053,7 +11111,9 @@
       <c r="J153" s="1"/>
       <c r="K153" s="1"/>
       <c r="L153" s="1"/>
-      <c r="M153" s="1"/>
+      <c r="M153" s="1" t="s">
+        <v>679</v>
+      </c>
       <c r="N153" s="1"/>
       <c r="O153" s="1"/>
       <c r="P153" s="1"/>

</xml_diff>

<commit_message>
updated data sheet and storage information
</commit_message>
<xml_diff>
--- a/Data/2018-08-14_master_datac_2018_collection_year.xlsx
+++ b/Data/2018-08-14_master_datac_2018_collection_year.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hinalkharva\Desktop\Circadian_rhythm_runs_seasonal_timing\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C23687C1-D729-4675-A5D4-39311F889DDC}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BEB5D37-2865-49DA-AF46-7A6CD4953C9E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="52065" yWindow="465" windowWidth="36360" windowHeight="21135" activeTab="2" xr2:uid="{C7477166-8A7C-B04A-9643-C277FEDCDAAB}"/>
+    <workbookView xWindow="52065" yWindow="465" windowWidth="36360" windowHeight="21135" activeTab="1" xr2:uid="{C7477166-8A7C-B04A-9643-C277FEDCDAAB}"/>
   </bookViews>
   <sheets>
     <sheet name="Maggot_Collections" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11742" uniqueCount="896">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12225" uniqueCount="913">
   <si>
     <t>Ind_ID</t>
   </si>
@@ -2715,6 +2715,57 @@
   </si>
   <si>
     <t>a9w45_18</t>
+  </si>
+  <si>
+    <t>A2-10-1</t>
+  </si>
+  <si>
+    <t>A2-10-2</t>
+  </si>
+  <si>
+    <t>A2-10-3</t>
+  </si>
+  <si>
+    <t>A2-10-4</t>
+  </si>
+  <si>
+    <t>A2-10-5</t>
+  </si>
+  <si>
+    <t>A2-10-6</t>
+  </si>
+  <si>
+    <t>A2-10-7</t>
+  </si>
+  <si>
+    <t>A2-10-8</t>
+  </si>
+  <si>
+    <t>A2-10-9</t>
+  </si>
+  <si>
+    <t>A2-10-10</t>
+  </si>
+  <si>
+    <t>A2-10-11</t>
+  </si>
+  <si>
+    <t>A2-10-12</t>
+  </si>
+  <si>
+    <t>A2-10-13</t>
+  </si>
+  <si>
+    <t>A2-10-14</t>
+  </si>
+  <si>
+    <t>A2-10-15</t>
+  </si>
+  <si>
+    <t>A2-10-16</t>
+  </si>
+  <si>
+    <t>A2-10-17</t>
   </si>
 </sst>
 </file>
@@ -3321,8 +3372,8 @@
   <dimension ref="A1:AC306"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A73" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P108" sqref="P108"/>
+      <pane ySplit="1" topLeftCell="A94" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F113" sqref="F113:M118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -13605,11 +13656,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92725FB9-1A17-2546-9DFA-6C0D39437891}">
-  <dimension ref="A1:AS1206"/>
+  <dimension ref="A1:AS1275"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K19" sqref="K19"/>
+    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A1219" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AE1243" sqref="AE1243"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -54010,6 +54061,15 @@
       <c r="K1119" t="s">
         <v>61</v>
       </c>
+      <c r="L1119">
+        <v>7000</v>
+      </c>
+      <c r="M1119" s="20">
+        <v>0.4301388888888889</v>
+      </c>
+      <c r="N1119">
+        <v>0.1301273</v>
+      </c>
       <c r="T1119" s="1" t="s">
         <v>221</v>
       </c>
@@ -54051,6 +54111,15 @@
       <c r="K1120" t="s">
         <v>61</v>
       </c>
+      <c r="L1120">
+        <v>7000</v>
+      </c>
+      <c r="M1120" s="20">
+        <v>0.43105324074074075</v>
+      </c>
+      <c r="N1120">
+        <v>0.60055080000000005</v>
+      </c>
       <c r="T1120" s="1" t="s">
         <v>221</v>
       </c>
@@ -54089,6 +54158,15 @@
       <c r="K1121" t="s">
         <v>61</v>
       </c>
+      <c r="L1121">
+        <v>7000</v>
+      </c>
+      <c r="M1121" s="20">
+        <v>0.43193287037037037</v>
+      </c>
+      <c r="N1121">
+        <v>0.14884349999999999</v>
+      </c>
       <c r="T1121" s="1" t="s">
         <v>221</v>
       </c>
@@ -54130,6 +54208,15 @@
       <c r="K1122" t="s">
         <v>61</v>
       </c>
+      <c r="L1122">
+        <v>7000</v>
+      </c>
+      <c r="M1122" s="20">
+        <v>0.43263888888888885</v>
+      </c>
+      <c r="N1122">
+        <v>0.40967320000000002</v>
+      </c>
       <c r="T1122" s="1" t="s">
         <v>221</v>
       </c>
@@ -54171,6 +54258,15 @@
       <c r="K1123" t="s">
         <v>61</v>
       </c>
+      <c r="L1123">
+        <v>7000</v>
+      </c>
+      <c r="M1123" s="20">
+        <v>0.43361111111111111</v>
+      </c>
+      <c r="N1123">
+        <v>5.0958499999999997E-2</v>
+      </c>
       <c r="T1123" s="1" t="s">
         <v>221</v>
       </c>
@@ -54212,6 +54308,15 @@
       <c r="K1124" t="s">
         <v>61</v>
       </c>
+      <c r="L1124">
+        <v>7000</v>
+      </c>
+      <c r="M1124" s="20">
+        <v>0.43446759259259254</v>
+      </c>
+      <c r="N1124">
+        <v>0.15245049999999999</v>
+      </c>
       <c r="T1124" s="1" t="s">
         <v>221</v>
       </c>
@@ -54250,6 +54355,15 @@
       <c r="K1125" t="s">
         <v>61</v>
       </c>
+      <c r="L1125">
+        <v>7000</v>
+      </c>
+      <c r="M1125" s="20">
+        <v>0.43534722222222227</v>
+      </c>
+      <c r="N1125">
+        <v>0.2787984</v>
+      </c>
       <c r="T1125" s="1" t="s">
         <v>221</v>
       </c>
@@ -54291,6 +54405,15 @@
       <c r="K1126" t="s">
         <v>61</v>
       </c>
+      <c r="L1126">
+        <v>7000</v>
+      </c>
+      <c r="M1126" s="20">
+        <v>0.43615740740740744</v>
+      </c>
+      <c r="N1126" s="21">
+        <v>5.437939E-2</v>
+      </c>
       <c r="T1126" s="1" t="s">
         <v>221</v>
       </c>
@@ -54332,6 +54455,15 @@
       <c r="K1127" t="s">
         <v>61</v>
       </c>
+      <c r="L1127">
+        <v>7000</v>
+      </c>
+      <c r="M1127" s="20">
+        <v>0.43687499999999996</v>
+      </c>
+      <c r="N1127" s="21">
+        <v>4.4645959999999998E-2</v>
+      </c>
       <c r="T1127" s="1" t="s">
         <v>221</v>
       </c>
@@ -54370,6 +54502,15 @@
       <c r="K1128" t="s">
         <v>61</v>
       </c>
+      <c r="L1128">
+        <v>7000</v>
+      </c>
+      <c r="M1128" s="20">
+        <v>0.43768518518518523</v>
+      </c>
+      <c r="N1128">
+        <v>0.1212297</v>
+      </c>
       <c r="T1128" s="1" t="s">
         <v>221</v>
       </c>
@@ -54408,6 +54549,15 @@
       <c r="K1129" t="s">
         <v>61</v>
       </c>
+      <c r="L1129">
+        <v>7000</v>
+      </c>
+      <c r="M1129" s="20">
+        <v>0.43853009259259257</v>
+      </c>
+      <c r="N1129">
+        <v>0.66719410000000001</v>
+      </c>
       <c r="T1129" s="1" t="s">
         <v>221</v>
       </c>
@@ -54449,6 +54599,15 @@
       <c r="K1130" t="s">
         <v>61</v>
       </c>
+      <c r="L1130">
+        <v>7000</v>
+      </c>
+      <c r="M1130" s="20">
+        <v>0.43950231481481478</v>
+      </c>
+      <c r="N1130">
+        <v>0.24837790000000001</v>
+      </c>
       <c r="T1130" s="1" t="s">
         <v>221</v>
       </c>
@@ -54490,6 +54649,15 @@
       <c r="K1131" t="s">
         <v>61</v>
       </c>
+      <c r="L1131">
+        <v>7000</v>
+      </c>
+      <c r="M1131" s="20">
+        <v>0.44027777777777777</v>
+      </c>
+      <c r="N1131">
+        <v>0.1230319</v>
+      </c>
       <c r="T1131" s="1" t="s">
         <v>221</v>
       </c>
@@ -54531,6 +54699,15 @@
       <c r="K1132" t="s">
         <v>61</v>
       </c>
+      <c r="L1132">
+        <v>7000</v>
+      </c>
+      <c r="M1132" s="20">
+        <v>0.44107638888888889</v>
+      </c>
+      <c r="N1132" s="21">
+        <v>6.4228830000000001E-2</v>
+      </c>
       <c r="T1132" s="1" t="s">
         <v>221</v>
       </c>
@@ -54572,6 +54749,15 @@
       <c r="K1133" t="s">
         <v>61</v>
       </c>
+      <c r="L1133">
+        <v>7000</v>
+      </c>
+      <c r="M1133" s="20">
+        <v>0.4418171296296296</v>
+      </c>
+      <c r="N1133">
+        <v>0.62002860000000004</v>
+      </c>
       <c r="T1133" s="1" t="s">
         <v>221</v>
       </c>
@@ -54610,6 +54796,15 @@
       <c r="K1134" t="s">
         <v>61</v>
       </c>
+      <c r="L1134">
+        <v>7000</v>
+      </c>
+      <c r="M1134" s="20">
+        <v>0.44268518518518518</v>
+      </c>
+      <c r="N1134" s="21">
+        <v>4.1810710000000001E-2</v>
+      </c>
       <c r="T1134" s="1" t="s">
         <v>221</v>
       </c>
@@ -54651,6 +54846,15 @@
       <c r="K1135" t="s">
         <v>61</v>
       </c>
+      <c r="L1135">
+        <v>7000</v>
+      </c>
+      <c r="M1135" s="20">
+        <v>0.44344907407407402</v>
+      </c>
+      <c r="N1135">
+        <v>0.17454430000000001</v>
+      </c>
       <c r="T1135" s="1" t="s">
         <v>221</v>
       </c>
@@ -54689,6 +54893,15 @@
       <c r="K1136" t="s">
         <v>61</v>
       </c>
+      <c r="L1136">
+        <v>7000</v>
+      </c>
+      <c r="M1136" s="20">
+        <v>0.44418981481481484</v>
+      </c>
+      <c r="N1136" s="21">
+        <v>4.3292450000000003E-2</v>
+      </c>
       <c r="T1136" s="1" t="s">
         <v>221</v>
       </c>
@@ -54727,6 +54940,15 @@
       <c r="K1137" t="s">
         <v>61</v>
       </c>
+      <c r="L1137">
+        <v>7000</v>
+      </c>
+      <c r="M1137" s="20">
+        <v>0.44491898148148151</v>
+      </c>
+      <c r="N1137">
+        <v>0.38923530000000001</v>
+      </c>
       <c r="T1137" s="1" t="s">
         <v>221</v>
       </c>
@@ -54768,6 +54990,15 @@
       <c r="K1138" t="s">
         <v>61</v>
       </c>
+      <c r="L1138">
+        <v>7000</v>
+      </c>
+      <c r="M1138" s="20">
+        <v>0.44579861111111113</v>
+      </c>
+      <c r="N1138" s="21">
+        <v>5.9499459999999997E-2</v>
+      </c>
       <c r="T1138" s="1" t="s">
         <v>221</v>
       </c>
@@ -54809,6 +55040,15 @@
       <c r="K1139" t="s">
         <v>61</v>
       </c>
+      <c r="L1139">
+        <v>7000</v>
+      </c>
+      <c r="M1139" s="20">
+        <v>0.44658564814814811</v>
+      </c>
+      <c r="N1139" s="21">
+        <v>6.9297280000000003E-2</v>
+      </c>
       <c r="T1139" s="1" t="s">
         <v>221</v>
       </c>
@@ -54850,6 +55090,15 @@
       <c r="K1140" t="s">
         <v>61</v>
       </c>
+      <c r="L1140">
+        <v>7000</v>
+      </c>
+      <c r="M1140" s="20">
+        <v>0.44747685185185188</v>
+      </c>
+      <c r="N1140">
+        <v>0.10623829999999999</v>
+      </c>
       <c r="T1140" s="1" t="s">
         <v>221</v>
       </c>
@@ -54891,6 +55140,15 @@
       <c r="K1141" t="s">
         <v>61</v>
       </c>
+      <c r="L1141">
+        <v>7000</v>
+      </c>
+      <c r="M1141" s="20">
+        <v>0.44822916666666668</v>
+      </c>
+      <c r="N1141">
+        <v>0.14765629999999999</v>
+      </c>
       <c r="T1141" s="1" t="s">
         <v>221</v>
       </c>
@@ -54932,6 +55190,15 @@
       <c r="K1142" t="s">
         <v>61</v>
       </c>
+      <c r="L1142">
+        <v>7000</v>
+      </c>
+      <c r="M1142" s="20">
+        <v>0.44899305555555552</v>
+      </c>
+      <c r="N1142">
+        <v>0.5812039</v>
+      </c>
       <c r="T1142" s="1" t="s">
         <v>221</v>
       </c>
@@ -54973,6 +55240,15 @@
       <c r="K1143" t="s">
         <v>61</v>
       </c>
+      <c r="L1143">
+        <v>7000</v>
+      </c>
+      <c r="M1143" s="20">
+        <v>0.44988425925925929</v>
+      </c>
+      <c r="N1143">
+        <v>0.10971740000000001</v>
+      </c>
       <c r="T1143" s="1" t="s">
         <v>221</v>
       </c>
@@ -55011,6 +55287,15 @@
       <c r="K1144" t="s">
         <v>61</v>
       </c>
+      <c r="L1144">
+        <v>7000</v>
+      </c>
+      <c r="M1144" s="20">
+        <v>0.45068287037037041</v>
+      </c>
+      <c r="N1144">
+        <v>0.4975908</v>
+      </c>
       <c r="T1144" s="1" t="s">
         <v>221</v>
       </c>
@@ -55049,6 +55334,15 @@
       <c r="K1145" t="s">
         <v>61</v>
       </c>
+      <c r="L1145">
+        <v>7000</v>
+      </c>
+      <c r="M1145" s="20">
+        <v>0.45151620370370371</v>
+      </c>
+      <c r="N1145">
+        <v>0.22076380000000001</v>
+      </c>
       <c r="T1145" s="1" t="s">
         <v>221</v>
       </c>
@@ -55090,6 +55384,15 @@
       <c r="K1146" t="s">
         <v>61</v>
       </c>
+      <c r="L1146">
+        <v>7000</v>
+      </c>
+      <c r="M1146" s="20">
+        <v>0.4522916666666667</v>
+      </c>
+      <c r="N1146" s="21">
+        <v>8.8099689999999994E-2</v>
+      </c>
       <c r="T1146" s="1" t="s">
         <v>221</v>
       </c>
@@ -55131,6 +55434,15 @@
       <c r="K1147" t="s">
         <v>61</v>
       </c>
+      <c r="L1147">
+        <v>7000</v>
+      </c>
+      <c r="M1147" s="20">
+        <v>0.45307870370370368</v>
+      </c>
+      <c r="N1147">
+        <v>0.17090340000000001</v>
+      </c>
       <c r="T1147" s="1" t="s">
         <v>221</v>
       </c>
@@ -55169,6 +55481,15 @@
       <c r="K1148" t="s">
         <v>61</v>
       </c>
+      <c r="L1148">
+        <v>7000</v>
+      </c>
+      <c r="M1148" s="20">
+        <v>0.45385416666666667</v>
+      </c>
+      <c r="N1148" s="21">
+        <v>4.8078509999999998E-2</v>
+      </c>
       <c r="T1148" s="1" t="s">
         <v>221</v>
       </c>
@@ -55210,6 +55531,15 @@
       <c r="K1149" t="s">
         <v>61</v>
       </c>
+      <c r="L1149">
+        <v>7000</v>
+      </c>
+      <c r="M1149" s="20">
+        <v>0.45456018518518521</v>
+      </c>
+      <c r="N1149" s="21">
+        <v>7.4357870000000006E-2</v>
+      </c>
       <c r="T1149" s="1" t="s">
         <v>221</v>
       </c>
@@ -55248,6 +55578,15 @@
       <c r="K1150" t="s">
         <v>61</v>
       </c>
+      <c r="L1150">
+        <v>7000</v>
+      </c>
+      <c r="M1150" s="20">
+        <v>0.455625</v>
+      </c>
+      <c r="N1150" s="21">
+        <v>5.6203120000000002E-2</v>
+      </c>
       <c r="T1150" s="1" t="s">
         <v>221</v>
       </c>
@@ -55289,6 +55628,15 @@
       <c r="K1151" t="s">
         <v>61</v>
       </c>
+      <c r="L1151">
+        <v>7000</v>
+      </c>
+      <c r="M1151" s="20">
+        <v>0.4563888888888889</v>
+      </c>
+      <c r="N1151">
+        <v>0.31155909999999998</v>
+      </c>
       <c r="T1151" s="1" t="s">
         <v>221</v>
       </c>
@@ -55330,6 +55678,15 @@
       <c r="K1152" t="s">
         <v>61</v>
       </c>
+      <c r="L1152">
+        <v>7000</v>
+      </c>
+      <c r="M1152" s="20">
+        <v>0.4571412037037037</v>
+      </c>
+      <c r="N1152" s="21">
+        <v>4.5546650000000001E-2</v>
+      </c>
       <c r="T1152" s="1" t="s">
         <v>221</v>
       </c>
@@ -55371,6 +55728,15 @@
       <c r="K1153" t="s">
         <v>61</v>
       </c>
+      <c r="L1153">
+        <v>7000</v>
+      </c>
+      <c r="M1153" s="20">
+        <v>0.45802083333333332</v>
+      </c>
+      <c r="N1153">
+        <v>0.46958719999999998</v>
+      </c>
       <c r="T1153" s="1" t="s">
         <v>221</v>
       </c>
@@ -55412,6 +55778,15 @@
       <c r="K1154" t="s">
         <v>61</v>
       </c>
+      <c r="L1154">
+        <v>7000</v>
+      </c>
+      <c r="M1154" s="20">
+        <v>0.45887731481481481</v>
+      </c>
+      <c r="N1154">
+        <v>0.50150130000000004</v>
+      </c>
       <c r="T1154" s="1" t="s">
         <v>221</v>
       </c>
@@ -55453,6 +55828,15 @@
       <c r="K1155" t="s">
         <v>61</v>
       </c>
+      <c r="L1155">
+        <v>7000</v>
+      </c>
+      <c r="M1155" s="20">
+        <v>0.4597222222222222</v>
+      </c>
+      <c r="N1155">
+        <v>0.3936133</v>
+      </c>
       <c r="T1155" s="1" t="s">
         <v>221</v>
       </c>
@@ -55494,6 +55878,15 @@
       <c r="K1156" t="s">
         <v>61</v>
       </c>
+      <c r="L1156">
+        <v>7000</v>
+      </c>
+      <c r="M1156" s="20">
+        <v>0.46064814814814814</v>
+      </c>
+      <c r="N1156">
+        <v>0.39171410000000001</v>
+      </c>
       <c r="T1156" s="1" t="s">
         <v>221</v>
       </c>
@@ -55535,6 +55928,15 @@
       <c r="K1157" t="s">
         <v>61</v>
       </c>
+      <c r="L1157">
+        <v>7000</v>
+      </c>
+      <c r="M1157" s="20">
+        <v>0.46144675925925926</v>
+      </c>
+      <c r="N1157">
+        <v>0.1244712</v>
+      </c>
       <c r="T1157" s="1" t="s">
         <v>221</v>
       </c>
@@ -55573,6 +55975,15 @@
       <c r="K1158" t="s">
         <v>61</v>
       </c>
+      <c r="L1158">
+        <v>7000</v>
+      </c>
+      <c r="M1158" s="20">
+        <v>0.46702546296296293</v>
+      </c>
+      <c r="N1158" s="21">
+        <v>8.5535920000000005E-3</v>
+      </c>
       <c r="T1158" s="1" t="s">
         <v>221</v>
       </c>
@@ -55605,6 +56016,15 @@
       <c r="K1159" t="s">
         <v>61</v>
       </c>
+      <c r="L1159">
+        <v>7000</v>
+      </c>
+      <c r="M1159" s="20">
+        <v>0.46770833333333334</v>
+      </c>
+      <c r="N1159" s="21">
+        <v>7.5197620000000001E-3</v>
+      </c>
       <c r="T1159" s="1" t="s">
         <v>221</v>
       </c>
@@ -55640,6 +56060,15 @@
       <c r="K1160" t="s">
         <v>61</v>
       </c>
+      <c r="L1160">
+        <v>6262</v>
+      </c>
+      <c r="M1160" s="20">
+        <v>0.4301388888888889</v>
+      </c>
+      <c r="N1160">
+        <v>0.1584024</v>
+      </c>
       <c r="T1160" s="1" t="s">
         <v>221</v>
       </c>
@@ -55681,6 +56110,15 @@
       <c r="K1161" t="s">
         <v>61</v>
       </c>
+      <c r="L1161">
+        <v>6262</v>
+      </c>
+      <c r="M1161" s="20">
+        <v>0.43105324074074075</v>
+      </c>
+      <c r="N1161">
+        <v>0.10583289999999999</v>
+      </c>
       <c r="T1161" s="1" t="s">
         <v>221</v>
       </c>
@@ -55719,6 +56157,15 @@
       <c r="K1162" t="s">
         <v>61</v>
       </c>
+      <c r="L1162">
+        <v>6262</v>
+      </c>
+      <c r="M1162" s="20">
+        <v>0.43193287037037037</v>
+      </c>
+      <c r="N1162" s="21">
+        <v>9.1916349999999994E-2</v>
+      </c>
       <c r="T1162" s="1" t="s">
         <v>221</v>
       </c>
@@ -55760,6 +56207,15 @@
       <c r="K1163" t="s">
         <v>61</v>
       </c>
+      <c r="L1163">
+        <v>6262</v>
+      </c>
+      <c r="M1163" s="20">
+        <v>0.43263888888888885</v>
+      </c>
+      <c r="N1163">
+        <v>0.65062030000000004</v>
+      </c>
       <c r="T1163" s="1" t="s">
         <v>221</v>
       </c>
@@ -55801,6 +56257,15 @@
       <c r="K1164" t="s">
         <v>61</v>
       </c>
+      <c r="L1164">
+        <v>6262</v>
+      </c>
+      <c r="M1164" s="20">
+        <v>0.43361111111111111</v>
+      </c>
+      <c r="N1164" s="21">
+        <v>9.8182210000000006E-2</v>
+      </c>
       <c r="T1164" s="1" t="s">
         <v>221</v>
       </c>
@@ -55842,6 +56307,15 @@
       <c r="K1165" t="s">
         <v>61</v>
       </c>
+      <c r="L1165">
+        <v>6262</v>
+      </c>
+      <c r="M1165" s="20">
+        <v>0.43446759259259254</v>
+      </c>
+      <c r="N1165" s="21">
+        <v>3.9442310000000001E-2</v>
+      </c>
       <c r="T1165" s="1" t="s">
         <v>221</v>
       </c>
@@ -55880,6 +56354,15 @@
       <c r="K1166" t="s">
         <v>61</v>
       </c>
+      <c r="L1166">
+        <v>6262</v>
+      </c>
+      <c r="M1166" s="20">
+        <v>0.43534722222222227</v>
+      </c>
+      <c r="N1166">
+        <v>0.14469389999999999</v>
+      </c>
       <c r="T1166" s="1" t="s">
         <v>221</v>
       </c>
@@ -55918,6 +56401,15 @@
       <c r="K1167" t="s">
         <v>61</v>
       </c>
+      <c r="L1167">
+        <v>6262</v>
+      </c>
+      <c r="M1167" s="20">
+        <v>0.43615740740740744</v>
+      </c>
+      <c r="N1167">
+        <v>0.1101157</v>
+      </c>
       <c r="T1167" s="1" t="s">
         <v>221</v>
       </c>
@@ -55956,6 +56448,15 @@
       <c r="K1168" t="s">
         <v>61</v>
       </c>
+      <c r="L1168">
+        <v>6262</v>
+      </c>
+      <c r="M1168" s="20">
+        <v>0.43687499999999996</v>
+      </c>
+      <c r="N1168">
+        <v>0.1828079</v>
+      </c>
       <c r="T1168" s="1" t="s">
         <v>221</v>
       </c>
@@ -55997,6 +56498,15 @@
       <c r="K1169" t="s">
         <v>61</v>
       </c>
+      <c r="L1169">
+        <v>6262</v>
+      </c>
+      <c r="M1169" s="20">
+        <v>0.43768518518518523</v>
+      </c>
+      <c r="N1169">
+        <v>0.1490496</v>
+      </c>
       <c r="T1169" s="1" t="s">
         <v>221</v>
       </c>
@@ -56038,6 +56548,15 @@
       <c r="K1170" t="s">
         <v>61</v>
       </c>
+      <c r="L1170">
+        <v>6262</v>
+      </c>
+      <c r="M1170" s="20">
+        <v>0.43853009259259257</v>
+      </c>
+      <c r="N1170">
+        <v>0.5322983</v>
+      </c>
       <c r="T1170" s="1" t="s">
         <v>221</v>
       </c>
@@ -56076,6 +56595,15 @@
       <c r="K1171" t="s">
         <v>61</v>
       </c>
+      <c r="L1171">
+        <v>6262</v>
+      </c>
+      <c r="M1171" s="20">
+        <v>0.43950231481481478</v>
+      </c>
+      <c r="N1171">
+        <v>0.1216599</v>
+      </c>
       <c r="T1171" s="1" t="s">
         <v>221</v>
       </c>
@@ -56114,6 +56642,15 @@
       <c r="K1172" t="s">
         <v>61</v>
       </c>
+      <c r="L1172">
+        <v>6262</v>
+      </c>
+      <c r="M1172" s="20">
+        <v>0.44027777777777777</v>
+      </c>
+      <c r="N1172">
+        <v>0.18624540000000001</v>
+      </c>
       <c r="T1172" s="1" t="s">
         <v>221</v>
       </c>
@@ -56155,6 +56692,15 @@
       <c r="K1173" t="s">
         <v>61</v>
       </c>
+      <c r="L1173">
+        <v>6262</v>
+      </c>
+      <c r="M1173" s="20">
+        <v>0.44107638888888889</v>
+      </c>
+      <c r="N1173">
+        <v>0.19425400000000001</v>
+      </c>
       <c r="T1173" s="1" t="s">
         <v>221</v>
       </c>
@@ -56196,6 +56742,15 @@
       <c r="K1174" t="s">
         <v>61</v>
       </c>
+      <c r="L1174">
+        <v>6262</v>
+      </c>
+      <c r="M1174" s="20">
+        <v>0.4418171296296296</v>
+      </c>
+      <c r="N1174">
+        <v>0.1177052</v>
+      </c>
       <c r="T1174" s="1" t="s">
         <v>221</v>
       </c>
@@ -56237,6 +56792,15 @@
       <c r="K1175" t="s">
         <v>61</v>
       </c>
+      <c r="L1175">
+        <v>6262</v>
+      </c>
+      <c r="M1175" s="20">
+        <v>0.44268518518518518</v>
+      </c>
+      <c r="N1175">
+        <v>0.12382840000000001</v>
+      </c>
       <c r="T1175" s="1" t="s">
         <v>221</v>
       </c>
@@ -56275,6 +56839,15 @@
       <c r="K1176" t="s">
         <v>61</v>
       </c>
+      <c r="L1176">
+        <v>6262</v>
+      </c>
+      <c r="M1176" s="20">
+        <v>0.44344907407407402</v>
+      </c>
+      <c r="N1176">
+        <v>7.0182300000000003E-2</v>
+      </c>
       <c r="T1176" s="1" t="s">
         <v>221</v>
       </c>
@@ -56313,6 +56886,15 @@
       <c r="K1177" t="s">
         <v>61</v>
       </c>
+      <c r="L1177">
+        <v>6262</v>
+      </c>
+      <c r="M1177" s="20">
+        <v>0.44418981481481484</v>
+      </c>
+      <c r="N1177">
+        <v>0.12599350000000001</v>
+      </c>
       <c r="T1177" s="1" t="s">
         <v>221</v>
       </c>
@@ -56351,6 +56933,15 @@
       <c r="K1178" t="s">
         <v>61</v>
       </c>
+      <c r="L1178">
+        <v>6262</v>
+      </c>
+      <c r="M1178" s="20">
+        <v>0.44491898148148151</v>
+      </c>
+      <c r="N1178">
+        <v>0.74829590000000001</v>
+      </c>
       <c r="T1178" s="1" t="s">
         <v>221</v>
       </c>
@@ -56392,6 +56983,15 @@
       <c r="K1179" t="s">
         <v>61</v>
       </c>
+      <c r="L1179">
+        <v>6262</v>
+      </c>
+      <c r="M1179" s="20">
+        <v>0.44579861111111113</v>
+      </c>
+      <c r="N1179" s="21">
+        <v>9.212236E-2</v>
+      </c>
       <c r="T1179" s="1" t="s">
         <v>221</v>
       </c>
@@ -56433,6 +57033,15 @@
       <c r="K1180" t="s">
         <v>61</v>
       </c>
+      <c r="L1180">
+        <v>6262</v>
+      </c>
+      <c r="M1180" s="20">
+        <v>0.44658564814814811</v>
+      </c>
+      <c r="N1180">
+        <v>0.92521350000000002</v>
+      </c>
       <c r="T1180" s="1" t="s">
         <v>221</v>
       </c>
@@ -56474,6 +57083,15 @@
       <c r="K1181" t="s">
         <v>61</v>
       </c>
+      <c r="L1181">
+        <v>6262</v>
+      </c>
+      <c r="M1181" s="20">
+        <v>0.44747685185185188</v>
+      </c>
+      <c r="N1181" s="21">
+        <v>2.3666880000000001E-2</v>
+      </c>
       <c r="T1181" s="1" t="s">
         <v>221</v>
       </c>
@@ -56515,6 +57133,15 @@
       <c r="K1182" t="s">
         <v>61</v>
       </c>
+      <c r="L1182">
+        <v>6262</v>
+      </c>
+      <c r="M1182" s="20">
+        <v>0.44822916666666668</v>
+      </c>
+      <c r="N1182">
+        <v>0.1208277</v>
+      </c>
       <c r="T1182" s="1" t="s">
         <v>221</v>
       </c>
@@ -56556,6 +57183,15 @@
       <c r="K1183" t="s">
         <v>61</v>
       </c>
+      <c r="L1183">
+        <v>6262</v>
+      </c>
+      <c r="M1183" s="20">
+        <v>0.44899305555555552</v>
+      </c>
+      <c r="N1183">
+        <v>0.13241720000000001</v>
+      </c>
       <c r="T1183" s="1" t="s">
         <v>221</v>
       </c>
@@ -56594,6 +57230,15 @@
       <c r="K1184" t="s">
         <v>61</v>
       </c>
+      <c r="L1184">
+        <v>6262</v>
+      </c>
+      <c r="M1184" s="20">
+        <v>0.44988425925925929</v>
+      </c>
+      <c r="N1184" s="21">
+        <v>8.1108730000000004E-2</v>
+      </c>
       <c r="T1184" s="1" t="s">
         <v>221</v>
       </c>
@@ -56635,6 +57280,15 @@
       <c r="K1185" t="s">
         <v>61</v>
       </c>
+      <c r="L1185">
+        <v>6262</v>
+      </c>
+      <c r="M1185" s="20">
+        <v>0.45068287037037041</v>
+      </c>
+      <c r="N1185">
+        <v>0.15521650000000001</v>
+      </c>
       <c r="T1185" s="1" t="s">
         <v>221</v>
       </c>
@@ -56676,6 +57330,15 @@
       <c r="K1186" t="s">
         <v>61</v>
       </c>
+      <c r="L1186">
+        <v>6262</v>
+      </c>
+      <c r="M1186" s="20">
+        <v>0.45151620370370371</v>
+      </c>
+      <c r="N1186">
+        <v>0.1090928</v>
+      </c>
       <c r="T1186" s="1" t="s">
         <v>221</v>
       </c>
@@ -56717,6 +57380,15 @@
       <c r="K1187" t="s">
         <v>61</v>
       </c>
+      <c r="L1187">
+        <v>6262</v>
+      </c>
+      <c r="M1187" s="20">
+        <v>0.4522916666666667</v>
+      </c>
+      <c r="N1187">
+        <v>0.1519279</v>
+      </c>
       <c r="T1187" s="1" t="s">
         <v>221</v>
       </c>
@@ -56758,6 +57430,15 @@
       <c r="K1188" t="s">
         <v>61</v>
       </c>
+      <c r="L1188">
+        <v>6262</v>
+      </c>
+      <c r="M1188" s="20">
+        <v>0.45307870370370368</v>
+      </c>
+      <c r="N1188">
+        <v>0.12259109999999999</v>
+      </c>
       <c r="T1188" s="1" t="s">
         <v>221</v>
       </c>
@@ -56796,6 +57477,15 @@
       <c r="K1189" t="s">
         <v>61</v>
       </c>
+      <c r="L1189">
+        <v>6262</v>
+      </c>
+      <c r="M1189" s="20">
+        <v>0.45385416666666667</v>
+      </c>
+      <c r="N1189" s="21">
+        <v>7.0612430000000004E-2</v>
+      </c>
       <c r="T1189" s="1" t="s">
         <v>221</v>
       </c>
@@ -56837,6 +57527,15 @@
       <c r="K1190" t="s">
         <v>61</v>
       </c>
+      <c r="L1190">
+        <v>6262</v>
+      </c>
+      <c r="M1190" s="20">
+        <v>0.45456018518518521</v>
+      </c>
+      <c r="N1190">
+        <v>0.8125405</v>
+      </c>
       <c r="T1190" s="1" t="s">
         <v>221</v>
       </c>
@@ -56875,6 +57574,15 @@
       <c r="K1191" t="s">
         <v>61</v>
       </c>
+      <c r="L1191">
+        <v>6262</v>
+      </c>
+      <c r="M1191" s="20">
+        <v>0.455625</v>
+      </c>
+      <c r="N1191" s="21">
+        <v>9.3835879999999997E-2</v>
+      </c>
       <c r="T1191" s="1" t="s">
         <v>221</v>
       </c>
@@ -56913,6 +57621,15 @@
       <c r="K1192" t="s">
         <v>61</v>
       </c>
+      <c r="L1192">
+        <v>6262</v>
+      </c>
+      <c r="M1192" s="20">
+        <v>0.4563888888888889</v>
+      </c>
+      <c r="N1192">
+        <v>0.16304379999999999</v>
+      </c>
       <c r="T1192" s="1" t="s">
         <v>221</v>
       </c>
@@ -56954,6 +57671,15 @@
       <c r="K1193" t="s">
         <v>61</v>
       </c>
+      <c r="L1193">
+        <v>6262</v>
+      </c>
+      <c r="M1193" s="20">
+        <v>0.4571412037037037</v>
+      </c>
+      <c r="N1193">
+        <v>0.1101207</v>
+      </c>
       <c r="T1193" s="1" t="s">
         <v>221</v>
       </c>
@@ -56995,6 +57721,15 @@
       <c r="K1194" t="s">
         <v>61</v>
       </c>
+      <c r="L1194">
+        <v>6262</v>
+      </c>
+      <c r="M1194" s="20">
+        <v>0.45802083333333332</v>
+      </c>
+      <c r="N1194" s="21">
+        <v>7.7204179999999997E-2</v>
+      </c>
       <c r="T1194" s="1" t="s">
         <v>221</v>
       </c>
@@ -57033,6 +57768,15 @@
       <c r="K1195" t="s">
         <v>61</v>
       </c>
+      <c r="L1195">
+        <v>6262</v>
+      </c>
+      <c r="M1195" s="20">
+        <v>0.45887731481481481</v>
+      </c>
+      <c r="N1195">
+        <v>0.21170269999999999</v>
+      </c>
       <c r="T1195" s="1" t="s">
         <v>221</v>
       </c>
@@ -57074,6 +57818,15 @@
       <c r="K1196" t="s">
         <v>61</v>
       </c>
+      <c r="L1196">
+        <v>6262</v>
+      </c>
+      <c r="M1196" s="20">
+        <v>0.4597222222222222</v>
+      </c>
+      <c r="N1196">
+        <v>1.3052060000000001</v>
+      </c>
       <c r="T1196" s="1" t="s">
         <v>221</v>
       </c>
@@ -57112,6 +57865,15 @@
       <c r="K1197" t="s">
         <v>61</v>
       </c>
+      <c r="L1197">
+        <v>6262</v>
+      </c>
+      <c r="M1197" s="20">
+        <v>0.46064814814814814</v>
+      </c>
+      <c r="N1197" s="21">
+        <v>9.2051980000000005E-2</v>
+      </c>
       <c r="T1197" s="1" t="s">
         <v>221</v>
       </c>
@@ -57150,6 +57912,15 @@
       <c r="K1198" t="s">
         <v>61</v>
       </c>
+      <c r="L1198">
+        <v>6262</v>
+      </c>
+      <c r="M1198" s="20">
+        <v>0.46144675925925926</v>
+      </c>
+      <c r="N1198">
+        <v>0.13875270000000001</v>
+      </c>
       <c r="T1198" s="1" t="s">
         <v>221</v>
       </c>
@@ -57188,6 +57959,15 @@
       <c r="K1199" t="s">
         <v>61</v>
       </c>
+      <c r="L1199">
+        <v>6262</v>
+      </c>
+      <c r="M1199" s="20">
+        <v>0.46222222222222226</v>
+      </c>
+      <c r="N1199">
+        <v>0.1227541</v>
+      </c>
       <c r="T1199" s="1" t="s">
         <v>221</v>
       </c>
@@ -57229,6 +58009,15 @@
       <c r="K1200" t="s">
         <v>61</v>
       </c>
+      <c r="L1200">
+        <v>6262</v>
+      </c>
+      <c r="M1200" s="20">
+        <v>0.46307870370370369</v>
+      </c>
+      <c r="N1200">
+        <v>0.1256034</v>
+      </c>
       <c r="T1200" s="1" t="s">
         <v>221</v>
       </c>
@@ -57270,6 +58059,15 @@
       <c r="K1201" t="s">
         <v>61</v>
       </c>
+      <c r="L1201">
+        <v>6262</v>
+      </c>
+      <c r="M1201" s="20">
+        <v>0.46387731481481481</v>
+      </c>
+      <c r="N1201" s="21">
+        <v>9.649373E-2</v>
+      </c>
       <c r="T1201" s="1" t="s">
         <v>221</v>
       </c>
@@ -57311,6 +58109,15 @@
       <c r="K1202" t="s">
         <v>61</v>
       </c>
+      <c r="L1202">
+        <v>6262</v>
+      </c>
+      <c r="M1202" s="20">
+        <v>0.46460648148148148</v>
+      </c>
+      <c r="N1202">
+        <v>0.57073850000000004</v>
+      </c>
       <c r="T1202" s="1" t="s">
         <v>221</v>
       </c>
@@ -57349,6 +58156,15 @@
       <c r="K1203" t="s">
         <v>61</v>
       </c>
+      <c r="L1203">
+        <v>6262</v>
+      </c>
+      <c r="M1203" s="20">
+        <v>0.46554398148148146</v>
+      </c>
+      <c r="N1203">
+        <v>8.7844199999999997E-2</v>
+      </c>
       <c r="T1203" s="1" t="s">
         <v>221</v>
       </c>
@@ -57390,6 +58206,15 @@
       <c r="K1204" t="s">
         <v>61</v>
       </c>
+      <c r="L1204">
+        <v>6262</v>
+      </c>
+      <c r="M1204" s="20">
+        <v>0.46626157407407409</v>
+      </c>
+      <c r="N1204">
+        <v>0.14297399999999999</v>
+      </c>
       <c r="T1204" s="1" t="s">
         <v>221</v>
       </c>
@@ -57428,6 +58253,15 @@
       <c r="K1205" t="s">
         <v>61</v>
       </c>
+      <c r="L1205">
+        <v>6262</v>
+      </c>
+      <c r="M1205" s="20">
+        <v>0.46702546296296293</v>
+      </c>
+      <c r="N1205" s="21">
+        <v>1.3670369999999999E-2</v>
+      </c>
       <c r="T1205" s="1" t="s">
         <v>221</v>
       </c>
@@ -57460,8 +58294,2226 @@
       <c r="K1206" t="s">
         <v>61</v>
       </c>
+      <c r="L1206">
+        <v>6262</v>
+      </c>
+      <c r="M1206" s="20">
+        <v>0.46770833333333334</v>
+      </c>
+      <c r="N1206" s="21">
+        <v>1.1283079999999999E-2</v>
+      </c>
       <c r="T1206" s="1" t="s">
         <v>221</v>
+      </c>
+    </row>
+    <row r="1207" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1207">
+        <v>1</v>
+      </c>
+      <c r="C1207" t="s">
+        <v>59</v>
+      </c>
+      <c r="G1207" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I1207" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="J1207">
+        <v>21</v>
+      </c>
+      <c r="K1207" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1207" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y1207" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z1207" t="s">
+        <v>896</v>
+      </c>
+    </row>
+    <row r="1208" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1208">
+        <v>2</v>
+      </c>
+      <c r="C1208" t="s">
+        <v>59</v>
+      </c>
+      <c r="G1208" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I1208" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="J1208">
+        <v>21</v>
+      </c>
+      <c r="K1208" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1208" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y1208" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z1208" t="s">
+        <v>897</v>
+      </c>
+    </row>
+    <row r="1209" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1209">
+        <v>3</v>
+      </c>
+      <c r="C1209" t="s">
+        <v>59</v>
+      </c>
+      <c r="G1209" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I1209" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="J1209">
+        <v>21</v>
+      </c>
+      <c r="K1209" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1209" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y1209" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z1209" t="s">
+        <v>898</v>
+      </c>
+    </row>
+    <row r="1210" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1210">
+        <v>4</v>
+      </c>
+      <c r="C1210" t="s">
+        <v>59</v>
+      </c>
+      <c r="G1210" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I1210" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="J1210">
+        <v>21</v>
+      </c>
+      <c r="K1210" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1210" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y1210" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z1210" t="s">
+        <v>899</v>
+      </c>
+    </row>
+    <row r="1211" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1211">
+        <v>5</v>
+      </c>
+      <c r="C1211" t="s">
+        <v>59</v>
+      </c>
+      <c r="G1211" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I1211" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="J1211">
+        <v>21</v>
+      </c>
+      <c r="K1211" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1211" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y1211" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z1211" t="s">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="1212" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1212">
+        <v>6</v>
+      </c>
+      <c r="C1212" t="s">
+        <v>59</v>
+      </c>
+      <c r="G1212" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I1212" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="J1212">
+        <v>21</v>
+      </c>
+      <c r="K1212" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1212" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y1212" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z1212" t="s">
+        <v>901</v>
+      </c>
+    </row>
+    <row r="1213" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1213">
+        <v>7</v>
+      </c>
+      <c r="C1213" t="s">
+        <v>59</v>
+      </c>
+      <c r="G1213" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I1213" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="J1213">
+        <v>21</v>
+      </c>
+      <c r="K1213" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1213" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y1213" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z1213" t="s">
+        <v>902</v>
+      </c>
+    </row>
+    <row r="1214" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1214">
+        <v>1</v>
+      </c>
+      <c r="C1214" t="s">
+        <v>59</v>
+      </c>
+      <c r="G1214" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I1214" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="J1214">
+        <v>21</v>
+      </c>
+      <c r="K1214" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1214" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y1214" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z1214" t="str">
+        <f>"A2-6"&amp;Y1214&amp;"-"&amp;AC1214</f>
+        <v>A2-6RT-A1</v>
+      </c>
+      <c r="AC1214" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="1215" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1215">
+        <v>2</v>
+      </c>
+      <c r="C1215" t="s">
+        <v>59</v>
+      </c>
+      <c r="G1215" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I1215" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="J1215">
+        <v>21</v>
+      </c>
+      <c r="K1215" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1215" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y1215" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z1215" t="str">
+        <f t="shared" ref="Z1215:Z1229" si="12">"A2-6"&amp;Y1215&amp;"-"&amp;AC1215</f>
+        <v>A2-6RT-A2</v>
+      </c>
+      <c r="AC1215" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="1216" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1216">
+        <v>3</v>
+      </c>
+      <c r="C1216" t="s">
+        <v>59</v>
+      </c>
+      <c r="G1216" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I1216" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="J1216">
+        <v>21</v>
+      </c>
+      <c r="K1216" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1216" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y1216" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z1216" t="str">
+        <f t="shared" si="12"/>
+        <v>A2-6RT-A3</v>
+      </c>
+      <c r="AC1216" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="1217" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1217">
+        <v>4</v>
+      </c>
+      <c r="C1217" t="s">
+        <v>59</v>
+      </c>
+      <c r="G1217" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I1217" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="J1217">
+        <v>21</v>
+      </c>
+      <c r="K1217" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1217" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y1217" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z1217" t="str">
+        <f t="shared" si="12"/>
+        <v>A2-6RT-A4</v>
+      </c>
+      <c r="AC1217" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="1218" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1218">
+        <v>5</v>
+      </c>
+      <c r="C1218" t="s">
+        <v>59</v>
+      </c>
+      <c r="G1218" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I1218" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="J1218">
+        <v>21</v>
+      </c>
+      <c r="K1218" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1218" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y1218" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z1218" t="str">
+        <f t="shared" si="12"/>
+        <v>A2-6RT-A5</v>
+      </c>
+      <c r="AC1218" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="1219" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1219">
+        <v>6</v>
+      </c>
+      <c r="C1219" t="s">
+        <v>59</v>
+      </c>
+      <c r="G1219" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I1219" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="J1219">
+        <v>21</v>
+      </c>
+      <c r="K1219" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1219" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y1219" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z1219" t="str">
+        <f t="shared" si="12"/>
+        <v>A2-6RT-A6</v>
+      </c>
+      <c r="AC1219" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="1220" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1220">
+        <v>7</v>
+      </c>
+      <c r="C1220" t="s">
+        <v>59</v>
+      </c>
+      <c r="G1220" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I1220" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="J1220">
+        <v>21</v>
+      </c>
+      <c r="K1220" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1220" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y1220" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z1220" t="str">
+        <f t="shared" si="12"/>
+        <v>A2-6RT-A7</v>
+      </c>
+      <c r="AC1220" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="1221" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1221">
+        <v>8</v>
+      </c>
+      <c r="C1221" t="s">
+        <v>59</v>
+      </c>
+      <c r="G1221" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I1221" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="J1221">
+        <v>21</v>
+      </c>
+      <c r="K1221" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1221" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y1221" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z1221" t="str">
+        <f t="shared" si="12"/>
+        <v>A2-6RT-A8</v>
+      </c>
+      <c r="AC1221" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="1222" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1222">
+        <v>1</v>
+      </c>
+      <c r="C1222" t="s">
+        <v>59</v>
+      </c>
+      <c r="G1222" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I1222" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="J1222">
+        <v>21</v>
+      </c>
+      <c r="K1222" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1222" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y1222" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z1222" t="str">
+        <f>"A2-6"&amp;Y1222&amp;"-"&amp;AC1222</f>
+        <v>A2-6SO-A1</v>
+      </c>
+      <c r="AC1222" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="1223" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1223">
+        <v>2</v>
+      </c>
+      <c r="C1223" t="s">
+        <v>59</v>
+      </c>
+      <c r="G1223" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I1223" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="J1223">
+        <v>21</v>
+      </c>
+      <c r="K1223" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1223" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y1223" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z1223" t="str">
+        <f t="shared" si="12"/>
+        <v>A2-6SO-A2</v>
+      </c>
+      <c r="AC1223" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="1224" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1224">
+        <v>3</v>
+      </c>
+      <c r="C1224" t="s">
+        <v>59</v>
+      </c>
+      <c r="G1224" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I1224" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="J1224">
+        <v>21</v>
+      </c>
+      <c r="K1224" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1224" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y1224" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z1224" t="str">
+        <f t="shared" si="12"/>
+        <v>A2-6SO-A3</v>
+      </c>
+      <c r="AC1224" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="1225" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1225">
+        <v>4</v>
+      </c>
+      <c r="C1225" t="s">
+        <v>59</v>
+      </c>
+      <c r="G1225" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I1225" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="J1225">
+        <v>21</v>
+      </c>
+      <c r="K1225" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1225" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y1225" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z1225" t="str">
+        <f t="shared" si="12"/>
+        <v>A2-6SO-A4</v>
+      </c>
+      <c r="AC1225" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="1226" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1226">
+        <v>5</v>
+      </c>
+      <c r="C1226" t="s">
+        <v>59</v>
+      </c>
+      <c r="G1226" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I1226" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="J1226">
+        <v>21</v>
+      </c>
+      <c r="K1226" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1226" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y1226" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z1226" t="str">
+        <f t="shared" si="12"/>
+        <v>A2-6SO-A5</v>
+      </c>
+      <c r="AC1226" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="1227" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1227">
+        <v>6</v>
+      </c>
+      <c r="C1227" t="s">
+        <v>59</v>
+      </c>
+      <c r="G1227" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I1227" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="J1227">
+        <v>21</v>
+      </c>
+      <c r="K1227" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1227" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y1227" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z1227" t="str">
+        <f t="shared" si="12"/>
+        <v>A2-6SO-A6</v>
+      </c>
+      <c r="AC1227" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="1228" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1228">
+        <v>7</v>
+      </c>
+      <c r="C1228" t="s">
+        <v>59</v>
+      </c>
+      <c r="G1228" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I1228" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="J1228">
+        <v>21</v>
+      </c>
+      <c r="K1228" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1228" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y1228" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z1228" t="str">
+        <f t="shared" si="12"/>
+        <v>A2-6SO-A7</v>
+      </c>
+      <c r="AC1228" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="1229" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1229">
+        <v>8</v>
+      </c>
+      <c r="C1229" t="s">
+        <v>59</v>
+      </c>
+      <c r="G1229" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I1229" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="J1229">
+        <v>21</v>
+      </c>
+      <c r="K1229" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1229" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y1229" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z1229" t="str">
+        <f t="shared" si="12"/>
+        <v>A2-6SO-A8</v>
+      </c>
+      <c r="AC1229" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="1230" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1230">
+        <v>8</v>
+      </c>
+      <c r="C1230" t="s">
+        <v>60</v>
+      </c>
+      <c r="G1230" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I1230" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="J1230">
+        <v>21</v>
+      </c>
+      <c r="K1230" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1230" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y1230" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z1230" t="s">
+        <v>903</v>
+      </c>
+    </row>
+    <row r="1231" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1231">
+        <v>9</v>
+      </c>
+      <c r="C1231" t="s">
+        <v>60</v>
+      </c>
+      <c r="G1231" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I1231" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="J1231">
+        <v>21</v>
+      </c>
+      <c r="K1231" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1231" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y1231" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z1231" t="str">
+        <f>"A2-6"&amp;Y1231&amp;"-"&amp;AC1231</f>
+        <v>A2-6RT-A9</v>
+      </c>
+      <c r="AC1231" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1232" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1232">
+        <v>10</v>
+      </c>
+      <c r="C1232" t="s">
+        <v>60</v>
+      </c>
+      <c r="G1232" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I1232" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="J1232">
+        <v>21</v>
+      </c>
+      <c r="K1232" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1232" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y1232" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z1232" t="str">
+        <f>"A2-6"&amp;Y1232&amp;"-"&amp;AC1232</f>
+        <v>A2-6RT-A10</v>
+      </c>
+      <c r="AC1232" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="1233" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1233">
+        <v>11</v>
+      </c>
+      <c r="C1233" t="s">
+        <v>60</v>
+      </c>
+      <c r="G1233" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I1233" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="J1233">
+        <v>21</v>
+      </c>
+      <c r="K1233" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1233" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y1233" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z1233" t="str">
+        <f>"A2-6"&amp;Y1233&amp;"-"&amp;AC1233</f>
+        <v>A2-6RT-A11</v>
+      </c>
+      <c r="AC1233" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="1234" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1234">
+        <v>9</v>
+      </c>
+      <c r="C1234" t="s">
+        <v>60</v>
+      </c>
+      <c r="G1234" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I1234" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="J1234">
+        <v>21</v>
+      </c>
+      <c r="K1234" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1234" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y1234" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z1234" t="str">
+        <f t="shared" ref="Z1234:Z1240" si="13">"A2-6"&amp;Y1234&amp;"-"&amp;AC1234</f>
+        <v>A2-6SO-A9</v>
+      </c>
+      <c r="AC1234" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1235" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1235">
+        <v>10</v>
+      </c>
+      <c r="C1235" t="s">
+        <v>60</v>
+      </c>
+      <c r="G1235" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I1235" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="J1235">
+        <v>21</v>
+      </c>
+      <c r="K1235" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1235" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y1235" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z1235" t="str">
+        <f t="shared" si="13"/>
+        <v>A2-6SO-A10</v>
+      </c>
+      <c r="AC1235" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="1236" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1236">
+        <v>11</v>
+      </c>
+      <c r="C1236" t="s">
+        <v>60</v>
+      </c>
+      <c r="G1236" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I1236" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="J1236">
+        <v>21</v>
+      </c>
+      <c r="K1236" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1236" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y1236" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z1236" t="str">
+        <f t="shared" si="13"/>
+        <v>A2-6SO-A11</v>
+      </c>
+      <c r="AC1236" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="1237" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1237">
+        <v>12</v>
+      </c>
+      <c r="C1237" t="s">
+        <v>202</v>
+      </c>
+      <c r="G1237" s="1" t="s">
+        <v>679</v>
+      </c>
+      <c r="I1237" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="J1237">
+        <v>6</v>
+      </c>
+      <c r="K1237" t="s">
+        <v>203</v>
+      </c>
+      <c r="T1237" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y1237" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z1237" t="str">
+        <f t="shared" si="13"/>
+        <v>A2-6RT-B1</v>
+      </c>
+      <c r="AC1237" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="1238" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1238">
+        <v>13</v>
+      </c>
+      <c r="C1238" t="s">
+        <v>202</v>
+      </c>
+      <c r="G1238" s="1" t="s">
+        <v>679</v>
+      </c>
+      <c r="I1238" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="J1238">
+        <v>6</v>
+      </c>
+      <c r="K1238" t="s">
+        <v>203</v>
+      </c>
+      <c r="T1238" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y1238" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z1238" t="str">
+        <f t="shared" si="13"/>
+        <v>A2-6RT-B2</v>
+      </c>
+      <c r="AC1238" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="1239" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1239">
+        <v>12</v>
+      </c>
+      <c r="C1239" t="s">
+        <v>202</v>
+      </c>
+      <c r="G1239" s="1" t="s">
+        <v>679</v>
+      </c>
+      <c r="I1239" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="J1239">
+        <v>6</v>
+      </c>
+      <c r="K1239" t="s">
+        <v>203</v>
+      </c>
+      <c r="T1239" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y1239" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z1239" t="str">
+        <f t="shared" si="13"/>
+        <v>A2-6SO-B1</v>
+      </c>
+      <c r="AC1239" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="1240" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1240">
+        <v>13</v>
+      </c>
+      <c r="C1240" t="s">
+        <v>202</v>
+      </c>
+      <c r="G1240" s="1" t="s">
+        <v>679</v>
+      </c>
+      <c r="I1240" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="J1240">
+        <v>6</v>
+      </c>
+      <c r="K1240" t="s">
+        <v>203</v>
+      </c>
+      <c r="T1240" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y1240" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z1240" t="str">
+        <f t="shared" si="13"/>
+        <v>A2-6SO-B2</v>
+      </c>
+      <c r="AC1240" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="1241" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1241">
+        <v>9</v>
+      </c>
+      <c r="C1241" t="s">
+        <v>60</v>
+      </c>
+      <c r="G1241" s="1" t="s">
+        <v>679</v>
+      </c>
+      <c r="I1241" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="J1241">
+        <v>6</v>
+      </c>
+      <c r="K1241" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1241" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y1241" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z1241" t="s">
+        <v>904</v>
+      </c>
+    </row>
+    <row r="1242" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1242">
+        <v>14</v>
+      </c>
+      <c r="C1242" t="s">
+        <v>60</v>
+      </c>
+      <c r="G1242" s="1" t="s">
+        <v>679</v>
+      </c>
+      <c r="I1242" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="J1242">
+        <v>6</v>
+      </c>
+      <c r="K1242" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1242" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y1242" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z1242" t="str">
+        <f>"A2-6"&amp;Y1242&amp;"-"&amp;AC1242</f>
+        <v>A2-6RT-C1</v>
+      </c>
+      <c r="AC1242" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="1243" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1243">
+        <v>15</v>
+      </c>
+      <c r="C1243" t="s">
+        <v>60</v>
+      </c>
+      <c r="G1243" s="1" t="s">
+        <v>679</v>
+      </c>
+      <c r="I1243" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="J1243">
+        <v>6</v>
+      </c>
+      <c r="K1243" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1243" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y1243" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z1243" t="str">
+        <f>"A2-6"&amp;Y1243&amp;"-"&amp;AC1243</f>
+        <v>A2-6RT-C2</v>
+      </c>
+      <c r="AC1243" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="1244" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1244">
+        <v>16</v>
+      </c>
+      <c r="C1244" t="s">
+        <v>60</v>
+      </c>
+      <c r="G1244" s="1" t="s">
+        <v>679</v>
+      </c>
+      <c r="I1244" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="J1244">
+        <v>6</v>
+      </c>
+      <c r="K1244" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1244" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y1244" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z1244" t="str">
+        <f t="shared" ref="Z1244:Z1247" si="14">"A2-6"&amp;Y1244&amp;"-"&amp;AC1244</f>
+        <v>A2-6RT-C3</v>
+      </c>
+      <c r="AC1244" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="1245" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1245">
+        <v>14</v>
+      </c>
+      <c r="C1245" t="s">
+        <v>60</v>
+      </c>
+      <c r="G1245" s="1" t="s">
+        <v>679</v>
+      </c>
+      <c r="I1245" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="J1245">
+        <v>6</v>
+      </c>
+      <c r="K1245" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1245" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y1245" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z1245" t="str">
+        <f t="shared" si="14"/>
+        <v>A2-6SO-C1</v>
+      </c>
+      <c r="AC1245" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="1246" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1246">
+        <v>15</v>
+      </c>
+      <c r="C1246" t="s">
+        <v>60</v>
+      </c>
+      <c r="G1246" s="1" t="s">
+        <v>679</v>
+      </c>
+      <c r="I1246" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="J1246">
+        <v>6</v>
+      </c>
+      <c r="K1246" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1246" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y1246" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z1246" t="str">
+        <f t="shared" si="14"/>
+        <v>A2-6SO-C2</v>
+      </c>
+      <c r="AC1246" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="1247" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1247">
+        <v>16</v>
+      </c>
+      <c r="C1247" t="s">
+        <v>60</v>
+      </c>
+      <c r="G1247" s="1" t="s">
+        <v>679</v>
+      </c>
+      <c r="I1247" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="J1247">
+        <v>6</v>
+      </c>
+      <c r="K1247" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1247" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y1247" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z1247" t="str">
+        <f t="shared" si="14"/>
+        <v>A2-6SO-C3</v>
+      </c>
+      <c r="AC1247" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="1248" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1248">
+        <v>10</v>
+      </c>
+      <c r="C1248" t="s">
+        <v>202</v>
+      </c>
+      <c r="G1248" s="1" t="s">
+        <v>679</v>
+      </c>
+      <c r="I1248" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="J1248">
+        <v>6</v>
+      </c>
+      <c r="K1248" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1248" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y1248" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z1248" t="s">
+        <v>905</v>
+      </c>
+    </row>
+    <row r="1249" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1249">
+        <v>11</v>
+      </c>
+      <c r="C1249" t="s">
+        <v>202</v>
+      </c>
+      <c r="G1249" s="1" t="s">
+        <v>679</v>
+      </c>
+      <c r="I1249" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="J1249">
+        <v>6</v>
+      </c>
+      <c r="K1249" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1249" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y1249" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z1249" t="s">
+        <v>906</v>
+      </c>
+    </row>
+    <row r="1250" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1250">
+        <v>12</v>
+      </c>
+      <c r="C1250" t="s">
+        <v>202</v>
+      </c>
+      <c r="G1250" s="1" t="s">
+        <v>679</v>
+      </c>
+      <c r="I1250" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="J1250">
+        <v>6</v>
+      </c>
+      <c r="K1250" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1250" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y1250" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z1250" t="s">
+        <v>907</v>
+      </c>
+    </row>
+    <row r="1251" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1251">
+        <v>13</v>
+      </c>
+      <c r="C1251" t="s">
+        <v>202</v>
+      </c>
+      <c r="G1251" s="1" t="s">
+        <v>679</v>
+      </c>
+      <c r="I1251" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="J1251">
+        <v>6</v>
+      </c>
+      <c r="K1251" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1251" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y1251" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z1251" t="s">
+        <v>908</v>
+      </c>
+    </row>
+    <row r="1252" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1252">
+        <v>14</v>
+      </c>
+      <c r="C1252" t="s">
+        <v>202</v>
+      </c>
+      <c r="G1252" s="1" t="s">
+        <v>679</v>
+      </c>
+      <c r="I1252" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="J1252">
+        <v>6</v>
+      </c>
+      <c r="K1252" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1252" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y1252" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z1252" t="s">
+        <v>909</v>
+      </c>
+    </row>
+    <row r="1253" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1253">
+        <v>15</v>
+      </c>
+      <c r="C1253" t="s">
+        <v>202</v>
+      </c>
+      <c r="G1253" s="1" t="s">
+        <v>679</v>
+      </c>
+      <c r="I1253" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="J1253">
+        <v>6</v>
+      </c>
+      <c r="K1253" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1253" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y1253" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z1253" t="s">
+        <v>910</v>
+      </c>
+    </row>
+    <row r="1254" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1254">
+        <v>16</v>
+      </c>
+      <c r="C1254" t="s">
+        <v>202</v>
+      </c>
+      <c r="G1254" s="1" t="s">
+        <v>679</v>
+      </c>
+      <c r="I1254" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="J1254">
+        <v>6</v>
+      </c>
+      <c r="K1254" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1254" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y1254" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z1254" t="s">
+        <v>911</v>
+      </c>
+    </row>
+    <row r="1255" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1255">
+        <v>17</v>
+      </c>
+      <c r="C1255" t="s">
+        <v>202</v>
+      </c>
+      <c r="G1255" s="1" t="s">
+        <v>679</v>
+      </c>
+      <c r="I1255" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="J1255">
+        <v>6</v>
+      </c>
+      <c r="K1255" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1255" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y1255" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z1255" t="s">
+        <v>912</v>
+      </c>
+    </row>
+    <row r="1256" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1256">
+        <v>17</v>
+      </c>
+      <c r="C1256" t="s">
+        <v>202</v>
+      </c>
+      <c r="G1256" s="1" t="s">
+        <v>679</v>
+      </c>
+      <c r="I1256" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="J1256">
+        <v>6</v>
+      </c>
+      <c r="K1256" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1256" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y1256" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z1256" t="str">
+        <f>"A2-6"&amp;Y1256&amp;"-"&amp;AC1256</f>
+        <v>A2-6RT-E1</v>
+      </c>
+      <c r="AC1256" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="1257" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1257">
+        <v>18</v>
+      </c>
+      <c r="C1257" t="s">
+        <v>202</v>
+      </c>
+      <c r="G1257" s="1" t="s">
+        <v>679</v>
+      </c>
+      <c r="I1257" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="J1257">
+        <v>6</v>
+      </c>
+      <c r="K1257" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1257" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y1257" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z1257" t="str">
+        <f t="shared" ref="Z1257:Z1275" si="15">"A2-6"&amp;Y1257&amp;"-"&amp;AC1257</f>
+        <v>A2-6RT-E2</v>
+      </c>
+      <c r="AC1257" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="1258" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1258">
+        <v>19</v>
+      </c>
+      <c r="C1258" t="s">
+        <v>202</v>
+      </c>
+      <c r="G1258" s="1" t="s">
+        <v>679</v>
+      </c>
+      <c r="I1258" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="J1258">
+        <v>6</v>
+      </c>
+      <c r="K1258" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1258" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y1258" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z1258" t="str">
+        <f t="shared" si="15"/>
+        <v>A2-6RT-E3</v>
+      </c>
+      <c r="AC1258" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="1259" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1259">
+        <v>20</v>
+      </c>
+      <c r="C1259" t="s">
+        <v>202</v>
+      </c>
+      <c r="G1259" s="1" t="s">
+        <v>679</v>
+      </c>
+      <c r="I1259" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="J1259">
+        <v>6</v>
+      </c>
+      <c r="K1259" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1259" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y1259" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z1259" t="str">
+        <f t="shared" si="15"/>
+        <v>A2-6RT-E4</v>
+      </c>
+      <c r="AC1259" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="1260" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1260">
+        <v>21</v>
+      </c>
+      <c r="C1260" t="s">
+        <v>202</v>
+      </c>
+      <c r="G1260" s="1" t="s">
+        <v>679</v>
+      </c>
+      <c r="I1260" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="J1260">
+        <v>6</v>
+      </c>
+      <c r="K1260" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1260" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y1260" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z1260" t="str">
+        <f t="shared" si="15"/>
+        <v>A2-6RT-E5</v>
+      </c>
+      <c r="AC1260" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="1261" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1261">
+        <v>22</v>
+      </c>
+      <c r="C1261" t="s">
+        <v>202</v>
+      </c>
+      <c r="G1261" s="1" t="s">
+        <v>679</v>
+      </c>
+      <c r="I1261" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="J1261">
+        <v>6</v>
+      </c>
+      <c r="K1261" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1261" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y1261" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z1261" t="str">
+        <f t="shared" si="15"/>
+        <v>A2-6RT-E6</v>
+      </c>
+      <c r="AC1261" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="1262" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1262">
+        <v>23</v>
+      </c>
+      <c r="C1262" t="s">
+        <v>202</v>
+      </c>
+      <c r="G1262" s="1" t="s">
+        <v>679</v>
+      </c>
+      <c r="I1262" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="J1262">
+        <v>6</v>
+      </c>
+      <c r="K1262" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1262" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y1262" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z1262" t="str">
+        <f t="shared" si="15"/>
+        <v>A2-6RT-E7</v>
+      </c>
+      <c r="AC1262" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="1263" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1263">
+        <v>24</v>
+      </c>
+      <c r="C1263" t="s">
+        <v>202</v>
+      </c>
+      <c r="G1263" s="1" t="s">
+        <v>679</v>
+      </c>
+      <c r="I1263" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="J1263">
+        <v>6</v>
+      </c>
+      <c r="K1263" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1263" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y1263" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z1263" t="str">
+        <f t="shared" si="15"/>
+        <v>A2-6RT-E8</v>
+      </c>
+      <c r="AC1263" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="1264" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1264">
+        <v>25</v>
+      </c>
+      <c r="C1264" t="s">
+        <v>202</v>
+      </c>
+      <c r="G1264" s="1" t="s">
+        <v>679</v>
+      </c>
+      <c r="I1264" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="J1264">
+        <v>6</v>
+      </c>
+      <c r="K1264" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1264" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y1264" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z1264" t="str">
+        <f t="shared" si="15"/>
+        <v>A2-6RT-E9</v>
+      </c>
+      <c r="AC1264" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="1265" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1265">
+        <v>26</v>
+      </c>
+      <c r="C1265" t="s">
+        <v>202</v>
+      </c>
+      <c r="G1265" s="1" t="s">
+        <v>679</v>
+      </c>
+      <c r="I1265" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="J1265">
+        <v>6</v>
+      </c>
+      <c r="K1265" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1265" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y1265" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z1265" t="str">
+        <f t="shared" si="15"/>
+        <v>A2-6RT-E10</v>
+      </c>
+      <c r="AC1265" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="1266" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1266">
+        <v>18</v>
+      </c>
+      <c r="C1266" t="s">
+        <v>202</v>
+      </c>
+      <c r="G1266" s="1" t="s">
+        <v>679</v>
+      </c>
+      <c r="I1266" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="J1266">
+        <v>6</v>
+      </c>
+      <c r="K1266" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1266" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y1266" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z1266" t="str">
+        <f t="shared" si="15"/>
+        <v>A2-6SO-E1</v>
+      </c>
+      <c r="AC1266" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="1267" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1267">
+        <v>19</v>
+      </c>
+      <c r="C1267" t="s">
+        <v>202</v>
+      </c>
+      <c r="G1267" s="1" t="s">
+        <v>679</v>
+      </c>
+      <c r="I1267" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="J1267">
+        <v>6</v>
+      </c>
+      <c r="K1267" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1267" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y1267" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z1267" t="str">
+        <f t="shared" si="15"/>
+        <v>A2-6SO-E2</v>
+      </c>
+      <c r="AC1267" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="1268" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1268">
+        <v>20</v>
+      </c>
+      <c r="C1268" t="s">
+        <v>202</v>
+      </c>
+      <c r="G1268" s="1" t="s">
+        <v>679</v>
+      </c>
+      <c r="I1268" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="J1268">
+        <v>6</v>
+      </c>
+      <c r="K1268" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1268" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y1268" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z1268" t="str">
+        <f t="shared" si="15"/>
+        <v>A2-6SO-E3</v>
+      </c>
+      <c r="AC1268" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="1269" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1269">
+        <v>21</v>
+      </c>
+      <c r="C1269" t="s">
+        <v>202</v>
+      </c>
+      <c r="G1269" s="1" t="s">
+        <v>679</v>
+      </c>
+      <c r="I1269" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="J1269">
+        <v>6</v>
+      </c>
+      <c r="K1269" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1269" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y1269" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z1269" t="str">
+        <f t="shared" si="15"/>
+        <v>A2-6SO-E4</v>
+      </c>
+      <c r="AC1269" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="1270" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1270">
+        <v>22</v>
+      </c>
+      <c r="C1270" t="s">
+        <v>202</v>
+      </c>
+      <c r="G1270" s="1" t="s">
+        <v>679</v>
+      </c>
+      <c r="I1270" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="J1270">
+        <v>6</v>
+      </c>
+      <c r="K1270" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1270" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y1270" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z1270" t="str">
+        <f t="shared" si="15"/>
+        <v>A2-6SO-E5</v>
+      </c>
+      <c r="AC1270" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="1271" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1271">
+        <v>23</v>
+      </c>
+      <c r="C1271" t="s">
+        <v>202</v>
+      </c>
+      <c r="G1271" s="1" t="s">
+        <v>679</v>
+      </c>
+      <c r="I1271" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="J1271">
+        <v>6</v>
+      </c>
+      <c r="K1271" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1271" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y1271" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z1271" t="str">
+        <f t="shared" si="15"/>
+        <v>A2-6SO-E6</v>
+      </c>
+      <c r="AC1271" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="1272" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1272">
+        <v>24</v>
+      </c>
+      <c r="C1272" t="s">
+        <v>202</v>
+      </c>
+      <c r="G1272" s="1" t="s">
+        <v>679</v>
+      </c>
+      <c r="I1272" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="J1272">
+        <v>6</v>
+      </c>
+      <c r="K1272" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1272" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y1272" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z1272" t="str">
+        <f t="shared" si="15"/>
+        <v>A2-6SO-E7</v>
+      </c>
+      <c r="AC1272" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="1273" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1273">
+        <v>25</v>
+      </c>
+      <c r="C1273" t="s">
+        <v>202</v>
+      </c>
+      <c r="G1273" s="1" t="s">
+        <v>679</v>
+      </c>
+      <c r="I1273" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="J1273">
+        <v>6</v>
+      </c>
+      <c r="K1273" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1273" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y1273" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z1273" t="str">
+        <f t="shared" si="15"/>
+        <v>A2-6SO-E8</v>
+      </c>
+      <c r="AC1273" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="1274" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1274">
+        <v>26</v>
+      </c>
+      <c r="C1274" t="s">
+        <v>202</v>
+      </c>
+      <c r="G1274" s="1" t="s">
+        <v>679</v>
+      </c>
+      <c r="I1274" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="J1274">
+        <v>6</v>
+      </c>
+      <c r="K1274" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1274" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y1274" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z1274" t="str">
+        <f t="shared" si="15"/>
+        <v>A2-6SO-E9</v>
+      </c>
+      <c r="AC1274" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="1275" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1275">
+        <v>27</v>
+      </c>
+      <c r="C1275" t="s">
+        <v>202</v>
+      </c>
+      <c r="G1275" s="1" t="s">
+        <v>679</v>
+      </c>
+      <c r="I1275" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="J1275">
+        <v>6</v>
+      </c>
+      <c r="K1275" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1275" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y1275" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z1275" t="str">
+        <f t="shared" si="15"/>
+        <v>A2-6SO-E10</v>
+      </c>
+      <c r="AC1275" t="s">
+        <v>249</v>
       </c>
     </row>
   </sheetData>
@@ -57474,8 +60526,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD836908-61FC-4C6A-BB55-EB17A2B99FDD}">
   <dimension ref="A1:M65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="M54" sqref="M54"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="I51" sqref="I51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
ENTERING DATa for cohort day 11 + 26 2081-09-10
</commit_message>
<xml_diff>
--- a/Data/2018-08-14_master_datac_2018_collection_year.xlsx
+++ b/Data/2018-08-14_master_datac_2018_collection_year.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andrew.nguyen\Desktop\Circadian_rhythm_runs_seasonal_timing\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E674E713-AD1D-4C39-A3CC-3AE7ABD7D033}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F387795C-743D-4F38-B26F-8AF3243BD0CA}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="52065" yWindow="465" windowWidth="36360" windowHeight="21135" activeTab="1" xr2:uid="{C7477166-8A7C-B04A-9643-C277FEDCDAAB}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12699" uniqueCount="913">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12793" uniqueCount="917">
   <si>
     <t>Ind_ID</t>
   </si>
@@ -2771,6 +2771,18 @@
   </si>
   <si>
     <t>A2-10-17</t>
+  </si>
+  <si>
+    <t>15:43</t>
+  </si>
+  <si>
+    <t>14:53</t>
+  </si>
+  <si>
+    <t>15:31</t>
+  </si>
+  <si>
+    <t>15:42</t>
   </si>
 </sst>
 </file>
@@ -13663,9 +13675,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92725FB9-1A17-2546-9DFA-6C0D39437891}">
   <dimension ref="A1:AS1369"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1333" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T1276" sqref="T1276:T1369"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A1185" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D1355" sqref="D1355"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -59278,7 +59290,7 @@
         <v>202</v>
       </c>
       <c r="G1237" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1237" s="1" t="s">
         <v>68</v>
@@ -59311,7 +59323,7 @@
         <v>202</v>
       </c>
       <c r="G1238" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1238" s="1" t="s">
         <v>68</v>
@@ -59344,7 +59356,7 @@
         <v>202</v>
       </c>
       <c r="G1239" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1239" s="1" t="s">
         <v>68</v>
@@ -59377,7 +59389,7 @@
         <v>202</v>
       </c>
       <c r="G1240" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1240" s="1" t="s">
         <v>68</v>
@@ -59410,7 +59422,7 @@
         <v>60</v>
       </c>
       <c r="G1241" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1241" s="1" t="s">
         <v>68</v>
@@ -59439,7 +59451,7 @@
         <v>60</v>
       </c>
       <c r="G1242" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1242" s="1" t="s">
         <v>68</v>
@@ -59472,7 +59484,7 @@
         <v>60</v>
       </c>
       <c r="G1243" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1243" s="1" t="s">
         <v>68</v>
@@ -59505,7 +59517,7 @@
         <v>60</v>
       </c>
       <c r="G1244" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1244" s="1" t="s">
         <v>68</v>
@@ -59538,7 +59550,7 @@
         <v>60</v>
       </c>
       <c r="G1245" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1245" s="1" t="s">
         <v>68</v>
@@ -59571,7 +59583,7 @@
         <v>60</v>
       </c>
       <c r="G1246" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1246" s="1" t="s">
         <v>68</v>
@@ -59604,7 +59616,7 @@
         <v>60</v>
       </c>
       <c r="G1247" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1247" s="1" t="s">
         <v>68</v>
@@ -59637,7 +59649,7 @@
         <v>202</v>
       </c>
       <c r="G1248" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1248" s="1" t="s">
         <v>68</v>
@@ -59666,7 +59678,7 @@
         <v>202</v>
       </c>
       <c r="G1249" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1249" s="1" t="s">
         <v>68</v>
@@ -59695,7 +59707,7 @@
         <v>202</v>
       </c>
       <c r="G1250" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1250" s="1" t="s">
         <v>68</v>
@@ -59724,7 +59736,7 @@
         <v>202</v>
       </c>
       <c r="G1251" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1251" s="1" t="s">
         <v>68</v>
@@ -59753,7 +59765,7 @@
         <v>202</v>
       </c>
       <c r="G1252" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1252" s="1" t="s">
         <v>68</v>
@@ -59782,7 +59794,7 @@
         <v>202</v>
       </c>
       <c r="G1253" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1253" s="1" t="s">
         <v>68</v>
@@ -59811,7 +59823,7 @@
         <v>202</v>
       </c>
       <c r="G1254" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1254" s="1" t="s">
         <v>68</v>
@@ -59840,7 +59852,7 @@
         <v>202</v>
       </c>
       <c r="G1255" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1255" s="1" t="s">
         <v>68</v>
@@ -59869,7 +59881,7 @@
         <v>202</v>
       </c>
       <c r="G1256" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1256" s="1" t="s">
         <v>68</v>
@@ -59902,7 +59914,7 @@
         <v>202</v>
       </c>
       <c r="G1257" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1257" s="1" t="s">
         <v>68</v>
@@ -59935,7 +59947,7 @@
         <v>202</v>
       </c>
       <c r="G1258" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1258" s="1" t="s">
         <v>68</v>
@@ -59968,7 +59980,7 @@
         <v>202</v>
       </c>
       <c r="G1259" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1259" s="1" t="s">
         <v>68</v>
@@ -60001,7 +60013,7 @@
         <v>202</v>
       </c>
       <c r="G1260" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1260" s="1" t="s">
         <v>68</v>
@@ -60034,7 +60046,7 @@
         <v>202</v>
       </c>
       <c r="G1261" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1261" s="1" t="s">
         <v>68</v>
@@ -60067,7 +60079,7 @@
         <v>202</v>
       </c>
       <c r="G1262" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1262" s="1" t="s">
         <v>68</v>
@@ -60100,7 +60112,7 @@
         <v>202</v>
       </c>
       <c r="G1263" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1263" s="1" t="s">
         <v>68</v>
@@ -60133,7 +60145,7 @@
         <v>202</v>
       </c>
       <c r="G1264" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1264" s="1" t="s">
         <v>68</v>
@@ -60166,7 +60178,7 @@
         <v>202</v>
       </c>
       <c r="G1265" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1265" s="1" t="s">
         <v>68</v>
@@ -60199,7 +60211,7 @@
         <v>202</v>
       </c>
       <c r="G1266" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1266" s="1" t="s">
         <v>68</v>
@@ -60232,7 +60244,7 @@
         <v>202</v>
       </c>
       <c r="G1267" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1267" s="1" t="s">
         <v>68</v>
@@ -60265,7 +60277,7 @@
         <v>202</v>
       </c>
       <c r="G1268" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1268" s="1" t="s">
         <v>68</v>
@@ -60298,7 +60310,7 @@
         <v>202</v>
       </c>
       <c r="G1269" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1269" s="1" t="s">
         <v>68</v>
@@ -60331,7 +60343,7 @@
         <v>202</v>
       </c>
       <c r="G1270" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1270" s="1" t="s">
         <v>68</v>
@@ -60364,7 +60376,7 @@
         <v>202</v>
       </c>
       <c r="G1271" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1271" s="1" t="s">
         <v>68</v>
@@ -60397,7 +60409,7 @@
         <v>202</v>
       </c>
       <c r="G1272" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1272" s="1" t="s">
         <v>68</v>
@@ -60430,7 +60442,7 @@
         <v>202</v>
       </c>
       <c r="G1273" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1273" s="1" t="s">
         <v>68</v>
@@ -60463,7 +60475,7 @@
         <v>202</v>
       </c>
       <c r="G1274" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1274" s="1" t="s">
         <v>68</v>
@@ -60496,7 +60508,7 @@
         <v>202</v>
       </c>
       <c r="G1275" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1275" s="1" t="s">
         <v>68</v>
@@ -60528,8 +60540,17 @@
       <c r="B1276" t="s">
         <v>230</v>
       </c>
+      <c r="C1276" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1276">
+        <v>6.7160000000000002</v>
+      </c>
+      <c r="E1276" s="1" t="s">
+        <v>913</v>
+      </c>
       <c r="G1276" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1276" s="1" t="s">
         <v>73</v>
@@ -60551,8 +60572,14 @@
       <c r="B1277" t="s">
         <v>230</v>
       </c>
+      <c r="C1277" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1277">
+        <v>7.7240000000000002</v>
+      </c>
       <c r="G1277" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1277" s="1" t="s">
         <v>73</v>
@@ -60574,8 +60601,14 @@
       <c r="B1278" t="s">
         <v>230</v>
       </c>
+      <c r="C1278" t="s">
+        <v>202</v>
+      </c>
+      <c r="D1278">
+        <v>9.0850000000000009</v>
+      </c>
       <c r="G1278" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1278" s="1" t="s">
         <v>73</v>
@@ -60597,8 +60630,14 @@
       <c r="B1279" t="s">
         <v>230</v>
       </c>
+      <c r="C1279" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1279">
+        <v>4.13</v>
+      </c>
       <c r="G1279" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1279" s="1" t="s">
         <v>73</v>
@@ -60620,14 +60659,20 @@
       <c r="B1280" t="s">
         <v>230</v>
       </c>
+      <c r="C1280" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1280">
+        <v>3.9710000000000001</v>
+      </c>
       <c r="G1280" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1280" s="1" t="s">
         <v>73</v>
       </c>
       <c r="J1280">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="K1280" t="s">
         <v>61</v>
@@ -60643,8 +60688,14 @@
       <c r="B1281" t="s">
         <v>230</v>
       </c>
+      <c r="C1281" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1281">
+        <v>5.95</v>
+      </c>
       <c r="G1281" s="1" t="s">
-        <v>679</v>
+        <v>88</v>
       </c>
       <c r="I1281" s="1" t="s">
         <v>73</v>
@@ -60666,8 +60717,14 @@
       <c r="B1282" t="s">
         <v>230</v>
       </c>
+      <c r="C1282" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1282">
+        <v>5.3639999999999999</v>
+      </c>
       <c r="G1282" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1282" s="1" t="s">
         <v>73</v>
@@ -60689,8 +60746,14 @@
       <c r="B1283" t="s">
         <v>230</v>
       </c>
+      <c r="C1283" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1283">
+        <v>4.3230000000000004</v>
+      </c>
       <c r="G1283" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1283" s="1" t="s">
         <v>73</v>
@@ -60712,8 +60775,14 @@
       <c r="B1284" t="s">
         <v>230</v>
       </c>
+      <c r="C1284" t="s">
+        <v>202</v>
+      </c>
+      <c r="D1284">
+        <v>9.5329999999999995</v>
+      </c>
       <c r="G1284" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1284" s="1" t="s">
         <v>73</v>
@@ -60735,8 +60804,14 @@
       <c r="B1285" t="s">
         <v>230</v>
       </c>
+      <c r="C1285" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1285">
+        <v>3.8</v>
+      </c>
       <c r="G1285" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1285" s="1" t="s">
         <v>73</v>
@@ -60758,8 +60833,14 @@
       <c r="B1286" t="s">
         <v>230</v>
       </c>
+      <c r="C1286" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1286">
+        <v>6.2489999999999997</v>
+      </c>
       <c r="G1286" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1286" s="1" t="s">
         <v>73</v>
@@ -60781,8 +60862,14 @@
       <c r="B1287" t="s">
         <v>230</v>
       </c>
+      <c r="C1287" t="s">
+        <v>202</v>
+      </c>
+      <c r="D1287">
+        <v>8.4640000000000004</v>
+      </c>
       <c r="G1287" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1287" s="1" t="s">
         <v>73</v>
@@ -60804,8 +60891,14 @@
       <c r="B1288" t="s">
         <v>230</v>
       </c>
+      <c r="C1288" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1288">
+        <v>6.0209999999999999</v>
+      </c>
       <c r="G1288" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1288" s="1" t="s">
         <v>73</v>
@@ -60827,8 +60920,14 @@
       <c r="B1289" t="s">
         <v>230</v>
       </c>
+      <c r="C1289" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1289">
+        <v>3.609</v>
+      </c>
       <c r="G1289" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1289" s="1" t="s">
         <v>73</v>
@@ -60850,8 +60949,14 @@
       <c r="B1290" t="s">
         <v>230</v>
       </c>
+      <c r="C1290" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1290">
+        <v>6.1059999999999999</v>
+      </c>
       <c r="G1290" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1290" s="1" t="s">
         <v>73</v>
@@ -60873,8 +60978,14 @@
       <c r="B1291" t="s">
         <v>230</v>
       </c>
+      <c r="C1291" t="s">
+        <v>202</v>
+      </c>
+      <c r="D1291">
+        <v>4.4729999999999999</v>
+      </c>
       <c r="G1291" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1291" s="1" t="s">
         <v>73</v>
@@ -60896,8 +61007,14 @@
       <c r="B1292" t="s">
         <v>230</v>
       </c>
+      <c r="C1292" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1292">
+        <v>4.4550000000000001</v>
+      </c>
       <c r="G1292" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1292" s="1" t="s">
         <v>73</v>
@@ -60919,8 +61036,14 @@
       <c r="B1293" t="s">
         <v>230</v>
       </c>
+      <c r="C1293" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1293">
+        <v>8.3889999999999993</v>
+      </c>
       <c r="G1293" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1293" s="1" t="s">
         <v>73</v>
@@ -60942,8 +61065,14 @@
       <c r="B1294" t="s">
         <v>230</v>
       </c>
+      <c r="C1294" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1294">
+        <v>5.899</v>
+      </c>
       <c r="G1294" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1294" s="1" t="s">
         <v>73</v>
@@ -60965,8 +61094,14 @@
       <c r="B1295" t="s">
         <v>230</v>
       </c>
+      <c r="C1295" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1295">
+        <v>6.7270000000000003</v>
+      </c>
       <c r="G1295" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1295" s="1" t="s">
         <v>73</v>
@@ -60988,8 +61123,14 @@
       <c r="B1296" t="s">
         <v>230</v>
       </c>
+      <c r="C1296" t="s">
+        <v>202</v>
+      </c>
+      <c r="D1296">
+        <v>6.3490000000000002</v>
+      </c>
       <c r="G1296" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1296" s="1" t="s">
         <v>73</v>
@@ -61011,8 +61152,14 @@
       <c r="B1297" t="s">
         <v>230</v>
       </c>
+      <c r="C1297" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1297">
+        <v>7.4909999999999997</v>
+      </c>
       <c r="G1297" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1297" s="1" t="s">
         <v>73</v>
@@ -61034,8 +61181,14 @@
       <c r="B1298" t="s">
         <v>230</v>
       </c>
+      <c r="C1298" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1298">
+        <v>6.1</v>
+      </c>
       <c r="G1298" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1298" s="1" t="s">
         <v>73</v>
@@ -61057,8 +61210,14 @@
       <c r="B1299" t="s">
         <v>230</v>
       </c>
+      <c r="C1299" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1299">
+        <v>5.4550000000000001</v>
+      </c>
       <c r="G1299" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1299" s="1" t="s">
         <v>73</v>
@@ -61080,8 +61239,14 @@
       <c r="B1300" t="s">
         <v>230</v>
       </c>
+      <c r="C1300" t="s">
+        <v>202</v>
+      </c>
+      <c r="D1300">
+        <v>4.0990000000000002</v>
+      </c>
       <c r="G1300" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1300" s="1" t="s">
         <v>73</v>
@@ -61103,8 +61268,14 @@
       <c r="B1301" t="s">
         <v>230</v>
       </c>
+      <c r="C1301" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1301">
+        <v>7.1120000000000001</v>
+      </c>
       <c r="G1301" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1301" s="1" t="s">
         <v>73</v>
@@ -61126,8 +61297,14 @@
       <c r="B1302" t="s">
         <v>230</v>
       </c>
+      <c r="C1302" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1302">
+        <v>6.2190000000000003</v>
+      </c>
       <c r="G1302" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1302" s="1" t="s">
         <v>73</v>
@@ -61149,8 +61326,14 @@
       <c r="B1303" t="s">
         <v>230</v>
       </c>
+      <c r="C1303" t="s">
+        <v>202</v>
+      </c>
+      <c r="D1303">
+        <v>6.2009999999999996</v>
+      </c>
       <c r="G1303" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1303" s="1" t="s">
         <v>73</v>
@@ -61172,8 +61355,14 @@
       <c r="B1304" t="s">
         <v>230</v>
       </c>
+      <c r="C1304" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1304">
+        <v>3.5619999999999998</v>
+      </c>
       <c r="G1304" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1304" s="1" t="s">
         <v>73</v>
@@ -61195,8 +61384,14 @@
       <c r="B1305" t="s">
         <v>230</v>
       </c>
+      <c r="C1305" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1305">
+        <v>8.8930000000000007</v>
+      </c>
       <c r="G1305" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1305" s="1" t="s">
         <v>73</v>
@@ -61218,8 +61413,14 @@
       <c r="B1306" t="s">
         <v>230</v>
       </c>
+      <c r="C1306" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1306">
+        <v>5.5910000000000002</v>
+      </c>
       <c r="G1306" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1306" s="1" t="s">
         <v>73</v>
@@ -61241,8 +61442,14 @@
       <c r="B1307" t="s">
         <v>230</v>
       </c>
+      <c r="C1307" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1307">
+        <v>6.0220000000000002</v>
+      </c>
       <c r="G1307" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1307" s="1" t="s">
         <v>73</v>
@@ -61264,8 +61471,14 @@
       <c r="B1308" t="s">
         <v>230</v>
       </c>
+      <c r="C1308" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1308">
+        <v>7.673</v>
+      </c>
       <c r="G1308" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1308" s="1" t="s">
         <v>73</v>
@@ -61287,8 +61500,14 @@
       <c r="B1309" t="s">
         <v>230</v>
       </c>
+      <c r="C1309" t="s">
+        <v>202</v>
+      </c>
+      <c r="D1309">
+        <v>5.13</v>
+      </c>
       <c r="G1309" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1309" s="1" t="s">
         <v>73</v>
@@ -61310,8 +61529,14 @@
       <c r="B1310" t="s">
         <v>230</v>
       </c>
+      <c r="C1310" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1310">
+        <v>4.7370000000000001</v>
+      </c>
       <c r="G1310" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1310" s="1" t="s">
         <v>73</v>
@@ -61333,8 +61558,14 @@
       <c r="B1311" t="s">
         <v>230</v>
       </c>
+      <c r="C1311" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1311">
+        <v>4.4433999999999996</v>
+      </c>
       <c r="G1311" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1311" s="1" t="s">
         <v>73</v>
@@ -61356,8 +61587,14 @@
       <c r="B1312" t="s">
         <v>230</v>
       </c>
+      <c r="C1312" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1312">
+        <v>5.7119999999999997</v>
+      </c>
       <c r="G1312" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1312" s="1" t="s">
         <v>73</v>
@@ -61379,8 +61616,14 @@
       <c r="B1313" t="s">
         <v>230</v>
       </c>
+      <c r="C1313" t="s">
+        <v>202</v>
+      </c>
+      <c r="D1313">
+        <v>6.2939999999999996</v>
+      </c>
       <c r="G1313" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1313" s="1" t="s">
         <v>73</v>
@@ -61402,8 +61645,14 @@
       <c r="B1314" t="s">
         <v>230</v>
       </c>
+      <c r="C1314" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1314">
+        <v>4.8949999999999996</v>
+      </c>
       <c r="G1314" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1314" s="1" t="s">
         <v>73</v>
@@ -61425,8 +61674,14 @@
       <c r="B1315" t="s">
         <v>230</v>
       </c>
+      <c r="C1315" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1315">
+        <v>7.6040000000000001</v>
+      </c>
       <c r="G1315" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1315" s="1" t="s">
         <v>73</v>
@@ -61448,8 +61703,14 @@
       <c r="B1316" t="s">
         <v>230</v>
       </c>
+      <c r="C1316" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1316">
+        <v>2.5790000000000002</v>
+      </c>
       <c r="G1316" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1316" s="1" t="s">
         <v>73</v>
@@ -61471,8 +61732,14 @@
       <c r="B1317" t="s">
         <v>230</v>
       </c>
+      <c r="C1317" t="s">
+        <v>202</v>
+      </c>
+      <c r="D1317">
+        <v>6.4279999999999999</v>
+      </c>
       <c r="G1317" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1317" s="1" t="s">
         <v>73</v>
@@ -61494,8 +61761,14 @@
       <c r="B1318" t="s">
         <v>230</v>
       </c>
+      <c r="C1318" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1318">
+        <v>6.4720000000000004</v>
+      </c>
       <c r="G1318" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1318" s="1" t="s">
         <v>73</v>
@@ -61517,8 +61790,14 @@
       <c r="B1319" t="s">
         <v>230</v>
       </c>
+      <c r="C1319" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1319">
+        <v>2.9670000000000001</v>
+      </c>
       <c r="G1319" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1319" s="1" t="s">
         <v>73</v>
@@ -61540,8 +61819,14 @@
       <c r="B1320" t="s">
         <v>230</v>
       </c>
+      <c r="C1320" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1320">
+        <v>4.9820000000000002</v>
+      </c>
       <c r="G1320" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1320" s="1" t="s">
         <v>73</v>
@@ -61567,7 +61852,7 @@
         <v>703</v>
       </c>
       <c r="G1321" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1321" s="1" t="s">
         <v>73</v>
@@ -61592,8 +61877,11 @@
       <c r="C1322" t="s">
         <v>703</v>
       </c>
+      <c r="E1322" s="1" t="s">
+        <v>914</v>
+      </c>
       <c r="G1322" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1322" s="1" t="s">
         <v>73</v>
@@ -61615,8 +61903,17 @@
       <c r="B1323" t="s">
         <v>231</v>
       </c>
+      <c r="C1323" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1323">
+        <v>6.867</v>
+      </c>
+      <c r="E1323" s="1" t="s">
+        <v>915</v>
+      </c>
       <c r="G1323" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1323" s="1" t="s">
         <v>73</v>
@@ -61638,8 +61935,14 @@
       <c r="B1324" t="s">
         <v>231</v>
       </c>
+      <c r="C1324" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1324">
+        <v>7.298</v>
+      </c>
       <c r="G1324" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1324" s="1" t="s">
         <v>73</v>
@@ -61661,8 +61964,14 @@
       <c r="B1325" t="s">
         <v>231</v>
       </c>
+      <c r="C1325" t="s">
+        <v>202</v>
+      </c>
+      <c r="D1325">
+        <v>9.9649999999999999</v>
+      </c>
       <c r="G1325" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1325" s="1" t="s">
         <v>73</v>
@@ -61684,8 +61993,14 @@
       <c r="B1326" t="s">
         <v>231</v>
       </c>
+      <c r="C1326" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1326">
+        <v>6.6909999999999998</v>
+      </c>
       <c r="G1326" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1326" s="1" t="s">
         <v>73</v>
@@ -61707,8 +62022,14 @@
       <c r="B1327" t="s">
         <v>231</v>
       </c>
+      <c r="C1327" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1327">
+        <v>8.3559999999999999</v>
+      </c>
       <c r="G1327" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1327" s="1" t="s">
         <v>73</v>
@@ -61730,8 +62051,14 @@
       <c r="B1328" t="s">
         <v>231</v>
       </c>
+      <c r="C1328" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1328">
+        <v>8.0210000000000008</v>
+      </c>
       <c r="G1328" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1328" s="1" t="s">
         <v>73</v>
@@ -61753,8 +62080,14 @@
       <c r="B1329" t="s">
         <v>231</v>
       </c>
+      <c r="C1329" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1329">
+        <v>6.681</v>
+      </c>
       <c r="G1329" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1329" s="1" t="s">
         <v>73</v>
@@ -61776,8 +62109,14 @@
       <c r="B1330" t="s">
         <v>231</v>
       </c>
+      <c r="C1330" t="s">
+        <v>202</v>
+      </c>
+      <c r="D1330">
+        <v>9.5020000000000007</v>
+      </c>
       <c r="G1330" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1330" s="1" t="s">
         <v>73</v>
@@ -61799,8 +62138,14 @@
       <c r="B1331" t="s">
         <v>231</v>
       </c>
+      <c r="C1331" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1331">
+        <v>6.3630000000000004</v>
+      </c>
       <c r="G1331" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1331" s="1" t="s">
         <v>73</v>
@@ -61822,8 +62167,14 @@
       <c r="B1332" t="s">
         <v>231</v>
       </c>
+      <c r="C1332" t="s">
+        <v>202</v>
+      </c>
+      <c r="D1332">
+        <v>8.8040000000000003</v>
+      </c>
       <c r="G1332" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1332" s="1" t="s">
         <v>73</v>
@@ -61845,8 +62196,14 @@
       <c r="B1333" t="s">
         <v>231</v>
       </c>
+      <c r="C1333" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1333">
+        <v>5.5339999999999998</v>
+      </c>
       <c r="G1333" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1333" s="1" t="s">
         <v>73</v>
@@ -61868,8 +62225,14 @@
       <c r="B1334" t="s">
         <v>231</v>
       </c>
+      <c r="C1334" t="s">
+        <v>202</v>
+      </c>
+      <c r="D1334">
+        <v>7.6710000000000003</v>
+      </c>
       <c r="G1334" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1334" s="1" t="s">
         <v>73</v>
@@ -61891,8 +62254,14 @@
       <c r="B1335" t="s">
         <v>231</v>
       </c>
+      <c r="C1335" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1335">
+        <v>7.39</v>
+      </c>
       <c r="G1335" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1335" s="1" t="s">
         <v>73</v>
@@ -61914,14 +62283,20 @@
       <c r="B1336" t="s">
         <v>231</v>
       </c>
+      <c r="C1336" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1336">
+        <v>5.1260000000000003</v>
+      </c>
       <c r="G1336" s="1" t="s">
-        <v>679</v>
+        <v>88</v>
       </c>
       <c r="I1336" s="1" t="s">
         <v>73</v>
       </c>
       <c r="J1336">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="K1336" t="s">
         <v>61</v>
@@ -61937,8 +62312,14 @@
       <c r="B1337" t="s">
         <v>231</v>
       </c>
+      <c r="C1337" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1337">
+        <v>6.9589999999999996</v>
+      </c>
       <c r="G1337" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1337" s="1" t="s">
         <v>73</v>
@@ -61960,8 +62341,14 @@
       <c r="B1338" t="s">
         <v>231</v>
       </c>
+      <c r="C1338" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1338">
+        <v>8.7680000000000007</v>
+      </c>
       <c r="G1338" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1338" s="1" t="s">
         <v>73</v>
@@ -61983,8 +62370,14 @@
       <c r="B1339" t="s">
         <v>231</v>
       </c>
+      <c r="C1339" t="s">
+        <v>202</v>
+      </c>
+      <c r="D1339">
+        <v>10.502000000000001</v>
+      </c>
       <c r="G1339" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1339" s="1" t="s">
         <v>73</v>
@@ -62006,8 +62399,14 @@
       <c r="B1340" t="s">
         <v>231</v>
       </c>
+      <c r="C1340" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1340">
+        <v>9.0399999999999991</v>
+      </c>
       <c r="G1340" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1340" s="1" t="s">
         <v>73</v>
@@ -62029,8 +62428,14 @@
       <c r="B1341" t="s">
         <v>231</v>
       </c>
+      <c r="C1341" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1341">
+        <v>6.0670000000000002</v>
+      </c>
       <c r="G1341" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1341" s="1" t="s">
         <v>73</v>
@@ -62052,8 +62457,14 @@
       <c r="B1342" t="s">
         <v>231</v>
       </c>
+      <c r="C1342" t="s">
+        <v>202</v>
+      </c>
+      <c r="D1342">
+        <v>9.3469999999999995</v>
+      </c>
       <c r="G1342" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1342" s="1" t="s">
         <v>73</v>
@@ -62075,8 +62486,14 @@
       <c r="B1343" t="s">
         <v>231</v>
       </c>
+      <c r="C1343" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1343">
+        <v>4.3140000000000001</v>
+      </c>
       <c r="G1343" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1343" s="1" t="s">
         <v>73</v>
@@ -62098,8 +62515,14 @@
       <c r="B1344" t="s">
         <v>231</v>
       </c>
+      <c r="C1344" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1344">
+        <v>4.093</v>
+      </c>
       <c r="G1344" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1344" s="1" t="s">
         <v>73</v>
@@ -62121,8 +62544,14 @@
       <c r="B1345" t="s">
         <v>231</v>
       </c>
+      <c r="C1345" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1345">
+        <v>6.7720000000000002</v>
+      </c>
       <c r="G1345" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1345" s="1" t="s">
         <v>73</v>
@@ -62144,8 +62573,14 @@
       <c r="B1346" t="s">
         <v>231</v>
       </c>
+      <c r="C1346" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1346">
+        <v>4.3959999999999999</v>
+      </c>
       <c r="G1346" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1346" s="1" t="s">
         <v>73</v>
@@ -62167,8 +62602,14 @@
       <c r="B1347" t="s">
         <v>231</v>
       </c>
+      <c r="C1347" t="s">
+        <v>202</v>
+      </c>
+      <c r="D1347">
+        <v>6.891</v>
+      </c>
       <c r="G1347" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1347" s="1" t="s">
         <v>73</v>
@@ -62190,8 +62631,14 @@
       <c r="B1348" t="s">
         <v>231</v>
       </c>
+      <c r="C1348" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1348">
+        <v>4.5590000000000002</v>
+      </c>
       <c r="G1348" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1348" s="1" t="s">
         <v>73</v>
@@ -62213,8 +62660,14 @@
       <c r="B1349" t="s">
         <v>231</v>
       </c>
+      <c r="C1349" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1349">
+        <v>3.1989999999999998</v>
+      </c>
       <c r="G1349" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1349" s="1" t="s">
         <v>73</v>
@@ -62236,8 +62689,14 @@
       <c r="B1350" t="s">
         <v>231</v>
       </c>
+      <c r="C1350" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1350">
+        <v>6.335</v>
+      </c>
       <c r="G1350" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1350" s="1" t="s">
         <v>73</v>
@@ -62259,8 +62718,14 @@
       <c r="B1351" t="s">
         <v>231</v>
       </c>
+      <c r="C1351" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1351">
+        <v>4.9560000000000004</v>
+      </c>
       <c r="G1351" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1351" s="1" t="s">
         <v>73</v>
@@ -62282,8 +62747,14 @@
       <c r="B1352" t="s">
         <v>231</v>
       </c>
+      <c r="C1352" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1352">
+        <v>6.29</v>
+      </c>
       <c r="G1352" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1352" s="1" t="s">
         <v>73</v>
@@ -62305,8 +62776,14 @@
       <c r="B1353" t="s">
         <v>231</v>
       </c>
+      <c r="C1353" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1353">
+        <v>5.0940000000000003</v>
+      </c>
       <c r="G1353" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1353" s="1" t="s">
         <v>73</v>
@@ -62328,8 +62805,14 @@
       <c r="B1354" t="s">
         <v>231</v>
       </c>
+      <c r="C1354" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1354">
+        <v>7.0910000000000002</v>
+      </c>
       <c r="G1354" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1354" s="1" t="s">
         <v>73</v>
@@ -62351,8 +62834,14 @@
       <c r="B1355" t="s">
         <v>231</v>
       </c>
+      <c r="C1355" t="s">
+        <v>202</v>
+      </c>
+      <c r="D1355">
+        <v>6.31</v>
+      </c>
       <c r="G1355" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1355" s="1" t="s">
         <v>73</v>
@@ -62374,8 +62863,14 @@
       <c r="B1356" t="s">
         <v>231</v>
       </c>
+      <c r="C1356" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1356">
+        <v>4.8019999999999996</v>
+      </c>
       <c r="G1356" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1356" s="1" t="s">
         <v>73</v>
@@ -62397,8 +62892,14 @@
       <c r="B1357" t="s">
         <v>231</v>
       </c>
+      <c r="C1357" t="s">
+        <v>202</v>
+      </c>
+      <c r="D1357">
+        <v>8.8569999999999993</v>
+      </c>
       <c r="G1357" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1357" s="1" t="s">
         <v>73</v>
@@ -62420,8 +62921,14 @@
       <c r="B1358" t="s">
         <v>231</v>
       </c>
+      <c r="C1358" t="s">
+        <v>202</v>
+      </c>
+      <c r="D1358">
+        <v>5.742</v>
+      </c>
       <c r="G1358" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1358" s="1" t="s">
         <v>73</v>
@@ -62443,8 +62950,14 @@
       <c r="B1359" t="s">
         <v>231</v>
       </c>
+      <c r="C1359" t="s">
+        <v>202</v>
+      </c>
+      <c r="D1359">
+        <v>5.6</v>
+      </c>
       <c r="G1359" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1359" s="1" t="s">
         <v>73</v>
@@ -62466,8 +62979,14 @@
       <c r="B1360" t="s">
         <v>231</v>
       </c>
+      <c r="C1360" t="s">
+        <v>202</v>
+      </c>
+      <c r="D1360">
+        <v>5.4820000000000002</v>
+      </c>
       <c r="G1360" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1360" s="1" t="s">
         <v>73</v>
@@ -62489,8 +63008,14 @@
       <c r="B1361" t="s">
         <v>231</v>
       </c>
+      <c r="C1361" t="s">
+        <v>202</v>
+      </c>
+      <c r="D1361">
+        <v>5.2889999999999997</v>
+      </c>
       <c r="G1361" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1361" s="1" t="s">
         <v>73</v>
@@ -62512,8 +63037,14 @@
       <c r="B1362" t="s">
         <v>231</v>
       </c>
+      <c r="C1362" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1362">
+        <v>6.351</v>
+      </c>
       <c r="G1362" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1362" s="1" t="s">
         <v>73</v>
@@ -62535,8 +63066,14 @@
       <c r="B1363" t="s">
         <v>231</v>
       </c>
+      <c r="C1363" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1363">
+        <v>7.6289999999999996</v>
+      </c>
       <c r="G1363" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1363" s="1" t="s">
         <v>73</v>
@@ -62558,8 +63095,14 @@
       <c r="B1364" t="s">
         <v>231</v>
       </c>
+      <c r="C1364" t="s">
+        <v>202</v>
+      </c>
+      <c r="D1364">
+        <v>8.1120000000000001</v>
+      </c>
       <c r="G1364" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1364" s="1" t="s">
         <v>73</v>
@@ -62581,8 +63124,14 @@
       <c r="B1365" t="s">
         <v>231</v>
       </c>
+      <c r="C1365" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1365">
+        <v>7.4859999999999998</v>
+      </c>
       <c r="G1365" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1365" s="1" t="s">
         <v>73</v>
@@ -62604,8 +63153,14 @@
       <c r="B1366" t="s">
         <v>231</v>
       </c>
+      <c r="C1366" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1366">
+        <v>7.1859999999999999</v>
+      </c>
       <c r="G1366" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1366" s="1" t="s">
         <v>73</v>
@@ -62627,8 +63182,14 @@
       <c r="B1367" t="s">
         <v>231</v>
       </c>
+      <c r="C1367" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1367">
+        <v>7.4470000000000001</v>
+      </c>
       <c r="G1367" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1367" s="1" t="s">
         <v>73</v>
@@ -62654,7 +63215,7 @@
         <v>703</v>
       </c>
       <c r="G1368" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1368" s="1" t="s">
         <v>73</v>
@@ -62679,8 +63240,11 @@
       <c r="C1369" t="s">
         <v>703</v>
       </c>
+      <c r="E1369" s="1" t="s">
+        <v>916</v>
+      </c>
       <c r="G1369" s="1" t="s">
-        <v>679</v>
+        <v>188</v>
       </c>
       <c r="I1369" s="1" t="s">
         <v>73</v>

</xml_diff>

<commit_message>
adding day 10 date to srpeadsheet for last cohrot
</commit_message>
<xml_diff>
--- a/Data/2018-08-14_master_datac_2018_collection_year.xlsx
+++ b/Data/2018-08-14_master_datac_2018_collection_year.xlsx
@@ -8,31 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anbe642/zScience/Circadian_rhythm_runs_seasonal_timing/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96A93065-3259-464A-9245-E7059754067E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B24684D-947B-F848-BC6F-9CCA8EB3BB63}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9860" yWindow="9540" windowWidth="36360" windowHeight="21140" activeTab="1" xr2:uid="{C7477166-8A7C-B04A-9643-C277FEDCDAAB}"/>
+    <workbookView xWindow="9860" yWindow="7660" windowWidth="36360" windowHeight="21140" activeTab="1" xr2:uid="{C7477166-8A7C-B04A-9643-C277FEDCDAAB}"/>
   </bookViews>
   <sheets>
     <sheet name="Maggot_Collections" sheetId="2" r:id="rId1"/>
     <sheet name="Data_collect" sheetId="1" r:id="rId2"/>
     <sheet name="Pupal_Splits" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13033" uniqueCount="1007">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13127" uniqueCount="1007">
   <si>
     <t>Ind_ID</t>
   </si>
@@ -13946,8 +13941,8 @@
   <dimension ref="A1:AS1369"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1356" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Z1276" sqref="Z1276:Z1369"/>
+      <pane ySplit="1" topLeftCell="A1210" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H1276" sqref="H1276:H1369"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -60822,6 +60817,9 @@
       <c r="G1276" s="1" t="s">
         <v>188</v>
       </c>
+      <c r="H1276" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="I1276" s="1" t="s">
         <v>73</v>
       </c>
@@ -60857,6 +60855,9 @@
       <c r="G1277" s="1" t="s">
         <v>188</v>
       </c>
+      <c r="H1277" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="I1277" s="1" t="s">
         <v>73</v>
       </c>
@@ -60895,6 +60896,9 @@
       <c r="G1278" s="1" t="s">
         <v>188</v>
       </c>
+      <c r="H1278" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="I1278" s="1" t="s">
         <v>73</v>
       </c>
@@ -60933,6 +60937,9 @@
       <c r="G1279" s="1" t="s">
         <v>188</v>
       </c>
+      <c r="H1279" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="I1279" s="1" t="s">
         <v>73</v>
       </c>
@@ -60971,6 +60978,9 @@
       <c r="G1280" s="1" t="s">
         <v>188</v>
       </c>
+      <c r="H1280" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="I1280" s="1" t="s">
         <v>73</v>
       </c>
@@ -61009,6 +61019,9 @@
       <c r="G1281" s="1" t="s">
         <v>88</v>
       </c>
+      <c r="H1281" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="I1281" s="1" t="s">
         <v>73</v>
       </c>
@@ -61047,6 +61060,9 @@
       <c r="G1282" s="1" t="s">
         <v>188</v>
       </c>
+      <c r="H1282" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="I1282" s="1" t="s">
         <v>73</v>
       </c>
@@ -61082,6 +61098,9 @@
       <c r="G1283" s="1" t="s">
         <v>188</v>
       </c>
+      <c r="H1283" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="I1283" s="1" t="s">
         <v>73</v>
       </c>
@@ -61120,6 +61139,9 @@
       <c r="G1284" s="1" t="s">
         <v>188</v>
       </c>
+      <c r="H1284" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="I1284" s="1" t="s">
         <v>73</v>
       </c>
@@ -61158,6 +61180,9 @@
       <c r="G1285" s="1" t="s">
         <v>188</v>
       </c>
+      <c r="H1285" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="I1285" s="1" t="s">
         <v>73</v>
       </c>
@@ -61193,6 +61218,9 @@
       <c r="G1286" s="1" t="s">
         <v>188</v>
       </c>
+      <c r="H1286" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="I1286" s="1" t="s">
         <v>73</v>
       </c>
@@ -61228,6 +61256,9 @@
       <c r="G1287" s="1" t="s">
         <v>188</v>
       </c>
+      <c r="H1287" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="I1287" s="1" t="s">
         <v>73</v>
       </c>
@@ -61263,6 +61294,9 @@
       <c r="G1288" s="1" t="s">
         <v>188</v>
       </c>
+      <c r="H1288" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="I1288" s="1" t="s">
         <v>73</v>
       </c>
@@ -61301,6 +61335,9 @@
       <c r="G1289" s="1" t="s">
         <v>188</v>
       </c>
+      <c r="H1289" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="I1289" s="1" t="s">
         <v>73</v>
       </c>
@@ -61339,6 +61376,9 @@
       <c r="G1290" s="1" t="s">
         <v>188</v>
       </c>
+      <c r="H1290" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="I1290" s="1" t="s">
         <v>73</v>
       </c>
@@ -61377,6 +61417,9 @@
       <c r="G1291" s="1" t="s">
         <v>188</v>
       </c>
+      <c r="H1291" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="I1291" s="1" t="s">
         <v>73</v>
       </c>
@@ -61415,6 +61458,9 @@
       <c r="G1292" s="1" t="s">
         <v>188</v>
       </c>
+      <c r="H1292" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="I1292" s="1" t="s">
         <v>73</v>
       </c>
@@ -61453,6 +61499,9 @@
       <c r="G1293" s="1" t="s">
         <v>188</v>
       </c>
+      <c r="H1293" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="I1293" s="1" t="s">
         <v>73</v>
       </c>
@@ -61491,6 +61540,9 @@
       <c r="G1294" s="1" t="s">
         <v>188</v>
       </c>
+      <c r="H1294" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="I1294" s="1" t="s">
         <v>73</v>
       </c>
@@ -61526,6 +61578,9 @@
       <c r="G1295" s="1" t="s">
         <v>188</v>
       </c>
+      <c r="H1295" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="I1295" s="1" t="s">
         <v>73</v>
       </c>
@@ -61561,6 +61616,9 @@
       <c r="G1296" s="1" t="s">
         <v>188</v>
       </c>
+      <c r="H1296" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="I1296" s="1" t="s">
         <v>73</v>
       </c>
@@ -61599,6 +61657,9 @@
       <c r="G1297" s="1" t="s">
         <v>188</v>
       </c>
+      <c r="H1297" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="I1297" s="1" t="s">
         <v>73</v>
       </c>
@@ -61637,6 +61698,9 @@
       <c r="G1298" s="1" t="s">
         <v>188</v>
       </c>
+      <c r="H1298" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="I1298" s="1" t="s">
         <v>73</v>
       </c>
@@ -61675,6 +61739,9 @@
       <c r="G1299" s="1" t="s">
         <v>188</v>
       </c>
+      <c r="H1299" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="I1299" s="1" t="s">
         <v>73</v>
       </c>
@@ -61710,6 +61777,9 @@
       <c r="G1300" s="1" t="s">
         <v>188</v>
       </c>
+      <c r="H1300" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="I1300" s="1" t="s">
         <v>73</v>
       </c>
@@ -61745,6 +61815,9 @@
       <c r="G1301" s="1" t="s">
         <v>188</v>
       </c>
+      <c r="H1301" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="I1301" s="1" t="s">
         <v>73</v>
       </c>
@@ -61783,6 +61856,9 @@
       <c r="G1302" s="1" t="s">
         <v>188</v>
       </c>
+      <c r="H1302" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="I1302" s="1" t="s">
         <v>73</v>
       </c>
@@ -61821,6 +61897,9 @@
       <c r="G1303" s="1" t="s">
         <v>188</v>
       </c>
+      <c r="H1303" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="I1303" s="1" t="s">
         <v>73</v>
       </c>
@@ -61856,6 +61935,9 @@
       <c r="G1304" s="1" t="s">
         <v>188</v>
       </c>
+      <c r="H1304" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="I1304" s="1" t="s">
         <v>73</v>
       </c>
@@ -61894,6 +61976,9 @@
       <c r="G1305" s="1" t="s">
         <v>188</v>
       </c>
+      <c r="H1305" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="I1305" s="1" t="s">
         <v>73</v>
       </c>
@@ -61932,6 +62017,9 @@
       <c r="G1306" s="1" t="s">
         <v>188</v>
       </c>
+      <c r="H1306" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="I1306" s="1" t="s">
         <v>73</v>
       </c>
@@ -61970,6 +62058,9 @@
       <c r="G1307" s="1" t="s">
         <v>188</v>
       </c>
+      <c r="H1307" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="I1307" s="1" t="s">
         <v>73</v>
       </c>
@@ -62008,6 +62099,9 @@
       <c r="G1308" s="1" t="s">
         <v>188</v>
       </c>
+      <c r="H1308" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="I1308" s="1" t="s">
         <v>73</v>
       </c>
@@ -62046,6 +62140,9 @@
       <c r="G1309" s="1" t="s">
         <v>188</v>
       </c>
+      <c r="H1309" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="I1309" s="1" t="s">
         <v>73</v>
       </c>
@@ -62084,6 +62181,9 @@
       <c r="G1310" s="1" t="s">
         <v>188</v>
       </c>
+      <c r="H1310" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="I1310" s="1" t="s">
         <v>73</v>
       </c>
@@ -62122,6 +62222,9 @@
       <c r="G1311" s="1" t="s">
         <v>188</v>
       </c>
+      <c r="H1311" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="I1311" s="1" t="s">
         <v>73</v>
       </c>
@@ -62160,6 +62263,9 @@
       <c r="G1312" s="1" t="s">
         <v>188</v>
       </c>
+      <c r="H1312" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="I1312" s="1" t="s">
         <v>73</v>
       </c>
@@ -62198,6 +62304,9 @@
       <c r="G1313" s="1" t="s">
         <v>188</v>
       </c>
+      <c r="H1313" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="I1313" s="1" t="s">
         <v>73</v>
       </c>
@@ -62236,6 +62345,9 @@
       <c r="G1314" s="1" t="s">
         <v>188</v>
       </c>
+      <c r="H1314" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="I1314" s="1" t="s">
         <v>73</v>
       </c>
@@ -62274,6 +62386,9 @@
       <c r="G1315" s="1" t="s">
         <v>188</v>
       </c>
+      <c r="H1315" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="I1315" s="1" t="s">
         <v>73</v>
       </c>
@@ -62312,6 +62427,9 @@
       <c r="G1316" s="1" t="s">
         <v>188</v>
       </c>
+      <c r="H1316" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="I1316" s="1" t="s">
         <v>73</v>
       </c>
@@ -62347,6 +62465,9 @@
       <c r="G1317" s="1" t="s">
         <v>188</v>
       </c>
+      <c r="H1317" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="I1317" s="1" t="s">
         <v>73</v>
       </c>
@@ -62382,6 +62503,9 @@
       <c r="G1318" s="1" t="s">
         <v>188</v>
       </c>
+      <c r="H1318" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="I1318" s="1" t="s">
         <v>73</v>
       </c>
@@ -62420,6 +62544,9 @@
       <c r="G1319" s="1" t="s">
         <v>188</v>
       </c>
+      <c r="H1319" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="I1319" s="1" t="s">
         <v>73</v>
       </c>
@@ -62458,6 +62585,9 @@
       <c r="G1320" s="1" t="s">
         <v>188</v>
       </c>
+      <c r="H1320" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="I1320" s="1" t="s">
         <v>73</v>
       </c>
@@ -62490,6 +62620,9 @@
       <c r="G1321" s="1" t="s">
         <v>188</v>
       </c>
+      <c r="H1321" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="I1321" s="1" t="s">
         <v>73</v>
       </c>
@@ -62519,6 +62652,9 @@
       <c r="G1322" s="1" t="s">
         <v>188</v>
       </c>
+      <c r="H1322" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="I1322" s="1" t="s">
         <v>73</v>
       </c>
@@ -62551,6 +62687,9 @@
       <c r="G1323" s="1" t="s">
         <v>188</v>
       </c>
+      <c r="H1323" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="I1323" s="1" t="s">
         <v>73</v>
       </c>
@@ -62589,6 +62728,9 @@
       <c r="G1324" s="1" t="s">
         <v>188</v>
       </c>
+      <c r="H1324" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="I1324" s="1" t="s">
         <v>73</v>
       </c>
@@ -62627,6 +62769,9 @@
       <c r="G1325" s="1" t="s">
         <v>188</v>
       </c>
+      <c r="H1325" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="I1325" s="1" t="s">
         <v>73</v>
       </c>
@@ -62662,6 +62807,9 @@
       <c r="G1326" s="1" t="s">
         <v>188</v>
       </c>
+      <c r="H1326" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="I1326" s="1" t="s">
         <v>73</v>
       </c>
@@ -62697,6 +62845,9 @@
       <c r="G1327" s="1" t="s">
         <v>188</v>
       </c>
+      <c r="H1327" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="I1327" s="1" t="s">
         <v>73</v>
       </c>
@@ -62735,6 +62886,9 @@
       <c r="G1328" s="1" t="s">
         <v>188</v>
       </c>
+      <c r="H1328" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="I1328" s="1" t="s">
         <v>73</v>
       </c>
@@ -62770,6 +62924,9 @@
       <c r="G1329" s="1" t="s">
         <v>188</v>
       </c>
+      <c r="H1329" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="I1329" s="1" t="s">
         <v>73</v>
       </c>
@@ -62808,6 +62965,9 @@
       <c r="G1330" s="1" t="s">
         <v>188</v>
       </c>
+      <c r="H1330" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="I1330" s="1" t="s">
         <v>73</v>
       </c>
@@ -62846,6 +63006,9 @@
       <c r="G1331" s="1" t="s">
         <v>188</v>
       </c>
+      <c r="H1331" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="I1331" s="1" t="s">
         <v>73</v>
       </c>
@@ -62884,6 +63047,9 @@
       <c r="G1332" s="1" t="s">
         <v>188</v>
       </c>
+      <c r="H1332" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="I1332" s="1" t="s">
         <v>73</v>
       </c>
@@ -62919,6 +63085,9 @@
       <c r="G1333" s="1" t="s">
         <v>188</v>
       </c>
+      <c r="H1333" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="I1333" s="1" t="s">
         <v>73</v>
       </c>
@@ -62954,6 +63123,9 @@
       <c r="G1334" s="1" t="s">
         <v>188</v>
       </c>
+      <c r="H1334" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="I1334" s="1" t="s">
         <v>73</v>
       </c>
@@ -62989,6 +63161,9 @@
       <c r="G1335" s="1" t="s">
         <v>188</v>
       </c>
+      <c r="H1335" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="I1335" s="1" t="s">
         <v>73</v>
       </c>
@@ -63024,6 +63199,9 @@
       <c r="G1336" s="1" t="s">
         <v>88</v>
       </c>
+      <c r="H1336" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="I1336" s="1" t="s">
         <v>73</v>
       </c>
@@ -63059,6 +63237,9 @@
       <c r="G1337" s="1" t="s">
         <v>188</v>
       </c>
+      <c r="H1337" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="I1337" s="1" t="s">
         <v>73</v>
       </c>
@@ -63097,6 +63278,9 @@
       <c r="G1338" s="1" t="s">
         <v>188</v>
       </c>
+      <c r="H1338" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="I1338" s="1" t="s">
         <v>73</v>
       </c>
@@ -63135,6 +63319,9 @@
       <c r="G1339" s="1" t="s">
         <v>188</v>
       </c>
+      <c r="H1339" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="I1339" s="1" t="s">
         <v>73</v>
       </c>
@@ -63173,6 +63360,9 @@
       <c r="G1340" s="1" t="s">
         <v>188</v>
       </c>
+      <c r="H1340" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="I1340" s="1" t="s">
         <v>73</v>
       </c>
@@ -63211,6 +63401,9 @@
       <c r="G1341" s="1" t="s">
         <v>188</v>
       </c>
+      <c r="H1341" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="I1341" s="1" t="s">
         <v>73</v>
       </c>
@@ -63249,6 +63442,9 @@
       <c r="G1342" s="1" t="s">
         <v>188</v>
       </c>
+      <c r="H1342" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="I1342" s="1" t="s">
         <v>73</v>
       </c>
@@ -63287,6 +63483,9 @@
       <c r="G1343" s="1" t="s">
         <v>188</v>
       </c>
+      <c r="H1343" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="I1343" s="1" t="s">
         <v>73</v>
       </c>
@@ -63322,6 +63521,9 @@
       <c r="G1344" s="1" t="s">
         <v>188</v>
       </c>
+      <c r="H1344" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="I1344" s="1" t="s">
         <v>73</v>
       </c>
@@ -63360,6 +63562,9 @@
       <c r="G1345" s="1" t="s">
         <v>188</v>
       </c>
+      <c r="H1345" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="I1345" s="1" t="s">
         <v>73</v>
       </c>
@@ -63398,6 +63603,9 @@
       <c r="G1346" s="1" t="s">
         <v>188</v>
       </c>
+      <c r="H1346" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="I1346" s="1" t="s">
         <v>73</v>
       </c>
@@ -63436,6 +63644,9 @@
       <c r="G1347" s="1" t="s">
         <v>188</v>
       </c>
+      <c r="H1347" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="I1347" s="1" t="s">
         <v>73</v>
       </c>
@@ -63474,6 +63685,9 @@
       <c r="G1348" s="1" t="s">
         <v>188</v>
       </c>
+      <c r="H1348" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="I1348" s="1" t="s">
         <v>73</v>
       </c>
@@ -63512,6 +63726,9 @@
       <c r="G1349" s="1" t="s">
         <v>188</v>
       </c>
+      <c r="H1349" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="I1349" s="1" t="s">
         <v>73</v>
       </c>
@@ -63547,6 +63764,9 @@
       <c r="G1350" s="1" t="s">
         <v>188</v>
       </c>
+      <c r="H1350" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="I1350" s="1" t="s">
         <v>73</v>
       </c>
@@ -63585,6 +63805,9 @@
       <c r="G1351" s="1" t="s">
         <v>188</v>
       </c>
+      <c r="H1351" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="I1351" s="1" t="s">
         <v>73</v>
       </c>
@@ -63620,6 +63843,9 @@
       <c r="G1352" s="1" t="s">
         <v>188</v>
       </c>
+      <c r="H1352" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="I1352" s="1" t="s">
         <v>73</v>
       </c>
@@ -63658,6 +63884,9 @@
       <c r="G1353" s="1" t="s">
         <v>188</v>
       </c>
+      <c r="H1353" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="I1353" s="1" t="s">
         <v>73</v>
       </c>
@@ -63696,6 +63925,9 @@
       <c r="G1354" s="1" t="s">
         <v>188</v>
       </c>
+      <c r="H1354" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="I1354" s="1" t="s">
         <v>73</v>
       </c>
@@ -63731,6 +63963,9 @@
       <c r="G1355" s="1" t="s">
         <v>188</v>
       </c>
+      <c r="H1355" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="I1355" s="1" t="s">
         <v>73</v>
       </c>
@@ -63769,6 +64004,9 @@
       <c r="G1356" s="1" t="s">
         <v>188</v>
       </c>
+      <c r="H1356" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="I1356" s="1" t="s">
         <v>73</v>
       </c>
@@ -63804,6 +64042,9 @@
       <c r="G1357" s="1" t="s">
         <v>188</v>
       </c>
+      <c r="H1357" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="I1357" s="1" t="s">
         <v>73</v>
       </c>
@@ -63842,6 +64083,9 @@
       <c r="G1358" s="1" t="s">
         <v>188</v>
       </c>
+      <c r="H1358" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="I1358" s="1" t="s">
         <v>73</v>
       </c>
@@ -63880,6 +64124,9 @@
       <c r="G1359" s="1" t="s">
         <v>188</v>
       </c>
+      <c r="H1359" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="I1359" s="1" t="s">
         <v>73</v>
       </c>
@@ -63918,6 +64165,9 @@
       <c r="G1360" s="1" t="s">
         <v>188</v>
       </c>
+      <c r="H1360" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="I1360" s="1" t="s">
         <v>73</v>
       </c>
@@ -63956,6 +64206,9 @@
       <c r="G1361" s="1" t="s">
         <v>188</v>
       </c>
+      <c r="H1361" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="I1361" s="1" t="s">
         <v>73</v>
       </c>
@@ -63991,6 +64244,9 @@
       <c r="G1362" s="1" t="s">
         <v>188</v>
       </c>
+      <c r="H1362" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="I1362" s="1" t="s">
         <v>73</v>
       </c>
@@ -64029,6 +64285,9 @@
       <c r="G1363" s="1" t="s">
         <v>188</v>
       </c>
+      <c r="H1363" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="I1363" s="1" t="s">
         <v>73</v>
       </c>
@@ -64064,6 +64323,9 @@
       <c r="G1364" s="1" t="s">
         <v>188</v>
       </c>
+      <c r="H1364" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="I1364" s="1" t="s">
         <v>73</v>
       </c>
@@ -64102,6 +64364,9 @@
       <c r="G1365" s="1" t="s">
         <v>188</v>
       </c>
+      <c r="H1365" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="I1365" s="1" t="s">
         <v>73</v>
       </c>
@@ -64140,6 +64405,9 @@
       <c r="G1366" s="1" t="s">
         <v>188</v>
       </c>
+      <c r="H1366" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="I1366" s="1" t="s">
         <v>73</v>
       </c>
@@ -64175,6 +64443,9 @@
       <c r="G1367" s="1" t="s">
         <v>188</v>
       </c>
+      <c r="H1367" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="I1367" s="1" t="s">
         <v>73</v>
       </c>
@@ -64207,6 +64478,9 @@
       <c r="G1368" s="1" t="s">
         <v>188</v>
       </c>
+      <c r="H1368" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="I1368" s="1" t="s">
         <v>73</v>
       </c>
@@ -64235,6 +64509,9 @@
       </c>
       <c r="G1369" s="1" t="s">
         <v>188</v>
+      </c>
+      <c r="H1369" s="1" t="s">
+        <v>83</v>
       </c>
       <c r="I1369" s="1" t="s">
         <v>73</v>

</xml_diff>

<commit_message>
hinal data add pupal counts
</commit_message>
<xml_diff>
--- a/Data/2018-08-14_master_datac_2018_collection_year.xlsx
+++ b/Data/2018-08-14_master_datac_2018_collection_year.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andrew.nguyen\Desktop\Circadian_rhythm_runs_seasonal_timing\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hinalkharva\Desktop\Circadian_rhythm_runs_seasonal_timing\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41377E4F-19DF-4130-A9B3-8592998EC557}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BB6CCEB-9DBA-42C8-8A87-103023EED676}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9855" yWindow="7665" windowWidth="36360" windowHeight="21135" activeTab="1" xr2:uid="{C7477166-8A7C-B04A-9643-C277FEDCDAAB}"/>
+    <workbookView xWindow="9855" yWindow="7665" windowWidth="36360" windowHeight="21135" activeTab="2" xr2:uid="{C7477166-8A7C-B04A-9643-C277FEDCDAAB}"/>
   </bookViews>
   <sheets>
     <sheet name="Maggot_Collections" sheetId="2" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13666" uniqueCount="1027">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13746" uniqueCount="1027">
   <si>
     <t>Ind_ID</t>
   </si>
@@ -14005,9 +14005,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92725FB9-1A17-2546-9DFA-6C0D39437891}">
   <dimension ref="A1:AS1452"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1409" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AD1431" sqref="AD1431"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A1373" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J1370" sqref="J1370"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -67606,10 +67606,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD836908-61FC-4C6A-BB55-EB17A2B99FDD}">
-  <dimension ref="A1:M65"/>
+  <dimension ref="A1:M81"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="I51" sqref="I51"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="E68" sqref="E68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -69062,31 +69062,330 @@
         <v>4</v>
       </c>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A58" s="62" t="s">
+        <v>58</v>
+      </c>
+      <c r="B58" s="42" t="s">
+        <v>59</v>
+      </c>
+      <c r="C58" s="42" t="s">
+        <v>61</v>
+      </c>
+      <c r="D58" s="42" t="s">
+        <v>88</v>
+      </c>
+      <c r="F58" s="42" t="s">
+        <v>69</v>
+      </c>
+      <c r="G58">
+        <v>64</v>
+      </c>
+      <c r="I58">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A59" s="62" t="s">
+        <v>58</v>
+      </c>
+      <c r="B59" s="42" t="s">
+        <v>59</v>
+      </c>
+      <c r="C59" s="42" t="s">
+        <v>61</v>
+      </c>
+      <c r="D59" s="42" t="s">
+        <v>188</v>
+      </c>
+      <c r="F59" s="42" t="s">
+        <v>69</v>
+      </c>
+      <c r="J59">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A60" s="62" t="s">
+        <v>58</v>
+      </c>
+      <c r="B60" s="42" t="s">
+        <v>60</v>
+      </c>
+      <c r="C60" s="42" t="s">
+        <v>61</v>
+      </c>
+      <c r="D60" s="42" t="s">
+        <v>88</v>
+      </c>
+      <c r="F60" s="42" t="s">
+        <v>69</v>
+      </c>
+      <c r="J60">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A61" s="62" t="s">
+        <v>58</v>
+      </c>
+      <c r="B61" s="42" t="s">
+        <v>60</v>
+      </c>
+      <c r="C61" s="42" t="s">
+        <v>61</v>
+      </c>
+      <c r="D61" s="42" t="s">
+        <v>188</v>
+      </c>
+      <c r="F61" s="42" t="s">
+        <v>69</v>
+      </c>
+      <c r="J61">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A62" s="62" t="s">
+        <v>195</v>
+      </c>
+      <c r="B62" s="42" t="s">
+        <v>197</v>
+      </c>
+      <c r="C62" s="42" t="s">
+        <v>61</v>
+      </c>
+      <c r="D62" s="42" t="s">
+        <v>188</v>
+      </c>
+      <c r="F62" s="42" t="s">
+        <v>69</v>
+      </c>
+      <c r="J62">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A63" s="62" t="s">
+        <v>195</v>
+      </c>
+      <c r="B63" s="42" t="s">
+        <v>713</v>
+      </c>
+      <c r="C63" s="42" t="s">
+        <v>61</v>
+      </c>
+      <c r="D63" s="42" t="s">
+        <v>188</v>
+      </c>
+      <c r="F63" s="42" t="s">
+        <v>69</v>
+      </c>
+      <c r="J63">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A64" s="62" t="s">
+        <v>195</v>
+      </c>
+      <c r="B64" s="42" t="s">
+        <v>208</v>
+      </c>
+      <c r="C64" s="42" t="s">
+        <v>61</v>
+      </c>
+      <c r="D64" s="42" t="s">
+        <v>188</v>
+      </c>
+      <c r="F64" s="42" t="s">
+        <v>69</v>
+      </c>
+      <c r="J64">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A65" s="62" t="s">
+        <v>195</v>
+      </c>
+      <c r="B65" s="42" t="s">
+        <v>202</v>
+      </c>
+      <c r="C65" t="s">
+        <v>714</v>
+      </c>
+      <c r="D65" s="42" t="s">
+        <v>188</v>
+      </c>
+      <c r="F65" s="42" t="s">
+        <v>69</v>
+      </c>
+      <c r="L65">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A66" s="62" t="s">
+        <v>58</v>
+      </c>
+      <c r="B66" s="42" t="s">
+        <v>59</v>
+      </c>
+      <c r="C66" s="42" t="s">
+        <v>61</v>
+      </c>
+      <c r="D66" s="42" t="s">
+        <v>88</v>
+      </c>
+      <c r="F66" s="42" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A67" s="62" t="s">
+        <v>58</v>
+      </c>
+      <c r="B67" s="42" t="s">
+        <v>59</v>
+      </c>
+      <c r="C67" s="42" t="s">
+        <v>61</v>
+      </c>
+      <c r="D67" s="42" t="s">
+        <v>188</v>
+      </c>
+      <c r="F67" s="42" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A68" s="62" t="s">
+        <v>58</v>
+      </c>
+      <c r="B68" s="42" t="s">
+        <v>60</v>
+      </c>
+      <c r="C68" s="42" t="s">
+        <v>61</v>
+      </c>
+      <c r="D68" s="42" t="s">
+        <v>88</v>
+      </c>
+      <c r="F68" s="42" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A69" s="62" t="s">
+        <v>58</v>
+      </c>
+      <c r="B69" s="42" t="s">
+        <v>60</v>
+      </c>
+      <c r="C69" s="42" t="s">
+        <v>61</v>
+      </c>
+      <c r="D69" s="42" t="s">
+        <v>188</v>
+      </c>
+      <c r="F69" s="42" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A70" s="62" t="s">
+        <v>195</v>
+      </c>
+      <c r="B70" s="42" t="s">
+        <v>197</v>
+      </c>
+      <c r="C70" s="42" t="s">
+        <v>61</v>
+      </c>
+      <c r="D70" s="42" t="s">
+        <v>188</v>
+      </c>
+      <c r="F70" s="42" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A71" s="62" t="s">
+        <v>195</v>
+      </c>
+      <c r="B71" s="42" t="s">
+        <v>713</v>
+      </c>
+      <c r="C71" s="42" t="s">
+        <v>61</v>
+      </c>
+      <c r="D71" s="42" t="s">
+        <v>188</v>
+      </c>
+      <c r="F71" s="42" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A72" s="62" t="s">
+        <v>195</v>
+      </c>
+      <c r="B72" s="42" t="s">
+        <v>208</v>
+      </c>
+      <c r="C72" s="42" t="s">
+        <v>61</v>
+      </c>
+      <c r="D72" s="42" t="s">
+        <v>188</v>
+      </c>
+      <c r="F72" s="42" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A73" s="62" t="s">
+        <v>195</v>
+      </c>
+      <c r="B73" s="42" t="s">
+        <v>202</v>
+      </c>
+      <c r="C73" t="s">
+        <v>714</v>
+      </c>
+      <c r="D73" s="42" t="s">
+        <v>188</v>
+      </c>
+      <c r="F73" s="42" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
         <v>228</v>
       </c>
-      <c r="G65">
+      <c r="G81">
         <f>SUM(G2:G30)</f>
         <v>2560</v>
       </c>
-      <c r="H65">
+      <c r="H81">
         <f>SUM(H2:H49)</f>
         <v>533</v>
       </c>
-      <c r="I65">
+      <c r="I81">
         <f>SUM(I2:I49)</f>
         <v>106</v>
       </c>
-      <c r="J65">
+      <c r="J81">
         <f>SUM(J2:J51)</f>
         <v>1045</v>
       </c>
-      <c r="K65">
-        <f>SUM(G65:J65)</f>
+      <c r="K81">
+        <f>SUM(G81:J81)</f>
         <v>4244</v>
       </c>
-      <c r="M65">
+      <c r="M81">
         <f>SUM(M29:M51)</f>
         <v>13</v>
       </c>

</xml_diff>

<commit_message>
entering data for day 12 +27 cohort 2018-09-11
</commit_message>
<xml_diff>
--- a/Data/2018-08-14_master_datac_2018_collection_year.xlsx
+++ b/Data/2018-08-14_master_datac_2018_collection_year.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hinalkharva\Desktop\Circadian_rhythm_runs_seasonal_timing\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andrew.nguyen\Desktop\Circadian_rhythm_runs_seasonal_timing\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80F6870C-B863-4568-8C79-879673AE49E8}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCBEB131-F759-46DF-9F33-5CE324F0CC2E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9855" yWindow="7665" windowWidth="36360" windowHeight="21135" xr2:uid="{C7477166-8A7C-B04A-9643-C277FEDCDAAB}"/>
+    <workbookView xWindow="9855" yWindow="7665" windowWidth="36360" windowHeight="21135" activeTab="1" xr2:uid="{C7477166-8A7C-B04A-9643-C277FEDCDAAB}"/>
   </bookViews>
   <sheets>
     <sheet name="Maggot_Collections" sheetId="2" r:id="rId1"/>
@@ -22,12 +22,17 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13771" uniqueCount="1029">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14425" uniqueCount="1033">
   <si>
     <t>Ind_ID</t>
   </si>
@@ -3114,6 +3119,18 @@
   </si>
   <si>
     <t>20+6=26</t>
+  </si>
+  <si>
+    <t>15:05</t>
+  </si>
+  <si>
+    <t>15:21</t>
+  </si>
+  <si>
+    <t>14:55</t>
+  </si>
+  <si>
+    <t>15:04</t>
   </si>
 </sst>
 </file>
@@ -3719,7 +3736,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D3F78F5-4EA8-6A42-B216-41A8EC7A5E8D}">
   <dimension ref="A1:AC306"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A139" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="L160" sqref="L160"/>
     </sheetView>
@@ -14113,11 +14130,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92725FB9-1A17-2546-9DFA-6C0D39437891}">
-  <dimension ref="A1:AS1452"/>
+  <dimension ref="A1:AS1539"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1373" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J1370" sqref="J1370"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A1518" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D1538" sqref="D1538"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -67696,16 +67713,2977 @@
         <v>244</v>
       </c>
     </row>
+    <row r="1447" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1447">
+        <v>1</v>
+      </c>
+      <c r="B1447" t="s">
+        <v>387</v>
+      </c>
+      <c r="C1447" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1447">
+        <v>9.9450000000000003</v>
+      </c>
+      <c r="E1447" s="1" t="s">
+        <v>1029</v>
+      </c>
+      <c r="G1447" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H1447" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="I1447" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1447">
+        <v>12</v>
+      </c>
+      <c r="K1447" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1447" s="1" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="1448" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1448">
+        <v>2</v>
+      </c>
+      <c r="B1448" t="s">
+        <v>387</v>
+      </c>
+      <c r="C1448" t="s">
+        <v>202</v>
+      </c>
+      <c r="D1448">
+        <v>6.7670000000000003</v>
+      </c>
+      <c r="G1448" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H1448" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="I1448" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1448">
+        <v>12</v>
+      </c>
+      <c r="K1448" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1448" s="1" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="1449" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1449">
+        <v>3</v>
+      </c>
+      <c r="B1449" t="s">
+        <v>387</v>
+      </c>
+      <c r="C1449" t="s">
+        <v>202</v>
+      </c>
+      <c r="D1449">
+        <v>6.2880000000000003</v>
+      </c>
+      <c r="G1449" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H1449" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="I1449" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1449">
+        <v>12</v>
+      </c>
+      <c r="K1449" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1449" s="1" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="1450" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1450">
+        <v>4</v>
+      </c>
+      <c r="B1450" t="s">
+        <v>387</v>
+      </c>
+      <c r="C1450" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1450">
+        <v>6.0259999999999998</v>
+      </c>
+      <c r="G1450" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H1450" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="I1450" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1450">
+        <v>12</v>
+      </c>
+      <c r="K1450" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1450" s="1" t="s">
+        <v>543</v>
+      </c>
+    </row>
     <row r="1451" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="C1451">
-        <f>45-14</f>
+      <c r="A1451">
+        <v>5</v>
+      </c>
+      <c r="B1451" t="s">
+        <v>387</v>
+      </c>
+      <c r="C1451" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1451">
+        <v>4.2880000000000003</v>
+      </c>
+      <c r="G1451" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H1451" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="I1451" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1451">
+        <v>12</v>
+      </c>
+      <c r="K1451" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1451" s="1" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="1452" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1452">
+        <v>6</v>
+      </c>
+      <c r="B1452" t="s">
+        <v>387</v>
+      </c>
+      <c r="C1452" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1452">
+        <v>10.43</v>
+      </c>
+      <c r="G1452" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H1452" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="I1452" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1452">
+        <v>12</v>
+      </c>
+      <c r="K1452" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1452" s="1" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="1453" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1453">
+        <v>7</v>
+      </c>
+      <c r="B1453" t="s">
+        <v>387</v>
+      </c>
+      <c r="C1453" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1453">
+        <v>5.851</v>
+      </c>
+      <c r="G1453" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H1453" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="I1453" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1453">
+        <v>12</v>
+      </c>
+      <c r="K1453" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1453" s="1" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="1454" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1454">
+        <v>8</v>
+      </c>
+      <c r="B1454" t="s">
+        <v>387</v>
+      </c>
+      <c r="C1454" t="s">
+        <v>202</v>
+      </c>
+      <c r="D1454">
+        <v>6.2949999999999999</v>
+      </c>
+      <c r="G1454" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H1454" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="I1454" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1454">
+        <v>12</v>
+      </c>
+      <c r="K1454" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1454" s="1" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="1455" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1455">
+        <v>9</v>
+      </c>
+      <c r="B1455" t="s">
+        <v>387</v>
+      </c>
+      <c r="C1455" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1455">
+        <v>7.6219999999999999</v>
+      </c>
+      <c r="G1455" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H1455" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="I1455" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1455">
+        <v>12</v>
+      </c>
+      <c r="K1455" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1455" s="1" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="1456" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1456">
+        <v>10</v>
+      </c>
+      <c r="B1456" t="s">
+        <v>387</v>
+      </c>
+      <c r="C1456" t="s">
+        <v>202</v>
+      </c>
+      <c r="D1456">
+        <v>8.7119999999999997</v>
+      </c>
+      <c r="G1456" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H1456" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="I1456" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1456">
+        <v>12</v>
+      </c>
+      <c r="K1456" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1456" s="1" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="1457" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1457">
+        <v>11</v>
+      </c>
+      <c r="B1457" t="s">
+        <v>387</v>
+      </c>
+      <c r="C1457" t="s">
+        <v>202</v>
+      </c>
+      <c r="D1457">
+        <v>3.8340000000000001</v>
+      </c>
+      <c r="G1457" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H1457" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="I1457" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1457">
+        <v>12</v>
+      </c>
+      <c r="K1457" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1457" s="1" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="1458" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1458">
+        <v>12</v>
+      </c>
+      <c r="B1458" t="s">
+        <v>387</v>
+      </c>
+      <c r="C1458" t="s">
+        <v>202</v>
+      </c>
+      <c r="D1458">
+        <v>7.4710000000000001</v>
+      </c>
+      <c r="G1458" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H1458" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="I1458" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1458">
+        <v>12</v>
+      </c>
+      <c r="K1458" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1458" s="1" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="1459" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1459">
+        <v>13</v>
+      </c>
+      <c r="B1459" t="s">
+        <v>387</v>
+      </c>
+      <c r="C1459" t="s">
+        <v>202</v>
+      </c>
+      <c r="D1459">
+        <v>9.6280000000000001</v>
+      </c>
+      <c r="G1459" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H1459" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="I1459" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1459">
+        <v>12</v>
+      </c>
+      <c r="K1459" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1459" s="1" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="1460" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1460">
+        <v>14</v>
+      </c>
+      <c r="B1460" t="s">
+        <v>387</v>
+      </c>
+      <c r="C1460" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1460">
+        <v>10.476000000000001</v>
+      </c>
+      <c r="G1460" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H1460" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="I1460" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1460">
+        <v>12</v>
+      </c>
+      <c r="K1460" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1460" s="1" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="1461" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1461">
+        <v>15</v>
+      </c>
+      <c r="B1461" t="s">
+        <v>387</v>
+      </c>
+      <c r="C1461" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1461">
+        <v>9.1859999999999999</v>
+      </c>
+      <c r="G1461" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H1461" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="I1461" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1461">
+        <v>12</v>
+      </c>
+      <c r="K1461" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1461" s="1" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="1462" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1462">
+        <v>16</v>
+      </c>
+      <c r="B1462" t="s">
+        <v>387</v>
+      </c>
+      <c r="C1462" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1462">
+        <v>6.2270000000000003</v>
+      </c>
+      <c r="G1462" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H1462" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="I1462" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1462">
+        <v>12</v>
+      </c>
+      <c r="K1462" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1462" s="1" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="1463" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1463">
+        <v>17</v>
+      </c>
+      <c r="B1463" t="s">
+        <v>387</v>
+      </c>
+      <c r="C1463" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1463">
+        <v>6.7060000000000004</v>
+      </c>
+      <c r="G1463" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H1463" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="I1463" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1463">
+        <v>12</v>
+      </c>
+      <c r="K1463" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1463" s="1" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="1464" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1464">
+        <v>18</v>
+      </c>
+      <c r="B1464" t="s">
+        <v>387</v>
+      </c>
+      <c r="C1464" t="s">
+        <v>202</v>
+      </c>
+      <c r="D1464">
+        <v>9.0090000000000003</v>
+      </c>
+      <c r="G1464" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H1464" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="I1464" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1464">
+        <v>12</v>
+      </c>
+      <c r="K1464" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1464" s="1" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="1465" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1465">
+        <v>19</v>
+      </c>
+      <c r="B1465" t="s">
+        <v>387</v>
+      </c>
+      <c r="C1465" t="s">
+        <v>202</v>
+      </c>
+      <c r="D1465">
+        <v>7.7359999999999998</v>
+      </c>
+      <c r="G1465" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H1465" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="I1465" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1465">
+        <v>12</v>
+      </c>
+      <c r="K1465" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1465" s="1" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="1466" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1466">
+        <v>20</v>
+      </c>
+      <c r="B1466" t="s">
+        <v>387</v>
+      </c>
+      <c r="C1466" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1466">
+        <v>6.1139999999999999</v>
+      </c>
+      <c r="G1466" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H1466" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="I1466" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1466">
+        <v>12</v>
+      </c>
+      <c r="K1466" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1466" s="1" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="1467" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1467">
+        <v>21</v>
+      </c>
+      <c r="B1467" t="s">
+        <v>387</v>
+      </c>
+      <c r="C1467" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1467">
+        <v>8.2189999999999994</v>
+      </c>
+      <c r="G1467" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H1467" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="I1467" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1467">
+        <v>12</v>
+      </c>
+      <c r="K1467" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1467" s="1" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="1468" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1468">
+        <v>22</v>
+      </c>
+      <c r="B1468" t="s">
+        <v>387</v>
+      </c>
+      <c r="C1468" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1468">
+        <v>8.39</v>
+      </c>
+      <c r="G1468" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H1468" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="I1468" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1468">
+        <v>12</v>
+      </c>
+      <c r="K1468" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1468" s="1" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="1469" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1469">
+        <v>23</v>
+      </c>
+      <c r="B1469" t="s">
+        <v>387</v>
+      </c>
+      <c r="C1469" t="s">
+        <v>202</v>
+      </c>
+      <c r="D1469">
+        <v>6.5590000000000002</v>
+      </c>
+      <c r="G1469" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H1469" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="I1469" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1469">
+        <v>12</v>
+      </c>
+      <c r="K1469" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1469" s="1" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="1470" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1470">
+        <v>24</v>
+      </c>
+      <c r="B1470" t="s">
+        <v>387</v>
+      </c>
+      <c r="C1470" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1470">
+        <v>6.9390000000000001</v>
+      </c>
+      <c r="G1470" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H1470" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="I1470" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1470">
+        <v>12</v>
+      </c>
+      <c r="K1470" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1470" s="1" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="1471" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1471">
+        <v>25</v>
+      </c>
+      <c r="B1471" t="s">
+        <v>387</v>
+      </c>
+      <c r="C1471" t="s">
+        <v>202</v>
+      </c>
+      <c r="D1471">
+        <v>4.8849999999999998</v>
+      </c>
+      <c r="G1471" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H1471" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="I1471" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1471">
+        <v>12</v>
+      </c>
+      <c r="K1471" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1471" s="1" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="1472" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1472">
+        <v>26</v>
+      </c>
+      <c r="B1472" t="s">
+        <v>387</v>
+      </c>
+      <c r="C1472" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1472">
+        <v>7.5970000000000004</v>
+      </c>
+      <c r="G1472" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H1472" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="I1472" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1472">
+        <v>12</v>
+      </c>
+      <c r="K1472" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1472" s="1" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="1473" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1473">
+        <v>27</v>
+      </c>
+      <c r="B1473" t="s">
+        <v>387</v>
+      </c>
+      <c r="C1473" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1473">
+        <v>4.585</v>
+      </c>
+      <c r="G1473" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H1473" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="I1473" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1473">
+        <v>12</v>
+      </c>
+      <c r="K1473" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1473" s="1" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="1474" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1474">
+        <v>28</v>
+      </c>
+      <c r="B1474" t="s">
+        <v>387</v>
+      </c>
+      <c r="C1474" t="s">
+        <v>202</v>
+      </c>
+      <c r="D1474">
+        <v>7.5910000000000002</v>
+      </c>
+      <c r="G1474" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H1474" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="I1474" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1474">
+        <v>12</v>
+      </c>
+      <c r="K1474" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1474" s="1" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="1475" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1475">
+        <v>29</v>
+      </c>
+      <c r="B1475" t="s">
+        <v>387</v>
+      </c>
+      <c r="C1475" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1475">
+        <v>8.3819999999999997</v>
+      </c>
+      <c r="G1475" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H1475" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="I1475" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1475">
+        <v>12</v>
+      </c>
+      <c r="K1475" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1475" s="1" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="1476" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1476">
+        <v>30</v>
+      </c>
+      <c r="B1476" t="s">
+        <v>387</v>
+      </c>
+      <c r="C1476" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1476">
+        <v>6.734</v>
+      </c>
+      <c r="G1476" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H1476" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="I1476" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1476">
+        <v>12</v>
+      </c>
+      <c r="K1476" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1476" s="1" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="1477" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1477">
         <v>31</v>
       </c>
-    </row>
-    <row r="1452" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="C1452">
-        <f>C1451/2</f>
-        <v>15.5</v>
+      <c r="B1477" t="s">
+        <v>387</v>
+      </c>
+      <c r="C1477" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1477">
+        <v>6.3010000000000002</v>
+      </c>
+      <c r="G1477" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H1477" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="I1477" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1477">
+        <v>12</v>
+      </c>
+      <c r="K1477" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1477" s="1" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="1478" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1478">
+        <v>32</v>
+      </c>
+      <c r="B1478" t="s">
+        <v>387</v>
+      </c>
+      <c r="C1478" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1478">
+        <v>4.1059999999999999</v>
+      </c>
+      <c r="G1478" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H1478" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="I1478" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1478">
+        <v>12</v>
+      </c>
+      <c r="K1478" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1478" s="1" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="1479" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1479">
+        <v>33</v>
+      </c>
+      <c r="B1479" t="s">
+        <v>387</v>
+      </c>
+      <c r="C1479" t="s">
+        <v>202</v>
+      </c>
+      <c r="D1479">
+        <v>6.7290000000000001</v>
+      </c>
+      <c r="G1479" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H1479" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="I1479" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1479">
+        <v>12</v>
+      </c>
+      <c r="K1479" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1479" s="1" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="1480" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1480">
+        <v>34</v>
+      </c>
+      <c r="B1480" t="s">
+        <v>387</v>
+      </c>
+      <c r="C1480" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1480">
+        <v>9.718</v>
+      </c>
+      <c r="G1480" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H1480" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="I1480" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1480">
+        <v>12</v>
+      </c>
+      <c r="K1480" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1480" s="1" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="1481" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1481">
+        <v>35</v>
+      </c>
+      <c r="B1481" t="s">
+        <v>387</v>
+      </c>
+      <c r="C1481" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1481">
+        <v>6.7759999999999998</v>
+      </c>
+      <c r="G1481" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H1481" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="I1481" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1481">
+        <v>12</v>
+      </c>
+      <c r="K1481" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1481" s="1" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="1482" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1482">
+        <v>36</v>
+      </c>
+      <c r="B1482" t="s">
+        <v>387</v>
+      </c>
+      <c r="C1482" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1482">
+        <v>6.3460000000000001</v>
+      </c>
+      <c r="G1482" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H1482" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="I1482" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1482">
+        <v>12</v>
+      </c>
+      <c r="K1482" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1482" s="1" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="1483" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1483">
+        <v>37</v>
+      </c>
+      <c r="B1483" t="s">
+        <v>387</v>
+      </c>
+      <c r="C1483" t="s">
+        <v>202</v>
+      </c>
+      <c r="D1483">
+        <v>7.0140000000000002</v>
+      </c>
+      <c r="G1483" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H1483" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="I1483" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1483">
+        <v>12</v>
+      </c>
+      <c r="K1483" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1483" s="1" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="1484" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1484">
+        <v>38</v>
+      </c>
+      <c r="B1484" t="s">
+        <v>387</v>
+      </c>
+      <c r="C1484" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1484">
+        <v>6.0090000000000003</v>
+      </c>
+      <c r="G1484" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H1484" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="I1484" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1484">
+        <v>12</v>
+      </c>
+      <c r="K1484" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1484" s="1" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="1485" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1485">
+        <v>39</v>
+      </c>
+      <c r="B1485" t="s">
+        <v>387</v>
+      </c>
+      <c r="C1485" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1485">
+        <v>6.5359999999999996</v>
+      </c>
+      <c r="G1485" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H1485" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="I1485" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1485">
+        <v>12</v>
+      </c>
+      <c r="K1485" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1485" s="1" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="1486" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1486">
+        <v>40</v>
+      </c>
+      <c r="B1486" t="s">
+        <v>387</v>
+      </c>
+      <c r="C1486" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1486">
+        <v>4.827</v>
+      </c>
+      <c r="G1486" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H1486" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="I1486" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1486">
+        <v>12</v>
+      </c>
+      <c r="K1486" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1486" s="1" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="1487" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1487">
+        <v>41</v>
+      </c>
+      <c r="B1487" t="s">
+        <v>387</v>
+      </c>
+      <c r="C1487" t="s">
+        <v>202</v>
+      </c>
+      <c r="D1487">
+        <v>7.7030000000000003</v>
+      </c>
+      <c r="G1487" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H1487" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="I1487" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1487">
+        <v>12</v>
+      </c>
+      <c r="K1487" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1487" s="1" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="1488" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1488">
+        <v>42</v>
+      </c>
+      <c r="B1488" t="s">
+        <v>387</v>
+      </c>
+      <c r="C1488" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1488">
+        <v>3.8639999999999999</v>
+      </c>
+      <c r="G1488" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H1488" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="I1488" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1488">
+        <v>12</v>
+      </c>
+      <c r="K1488" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1488" s="1" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="1489" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1489">
+        <v>43</v>
+      </c>
+      <c r="B1489" t="s">
+        <v>387</v>
+      </c>
+      <c r="C1489" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1489">
+        <v>4.0410000000000004</v>
+      </c>
+      <c r="G1489" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H1489" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="I1489" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1489">
+        <v>12</v>
+      </c>
+      <c r="K1489" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1489" s="1" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="1490" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1490">
+        <v>44</v>
+      </c>
+      <c r="B1490" t="s">
+        <v>387</v>
+      </c>
+      <c r="C1490" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1490">
+        <v>5.5960000000000001</v>
+      </c>
+      <c r="G1490" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H1490" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="I1490" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1490">
+        <v>12</v>
+      </c>
+      <c r="K1490" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1490" s="1" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="1491" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1491">
+        <v>46</v>
+      </c>
+      <c r="B1491" t="s">
+        <v>387</v>
+      </c>
+      <c r="C1491" t="s">
+        <v>703</v>
+      </c>
+      <c r="G1491" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H1491" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="I1491" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1491">
+        <v>12</v>
+      </c>
+      <c r="K1491" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1491" s="1" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="1492" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1492">
+        <v>47</v>
+      </c>
+      <c r="B1492" t="s">
+        <v>387</v>
+      </c>
+      <c r="C1492" t="s">
+        <v>703</v>
+      </c>
+      <c r="E1492" s="1" t="s">
+        <v>1030</v>
+      </c>
+      <c r="G1492" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H1492" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="I1492" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1492">
+        <v>12</v>
+      </c>
+      <c r="K1492" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1492" s="1" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="1493" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1493">
+        <v>1</v>
+      </c>
+      <c r="B1493" t="s">
+        <v>230</v>
+      </c>
+      <c r="C1493" t="s">
+        <v>202</v>
+      </c>
+      <c r="D1493">
+        <v>8.5470000000000006</v>
+      </c>
+      <c r="E1493" s="1" t="s">
+        <v>1031</v>
+      </c>
+      <c r="G1493" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H1493" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="I1493" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1493">
+        <v>12</v>
+      </c>
+      <c r="K1493" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1493" s="1" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="1494" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1494">
+        <v>2</v>
+      </c>
+      <c r="B1494" t="s">
+        <v>230</v>
+      </c>
+      <c r="C1494" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1494">
+        <v>6.9240000000000004</v>
+      </c>
+      <c r="G1494" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H1494" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="I1494" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1494">
+        <v>12</v>
+      </c>
+      <c r="K1494" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1494" s="1" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="1495" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1495">
+        <v>3</v>
+      </c>
+      <c r="B1495" t="s">
+        <v>230</v>
+      </c>
+      <c r="C1495" t="s">
+        <v>202</v>
+      </c>
+      <c r="D1495">
+        <v>5.2089999999999996</v>
+      </c>
+      <c r="G1495" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H1495" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="I1495" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1495">
+        <v>12</v>
+      </c>
+      <c r="K1495" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1495" s="1" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="1496" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1496">
+        <v>4</v>
+      </c>
+      <c r="B1496" t="s">
+        <v>230</v>
+      </c>
+      <c r="C1496" t="s">
+        <v>202</v>
+      </c>
+      <c r="D1496">
+        <v>6.3010000000000002</v>
+      </c>
+      <c r="G1496" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H1496" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="I1496" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1496">
+        <v>12</v>
+      </c>
+      <c r="K1496" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1496" s="1" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="1497" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1497">
+        <v>5</v>
+      </c>
+      <c r="B1497" t="s">
+        <v>230</v>
+      </c>
+      <c r="C1497" t="s">
+        <v>202</v>
+      </c>
+      <c r="D1497">
+        <v>9.7880000000000003</v>
+      </c>
+      <c r="G1497" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H1497" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="I1497" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1497">
+        <v>12</v>
+      </c>
+      <c r="K1497" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1497" s="1" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="1498" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1498">
+        <v>6</v>
+      </c>
+      <c r="B1498" t="s">
+        <v>230</v>
+      </c>
+      <c r="C1498" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1498">
+        <v>6.85</v>
+      </c>
+      <c r="G1498" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H1498" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="I1498" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1498">
+        <v>12</v>
+      </c>
+      <c r="K1498" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1498" s="1" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="1499" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1499">
+        <v>7</v>
+      </c>
+      <c r="B1499" t="s">
+        <v>230</v>
+      </c>
+      <c r="C1499" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1499">
+        <v>5.7750000000000004</v>
+      </c>
+      <c r="G1499" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H1499" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="I1499" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1499">
+        <v>12</v>
+      </c>
+      <c r="K1499" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1499" s="1" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="1500" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1500">
+        <v>8</v>
+      </c>
+      <c r="B1500" t="s">
+        <v>230</v>
+      </c>
+      <c r="C1500" t="s">
+        <v>202</v>
+      </c>
+      <c r="D1500">
+        <v>3.5619999999999998</v>
+      </c>
+      <c r="G1500" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H1500" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="I1500" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1500">
+        <v>12</v>
+      </c>
+      <c r="K1500" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1500" s="1" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="1501" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1501">
+        <v>9</v>
+      </c>
+      <c r="B1501" t="s">
+        <v>230</v>
+      </c>
+      <c r="C1501" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1501">
+        <v>5.1440000000000001</v>
+      </c>
+      <c r="G1501" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H1501" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="I1501" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1501">
+        <v>12</v>
+      </c>
+      <c r="K1501" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1501" s="1" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="1502" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1502">
+        <v>10</v>
+      </c>
+      <c r="B1502" t="s">
+        <v>230</v>
+      </c>
+      <c r="D1502">
+        <v>5.12</v>
+      </c>
+      <c r="G1502" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H1502" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="I1502" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1502">
+        <v>12</v>
+      </c>
+      <c r="K1502" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1502" s="1" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="1503" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1503">
+        <v>11</v>
+      </c>
+      <c r="B1503" t="s">
+        <v>230</v>
+      </c>
+      <c r="C1503" t="s">
+        <v>202</v>
+      </c>
+      <c r="D1503">
+        <v>6.7359999999999998</v>
+      </c>
+      <c r="G1503" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H1503" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="I1503" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1503">
+        <v>12</v>
+      </c>
+      <c r="K1503" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1503" s="1" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="1504" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1504">
+        <v>12</v>
+      </c>
+      <c r="B1504" t="s">
+        <v>230</v>
+      </c>
+      <c r="C1504" t="s">
+        <v>202</v>
+      </c>
+      <c r="D1504">
+        <v>10.657999999999999</v>
+      </c>
+      <c r="G1504" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H1504" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="I1504" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1504">
+        <v>12</v>
+      </c>
+      <c r="K1504" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1504" s="1" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="1505" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1505">
+        <v>13</v>
+      </c>
+      <c r="B1505" t="s">
+        <v>230</v>
+      </c>
+      <c r="C1505" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1505">
+        <v>6.9820000000000002</v>
+      </c>
+      <c r="G1505" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H1505" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="I1505" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1505">
+        <v>12</v>
+      </c>
+      <c r="K1505" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1505" s="1" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="1506" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1506">
+        <v>14</v>
+      </c>
+      <c r="B1506" t="s">
+        <v>230</v>
+      </c>
+      <c r="C1506" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1506">
+        <v>7.726</v>
+      </c>
+      <c r="G1506" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H1506" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="I1506" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1506">
+        <v>12</v>
+      </c>
+      <c r="K1506" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1506" s="1" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="1507" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1507">
+        <v>15</v>
+      </c>
+      <c r="B1507" t="s">
+        <v>230</v>
+      </c>
+      <c r="C1507" t="s">
+        <v>202</v>
+      </c>
+      <c r="D1507">
+        <v>11.287000000000001</v>
+      </c>
+      <c r="G1507" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H1507" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="I1507" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1507">
+        <v>12</v>
+      </c>
+      <c r="K1507" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1507" s="1" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="1508" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1508">
+        <v>16</v>
+      </c>
+      <c r="B1508" t="s">
+        <v>230</v>
+      </c>
+      <c r="C1508" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1508">
+        <v>4.548</v>
+      </c>
+      <c r="G1508" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H1508" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="I1508" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1508">
+        <v>12</v>
+      </c>
+      <c r="K1508" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1508" s="1" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="1509" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1509">
+        <v>17</v>
+      </c>
+      <c r="B1509" t="s">
+        <v>230</v>
+      </c>
+      <c r="C1509" t="s">
+        <v>202</v>
+      </c>
+      <c r="D1509">
+        <v>6.6189999999999998</v>
+      </c>
+      <c r="G1509" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H1509" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="I1509" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1509">
+        <v>12</v>
+      </c>
+      <c r="K1509" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1509" s="1" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="1510" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1510">
+        <v>18</v>
+      </c>
+      <c r="B1510" t="s">
+        <v>230</v>
+      </c>
+      <c r="C1510" t="s">
+        <v>202</v>
+      </c>
+      <c r="D1510">
+        <v>8.4849999999999994</v>
+      </c>
+      <c r="G1510" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H1510" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="I1510" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1510">
+        <v>12</v>
+      </c>
+      <c r="K1510" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1510" s="1" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="1511" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1511">
+        <v>19</v>
+      </c>
+      <c r="B1511" t="s">
+        <v>230</v>
+      </c>
+      <c r="C1511" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1511">
+        <v>6.774</v>
+      </c>
+      <c r="G1511" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H1511" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="I1511" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1511">
+        <v>12</v>
+      </c>
+      <c r="K1511" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1511" s="1" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="1512" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1512">
+        <v>20</v>
+      </c>
+      <c r="B1512" t="s">
+        <v>230</v>
+      </c>
+      <c r="C1512" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1512">
+        <v>3.5569999999999999</v>
+      </c>
+      <c r="G1512" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H1512" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="I1512" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1512">
+        <v>12</v>
+      </c>
+      <c r="K1512" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1512" s="1" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="1513" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1513">
+        <v>21</v>
+      </c>
+      <c r="B1513" t="s">
+        <v>230</v>
+      </c>
+      <c r="C1513" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1513">
+        <v>9.3320000000000007</v>
+      </c>
+      <c r="G1513" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H1513" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="I1513" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1513">
+        <v>12</v>
+      </c>
+      <c r="K1513" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1513" s="1" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="1514" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1514">
+        <v>22</v>
+      </c>
+      <c r="B1514" t="s">
+        <v>230</v>
+      </c>
+      <c r="C1514" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1514">
+        <v>5.109</v>
+      </c>
+      <c r="G1514" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H1514" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="I1514" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1514">
+        <v>12</v>
+      </c>
+      <c r="K1514" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1514" s="1" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="1515" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1515">
+        <v>23</v>
+      </c>
+      <c r="B1515" t="s">
+        <v>230</v>
+      </c>
+      <c r="C1515" t="s">
+        <v>202</v>
+      </c>
+      <c r="D1515">
+        <v>9.2089999999999996</v>
+      </c>
+      <c r="G1515" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H1515" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="I1515" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1515">
+        <v>12</v>
+      </c>
+      <c r="K1515" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1515" s="1" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="1516" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1516">
+        <v>24</v>
+      </c>
+      <c r="B1516" t="s">
+        <v>230</v>
+      </c>
+      <c r="C1516" t="s">
+        <v>202</v>
+      </c>
+      <c r="D1516">
+        <v>6.59</v>
+      </c>
+      <c r="G1516" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H1516" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="I1516" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1516">
+        <v>12</v>
+      </c>
+      <c r="K1516" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1516" s="1" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="1517" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1517">
+        <v>25</v>
+      </c>
+      <c r="B1517" t="s">
+        <v>230</v>
+      </c>
+      <c r="C1517" t="s">
+        <v>202</v>
+      </c>
+      <c r="D1517">
+        <v>9.2070000000000007</v>
+      </c>
+      <c r="G1517" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H1517" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="I1517" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1517">
+        <v>12</v>
+      </c>
+      <c r="K1517" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1517" s="1" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="1518" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1518">
+        <v>26</v>
+      </c>
+      <c r="B1518" t="s">
+        <v>230</v>
+      </c>
+      <c r="C1518" t="s">
+        <v>202</v>
+      </c>
+      <c r="D1518">
+        <v>9.74</v>
+      </c>
+      <c r="G1518" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H1518" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="I1518" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1518">
+        <v>12</v>
+      </c>
+      <c r="K1518" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1518" s="1" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="1519" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1519">
+        <v>27</v>
+      </c>
+      <c r="B1519" t="s">
+        <v>230</v>
+      </c>
+      <c r="C1519" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1519">
+        <v>7.04</v>
+      </c>
+      <c r="G1519" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H1519" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="I1519" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1519">
+        <v>12</v>
+      </c>
+      <c r="K1519" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1519" s="1" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="1520" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1520">
+        <v>28</v>
+      </c>
+      <c r="B1520" t="s">
+        <v>230</v>
+      </c>
+      <c r="C1520" t="s">
+        <v>202</v>
+      </c>
+      <c r="D1520">
+        <v>5.22</v>
+      </c>
+      <c r="G1520" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H1520" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="I1520" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1520">
+        <v>12</v>
+      </c>
+      <c r="K1520" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1520" s="1" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="1521" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1521">
+        <v>29</v>
+      </c>
+      <c r="B1521" t="s">
+        <v>230</v>
+      </c>
+      <c r="C1521" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1521">
+        <v>4.6470000000000002</v>
+      </c>
+      <c r="G1521" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H1521" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="I1521" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1521">
+        <v>12</v>
+      </c>
+      <c r="K1521" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1521" s="1" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="1522" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1522">
+        <v>30</v>
+      </c>
+      <c r="B1522" t="s">
+        <v>230</v>
+      </c>
+      <c r="C1522" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1522">
+        <v>8.48</v>
+      </c>
+      <c r="G1522" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H1522" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="I1522" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1522">
+        <v>12</v>
+      </c>
+      <c r="K1522" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1522" s="1" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="1523" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1523">
+        <v>31</v>
+      </c>
+      <c r="B1523" t="s">
+        <v>230</v>
+      </c>
+      <c r="C1523" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1523">
+        <v>6.6769999999999996</v>
+      </c>
+      <c r="G1523" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H1523" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="I1523" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1523">
+        <v>12</v>
+      </c>
+      <c r="K1523" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1523" s="1" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="1524" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1524">
+        <v>32</v>
+      </c>
+      <c r="B1524" t="s">
+        <v>230</v>
+      </c>
+      <c r="C1524" t="s">
+        <v>202</v>
+      </c>
+      <c r="D1524">
+        <v>6.6959999999999997</v>
+      </c>
+      <c r="G1524" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H1524" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="I1524" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1524">
+        <v>12</v>
+      </c>
+      <c r="K1524" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1524" s="1" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="1525" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1525">
+        <v>33</v>
+      </c>
+      <c r="B1525" t="s">
+        <v>230</v>
+      </c>
+      <c r="C1525" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1525">
+        <v>9.2850000000000001</v>
+      </c>
+      <c r="G1525" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H1525" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="I1525" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1525">
+        <v>12</v>
+      </c>
+      <c r="K1525" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1525" s="1" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="1526" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1526">
+        <v>34</v>
+      </c>
+      <c r="B1526" t="s">
+        <v>230</v>
+      </c>
+      <c r="C1526" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1526">
+        <v>6.6029999999999998</v>
+      </c>
+      <c r="G1526" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H1526" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="I1526" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1526">
+        <v>12</v>
+      </c>
+      <c r="K1526" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1526" s="1" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="1527" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1527">
+        <v>35</v>
+      </c>
+      <c r="B1527" t="s">
+        <v>230</v>
+      </c>
+      <c r="C1527" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1527">
+        <v>4.7850000000000001</v>
+      </c>
+      <c r="G1527" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H1527" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="I1527" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1527">
+        <v>12</v>
+      </c>
+      <c r="K1527" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1527" s="1" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="1528" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1528">
+        <v>36</v>
+      </c>
+      <c r="B1528" t="s">
+        <v>230</v>
+      </c>
+      <c r="C1528" t="s">
+        <v>202</v>
+      </c>
+      <c r="D1528">
+        <v>7.3460000000000001</v>
+      </c>
+      <c r="G1528" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H1528" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="I1528" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1528">
+        <v>12</v>
+      </c>
+      <c r="K1528" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1528" s="1" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="1529" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1529">
+        <v>37</v>
+      </c>
+      <c r="B1529" t="s">
+        <v>230</v>
+      </c>
+      <c r="C1529" t="s">
+        <v>202</v>
+      </c>
+      <c r="D1529">
+        <v>9.234</v>
+      </c>
+      <c r="G1529" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H1529" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="I1529" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1529">
+        <v>12</v>
+      </c>
+      <c r="K1529" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1529" s="1" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="1530" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1530">
+        <v>38</v>
+      </c>
+      <c r="B1530" t="s">
+        <v>230</v>
+      </c>
+      <c r="C1530" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1530">
+        <v>7.44</v>
+      </c>
+      <c r="G1530" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H1530" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="I1530" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1530">
+        <v>12</v>
+      </c>
+      <c r="K1530" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1530" s="1" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="1531" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1531">
+        <v>39</v>
+      </c>
+      <c r="B1531" t="s">
+        <v>230</v>
+      </c>
+      <c r="C1531" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1531">
+        <v>4.7549999999999999</v>
+      </c>
+      <c r="G1531" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H1531" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="I1531" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1531">
+        <v>12</v>
+      </c>
+      <c r="K1531" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1531" s="1" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="1532" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1532">
+        <v>40</v>
+      </c>
+      <c r="B1532" t="s">
+        <v>230</v>
+      </c>
+      <c r="C1532" t="s">
+        <v>202</v>
+      </c>
+      <c r="D1532">
+        <v>3.3210000000000002</v>
+      </c>
+      <c r="G1532" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H1532" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="I1532" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1532">
+        <v>12</v>
+      </c>
+      <c r="K1532" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1532" s="1" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="1533" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1533">
+        <v>41</v>
+      </c>
+      <c r="B1533" t="s">
+        <v>230</v>
+      </c>
+      <c r="C1533" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1533">
+        <v>10.071999999999999</v>
+      </c>
+      <c r="G1533" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H1533" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="I1533" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1533">
+        <v>12</v>
+      </c>
+      <c r="K1533" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1533" s="1" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="1534" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1534">
+        <v>42</v>
+      </c>
+      <c r="B1534" t="s">
+        <v>230</v>
+      </c>
+      <c r="C1534" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1534">
+        <v>7.7770000000000001</v>
+      </c>
+      <c r="G1534" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H1534" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="I1534" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1534">
+        <v>12</v>
+      </c>
+      <c r="K1534" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1534" s="1" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="1535" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1535">
+        <v>43</v>
+      </c>
+      <c r="B1535" t="s">
+        <v>230</v>
+      </c>
+      <c r="C1535" t="s">
+        <v>202</v>
+      </c>
+      <c r="D1535">
+        <v>6.66</v>
+      </c>
+      <c r="G1535" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H1535" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="I1535" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1535">
+        <v>12</v>
+      </c>
+      <c r="K1535" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1535" s="1" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="1536" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1536">
+        <v>44</v>
+      </c>
+      <c r="B1536" t="s">
+        <v>230</v>
+      </c>
+      <c r="C1536" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1536">
+        <v>7.2690000000000001</v>
+      </c>
+      <c r="G1536" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H1536" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="I1536" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1536">
+        <v>12</v>
+      </c>
+      <c r="K1536" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1536" s="1" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="1537" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1537">
+        <v>45</v>
+      </c>
+      <c r="B1537" t="s">
+        <v>230</v>
+      </c>
+      <c r="C1537" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1537">
+        <v>10.558</v>
+      </c>
+      <c r="G1537" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H1537" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="I1537" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1537">
+        <v>12</v>
+      </c>
+      <c r="K1537" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1537" s="1" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="1538" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1538">
+        <v>46</v>
+      </c>
+      <c r="B1538" t="s">
+        <v>230</v>
+      </c>
+      <c r="C1538" t="s">
+        <v>703</v>
+      </c>
+      <c r="G1538" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H1538" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="I1538" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1538">
+        <v>12</v>
+      </c>
+      <c r="K1538" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1538" s="1" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="1539" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1539">
+        <v>47</v>
+      </c>
+      <c r="B1539" t="s">
+        <v>230</v>
+      </c>
+      <c r="C1539" t="s">
+        <v>703</v>
+      </c>
+      <c r="E1539" s="1" t="s">
+        <v>1032</v>
+      </c>
+      <c r="G1539" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H1539" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="I1539" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1539">
+        <v>12</v>
+      </c>
+      <c r="K1539" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1539" s="1" t="s">
+        <v>543</v>
       </c>
     </row>
   </sheetData>
@@ -67718,7 +70696,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD836908-61FC-4C6A-BB55-EB17A2B99FDD}">
   <dimension ref="A1:M81"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" workbookViewId="0">
+    <sheetView topLeftCell="A58" workbookViewId="0">
       <selection activeCell="E68" sqref="E68"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
updating data; 2018-09-07 day 8+23 cohort
</commit_message>
<xml_diff>
--- a/Data/2018-08-14_master_datac_2018_collection_year.xlsx
+++ b/Data/2018-08-14_master_datac_2018_collection_year.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hinalkharva\Desktop\Circadian_rhythm_runs_seasonal_timing\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andrew.nguyen\Desktop\Circadian_rhythm_runs_seasonal_timing\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B7EE206-9823-483D-B370-0F28D9BEA8F0}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1774D466-7C6B-495E-B119-165896CE07F0}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9855" yWindow="7665" windowWidth="36360" windowHeight="21135" activeTab="2" xr2:uid="{C7477166-8A7C-B04A-9643-C277FEDCDAAB}"/>
+    <workbookView xWindow="9855" yWindow="7665" windowWidth="36360" windowHeight="21135" activeTab="1" xr2:uid="{C7477166-8A7C-B04A-9643-C277FEDCDAAB}"/>
   </bookViews>
   <sheets>
     <sheet name="Maggot_Collections" sheetId="2" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14425" uniqueCount="1033">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14775" uniqueCount="1048">
   <si>
     <t>Ind_ID</t>
   </si>
@@ -3131,6 +3131,51 @@
   </si>
   <si>
     <t>15:04</t>
+  </si>
+  <si>
+    <t>A2-8-1</t>
+  </si>
+  <si>
+    <t>A2-8-2</t>
+  </si>
+  <si>
+    <t>A2-8-3</t>
+  </si>
+  <si>
+    <t>A2-8-4</t>
+  </si>
+  <si>
+    <t>A2-8-5</t>
+  </si>
+  <si>
+    <t>A2-8-6</t>
+  </si>
+  <si>
+    <t>A2-8-7</t>
+  </si>
+  <si>
+    <t>A2-8-8</t>
+  </si>
+  <si>
+    <t>A2-8-9</t>
+  </si>
+  <si>
+    <t>A2-8-10</t>
+  </si>
+  <si>
+    <t>A2-8-11</t>
+  </si>
+  <si>
+    <t>A2-8-12</t>
+  </si>
+  <si>
+    <t>A2-8-13</t>
+  </si>
+  <si>
+    <t>A2-8-14</t>
+  </si>
+  <si>
+    <t>A2-8-15</t>
   </si>
 </sst>
 </file>
@@ -14130,11 +14175,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92725FB9-1A17-2546-9DFA-6C0D39437891}">
-  <dimension ref="A1:AS1539"/>
+  <dimension ref="A1:AS1589"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1518" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D1538" sqref="D1538"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A1563" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G1581" sqref="G1581"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -70593,7 +70638,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="1537" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1537" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1537">
         <v>45</v>
       </c>
@@ -70625,7 +70670,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="1538" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1538" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1538">
         <v>46</v>
       </c>
@@ -70654,7 +70699,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="1539" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1539" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1539">
         <v>47</v>
       </c>
@@ -70684,6 +70729,1596 @@
       </c>
       <c r="T1539" s="1" t="s">
         <v>543</v>
+      </c>
+    </row>
+    <row r="1540" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1540">
+        <v>1</v>
+      </c>
+      <c r="C1540" t="s">
+        <v>60</v>
+      </c>
+      <c r="G1540" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I1540" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J1540">
+        <v>23</v>
+      </c>
+      <c r="K1540" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1540" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="Y1540" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z1540" t="str">
+        <f>"A2-8"&amp;Y1540&amp;"-"&amp;AC1540</f>
+        <v>A2-8RT-A1</v>
+      </c>
+      <c r="AC1540" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="1541" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1541">
+        <v>1</v>
+      </c>
+      <c r="C1541" t="s">
+        <v>60</v>
+      </c>
+      <c r="G1541" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I1541" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J1541">
+        <v>23</v>
+      </c>
+      <c r="K1541" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1541" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="Y1541" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z1541" t="str">
+        <f>"A2-8"&amp;Y1541&amp;"-"&amp;AC1541</f>
+        <v>A2-8SO-A1</v>
+      </c>
+      <c r="AC1541" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="1542" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1542">
+        <v>1</v>
+      </c>
+      <c r="C1542" t="s">
+        <v>60</v>
+      </c>
+      <c r="G1542" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1542" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J1542">
+        <v>8</v>
+      </c>
+      <c r="K1542" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1542" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="Y1542" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z1542" t="s">
+        <v>1033</v>
+      </c>
+    </row>
+    <row r="1543" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1543">
+        <v>2</v>
+      </c>
+      <c r="C1543" t="s">
+        <v>60</v>
+      </c>
+      <c r="G1543" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1543" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J1543">
+        <v>8</v>
+      </c>
+      <c r="K1543" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1543" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="Y1543" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z1543" t="str">
+        <f t="shared" ref="Z1543:Z1545" si="21">"A2-8"&amp;Y1543&amp;"-"&amp;AC1543</f>
+        <v>A2-8RT-A2</v>
+      </c>
+      <c r="AC1543" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="1544" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1544">
+        <v>2</v>
+      </c>
+      <c r="C1544" t="s">
+        <v>60</v>
+      </c>
+      <c r="G1544" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1544" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J1544">
+        <v>8</v>
+      </c>
+      <c r="K1544" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1544" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="Y1544" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z1544" t="str">
+        <f t="shared" si="21"/>
+        <v>A2-8SO-A2</v>
+      </c>
+      <c r="AC1544" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="1545" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1545">
+        <v>3</v>
+      </c>
+      <c r="C1545" t="s">
+        <v>60</v>
+      </c>
+      <c r="G1545" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1545" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J1545">
+        <v>8</v>
+      </c>
+      <c r="K1545" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1545" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="Y1545" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z1545" t="str">
+        <f t="shared" si="21"/>
+        <v>A2-8SO-H1</v>
+      </c>
+      <c r="AC1545" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="1546" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1546">
+        <v>2</v>
+      </c>
+      <c r="C1546" t="s">
+        <v>59</v>
+      </c>
+      <c r="G1546" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I1546" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J1546">
+        <v>23</v>
+      </c>
+      <c r="K1546" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1546" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="Y1546" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z1546" t="s">
+        <v>1034</v>
+      </c>
+    </row>
+    <row r="1547" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1547">
+        <v>3</v>
+      </c>
+      <c r="C1547" t="s">
+        <v>59</v>
+      </c>
+      <c r="G1547" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I1547" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J1547">
+        <v>23</v>
+      </c>
+      <c r="K1547" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1547" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="Y1547" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z1547" t="s">
+        <v>1035</v>
+      </c>
+    </row>
+    <row r="1548" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1548">
+        <v>4</v>
+      </c>
+      <c r="C1548" t="s">
+        <v>59</v>
+      </c>
+      <c r="G1548" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I1548" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J1548">
+        <v>23</v>
+      </c>
+      <c r="K1548" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1548" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="Y1548" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z1548" t="s">
+        <v>1036</v>
+      </c>
+    </row>
+    <row r="1549" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1549">
+        <v>3</v>
+      </c>
+      <c r="C1549" t="s">
+        <v>59</v>
+      </c>
+      <c r="G1549" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I1549" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J1549">
+        <v>23</v>
+      </c>
+      <c r="K1549" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1549" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="Y1549" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z1549" t="str">
+        <f t="shared" ref="Z1549:Z1554" si="22">"A2-8"&amp;Y1549&amp;"-"&amp;AC1549</f>
+        <v>A2-8RT-A3</v>
+      </c>
+      <c r="AC1549" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="1550" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1550">
+        <v>4</v>
+      </c>
+      <c r="C1550" t="s">
+        <v>59</v>
+      </c>
+      <c r="G1550" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I1550" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J1550">
+        <v>23</v>
+      </c>
+      <c r="K1550" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1550" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="Y1550" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z1550" t="str">
+        <f t="shared" si="22"/>
+        <v>A2-8RT-A4</v>
+      </c>
+      <c r="AC1550" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="1551" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1551">
+        <v>5</v>
+      </c>
+      <c r="C1551" t="s">
+        <v>59</v>
+      </c>
+      <c r="G1551" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I1551" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J1551">
+        <v>23</v>
+      </c>
+      <c r="K1551" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1551" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="Y1551" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z1551" t="str">
+        <f t="shared" si="22"/>
+        <v>A2-8RT-A5</v>
+      </c>
+      <c r="AC1551" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="1552" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1552">
+        <v>4</v>
+      </c>
+      <c r="C1552" t="s">
+        <v>59</v>
+      </c>
+      <c r="G1552" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I1552" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J1552">
+        <v>23</v>
+      </c>
+      <c r="K1552" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1552" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="Y1552" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z1552" t="str">
+        <f t="shared" si="22"/>
+        <v>A2-8SO-A3</v>
+      </c>
+      <c r="AC1552" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="1553" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1553">
+        <v>5</v>
+      </c>
+      <c r="C1553" t="s">
+        <v>59</v>
+      </c>
+      <c r="G1553" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I1553" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J1553">
+        <v>23</v>
+      </c>
+      <c r="K1553" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1553" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="Y1553" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z1553" t="str">
+        <f t="shared" si="22"/>
+        <v>A2-8SO-A4</v>
+      </c>
+      <c r="AC1553" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="1554" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1554">
+        <v>6</v>
+      </c>
+      <c r="C1554" t="s">
+        <v>59</v>
+      </c>
+      <c r="G1554" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I1554" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J1554">
+        <v>23</v>
+      </c>
+      <c r="K1554" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1554" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="Y1554" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z1554" t="str">
+        <f t="shared" si="22"/>
+        <v>A2-8SO-A5</v>
+      </c>
+      <c r="AC1554" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="1555" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1555">
+        <v>5</v>
+      </c>
+      <c r="C1555" t="s">
+        <v>202</v>
+      </c>
+      <c r="G1555" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1555" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J1555">
+        <v>8</v>
+      </c>
+      <c r="K1555" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1555" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="Y1555" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z1555" t="s">
+        <v>1037</v>
+      </c>
+    </row>
+    <row r="1556" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1556">
+        <v>6</v>
+      </c>
+      <c r="C1556" t="s">
+        <v>202</v>
+      </c>
+      <c r="G1556" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1556" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J1556">
+        <v>8</v>
+      </c>
+      <c r="K1556" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1556" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="Y1556" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z1556" t="s">
+        <v>1038</v>
+      </c>
+    </row>
+    <row r="1557" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1557">
+        <v>7</v>
+      </c>
+      <c r="C1557" t="s">
+        <v>202</v>
+      </c>
+      <c r="G1557" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1557" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J1557">
+        <v>8</v>
+      </c>
+      <c r="K1557" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1557" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="Y1557" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z1557" t="s">
+        <v>1039</v>
+      </c>
+    </row>
+    <row r="1558" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1558">
+        <v>8</v>
+      </c>
+      <c r="C1558" t="s">
+        <v>202</v>
+      </c>
+      <c r="G1558" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1558" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J1558">
+        <v>8</v>
+      </c>
+      <c r="K1558" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1558" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="Y1558" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z1558" t="s">
+        <v>1040</v>
+      </c>
+    </row>
+    <row r="1559" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1559">
+        <v>9</v>
+      </c>
+      <c r="C1559" t="s">
+        <v>202</v>
+      </c>
+      <c r="G1559" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1559" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J1559">
+        <v>8</v>
+      </c>
+      <c r="K1559" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1559" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="Y1559" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z1559" t="s">
+        <v>1041</v>
+      </c>
+    </row>
+    <row r="1560" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1560">
+        <v>10</v>
+      </c>
+      <c r="C1560" t="s">
+        <v>202</v>
+      </c>
+      <c r="G1560" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1560" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J1560">
+        <v>8</v>
+      </c>
+      <c r="K1560" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1560" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="Y1560" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z1560" t="s">
+        <v>1042</v>
+      </c>
+    </row>
+    <row r="1561" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1561">
+        <v>11</v>
+      </c>
+      <c r="C1561" t="s">
+        <v>202</v>
+      </c>
+      <c r="G1561" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1561" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J1561">
+        <v>8</v>
+      </c>
+      <c r="K1561" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1561" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="Y1561" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z1561" t="s">
+        <v>1043</v>
+      </c>
+    </row>
+    <row r="1562" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1562">
+        <v>12</v>
+      </c>
+      <c r="C1562" t="s">
+        <v>202</v>
+      </c>
+      <c r="G1562" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1562" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J1562">
+        <v>8</v>
+      </c>
+      <c r="K1562" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1562" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="Y1562" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z1562" t="s">
+        <v>1044</v>
+      </c>
+    </row>
+    <row r="1563" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1563">
+        <v>13</v>
+      </c>
+      <c r="C1563" t="s">
+        <v>202</v>
+      </c>
+      <c r="G1563" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1563" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J1563">
+        <v>8</v>
+      </c>
+      <c r="K1563" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1563" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="Y1563" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z1563" t="s">
+        <v>1045</v>
+      </c>
+    </row>
+    <row r="1564" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1564">
+        <v>14</v>
+      </c>
+      <c r="C1564" t="s">
+        <v>202</v>
+      </c>
+      <c r="G1564" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1564" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J1564">
+        <v>8</v>
+      </c>
+      <c r="K1564" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1564" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="Y1564" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z1564" t="s">
+        <v>1046</v>
+      </c>
+    </row>
+    <row r="1565" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1565">
+        <v>15</v>
+      </c>
+      <c r="C1565" t="s">
+        <v>202</v>
+      </c>
+      <c r="G1565" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1565" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J1565">
+        <v>8</v>
+      </c>
+      <c r="K1565" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1565" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="Y1565" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z1565" t="s">
+        <v>1047</v>
+      </c>
+    </row>
+    <row r="1566" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1566">
+        <v>6</v>
+      </c>
+      <c r="C1566" t="s">
+        <v>202</v>
+      </c>
+      <c r="G1566" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1566" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J1566">
+        <v>8</v>
+      </c>
+      <c r="K1566" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1566" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="Y1566" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z1566" t="str">
+        <f t="shared" ref="Z1566:Z1589" si="23">"A2-8"&amp;Y1566&amp;"-"&amp;AC1566</f>
+        <v>A2-8RT-E1</v>
+      </c>
+      <c r="AC1566" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="1567" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1567">
+        <v>7</v>
+      </c>
+      <c r="C1567" t="s">
+        <v>202</v>
+      </c>
+      <c r="G1567" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1567" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J1567">
+        <v>8</v>
+      </c>
+      <c r="K1567" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1567" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="Y1567" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z1567" t="str">
+        <f t="shared" si="23"/>
+        <v>A2-8RT-E2</v>
+      </c>
+      <c r="AC1567" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="1568" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1568">
+        <v>8</v>
+      </c>
+      <c r="C1568" t="s">
+        <v>202</v>
+      </c>
+      <c r="G1568" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1568" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J1568">
+        <v>8</v>
+      </c>
+      <c r="K1568" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1568" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="Y1568" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z1568" t="str">
+        <f t="shared" si="23"/>
+        <v>A2-8RT-E3</v>
+      </c>
+      <c r="AC1568" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="1569" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1569">
+        <v>9</v>
+      </c>
+      <c r="C1569" t="s">
+        <v>202</v>
+      </c>
+      <c r="G1569" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1569" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J1569">
+        <v>8</v>
+      </c>
+      <c r="K1569" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1569" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="Y1569" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z1569" t="str">
+        <f t="shared" si="23"/>
+        <v>A2-8RT-E4</v>
+      </c>
+      <c r="AC1569" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="1570" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1570">
+        <v>10</v>
+      </c>
+      <c r="C1570" t="s">
+        <v>202</v>
+      </c>
+      <c r="G1570" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1570" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J1570">
+        <v>8</v>
+      </c>
+      <c r="K1570" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1570" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="Y1570" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z1570" t="str">
+        <f t="shared" si="23"/>
+        <v>A2-8RT-E5</v>
+      </c>
+      <c r="AC1570" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="1571" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1571">
+        <v>11</v>
+      </c>
+      <c r="C1571" t="s">
+        <v>202</v>
+      </c>
+      <c r="G1571" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1571" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J1571">
+        <v>8</v>
+      </c>
+      <c r="K1571" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1571" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="Y1571" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z1571" t="str">
+        <f t="shared" si="23"/>
+        <v>A2-8RT-E6</v>
+      </c>
+      <c r="AC1571" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="1572" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1572">
+        <v>12</v>
+      </c>
+      <c r="C1572" t="s">
+        <v>202</v>
+      </c>
+      <c r="G1572" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1572" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J1572">
+        <v>8</v>
+      </c>
+      <c r="K1572" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1572" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="Y1572" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z1572" t="str">
+        <f t="shared" si="23"/>
+        <v>A2-8RT-E7</v>
+      </c>
+      <c r="AC1572" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="1573" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1573">
+        <v>13</v>
+      </c>
+      <c r="C1573" t="s">
+        <v>202</v>
+      </c>
+      <c r="G1573" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1573" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J1573">
+        <v>8</v>
+      </c>
+      <c r="K1573" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1573" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="Y1573" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z1573" t="str">
+        <f t="shared" si="23"/>
+        <v>A2-8RT-E8</v>
+      </c>
+      <c r="AC1573" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="1574" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1574">
+        <v>14</v>
+      </c>
+      <c r="C1574" t="s">
+        <v>202</v>
+      </c>
+      <c r="G1574" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1574" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J1574">
+        <v>8</v>
+      </c>
+      <c r="K1574" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1574" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="Y1574" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z1574" t="str">
+        <f t="shared" si="23"/>
+        <v>A2-8RT-E9</v>
+      </c>
+      <c r="AC1574" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="1575" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1575">
+        <v>15</v>
+      </c>
+      <c r="C1575" t="s">
+        <v>202</v>
+      </c>
+      <c r="G1575" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1575" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J1575">
+        <v>8</v>
+      </c>
+      <c r="K1575" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1575" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="Y1575" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z1575" t="str">
+        <f t="shared" si="23"/>
+        <v>A2-8RT-E10</v>
+      </c>
+      <c r="AC1575" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="1576" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1576">
+        <v>16</v>
+      </c>
+      <c r="C1576" t="s">
+        <v>202</v>
+      </c>
+      <c r="G1576" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1576" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J1576">
+        <v>8</v>
+      </c>
+      <c r="K1576" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1576" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="Y1576" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z1576" t="str">
+        <f t="shared" si="23"/>
+        <v>A2-8RT-E11</v>
+      </c>
+      <c r="AC1576" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="1577" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1577">
+        <v>17</v>
+      </c>
+      <c r="C1577" t="s">
+        <v>202</v>
+      </c>
+      <c r="G1577" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1577" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J1577">
+        <v>8</v>
+      </c>
+      <c r="K1577" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1577" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="Y1577" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z1577" t="str">
+        <f t="shared" si="23"/>
+        <v>A2-8RT-E12</v>
+      </c>
+      <c r="AC1577" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="1578" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1578">
+        <v>7</v>
+      </c>
+      <c r="C1578" t="s">
+        <v>202</v>
+      </c>
+      <c r="G1578" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1578" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J1578">
+        <v>8</v>
+      </c>
+      <c r="K1578" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1578" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="Y1578" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z1578" t="str">
+        <f t="shared" si="23"/>
+        <v>A2-8SO-E1</v>
+      </c>
+      <c r="AC1578" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="1579" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1579">
+        <v>8</v>
+      </c>
+      <c r="C1579" t="s">
+        <v>202</v>
+      </c>
+      <c r="G1579" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1579" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J1579">
+        <v>8</v>
+      </c>
+      <c r="K1579" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1579" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="Y1579" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z1579" t="str">
+        <f t="shared" si="23"/>
+        <v>A2-8SO-E2</v>
+      </c>
+      <c r="AC1579" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="1580" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1580">
+        <v>9</v>
+      </c>
+      <c r="C1580" t="s">
+        <v>202</v>
+      </c>
+      <c r="G1580" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1580" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J1580">
+        <v>8</v>
+      </c>
+      <c r="K1580" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1580" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="Y1580" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z1580" t="str">
+        <f t="shared" si="23"/>
+        <v>A2-8SO-E3</v>
+      </c>
+      <c r="AC1580" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="1581" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1581">
+        <v>10</v>
+      </c>
+      <c r="C1581" t="s">
+        <v>202</v>
+      </c>
+      <c r="G1581" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1581" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J1581">
+        <v>8</v>
+      </c>
+      <c r="K1581" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1581" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="Y1581" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z1581" t="str">
+        <f t="shared" si="23"/>
+        <v>A2-8SO-E4</v>
+      </c>
+      <c r="AC1581" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="1582" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1582">
+        <v>11</v>
+      </c>
+      <c r="C1582" t="s">
+        <v>202</v>
+      </c>
+      <c r="G1582" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1582" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J1582">
+        <v>8</v>
+      </c>
+      <c r="K1582" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1582" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="Y1582" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z1582" t="str">
+        <f t="shared" si="23"/>
+        <v>A2-8SO-E5</v>
+      </c>
+      <c r="AC1582" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="1583" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1583">
+        <v>12</v>
+      </c>
+      <c r="C1583" t="s">
+        <v>202</v>
+      </c>
+      <c r="G1583" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1583" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J1583">
+        <v>8</v>
+      </c>
+      <c r="K1583" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1583" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="Y1583" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z1583" t="str">
+        <f t="shared" si="23"/>
+        <v>A2-8SO-E6</v>
+      </c>
+      <c r="AC1583" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="1584" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1584">
+        <v>13</v>
+      </c>
+      <c r="C1584" t="s">
+        <v>202</v>
+      </c>
+      <c r="G1584" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1584" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J1584">
+        <v>8</v>
+      </c>
+      <c r="K1584" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1584" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="Y1584" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z1584" t="str">
+        <f t="shared" si="23"/>
+        <v>A2-8SO-E7</v>
+      </c>
+      <c r="AC1584" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="1585" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1585">
+        <v>14</v>
+      </c>
+      <c r="C1585" t="s">
+        <v>202</v>
+      </c>
+      <c r="G1585" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1585" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J1585">
+        <v>8</v>
+      </c>
+      <c r="K1585" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1585" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="Y1585" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z1585" t="str">
+        <f t="shared" si="23"/>
+        <v>A2-8SO-E8</v>
+      </c>
+      <c r="AC1585" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="1586" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1586">
+        <v>15</v>
+      </c>
+      <c r="C1586" t="s">
+        <v>202</v>
+      </c>
+      <c r="G1586" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1586" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J1586">
+        <v>8</v>
+      </c>
+      <c r="K1586" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1586" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="Y1586" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z1586" t="str">
+        <f t="shared" si="23"/>
+        <v>A2-8SO-E9</v>
+      </c>
+      <c r="AC1586" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="1587" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1587">
+        <v>16</v>
+      </c>
+      <c r="C1587" t="s">
+        <v>202</v>
+      </c>
+      <c r="G1587" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1587" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J1587">
+        <v>8</v>
+      </c>
+      <c r="K1587" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1587" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="Y1587" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z1587" t="str">
+        <f t="shared" si="23"/>
+        <v>A2-8SO-E10</v>
+      </c>
+      <c r="AC1587" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="1588" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1588">
+        <v>17</v>
+      </c>
+      <c r="C1588" t="s">
+        <v>202</v>
+      </c>
+      <c r="G1588" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1588" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J1588">
+        <v>8</v>
+      </c>
+      <c r="K1588" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1588" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="Y1588" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z1588" t="str">
+        <f t="shared" si="23"/>
+        <v>A2-8SO-E11</v>
+      </c>
+      <c r="AC1588" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="1589" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1589">
+        <v>18</v>
+      </c>
+      <c r="C1589" t="s">
+        <v>202</v>
+      </c>
+      <c r="G1589" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1589" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J1589">
+        <v>8</v>
+      </c>
+      <c r="K1589" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1589" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="Y1589" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z1589" t="str">
+        <f t="shared" si="23"/>
+        <v>A2-8SO-E12</v>
+      </c>
+      <c r="AC1589" t="s">
+        <v>176</v>
       </c>
     </row>
   </sheetData>
@@ -70696,7 +72331,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD836908-61FC-4C6A-BB55-EB17A2B99FDD}">
   <dimension ref="A1:M81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+    <sheetView topLeftCell="A55" workbookViewId="0">
       <selection activeCell="I75" sqref="I75"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
entering data for cohort 9 + 24; 2018-09-08 day 14 weights
</commit_message>
<xml_diff>
--- a/Data/2018-08-14_master_datac_2018_collection_year.xlsx
+++ b/Data/2018-08-14_master_datac_2018_collection_year.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andrew.nguyen\Desktop\Circadian_rhythm_runs_seasonal_timing\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1774D466-7C6B-495E-B119-165896CE07F0}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CF50C1B-DA83-48FE-9189-170B76194D81}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9855" yWindow="7665" windowWidth="36360" windowHeight="21135" activeTab="1" xr2:uid="{C7477166-8A7C-B04A-9643-C277FEDCDAAB}"/>
   </bookViews>
@@ -14177,9 +14177,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92725FB9-1A17-2546-9DFA-6C0D39437891}">
   <dimension ref="A1:AS1589"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1563" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G1581" sqref="G1581"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A1058" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P1084" sqref="P1084"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -48897,6 +48897,12 @@
       <c r="N990">
         <v>0.1599476</v>
       </c>
+      <c r="O990">
+        <v>3.8660000000000001</v>
+      </c>
+      <c r="P990" s="64">
+        <v>0.50347222222222221</v>
+      </c>
       <c r="T990" s="1" t="s">
         <v>213</v>
       </c>
@@ -48947,6 +48953,9 @@
       <c r="N991">
         <v>0.45276509999999998</v>
       </c>
+      <c r="O991">
+        <v>5.8639999999999999</v>
+      </c>
       <c r="T991" s="1" t="s">
         <v>213</v>
       </c>
@@ -48997,6 +49006,9 @@
       <c r="N992" s="21">
         <v>4.0381090000000001E-2</v>
       </c>
+      <c r="O992">
+        <v>6.5209999999999999</v>
+      </c>
       <c r="T992" s="1" t="s">
         <v>213</v>
       </c>
@@ -49044,6 +49056,9 @@
       <c r="N993">
         <v>0.35760560000000002</v>
       </c>
+      <c r="O993">
+        <v>2.5350000000000001</v>
+      </c>
       <c r="T993" s="1" t="s">
         <v>213</v>
       </c>
@@ -49091,6 +49106,9 @@
       <c r="N994" s="21">
         <v>6.4647609999999994E-2</v>
       </c>
+      <c r="O994">
+        <v>5.944</v>
+      </c>
       <c r="T994" s="1" t="s">
         <v>213</v>
       </c>
@@ -49138,6 +49156,9 @@
       <c r="N995">
         <v>0.1237704</v>
       </c>
+      <c r="O995">
+        <v>8.7119999999999997</v>
+      </c>
       <c r="T995" s="1" t="s">
         <v>213</v>
       </c>
@@ -49188,6 +49209,9 @@
       <c r="N996" s="21">
         <v>6.7688979999999996E-2</v>
       </c>
+      <c r="O996">
+        <v>10.154</v>
+      </c>
       <c r="T996" s="1" t="s">
         <v>213</v>
       </c>
@@ -49238,6 +49262,9 @@
       <c r="N997" s="21">
         <v>6.9644049999999999E-2</v>
       </c>
+      <c r="O997">
+        <v>7.5780000000000003</v>
+      </c>
       <c r="T997" s="1" t="s">
         <v>213</v>
       </c>
@@ -49288,6 +49315,9 @@
       <c r="N998">
         <v>0.37370199999999998</v>
       </c>
+      <c r="O998">
+        <v>5.069</v>
+      </c>
       <c r="T998" s="1" t="s">
         <v>213</v>
       </c>
@@ -49338,6 +49368,9 @@
       <c r="N999">
         <v>0.39185619999999999</v>
       </c>
+      <c r="O999">
+        <v>3.093</v>
+      </c>
       <c r="T999" s="1" t="s">
         <v>213</v>
       </c>
@@ -49388,6 +49421,9 @@
       <c r="N1000">
         <v>0.1216961</v>
       </c>
+      <c r="O1000">
+        <v>7.6280000000000001</v>
+      </c>
       <c r="T1000" s="1" t="s">
         <v>213</v>
       </c>
@@ -49438,6 +49474,9 @@
       <c r="N1001" s="21">
         <v>5.6496449999999997E-2</v>
       </c>
+      <c r="O1001">
+        <v>4.6539999999999999</v>
+      </c>
       <c r="T1001" s="1" t="s">
         <v>213</v>
       </c>
@@ -49485,6 +49524,9 @@
       <c r="N1002" s="21">
         <v>5.0329440000000003E-2</v>
       </c>
+      <c r="O1002">
+        <v>8.1679999999999993</v>
+      </c>
       <c r="T1002" s="1" t="s">
         <v>213</v>
       </c>
@@ -49532,6 +49574,9 @@
       <c r="N1003" s="21">
         <v>7.7695219999999995E-2</v>
       </c>
+      <c r="O1003">
+        <v>6.04</v>
+      </c>
       <c r="T1003" s="1" t="s">
         <v>213</v>
       </c>
@@ -49582,6 +49627,9 @@
       <c r="N1004" s="21">
         <v>8.1830490000000006E-2</v>
       </c>
+      <c r="O1004">
+        <v>6.1619999999999999</v>
+      </c>
       <c r="T1004" s="1" t="s">
         <v>213</v>
       </c>
@@ -49629,6 +49677,9 @@
       <c r="N1005" s="21">
         <v>7.4962589999999996E-2</v>
       </c>
+      <c r="O1005">
+        <v>6.9690000000000003</v>
+      </c>
       <c r="T1005" s="1" t="s">
         <v>213</v>
       </c>
@@ -49679,6 +49730,9 @@
       <c r="N1006" s="21">
         <v>6.2480430000000003E-2</v>
       </c>
+      <c r="O1006">
+        <v>7.3609999999999998</v>
+      </c>
       <c r="T1006" s="1" t="s">
         <v>213</v>
       </c>
@@ -49726,6 +49780,9 @@
       <c r="N1007" s="21">
         <v>5.5404040000000002E-2</v>
       </c>
+      <c r="O1007">
+        <v>5.7240000000000002</v>
+      </c>
       <c r="T1007" s="1" t="s">
         <v>213</v>
       </c>
@@ -49776,6 +49833,9 @@
       <c r="N1008" s="21">
         <v>4.8383839999999997E-2</v>
       </c>
+      <c r="O1008">
+        <v>6.915</v>
+      </c>
       <c r="T1008" s="1" t="s">
         <v>213</v>
       </c>
@@ -49826,6 +49886,9 @@
       <c r="N1009">
         <v>0.48377959999999998</v>
       </c>
+      <c r="O1009">
+        <v>5.2919999999999998</v>
+      </c>
       <c r="T1009" s="1" t="s">
         <v>213</v>
       </c>
@@ -49876,6 +49939,9 @@
       <c r="N1010" s="21">
         <v>5.4492539999999999E-2</v>
       </c>
+      <c r="O1010">
+        <v>7.4740000000000002</v>
+      </c>
       <c r="T1010" s="1" t="s">
         <v>213</v>
       </c>
@@ -49926,6 +49992,9 @@
       <c r="N1011" s="21">
         <v>7.0734630000000007E-2</v>
       </c>
+      <c r="O1011">
+        <v>6.5780000000000003</v>
+      </c>
       <c r="T1011" s="1" t="s">
         <v>213</v>
       </c>
@@ -49976,6 +50045,9 @@
       <c r="N1012">
         <v>0.32921420000000001</v>
       </c>
+      <c r="O1012">
+        <v>4.359</v>
+      </c>
       <c r="T1012" s="1" t="s">
         <v>213</v>
       </c>
@@ -50023,6 +50095,9 @@
       <c r="N1013" s="21">
         <v>9.3297779999999997E-2</v>
       </c>
+      <c r="O1013">
+        <v>7.157</v>
+      </c>
       <c r="T1013" s="1" t="s">
         <v>213</v>
       </c>
@@ -50070,6 +50145,9 @@
       <c r="N1014" s="21">
         <v>5.9871340000000002E-2</v>
       </c>
+      <c r="O1014">
+        <v>8.0410000000000004</v>
+      </c>
       <c r="T1014" s="1" t="s">
         <v>213</v>
       </c>
@@ -50117,6 +50195,9 @@
       <c r="N1015" s="21">
         <v>9.1106820000000005E-2</v>
       </c>
+      <c r="O1015">
+        <v>6.9279999999999999</v>
+      </c>
       <c r="T1015" s="1" t="s">
         <v>213</v>
       </c>
@@ -50167,6 +50248,9 @@
       <c r="N1016" s="21">
         <v>7.4969049999999995E-2</v>
       </c>
+      <c r="O1016">
+        <v>6.2720000000000002</v>
+      </c>
       <c r="T1016" s="1" t="s">
         <v>213</v>
       </c>
@@ -50217,6 +50301,9 @@
       <c r="N1017">
         <v>0.2690111</v>
       </c>
+      <c r="O1017">
+        <v>3.1739999999999999</v>
+      </c>
       <c r="T1017" s="1" t="s">
         <v>213</v>
       </c>
@@ -50267,6 +50354,9 @@
       <c r="N1018" s="21">
         <v>7.4936610000000001E-2</v>
       </c>
+      <c r="O1018">
+        <v>7.1539999999999999</v>
+      </c>
       <c r="T1018" s="1" t="s">
         <v>213</v>
       </c>
@@ -50317,6 +50407,9 @@
       <c r="N1019" s="21">
         <v>9.009578E-2</v>
       </c>
+      <c r="O1019">
+        <v>7.274</v>
+      </c>
       <c r="T1019" s="1" t="s">
         <v>213</v>
       </c>
@@ -50367,6 +50460,9 @@
       <c r="N1020" s="21">
         <v>7.5274859999999999E-2</v>
       </c>
+      <c r="O1020">
+        <v>6.7649999999999997</v>
+      </c>
       <c r="T1020" s="1" t="s">
         <v>213</v>
       </c>
@@ -50417,6 +50513,9 @@
       <c r="N1021" s="21">
         <v>8.6463960000000006E-2</v>
       </c>
+      <c r="O1021">
+        <v>8.6769999999999996</v>
+      </c>
       <c r="T1021" s="1" t="s">
         <v>213</v>
       </c>
@@ -50464,6 +50563,9 @@
       <c r="N1022" s="21">
         <v>7.8758170000000002E-2</v>
       </c>
+      <c r="O1022">
+        <v>7.0650000000000004</v>
+      </c>
       <c r="T1022" s="1" t="s">
         <v>213</v>
       </c>
@@ -50514,6 +50616,9 @@
       <c r="N1023" s="21">
         <v>9.1868320000000003E-2</v>
       </c>
+      <c r="O1023">
+        <v>6.4749999999999996</v>
+      </c>
       <c r="T1023" s="1" t="s">
         <v>213</v>
       </c>
@@ -50561,6 +50666,9 @@
       <c r="N1024">
         <v>0.30310769999999998</v>
       </c>
+      <c r="O1024">
+        <v>3.9529999999999998</v>
+      </c>
       <c r="T1024" s="1" t="s">
         <v>213</v>
       </c>
@@ -50608,6 +50716,9 @@
       <c r="N1025" s="21">
         <v>6.4114069999999995E-2</v>
       </c>
+      <c r="O1025">
+        <v>6.383</v>
+      </c>
       <c r="T1025" s="1" t="s">
         <v>213</v>
       </c>
@@ -50658,6 +50769,9 @@
       <c r="N1026">
         <v>0.1605722</v>
       </c>
+      <c r="O1026">
+        <v>8.75</v>
+      </c>
       <c r="T1026" s="1" t="s">
         <v>213</v>
       </c>
@@ -50705,6 +50819,9 @@
       <c r="N1027">
         <v>0.52054400000000001</v>
       </c>
+      <c r="O1027">
+        <v>6.1429999999999998</v>
+      </c>
       <c r="T1027" s="1" t="s">
         <v>213</v>
       </c>
@@ -50755,6 +50872,9 @@
       <c r="N1028" s="21">
         <v>7.247344E-2</v>
       </c>
+      <c r="O1028">
+        <v>5.0549999999999997</v>
+      </c>
       <c r="T1028" s="1" t="s">
         <v>213</v>
       </c>
@@ -50805,6 +50925,9 @@
       <c r="N1029">
         <v>0.43283549999999998</v>
       </c>
+      <c r="O1029">
+        <v>6.0220000000000002</v>
+      </c>
       <c r="T1029" s="1" t="s">
         <v>213</v>
       </c>
@@ -50852,6 +50975,9 @@
       <c r="N1030">
         <v>0.5201945</v>
       </c>
+      <c r="O1030">
+        <v>4.7859999999999996</v>
+      </c>
       <c r="T1030" s="1" t="s">
         <v>213</v>
       </c>
@@ -50902,6 +51028,9 @@
       <c r="N1031" s="21">
         <v>6.5045919999999993E-2</v>
       </c>
+      <c r="O1031">
+        <v>4.7619999999999996</v>
+      </c>
       <c r="T1031" s="1" t="s">
         <v>213</v>
       </c>
@@ -50952,6 +51081,9 @@
       <c r="N1032" s="21">
         <v>5.0732770000000003E-2</v>
       </c>
+      <c r="O1032">
+        <v>9.3970000000000002</v>
+      </c>
       <c r="T1032" s="1" t="s">
         <v>213</v>
       </c>
@@ -50999,6 +51131,9 @@
       <c r="N1033" s="21">
         <v>4.7503950000000003E-2</v>
       </c>
+      <c r="O1033">
+        <v>4.6040000000000001</v>
+      </c>
       <c r="T1033" s="1" t="s">
         <v>213</v>
       </c>
@@ -51049,6 +51184,9 @@
       <c r="N1034">
         <v>0.13220019999999999</v>
       </c>
+      <c r="O1034">
+        <v>2.9</v>
+      </c>
       <c r="T1034" s="1" t="s">
         <v>213</v>
       </c>
@@ -51137,6 +51275,9 @@
       <c r="N1036" s="21">
         <v>9.6405880000000003E-3</v>
       </c>
+      <c r="P1036" s="64">
+        <v>0.51111111111111118</v>
+      </c>
       <c r="T1036" s="1" t="s">
         <v>213</v>
       </c>
@@ -51181,6 +51322,12 @@
       <c r="N1037">
         <v>0.53582229999999997</v>
       </c>
+      <c r="O1037">
+        <v>3.9279999999999999</v>
+      </c>
+      <c r="P1037" s="64">
+        <v>0.51250000000000007</v>
+      </c>
       <c r="T1037" s="1" t="s">
         <v>213</v>
       </c>
@@ -51231,6 +51378,9 @@
       <c r="N1038">
         <v>0.1563206</v>
       </c>
+      <c r="O1038">
+        <v>8.9580000000000002</v>
+      </c>
       <c r="T1038" s="1" t="s">
         <v>213</v>
       </c>
@@ -51278,6 +51428,9 @@
       <c r="N1039">
         <v>0.1032771</v>
       </c>
+      <c r="O1039">
+        <v>4.6150000000000002</v>
+      </c>
       <c r="T1039" s="1" t="s">
         <v>213</v>
       </c>
@@ -51328,6 +51481,9 @@
       <c r="N1040">
         <v>0.12387380000000001</v>
       </c>
+      <c r="O1040">
+        <v>6.6689999999999996</v>
+      </c>
       <c r="T1040" s="1" t="s">
         <v>213</v>
       </c>
@@ -51375,6 +51531,9 @@
       <c r="N1041">
         <v>0.17735790000000001</v>
       </c>
+      <c r="O1041">
+        <v>8.8870000000000005</v>
+      </c>
       <c r="T1041" s="1" t="s">
         <v>213</v>
       </c>
@@ -51425,6 +51584,9 @@
       <c r="N1042">
         <v>1.2198629999999999</v>
       </c>
+      <c r="O1042">
+        <v>9.0180000000000007</v>
+      </c>
       <c r="T1042" s="1" t="s">
         <v>213</v>
       </c>
@@ -51472,6 +51634,9 @@
       <c r="N1043">
         <v>0.1508727</v>
       </c>
+      <c r="O1043">
+        <v>8.1590000000000007</v>
+      </c>
       <c r="T1043" s="1" t="s">
         <v>213</v>
       </c>
@@ -51522,6 +51687,9 @@
       <c r="N1044" s="21">
         <v>7.9226580000000005E-2</v>
       </c>
+      <c r="O1044">
+        <v>4.548</v>
+      </c>
       <c r="T1044" s="1" t="s">
         <v>213</v>
       </c>
@@ -51572,6 +51740,9 @@
       <c r="N1045" s="21">
         <v>7.9388280000000006E-2</v>
       </c>
+      <c r="O1045">
+        <v>8.09</v>
+      </c>
       <c r="T1045" s="1" t="s">
         <v>213</v>
       </c>
@@ -51622,6 +51793,9 @@
       <c r="N1046">
         <v>0.14393410000000001</v>
       </c>
+      <c r="O1046">
+        <v>6.5</v>
+      </c>
       <c r="T1046" s="1" t="s">
         <v>213</v>
       </c>
@@ -51669,6 +51843,9 @@
       <c r="N1047">
         <v>0.117183</v>
       </c>
+      <c r="O1047">
+        <v>7.5149999999999997</v>
+      </c>
       <c r="T1047" s="1" t="s">
         <v>213</v>
       </c>
@@ -51716,6 +51893,9 @@
       <c r="N1048">
         <v>0.82421829999999996</v>
       </c>
+      <c r="O1048">
+        <v>5.8650000000000002</v>
+      </c>
       <c r="T1048" s="1" t="s">
         <v>213</v>
       </c>
@@ -51766,6 +51946,9 @@
       <c r="N1049">
         <v>0.1126433</v>
       </c>
+      <c r="O1049">
+        <v>7.5060000000000002</v>
+      </c>
       <c r="T1049" s="1" t="s">
         <v>213</v>
       </c>
@@ -51813,6 +51996,9 @@
       <c r="N1050">
         <v>0.66805639999999999</v>
       </c>
+      <c r="O1050">
+        <v>3.35</v>
+      </c>
       <c r="T1050" s="1" t="s">
         <v>213</v>
       </c>
@@ -51863,6 +52049,9 @@
       <c r="N1051" s="21">
         <v>6.4429570000000005E-2</v>
       </c>
+      <c r="O1051">
+        <v>5.3849999999999998</v>
+      </c>
       <c r="T1051" s="1" t="s">
         <v>213</v>
       </c>
@@ -51910,6 +52099,9 @@
       <c r="N1052">
         <v>7.8821500000000003E-2</v>
       </c>
+      <c r="O1052">
+        <v>7.492</v>
+      </c>
       <c r="T1052" s="1" t="s">
         <v>213</v>
       </c>
@@ -51960,6 +52152,9 @@
       <c r="N1053">
         <v>8.7887499999999993E-2</v>
       </c>
+      <c r="O1053">
+        <v>8.532</v>
+      </c>
       <c r="T1053" s="1" t="s">
         <v>213</v>
       </c>
@@ -52010,6 +52205,9 @@
       <c r="N1054" s="21">
         <v>9.0903639999999994E-2</v>
       </c>
+      <c r="O1054">
+        <v>4.6520000000000001</v>
+      </c>
       <c r="T1054" s="1" t="s">
         <v>213</v>
       </c>
@@ -52060,6 +52258,9 @@
       <c r="N1055" s="21">
         <v>5.9986780000000003E-2</v>
       </c>
+      <c r="O1055">
+        <v>6.2969999999999997</v>
+      </c>
       <c r="T1055" s="1" t="s">
         <v>213</v>
       </c>
@@ -52110,6 +52311,9 @@
       <c r="N1056">
         <v>0.1607354</v>
       </c>
+      <c r="O1056">
+        <v>10.377000000000001</v>
+      </c>
       <c r="T1056" s="1" t="s">
         <v>213</v>
       </c>
@@ -52157,6 +52361,9 @@
       <c r="N1057">
         <v>0.1230528</v>
       </c>
+      <c r="O1057">
+        <v>5.2690000000000001</v>
+      </c>
       <c r="T1057" s="1" t="s">
         <v>213</v>
       </c>
@@ -52207,6 +52414,9 @@
       <c r="N1058">
         <v>0.12855800000000001</v>
       </c>
+      <c r="O1058">
+        <v>6.4260000000000002</v>
+      </c>
       <c r="T1058" s="1" t="s">
         <v>213</v>
       </c>
@@ -52257,6 +52467,9 @@
       <c r="N1059" s="21">
         <v>7.2165549999999995E-2</v>
       </c>
+      <c r="O1059">
+        <v>7.1230000000000002</v>
+      </c>
       <c r="T1059" s="1" t="s">
         <v>213</v>
       </c>
@@ -52307,6 +52520,9 @@
       <c r="N1060">
         <v>0.79508699999999999</v>
       </c>
+      <c r="O1060">
+        <v>7.5039999999999996</v>
+      </c>
       <c r="T1060" s="1" t="s">
         <v>213</v>
       </c>
@@ -52357,6 +52573,9 @@
       <c r="N1061">
         <v>0.1354204</v>
       </c>
+      <c r="O1061">
+        <v>5.0339999999999998</v>
+      </c>
       <c r="T1061" s="1" t="s">
         <v>213</v>
       </c>
@@ -52407,6 +52626,9 @@
       <c r="N1062" s="21">
         <v>8.4525180000000005E-2</v>
       </c>
+      <c r="O1062">
+        <v>6.9630000000000001</v>
+      </c>
       <c r="T1062" s="1" t="s">
         <v>213</v>
       </c>
@@ -52454,6 +52676,9 @@
       <c r="N1063">
         <v>1.0307489999999999</v>
       </c>
+      <c r="O1063">
+        <v>7.9630000000000001</v>
+      </c>
       <c r="T1063" s="1" t="s">
         <v>213</v>
       </c>
@@ -52504,6 +52729,9 @@
       <c r="N1064" s="21">
         <v>9.0086669999999994E-2</v>
       </c>
+      <c r="O1064">
+        <v>5.6749999999999998</v>
+      </c>
       <c r="T1064" s="1" t="s">
         <v>213</v>
       </c>
@@ -52554,6 +52782,9 @@
       <c r="N1065">
         <v>0.101032</v>
       </c>
+      <c r="O1065">
+        <v>4.5439999999999996</v>
+      </c>
       <c r="T1065" s="1" t="s">
         <v>213</v>
       </c>
@@ -52601,6 +52832,9 @@
       <c r="N1066">
         <v>1.315436</v>
       </c>
+      <c r="O1066">
+        <v>6.0140000000000002</v>
+      </c>
       <c r="T1066" s="1" t="s">
         <v>213</v>
       </c>
@@ -52648,6 +52882,9 @@
       <c r="N1067" s="21">
         <v>6.2707470000000001E-2</v>
       </c>
+      <c r="O1067">
+        <v>4.7009999999999996</v>
+      </c>
       <c r="T1067" s="1" t="s">
         <v>213</v>
       </c>
@@ -52698,6 +52935,9 @@
       <c r="N1068">
         <v>0.86417460000000001</v>
       </c>
+      <c r="O1068">
+        <v>5.9630000000000001</v>
+      </c>
       <c r="T1068" s="1" t="s">
         <v>213</v>
       </c>
@@ -52748,6 +52988,9 @@
       <c r="N1069" s="21">
         <v>8.6048449999999999E-2</v>
       </c>
+      <c r="O1069">
+        <v>6.3940000000000001</v>
+      </c>
       <c r="T1069" s="1" t="s">
         <v>213</v>
       </c>
@@ -52798,6 +53041,9 @@
       <c r="N1070">
         <v>0.1086746</v>
       </c>
+      <c r="O1070">
+        <v>7.2279999999999998</v>
+      </c>
       <c r="T1070" s="1" t="s">
         <v>213</v>
       </c>
@@ -52845,6 +53091,9 @@
       <c r="N1071" s="21">
         <v>9.0717629999999994E-2</v>
       </c>
+      <c r="O1071">
+        <v>7.9370000000000003</v>
+      </c>
       <c r="T1071" s="1" t="s">
         <v>213</v>
       </c>
@@ -52895,6 +53144,9 @@
       <c r="N1072" s="21">
         <v>8.322562E-2</v>
       </c>
+      <c r="O1072">
+        <v>6.3869999999999996</v>
+      </c>
       <c r="T1072" s="1" t="s">
         <v>213</v>
       </c>
@@ -52945,6 +53197,9 @@
       <c r="N1073">
         <v>0.1316833</v>
       </c>
+      <c r="O1073">
+        <v>5.88</v>
+      </c>
       <c r="T1073" s="1" t="s">
         <v>213</v>
       </c>
@@ -52995,6 +53250,9 @@
       <c r="N1074">
         <v>1.022467</v>
       </c>
+      <c r="O1074">
+        <v>6.4349999999999996</v>
+      </c>
       <c r="T1074" s="1" t="s">
         <v>213</v>
       </c>
@@ -53045,6 +53303,9 @@
       <c r="N1075">
         <v>0.10568180000000001</v>
       </c>
+      <c r="O1075">
+        <v>6.1459999999999999</v>
+      </c>
       <c r="T1075" s="1" t="s">
         <v>213</v>
       </c>
@@ -53095,6 +53356,9 @@
       <c r="N1076" s="21">
         <v>5.720592E-2</v>
       </c>
+      <c r="O1076">
+        <v>5.407</v>
+      </c>
       <c r="T1076" s="1" t="s">
         <v>213</v>
       </c>
@@ -53145,6 +53409,9 @@
       <c r="N1077">
         <v>0.80207340000000005</v>
       </c>
+      <c r="O1077">
+        <v>6.9779999999999998</v>
+      </c>
       <c r="T1077" s="1" t="s">
         <v>213</v>
       </c>
@@ -53195,6 +53462,9 @@
       <c r="N1078">
         <v>0.17547650000000001</v>
       </c>
+      <c r="O1078">
+        <v>8.4009999999999998</v>
+      </c>
       <c r="T1078" s="1" t="s">
         <v>213</v>
       </c>
@@ -53242,6 +53512,9 @@
       <c r="N1079">
         <v>0.17211609999999999</v>
       </c>
+      <c r="O1079">
+        <v>8.173</v>
+      </c>
       <c r="T1079" s="1" t="s">
         <v>213</v>
       </c>
@@ -53292,6 +53565,9 @@
       <c r="N1080">
         <v>0.1636775</v>
       </c>
+      <c r="O1080">
+        <v>9.391</v>
+      </c>
       <c r="T1080" s="1" t="s">
         <v>213</v>
       </c>
@@ -53342,6 +53618,9 @@
       <c r="N1081" s="21">
         <v>7.8189869999999995E-2</v>
       </c>
+      <c r="O1081">
+        <v>6.9619999999999997</v>
+      </c>
       <c r="T1081" s="1" t="s">
         <v>213</v>
       </c>
@@ -53429,6 +53708,9 @@
       </c>
       <c r="N1083" s="21">
         <v>1.234064E-2</v>
+      </c>
+      <c r="P1083" s="64">
+        <v>0.5180555555555556</v>
       </c>
       <c r="T1083" s="1" t="s">
         <v>213</v>

</xml_diff>

<commit_message>
adding respirometry data, day 11, cohort day 12+27 (2018-09-11)
</commit_message>
<xml_diff>
--- a/Data/2018-08-14_master_datac_2018_collection_year.xlsx
+++ b/Data/2018-08-14_master_datac_2018_collection_year.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andrew.nguyen\Desktop\Circadian_rhythm_runs_seasonal_timing\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CF50C1B-DA83-48FE-9189-170B76194D81}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0E4516F-027F-4976-9A09-5AED14F8A23A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9855" yWindow="7665" windowWidth="36360" windowHeight="21135" activeTab="1" xr2:uid="{C7477166-8A7C-B04A-9643-C277FEDCDAAB}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14775" uniqueCount="1048">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14767" uniqueCount="1047">
   <si>
     <t>Ind_ID</t>
   </si>
@@ -3116,9 +3116,6 @@
   </si>
   <si>
     <t>MSU F+ W,ATC</t>
-  </si>
-  <si>
-    <t>20+6=26</t>
   </si>
   <si>
     <t>15:05</t>
@@ -3781,9 +3778,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D3F78F5-4EA8-6A42-B216-41A8EC7A5E8D}">
   <dimension ref="A1:AC306"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A139" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L160" sqref="L160"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A136" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I158" sqref="I158"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -12515,8 +12512,8 @@
       <c r="H157" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="I157" t="s">
-        <v>1028</v>
+      <c r="I157">
+        <v>26</v>
       </c>
       <c r="J157" s="1"/>
       <c r="K157" s="1"/>
@@ -14175,11 +14172,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92725FB9-1A17-2546-9DFA-6C0D39437891}">
-  <dimension ref="A1:AS1589"/>
+  <dimension ref="A1:AS1588"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1058" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P1084" sqref="P1084"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A1519" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O1534" sqref="O1534"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -68054,7 +68051,7 @@
         <v>9.9450000000000003</v>
       </c>
       <c r="E1447" s="1" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
       <c r="G1447" s="1" t="s">
         <v>188</v>
@@ -68070,6 +68067,15 @@
       </c>
       <c r="K1447" t="s">
         <v>61</v>
+      </c>
+      <c r="L1447">
+        <v>7000</v>
+      </c>
+      <c r="M1447" s="20">
+        <v>0.54716435185185186</v>
+      </c>
+      <c r="N1447">
+        <v>0.11119329999999999</v>
       </c>
       <c r="T1447" s="1" t="s">
         <v>543</v>
@@ -68103,6 +68109,15 @@
       <c r="K1448" t="s">
         <v>61</v>
       </c>
+      <c r="L1448">
+        <v>7000</v>
+      </c>
+      <c r="M1448" s="20">
+        <v>0.54812499999999997</v>
+      </c>
+      <c r="N1448" s="21">
+        <v>5.3186789999999998E-2</v>
+      </c>
       <c r="T1448" s="1" t="s">
         <v>543</v>
       </c>
@@ -68135,6 +68150,15 @@
       <c r="K1449" t="s">
         <v>61</v>
       </c>
+      <c r="L1449">
+        <v>7000</v>
+      </c>
+      <c r="M1449" s="20">
+        <v>0.54890046296296291</v>
+      </c>
+      <c r="N1449">
+        <v>0.7526349</v>
+      </c>
       <c r="T1449" s="1" t="s">
         <v>543</v>
       </c>
@@ -68167,6 +68191,15 @@
       <c r="K1450" t="s">
         <v>61</v>
       </c>
+      <c r="L1450">
+        <v>7000</v>
+      </c>
+      <c r="M1450" s="20">
+        <v>0.54982638888888891</v>
+      </c>
+      <c r="N1450" s="21">
+        <v>9.4618980000000005E-2</v>
+      </c>
       <c r="T1450" s="1" t="s">
         <v>543</v>
       </c>
@@ -68199,6 +68232,15 @@
       <c r="K1451" t="s">
         <v>61</v>
       </c>
+      <c r="L1451">
+        <v>7000</v>
+      </c>
+      <c r="M1451" s="20">
+        <v>0.55064814814814811</v>
+      </c>
+      <c r="N1451">
+        <v>0.52073619999999998</v>
+      </c>
       <c r="T1451" s="1" t="s">
         <v>543</v>
       </c>
@@ -68231,6 +68273,15 @@
       <c r="K1452" t="s">
         <v>61</v>
       </c>
+      <c r="L1452">
+        <v>7000</v>
+      </c>
+      <c r="M1452" s="20">
+        <v>0.55156250000000007</v>
+      </c>
+      <c r="N1452">
+        <v>0.95152910000000002</v>
+      </c>
       <c r="T1452" s="1" t="s">
         <v>543</v>
       </c>
@@ -68263,6 +68314,15 @@
       <c r="K1453" t="s">
         <v>61</v>
       </c>
+      <c r="L1453">
+        <v>7000</v>
+      </c>
+      <c r="M1453" s="20">
+        <v>0.55246527777777776</v>
+      </c>
+      <c r="N1453" s="21">
+        <v>4.8348139999999998E-2</v>
+      </c>
       <c r="T1453" s="1" t="s">
         <v>543</v>
       </c>
@@ -68295,6 +68355,15 @@
       <c r="K1454" t="s">
         <v>61</v>
       </c>
+      <c r="L1454">
+        <v>7000</v>
+      </c>
+      <c r="M1454" s="20">
+        <v>0.5534027777777778</v>
+      </c>
+      <c r="N1454" s="21">
+        <v>8.4228460000000005E-2</v>
+      </c>
       <c r="T1454" s="1" t="s">
         <v>543</v>
       </c>
@@ -68327,6 +68396,15 @@
       <c r="K1455" t="s">
         <v>61</v>
       </c>
+      <c r="L1455">
+        <v>7000</v>
+      </c>
+      <c r="M1455" s="20">
+        <v>0.55472222222222223</v>
+      </c>
+      <c r="N1455">
+        <v>0.88255039999999996</v>
+      </c>
       <c r="T1455" s="1" t="s">
         <v>543</v>
       </c>
@@ -68359,6 +68437,15 @@
       <c r="K1456" t="s">
         <v>61</v>
       </c>
+      <c r="L1456">
+        <v>7000</v>
+      </c>
+      <c r="M1456" s="20">
+        <v>0.55564814814814811</v>
+      </c>
+      <c r="N1456">
+        <v>0.77142619999999995</v>
+      </c>
       <c r="T1456" s="1" t="s">
         <v>543</v>
       </c>
@@ -68391,6 +68478,15 @@
       <c r="K1457" t="s">
         <v>61</v>
       </c>
+      <c r="L1457">
+        <v>7000</v>
+      </c>
+      <c r="M1457" s="20">
+        <v>0.55658564814814815</v>
+      </c>
+      <c r="N1457">
+        <v>0.39931139999999998</v>
+      </c>
       <c r="T1457" s="1" t="s">
         <v>543</v>
       </c>
@@ -68423,6 +68519,15 @@
       <c r="K1458" t="s">
         <v>61</v>
       </c>
+      <c r="L1458">
+        <v>7000</v>
+      </c>
+      <c r="M1458" s="20">
+        <v>0.55744212962962958</v>
+      </c>
+      <c r="N1458" s="21">
+        <v>7.4997530000000007E-2</v>
+      </c>
       <c r="T1458" s="1" t="s">
         <v>543</v>
       </c>
@@ -68455,6 +68560,15 @@
       <c r="K1459" t="s">
         <v>61</v>
       </c>
+      <c r="L1459">
+        <v>7000</v>
+      </c>
+      <c r="M1459" s="20">
+        <v>0.5584837962962963</v>
+      </c>
+      <c r="N1459">
+        <v>0.15808900000000001</v>
+      </c>
       <c r="T1459" s="1" t="s">
         <v>543</v>
       </c>
@@ -68487,6 +68601,15 @@
       <c r="K1460" t="s">
         <v>61</v>
       </c>
+      <c r="L1460">
+        <v>7000</v>
+      </c>
+      <c r="M1460" s="20">
+        <v>0.55925925925925923</v>
+      </c>
+      <c r="N1460">
+        <v>0.12554589999999999</v>
+      </c>
       <c r="T1460" s="1" t="s">
         <v>543</v>
       </c>
@@ -68519,6 +68642,15 @@
       <c r="K1461" t="s">
         <v>61</v>
       </c>
+      <c r="L1461">
+        <v>7000</v>
+      </c>
+      <c r="M1461" s="20">
+        <v>0.5600694444444444</v>
+      </c>
+      <c r="N1461" s="21">
+        <v>7.3684369999999999E-2</v>
+      </c>
       <c r="T1461" s="1" t="s">
         <v>543</v>
       </c>
@@ -68551,6 +68683,15 @@
       <c r="K1462" t="s">
         <v>61</v>
       </c>
+      <c r="L1462">
+        <v>7000</v>
+      </c>
+      <c r="M1462" s="20">
+        <v>0.56090277777777775</v>
+      </c>
+      <c r="N1462">
+        <v>8.7774199999999997E-2</v>
+      </c>
       <c r="T1462" s="1" t="s">
         <v>543</v>
       </c>
@@ -68583,6 +68724,15 @@
       <c r="K1463" t="s">
         <v>61</v>
       </c>
+      <c r="L1463">
+        <v>7000</v>
+      </c>
+      <c r="M1463" s="20">
+        <v>0.5617361111111111</v>
+      </c>
+      <c r="N1463">
+        <v>0.66200300000000001</v>
+      </c>
       <c r="T1463" s="1" t="s">
         <v>543</v>
       </c>
@@ -68615,6 +68765,15 @@
       <c r="K1464" t="s">
         <v>61</v>
       </c>
+      <c r="L1464">
+        <v>7000</v>
+      </c>
+      <c r="M1464" s="20">
+        <v>0.56265046296296295</v>
+      </c>
+      <c r="N1464">
+        <v>0.1132678</v>
+      </c>
       <c r="T1464" s="1" t="s">
         <v>543</v>
       </c>
@@ -68647,6 +68806,15 @@
       <c r="K1465" t="s">
         <v>61</v>
       </c>
+      <c r="L1465">
+        <v>7000</v>
+      </c>
+      <c r="M1465" s="20">
+        <v>0.56343750000000004</v>
+      </c>
+      <c r="N1465">
+        <v>8.0909300000000003E-2</v>
+      </c>
       <c r="T1465" s="1" t="s">
         <v>543</v>
       </c>
@@ -68679,6 +68847,15 @@
       <c r="K1466" t="s">
         <v>61</v>
       </c>
+      <c r="L1466">
+        <v>7000</v>
+      </c>
+      <c r="M1466" s="20">
+        <v>0.56428240740740743</v>
+      </c>
+      <c r="N1466" s="21">
+        <v>8.5724170000000002E-2</v>
+      </c>
       <c r="T1466" s="1" t="s">
         <v>543</v>
       </c>
@@ -68711,6 +68888,15 @@
       <c r="K1467" t="s">
         <v>61</v>
       </c>
+      <c r="L1467">
+        <v>7000</v>
+      </c>
+      <c r="M1467" s="20">
+        <v>0.56505787037037036</v>
+      </c>
+      <c r="N1467" s="21">
+        <v>7.1258589999999997E-2</v>
+      </c>
       <c r="T1467" s="1" t="s">
         <v>543</v>
       </c>
@@ -68743,6 +68929,15 @@
       <c r="K1468" t="s">
         <v>61</v>
       </c>
+      <c r="L1468">
+        <v>7000</v>
+      </c>
+      <c r="M1468" s="20">
+        <v>0.56575231481481481</v>
+      </c>
+      <c r="N1468">
+        <v>0.1029881</v>
+      </c>
       <c r="T1468" s="1" t="s">
         <v>543</v>
       </c>
@@ -68775,6 +68970,15 @@
       <c r="K1469" t="s">
         <v>61</v>
       </c>
+      <c r="L1469">
+        <v>7000</v>
+      </c>
+      <c r="M1469" s="20">
+        <v>0.56653935185185189</v>
+      </c>
+      <c r="N1469">
+        <v>0.51681129999999997</v>
+      </c>
       <c r="T1469" s="1" t="s">
         <v>543</v>
       </c>
@@ -68807,6 +69011,15 @@
       <c r="K1470" t="s">
         <v>61</v>
       </c>
+      <c r="L1470">
+        <v>7000</v>
+      </c>
+      <c r="M1470" s="20">
+        <v>0.56738425925925928</v>
+      </c>
+      <c r="N1470" s="21">
+        <v>8.2367170000000003E-2</v>
+      </c>
       <c r="T1470" s="1" t="s">
         <v>543</v>
       </c>
@@ -68839,6 +69052,15 @@
       <c r="K1471" t="s">
         <v>61</v>
       </c>
+      <c r="L1471">
+        <v>7000</v>
+      </c>
+      <c r="M1471" s="20">
+        <v>0.5682638888888889</v>
+      </c>
+      <c r="N1471" s="21">
+        <v>4.8787209999999998E-2</v>
+      </c>
       <c r="T1471" s="1" t="s">
         <v>543</v>
       </c>
@@ -68871,6 +69093,15 @@
       <c r="K1472" t="s">
         <v>61</v>
       </c>
+      <c r="L1472">
+        <v>7000</v>
+      </c>
+      <c r="M1472" s="20">
+        <v>0.56909722222222225</v>
+      </c>
+      <c r="N1472">
+        <v>1.0868409999999999</v>
+      </c>
       <c r="T1472" s="1" t="s">
         <v>543</v>
       </c>
@@ -68903,6 +69134,15 @@
       <c r="K1473" t="s">
         <v>61</v>
       </c>
+      <c r="L1473">
+        <v>7000</v>
+      </c>
+      <c r="M1473" s="20">
+        <v>0.56997685185185187</v>
+      </c>
+      <c r="N1473" s="21">
+        <v>7.1211259999999998E-2</v>
+      </c>
       <c r="T1473" s="1" t="s">
         <v>543</v>
       </c>
@@ -68935,6 +69175,15 @@
       <c r="K1474" t="s">
         <v>61</v>
       </c>
+      <c r="L1474">
+        <v>7000</v>
+      </c>
+      <c r="M1474" s="20">
+        <v>0.57071759259259258</v>
+      </c>
+      <c r="N1474" s="21">
+        <v>8.2078910000000005E-2</v>
+      </c>
       <c r="T1474" s="1" t="s">
         <v>543</v>
       </c>
@@ -68967,6 +69216,15 @@
       <c r="K1475" t="s">
         <v>61</v>
       </c>
+      <c r="L1475">
+        <v>7000</v>
+      </c>
+      <c r="M1475" s="20">
+        <v>0.57168981481481485</v>
+      </c>
+      <c r="N1475" s="21">
+        <v>4.9959980000000001E-2</v>
+      </c>
       <c r="T1475" s="1" t="s">
         <v>543</v>
       </c>
@@ -68999,6 +69257,15 @@
       <c r="K1476" t="s">
         <v>61</v>
       </c>
+      <c r="L1476">
+        <v>7000</v>
+      </c>
+      <c r="M1476" s="20">
+        <v>0.58685185185185185</v>
+      </c>
+      <c r="N1476">
+        <v>0.15220590000000001</v>
+      </c>
       <c r="T1476" s="1" t="s">
         <v>543</v>
       </c>
@@ -69031,6 +69298,15 @@
       <c r="K1477" t="s">
         <v>61</v>
       </c>
+      <c r="L1477">
+        <v>7000</v>
+      </c>
+      <c r="M1477" s="20">
+        <v>0.58784722222222219</v>
+      </c>
+      <c r="N1477">
+        <v>0.69956680000000004</v>
+      </c>
       <c r="T1477" s="1" t="s">
         <v>543</v>
       </c>
@@ -69063,6 +69339,15 @@
       <c r="K1478" t="s">
         <v>61</v>
       </c>
+      <c r="L1478">
+        <v>7000</v>
+      </c>
+      <c r="M1478" s="20">
+        <v>0.58877314814814818</v>
+      </c>
+      <c r="N1478">
+        <v>0.3984354</v>
+      </c>
       <c r="T1478" s="1" t="s">
         <v>543</v>
       </c>
@@ -69095,6 +69380,15 @@
       <c r="K1479" t="s">
         <v>61</v>
       </c>
+      <c r="L1479">
+        <v>7000</v>
+      </c>
+      <c r="M1479" s="20">
+        <v>0.5895717592592592</v>
+      </c>
+      <c r="N1479" s="21">
+        <v>5.1939730000000003E-2</v>
+      </c>
       <c r="T1479" s="1" t="s">
         <v>543</v>
       </c>
@@ -69127,6 +69421,15 @@
       <c r="K1480" t="s">
         <v>61</v>
       </c>
+      <c r="L1480">
+        <v>7000</v>
+      </c>
+      <c r="M1480" s="20">
+        <v>0.59054398148148146</v>
+      </c>
+      <c r="N1480">
+        <v>0.13050329999999999</v>
+      </c>
       <c r="T1480" s="1" t="s">
         <v>543</v>
       </c>
@@ -69159,6 +69462,15 @@
       <c r="K1481" t="s">
         <v>61</v>
       </c>
+      <c r="L1481">
+        <v>7000</v>
+      </c>
+      <c r="M1481" s="20">
+        <v>0.59138888888888885</v>
+      </c>
+      <c r="N1481">
+        <v>0.60580299999999998</v>
+      </c>
       <c r="T1481" s="1" t="s">
         <v>543</v>
       </c>
@@ -69191,6 +69503,15 @@
       <c r="K1482" t="s">
         <v>61</v>
       </c>
+      <c r="L1482">
+        <v>7000</v>
+      </c>
+      <c r="M1482" s="20">
+        <v>0.59234953703703697</v>
+      </c>
+      <c r="N1482" s="21">
+        <v>8.1174049999999998E-2</v>
+      </c>
       <c r="T1482" s="1" t="s">
         <v>543</v>
       </c>
@@ -69223,6 +69544,15 @@
       <c r="K1483" t="s">
         <v>61</v>
       </c>
+      <c r="L1483">
+        <v>7000</v>
+      </c>
+      <c r="M1483" s="20">
+        <v>0.59315972222222224</v>
+      </c>
+      <c r="N1483">
+        <v>0.1057719</v>
+      </c>
       <c r="T1483" s="1" t="s">
         <v>543</v>
       </c>
@@ -69255,6 +69585,15 @@
       <c r="K1484" t="s">
         <v>61</v>
       </c>
+      <c r="L1484">
+        <v>7000</v>
+      </c>
+      <c r="M1484" s="20">
+        <v>0.59400462962962963</v>
+      </c>
+      <c r="N1484">
+        <v>0.1035157</v>
+      </c>
       <c r="T1484" s="1" t="s">
         <v>543</v>
       </c>
@@ -69287,6 +69626,15 @@
       <c r="K1485" t="s">
         <v>61</v>
       </c>
+      <c r="L1485">
+        <v>7000</v>
+      </c>
+      <c r="M1485" s="20">
+        <v>0.59483796296296299</v>
+      </c>
+      <c r="N1485" s="21">
+        <v>9.477373E-2</v>
+      </c>
       <c r="T1485" s="1" t="s">
         <v>543</v>
       </c>
@@ -69319,6 +69667,15 @@
       <c r="K1486" t="s">
         <v>61</v>
       </c>
+      <c r="L1486">
+        <v>7000</v>
+      </c>
+      <c r="M1486" s="20">
+        <v>0.59561342592592592</v>
+      </c>
+      <c r="N1486" s="21">
+        <v>4.9693139999999997E-2</v>
+      </c>
       <c r="T1486" s="1" t="s">
         <v>543</v>
       </c>
@@ -69351,6 +69708,15 @@
       <c r="K1487" t="s">
         <v>61</v>
       </c>
+      <c r="L1487">
+        <v>7000</v>
+      </c>
+      <c r="M1487" s="20">
+        <v>0.59636574074074067</v>
+      </c>
+      <c r="N1487">
+        <v>0.1017332</v>
+      </c>
       <c r="T1487" s="1" t="s">
         <v>543</v>
       </c>
@@ -69383,6 +69749,15 @@
       <c r="K1488" t="s">
         <v>61</v>
       </c>
+      <c r="L1488">
+        <v>7000</v>
+      </c>
+      <c r="M1488" s="20">
+        <v>0.59717592592592594</v>
+      </c>
+      <c r="N1488">
+        <v>0.46535840000000001</v>
+      </c>
       <c r="T1488" s="1" t="s">
         <v>543</v>
       </c>
@@ -69415,6 +69790,15 @@
       <c r="K1489" t="s">
         <v>61</v>
       </c>
+      <c r="L1489">
+        <v>7000</v>
+      </c>
+      <c r="M1489" s="20">
+        <v>0.59809027777777779</v>
+      </c>
+      <c r="N1489" s="21">
+        <v>7.2860190000000005E-2</v>
+      </c>
       <c r="T1489" s="1" t="s">
         <v>543</v>
       </c>
@@ -69447,6 +69831,15 @@
       <c r="K1490" t="s">
         <v>61</v>
       </c>
+      <c r="L1490">
+        <v>7000</v>
+      </c>
+      <c r="M1490" s="20">
+        <v>0.59894675925925933</v>
+      </c>
+      <c r="N1490" s="21">
+        <v>8.4767430000000005E-2</v>
+      </c>
       <c r="T1490" s="1" t="s">
         <v>543</v>
       </c>
@@ -69476,6 +69869,15 @@
       <c r="K1491" t="s">
         <v>61</v>
       </c>
+      <c r="L1491">
+        <v>7000</v>
+      </c>
+      <c r="M1491" s="20">
+        <v>0.59978009259259257</v>
+      </c>
+      <c r="N1491" s="21">
+        <v>4.8005579999999999E-3</v>
+      </c>
       <c r="T1491" s="1" t="s">
         <v>543</v>
       </c>
@@ -69491,7 +69893,7 @@
         <v>703</v>
       </c>
       <c r="E1492" s="1" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="G1492" s="1" t="s">
         <v>188</v>
@@ -69507,6 +69909,15 @@
       </c>
       <c r="K1492" t="s">
         <v>61</v>
+      </c>
+      <c r="L1492">
+        <v>7000</v>
+      </c>
+      <c r="M1492" s="20">
+        <v>0.60063657407407411</v>
+      </c>
+      <c r="N1492" s="21">
+        <v>6.7642880000000002E-3</v>
       </c>
       <c r="T1492" s="1" t="s">
         <v>543</v>
@@ -69526,7 +69937,7 @@
         <v>8.5470000000000006</v>
       </c>
       <c r="E1493" s="1" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
       <c r="G1493" s="1" t="s">
         <v>188</v>
@@ -69542,6 +69953,15 @@
       </c>
       <c r="K1493" t="s">
         <v>61</v>
+      </c>
+      <c r="L1493">
+        <v>6262</v>
+      </c>
+      <c r="M1493" s="20">
+        <v>0.54716435185185186</v>
+      </c>
+      <c r="N1493">
+        <v>0.15717390000000001</v>
       </c>
       <c r="T1493" s="1" t="s">
         <v>543</v>
@@ -69575,6 +69995,15 @@
       <c r="K1494" t="s">
         <v>61</v>
       </c>
+      <c r="L1494">
+        <v>6262</v>
+      </c>
+      <c r="M1494" s="20">
+        <v>0.54812499999999997</v>
+      </c>
+      <c r="N1494" s="21">
+        <v>6.162865E-2</v>
+      </c>
       <c r="T1494" s="1" t="s">
         <v>543</v>
       </c>
@@ -69607,6 +70036,15 @@
       <c r="K1495" t="s">
         <v>61</v>
       </c>
+      <c r="L1495">
+        <v>6262</v>
+      </c>
+      <c r="M1495" s="20">
+        <v>0.54890046296296291</v>
+      </c>
+      <c r="N1495">
+        <v>8.2220000000000001E-2</v>
+      </c>
       <c r="T1495" s="1" t="s">
         <v>543</v>
       </c>
@@ -69639,6 +70077,15 @@
       <c r="K1496" t="s">
         <v>61</v>
       </c>
+      <c r="L1496">
+        <v>6262</v>
+      </c>
+      <c r="M1496" s="20">
+        <v>0.54982638888888891</v>
+      </c>
+      <c r="N1496" s="21">
+        <v>9.8212679999999997E-2</v>
+      </c>
       <c r="T1496" s="1" t="s">
         <v>543</v>
       </c>
@@ -69671,6 +70118,15 @@
       <c r="K1497" t="s">
         <v>61</v>
       </c>
+      <c r="L1497">
+        <v>6262</v>
+      </c>
+      <c r="M1497" s="20">
+        <v>0.55064814814814811</v>
+      </c>
+      <c r="N1497">
+        <v>0.16146360000000001</v>
+      </c>
       <c r="T1497" s="1" t="s">
         <v>543</v>
       </c>
@@ -69703,6 +70159,15 @@
       <c r="K1498" t="s">
         <v>61</v>
       </c>
+      <c r="L1498">
+        <v>6262</v>
+      </c>
+      <c r="M1498" s="20">
+        <v>0.55156250000000007</v>
+      </c>
+      <c r="N1498">
+        <v>0.12601699999999999</v>
+      </c>
       <c r="T1498" s="1" t="s">
         <v>543</v>
       </c>
@@ -69735,6 +70200,15 @@
       <c r="K1499" t="s">
         <v>61</v>
       </c>
+      <c r="L1499">
+        <v>6262</v>
+      </c>
+      <c r="M1499" s="20">
+        <v>0.55246527777777776</v>
+      </c>
+      <c r="N1499">
+        <v>0.74786710000000001</v>
+      </c>
       <c r="T1499" s="1" t="s">
         <v>543</v>
       </c>
@@ -69767,22 +70241,28 @@
       <c r="K1500" t="s">
         <v>61</v>
       </c>
+      <c r="L1500">
+        <v>6262</v>
+      </c>
+      <c r="M1500" s="20">
+        <v>0.5534027777777778</v>
+      </c>
+      <c r="N1500">
+        <v>0.41121639999999998</v>
+      </c>
       <c r="T1500" s="1" t="s">
         <v>543</v>
       </c>
     </row>
     <row r="1501" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1501">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B1501" t="s">
         <v>230</v>
       </c>
-      <c r="C1501" t="s">
-        <v>59</v>
-      </c>
       <c r="D1501">
-        <v>5.1440000000000001</v>
+        <v>5.12</v>
       </c>
       <c r="G1501" s="1" t="s">
         <v>188</v>
@@ -69799,19 +70279,31 @@
       <c r="K1501" t="s">
         <v>61</v>
       </c>
+      <c r="L1501">
+        <v>6262</v>
+      </c>
+      <c r="M1501" s="20">
+        <v>0.55564814814814811</v>
+      </c>
+      <c r="N1501">
+        <v>0.16220039999999999</v>
+      </c>
       <c r="T1501" s="1" t="s">
         <v>543</v>
       </c>
     </row>
     <row r="1502" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1502">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B1502" t="s">
         <v>230</v>
       </c>
+      <c r="C1502" t="s">
+        <v>202</v>
+      </c>
       <c r="D1502">
-        <v>5.12</v>
+        <v>6.7359999999999998</v>
       </c>
       <c r="G1502" s="1" t="s">
         <v>188</v>
@@ -69828,13 +70320,22 @@
       <c r="K1502" t="s">
         <v>61</v>
       </c>
+      <c r="L1502">
+        <v>6262</v>
+      </c>
+      <c r="M1502" s="20">
+        <v>0.55658564814814815</v>
+      </c>
+      <c r="N1502">
+        <v>0.11998350000000001</v>
+      </c>
       <c r="T1502" s="1" t="s">
         <v>543</v>
       </c>
     </row>
     <row r="1503" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1503">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B1503" t="s">
         <v>230</v>
@@ -69843,7 +70344,7 @@
         <v>202</v>
       </c>
       <c r="D1503">
-        <v>6.7359999999999998</v>
+        <v>10.657999999999999</v>
       </c>
       <c r="G1503" s="1" t="s">
         <v>188</v>
@@ -69860,22 +70361,31 @@
       <c r="K1503" t="s">
         <v>61</v>
       </c>
+      <c r="L1503">
+        <v>6262</v>
+      </c>
+      <c r="M1503" s="20">
+        <v>0.55744212962962958</v>
+      </c>
+      <c r="N1503">
+        <v>0.28798309999999999</v>
+      </c>
       <c r="T1503" s="1" t="s">
         <v>543</v>
       </c>
     </row>
     <row r="1504" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1504">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B1504" t="s">
         <v>230</v>
       </c>
       <c r="C1504" t="s">
-        <v>202</v>
+        <v>60</v>
       </c>
       <c r="D1504">
-        <v>10.657999999999999</v>
+        <v>6.9820000000000002</v>
       </c>
       <c r="G1504" s="1" t="s">
         <v>188</v>
@@ -69892,22 +70402,31 @@
       <c r="K1504" t="s">
         <v>61</v>
       </c>
+      <c r="L1504">
+        <v>6262</v>
+      </c>
+      <c r="M1504" s="20">
+        <v>0.5584837962962963</v>
+      </c>
+      <c r="N1504">
+        <v>0.13428760000000001</v>
+      </c>
       <c r="T1504" s="1" t="s">
         <v>543</v>
       </c>
     </row>
     <row r="1505" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1505">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B1505" t="s">
         <v>230</v>
       </c>
       <c r="C1505" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D1505">
-        <v>6.9820000000000002</v>
+        <v>7.726</v>
       </c>
       <c r="G1505" s="1" t="s">
         <v>188</v>
@@ -69924,22 +70443,31 @@
       <c r="K1505" t="s">
         <v>61</v>
       </c>
+      <c r="L1505">
+        <v>6262</v>
+      </c>
+      <c r="M1505" s="20">
+        <v>0.55925925925925923</v>
+      </c>
+      <c r="N1505">
+        <v>0.13631480000000001</v>
+      </c>
       <c r="T1505" s="1" t="s">
         <v>543</v>
       </c>
     </row>
     <row r="1506" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1506">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B1506" t="s">
         <v>230</v>
       </c>
       <c r="C1506" t="s">
-        <v>59</v>
+        <v>202</v>
       </c>
       <c r="D1506">
-        <v>7.726</v>
+        <v>11.287000000000001</v>
       </c>
       <c r="G1506" s="1" t="s">
         <v>188</v>
@@ -69956,22 +70484,31 @@
       <c r="K1506" t="s">
         <v>61</v>
       </c>
+      <c r="L1506">
+        <v>6262</v>
+      </c>
+      <c r="M1506" s="20">
+        <v>0.5600694444444444</v>
+      </c>
+      <c r="N1506">
+        <v>0.19356899999999999</v>
+      </c>
       <c r="T1506" s="1" t="s">
         <v>543</v>
       </c>
     </row>
     <row r="1507" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1507">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B1507" t="s">
         <v>230</v>
       </c>
       <c r="C1507" t="s">
-        <v>202</v>
+        <v>59</v>
       </c>
       <c r="D1507">
-        <v>11.287000000000001</v>
+        <v>4.548</v>
       </c>
       <c r="G1507" s="1" t="s">
         <v>188</v>
@@ -69988,22 +70525,31 @@
       <c r="K1507" t="s">
         <v>61</v>
       </c>
+      <c r="L1507">
+        <v>6262</v>
+      </c>
+      <c r="M1507" s="20">
+        <v>0.56090277777777775</v>
+      </c>
+      <c r="N1507">
+        <v>0.5350066</v>
+      </c>
       <c r="T1507" s="1" t="s">
         <v>543</v>
       </c>
     </row>
     <row r="1508" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1508">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B1508" t="s">
         <v>230</v>
       </c>
       <c r="C1508" t="s">
-        <v>59</v>
+        <v>202</v>
       </c>
       <c r="D1508">
-        <v>4.548</v>
+        <v>6.6189999999999998</v>
       </c>
       <c r="G1508" s="1" t="s">
         <v>188</v>
@@ -70020,13 +70566,22 @@
       <c r="K1508" t="s">
         <v>61</v>
       </c>
+      <c r="L1508">
+        <v>6262</v>
+      </c>
+      <c r="M1508" s="20">
+        <v>0.5617361111111111</v>
+      </c>
+      <c r="N1508" s="21">
+        <v>6.0000520000000002E-2</v>
+      </c>
       <c r="T1508" s="1" t="s">
         <v>543</v>
       </c>
     </row>
     <row r="1509" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1509">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B1509" t="s">
         <v>230</v>
@@ -70035,7 +70590,7 @@
         <v>202</v>
       </c>
       <c r="D1509">
-        <v>6.6189999999999998</v>
+        <v>8.4849999999999994</v>
       </c>
       <c r="G1509" s="1" t="s">
         <v>188</v>
@@ -70052,22 +70607,31 @@
       <c r="K1509" t="s">
         <v>61</v>
       </c>
+      <c r="L1509">
+        <v>6262</v>
+      </c>
+      <c r="M1509" s="20">
+        <v>0.56265046296296295</v>
+      </c>
+      <c r="N1509">
+        <v>0.15038470000000001</v>
+      </c>
       <c r="T1509" s="1" t="s">
         <v>543</v>
       </c>
     </row>
     <row r="1510" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1510">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B1510" t="s">
         <v>230</v>
       </c>
       <c r="C1510" t="s">
-        <v>202</v>
+        <v>59</v>
       </c>
       <c r="D1510">
-        <v>8.4849999999999994</v>
+        <v>6.774</v>
       </c>
       <c r="G1510" s="1" t="s">
         <v>188</v>
@@ -70084,13 +70648,22 @@
       <c r="K1510" t="s">
         <v>61</v>
       </c>
+      <c r="L1510">
+        <v>6262</v>
+      </c>
+      <c r="M1510" s="20">
+        <v>0.56343750000000004</v>
+      </c>
+      <c r="N1510">
+        <v>0.97502679999999997</v>
+      </c>
       <c r="T1510" s="1" t="s">
         <v>543</v>
       </c>
     </row>
     <row r="1511" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1511">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B1511" t="s">
         <v>230</v>
@@ -70099,7 +70672,7 @@
         <v>59</v>
       </c>
       <c r="D1511">
-        <v>6.774</v>
+        <v>3.5569999999999999</v>
       </c>
       <c r="G1511" s="1" t="s">
         <v>188</v>
@@ -70116,13 +70689,22 @@
       <c r="K1511" t="s">
         <v>61</v>
       </c>
+      <c r="L1511">
+        <v>6262</v>
+      </c>
+      <c r="M1511" s="20">
+        <v>0.56428240740740743</v>
+      </c>
+      <c r="N1511">
+        <v>0.66546090000000002</v>
+      </c>
       <c r="T1511" s="1" t="s">
         <v>543</v>
       </c>
     </row>
     <row r="1512" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1512">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B1512" t="s">
         <v>230</v>
@@ -70131,7 +70713,7 @@
         <v>59</v>
       </c>
       <c r="D1512">
-        <v>3.5569999999999999</v>
+        <v>9.3320000000000007</v>
       </c>
       <c r="G1512" s="1" t="s">
         <v>188</v>
@@ -70148,22 +70730,31 @@
       <c r="K1512" t="s">
         <v>61</v>
       </c>
+      <c r="L1512">
+        <v>6262</v>
+      </c>
+      <c r="M1512" s="20">
+        <v>0.56505787037037036</v>
+      </c>
+      <c r="N1512" s="21">
+        <v>9.3566789999999997E-2</v>
+      </c>
       <c r="T1512" s="1" t="s">
         <v>543</v>
       </c>
     </row>
     <row r="1513" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1513">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B1513" t="s">
         <v>230</v>
       </c>
       <c r="C1513" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D1513">
-        <v>9.3320000000000007</v>
+        <v>5.109</v>
       </c>
       <c r="G1513" s="1" t="s">
         <v>188</v>
@@ -70180,22 +70771,31 @@
       <c r="K1513" t="s">
         <v>61</v>
       </c>
+      <c r="L1513">
+        <v>6262</v>
+      </c>
+      <c r="M1513" s="20">
+        <v>0.56575231481481481</v>
+      </c>
+      <c r="N1513">
+        <v>0.65741590000000005</v>
+      </c>
       <c r="T1513" s="1" t="s">
         <v>543</v>
       </c>
     </row>
     <row r="1514" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1514">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B1514" t="s">
         <v>230</v>
       </c>
       <c r="C1514" t="s">
-        <v>60</v>
+        <v>202</v>
       </c>
       <c r="D1514">
-        <v>5.109</v>
+        <v>9.2089999999999996</v>
       </c>
       <c r="G1514" s="1" t="s">
         <v>188</v>
@@ -70212,13 +70812,22 @@
       <c r="K1514" t="s">
         <v>61</v>
       </c>
+      <c r="L1514">
+        <v>6262</v>
+      </c>
+      <c r="M1514" s="20">
+        <v>0.56653935185185189</v>
+      </c>
+      <c r="N1514">
+        <v>0.30046250000000002</v>
+      </c>
       <c r="T1514" s="1" t="s">
         <v>543</v>
       </c>
     </row>
     <row r="1515" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1515">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B1515" t="s">
         <v>230</v>
@@ -70227,7 +70836,7 @@
         <v>202</v>
       </c>
       <c r="D1515">
-        <v>9.2089999999999996</v>
+        <v>6.59</v>
       </c>
       <c r="G1515" s="1" t="s">
         <v>188</v>
@@ -70244,13 +70853,22 @@
       <c r="K1515" t="s">
         <v>61</v>
       </c>
+      <c r="L1515">
+        <v>6262</v>
+      </c>
+      <c r="M1515" s="20">
+        <v>0.56738425925925928</v>
+      </c>
+      <c r="N1515">
+        <v>1.2963439999999999</v>
+      </c>
       <c r="T1515" s="1" t="s">
         <v>543</v>
       </c>
     </row>
     <row r="1516" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1516">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B1516" t="s">
         <v>230</v>
@@ -70259,7 +70877,7 @@
         <v>202</v>
       </c>
       <c r="D1516">
-        <v>6.59</v>
+        <v>9.2070000000000007</v>
       </c>
       <c r="G1516" s="1" t="s">
         <v>188</v>
@@ -70276,13 +70894,22 @@
       <c r="K1516" t="s">
         <v>61</v>
       </c>
+      <c r="L1516">
+        <v>6262</v>
+      </c>
+      <c r="M1516" s="20">
+        <v>0.5682638888888889</v>
+      </c>
+      <c r="N1516">
+        <v>0.13023950000000001</v>
+      </c>
       <c r="T1516" s="1" t="s">
         <v>543</v>
       </c>
     </row>
     <row r="1517" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1517">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B1517" t="s">
         <v>230</v>
@@ -70291,7 +70918,7 @@
         <v>202</v>
       </c>
       <c r="D1517">
-        <v>9.2070000000000007</v>
+        <v>9.74</v>
       </c>
       <c r="G1517" s="1" t="s">
         <v>188</v>
@@ -70308,22 +70935,31 @@
       <c r="K1517" t="s">
         <v>61</v>
       </c>
+      <c r="L1517">
+        <v>6262</v>
+      </c>
+      <c r="M1517" s="20">
+        <v>0.56909722222222225</v>
+      </c>
+      <c r="N1517">
+        <v>1.447495</v>
+      </c>
       <c r="T1517" s="1" t="s">
         <v>543</v>
       </c>
     </row>
     <row r="1518" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1518">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B1518" t="s">
         <v>230</v>
       </c>
       <c r="C1518" t="s">
-        <v>202</v>
+        <v>59</v>
       </c>
       <c r="D1518">
-        <v>9.74</v>
+        <v>7.04</v>
       </c>
       <c r="G1518" s="1" t="s">
         <v>188</v>
@@ -70340,22 +70976,31 @@
       <c r="K1518" t="s">
         <v>61</v>
       </c>
+      <c r="L1518">
+        <v>6262</v>
+      </c>
+      <c r="M1518" s="20">
+        <v>0.56997685185185187</v>
+      </c>
+      <c r="N1518" s="21">
+        <v>9.7641610000000004E-2</v>
+      </c>
       <c r="T1518" s="1" t="s">
         <v>543</v>
       </c>
     </row>
     <row r="1519" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1519">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B1519" t="s">
         <v>230</v>
       </c>
       <c r="C1519" t="s">
-        <v>59</v>
+        <v>202</v>
       </c>
       <c r="D1519">
-        <v>7.04</v>
+        <v>5.22</v>
       </c>
       <c r="G1519" s="1" t="s">
         <v>188</v>
@@ -70372,22 +71017,31 @@
       <c r="K1519" t="s">
         <v>61</v>
       </c>
+      <c r="L1519">
+        <v>6262</v>
+      </c>
+      <c r="M1519" s="20">
+        <v>0.57071759259259258</v>
+      </c>
+      <c r="N1519">
+        <v>0.1410206</v>
+      </c>
       <c r="T1519" s="1" t="s">
         <v>543</v>
       </c>
     </row>
     <row r="1520" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1520">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B1520" t="s">
         <v>230</v>
       </c>
       <c r="C1520" t="s">
-        <v>202</v>
+        <v>59</v>
       </c>
       <c r="D1520">
-        <v>5.22</v>
+        <v>4.6470000000000002</v>
       </c>
       <c r="G1520" s="1" t="s">
         <v>188</v>
@@ -70404,13 +71058,22 @@
       <c r="K1520" t="s">
         <v>61</v>
       </c>
+      <c r="L1520">
+        <v>6262</v>
+      </c>
+      <c r="M1520" s="20">
+        <v>0.57168981481481485</v>
+      </c>
+      <c r="N1520">
+        <v>0.1130158</v>
+      </c>
       <c r="T1520" s="1" t="s">
         <v>543</v>
       </c>
     </row>
     <row r="1521" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1521">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B1521" t="s">
         <v>230</v>
@@ -70419,7 +71082,7 @@
         <v>59</v>
       </c>
       <c r="D1521">
-        <v>4.6470000000000002</v>
+        <v>8.48</v>
       </c>
       <c r="G1521" s="1" t="s">
         <v>188</v>
@@ -70436,13 +71099,22 @@
       <c r="K1521" t="s">
         <v>61</v>
       </c>
+      <c r="L1521">
+        <v>6262</v>
+      </c>
+      <c r="M1521" s="20">
+        <v>0.58685185185185185</v>
+      </c>
+      <c r="N1521">
+        <v>1.349885</v>
+      </c>
       <c r="T1521" s="1" t="s">
         <v>543</v>
       </c>
     </row>
     <row r="1522" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1522">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B1522" t="s">
         <v>230</v>
@@ -70451,7 +71123,7 @@
         <v>59</v>
       </c>
       <c r="D1522">
-        <v>8.48</v>
+        <v>6.6769999999999996</v>
       </c>
       <c r="G1522" s="1" t="s">
         <v>188</v>
@@ -70468,22 +71140,31 @@
       <c r="K1522" t="s">
         <v>61</v>
       </c>
+      <c r="L1522">
+        <v>6262</v>
+      </c>
+      <c r="M1522" s="20">
+        <v>0.58784722222222219</v>
+      </c>
+      <c r="N1522">
+        <v>0.13410610000000001</v>
+      </c>
       <c r="T1522" s="1" t="s">
         <v>543</v>
       </c>
     </row>
     <row r="1523" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1523">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B1523" t="s">
         <v>230</v>
       </c>
       <c r="C1523" t="s">
-        <v>59</v>
+        <v>202</v>
       </c>
       <c r="D1523">
-        <v>6.6769999999999996</v>
+        <v>6.6959999999999997</v>
       </c>
       <c r="G1523" s="1" t="s">
         <v>188</v>
@@ -70500,22 +71181,31 @@
       <c r="K1523" t="s">
         <v>61</v>
       </c>
+      <c r="L1523">
+        <v>6262</v>
+      </c>
+      <c r="M1523" s="20">
+        <v>0.58877314814814818</v>
+      </c>
+      <c r="N1523">
+        <v>0.141983</v>
+      </c>
       <c r="T1523" s="1" t="s">
         <v>543</v>
       </c>
     </row>
     <row r="1524" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1524">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B1524" t="s">
         <v>230</v>
       </c>
       <c r="C1524" t="s">
-        <v>202</v>
+        <v>59</v>
       </c>
       <c r="D1524">
-        <v>6.6959999999999997</v>
+        <v>9.2850000000000001</v>
       </c>
       <c r="G1524" s="1" t="s">
         <v>188</v>
@@ -70532,13 +71222,22 @@
       <c r="K1524" t="s">
         <v>61</v>
       </c>
+      <c r="L1524">
+        <v>6262</v>
+      </c>
+      <c r="M1524" s="20">
+        <v>0.5895717592592592</v>
+      </c>
+      <c r="N1524">
+        <v>1.445303</v>
+      </c>
       <c r="T1524" s="1" t="s">
         <v>543</v>
       </c>
     </row>
     <row r="1525" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1525">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B1525" t="s">
         <v>230</v>
@@ -70547,7 +71246,7 @@
         <v>59</v>
       </c>
       <c r="D1525">
-        <v>9.2850000000000001</v>
+        <v>6.6029999999999998</v>
       </c>
       <c r="G1525" s="1" t="s">
         <v>188</v>
@@ -70564,13 +71263,22 @@
       <c r="K1525" t="s">
         <v>61</v>
       </c>
+      <c r="L1525">
+        <v>6262</v>
+      </c>
+      <c r="M1525" s="20">
+        <v>0.59054398148148146</v>
+      </c>
+      <c r="N1525">
+        <v>0.24498300000000001</v>
+      </c>
       <c r="T1525" s="1" t="s">
         <v>543</v>
       </c>
     </row>
     <row r="1526" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1526">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B1526" t="s">
         <v>230</v>
@@ -70579,7 +71287,7 @@
         <v>59</v>
       </c>
       <c r="D1526">
-        <v>6.6029999999999998</v>
+        <v>4.7850000000000001</v>
       </c>
       <c r="G1526" s="1" t="s">
         <v>188</v>
@@ -70596,22 +71304,31 @@
       <c r="K1526" t="s">
         <v>61</v>
       </c>
+      <c r="L1526">
+        <v>6262</v>
+      </c>
+      <c r="M1526" s="20">
+        <v>0.59138888888888885</v>
+      </c>
+      <c r="N1526">
+        <v>0.1769606</v>
+      </c>
       <c r="T1526" s="1" t="s">
         <v>543</v>
       </c>
     </row>
     <row r="1527" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1527">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B1527" t="s">
         <v>230</v>
       </c>
       <c r="C1527" t="s">
-        <v>59</v>
+        <v>202</v>
       </c>
       <c r="D1527">
-        <v>4.7850000000000001</v>
+        <v>7.3460000000000001</v>
       </c>
       <c r="G1527" s="1" t="s">
         <v>188</v>
@@ -70628,13 +71345,22 @@
       <c r="K1527" t="s">
         <v>61</v>
       </c>
+      <c r="L1527">
+        <v>6262</v>
+      </c>
+      <c r="M1527" s="20">
+        <v>0.59234953703703697</v>
+      </c>
+      <c r="N1527">
+        <v>0.18763569999999999</v>
+      </c>
       <c r="T1527" s="1" t="s">
         <v>543</v>
       </c>
     </row>
     <row r="1528" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1528">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B1528" t="s">
         <v>230</v>
@@ -70643,7 +71369,7 @@
         <v>202</v>
       </c>
       <c r="D1528">
-        <v>7.3460000000000001</v>
+        <v>9.234</v>
       </c>
       <c r="G1528" s="1" t="s">
         <v>188</v>
@@ -70660,22 +71386,31 @@
       <c r="K1528" t="s">
         <v>61</v>
       </c>
+      <c r="L1528">
+        <v>6262</v>
+      </c>
+      <c r="M1528" s="20">
+        <v>0.59315972222222224</v>
+      </c>
+      <c r="N1528">
+        <v>0.2054723</v>
+      </c>
       <c r="T1528" s="1" t="s">
         <v>543</v>
       </c>
     </row>
     <row r="1529" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1529">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B1529" t="s">
         <v>230</v>
       </c>
       <c r="C1529" t="s">
-        <v>202</v>
+        <v>59</v>
       </c>
       <c r="D1529">
-        <v>9.234</v>
+        <v>7.44</v>
       </c>
       <c r="G1529" s="1" t="s">
         <v>188</v>
@@ -70692,13 +71427,22 @@
       <c r="K1529" t="s">
         <v>61</v>
       </c>
+      <c r="L1529">
+        <v>6262</v>
+      </c>
+      <c r="M1529" s="20">
+        <v>0.59400462962962963</v>
+      </c>
+      <c r="N1529">
+        <v>0.1292025</v>
+      </c>
       <c r="T1529" s="1" t="s">
         <v>543</v>
       </c>
     </row>
     <row r="1530" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1530">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B1530" t="s">
         <v>230</v>
@@ -70707,7 +71451,7 @@
         <v>59</v>
       </c>
       <c r="D1530">
-        <v>7.44</v>
+        <v>4.7549999999999999</v>
       </c>
       <c r="G1530" s="1" t="s">
         <v>188</v>
@@ -70724,22 +71468,31 @@
       <c r="K1530" t="s">
         <v>61</v>
       </c>
+      <c r="L1530">
+        <v>6262</v>
+      </c>
+      <c r="M1530" s="20">
+        <v>0.59483796296296299</v>
+      </c>
+      <c r="N1530">
+        <v>6.6984799999999997E-2</v>
+      </c>
       <c r="T1530" s="1" t="s">
         <v>543</v>
       </c>
     </row>
     <row r="1531" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1531">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B1531" t="s">
         <v>230</v>
       </c>
       <c r="C1531" t="s">
-        <v>59</v>
+        <v>202</v>
       </c>
       <c r="D1531">
-        <v>4.7549999999999999</v>
+        <v>3.3210000000000002</v>
       </c>
       <c r="G1531" s="1" t="s">
         <v>188</v>
@@ -70756,22 +71509,31 @@
       <c r="K1531" t="s">
         <v>61</v>
       </c>
+      <c r="L1531">
+        <v>6262</v>
+      </c>
+      <c r="M1531" s="20">
+        <v>0.59561342592592592</v>
+      </c>
+      <c r="N1531" s="21">
+        <v>9.1267319999999999E-2</v>
+      </c>
       <c r="T1531" s="1" t="s">
         <v>543</v>
       </c>
     </row>
     <row r="1532" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1532">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B1532" t="s">
         <v>230</v>
       </c>
       <c r="C1532" t="s">
-        <v>202</v>
+        <v>59</v>
       </c>
       <c r="D1532">
-        <v>3.3210000000000002</v>
+        <v>10.071999999999999</v>
       </c>
       <c r="G1532" s="1" t="s">
         <v>188</v>
@@ -70788,13 +71550,22 @@
       <c r="K1532" t="s">
         <v>61</v>
       </c>
+      <c r="L1532">
+        <v>6262</v>
+      </c>
+      <c r="M1532" s="20">
+        <v>0.59636574074074067</v>
+      </c>
+      <c r="N1532">
+        <v>0.30558649999999998</v>
+      </c>
       <c r="T1532" s="1" t="s">
         <v>543</v>
       </c>
     </row>
     <row r="1533" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1533">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B1533" t="s">
         <v>230</v>
@@ -70803,7 +71574,7 @@
         <v>59</v>
       </c>
       <c r="D1533">
-        <v>10.071999999999999</v>
+        <v>7.7770000000000001</v>
       </c>
       <c r="G1533" s="1" t="s">
         <v>188</v>
@@ -70820,22 +71591,31 @@
       <c r="K1533" t="s">
         <v>61</v>
       </c>
+      <c r="L1533">
+        <v>6262</v>
+      </c>
+      <c r="M1533" s="20">
+        <v>0.59717592592592594</v>
+      </c>
+      <c r="N1533">
+        <v>0.1735042</v>
+      </c>
       <c r="T1533" s="1" t="s">
         <v>543</v>
       </c>
     </row>
     <row r="1534" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1534">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B1534" t="s">
         <v>230</v>
       </c>
       <c r="C1534" t="s">
-        <v>59</v>
+        <v>202</v>
       </c>
       <c r="D1534">
-        <v>7.7770000000000001</v>
+        <v>6.66</v>
       </c>
       <c r="G1534" s="1" t="s">
         <v>188</v>
@@ -70852,22 +71632,31 @@
       <c r="K1534" t="s">
         <v>61</v>
       </c>
+      <c r="L1534">
+        <v>6262</v>
+      </c>
+      <c r="M1534" s="20">
+        <v>0.59809027777777779</v>
+      </c>
+      <c r="N1534">
+        <v>0.1981745</v>
+      </c>
       <c r="T1534" s="1" t="s">
         <v>543</v>
       </c>
     </row>
     <row r="1535" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1535">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B1535" t="s">
         <v>230</v>
       </c>
       <c r="C1535" t="s">
-        <v>202</v>
+        <v>59</v>
       </c>
       <c r="D1535">
-        <v>6.66</v>
+        <v>7.2690000000000001</v>
       </c>
       <c r="G1535" s="1" t="s">
         <v>188</v>
@@ -70884,13 +71673,22 @@
       <c r="K1535" t="s">
         <v>61</v>
       </c>
+      <c r="L1535">
+        <v>6262</v>
+      </c>
+      <c r="M1535" s="20">
+        <v>0.59894675925925933</v>
+      </c>
+      <c r="N1535">
+        <v>0.82277009999999995</v>
+      </c>
       <c r="T1535" s="1" t="s">
         <v>543</v>
       </c>
     </row>
     <row r="1536" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1536">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B1536" t="s">
         <v>230</v>
@@ -70899,7 +71697,7 @@
         <v>59</v>
       </c>
       <c r="D1536">
-        <v>7.2690000000000001</v>
+        <v>10.558</v>
       </c>
       <c r="G1536" s="1" t="s">
         <v>188</v>
@@ -70916,22 +71714,28 @@
       <c r="K1536" t="s">
         <v>61</v>
       </c>
+      <c r="L1536">
+        <v>6262</v>
+      </c>
+      <c r="M1536" s="20">
+        <v>0.59978009259259257</v>
+      </c>
+      <c r="N1536">
+        <v>0.1188077</v>
+      </c>
       <c r="T1536" s="1" t="s">
         <v>543</v>
       </c>
     </row>
     <row r="1537" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1537">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B1537" t="s">
         <v>230</v>
       </c>
       <c r="C1537" t="s">
-        <v>59</v>
-      </c>
-      <c r="D1537">
-        <v>10.558</v>
+        <v>703</v>
       </c>
       <c r="G1537" s="1" t="s">
         <v>188</v>
@@ -70948,13 +71752,22 @@
       <c r="K1537" t="s">
         <v>61</v>
       </c>
+      <c r="L1537">
+        <v>6262</v>
+      </c>
+      <c r="M1537" s="20">
+        <v>0.60063657407407411</v>
+      </c>
+      <c r="N1537" s="21">
+        <v>1.6983680000000001E-2</v>
+      </c>
       <c r="T1537" s="1" t="s">
         <v>543</v>
       </c>
     </row>
     <row r="1538" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1538">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B1538" t="s">
         <v>230</v>
@@ -70962,6 +71775,9 @@
       <c r="C1538" t="s">
         <v>703</v>
       </c>
+      <c r="E1538" s="1" t="s">
+        <v>1031</v>
+      </c>
       <c r="G1538" s="1" t="s">
         <v>188</v>
       </c>
@@ -70977,40 +71793,44 @@
       <c r="K1538" t="s">
         <v>61</v>
       </c>
+      <c r="L1538">
+        <v>6262</v>
+      </c>
       <c r="T1538" s="1" t="s">
         <v>543</v>
       </c>
     </row>
     <row r="1539" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1539">
-        <v>47</v>
-      </c>
-      <c r="B1539" t="s">
-        <v>230</v>
+        <v>1</v>
       </c>
       <c r="C1539" t="s">
-        <v>703</v>
-      </c>
-      <c r="E1539" s="1" t="s">
-        <v>1032</v>
+        <v>60</v>
       </c>
       <c r="G1539" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="H1539" s="1" t="s">
-        <v>198</v>
+        <v>88</v>
       </c>
       <c r="I1539" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="J1539">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="K1539" t="s">
         <v>61</v>
       </c>
       <c r="T1539" s="1" t="s">
-        <v>543</v>
+        <v>194</v>
+      </c>
+      <c r="Y1539" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z1539" t="str">
+        <f>"A2-8"&amp;Y1539&amp;"-"&amp;AC1539</f>
+        <v>A2-8RT-A1</v>
+      </c>
+      <c r="AC1539" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="1540" spans="1:29" x14ac:dyDescent="0.25">
@@ -71036,11 +71856,11 @@
         <v>194</v>
       </c>
       <c r="Y1540" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="Z1540" t="str">
         <f>"A2-8"&amp;Y1540&amp;"-"&amp;AC1540</f>
-        <v>A2-8RT-A1</v>
+        <v>A2-8SO-A1</v>
       </c>
       <c r="AC1540" t="s">
         <v>248</v>
@@ -71054,13 +71874,13 @@
         <v>60</v>
       </c>
       <c r="G1541" s="1" t="s">
-        <v>88</v>
+        <v>188</v>
       </c>
       <c r="I1541" s="1" t="s">
         <v>70</v>
       </c>
       <c r="J1541">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="K1541" t="s">
         <v>61</v>
@@ -71069,19 +71889,15 @@
         <v>194</v>
       </c>
       <c r="Y1541" t="s">
-        <v>87</v>
-      </c>
-      <c r="Z1541" t="str">
-        <f>"A2-8"&amp;Y1541&amp;"-"&amp;AC1541</f>
-        <v>A2-8SO-A1</v>
-      </c>
-      <c r="AC1541" t="s">
-        <v>248</v>
+        <v>85</v>
+      </c>
+      <c r="Z1541" t="s">
+        <v>1032</v>
       </c>
     </row>
     <row r="1542" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1542">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C1542" t="s">
         <v>60</v>
@@ -71102,10 +71918,14 @@
         <v>194</v>
       </c>
       <c r="Y1542" t="s">
-        <v>85</v>
-      </c>
-      <c r="Z1542" t="s">
-        <v>1033</v>
+        <v>86</v>
+      </c>
+      <c r="Z1542" t="str">
+        <f t="shared" ref="Z1542:Z1544" si="21">"A2-8"&amp;Y1542&amp;"-"&amp;AC1542</f>
+        <v>A2-8RT-A2</v>
+      </c>
+      <c r="AC1542" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="1543" spans="1:29" x14ac:dyDescent="0.25">
@@ -71131,11 +71951,11 @@
         <v>194</v>
       </c>
       <c r="Y1543" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="Z1543" t="str">
-        <f t="shared" ref="Z1543:Z1545" si="21">"A2-8"&amp;Y1543&amp;"-"&amp;AC1543</f>
-        <v>A2-8RT-A2</v>
+        <f t="shared" si="21"/>
+        <v>A2-8SO-A2</v>
       </c>
       <c r="AC1543" t="s">
         <v>121</v>
@@ -71143,7 +71963,7 @@
     </row>
     <row r="1544" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1544">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C1544" t="s">
         <v>60</v>
@@ -71168,27 +71988,27 @@
       </c>
       <c r="Z1544" t="str">
         <f t="shared" si="21"/>
-        <v>A2-8SO-A2</v>
+        <v>A2-8SO-H1</v>
       </c>
       <c r="AC1544" t="s">
-        <v>121</v>
+        <v>240</v>
       </c>
     </row>
     <row r="1545" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1545">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C1545" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G1545" s="1" t="s">
-        <v>188</v>
+        <v>88</v>
       </c>
       <c r="I1545" s="1" t="s">
         <v>70</v>
       </c>
       <c r="J1545">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="K1545" t="s">
         <v>61</v>
@@ -71197,19 +72017,15 @@
         <v>194</v>
       </c>
       <c r="Y1545" t="s">
-        <v>87</v>
-      </c>
-      <c r="Z1545" t="str">
-        <f t="shared" si="21"/>
-        <v>A2-8SO-H1</v>
-      </c>
-      <c r="AC1545" t="s">
-        <v>240</v>
+        <v>85</v>
+      </c>
+      <c r="Z1545" t="s">
+        <v>1033</v>
       </c>
     </row>
     <row r="1546" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1546">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C1546" t="s">
         <v>59</v>
@@ -71238,7 +72054,7 @@
     </row>
     <row r="1547" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1547">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C1547" t="s">
         <v>59</v>
@@ -71267,7 +72083,7 @@
     </row>
     <row r="1548" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1548">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C1548" t="s">
         <v>59</v>
@@ -71288,15 +72104,19 @@
         <v>194</v>
       </c>
       <c r="Y1548" t="s">
-        <v>85</v>
-      </c>
-      <c r="Z1548" t="s">
-        <v>1036</v>
+        <v>86</v>
+      </c>
+      <c r="Z1548" t="str">
+        <f t="shared" ref="Z1548:Z1553" si="22">"A2-8"&amp;Y1548&amp;"-"&amp;AC1548</f>
+        <v>A2-8RT-A3</v>
+      </c>
+      <c r="AC1548" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="1549" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1549">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C1549" t="s">
         <v>59</v>
@@ -71320,16 +72140,16 @@
         <v>86</v>
       </c>
       <c r="Z1549" t="str">
-        <f t="shared" ref="Z1549:Z1554" si="22">"A2-8"&amp;Y1549&amp;"-"&amp;AC1549</f>
-        <v>A2-8RT-A3</v>
+        <f t="shared" si="22"/>
+        <v>A2-8RT-A4</v>
       </c>
       <c r="AC1549" t="s">
-        <v>246</v>
+        <v>253</v>
       </c>
     </row>
     <row r="1550" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1550">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C1550" t="s">
         <v>59</v>
@@ -71354,15 +72174,15 @@
       </c>
       <c r="Z1550" t="str">
         <f t="shared" si="22"/>
-        <v>A2-8RT-A4</v>
+        <v>A2-8RT-A5</v>
       </c>
       <c r="AC1550" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
     </row>
     <row r="1551" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1551">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C1551" t="s">
         <v>59</v>
@@ -71383,19 +72203,19 @@
         <v>194</v>
       </c>
       <c r="Y1551" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="Z1551" t="str">
         <f t="shared" si="22"/>
-        <v>A2-8RT-A5</v>
+        <v>A2-8SO-A3</v>
       </c>
       <c r="AC1551" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="1552" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1552">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C1552" t="s">
         <v>59</v>
@@ -71420,15 +72240,15 @@
       </c>
       <c r="Z1552" t="str">
         <f t="shared" si="22"/>
-        <v>A2-8SO-A3</v>
+        <v>A2-8SO-A4</v>
       </c>
       <c r="AC1552" t="s">
-        <v>246</v>
+        <v>253</v>
       </c>
     </row>
     <row r="1553" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1553">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C1553" t="s">
         <v>59</v>
@@ -71453,27 +72273,27 @@
       </c>
       <c r="Z1553" t="str">
         <f t="shared" si="22"/>
-        <v>A2-8SO-A4</v>
+        <v>A2-8SO-A5</v>
       </c>
       <c r="AC1553" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
     </row>
     <row r="1554" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1554">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C1554" t="s">
-        <v>59</v>
+        <v>202</v>
       </c>
       <c r="G1554" s="1" t="s">
-        <v>88</v>
+        <v>188</v>
       </c>
       <c r="I1554" s="1" t="s">
         <v>70</v>
       </c>
       <c r="J1554">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="K1554" t="s">
         <v>61</v>
@@ -71482,19 +72302,15 @@
         <v>194</v>
       </c>
       <c r="Y1554" t="s">
-        <v>87</v>
-      </c>
-      <c r="Z1554" t="str">
-        <f t="shared" si="22"/>
-        <v>A2-8SO-A5</v>
-      </c>
-      <c r="AC1554" t="s">
-        <v>247</v>
+        <v>85</v>
+      </c>
+      <c r="Z1554" t="s">
+        <v>1036</v>
       </c>
     </row>
     <row r="1555" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1555">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C1555" t="s">
         <v>202</v>
@@ -71523,7 +72339,7 @@
     </row>
     <row r="1556" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1556">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C1556" t="s">
         <v>202</v>
@@ -71552,7 +72368,7 @@
     </row>
     <row r="1557" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1557">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C1557" t="s">
         <v>202</v>
@@ -71581,7 +72397,7 @@
     </row>
     <row r="1558" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1558">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C1558" t="s">
         <v>202</v>
@@ -71610,7 +72426,7 @@
     </row>
     <row r="1559" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1559">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C1559" t="s">
         <v>202</v>
@@ -71639,7 +72455,7 @@
     </row>
     <row r="1560" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1560">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C1560" t="s">
         <v>202</v>
@@ -71668,7 +72484,7 @@
     </row>
     <row r="1561" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1561">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C1561" t="s">
         <v>202</v>
@@ -71697,7 +72513,7 @@
     </row>
     <row r="1562" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1562">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C1562" t="s">
         <v>202</v>
@@ -71726,7 +72542,7 @@
     </row>
     <row r="1563" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1563">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C1563" t="s">
         <v>202</v>
@@ -71755,7 +72571,7 @@
     </row>
     <row r="1564" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1564">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C1564" t="s">
         <v>202</v>
@@ -71784,7 +72600,7 @@
     </row>
     <row r="1565" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1565">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="C1565" t="s">
         <v>202</v>
@@ -71805,15 +72621,19 @@
         <v>194</v>
       </c>
       <c r="Y1565" t="s">
-        <v>85</v>
-      </c>
-      <c r="Z1565" t="s">
-        <v>1047</v>
+        <v>86</v>
+      </c>
+      <c r="Z1565" t="str">
+        <f t="shared" ref="Z1565:Z1588" si="23">"A2-8"&amp;Y1565&amp;"-"&amp;AC1565</f>
+        <v>A2-8RT-E1</v>
+      </c>
+      <c r="AC1565" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="1566" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1566">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C1566" t="s">
         <v>202</v>
@@ -71837,16 +72657,16 @@
         <v>86</v>
       </c>
       <c r="Z1566" t="str">
-        <f t="shared" ref="Z1566:Z1589" si="23">"A2-8"&amp;Y1566&amp;"-"&amp;AC1566</f>
-        <v>A2-8RT-E1</v>
+        <f t="shared" si="23"/>
+        <v>A2-8RT-E2</v>
       </c>
       <c r="AC1566" t="s">
-        <v>138</v>
+        <v>179</v>
       </c>
     </row>
     <row r="1567" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1567">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C1567" t="s">
         <v>202</v>
@@ -71871,15 +72691,15 @@
       </c>
       <c r="Z1567" t="str">
         <f t="shared" si="23"/>
-        <v>A2-8RT-E2</v>
+        <v>A2-8RT-E3</v>
       </c>
       <c r="AC1567" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="1568" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1568">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C1568" t="s">
         <v>202</v>
@@ -71904,15 +72724,15 @@
       </c>
       <c r="Z1568" t="str">
         <f t="shared" si="23"/>
-        <v>A2-8RT-E3</v>
+        <v>A2-8RT-E4</v>
       </c>
       <c r="AC1568" t="s">
-        <v>180</v>
+        <v>398</v>
       </c>
     </row>
     <row r="1569" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1569">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C1569" t="s">
         <v>202</v>
@@ -71937,15 +72757,15 @@
       </c>
       <c r="Z1569" t="str">
         <f t="shared" si="23"/>
-        <v>A2-8RT-E4</v>
+        <v>A2-8RT-E5</v>
       </c>
       <c r="AC1569" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
     </row>
     <row r="1570" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1570">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C1570" t="s">
         <v>202</v>
@@ -71970,15 +72790,15 @@
       </c>
       <c r="Z1570" t="str">
         <f t="shared" si="23"/>
-        <v>A2-8RT-E5</v>
+        <v>A2-8RT-E6</v>
       </c>
       <c r="AC1570" t="s">
-        <v>399</v>
+        <v>157</v>
       </c>
     </row>
     <row r="1571" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1571">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C1571" t="s">
         <v>202</v>
@@ -72003,15 +72823,15 @@
       </c>
       <c r="Z1571" t="str">
         <f t="shared" si="23"/>
-        <v>A2-8RT-E6</v>
+        <v>A2-8RT-E7</v>
       </c>
       <c r="AC1571" t="s">
-        <v>157</v>
+        <v>132</v>
       </c>
     </row>
     <row r="1572" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1572">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C1572" t="s">
         <v>202</v>
@@ -72036,15 +72856,15 @@
       </c>
       <c r="Z1572" t="str">
         <f t="shared" si="23"/>
-        <v>A2-8RT-E7</v>
+        <v>A2-8RT-E8</v>
       </c>
       <c r="AC1572" t="s">
-        <v>132</v>
+        <v>386</v>
       </c>
     </row>
     <row r="1573" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1573">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C1573" t="s">
         <v>202</v>
@@ -72069,15 +72889,15 @@
       </c>
       <c r="Z1573" t="str">
         <f t="shared" si="23"/>
-        <v>A2-8RT-E8</v>
+        <v>A2-8RT-E9</v>
       </c>
       <c r="AC1573" t="s">
-        <v>386</v>
+        <v>168</v>
       </c>
     </row>
     <row r="1574" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1574">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C1574" t="s">
         <v>202</v>
@@ -72102,15 +72922,15 @@
       </c>
       <c r="Z1574" t="str">
         <f t="shared" si="23"/>
-        <v>A2-8RT-E9</v>
+        <v>A2-8RT-E10</v>
       </c>
       <c r="AC1574" t="s">
-        <v>168</v>
+        <v>249</v>
       </c>
     </row>
     <row r="1575" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1575">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C1575" t="s">
         <v>202</v>
@@ -72135,15 +72955,15 @@
       </c>
       <c r="Z1575" t="str">
         <f t="shared" si="23"/>
-        <v>A2-8RT-E10</v>
+        <v>A2-8RT-E11</v>
       </c>
       <c r="AC1575" t="s">
-        <v>249</v>
+        <v>432</v>
       </c>
     </row>
     <row r="1576" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1576">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C1576" t="s">
         <v>202</v>
@@ -72168,15 +72988,15 @@
       </c>
       <c r="Z1576" t="str">
         <f t="shared" si="23"/>
-        <v>A2-8RT-E11</v>
+        <v>A2-8RT-E12</v>
       </c>
       <c r="AC1576" t="s">
-        <v>432</v>
+        <v>176</v>
       </c>
     </row>
     <row r="1577" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1577">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="C1577" t="s">
         <v>202</v>
@@ -72197,19 +73017,19 @@
         <v>194</v>
       </c>
       <c r="Y1577" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="Z1577" t="str">
         <f t="shared" si="23"/>
-        <v>A2-8RT-E12</v>
+        <v>A2-8SO-E1</v>
       </c>
       <c r="AC1577" t="s">
-        <v>176</v>
+        <v>138</v>
       </c>
     </row>
     <row r="1578" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1578">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C1578" t="s">
         <v>202</v>
@@ -72234,15 +73054,15 @@
       </c>
       <c r="Z1578" t="str">
         <f t="shared" si="23"/>
-        <v>A2-8SO-E1</v>
+        <v>A2-8SO-E2</v>
       </c>
       <c r="AC1578" t="s">
-        <v>138</v>
+        <v>179</v>
       </c>
     </row>
     <row r="1579" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1579">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C1579" t="s">
         <v>202</v>
@@ -72267,15 +73087,15 @@
       </c>
       <c r="Z1579" t="str">
         <f t="shared" si="23"/>
-        <v>A2-8SO-E2</v>
+        <v>A2-8SO-E3</v>
       </c>
       <c r="AC1579" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="1580" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1580">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C1580" t="s">
         <v>202</v>
@@ -72300,15 +73120,15 @@
       </c>
       <c r="Z1580" t="str">
         <f t="shared" si="23"/>
-        <v>A2-8SO-E3</v>
+        <v>A2-8SO-E4</v>
       </c>
       <c r="AC1580" t="s">
-        <v>180</v>
+        <v>398</v>
       </c>
     </row>
     <row r="1581" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1581">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C1581" t="s">
         <v>202</v>
@@ -72333,15 +73153,15 @@
       </c>
       <c r="Z1581" t="str">
         <f t="shared" si="23"/>
-        <v>A2-8SO-E4</v>
+        <v>A2-8SO-E5</v>
       </c>
       <c r="AC1581" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
     </row>
     <row r="1582" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1582">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C1582" t="s">
         <v>202</v>
@@ -72366,15 +73186,15 @@
       </c>
       <c r="Z1582" t="str">
         <f t="shared" si="23"/>
-        <v>A2-8SO-E5</v>
+        <v>A2-8SO-E6</v>
       </c>
       <c r="AC1582" t="s">
-        <v>399</v>
+        <v>157</v>
       </c>
     </row>
     <row r="1583" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1583">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C1583" t="s">
         <v>202</v>
@@ -72399,15 +73219,15 @@
       </c>
       <c r="Z1583" t="str">
         <f t="shared" si="23"/>
-        <v>A2-8SO-E6</v>
+        <v>A2-8SO-E7</v>
       </c>
       <c r="AC1583" t="s">
-        <v>157</v>
+        <v>132</v>
       </c>
     </row>
     <row r="1584" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1584">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C1584" t="s">
         <v>202</v>
@@ -72432,15 +73252,15 @@
       </c>
       <c r="Z1584" t="str">
         <f t="shared" si="23"/>
-        <v>A2-8SO-E7</v>
+        <v>A2-8SO-E8</v>
       </c>
       <c r="AC1584" t="s">
-        <v>132</v>
+        <v>386</v>
       </c>
     </row>
     <row r="1585" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1585">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C1585" t="s">
         <v>202</v>
@@ -72465,15 +73285,15 @@
       </c>
       <c r="Z1585" t="str">
         <f t="shared" si="23"/>
-        <v>A2-8SO-E8</v>
+        <v>A2-8SO-E9</v>
       </c>
       <c r="AC1585" t="s">
-        <v>386</v>
+        <v>168</v>
       </c>
     </row>
     <row r="1586" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1586">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C1586" t="s">
         <v>202</v>
@@ -72498,15 +73318,15 @@
       </c>
       <c r="Z1586" t="str">
         <f t="shared" si="23"/>
-        <v>A2-8SO-E9</v>
+        <v>A2-8SO-E10</v>
       </c>
       <c r="AC1586" t="s">
-        <v>168</v>
+        <v>249</v>
       </c>
     </row>
     <row r="1587" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1587">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C1587" t="s">
         <v>202</v>
@@ -72531,15 +73351,15 @@
       </c>
       <c r="Z1587" t="str">
         <f t="shared" si="23"/>
-        <v>A2-8SO-E10</v>
+        <v>A2-8SO-E11</v>
       </c>
       <c r="AC1587" t="s">
-        <v>249</v>
+        <v>432</v>
       </c>
     </row>
     <row r="1588" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1588">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C1588" t="s">
         <v>202</v>
@@ -72564,42 +73384,9 @@
       </c>
       <c r="Z1588" t="str">
         <f t="shared" si="23"/>
-        <v>A2-8SO-E11</v>
+        <v>A2-8SO-E12</v>
       </c>
       <c r="AC1588" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="1589" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A1589">
-        <v>18</v>
-      </c>
-      <c r="C1589" t="s">
-        <v>202</v>
-      </c>
-      <c r="G1589" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="I1589" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="J1589">
-        <v>8</v>
-      </c>
-      <c r="K1589" t="s">
-        <v>61</v>
-      </c>
-      <c r="T1589" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="Y1589" t="s">
-        <v>87</v>
-      </c>
-      <c r="Z1589" t="str">
-        <f t="shared" si="23"/>
-        <v>A2-8SO-E12</v>
-      </c>
-      <c r="AC1589" t="s">
         <v>176</v>
       </c>
     </row>

</xml_diff>

<commit_message>
entering day 14 weights 2018-09-09 apple cohort day 10+25
</commit_message>
<xml_diff>
--- a/Data/2018-08-14_master_datac_2018_collection_year.xlsx
+++ b/Data/2018-08-14_master_datac_2018_collection_year.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andrew.nguyen\Desktop\Circadian_rhythm_runs_seasonal_timing\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{026C3D52-68A1-4A7A-A61C-E3F5C6821888}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{445789D5-01ED-48E6-BE3A-B86E39B9A248}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9855" yWindow="7665" windowWidth="36360" windowHeight="21135" activeTab="1" xr2:uid="{C7477166-8A7C-B04A-9643-C277FEDCDAAB}"/>
   </bookViews>
@@ -14175,8 +14175,8 @@
   <dimension ref="A1:AS1588"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1052" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L1065" sqref="L1065"/>
+      <pane ySplit="1" topLeftCell="A1184" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O1205" sqref="O1205"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -55294,6 +55294,9 @@
       <c r="N1119">
         <v>0.1301273</v>
       </c>
+      <c r="O1119">
+        <v>6.42</v>
+      </c>
       <c r="T1119" s="1" t="s">
         <v>221</v>
       </c>
@@ -55344,6 +55347,9 @@
       <c r="N1120">
         <v>0.60055080000000005</v>
       </c>
+      <c r="O1120">
+        <v>4.234</v>
+      </c>
       <c r="T1120" s="1" t="s">
         <v>221</v>
       </c>
@@ -55391,6 +55397,9 @@
       <c r="N1121">
         <v>0.14884349999999999</v>
       </c>
+      <c r="O1121">
+        <v>6.5389999999999997</v>
+      </c>
       <c r="T1121" s="1" t="s">
         <v>221</v>
       </c>
@@ -55441,6 +55450,9 @@
       <c r="N1122">
         <v>0.40967320000000002</v>
       </c>
+      <c r="O1122">
+        <v>3.056</v>
+      </c>
       <c r="T1122" s="1" t="s">
         <v>221</v>
       </c>
@@ -55491,6 +55503,9 @@
       <c r="N1123">
         <v>5.0958499999999997E-2</v>
       </c>
+      <c r="O1123">
+        <v>7.0469999999999997</v>
+      </c>
       <c r="T1123" s="1" t="s">
         <v>221</v>
       </c>
@@ -55541,6 +55556,9 @@
       <c r="N1124">
         <v>0.15245049999999999</v>
       </c>
+      <c r="O1124">
+        <v>4.3899999999999997</v>
+      </c>
       <c r="T1124" s="1" t="s">
         <v>221</v>
       </c>
@@ -55588,6 +55606,9 @@
       <c r="N1125">
         <v>0.2787984</v>
       </c>
+      <c r="O1125">
+        <v>3.7320000000000002</v>
+      </c>
       <c r="T1125" s="1" t="s">
         <v>221</v>
       </c>
@@ -55638,6 +55659,9 @@
       <c r="N1126" s="21">
         <v>5.437939E-2</v>
       </c>
+      <c r="O1126">
+        <v>5.42</v>
+      </c>
       <c r="T1126" s="1" t="s">
         <v>221</v>
       </c>
@@ -55688,6 +55712,9 @@
       <c r="N1127" s="21">
         <v>4.4645959999999998E-2</v>
       </c>
+      <c r="O1127">
+        <v>4.117</v>
+      </c>
       <c r="T1127" s="1" t="s">
         <v>221</v>
       </c>
@@ -55735,6 +55762,9 @@
       <c r="N1128">
         <v>0.1212297</v>
       </c>
+      <c r="O1128">
+        <v>6.0730000000000004</v>
+      </c>
       <c r="T1128" s="1" t="s">
         <v>221</v>
       </c>
@@ -55782,6 +55812,9 @@
       <c r="N1129">
         <v>0.66719410000000001</v>
       </c>
+      <c r="O1129">
+        <v>6.6859999999999999</v>
+      </c>
       <c r="T1129" s="1" t="s">
         <v>221</v>
       </c>
@@ -55832,6 +55865,9 @@
       <c r="N1130">
         <v>0.24837790000000001</v>
       </c>
+      <c r="O1130">
+        <v>2.9689999999999999</v>
+      </c>
       <c r="T1130" s="1" t="s">
         <v>221</v>
       </c>
@@ -55882,6 +55918,9 @@
       <c r="N1131">
         <v>0.1230319</v>
       </c>
+      <c r="O1131">
+        <v>7.367</v>
+      </c>
       <c r="T1131" s="1" t="s">
         <v>221</v>
       </c>
@@ -55932,6 +55971,9 @@
       <c r="N1132" s="21">
         <v>6.4228830000000001E-2</v>
       </c>
+      <c r="O1132">
+        <v>8.0570000000000004</v>
+      </c>
       <c r="T1132" s="1" t="s">
         <v>221</v>
       </c>
@@ -55982,6 +56024,9 @@
       <c r="N1133">
         <v>0.62002860000000004</v>
       </c>
+      <c r="O1133">
+        <v>5.681</v>
+      </c>
       <c r="T1133" s="1" t="s">
         <v>221</v>
       </c>
@@ -56029,6 +56074,9 @@
       <c r="N1134" s="21">
         <v>4.1810710000000001E-2</v>
       </c>
+      <c r="O1134">
+        <v>3.363</v>
+      </c>
       <c r="T1134" s="1" t="s">
         <v>221</v>
       </c>
@@ -56126,6 +56174,9 @@
       <c r="N1136" s="21">
         <v>4.3292450000000003E-2</v>
       </c>
+      <c r="O1136">
+        <v>4.3920000000000003</v>
+      </c>
       <c r="T1136" s="1" t="s">
         <v>221</v>
       </c>
@@ -56173,6 +56224,9 @@
       <c r="N1137">
         <v>0.38923530000000001</v>
       </c>
+      <c r="O1137">
+        <v>4.1479999999999997</v>
+      </c>
       <c r="T1137" s="1" t="s">
         <v>221</v>
       </c>
@@ -56223,6 +56277,9 @@
       <c r="N1138" s="21">
         <v>5.9499459999999997E-2</v>
       </c>
+      <c r="O1138">
+        <v>2.76</v>
+      </c>
       <c r="T1138" s="1" t="s">
         <v>221</v>
       </c>
@@ -56273,6 +56330,9 @@
       <c r="N1139" s="21">
         <v>6.9297280000000003E-2</v>
       </c>
+      <c r="O1139">
+        <v>6.2119999999999997</v>
+      </c>
       <c r="T1139" s="1" t="s">
         <v>221</v>
       </c>
@@ -56323,6 +56383,9 @@
       <c r="N1140">
         <v>0.10623829999999999</v>
       </c>
+      <c r="O1140">
+        <v>4.5620000000000003</v>
+      </c>
       <c r="T1140" s="1" t="s">
         <v>221</v>
       </c>
@@ -56373,6 +56436,9 @@
       <c r="N1141">
         <v>0.14765629999999999</v>
       </c>
+      <c r="O1141">
+        <v>4.2720000000000002</v>
+      </c>
       <c r="T1141" s="1" t="s">
         <v>221</v>
       </c>
@@ -56423,6 +56489,9 @@
       <c r="N1142">
         <v>0.5812039</v>
       </c>
+      <c r="O1142">
+        <v>6.4859999999999998</v>
+      </c>
       <c r="T1142" s="1" t="s">
         <v>221</v>
       </c>
@@ -56473,6 +56542,9 @@
       <c r="N1143">
         <v>0.10971740000000001</v>
       </c>
+      <c r="O1143">
+        <v>4.6349999999999998</v>
+      </c>
       <c r="T1143" s="1" t="s">
         <v>221</v>
       </c>
@@ -56520,6 +56592,9 @@
       <c r="N1144">
         <v>0.4975908</v>
       </c>
+      <c r="O1144">
+        <v>4.8609999999999998</v>
+      </c>
       <c r="T1144" s="1" t="s">
         <v>221</v>
       </c>
@@ -56567,6 +56642,9 @@
       <c r="N1145">
         <v>0.22076380000000001</v>
       </c>
+      <c r="O1145">
+        <v>6.4470000000000001</v>
+      </c>
       <c r="T1145" s="1" t="s">
         <v>221</v>
       </c>
@@ -56617,6 +56695,9 @@
       <c r="N1146" s="21">
         <v>8.8099689999999994E-2</v>
       </c>
+      <c r="O1146">
+        <v>2.1749999999999998</v>
+      </c>
       <c r="T1146" s="1" t="s">
         <v>221</v>
       </c>
@@ -56667,6 +56748,9 @@
       <c r="N1147">
         <v>0.17090340000000001</v>
       </c>
+      <c r="O1147">
+        <v>2.0030000000000001</v>
+      </c>
       <c r="T1147" s="1" t="s">
         <v>221</v>
       </c>
@@ -56714,6 +56798,9 @@
       <c r="N1148" s="21">
         <v>4.8078509999999998E-2</v>
       </c>
+      <c r="O1148">
+        <v>4.4640000000000004</v>
+      </c>
       <c r="T1148" s="1" t="s">
         <v>221</v>
       </c>
@@ -56764,6 +56851,9 @@
       <c r="N1149" s="21">
         <v>7.4357870000000006E-2</v>
       </c>
+      <c r="O1149">
+        <v>3.859</v>
+      </c>
       <c r="T1149" s="1" t="s">
         <v>221</v>
       </c>
@@ -56811,6 +56901,9 @@
       <c r="N1150" s="21">
         <v>5.6203120000000002E-2</v>
       </c>
+      <c r="O1150">
+        <v>5.3280000000000003</v>
+      </c>
       <c r="T1150" s="1" t="s">
         <v>221</v>
       </c>
@@ -56861,6 +56954,9 @@
       <c r="N1151">
         <v>0.31155909999999998</v>
       </c>
+      <c r="O1151">
+        <v>2.4990000000000001</v>
+      </c>
       <c r="T1151" s="1" t="s">
         <v>221</v>
       </c>
@@ -56911,6 +57007,9 @@
       <c r="N1152" s="21">
         <v>4.5546650000000001E-2</v>
       </c>
+      <c r="O1152">
+        <v>5.4260000000000002</v>
+      </c>
       <c r="T1152" s="1" t="s">
         <v>221</v>
       </c>
@@ -56961,6 +57060,9 @@
       <c r="N1153">
         <v>0.46958719999999998</v>
       </c>
+      <c r="O1153">
+        <v>4.2110000000000003</v>
+      </c>
       <c r="T1153" s="1" t="s">
         <v>221</v>
       </c>
@@ -57011,6 +57113,9 @@
       <c r="N1154">
         <v>0.50150130000000004</v>
       </c>
+      <c r="O1154">
+        <v>4.2389999999999999</v>
+      </c>
       <c r="T1154" s="1" t="s">
         <v>221</v>
       </c>
@@ -57061,6 +57166,9 @@
       <c r="N1155">
         <v>0.3936133</v>
       </c>
+      <c r="O1155">
+        <v>3.8039999999999998</v>
+      </c>
       <c r="T1155" s="1" t="s">
         <v>221</v>
       </c>
@@ -57111,6 +57219,9 @@
       <c r="N1156">
         <v>0.39171410000000001</v>
       </c>
+      <c r="O1156">
+        <v>2.3069999999999999</v>
+      </c>
       <c r="T1156" s="1" t="s">
         <v>221</v>
       </c>
@@ -57161,6 +57272,9 @@
       <c r="N1157">
         <v>0.1244712</v>
       </c>
+      <c r="O1157">
+        <v>5.0039999999999996</v>
+      </c>
       <c r="T1157" s="1" t="s">
         <v>221</v>
       </c>
@@ -57293,6 +57407,9 @@
       <c r="N1160">
         <v>0.1584024</v>
       </c>
+      <c r="O1160">
+        <v>6.0919999999999996</v>
+      </c>
       <c r="T1160" s="1" t="s">
         <v>221</v>
       </c>
@@ -57343,6 +57460,9 @@
       <c r="N1161">
         <v>0.10583289999999999</v>
       </c>
+      <c r="O1161">
+        <v>8.3059999999999992</v>
+      </c>
       <c r="T1161" s="1" t="s">
         <v>221</v>
       </c>
@@ -57390,6 +57510,9 @@
       <c r="N1162" s="21">
         <v>9.1916349999999994E-2</v>
       </c>
+      <c r="O1162">
+        <v>6.407</v>
+      </c>
       <c r="T1162" s="1" t="s">
         <v>221</v>
       </c>
@@ -57440,6 +57563,9 @@
       <c r="N1163">
         <v>0.65062030000000004</v>
       </c>
+      <c r="O1163">
+        <v>3.2919999999999998</v>
+      </c>
       <c r="T1163" s="1" t="s">
         <v>221</v>
       </c>
@@ -57490,6 +57616,9 @@
       <c r="N1164" s="21">
         <v>9.8182210000000006E-2</v>
       </c>
+      <c r="O1164">
+        <v>4.1429999999999998</v>
+      </c>
       <c r="T1164" s="1" t="s">
         <v>221</v>
       </c>
@@ -57540,6 +57669,9 @@
       <c r="N1165" s="21">
         <v>3.9442310000000001E-2</v>
       </c>
+      <c r="O1165">
+        <v>7.0309999999999997</v>
+      </c>
       <c r="T1165" s="1" t="s">
         <v>221</v>
       </c>
@@ -57587,6 +57719,9 @@
       <c r="N1166">
         <v>0.14469389999999999</v>
       </c>
+      <c r="O1166">
+        <v>8.7889999999999997</v>
+      </c>
       <c r="T1166" s="1" t="s">
         <v>221</v>
       </c>
@@ -57634,6 +57769,9 @@
       <c r="N1167">
         <v>0.1101157</v>
       </c>
+      <c r="O1167">
+        <v>7.0149999999999997</v>
+      </c>
       <c r="T1167" s="1" t="s">
         <v>221</v>
       </c>
@@ -57681,6 +57819,9 @@
       <c r="N1168">
         <v>0.1828079</v>
       </c>
+      <c r="O1168">
+        <v>7.1580000000000004</v>
+      </c>
       <c r="T1168" s="1" t="s">
         <v>221</v>
       </c>
@@ -57731,6 +57872,9 @@
       <c r="N1169">
         <v>0.1490496</v>
       </c>
+      <c r="O1169">
+        <v>8.5190000000000001</v>
+      </c>
       <c r="T1169" s="1" t="s">
         <v>221</v>
       </c>
@@ -57781,6 +57925,9 @@
       <c r="N1170">
         <v>0.5322983</v>
       </c>
+      <c r="O1170">
+        <v>6.7619999999999996</v>
+      </c>
       <c r="T1170" s="1" t="s">
         <v>221</v>
       </c>
@@ -57828,6 +57975,9 @@
       <c r="N1171">
         <v>0.1216599</v>
       </c>
+      <c r="O1171">
+        <v>10.576000000000001</v>
+      </c>
       <c r="T1171" s="1" t="s">
         <v>221</v>
       </c>
@@ -57875,6 +58025,9 @@
       <c r="N1172">
         <v>0.18624540000000001</v>
       </c>
+      <c r="O1172">
+        <v>9.1560000000000006</v>
+      </c>
       <c r="T1172" s="1" t="s">
         <v>221</v>
       </c>
@@ -57925,6 +58078,9 @@
       <c r="N1173">
         <v>0.19425400000000001</v>
       </c>
+      <c r="O1173">
+        <v>9.31</v>
+      </c>
       <c r="T1173" s="1" t="s">
         <v>221</v>
       </c>
@@ -57975,6 +58131,9 @@
       <c r="N1174">
         <v>0.1177052</v>
       </c>
+      <c r="O1174">
+        <v>6.6219999999999999</v>
+      </c>
       <c r="T1174" s="1" t="s">
         <v>221</v>
       </c>
@@ -58025,6 +58184,9 @@
       <c r="N1175">
         <v>0.12382840000000001</v>
       </c>
+      <c r="O1175">
+        <v>8.5129999999999999</v>
+      </c>
       <c r="T1175" s="1" t="s">
         <v>221</v>
       </c>
@@ -58072,6 +58234,9 @@
       <c r="N1176">
         <v>7.0182300000000003E-2</v>
       </c>
+      <c r="O1176">
+        <v>8.5150000000000006</v>
+      </c>
       <c r="T1176" s="1" t="s">
         <v>221</v>
       </c>
@@ -58119,6 +58284,9 @@
       <c r="N1177">
         <v>0.12599350000000001</v>
       </c>
+      <c r="O1177">
+        <v>4.6950000000000003</v>
+      </c>
       <c r="T1177" s="1" t="s">
         <v>221</v>
       </c>
@@ -58166,6 +58334,9 @@
       <c r="N1178">
         <v>0.74829590000000001</v>
       </c>
+      <c r="O1178">
+        <v>4.7610000000000001</v>
+      </c>
       <c r="T1178" s="1" t="s">
         <v>221</v>
       </c>
@@ -58216,6 +58387,9 @@
       <c r="N1179" s="21">
         <v>9.212236E-2</v>
       </c>
+      <c r="O1179">
+        <v>7.3890000000000002</v>
+      </c>
       <c r="T1179" s="1" t="s">
         <v>221</v>
       </c>
@@ -58266,6 +58440,9 @@
       <c r="N1180">
         <v>0.92521350000000002</v>
       </c>
+      <c r="O1180">
+        <v>5.734</v>
+      </c>
       <c r="T1180" s="1" t="s">
         <v>221</v>
       </c>
@@ -58316,6 +58493,9 @@
       <c r="N1181" s="21">
         <v>2.3666880000000001E-2</v>
       </c>
+      <c r="O1181">
+        <v>2.38</v>
+      </c>
       <c r="T1181" s="1" t="s">
         <v>221</v>
       </c>
@@ -58366,6 +58546,9 @@
       <c r="N1182">
         <v>0.1208277</v>
       </c>
+      <c r="O1182">
+        <v>5.593</v>
+      </c>
       <c r="T1182" s="1" t="s">
         <v>221</v>
       </c>
@@ -58416,6 +58599,9 @@
       <c r="N1183">
         <v>0.13241720000000001</v>
       </c>
+      <c r="O1183">
+        <v>6.86</v>
+      </c>
       <c r="T1183" s="1" t="s">
         <v>221</v>
       </c>
@@ -58463,6 +58649,9 @@
       <c r="N1184" s="21">
         <v>8.1108730000000004E-2</v>
       </c>
+      <c r="O1184">
+        <v>4.9829999999999997</v>
+      </c>
       <c r="T1184" s="1" t="s">
         <v>221</v>
       </c>
@@ -58513,6 +58702,9 @@
       <c r="N1185">
         <v>0.15521650000000001</v>
       </c>
+      <c r="O1185">
+        <v>3.86</v>
+      </c>
       <c r="T1185" s="1" t="s">
         <v>221</v>
       </c>
@@ -58563,6 +58755,9 @@
       <c r="N1186">
         <v>0.1090928</v>
       </c>
+      <c r="O1186">
+        <v>7.343</v>
+      </c>
       <c r="T1186" s="1" t="s">
         <v>221</v>
       </c>
@@ -58613,6 +58808,9 @@
       <c r="N1187">
         <v>0.1519279</v>
       </c>
+      <c r="O1187">
+        <v>7.07</v>
+      </c>
       <c r="T1187" s="1" t="s">
         <v>221</v>
       </c>
@@ -58663,6 +58861,9 @@
       <c r="N1188">
         <v>0.12259109999999999</v>
       </c>
+      <c r="O1188">
+        <v>7.4320000000000004</v>
+      </c>
       <c r="T1188" s="1" t="s">
         <v>221</v>
       </c>
@@ -58710,6 +58911,9 @@
       <c r="N1189" s="21">
         <v>7.0612430000000004E-2</v>
       </c>
+      <c r="O1189">
+        <v>6.4189999999999996</v>
+      </c>
       <c r="T1189" s="1" t="s">
         <v>221</v>
       </c>
@@ -58760,6 +58964,9 @@
       <c r="N1190">
         <v>0.8125405</v>
       </c>
+      <c r="O1190">
+        <v>6.8949999999999996</v>
+      </c>
       <c r="T1190" s="1" t="s">
         <v>221</v>
       </c>
@@ -58807,6 +59014,9 @@
       <c r="N1191" s="21">
         <v>9.3835879999999997E-2</v>
       </c>
+      <c r="O1191">
+        <v>6.8449999999999998</v>
+      </c>
       <c r="T1191" s="1" t="s">
         <v>221</v>
       </c>
@@ -58854,6 +59064,9 @@
       <c r="N1192">
         <v>0.16304379999999999</v>
       </c>
+      <c r="O1192">
+        <v>6.7919999999999998</v>
+      </c>
       <c r="T1192" s="1" t="s">
         <v>221</v>
       </c>
@@ -58904,6 +59117,9 @@
       <c r="N1193">
         <v>0.1101207</v>
       </c>
+      <c r="O1193">
+        <v>4.625</v>
+      </c>
       <c r="T1193" s="1" t="s">
         <v>221</v>
       </c>
@@ -58954,6 +59170,9 @@
       <c r="N1194" s="21">
         <v>7.7204179999999997E-2</v>
       </c>
+      <c r="O1194">
+        <v>5.7240000000000002</v>
+      </c>
       <c r="T1194" s="1" t="s">
         <v>221</v>
       </c>
@@ -59001,6 +59220,9 @@
       <c r="N1195">
         <v>0.21170269999999999</v>
       </c>
+      <c r="O1195">
+        <v>6.2489999999999997</v>
+      </c>
       <c r="T1195" s="1" t="s">
         <v>221</v>
       </c>
@@ -59051,6 +59273,9 @@
       <c r="N1196">
         <v>1.3052060000000001</v>
       </c>
+      <c r="O1196">
+        <v>1.3979999999999999</v>
+      </c>
       <c r="T1196" s="1" t="s">
         <v>221</v>
       </c>
@@ -59098,6 +59323,9 @@
       <c r="N1197" s="21">
         <v>9.2051980000000005E-2</v>
       </c>
+      <c r="O1197">
+        <v>8.6809999999999992</v>
+      </c>
       <c r="T1197" s="1" t="s">
         <v>221</v>
       </c>
@@ -59145,6 +59373,9 @@
       <c r="N1198">
         <v>0.13875270000000001</v>
       </c>
+      <c r="O1198">
+        <v>8.0120000000000005</v>
+      </c>
       <c r="T1198" s="1" t="s">
         <v>221</v>
       </c>
@@ -59192,6 +59423,9 @@
       <c r="N1199">
         <v>0.1227541</v>
       </c>
+      <c r="O1199">
+        <v>6.5369999999999999</v>
+      </c>
       <c r="T1199" s="1" t="s">
         <v>221</v>
       </c>
@@ -59242,6 +59476,9 @@
       <c r="N1200">
         <v>0.1256034</v>
       </c>
+      <c r="O1200">
+        <v>6.6769999999999996</v>
+      </c>
       <c r="T1200" s="1" t="s">
         <v>221</v>
       </c>
@@ -59292,6 +59529,9 @@
       <c r="N1201" s="21">
         <v>9.649373E-2</v>
       </c>
+      <c r="O1201">
+        <v>4.2430000000000003</v>
+      </c>
       <c r="T1201" s="1" t="s">
         <v>221</v>
       </c>
@@ -59342,6 +59582,9 @@
       <c r="N1202">
         <v>0.57073850000000004</v>
       </c>
+      <c r="O1202">
+        <v>3.5390000000000001</v>
+      </c>
       <c r="T1202" s="1" t="s">
         <v>221</v>
       </c>
@@ -59389,6 +59632,9 @@
       <c r="N1203">
         <v>8.7844199999999997E-2</v>
       </c>
+      <c r="O1203">
+        <v>6.6210000000000004</v>
+      </c>
       <c r="T1203" s="1" t="s">
         <v>221</v>
       </c>
@@ -59438,6 +59684,9 @@
       </c>
       <c r="N1204">
         <v>0.14297399999999999</v>
+      </c>
+      <c r="O1204">
+        <v>7.12</v>
       </c>
       <c r="T1204" s="1" t="s">
         <v>221</v>

</xml_diff>

<commit_message>
entering purge times for 2018-09-11 cohort day 12 + 27
</commit_message>
<xml_diff>
--- a/Data/2018-08-14_master_datac_2018_collection_year.xlsx
+++ b/Data/2018-08-14_master_datac_2018_collection_year.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andrew.nguyen\Desktop\Circadian_rhythm_runs_seasonal_timing\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C188D006-F1E9-4A55-A522-4088B5BD3D07}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ABE3223-7CFB-455A-BBA5-F6371FEAA32A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3345" yWindow="465" windowWidth="47520" windowHeight="26880" activeTab="1" xr2:uid="{C7477166-8A7C-B04A-9643-C277FEDCDAAB}"/>
   </bookViews>
@@ -15217,8 +15217,8 @@
   <dimension ref="A1:AV1806"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1465" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O1472" sqref="O1472"/>
+      <pane ySplit="1" topLeftCell="A1444" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P1450" sqref="P1450"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -72326,6 +72326,9 @@
       <c r="O1449">
         <v>9.2520000000000007</v>
       </c>
+      <c r="P1449" s="63">
+        <v>0.60347222222222219</v>
+      </c>
       <c r="W1449" s="1" t="s">
         <v>540</v>
       </c>
@@ -74297,6 +74300,9 @@
       <c r="N1494" s="20">
         <v>6.7642880000000002E-3</v>
       </c>
+      <c r="P1494" s="63">
+        <v>0.60972222222222217</v>
+      </c>
       <c r="W1494" s="1" t="s">
         <v>540</v>
       </c>
@@ -74344,6 +74350,9 @@
       <c r="O1495">
         <v>8.5239999999999991</v>
       </c>
+      <c r="P1495" s="63">
+        <v>0.61041666666666672</v>
+      </c>
       <c r="W1495" s="1" t="s">
         <v>540</v>
       </c>
@@ -76305,6 +76314,9 @@
       </c>
       <c r="L1540">
         <v>6262</v>
+      </c>
+      <c r="P1540" s="63">
+        <v>0.61597222222222225</v>
       </c>
       <c r="W1540" s="1" t="s">
         <v>540</v>

</xml_diff>

<commit_message>
adding day 20 pupal weights
</commit_message>
<xml_diff>
--- a/Data/2018-08-14_master_datac_2018_collection_year.xlsx
+++ b/Data/2018-08-14_master_datac_2018_collection_year.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hinalkharva\Desktop\Circadian_rhythm_runs_seasonal_timing\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andrew.nguyen\Desktop\Circadian_rhythm_runs_seasonal_timing\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4195ACDD-80E1-4728-9AD4-CA3C6FDEB3E4}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFA3577B-4618-4A2D-B596-596316DE6955}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3345" yWindow="465" windowWidth="47520" windowHeight="26880" activeTab="2" xr2:uid="{C7477166-8A7C-B04A-9643-C277FEDCDAAB}"/>
+    <workbookView xWindow="3345" yWindow="465" windowWidth="47520" windowHeight="26880" activeTab="1" xr2:uid="{C7477166-8A7C-B04A-9643-C277FEDCDAAB}"/>
   </bookViews>
   <sheets>
     <sheet name="Maggot_Collections" sheetId="2" r:id="rId1"/>
@@ -22,12 +22,17 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16818" uniqueCount="1067">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16877" uniqueCount="1067">
   <si>
     <t>Ind_ID</t>
   </si>
@@ -3234,9 +3239,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="166" formatCode="0.000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -3428,7 +3434,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -3534,6 +3540,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3852,7 +3860,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A121" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K135" sqref="K135"/>
+      <selection pane="bottomLeft" activeCell="A125" sqref="A125:XFD128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -16190,11 +16198,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92725FB9-1A17-2546-9DFA-6C0D39437891}">
-  <dimension ref="A1:AV1813"/>
+  <dimension ref="A1:AV1815"/>
   <sheetViews>
-    <sheetView topLeftCell="X1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A473" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AK489" sqref="AK489"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A1610" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L1663" sqref="L1663"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -16202,6 +16210,7 @@
     <col min="5" max="5" width="11" style="1"/>
     <col min="7" max="7" width="13.625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="11" style="1"/>
+    <col min="19" max="19" width="11" style="87"/>
     <col min="23" max="23" width="15.375" style="1" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="11" style="9"/>
     <col min="34" max="34" width="16.875" bestFit="1" customWidth="1"/>
@@ -16265,7 +16274,7 @@
       <c r="R1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="S1" s="87" t="s">
         <v>1049</v>
       </c>
       <c r="T1" s="1" t="s">
@@ -19632,7 +19641,6 @@
       <c r="R93" s="20">
         <v>9.3841980000000005E-2</v>
       </c>
-      <c r="S93" s="20"/>
       <c r="T93" s="20"/>
       <c r="U93" s="20"/>
       <c r="W93" s="1" t="s">
@@ -19797,7 +19805,6 @@
       <c r="R96" s="20">
         <v>6.7306560000000001E-2</v>
       </c>
-      <c r="S96" s="20"/>
       <c r="T96" s="20"/>
       <c r="U96" s="20"/>
       <c r="W96" s="1" t="s">
@@ -20021,7 +20028,6 @@
       <c r="R100" s="20">
         <v>9.2095869999999996E-2</v>
       </c>
-      <c r="S100" s="20"/>
       <c r="T100" s="20"/>
       <c r="U100" s="20"/>
       <c r="W100" s="1" t="s">
@@ -20080,7 +20086,6 @@
       <c r="R101" s="20">
         <v>1.8792840000000002E-2</v>
       </c>
-      <c r="S101" s="20"/>
       <c r="T101" s="20"/>
       <c r="U101" s="20"/>
       <c r="W101" s="1" t="s">
@@ -20304,7 +20309,6 @@
       <c r="R105" s="20">
         <v>5.4811239999999997E-2</v>
       </c>
-      <c r="S105" s="20"/>
       <c r="T105" s="20"/>
       <c r="U105" s="20"/>
       <c r="W105" s="1" t="s">
@@ -20528,7 +20532,6 @@
       <c r="R109" s="20">
         <v>6.8877270000000004E-2</v>
       </c>
-      <c r="S109" s="20"/>
       <c r="T109" s="20"/>
       <c r="U109" s="20"/>
       <c r="W109" s="1" t="s">
@@ -20696,7 +20699,6 @@
       <c r="R112" s="20">
         <v>7.8091389999999997E-2</v>
       </c>
-      <c r="S112" s="20"/>
       <c r="T112" s="20"/>
       <c r="U112" s="20"/>
       <c r="W112" s="1" t="s">
@@ -20808,7 +20810,6 @@
       <c r="R114" s="20">
         <v>5.8797219999999997E-2</v>
       </c>
-      <c r="S114" s="20"/>
       <c r="T114" s="20"/>
       <c r="U114" s="20"/>
       <c r="W114" s="1" t="s">
@@ -20867,7 +20868,6 @@
       <c r="R115" s="20">
         <v>5.6046890000000002E-2</v>
       </c>
-      <c r="S115" s="20"/>
       <c r="T115" s="20"/>
       <c r="U115" s="20"/>
       <c r="W115" s="1" t="s">
@@ -21159,7 +21159,6 @@
       <c r="R120" s="20">
         <v>6.6891190000000003E-2</v>
       </c>
-      <c r="S120" s="20"/>
       <c r="T120" s="20"/>
       <c r="U120" s="20"/>
       <c r="W120" s="1" t="s">
@@ -21380,7 +21379,6 @@
       <c r="R124" s="20">
         <v>5.8403950000000003E-2</v>
       </c>
-      <c r="S124" s="20"/>
       <c r="T124" s="20"/>
       <c r="U124" s="20"/>
       <c r="W124" s="1" t="s">
@@ -21713,7 +21711,6 @@
       <c r="R130" s="20">
         <v>3.2818470000000002E-2</v>
       </c>
-      <c r="S130" s="20"/>
       <c r="T130" s="20"/>
       <c r="U130" s="20"/>
       <c r="W130" s="1" t="s">
@@ -21825,7 +21822,6 @@
       <c r="R132" s="20">
         <v>7.4718629999999994E-2</v>
       </c>
-      <c r="S132" s="20"/>
       <c r="T132" s="20"/>
       <c r="U132" s="20"/>
       <c r="W132" s="1" t="s">
@@ -21940,7 +21936,6 @@
       <c r="R134" s="20">
         <v>7.1035319999999999E-2</v>
       </c>
-      <c r="S134" s="20"/>
       <c r="T134" s="20"/>
       <c r="U134" s="20"/>
       <c r="W134" s="1" t="s">
@@ -22052,7 +22047,6 @@
       <c r="R136" s="20">
         <v>6.2879640000000001E-2</v>
       </c>
-      <c r="S136" s="20"/>
       <c r="T136" s="20"/>
       <c r="U136" s="20"/>
       <c r="W136" s="1" t="s">
@@ -22105,7 +22099,6 @@
       <c r="R137" s="20">
         <v>1.6587950000000001E-2</v>
       </c>
-      <c r="S137" s="20"/>
       <c r="T137" s="20"/>
       <c r="U137" s="20"/>
       <c r="W137" s="1" t="s">
@@ -22155,7 +22148,6 @@
       <c r="R138" s="20">
         <v>1.581923E-2</v>
       </c>
-      <c r="S138" s="20"/>
       <c r="T138" s="20"/>
       <c r="U138" s="20"/>
       <c r="W138" s="1" t="s">
@@ -22208,7 +22200,6 @@
       <c r="R139" s="20">
         <v>3.7967649999999999E-2</v>
       </c>
-      <c r="S139" s="20"/>
       <c r="T139" s="20"/>
       <c r="U139" s="20"/>
       <c r="W139" s="1" t="s">
@@ -22338,7 +22329,6 @@
       <c r="R141" s="20">
         <v>7.6291429999999993E-2</v>
       </c>
-      <c r="S141" s="20"/>
       <c r="T141" s="20"/>
       <c r="U141" s="20"/>
       <c r="W141" s="1" t="s">
@@ -22453,7 +22443,6 @@
       <c r="R143" s="20">
         <v>1.5805650000000001E-2</v>
       </c>
-      <c r="S143" s="20"/>
       <c r="T143" s="20"/>
       <c r="U143" s="20"/>
       <c r="W143" s="1" t="s">
@@ -22512,7 +22501,6 @@
       <c r="R144" s="20">
         <v>6.9724019999999998E-2</v>
       </c>
-      <c r="S144" s="20"/>
       <c r="T144" s="20"/>
       <c r="U144" s="20"/>
       <c r="W144" s="1" t="s">
@@ -22571,7 +22559,6 @@
       <c r="R145" s="20">
         <v>9.1359460000000003E-2</v>
       </c>
-      <c r="S145" s="20"/>
       <c r="T145" s="20"/>
       <c r="U145" s="20"/>
       <c r="W145" s="1" t="s">
@@ -22686,7 +22673,6 @@
       <c r="R147" s="20">
         <v>6.5931310000000007E-2</v>
       </c>
-      <c r="S147" s="20"/>
       <c r="T147" s="20"/>
       <c r="U147" s="20"/>
       <c r="W147" s="1" t="s">
@@ -22904,7 +22890,6 @@
       <c r="R151" s="20">
         <v>9.3718270000000006E-2</v>
       </c>
-      <c r="S151" s="20"/>
       <c r="T151" s="20"/>
       <c r="U151" s="20"/>
       <c r="W151" s="1" t="s">
@@ -23075,7 +23060,6 @@
       <c r="R154" s="20">
         <v>8.5026729999999995E-2</v>
       </c>
-      <c r="S154" s="20"/>
       <c r="T154" s="20"/>
       <c r="U154" s="20"/>
       <c r="W154" s="1" t="s">
@@ -23131,7 +23115,6 @@
       <c r="R155" s="20">
         <v>6.3941949999999997E-2</v>
       </c>
-      <c r="S155" s="20"/>
       <c r="T155" s="20"/>
       <c r="U155" s="20"/>
       <c r="W155" s="1" t="s">
@@ -23190,7 +23173,6 @@
       <c r="R156" s="20">
         <v>7.269246E-2</v>
       </c>
-      <c r="S156" s="20"/>
       <c r="T156" s="20"/>
       <c r="U156" s="20"/>
       <c r="W156" s="1" t="s">
@@ -23414,7 +23396,6 @@
       <c r="R160" s="20">
         <v>9.3654630000000003E-2</v>
       </c>
-      <c r="S160" s="20"/>
       <c r="T160" s="20"/>
       <c r="U160" s="20"/>
       <c r="W160" s="1" t="s">
@@ -23526,7 +23507,6 @@
       <c r="R162" s="20">
         <v>8.2966780000000004E-2</v>
       </c>
-      <c r="S162" s="20"/>
       <c r="T162" s="20"/>
       <c r="U162" s="20"/>
       <c r="W162" s="1" t="s">
@@ -23582,7 +23562,6 @@
       <c r="R163" s="20">
         <v>7.9145419999999994E-2</v>
       </c>
-      <c r="S163" s="20"/>
       <c r="T163" s="20"/>
       <c r="U163" s="20"/>
       <c r="W163" s="1" t="s">
@@ -23638,7 +23617,6 @@
       <c r="R164" s="20">
         <v>5.0435460000000001E-2</v>
       </c>
-      <c r="S164" s="20"/>
       <c r="T164" s="20"/>
       <c r="U164" s="20"/>
       <c r="W164" s="1" t="s">
@@ -23803,7 +23781,6 @@
       <c r="R167" s="20">
         <v>5.3724180000000003E-2</v>
       </c>
-      <c r="S167" s="20"/>
       <c r="T167" s="20"/>
       <c r="U167" s="20"/>
       <c r="W167" s="1" t="s">
@@ -23918,7 +23895,6 @@
       <c r="R169" s="20">
         <v>4.5041770000000002E-2</v>
       </c>
-      <c r="S169" s="20"/>
       <c r="T169" s="20"/>
       <c r="U169" s="20"/>
       <c r="W169" s="1" t="s">
@@ -24033,7 +24009,6 @@
       <c r="R171" s="20">
         <v>5.9019240000000001E-2</v>
       </c>
-      <c r="S171" s="20"/>
       <c r="T171" s="20"/>
       <c r="U171" s="20"/>
       <c r="W171" s="1" t="s">
@@ -24148,7 +24123,6 @@
       <c r="R173" s="20">
         <v>7.8043669999999996E-2</v>
       </c>
-      <c r="S173" s="20"/>
       <c r="T173" s="20"/>
       <c r="U173" s="20"/>
       <c r="W173" s="1" t="s">
@@ -24207,7 +24181,6 @@
       <c r="R174" s="20">
         <v>4.7387520000000002E-2</v>
       </c>
-      <c r="S174" s="20"/>
       <c r="T174" s="20"/>
       <c r="U174" s="20"/>
       <c r="W174" s="1" t="s">
@@ -24266,7 +24239,6 @@
       <c r="R175" s="20">
         <v>4.2132469999999998E-2</v>
       </c>
-      <c r="S175" s="20"/>
       <c r="T175" s="20"/>
       <c r="U175" s="20"/>
       <c r="W175" s="1" t="s">
@@ -24378,7 +24350,6 @@
       <c r="R177" s="20">
         <v>6.3697229999999994E-2</v>
       </c>
-      <c r="S177" s="20"/>
       <c r="T177" s="20"/>
       <c r="U177" s="20"/>
       <c r="W177" s="1" t="s">
@@ -24437,7 +24408,6 @@
       <c r="R178" s="20">
         <v>6.2188559999999997E-2</v>
       </c>
-      <c r="S178" s="20"/>
       <c r="T178" s="20"/>
       <c r="U178" s="20"/>
       <c r="W178" s="1" t="s">
@@ -24658,7 +24628,6 @@
       <c r="R182" s="20">
         <v>1.5951770000000001E-2</v>
       </c>
-      <c r="S182" s="20"/>
       <c r="T182" s="20"/>
       <c r="U182" s="20"/>
       <c r="W182" s="1" t="s">
@@ -24717,7 +24686,6 @@
       <c r="R183" s="20">
         <v>4.3760340000000002E-2</v>
       </c>
-      <c r="S183" s="20"/>
       <c r="T183" s="20"/>
       <c r="U183" s="20"/>
       <c r="W183" s="1" t="s">
@@ -24770,7 +24738,6 @@
       <c r="R184" s="20">
         <v>1.043992E-2</v>
       </c>
-      <c r="S184" s="20"/>
       <c r="T184" s="20"/>
       <c r="U184" s="20"/>
       <c r="W184" s="1" t="s">
@@ -24820,7 +24787,6 @@
       <c r="R185" s="20">
         <v>1.086523E-2</v>
       </c>
-      <c r="S185" s="20"/>
       <c r="T185" s="20"/>
       <c r="U185" s="20"/>
       <c r="W185" s="1" t="s">
@@ -28025,7 +27991,6 @@
       </c>
       <c r="Q276" s="19"/>
       <c r="R276" s="20"/>
-      <c r="S276" s="20"/>
       <c r="T276" s="20"/>
       <c r="U276" s="20"/>
       <c r="W276" s="1" t="s">
@@ -28140,7 +28105,6 @@
       <c r="R278" s="20">
         <v>6.3613429999999999E-2</v>
       </c>
-      <c r="S278" s="20"/>
       <c r="T278" s="20"/>
       <c r="U278" s="20"/>
       <c r="W278" s="1" t="s">
@@ -28361,7 +28325,6 @@
       <c r="R282" s="20">
         <v>5.0382509999999998E-2</v>
       </c>
-      <c r="S282" s="20"/>
       <c r="T282" s="20"/>
       <c r="U282" s="20"/>
       <c r="W282" s="1" t="s">
@@ -28417,7 +28380,6 @@
       <c r="R283" s="20">
         <v>6.092533E-2</v>
       </c>
-      <c r="S283" s="20"/>
       <c r="T283" s="20"/>
       <c r="U283" s="20"/>
       <c r="W283" s="1" t="s">
@@ -28588,7 +28550,6 @@
       <c r="R286" s="20">
         <v>8.8426560000000001E-2</v>
       </c>
-      <c r="S286" s="20"/>
       <c r="T286" s="20"/>
       <c r="U286" s="20"/>
       <c r="W286" s="1" t="s">
@@ -28865,7 +28826,6 @@
       <c r="R291" s="20">
         <v>1.426873E-2</v>
       </c>
-      <c r="S291" s="20"/>
       <c r="T291" s="20"/>
       <c r="U291" s="20"/>
       <c r="W291" s="1" t="s">
@@ -28977,7 +28937,6 @@
       <c r="R293" s="20">
         <v>3.9550410000000001E-2</v>
       </c>
-      <c r="S293" s="20"/>
       <c r="T293" s="20"/>
       <c r="U293" s="20"/>
       <c r="W293" s="1" t="s">
@@ -29036,7 +28995,6 @@
       <c r="R294" s="20">
         <v>8.7507109999999999E-2</v>
       </c>
-      <c r="S294" s="20"/>
       <c r="T294" s="20"/>
       <c r="U294" s="20"/>
       <c r="W294" s="1" t="s">
@@ -29145,7 +29103,6 @@
       <c r="R296" s="20">
         <v>8.9112589999999995E-3</v>
       </c>
-      <c r="S296" s="20"/>
       <c r="T296" s="20"/>
       <c r="U296" s="20"/>
       <c r="W296" s="1" t="s">
@@ -29198,7 +29155,6 @@
       <c r="R297" s="20">
         <v>7.8984769999999992E-3</v>
       </c>
-      <c r="S297" s="20"/>
       <c r="T297" s="20"/>
       <c r="U297" s="20"/>
       <c r="W297" s="1" t="s">
@@ -49573,6 +49529,7 @@
       <c r="K908" s="56" t="s">
         <v>60</v>
       </c>
+      <c r="S908" s="88"/>
       <c r="W908" s="57" t="s">
         <v>78</v>
       </c>
@@ -52220,6 +52177,9 @@
       <c r="R999">
         <v>0.15616920000000001</v>
       </c>
+      <c r="S999" s="87">
+        <v>3.6840000000000002</v>
+      </c>
       <c r="W999" s="1" t="s">
         <v>212</v>
       </c>
@@ -52279,6 +52239,9 @@
       <c r="R1000">
         <v>0.39721339999999999</v>
       </c>
+      <c r="S1000" s="87">
+        <v>5.6909999999999998</v>
+      </c>
       <c r="W1000" s="1" t="s">
         <v>212</v>
       </c>
@@ -52338,7 +52301,6 @@
       <c r="R1001" s="20">
         <v>2.3583980000000001E-2</v>
       </c>
-      <c r="S1001" s="20"/>
       <c r="T1001" s="20"/>
       <c r="U1001" s="20"/>
       <c r="W1001" s="1" t="s">
@@ -52453,7 +52415,6 @@
       <c r="R1003" s="20">
         <v>6.8221560000000001E-2</v>
       </c>
-      <c r="S1003" s="20"/>
       <c r="T1003" s="20"/>
       <c r="U1003" s="20"/>
       <c r="W1003" s="1" t="s">
@@ -52512,7 +52473,9 @@
       <c r="R1004" s="20">
         <v>3.538898E-2</v>
       </c>
-      <c r="S1004" s="20"/>
+      <c r="S1004" s="87">
+        <v>8.6590000000000007</v>
+      </c>
       <c r="T1004" s="20"/>
       <c r="U1004" s="20"/>
       <c r="W1004" s="1" t="s">
@@ -52574,7 +52537,9 @@
       <c r="R1005" s="20">
         <v>6.7594890000000005E-2</v>
       </c>
-      <c r="S1005" s="20"/>
+      <c r="S1005" s="87">
+        <v>10.084</v>
+      </c>
       <c r="T1005" s="20"/>
       <c r="U1005" s="20"/>
       <c r="W1005" s="1" t="s">
@@ -52636,7 +52601,6 @@
       <c r="R1006" s="20">
         <v>4.5329040000000001E-2</v>
       </c>
-      <c r="S1006" s="20"/>
       <c r="T1006" s="20"/>
       <c r="U1006" s="20"/>
       <c r="W1006" s="1" t="s">
@@ -52757,6 +52721,9 @@
       <c r="R1008">
         <v>0.34544859999999999</v>
       </c>
+      <c r="S1008" s="87">
+        <v>2.9660000000000002</v>
+      </c>
       <c r="W1008" s="1" t="s">
         <v>212</v>
       </c>
@@ -52816,6 +52783,9 @@
       <c r="R1009">
         <v>0.49454769999999998</v>
       </c>
+      <c r="S1009" s="87">
+        <v>3.2120000000000002</v>
+      </c>
       <c r="W1009" s="1" t="s">
         <v>212</v>
       </c>
@@ -52875,7 +52845,6 @@
       <c r="R1010" s="20">
         <v>1.9581439999999999E-2</v>
       </c>
-      <c r="S1010" s="20"/>
       <c r="T1010" s="20"/>
       <c r="U1010" s="20"/>
       <c r="W1010" s="1" t="s">
@@ -52934,7 +52903,6 @@
       <c r="R1011" s="20">
         <v>3.0850539999999999E-2</v>
       </c>
-      <c r="S1011" s="20"/>
       <c r="T1011" s="20"/>
       <c r="U1011" s="20"/>
       <c r="W1011" s="1" t="s">
@@ -52993,7 +52961,6 @@
       <c r="R1012" s="20">
         <v>4.2812969999999999E-2</v>
       </c>
-      <c r="S1012" s="20"/>
       <c r="T1012" s="20"/>
       <c r="U1012" s="20"/>
       <c r="W1012" s="1" t="s">
@@ -53055,7 +53022,6 @@
       <c r="R1013" s="20">
         <v>5.1153049999999999E-2</v>
       </c>
-      <c r="S1013" s="20"/>
       <c r="T1013" s="20"/>
       <c r="U1013" s="20"/>
       <c r="W1013" s="1" t="s">
@@ -53114,7 +53080,6 @@
       <c r="R1014" s="20">
         <v>2.286345E-2</v>
       </c>
-      <c r="S1014" s="20"/>
       <c r="T1014" s="20"/>
       <c r="U1014" s="20"/>
       <c r="W1014" s="1" t="s">
@@ -53176,7 +53141,9 @@
       <c r="R1015" s="20">
         <v>3.7739549999999997E-2</v>
       </c>
-      <c r="S1015" s="20"/>
+      <c r="S1015" s="87">
+        <v>6.9320000000000004</v>
+      </c>
       <c r="T1015" s="20"/>
       <c r="U1015" s="20"/>
       <c r="W1015" s="1" t="s">
@@ -53235,7 +53202,6 @@
       <c r="R1016" s="20">
         <v>4.1007309999999998E-2</v>
       </c>
-      <c r="S1016" s="20"/>
       <c r="T1016" s="20"/>
       <c r="U1016" s="20"/>
       <c r="W1016" s="1" t="s">
@@ -53297,7 +53263,6 @@
       <c r="R1017" s="20">
         <v>6.8838070000000001E-2</v>
       </c>
-      <c r="S1017" s="20"/>
       <c r="T1017" s="20"/>
       <c r="U1017" s="20"/>
       <c r="W1017" s="1" t="s">
@@ -53418,7 +53383,6 @@
       <c r="R1019" s="20">
         <v>3.8323740000000002E-2</v>
       </c>
-      <c r="S1019" s="20"/>
       <c r="T1019" s="20"/>
       <c r="U1019" s="20"/>
       <c r="W1019" s="1" t="s">
@@ -53480,7 +53444,6 @@
       <c r="R1020" s="20">
         <v>6.0473840000000001E-2</v>
       </c>
-      <c r="S1020" s="20"/>
       <c r="T1020" s="20"/>
       <c r="U1020" s="20"/>
       <c r="W1020" s="1" t="s">
@@ -53542,7 +53505,6 @@
       <c r="R1021" s="20">
         <v>3.7063169999999999E-2</v>
       </c>
-      <c r="S1021" s="20"/>
       <c r="T1021" s="20"/>
       <c r="U1021" s="20"/>
       <c r="W1021" s="1" t="s">
@@ -53601,7 +53563,6 @@
       <c r="R1022" s="20">
         <v>6.3298969999999996E-2</v>
       </c>
-      <c r="S1022" s="20"/>
       <c r="T1022" s="20"/>
       <c r="U1022" s="20"/>
       <c r="W1022" s="1" t="s">
@@ -53660,7 +53621,6 @@
       <c r="R1023" s="20">
         <v>3.2576130000000002E-2</v>
       </c>
-      <c r="S1023" s="20"/>
       <c r="T1023" s="20"/>
       <c r="U1023" s="20"/>
       <c r="W1023" s="1" t="s">
@@ -53719,7 +53679,9 @@
       <c r="R1024" s="20">
         <v>6.7977120000000002E-2</v>
       </c>
-      <c r="S1024" s="20"/>
+      <c r="S1024" s="87">
+        <v>6.7750000000000004</v>
+      </c>
       <c r="T1024" s="20"/>
       <c r="U1024" s="20"/>
       <c r="W1024" s="1" t="s">
@@ -53781,7 +53743,6 @@
       <c r="R1025" s="20">
         <v>3.7571889999999997E-2</v>
       </c>
-      <c r="S1025" s="20"/>
       <c r="T1025" s="20"/>
       <c r="U1025" s="20"/>
       <c r="W1025" s="1" t="s">
@@ -53843,6 +53804,9 @@
       <c r="R1026">
         <v>0.2293914</v>
       </c>
+      <c r="S1026" s="87">
+        <v>2.6760000000000002</v>
+      </c>
       <c r="W1026" s="1" t="s">
         <v>212</v>
       </c>
@@ -53961,7 +53925,9 @@
       <c r="R1028" s="20">
         <v>6.2800030000000007E-2</v>
       </c>
-      <c r="S1028" s="20"/>
+      <c r="S1028" s="87">
+        <v>7.2329999999999997</v>
+      </c>
       <c r="T1028" s="20"/>
       <c r="U1028" s="20"/>
       <c r="W1028" s="1" t="s">
@@ -54023,7 +53989,6 @@
       <c r="R1029" s="20">
         <v>3.5981880000000001E-2</v>
       </c>
-      <c r="S1029" s="20"/>
       <c r="T1029" s="20"/>
       <c r="U1029" s="20"/>
       <c r="W1029" s="1" t="s">
@@ -54085,7 +54050,6 @@
       <c r="R1030" s="20">
         <v>7.8652479999999997E-2</v>
       </c>
-      <c r="S1030" s="20"/>
       <c r="T1030" s="20"/>
       <c r="U1030" s="20"/>
       <c r="W1030" s="1" t="s">
@@ -54144,6 +54108,9 @@
       <c r="R1031">
         <v>2.6046099999999999E-2</v>
       </c>
+      <c r="S1031" s="87">
+        <v>7.0069999999999997</v>
+      </c>
       <c r="W1031" s="1" t="s">
         <v>212</v>
       </c>
@@ -54203,7 +54170,6 @@
       <c r="R1032" s="20">
         <v>3.8316059999999999E-2</v>
       </c>
-      <c r="S1032" s="20"/>
       <c r="T1032" s="20"/>
       <c r="U1032" s="20"/>
       <c r="W1032" s="1" t="s">
@@ -54318,7 +54284,6 @@
       <c r="R1034" s="20">
         <v>3.2625309999999998E-2</v>
       </c>
-      <c r="S1034" s="20"/>
       <c r="T1034" s="20"/>
       <c r="U1034" s="20"/>
       <c r="W1034" s="1" t="s">
@@ -54380,7 +54345,6 @@
       <c r="R1035" s="20">
         <v>5.0918829999999998E-2</v>
       </c>
-      <c r="S1035" s="20"/>
       <c r="T1035" s="20"/>
       <c r="U1035" s="20"/>
       <c r="W1035" s="1" t="s">
@@ -54498,7 +54462,6 @@
       <c r="R1037" s="20">
         <v>5.2390630000000001E-2</v>
       </c>
-      <c r="S1037" s="20"/>
       <c r="T1037" s="20"/>
       <c r="U1037" s="20"/>
       <c r="W1037" s="1" t="s">
@@ -54675,7 +54638,9 @@
       <c r="R1040" s="20">
         <v>5.6775119999999998E-2</v>
       </c>
-      <c r="S1040" s="20"/>
+      <c r="S1040" s="87">
+        <v>4.681</v>
+      </c>
       <c r="T1040" s="20"/>
       <c r="U1040" s="20"/>
       <c r="W1040" s="1" t="s">
@@ -54737,7 +54702,6 @@
       <c r="R1041" s="20">
         <v>3.3313009999999997E-2</v>
       </c>
-      <c r="S1041" s="20"/>
       <c r="T1041" s="20"/>
       <c r="U1041" s="20"/>
       <c r="W1041" s="1" t="s">
@@ -54796,7 +54760,6 @@
       <c r="R1042" s="20">
         <v>5.6059730000000002E-2</v>
       </c>
-      <c r="S1042" s="20"/>
       <c r="T1042" s="20"/>
       <c r="U1042" s="20"/>
       <c r="W1042" s="1" t="s">
@@ -54858,7 +54821,9 @@
       <c r="R1043" s="20">
         <v>4.9339939999999999E-2</v>
       </c>
-      <c r="S1043" s="20"/>
+      <c r="S1043" s="87">
+        <v>4.5060000000000002</v>
+      </c>
       <c r="T1043" s="20"/>
       <c r="U1043" s="20"/>
       <c r="W1043" s="1" t="s">
@@ -54914,7 +54879,6 @@
       <c r="R1044" s="20">
         <v>3.5161099999999998E-3</v>
       </c>
-      <c r="S1044" s="20"/>
       <c r="T1044" s="20"/>
       <c r="U1044" s="20"/>
       <c r="W1044" s="1" t="s">
@@ -54963,7 +54927,6 @@
       </c>
       <c r="Q1045" s="19"/>
       <c r="R1045" s="20"/>
-      <c r="S1045" s="20"/>
       <c r="T1045" s="20"/>
       <c r="U1045" s="20"/>
       <c r="W1045" s="1" t="s">
@@ -55016,7 +54979,15 @@
       <c r="P1046" s="63">
         <v>0.51250000000000007</v>
       </c>
-      <c r="Q1046" s="19"/>
+      <c r="Q1046" s="19">
+        <v>0.13313657407407406</v>
+      </c>
+      <c r="R1046">
+        <v>0.50553579999999998</v>
+      </c>
+      <c r="S1046" s="87">
+        <v>3.84</v>
+      </c>
       <c r="W1046" s="1" t="s">
         <v>212</v>
       </c>
@@ -55070,7 +55041,12 @@
       <c r="O1047">
         <v>8.9580000000000002</v>
       </c>
-      <c r="Q1047" s="19"/>
+      <c r="Q1047" s="19">
+        <v>0.13425925925925927</v>
+      </c>
+      <c r="R1047" s="20">
+        <v>0.08</v>
+      </c>
       <c r="W1047" s="1" t="s">
         <v>212</v>
       </c>
@@ -55121,7 +55097,15 @@
       <c r="O1048">
         <v>4.6150000000000002</v>
       </c>
-      <c r="Q1048" s="19"/>
+      <c r="Q1048" s="19">
+        <v>0.13548611111111111</v>
+      </c>
+      <c r="R1048">
+        <v>0.1138884</v>
+      </c>
+      <c r="S1048" s="87">
+        <v>4.5090000000000003</v>
+      </c>
       <c r="W1048" s="1" t="s">
         <v>212</v>
       </c>
@@ -55175,7 +55159,12 @@
       <c r="O1049">
         <v>6.6689999999999996</v>
       </c>
-      <c r="Q1049" s="19"/>
+      <c r="Q1049" s="19">
+        <v>0.13733796296296297</v>
+      </c>
+      <c r="R1049">
+        <v>0.10934439999999999</v>
+      </c>
       <c r="W1049" s="1" t="s">
         <v>212</v>
       </c>
@@ -55226,7 +55215,15 @@
       <c r="O1050">
         <v>8.8870000000000005</v>
       </c>
-      <c r="Q1050" s="19"/>
+      <c r="Q1050" s="19">
+        <v>0.13846064814814815</v>
+      </c>
+      <c r="R1050">
+        <v>0.1147683</v>
+      </c>
+      <c r="S1050" s="87">
+        <v>8.8439999999999994</v>
+      </c>
       <c r="W1050" s="1" t="s">
         <v>212</v>
       </c>
@@ -55280,7 +55277,12 @@
       <c r="O1051">
         <v>9.0180000000000007</v>
       </c>
-      <c r="Q1051" s="19"/>
+      <c r="Q1051" s="19">
+        <v>0.1396412037037037</v>
+      </c>
+      <c r="R1051">
+        <v>0.98723830000000001</v>
+      </c>
       <c r="W1051" s="1" t="s">
         <v>212</v>
       </c>
@@ -55331,7 +55333,15 @@
       <c r="O1052">
         <v>8.1590000000000007</v>
       </c>
-      <c r="Q1052" s="19"/>
+      <c r="Q1052" s="19">
+        <v>0.14057870370370371</v>
+      </c>
+      <c r="R1052">
+        <v>0.13742019999999999</v>
+      </c>
+      <c r="S1052" s="87">
+        <v>8.0879999999999992</v>
+      </c>
       <c r="W1052" s="1" t="s">
         <v>212</v>
       </c>
@@ -55385,7 +55395,12 @@
       <c r="O1053">
         <v>4.548</v>
       </c>
-      <c r="Q1053" s="19"/>
+      <c r="Q1053" s="19">
+        <v>0.14156250000000001</v>
+      </c>
+      <c r="R1053" s="20">
+        <v>4.9700000000000001E-2</v>
+      </c>
       <c r="W1053" s="1" t="s">
         <v>212</v>
       </c>
@@ -55439,7 +55454,15 @@
       <c r="O1054">
         <v>8.09</v>
       </c>
-      <c r="Q1054" s="19"/>
+      <c r="Q1054" s="19">
+        <v>0.14239583333333333</v>
+      </c>
+      <c r="R1054" s="20">
+        <v>7.7799999999999994E-2</v>
+      </c>
+      <c r="S1054" s="87">
+        <v>8.0429999999999993</v>
+      </c>
       <c r="W1054" s="1" t="s">
         <v>212</v>
       </c>
@@ -55493,7 +55516,12 @@
       <c r="O1055">
         <v>6.5</v>
       </c>
-      <c r="Q1055" s="19"/>
+      <c r="Q1055" s="19">
+        <v>0.14349537037037038</v>
+      </c>
+      <c r="R1055" s="20">
+        <v>5.6000000000000001E-2</v>
+      </c>
       <c r="W1055" s="1" t="s">
         <v>212</v>
       </c>
@@ -55544,7 +55572,12 @@
       <c r="O1056">
         <v>7.5149999999999997</v>
       </c>
-      <c r="Q1056" s="19"/>
+      <c r="Q1056" s="19">
+        <v>0.14466435185185186</v>
+      </c>
+      <c r="R1056" s="20">
+        <v>6.9500000000000006E-2</v>
+      </c>
       <c r="W1056" s="1" t="s">
         <v>212</v>
       </c>
@@ -55595,7 +55628,15 @@
       <c r="O1057">
         <v>5.8650000000000002</v>
       </c>
-      <c r="Q1057" s="19"/>
+      <c r="Q1057" s="19">
+        <v>0.14563657407407407</v>
+      </c>
+      <c r="R1057">
+        <v>0.66290579999999999</v>
+      </c>
+      <c r="S1057" s="87">
+        <v>5.7190000000000003</v>
+      </c>
       <c r="W1057" s="1" t="s">
         <v>212</v>
       </c>
@@ -55649,7 +55690,12 @@
       <c r="O1058">
         <v>7.5060000000000002</v>
       </c>
-      <c r="Q1058" s="19"/>
+      <c r="Q1058" s="19">
+        <v>0.14648148148148146</v>
+      </c>
+      <c r="R1058" s="20">
+        <v>5.1499999999999997E-2</v>
+      </c>
       <c r="W1058" s="1" t="s">
         <v>212</v>
       </c>
@@ -55700,7 +55746,12 @@
       <c r="O1059">
         <v>3.35</v>
       </c>
-      <c r="Q1059" s="19"/>
+      <c r="Q1059" s="19">
+        <v>0.14712962962962964</v>
+      </c>
+      <c r="R1059">
+        <v>0.58029260000000005</v>
+      </c>
       <c r="W1059" s="1" t="s">
         <v>212</v>
       </c>
@@ -55754,9 +55805,12 @@
       <c r="O1060">
         <v>5.3849999999999998</v>
       </c>
-      <c r="Q1060" s="19"/>
-      <c r="R1060" s="20"/>
-      <c r="S1060" s="20"/>
+      <c r="Q1060" s="19">
+        <v>0.14789351851851854</v>
+      </c>
+      <c r="R1060" s="20">
+        <v>4.36E-2</v>
+      </c>
       <c r="T1060" s="20"/>
       <c r="U1060" s="20"/>
       <c r="W1060" s="1" t="s">
@@ -55809,9 +55863,12 @@
       <c r="O1061">
         <v>7.492</v>
       </c>
-      <c r="Q1061" s="19"/>
-      <c r="R1061" s="20"/>
-      <c r="S1061" s="20"/>
+      <c r="Q1061" s="19">
+        <v>0.14850694444444446</v>
+      </c>
+      <c r="R1061" s="20">
+        <v>6.0299999999999999E-2</v>
+      </c>
       <c r="T1061" s="20"/>
       <c r="U1061" s="20"/>
       <c r="W1061" s="1" t="s">
@@ -55867,9 +55924,12 @@
       <c r="O1062">
         <v>8.532</v>
       </c>
-      <c r="Q1062" s="19"/>
-      <c r="R1062" s="20"/>
-      <c r="S1062" s="20"/>
+      <c r="Q1062" s="19">
+        <v>0.1492361111111111</v>
+      </c>
+      <c r="R1062" s="20">
+        <v>6.0299999999999999E-2</v>
+      </c>
       <c r="T1062" s="20"/>
       <c r="U1062" s="20"/>
       <c r="W1062" s="1" t="s">
@@ -55925,7 +55985,15 @@
       <c r="O1063">
         <v>4.6520000000000001</v>
       </c>
-      <c r="Q1063" s="19"/>
+      <c r="Q1063" s="19">
+        <v>0.15042824074074074</v>
+      </c>
+      <c r="R1063">
+        <v>4.8223700000000001E-2</v>
+      </c>
+      <c r="S1063" s="87">
+        <v>4.6150000000000002</v>
+      </c>
       <c r="W1063" s="1" t="s">
         <v>212</v>
       </c>
@@ -55979,7 +56047,15 @@
       <c r="O1064">
         <v>6.2969999999999997</v>
       </c>
-      <c r="Q1064" s="19"/>
+      <c r="Q1064" s="19">
+        <v>0.15119212962962963</v>
+      </c>
+      <c r="R1064" s="20">
+        <v>4.6199999999999998E-2</v>
+      </c>
+      <c r="S1064" s="87">
+        <v>6.2309999999999999</v>
+      </c>
       <c r="W1064" s="1" t="s">
         <v>212</v>
       </c>
@@ -56033,9 +56109,12 @@
       <c r="O1065">
         <v>10.377000000000001</v>
       </c>
-      <c r="Q1065" s="19"/>
-      <c r="R1065" s="20"/>
-      <c r="S1065" s="20"/>
+      <c r="Q1065" s="19">
+        <v>0.15189814814814814</v>
+      </c>
+      <c r="R1065">
+        <v>0.153201</v>
+      </c>
       <c r="T1065" s="20"/>
       <c r="U1065" s="20"/>
       <c r="W1065" s="1" t="s">
@@ -56088,9 +56167,12 @@
       <c r="O1066">
         <v>5.2690000000000001</v>
       </c>
-      <c r="Q1066" s="19"/>
-      <c r="R1066" s="20"/>
-      <c r="S1066" s="20"/>
+      <c r="Q1066" s="19">
+        <v>0.15275462962962963</v>
+      </c>
+      <c r="R1066">
+        <v>0.1001158</v>
+      </c>
       <c r="T1066" s="20"/>
       <c r="U1066" s="20"/>
       <c r="W1066" s="1" t="s">
@@ -56146,9 +56228,12 @@
       <c r="O1067">
         <v>6.4260000000000002</v>
       </c>
-      <c r="Q1067" s="19"/>
-      <c r="R1067" s="20"/>
-      <c r="S1067" s="20"/>
+      <c r="Q1067" s="19">
+        <v>0.1534837962962963</v>
+      </c>
+      <c r="R1067" s="20">
+        <v>4.65E-2</v>
+      </c>
       <c r="T1067" s="20"/>
       <c r="U1067" s="20"/>
       <c r="W1067" s="1" t="s">
@@ -56204,7 +56289,12 @@
       <c r="O1068">
         <v>7.1230000000000002</v>
       </c>
-      <c r="Q1068" s="19"/>
+      <c r="Q1068" s="19">
+        <v>0.15416666666666667</v>
+      </c>
+      <c r="R1068">
+        <v>0.20662230000000001</v>
+      </c>
       <c r="W1068" s="1" t="s">
         <v>212</v>
       </c>
@@ -56264,6 +56354,9 @@
       <c r="R1069">
         <v>0.67326960000000002</v>
       </c>
+      <c r="S1069" s="87">
+        <v>7.266</v>
+      </c>
       <c r="W1069" s="1" t="s">
         <v>212</v>
       </c>
@@ -56323,6 +56416,9 @@
       <c r="R1070">
         <v>5.2211100000000003E-2</v>
       </c>
+      <c r="S1070" s="87">
+        <v>4.992</v>
+      </c>
       <c r="W1070" s="1" t="s">
         <v>212</v>
       </c>
@@ -56438,6 +56534,9 @@
       <c r="R1072">
         <v>0.87855970000000005</v>
       </c>
+      <c r="S1072" s="87">
+        <v>7.7169999999999996</v>
+      </c>
       <c r="W1072" s="1" t="s">
         <v>212</v>
       </c>
@@ -56497,7 +56596,9 @@
       <c r="R1073" s="20">
         <v>7.7842049999999996E-2</v>
       </c>
-      <c r="S1073" s="20"/>
+      <c r="S1073" s="87">
+        <v>5.6390000000000002</v>
+      </c>
       <c r="T1073" s="20"/>
       <c r="U1073" s="20"/>
       <c r="W1073" s="1" t="s">
@@ -56559,7 +56660,6 @@
       <c r="R1074" s="20">
         <v>5.4163450000000002E-2</v>
       </c>
-      <c r="S1074" s="20"/>
       <c r="T1074" s="20"/>
       <c r="U1074" s="20"/>
       <c r="W1074" s="1" t="s">
@@ -56674,7 +56774,9 @@
       <c r="R1076" s="20">
         <v>9.7645419999999997E-2</v>
       </c>
-      <c r="S1076" s="20"/>
+      <c r="S1076" s="87">
+        <v>4.6589999999999998</v>
+      </c>
       <c r="T1076" s="20"/>
       <c r="U1076" s="20"/>
       <c r="W1076" s="1" t="s">
@@ -56795,7 +56897,6 @@
       <c r="R1078" s="20">
         <v>6.9289879999999998E-2</v>
       </c>
-      <c r="S1078" s="20"/>
       <c r="T1078" s="20"/>
       <c r="U1078" s="20"/>
       <c r="W1078" s="1" t="s">
@@ -56857,7 +56958,6 @@
       <c r="R1079" s="20">
         <v>5.2364380000000002E-2</v>
       </c>
-      <c r="S1079" s="20"/>
       <c r="T1079" s="20"/>
       <c r="U1079" s="20"/>
       <c r="W1079" s="1" t="s">
@@ -56916,7 +57016,6 @@
       <c r="R1080" s="20">
         <v>6.4290589999999995E-2</v>
       </c>
-      <c r="S1080" s="20"/>
       <c r="T1080" s="20"/>
       <c r="U1080" s="20"/>
       <c r="W1080" s="1" t="s">
@@ -56978,7 +57077,6 @@
       <c r="R1081" s="20">
         <v>9.0530920000000001E-2</v>
       </c>
-      <c r="S1081" s="20"/>
       <c r="T1081" s="20"/>
       <c r="U1081" s="20"/>
       <c r="W1081" s="1" t="s">
@@ -57040,6 +57138,9 @@
       <c r="R1082">
         <v>0.100104</v>
       </c>
+      <c r="S1082" s="87">
+        <v>5.8550000000000004</v>
+      </c>
       <c r="W1082" s="1" t="s">
         <v>212</v>
       </c>
@@ -57099,6 +57200,9 @@
       <c r="R1083">
         <v>0.83863100000000002</v>
       </c>
+      <c r="S1083" s="87">
+        <v>6.2359999999999998</v>
+      </c>
       <c r="W1083" s="1" t="s">
         <v>212</v>
       </c>
@@ -57158,7 +57262,9 @@
       <c r="R1084" s="20">
         <v>8.7913069999999996E-2</v>
       </c>
-      <c r="S1084" s="20"/>
+      <c r="S1084" s="87">
+        <v>6.1139999999999999</v>
+      </c>
       <c r="T1084" s="20"/>
       <c r="U1084" s="20"/>
       <c r="W1084" s="1" t="s">
@@ -57220,7 +57326,9 @@
       <c r="R1085" s="20">
         <v>4.6324850000000001E-2</v>
       </c>
-      <c r="S1085" s="20"/>
+      <c r="S1085" s="87">
+        <v>5.3920000000000003</v>
+      </c>
       <c r="T1085" s="20"/>
       <c r="U1085" s="20"/>
       <c r="W1085" s="1" t="s">
@@ -57397,6 +57505,9 @@
       <c r="R1088">
         <v>0.12033820000000001</v>
       </c>
+      <c r="S1088" s="87">
+        <v>8.1159999999999997</v>
+      </c>
       <c r="W1088" s="1" t="s">
         <v>212</v>
       </c>
@@ -57515,7 +57626,9 @@
       <c r="R1090" s="20">
         <v>8.5060430000000006E-2</v>
       </c>
-      <c r="S1090" s="20"/>
+      <c r="S1090" s="87">
+        <v>9.3450000000000006</v>
+      </c>
       <c r="T1090" s="20"/>
       <c r="U1090" s="20"/>
       <c r="W1090" s="1" t="s">
@@ -57571,7 +57684,6 @@
       <c r="R1091" s="20">
         <v>1.2087290000000001E-2</v>
       </c>
-      <c r="S1091" s="20"/>
       <c r="T1091" s="20"/>
       <c r="U1091" s="20"/>
       <c r="W1091" s="1" t="s">
@@ -57624,7 +57736,6 @@
       <c r="R1092" s="20">
         <v>1.661118E-2</v>
       </c>
-      <c r="S1092" s="20"/>
       <c r="T1092" s="20"/>
       <c r="U1092" s="20"/>
       <c r="W1092" s="1" t="s">
@@ -58913,7 +59024,6 @@
       <c r="R1130" s="20">
         <v>7.6561779999999996E-2</v>
       </c>
-      <c r="S1130" s="20"/>
       <c r="T1130" s="20"/>
       <c r="U1130" s="20"/>
       <c r="W1130" s="1" t="s">
@@ -59034,7 +59144,6 @@
       <c r="R1132" s="20">
         <v>3.407574E-2</v>
       </c>
-      <c r="S1132" s="20"/>
       <c r="T1132" s="20"/>
       <c r="U1132" s="20"/>
       <c r="W1132" s="1" t="s">
@@ -59211,7 +59320,6 @@
       <c r="R1135" s="20">
         <v>2.5523779999999999E-2</v>
       </c>
-      <c r="S1135" s="20"/>
       <c r="T1135" s="20"/>
       <c r="U1135" s="20"/>
       <c r="W1135" s="1" t="s">
@@ -59273,7 +59381,6 @@
       <c r="R1136" s="20">
         <v>3.6209190000000002E-2</v>
       </c>
-      <c r="S1136" s="20"/>
       <c r="T1136" s="20"/>
       <c r="U1136" s="20"/>
       <c r="W1136" s="1" t="s">
@@ -59332,7 +59439,6 @@
       <c r="R1137" s="20">
         <v>5.371836E-2</v>
       </c>
-      <c r="S1137" s="20"/>
       <c r="T1137" s="20"/>
       <c r="U1137" s="20"/>
       <c r="W1137" s="1" t="s">
@@ -59509,7 +59615,6 @@
       <c r="R1140" s="20">
         <v>9.1805330000000004E-2</v>
       </c>
-      <c r="S1140" s="20"/>
       <c r="T1140" s="20"/>
       <c r="U1140" s="20"/>
       <c r="W1140" s="1" t="s">
@@ -59571,7 +59676,6 @@
       <c r="R1141" s="20">
         <v>6.242495E-2</v>
       </c>
-      <c r="S1141" s="20"/>
       <c r="T1141" s="20"/>
       <c r="U1141" s="20"/>
       <c r="W1141" s="1" t="s">
@@ -59745,7 +59849,6 @@
       <c r="R1144" s="20">
         <v>4.4876819999999998E-3</v>
       </c>
-      <c r="S1144" s="20"/>
       <c r="T1144" s="20"/>
       <c r="U1144" s="20"/>
       <c r="W1144" s="1" t="s">
@@ -59804,7 +59907,6 @@
       <c r="R1145" s="20">
         <v>3.3541950000000001E-2</v>
       </c>
-      <c r="S1145" s="20"/>
       <c r="T1145" s="20"/>
       <c r="U1145" s="20"/>
       <c r="W1145" s="1" t="s">
@@ -59922,7 +60024,6 @@
       <c r="R1147" s="20">
         <v>3.1575810000000003E-2</v>
       </c>
-      <c r="S1147" s="20"/>
       <c r="T1147" s="20"/>
       <c r="U1147" s="20"/>
       <c r="W1147" s="1" t="s">
@@ -59984,7 +60085,6 @@
       <c r="R1148" s="20">
         <v>4.312788E-2</v>
       </c>
-      <c r="S1148" s="20"/>
       <c r="T1148" s="20"/>
       <c r="U1148" s="20"/>
       <c r="W1148" s="1" t="s">
@@ -60046,7 +60146,6 @@
       <c r="R1149" s="20">
         <v>8.6385959999999998E-2</v>
       </c>
-      <c r="S1149" s="20"/>
       <c r="T1149" s="20"/>
       <c r="U1149" s="20"/>
       <c r="W1149" s="1" t="s">
@@ -60226,7 +60325,6 @@
       <c r="R1152" s="20">
         <v>3.0590050000000001E-2</v>
       </c>
-      <c r="S1152" s="20"/>
       <c r="T1152" s="20"/>
       <c r="U1152" s="20"/>
       <c r="W1152" s="1" t="s">
@@ -60400,7 +60498,6 @@
       <c r="R1155" s="20">
         <v>4.4875369999999998E-2</v>
       </c>
-      <c r="S1155" s="20"/>
       <c r="T1155" s="20"/>
       <c r="U1155" s="20"/>
       <c r="W1155" s="1" t="s">
@@ -60462,7 +60559,6 @@
       <c r="R1156" s="20">
         <v>8.5794800000000004E-3</v>
       </c>
-      <c r="S1156" s="20"/>
       <c r="T1156" s="20"/>
       <c r="U1156" s="20"/>
       <c r="W1156" s="1" t="s">
@@ -60521,7 +60617,6 @@
       <c r="R1157" s="20">
         <v>2.9920080000000002E-2</v>
       </c>
-      <c r="S1157" s="20"/>
       <c r="T1157" s="20"/>
       <c r="U1157" s="20"/>
       <c r="W1157" s="1" t="s">
@@ -60583,7 +60678,6 @@
       <c r="R1158" s="20">
         <v>4.6791739999999998E-2</v>
       </c>
-      <c r="S1158" s="20"/>
       <c r="T1158" s="20"/>
       <c r="U1158" s="20"/>
       <c r="W1158" s="1" t="s">
@@ -60642,7 +60736,6 @@
       <c r="R1159" s="20">
         <v>5.5884540000000003E-2</v>
       </c>
-      <c r="S1159" s="20"/>
       <c r="T1159" s="20"/>
       <c r="U1159" s="20"/>
       <c r="W1159" s="1" t="s">
@@ -60763,7 +60856,6 @@
       <c r="R1161" s="20">
         <v>2.887698E-2</v>
       </c>
-      <c r="S1161" s="20"/>
       <c r="T1161" s="20"/>
       <c r="U1161" s="20"/>
       <c r="W1161" s="1" t="s">
@@ -60943,7 +61035,6 @@
       <c r="R1164" s="20">
         <v>7.1481139999999997E-3</v>
       </c>
-      <c r="S1164" s="20"/>
       <c r="T1164" s="20"/>
       <c r="U1164" s="20"/>
       <c r="W1164" s="1" t="s">
@@ -61064,7 +61155,6 @@
       <c r="R1166" s="20">
         <v>8.0072249999999998E-2</v>
       </c>
-      <c r="S1166" s="20"/>
       <c r="T1166" s="20"/>
       <c r="U1166" s="20"/>
       <c r="W1166" s="1" t="s">
@@ -61120,7 +61210,6 @@
       <c r="R1167" s="20">
         <v>4.0586750000000003E-3</v>
       </c>
-      <c r="S1167" s="20"/>
       <c r="T1167" s="20"/>
       <c r="U1167" s="20"/>
       <c r="W1167" s="1" t="s">
@@ -61173,7 +61262,6 @@
       <c r="R1168" s="20">
         <v>3.7804010000000001E-3</v>
       </c>
-      <c r="S1168" s="20"/>
       <c r="T1168" s="20"/>
       <c r="U1168" s="20"/>
       <c r="W1168" s="1" t="s">
@@ -61291,7 +61379,6 @@
       <c r="R1170" s="20">
         <v>7.2459109999999993E-2</v>
       </c>
-      <c r="S1170" s="20"/>
       <c r="T1170" s="20"/>
       <c r="U1170" s="20"/>
       <c r="W1170" s="1" t="s">
@@ -61350,7 +61437,6 @@
       <c r="R1171" s="20">
         <v>6.7099820000000004E-2</v>
       </c>
-      <c r="S1171" s="20"/>
       <c r="T1171" s="20"/>
       <c r="U1171" s="20"/>
       <c r="W1171" s="1" t="s">
@@ -61471,7 +61557,6 @@
       <c r="R1173" s="20">
         <v>8.0056939999999993E-2</v>
       </c>
-      <c r="S1173" s="20"/>
       <c r="T1173" s="20"/>
       <c r="U1173" s="20"/>
       <c r="W1173" s="1" t="s">
@@ -61533,7 +61618,6 @@
       <c r="R1174" s="20">
         <v>2.9959989999999999E-2</v>
       </c>
-      <c r="S1174" s="20"/>
       <c r="T1174" s="20"/>
       <c r="U1174" s="20"/>
       <c r="W1174" s="1" t="s">
@@ -61648,7 +61732,6 @@
       <c r="R1176" s="20">
         <v>5.729223E-2</v>
       </c>
-      <c r="S1176" s="20"/>
       <c r="T1176" s="20"/>
       <c r="U1176" s="20"/>
       <c r="W1176" s="1" t="s">
@@ -61707,7 +61790,6 @@
       <c r="R1177" s="20">
         <v>6.7415920000000004E-2</v>
       </c>
-      <c r="S1177" s="20"/>
       <c r="T1177" s="20"/>
       <c r="U1177" s="20"/>
       <c r="W1177" s="1" t="s">
@@ -61999,7 +62081,6 @@
       <c r="R1182" s="20">
         <v>8.6265679999999997E-2</v>
       </c>
-      <c r="S1182" s="20"/>
       <c r="T1182" s="20"/>
       <c r="U1182" s="20"/>
       <c r="W1182" s="1" t="s">
@@ -62120,7 +62201,6 @@
       <c r="R1184" s="20">
         <v>7.2858359999999997E-2</v>
       </c>
-      <c r="S1184" s="20"/>
       <c r="T1184" s="20"/>
       <c r="U1184" s="20"/>
       <c r="W1184" s="1" t="s">
@@ -62179,7 +62259,6 @@
       <c r="R1185" s="20">
         <v>5.7349049999999999E-2</v>
       </c>
-      <c r="S1185" s="20"/>
       <c r="T1185" s="20"/>
       <c r="U1185" s="20"/>
       <c r="W1185" s="1" t="s">
@@ -62238,7 +62317,6 @@
       <c r="R1186" s="20">
         <v>1.5913570000000001E-3</v>
       </c>
-      <c r="S1186" s="20"/>
       <c r="T1186" s="20"/>
       <c r="U1186" s="20"/>
       <c r="W1186" s="1" t="s">
@@ -62474,7 +62552,6 @@
       <c r="R1190" s="20">
         <v>1.278428E-2</v>
       </c>
-      <c r="S1190" s="20"/>
       <c r="T1190" s="20"/>
       <c r="U1190" s="20"/>
       <c r="W1190" s="1" t="s">
@@ -62651,7 +62728,6 @@
       <c r="R1193" s="20">
         <v>4.4572809999999997E-2</v>
       </c>
-      <c r="S1193" s="20"/>
       <c r="T1193" s="20"/>
       <c r="U1193" s="20"/>
       <c r="W1193" s="1" t="s">
@@ -62831,7 +62907,6 @@
       <c r="R1196" s="20">
         <v>8.5699609999999996E-2</v>
       </c>
-      <c r="S1196" s="20"/>
       <c r="T1196" s="20"/>
       <c r="U1196" s="20"/>
       <c r="W1196" s="1" t="s">
@@ -62893,7 +62968,6 @@
       <c r="R1197" s="20">
         <v>8.2060049999999995E-2</v>
       </c>
-      <c r="S1197" s="20"/>
       <c r="T1197" s="20"/>
       <c r="U1197" s="20"/>
       <c r="W1197" s="1" t="s">
@@ -62952,7 +63026,6 @@
       <c r="R1198" s="20">
         <v>5.9322079999999999E-2</v>
       </c>
-      <c r="S1198" s="20"/>
       <c r="T1198" s="20"/>
       <c r="U1198" s="20"/>
       <c r="W1198" s="1" t="s">
@@ -63070,7 +63143,6 @@
       <c r="R1200" s="20">
         <v>5.8869419999999999E-2</v>
       </c>
-      <c r="S1200" s="20"/>
       <c r="T1200" s="20"/>
       <c r="U1200" s="20"/>
       <c r="W1200" s="1" t="s">
@@ -63129,7 +63201,6 @@
       <c r="R1201" s="20">
         <v>8.1516149999999996E-2</v>
       </c>
-      <c r="S1201" s="20"/>
       <c r="T1201" s="20"/>
       <c r="U1201" s="20"/>
       <c r="W1201" s="1" t="s">
@@ -63250,7 +63321,6 @@
       <c r="R1203" s="20">
         <v>6.4529660000000003E-2</v>
       </c>
-      <c r="S1203" s="20"/>
       <c r="T1203" s="20"/>
       <c r="U1203" s="20"/>
       <c r="W1203" s="1" t="s">
@@ -63368,7 +63438,6 @@
       <c r="R1205" s="20">
         <v>1.4658559999999999E-2</v>
       </c>
-      <c r="S1205" s="20"/>
       <c r="T1205" s="20"/>
       <c r="U1205" s="20"/>
       <c r="W1205" s="1" t="s">
@@ -63427,7 +63496,6 @@
       <c r="R1206" s="20">
         <v>9.5663380000000006E-2</v>
       </c>
-      <c r="S1206" s="20"/>
       <c r="T1206" s="20"/>
       <c r="U1206" s="20"/>
       <c r="W1206" s="1" t="s">
@@ -63486,7 +63554,6 @@
       <c r="R1207" s="20">
         <v>6.6704650000000004E-2</v>
       </c>
-      <c r="S1207" s="20"/>
       <c r="T1207" s="20"/>
       <c r="U1207" s="20"/>
       <c r="W1207" s="1" t="s">
@@ -63604,7 +63671,6 @@
       <c r="R1209" s="20">
         <v>9.1252029999999998E-2</v>
       </c>
-      <c r="S1209" s="20"/>
       <c r="T1209" s="20"/>
       <c r="U1209" s="20"/>
       <c r="W1209" s="1" t="s">
@@ -63666,7 +63732,6 @@
       <c r="R1210" s="20">
         <v>5.2513480000000001E-2</v>
       </c>
-      <c r="S1210" s="20"/>
       <c r="T1210" s="20"/>
       <c r="U1210" s="20"/>
       <c r="W1210" s="1" t="s">
@@ -63784,7 +63849,6 @@
       <c r="R1212" s="20">
         <v>7.8847390000000003E-2</v>
       </c>
-      <c r="S1212" s="20"/>
       <c r="T1212" s="20"/>
       <c r="U1212" s="20"/>
       <c r="W1212" s="1" t="s">
@@ -63899,7 +63963,6 @@
       <c r="R1214" s="20">
         <v>1.033865E-2</v>
       </c>
-      <c r="S1214" s="20"/>
       <c r="T1214" s="20"/>
       <c r="U1214" s="20"/>
       <c r="W1214" s="1" t="s">
@@ -63952,7 +64015,6 @@
       <c r="R1215" s="20">
         <v>9.7152669999999997E-3</v>
       </c>
-      <c r="S1215" s="20"/>
       <c r="T1215" s="20"/>
       <c r="U1215" s="20"/>
       <c r="W1215" s="1" t="s">
@@ -80224,7 +80286,9 @@
       <c r="P1598" s="63"/>
       <c r="Q1598" s="19"/>
       <c r="R1598" s="20"/>
-      <c r="S1598" s="20"/>
+      <c r="S1598" s="87">
+        <v>3.7850000000000001</v>
+      </c>
       <c r="T1598" s="20"/>
       <c r="U1598" s="20"/>
       <c r="W1598" s="1" t="s">
@@ -80263,6 +80327,12 @@
       <c r="K1599" t="s">
         <v>60</v>
       </c>
+      <c r="S1599" s="87">
+        <v>8.673</v>
+      </c>
+      <c r="W1599" s="1" t="s">
+        <v>212</v>
+      </c>
       <c r="AB1599" t="s">
         <v>85</v>
       </c>
@@ -80296,6 +80366,12 @@
       <c r="K1600" t="s">
         <v>60</v>
       </c>
+      <c r="S1600" s="87">
+        <v>6.7759999999999998</v>
+      </c>
+      <c r="W1600" s="1" t="s">
+        <v>212</v>
+      </c>
       <c r="AB1600" t="s">
         <v>86</v>
       </c>
@@ -80329,6 +80405,12 @@
       <c r="K1601" t="s">
         <v>60</v>
       </c>
+      <c r="S1601" s="87">
+        <v>3.77</v>
+      </c>
+      <c r="W1601" s="1" t="s">
+        <v>212</v>
+      </c>
       <c r="AB1601" t="s">
         <v>85</v>
       </c>
@@ -80362,6 +80444,12 @@
       <c r="K1602" t="s">
         <v>60</v>
       </c>
+      <c r="S1602" s="87">
+        <v>6.7839999999999998</v>
+      </c>
+      <c r="W1602" s="1" t="s">
+        <v>212</v>
+      </c>
       <c r="AB1602" t="s">
         <v>86</v>
       </c>
@@ -80395,6 +80483,12 @@
       <c r="K1603" t="s">
         <v>60</v>
       </c>
+      <c r="S1603" s="87">
+        <v>2.6850000000000001</v>
+      </c>
+      <c r="W1603" s="1" t="s">
+        <v>212</v>
+      </c>
       <c r="AB1603" t="s">
         <v>86</v>
       </c>
@@ -80428,6 +80522,12 @@
       <c r="K1604" t="s">
         <v>60</v>
       </c>
+      <c r="S1604" s="87">
+        <v>2.9350000000000001</v>
+      </c>
+      <c r="W1604" s="1" t="s">
+        <v>212</v>
+      </c>
       <c r="AB1604" t="s">
         <v>86</v>
       </c>
@@ -80461,6 +80561,12 @@
       <c r="K1605" t="s">
         <v>60</v>
       </c>
+      <c r="S1605" s="87">
+        <v>5.6710000000000003</v>
+      </c>
+      <c r="W1605" s="1" t="s">
+        <v>212</v>
+      </c>
       <c r="AB1605" t="s">
         <v>86</v>
       </c>
@@ -80494,6 +80600,12 @@
       <c r="K1606" t="s">
         <v>60</v>
       </c>
+      <c r="S1606" s="87">
+        <v>1.998</v>
+      </c>
+      <c r="W1606" s="1" t="s">
+        <v>212</v>
+      </c>
       <c r="AB1606" t="s">
         <v>85</v>
       </c>
@@ -80527,6 +80639,12 @@
       <c r="K1607" t="s">
         <v>60</v>
       </c>
+      <c r="S1607" s="87">
+        <v>8.7219999999999995</v>
+      </c>
+      <c r="W1607" s="1" t="s">
+        <v>212</v>
+      </c>
       <c r="AB1607" t="s">
         <v>85</v>
       </c>
@@ -80560,6 +80678,12 @@
       <c r="K1608" t="s">
         <v>60</v>
       </c>
+      <c r="S1608" s="87">
+        <v>6.1420000000000003</v>
+      </c>
+      <c r="W1608" s="1" t="s">
+        <v>212</v>
+      </c>
       <c r="AB1608" t="s">
         <v>85</v>
       </c>
@@ -80593,6 +80717,12 @@
       <c r="K1609" t="s">
         <v>60</v>
       </c>
+      <c r="S1609" s="87">
+        <v>5.1260000000000003</v>
+      </c>
+      <c r="W1609" s="1" t="s">
+        <v>212</v>
+      </c>
       <c r="AB1609" t="s">
         <v>85</v>
       </c>
@@ -80626,6 +80756,12 @@
       <c r="K1610" t="s">
         <v>60</v>
       </c>
+      <c r="S1610" s="87">
+        <v>7.359</v>
+      </c>
+      <c r="W1610" s="1" t="s">
+        <v>212</v>
+      </c>
       <c r="AB1610" t="s">
         <v>86</v>
       </c>
@@ -80659,6 +80795,12 @@
       <c r="K1611" t="s">
         <v>60</v>
       </c>
+      <c r="S1611" s="87">
+        <v>5.1959999999999997</v>
+      </c>
+      <c r="W1611" s="1" t="s">
+        <v>212</v>
+      </c>
       <c r="AB1611" t="s">
         <v>86</v>
       </c>
@@ -80692,6 +80834,12 @@
       <c r="K1612" t="s">
         <v>60</v>
       </c>
+      <c r="S1612" s="87">
+        <v>5.8280000000000003</v>
+      </c>
+      <c r="W1612" s="1" t="s">
+        <v>212</v>
+      </c>
       <c r="AB1612" t="s">
         <v>85</v>
       </c>
@@ -80725,6 +80873,12 @@
       <c r="K1613" t="s">
         <v>60</v>
       </c>
+      <c r="S1613" s="87">
+        <v>4.093</v>
+      </c>
+      <c r="W1613" s="1" t="s">
+        <v>212</v>
+      </c>
       <c r="AB1613" t="s">
         <v>85</v>
       </c>
@@ -80758,6 +80912,12 @@
       <c r="K1614" t="s">
         <v>60</v>
       </c>
+      <c r="S1614" s="87">
+        <v>6.2629999999999999</v>
+      </c>
+      <c r="W1614" s="1" t="s">
+        <v>212</v>
+      </c>
       <c r="AB1614" t="s">
         <v>86</v>
       </c>
@@ -80791,6 +80951,12 @@
       <c r="K1615" t="s">
         <v>60</v>
       </c>
+      <c r="S1615" s="87">
+        <v>5.2160000000000002</v>
+      </c>
+      <c r="W1615" s="1" t="s">
+        <v>212</v>
+      </c>
       <c r="AB1615" t="s">
         <v>86</v>
       </c>
@@ -80824,6 +80990,12 @@
       <c r="K1616" t="s">
         <v>60</v>
       </c>
+      <c r="S1616" s="87">
+        <v>6.9880000000000004</v>
+      </c>
+      <c r="W1616" s="1" t="s">
+        <v>212</v>
+      </c>
       <c r="AB1616" t="s">
         <v>85</v>
       </c>
@@ -80857,6 +81029,12 @@
       <c r="K1617" t="s">
         <v>60</v>
       </c>
+      <c r="S1617" s="87">
+        <v>4.9649999999999999</v>
+      </c>
+      <c r="W1617" s="1" t="s">
+        <v>212</v>
+      </c>
       <c r="AB1617" t="s">
         <v>85</v>
       </c>
@@ -80890,6 +81068,12 @@
       <c r="K1618" t="s">
         <v>60</v>
       </c>
+      <c r="S1618" s="87">
+        <v>6.9420000000000002</v>
+      </c>
+      <c r="W1618" s="1" t="s">
+        <v>212</v>
+      </c>
       <c r="AB1618" t="s">
         <v>86</v>
       </c>
@@ -80923,6 +81107,12 @@
       <c r="K1619" t="s">
         <v>60</v>
       </c>
+      <c r="S1619" s="87">
+        <v>1.736</v>
+      </c>
+      <c r="W1619" s="1" t="s">
+        <v>212</v>
+      </c>
       <c r="AB1619" t="s">
         <v>85</v>
       </c>
@@ -80956,6 +81146,12 @@
       <c r="K1620" t="s">
         <v>60</v>
       </c>
+      <c r="S1620" s="87">
+        <v>5.0460000000000003</v>
+      </c>
+      <c r="W1620" s="1" t="s">
+        <v>212</v>
+      </c>
       <c r="AB1620" t="s">
         <v>85</v>
       </c>
@@ -80989,6 +81185,12 @@
       <c r="K1621" t="s">
         <v>60</v>
       </c>
+      <c r="S1621" s="87">
+        <v>7.5359999999999996</v>
+      </c>
+      <c r="W1621" s="1" t="s">
+        <v>212</v>
+      </c>
       <c r="AB1621" t="s">
         <v>86</v>
       </c>
@@ -81022,6 +81224,12 @@
       <c r="K1622" t="s">
         <v>60</v>
       </c>
+      <c r="S1622" s="87">
+        <v>5.4489999999999998</v>
+      </c>
+      <c r="W1622" s="1" t="s">
+        <v>212</v>
+      </c>
       <c r="AB1622" t="s">
         <v>85</v>
       </c>
@@ -81055,6 +81263,9 @@
       <c r="K1623" t="s">
         <v>60</v>
       </c>
+      <c r="W1623" s="1" t="s">
+        <v>212</v>
+      </c>
     </row>
     <row r="1624" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A1624">
@@ -81078,6 +81289,9 @@
       <c r="K1624" t="s">
         <v>60</v>
       </c>
+      <c r="W1624" s="1" t="s">
+        <v>212</v>
+      </c>
     </row>
     <row r="1625" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A1625">
@@ -81101,6 +81315,12 @@
       <c r="K1625" t="s">
         <v>60</v>
       </c>
+      <c r="S1625" s="87">
+        <v>7.5780000000000003</v>
+      </c>
+      <c r="W1625" s="1" t="s">
+        <v>212</v>
+      </c>
       <c r="AB1625" t="s">
         <v>85</v>
       </c>
@@ -81134,6 +81354,12 @@
       <c r="K1626" t="s">
         <v>60</v>
       </c>
+      <c r="S1626" s="87">
+        <v>6.9889999999999999</v>
+      </c>
+      <c r="W1626" s="1" t="s">
+        <v>212</v>
+      </c>
       <c r="AB1626" t="s">
         <v>85</v>
       </c>
@@ -81167,6 +81393,12 @@
       <c r="K1627" t="s">
         <v>60</v>
       </c>
+      <c r="S1627" s="87">
+        <v>8.3729999999999993</v>
+      </c>
+      <c r="W1627" s="1" t="s">
+        <v>212</v>
+      </c>
       <c r="AB1627" t="s">
         <v>85</v>
       </c>
@@ -81200,6 +81432,12 @@
       <c r="K1628" t="s">
         <v>60</v>
       </c>
+      <c r="S1628" s="87">
+        <v>3.165</v>
+      </c>
+      <c r="W1628" s="1" t="s">
+        <v>212</v>
+      </c>
       <c r="AB1628" t="s">
         <v>86</v>
       </c>
@@ -81233,6 +81471,12 @@
       <c r="K1629" t="s">
         <v>60</v>
       </c>
+      <c r="S1629" s="87">
+        <v>9.5709999999999997</v>
+      </c>
+      <c r="W1629" s="1" t="s">
+        <v>212</v>
+      </c>
       <c r="AB1629" t="s">
         <v>86</v>
       </c>
@@ -81266,6 +81510,12 @@
       <c r="K1630" t="s">
         <v>60</v>
       </c>
+      <c r="S1630" s="87">
+        <v>2.605</v>
+      </c>
+      <c r="W1630" s="1" t="s">
+        <v>212</v>
+      </c>
       <c r="AB1630" t="s">
         <v>86</v>
       </c>
@@ -81299,6 +81549,12 @@
       <c r="K1631" t="s">
         <v>60</v>
       </c>
+      <c r="S1631" s="87">
+        <v>6.2060000000000004</v>
+      </c>
+      <c r="W1631" s="1" t="s">
+        <v>212</v>
+      </c>
       <c r="AB1631" t="s">
         <v>85</v>
       </c>
@@ -81332,6 +81588,12 @@
       <c r="K1632" t="s">
         <v>60</v>
       </c>
+      <c r="S1632" s="87">
+        <v>4.6920000000000002</v>
+      </c>
+      <c r="W1632" s="1" t="s">
+        <v>212</v>
+      </c>
       <c r="AB1632" t="s">
         <v>86</v>
       </c>
@@ -81365,6 +81627,12 @@
       <c r="K1633" t="s">
         <v>60</v>
       </c>
+      <c r="S1633" s="87">
+        <v>3.1080000000000001</v>
+      </c>
+      <c r="W1633" s="1" t="s">
+        <v>212</v>
+      </c>
       <c r="AB1633" t="s">
         <v>85</v>
       </c>
@@ -81398,6 +81666,12 @@
       <c r="K1634" t="s">
         <v>60</v>
       </c>
+      <c r="S1634" s="87">
+        <v>5.5510000000000002</v>
+      </c>
+      <c r="W1634" s="1" t="s">
+        <v>212</v>
+      </c>
       <c r="AB1634" t="s">
         <v>86</v>
       </c>
@@ -81431,6 +81705,12 @@
       <c r="K1635" t="s">
         <v>60</v>
       </c>
+      <c r="S1635" s="87">
+        <v>4.4669999999999996</v>
+      </c>
+      <c r="W1635" s="1" t="s">
+        <v>212</v>
+      </c>
       <c r="AB1635" t="s">
         <v>85</v>
       </c>
@@ -81464,6 +81744,12 @@
       <c r="K1636" t="s">
         <v>60</v>
       </c>
+      <c r="S1636" s="87">
+        <v>5.7220000000000004</v>
+      </c>
+      <c r="W1636" s="1" t="s">
+        <v>212</v>
+      </c>
       <c r="AB1636" t="s">
         <v>85</v>
       </c>
@@ -81497,6 +81783,12 @@
       <c r="K1637" t="s">
         <v>60</v>
       </c>
+      <c r="S1637" s="87">
+        <v>2.702</v>
+      </c>
+      <c r="W1637" s="1" t="s">
+        <v>212</v>
+      </c>
       <c r="AB1637" t="s">
         <v>85</v>
       </c>
@@ -81530,6 +81822,12 @@
       <c r="K1638" t="s">
         <v>60</v>
       </c>
+      <c r="S1638" s="87">
+        <v>5.98</v>
+      </c>
+      <c r="W1638" s="1" t="s">
+        <v>212</v>
+      </c>
       <c r="AB1638" t="s">
         <v>85</v>
       </c>
@@ -81563,6 +81861,12 @@
       <c r="K1639" t="s">
         <v>60</v>
       </c>
+      <c r="S1639" s="87">
+        <v>7.1420000000000003</v>
+      </c>
+      <c r="W1639" s="1" t="s">
+        <v>212</v>
+      </c>
       <c r="AB1639" t="s">
         <v>86</v>
       </c>
@@ -81596,6 +81900,12 @@
       <c r="K1640" t="s">
         <v>60</v>
       </c>
+      <c r="S1640" s="87">
+        <v>3.8460000000000001</v>
+      </c>
+      <c r="W1640" s="1" t="s">
+        <v>212</v>
+      </c>
       <c r="AB1640" t="s">
         <v>86</v>
       </c>
@@ -81629,6 +81939,12 @@
       <c r="K1641" t="s">
         <v>60</v>
       </c>
+      <c r="S1641" s="87">
+        <v>4.28</v>
+      </c>
+      <c r="W1641" s="1" t="s">
+        <v>212</v>
+      </c>
       <c r="AB1641" t="s">
         <v>86</v>
       </c>
@@ -81662,6 +81978,12 @@
       <c r="K1642" t="s">
         <v>60</v>
       </c>
+      <c r="S1642" s="87">
+        <v>7.7489999999999997</v>
+      </c>
+      <c r="W1642" s="1" t="s">
+        <v>212</v>
+      </c>
       <c r="AB1642" t="s">
         <v>85</v>
       </c>
@@ -81695,6 +82017,12 @@
       <c r="K1643" t="s">
         <v>60</v>
       </c>
+      <c r="S1643" s="87">
+        <v>4.476</v>
+      </c>
+      <c r="W1643" s="1" t="s">
+        <v>212</v>
+      </c>
       <c r="AB1643" t="s">
         <v>85</v>
       </c>
@@ -81728,6 +82056,12 @@
       <c r="K1644" t="s">
         <v>60</v>
       </c>
+      <c r="S1644" s="87">
+        <v>2.1349999999999998</v>
+      </c>
+      <c r="W1644" s="1" t="s">
+        <v>212</v>
+      </c>
       <c r="AB1644" t="s">
         <v>85</v>
       </c>
@@ -81761,6 +82095,12 @@
       <c r="K1645" t="s">
         <v>60</v>
       </c>
+      <c r="S1645" s="87">
+        <v>2.8079999999999998</v>
+      </c>
+      <c r="W1645" s="1" t="s">
+        <v>212</v>
+      </c>
       <c r="AB1645" t="s">
         <v>85</v>
       </c>
@@ -81794,6 +82134,12 @@
       <c r="K1646" t="s">
         <v>60</v>
       </c>
+      <c r="S1646" s="87">
+        <v>4.67</v>
+      </c>
+      <c r="W1646" s="1" t="s">
+        <v>212</v>
+      </c>
       <c r="AB1646" t="s">
         <v>86</v>
       </c>
@@ -81827,6 +82173,12 @@
       <c r="K1647" t="s">
         <v>60</v>
       </c>
+      <c r="S1647" s="87">
+        <v>6.6849999999999996</v>
+      </c>
+      <c r="W1647" s="1" t="s">
+        <v>212</v>
+      </c>
       <c r="AB1647" t="s">
         <v>85</v>
       </c>
@@ -81860,6 +82212,12 @@
       <c r="K1648" t="s">
         <v>60</v>
       </c>
+      <c r="S1648" s="87">
+        <v>7.4770000000000003</v>
+      </c>
+      <c r="W1648" s="1" t="s">
+        <v>212</v>
+      </c>
       <c r="AB1648" t="s">
         <v>86</v>
       </c>
@@ -81893,6 +82251,12 @@
       <c r="K1649" t="s">
         <v>60</v>
       </c>
+      <c r="S1649" s="87">
+        <v>3.2719999999999998</v>
+      </c>
+      <c r="W1649" s="1" t="s">
+        <v>212</v>
+      </c>
       <c r="AB1649" t="s">
         <v>85</v>
       </c>
@@ -81926,6 +82290,9 @@
       <c r="K1650" t="s">
         <v>60</v>
       </c>
+      <c r="W1650" s="1" t="s">
+        <v>212</v>
+      </c>
     </row>
     <row r="1651" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A1651">
@@ -81949,6 +82316,9 @@
       <c r="K1651" t="s">
         <v>60</v>
       </c>
+      <c r="W1651" s="1" t="s">
+        <v>212</v>
+      </c>
     </row>
     <row r="1652" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A1652">
@@ -87011,6 +87381,34 @@
         <v>12</v>
       </c>
       <c r="K1813" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1814" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="G1814" s="1" t="s">
+        <v>676</v>
+      </c>
+      <c r="I1814" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1814">
+        <v>13</v>
+      </c>
+      <c r="K1814" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1815" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="G1815" s="1" t="s">
+        <v>676</v>
+      </c>
+      <c r="I1815" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1815">
+        <v>13</v>
+      </c>
+      <c r="K1815" t="s">
         <v>60</v>
       </c>
     </row>
@@ -87024,7 +87422,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD836908-61FC-4C6A-BB55-EB17A2B99FDD}">
   <dimension ref="A1:M81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
+    <sheetView topLeftCell="A65" workbookViewId="0">
       <selection activeCell="H83" sqref="H83"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
adding resp data for 2018-09-08 cohort day 9+24
</commit_message>
<xml_diff>
--- a/Data/2018-08-14_master_datac_2018_collection_year.xlsx
+++ b/Data/2018-08-14_master_datac_2018_collection_year.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andrew.nguyen\Desktop\Circadian_rhythm_runs_seasonal_timing\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70CA6FE2-D1BC-45FE-B5EE-640B6B17F7F3}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE9C68FB-2867-4512-A747-FC1EDD497F93}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3345" yWindow="465" windowWidth="47520" windowHeight="26880" activeTab="1" xr2:uid="{C7477166-8A7C-B04A-9643-C277FEDCDAAB}"/>
   </bookViews>
@@ -16828,9 +16828,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92725FB9-1A17-2546-9DFA-6C0D39437891}">
   <dimension ref="A1:AV1968"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1123" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="U1209" sqref="U1209"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A1627" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F1633" sqref="F1633"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -53605,6 +53605,15 @@
       <c r="S1001" s="87">
         <v>3.6840000000000002</v>
       </c>
+      <c r="T1001" s="63">
+        <v>0.5180555555555556</v>
+      </c>
+      <c r="U1001" s="19">
+        <v>0.40444444444444444</v>
+      </c>
+      <c r="V1001">
+        <v>0.37625449999999999</v>
+      </c>
       <c r="W1001" s="1" t="s">
         <v>212</v>
       </c>
@@ -53666,6 +53675,12 @@
       </c>
       <c r="S1002" s="87">
         <v>5.6909999999999998</v>
+      </c>
+      <c r="U1002" s="19">
+        <v>0.40554398148148146</v>
+      </c>
+      <c r="V1002">
+        <v>0.582067</v>
       </c>
       <c r="W1002" s="1" t="s">
         <v>212</v>
@@ -53902,7 +53917,12 @@
         <v>8.6590000000000007</v>
       </c>
       <c r="T1006" s="20"/>
-      <c r="U1006" s="20"/>
+      <c r="U1006" s="19">
+        <v>0.40651620370370373</v>
+      </c>
+      <c r="V1006" s="20">
+        <v>4.552051E-2</v>
+      </c>
       <c r="W1006" s="1" t="s">
         <v>212</v>
       </c>
@@ -53966,7 +53986,12 @@
         <v>10.084</v>
       </c>
       <c r="T1007" s="20"/>
-      <c r="U1007" s="20"/>
+      <c r="U1007" s="19">
+        <v>0.40761574074074075</v>
+      </c>
+      <c r="V1007" s="20">
+        <v>9.1842679999999996E-2</v>
+      </c>
       <c r="W1007" s="1" t="s">
         <v>212</v>
       </c>
@@ -54149,6 +54174,12 @@
       <c r="S1010" s="87">
         <v>2.9660000000000002</v>
       </c>
+      <c r="U1010" s="19">
+        <v>0.4085300925925926</v>
+      </c>
+      <c r="V1010">
+        <v>0.38952949999999997</v>
+      </c>
       <c r="W1010" s="1" t="s">
         <v>212</v>
       </c>
@@ -54210,6 +54241,12 @@
       </c>
       <c r="S1011" s="87">
         <v>3.2120000000000002</v>
+      </c>
+      <c r="U1011" s="19">
+        <v>0.40932870370370367</v>
+      </c>
+      <c r="V1011" s="20">
+        <v>9.0038380000000001E-3</v>
       </c>
       <c r="W1011" s="1" t="s">
         <v>212</v>
@@ -54570,7 +54607,12 @@
         <v>6.9320000000000004</v>
       </c>
       <c r="T1017" s="20"/>
-      <c r="U1017" s="20"/>
+      <c r="U1017" s="19">
+        <v>0.41033564814814816</v>
+      </c>
+      <c r="V1017" s="20">
+        <v>4.0442119999999998E-2</v>
+      </c>
       <c r="W1017" s="1" t="s">
         <v>212</v>
       </c>
@@ -55108,7 +55150,12 @@
         <v>6.7750000000000004</v>
       </c>
       <c r="T1026" s="20"/>
-      <c r="U1026" s="20"/>
+      <c r="U1026" s="19">
+        <v>0.41113425925925928</v>
+      </c>
+      <c r="V1026" s="20">
+        <v>7.2779490000000002E-2</v>
+      </c>
       <c r="W1026" s="1" t="s">
         <v>212</v>
       </c>
@@ -55232,6 +55279,12 @@
       <c r="S1028" s="87">
         <v>2.6760000000000002</v>
       </c>
+      <c r="U1028" s="19">
+        <v>0.41200231481481481</v>
+      </c>
+      <c r="V1028">
+        <v>0.25345240000000002</v>
+      </c>
       <c r="W1028" s="1" t="s">
         <v>212</v>
       </c>
@@ -55354,7 +55407,12 @@
         <v>7.2329999999999997</v>
       </c>
       <c r="T1030" s="20"/>
-      <c r="U1030" s="20"/>
+      <c r="U1030" s="19">
+        <v>0.4131481481481481</v>
+      </c>
+      <c r="V1030" s="20">
+        <v>9.456966E-2</v>
+      </c>
       <c r="W1030" s="1" t="s">
         <v>212</v>
       </c>
@@ -55536,6 +55594,12 @@
       <c r="S1033" s="87">
         <v>7.0069999999999997</v>
       </c>
+      <c r="U1033" s="19">
+        <v>0.41396990740740741</v>
+      </c>
+      <c r="V1033" s="20">
+        <v>3.3157359999999997E-2</v>
+      </c>
       <c r="W1033" s="1" t="s">
         <v>212</v>
       </c>
@@ -56004,6 +56068,16 @@
       <c r="R1041">
         <v>0.41844710000000002</v>
       </c>
+      <c r="S1041" s="87">
+        <v>4.681</v>
+      </c>
+      <c r="T1041" s="20"/>
+      <c r="U1041" s="19">
+        <v>0.4153587962962963</v>
+      </c>
+      <c r="V1041">
+        <v>0.55424850000000003</v>
+      </c>
       <c r="W1041" s="1" t="s">
         <v>212</v>
       </c>
@@ -56063,11 +56137,6 @@
       <c r="R1042" s="20">
         <v>5.6775119999999998E-2</v>
       </c>
-      <c r="S1042" s="87">
-        <v>4.681</v>
-      </c>
-      <c r="T1042" s="20"/>
-      <c r="U1042" s="20"/>
       <c r="W1042" s="1" t="s">
         <v>212</v>
       </c>
@@ -56185,8 +56254,16 @@
       <c r="R1044" s="20">
         <v>5.6059730000000002E-2</v>
       </c>
+      <c r="S1044" s="87">
+        <v>4.5060000000000002</v>
+      </c>
       <c r="T1044" s="20"/>
-      <c r="U1044" s="20"/>
+      <c r="U1044" s="19">
+        <v>0.41642361111111109</v>
+      </c>
+      <c r="V1044">
+        <v>3.8963299999999999E-2</v>
+      </c>
       <c r="W1044" s="1" t="s">
         <v>212</v>
       </c>
@@ -56246,11 +56323,6 @@
       <c r="R1045" s="20">
         <v>4.9339939999999999E-2</v>
       </c>
-      <c r="S1045" s="87">
-        <v>4.5060000000000002</v>
-      </c>
-      <c r="T1045" s="20"/>
-      <c r="U1045" s="20"/>
       <c r="W1045" s="1" t="s">
         <v>212</v>
       </c>
@@ -56304,8 +56376,12 @@
       <c r="R1046" s="20">
         <v>3.5161099999999998E-3</v>
       </c>
-      <c r="T1046" s="20"/>
-      <c r="U1046" s="20"/>
+      <c r="U1046" s="19">
+        <v>0.41717592592592595</v>
+      </c>
+      <c r="V1046" s="20">
+        <v>7.7733180000000004E-3</v>
+      </c>
       <c r="W1046" s="1" t="s">
         <v>212</v>
       </c>
@@ -56352,8 +56428,15 @@
       </c>
       <c r="Q1047" s="19"/>
       <c r="R1047" s="20"/>
-      <c r="T1047" s="20"/>
-      <c r="U1047" s="20"/>
+      <c r="T1047" s="63">
+        <v>0.52152777777777781</v>
+      </c>
+      <c r="U1047" s="19">
+        <v>0.41790509259259262</v>
+      </c>
+      <c r="V1047" s="20">
+        <v>8.9678620000000001E-3</v>
+      </c>
       <c r="W1047" s="1" t="s">
         <v>212</v>
       </c>
@@ -56413,6 +56496,15 @@
       <c r="S1048" s="87">
         <v>3.84</v>
       </c>
+      <c r="T1048" s="63">
+        <v>0.51388888888888895</v>
+      </c>
+      <c r="U1048" s="19">
+        <v>0.40444444444444444</v>
+      </c>
+      <c r="V1048">
+        <v>0.6237935</v>
+      </c>
       <c r="W1048" s="1" t="s">
         <v>212</v>
       </c>
@@ -56531,6 +56623,12 @@
       <c r="S1050" s="87">
         <v>4.5090000000000003</v>
       </c>
+      <c r="U1050" s="19">
+        <v>0.40554398148148146</v>
+      </c>
+      <c r="V1050">
+        <v>0.1238587</v>
+      </c>
       <c r="W1050" s="1" t="s">
         <v>212</v>
       </c>
@@ -56649,6 +56747,12 @@
       <c r="S1052" s="87">
         <v>8.8439999999999994</v>
       </c>
+      <c r="U1052" s="19">
+        <v>0.40651620370370373</v>
+      </c>
+      <c r="V1052">
+        <v>0.15238170000000001</v>
+      </c>
       <c r="W1052" s="1" t="s">
         <v>212</v>
       </c>
@@ -56767,6 +56871,12 @@
       <c r="S1054" s="87">
         <v>8.0879999999999992</v>
       </c>
+      <c r="U1054" s="19">
+        <v>0.40761574074074075</v>
+      </c>
+      <c r="V1054">
+        <v>0.17047129999999999</v>
+      </c>
       <c r="W1054" s="1" t="s">
         <v>212</v>
       </c>
@@ -56888,6 +56998,12 @@
       <c r="S1056" s="87">
         <v>8.0429999999999993</v>
       </c>
+      <c r="U1056" s="19">
+        <v>0.4085300925925926</v>
+      </c>
+      <c r="V1056" s="20">
+        <v>9.1255660000000002E-2</v>
+      </c>
       <c r="W1056" s="1" t="s">
         <v>212</v>
       </c>
@@ -57061,6 +57177,12 @@
       </c>
       <c r="S1059" s="87">
         <v>5.7190000000000003</v>
+      </c>
+      <c r="U1059" s="19">
+        <v>0.40932870370370367</v>
+      </c>
+      <c r="V1059">
+        <v>1.016689</v>
       </c>
       <c r="W1059" s="1" t="s">
         <v>212</v>
@@ -57419,6 +57541,12 @@
       <c r="S1065" s="87">
         <v>4.6150000000000002</v>
       </c>
+      <c r="U1065" s="19">
+        <v>0.41033564814814816</v>
+      </c>
+      <c r="V1065" s="20">
+        <v>7.3723109999999994E-2</v>
+      </c>
       <c r="W1065" s="1" t="s">
         <v>212</v>
       </c>
@@ -57480,6 +57608,12 @@
       </c>
       <c r="S1066" s="87">
         <v>6.2309999999999999</v>
+      </c>
+      <c r="U1066" s="19">
+        <v>0.41113425925925928</v>
+      </c>
+      <c r="V1066">
+        <v>0.1182262</v>
       </c>
       <c r="W1066" s="1" t="s">
         <v>212</v>
@@ -57782,6 +57916,12 @@
       <c r="S1071" s="87">
         <v>7.266</v>
       </c>
+      <c r="U1071" s="19">
+        <v>0.41200231481481481</v>
+      </c>
+      <c r="V1071">
+        <v>0.84839779999999998</v>
+      </c>
       <c r="W1071" s="1" t="s">
         <v>212</v>
       </c>
@@ -57844,6 +57984,12 @@
       <c r="S1072" s="87">
         <v>4.992</v>
       </c>
+      <c r="U1072" s="19">
+        <v>0.4131481481481481</v>
+      </c>
+      <c r="V1072">
+        <v>0.1049495</v>
+      </c>
       <c r="W1072" s="1" t="s">
         <v>212</v>
       </c>
@@ -57962,6 +58108,12 @@
       <c r="S1074" s="87">
         <v>7.7169999999999996</v>
       </c>
+      <c r="U1074" s="19">
+        <v>0.42108796296296297</v>
+      </c>
+      <c r="V1074">
+        <v>1.173006</v>
+      </c>
       <c r="W1074" s="1" t="s">
         <v>212</v>
       </c>
@@ -58025,7 +58177,12 @@
         <v>5.6390000000000002</v>
       </c>
       <c r="T1075" s="20"/>
-      <c r="U1075" s="20"/>
+      <c r="U1075" s="19">
+        <v>0.42224537037037035</v>
+      </c>
+      <c r="V1075">
+        <v>0.1000075</v>
+      </c>
       <c r="W1075" s="1" t="s">
         <v>212</v>
       </c>
@@ -58203,7 +58360,12 @@
         <v>4.6589999999999998</v>
       </c>
       <c r="T1078" s="20"/>
-      <c r="U1078" s="20"/>
+      <c r="U1078" s="19">
+        <v>0.4230902777777778</v>
+      </c>
+      <c r="V1078">
+        <v>0.40595619999999999</v>
+      </c>
       <c r="W1078" s="1" t="s">
         <v>212</v>
       </c>
@@ -58566,6 +58728,12 @@
       <c r="S1084" s="87">
         <v>5.8550000000000004</v>
       </c>
+      <c r="U1084" s="19">
+        <v>0.41396990740740741</v>
+      </c>
+      <c r="V1084">
+        <v>0.1220908</v>
+      </c>
       <c r="W1084" s="1" t="s">
         <v>212</v>
       </c>
@@ -58628,6 +58796,12 @@
       <c r="S1085" s="87">
         <v>6.2359999999999998</v>
       </c>
+      <c r="U1085" s="19">
+        <v>0.4153587962962963</v>
+      </c>
+      <c r="V1085">
+        <v>1.1370640000000001</v>
+      </c>
       <c r="W1085" s="1" t="s">
         <v>212</v>
       </c>
@@ -58691,7 +58865,12 @@
         <v>6.1139999999999999</v>
       </c>
       <c r="T1086" s="20"/>
-      <c r="U1086" s="20"/>
+      <c r="U1086" s="19">
+        <v>0.41642361111111109</v>
+      </c>
+      <c r="V1086" s="20">
+        <v>9.2584319999999998E-2</v>
+      </c>
       <c r="W1086" s="1" t="s">
         <v>212</v>
       </c>
@@ -58755,7 +58934,12 @@
         <v>5.3920000000000003</v>
       </c>
       <c r="T1087" s="20"/>
-      <c r="U1087" s="20"/>
+      <c r="U1087" s="19">
+        <v>0.41717592592592595</v>
+      </c>
+      <c r="V1087" s="20">
+        <v>5.834027E-2</v>
+      </c>
       <c r="W1087" s="1" t="s">
         <v>212</v>
       </c>
@@ -58933,6 +59117,12 @@
       <c r="S1090" s="87">
         <v>8.1159999999999997</v>
       </c>
+      <c r="U1090" s="19">
+        <v>0.41790509259259262</v>
+      </c>
+      <c r="V1090">
+        <v>0.11892030000000001</v>
+      </c>
       <c r="W1090" s="1" t="s">
         <v>212</v>
       </c>
@@ -58992,6 +59182,15 @@
       <c r="R1091">
         <v>0.1150355</v>
       </c>
+      <c r="S1091" s="87">
+        <v>9.3450000000000006</v>
+      </c>
+      <c r="U1091" s="19">
+        <v>0.41870370370370374</v>
+      </c>
+      <c r="V1091">
+        <v>0.1596909</v>
+      </c>
       <c r="W1091" s="1" t="s">
         <v>212</v>
       </c>
@@ -59050,9 +59249,6 @@
       </c>
       <c r="R1092" s="20">
         <v>8.5060430000000006E-2</v>
-      </c>
-      <c r="S1092" s="87">
-        <v>9.3450000000000006</v>
       </c>
       <c r="T1092" s="20"/>
       <c r="U1092" s="20"/>
@@ -59110,7 +59306,12 @@
         <v>1.2087290000000001E-2</v>
       </c>
       <c r="T1093" s="20"/>
-      <c r="U1093" s="20"/>
+      <c r="U1093" s="19">
+        <v>0.41957175925925921</v>
+      </c>
+      <c r="V1093" s="20">
+        <v>1.5942390000000001E-2</v>
+      </c>
       <c r="W1093" s="1" t="s">
         <v>212</v>
       </c>
@@ -59161,8 +59362,15 @@
       <c r="R1094" s="20">
         <v>1.661118E-2</v>
       </c>
-      <c r="T1094" s="20"/>
-      <c r="U1094" s="20"/>
+      <c r="T1094" s="63">
+        <v>0.5180555555555556</v>
+      </c>
+      <c r="U1094" s="19">
+        <v>0.42023148148148143</v>
+      </c>
+      <c r="V1094" s="20">
+        <v>1.5067260000000001E-2</v>
+      </c>
       <c r="W1094" s="1" t="s">
         <v>212</v>
       </c>
@@ -81764,7 +81972,12 @@
       <c r="T1600" s="63">
         <v>0.5180555555555556</v>
       </c>
-      <c r="U1600" s="20"/>
+      <c r="U1600" s="19">
+        <v>0.44604166666666667</v>
+      </c>
+      <c r="V1600" s="20">
+        <v>9.3209570000000005E-2</v>
+      </c>
       <c r="W1600" s="1" t="s">
         <v>212</v>
       </c>
@@ -81804,6 +82017,12 @@
       <c r="S1601" s="87">
         <v>8.673</v>
       </c>
+      <c r="U1601" s="19">
+        <v>0.44687499999999997</v>
+      </c>
+      <c r="V1601">
+        <v>0.13599749999999999</v>
+      </c>
       <c r="W1601" s="1" t="s">
         <v>212</v>
       </c>
@@ -81843,6 +82062,12 @@
       <c r="S1602" s="87">
         <v>6.7759999999999998</v>
       </c>
+      <c r="U1602" s="19">
+        <v>0.44778935185185187</v>
+      </c>
+      <c r="V1602">
+        <v>0.11902119999999999</v>
+      </c>
       <c r="W1602" s="1" t="s">
         <v>212</v>
       </c>
@@ -81882,6 +82107,12 @@
       <c r="S1603" s="87">
         <v>3.77</v>
       </c>
+      <c r="U1603" s="19">
+        <v>0.44856481481481486</v>
+      </c>
+      <c r="V1603" s="20">
+        <v>1.4868849999999999E-2</v>
+      </c>
       <c r="W1603" s="1" t="s">
         <v>212</v>
       </c>
@@ -81921,6 +82152,12 @@
       <c r="S1604" s="87">
         <v>6.7839999999999998</v>
       </c>
+      <c r="U1604" s="19">
+        <v>0.44930555555555557</v>
+      </c>
+      <c r="V1604">
+        <v>0.1134449</v>
+      </c>
       <c r="W1604" s="1" t="s">
         <v>212</v>
       </c>
@@ -81960,6 +82197,12 @@
       <c r="S1605" s="87">
         <v>2.6850000000000001</v>
       </c>
+      <c r="U1605" s="19">
+        <v>0.45019675925925928</v>
+      </c>
+      <c r="V1605">
+        <v>0.46991889999999997</v>
+      </c>
       <c r="W1605" s="1" t="s">
         <v>212</v>
       </c>
@@ -81999,6 +82242,12 @@
       <c r="S1606" s="87">
         <v>2.9350000000000001</v>
       </c>
+      <c r="U1606" s="19">
+        <v>0.45109953703703703</v>
+      </c>
+      <c r="V1606" s="20">
+        <v>6.4058210000000004E-2</v>
+      </c>
       <c r="W1606" s="1" t="s">
         <v>212</v>
       </c>
@@ -82038,6 +82287,12 @@
       <c r="S1607" s="87">
         <v>5.6710000000000003</v>
       </c>
+      <c r="U1607" s="19">
+        <v>0.45181712962962961</v>
+      </c>
+      <c r="V1607">
+        <v>0.37477969999999999</v>
+      </c>
       <c r="W1607" s="1" t="s">
         <v>212</v>
       </c>
@@ -82077,6 +82332,12 @@
       <c r="S1608" s="87">
         <v>1.998</v>
       </c>
+      <c r="U1608" s="19">
+        <v>0.45271990740740736</v>
+      </c>
+      <c r="V1608" s="20">
+        <v>1.549035E-2</v>
+      </c>
       <c r="W1608" s="1" t="s">
         <v>212</v>
       </c>
@@ -82116,6 +82377,12 @@
       <c r="S1609" s="87">
         <v>8.7219999999999995</v>
       </c>
+      <c r="U1609" s="19">
+        <v>0.45363425925925926</v>
+      </c>
+      <c r="V1609" s="20">
+        <v>9.6813510000000005E-2</v>
+      </c>
       <c r="W1609" s="1" t="s">
         <v>212</v>
       </c>
@@ -82155,6 +82422,12 @@
       <c r="S1610" s="87">
         <v>6.1420000000000003</v>
       </c>
+      <c r="U1610" s="19">
+        <v>0.45546296296296296</v>
+      </c>
+      <c r="V1610" s="20">
+        <v>9.0934639999999997E-2</v>
+      </c>
       <c r="W1610" s="1" t="s">
         <v>212</v>
       </c>
@@ -82194,6 +82467,12 @@
       <c r="S1611" s="87">
         <v>5.1260000000000003</v>
       </c>
+      <c r="U1611" s="19">
+        <v>0.45636574074074071</v>
+      </c>
+      <c r="V1611" s="20">
+        <v>6.2149749999999997E-2</v>
+      </c>
       <c r="W1611" s="1" t="s">
         <v>212</v>
       </c>
@@ -82233,6 +82512,12 @@
       <c r="S1612" s="87">
         <v>7.359</v>
       </c>
+      <c r="U1612" s="19">
+        <v>0.45710648148148153</v>
+      </c>
+      <c r="V1612">
+        <v>0.1052681</v>
+      </c>
       <c r="W1612" s="1" t="s">
         <v>212</v>
       </c>
@@ -82272,6 +82557,12 @@
       <c r="S1613" s="87">
         <v>5.1959999999999997</v>
       </c>
+      <c r="U1613" s="19">
+        <v>0.45788194444444441</v>
+      </c>
+      <c r="V1613">
+        <v>0.1244049</v>
+      </c>
       <c r="W1613" s="1" t="s">
         <v>212</v>
       </c>
@@ -82311,6 +82602,12 @@
       <c r="S1614" s="87">
         <v>5.8280000000000003</v>
       </c>
+      <c r="U1614" s="19">
+        <v>0.45869212962962963</v>
+      </c>
+      <c r="V1614">
+        <v>1.117494</v>
+      </c>
       <c r="W1614" s="1" t="s">
         <v>212</v>
       </c>
@@ -82350,6 +82647,12 @@
       <c r="S1615" s="87">
         <v>4.093</v>
       </c>
+      <c r="U1615" s="19">
+        <v>0.45973379629629635</v>
+      </c>
+      <c r="V1615" s="20">
+        <v>7.782994E-2</v>
+      </c>
       <c r="W1615" s="1" t="s">
         <v>212</v>
       </c>
@@ -82389,6 +82692,12 @@
       <c r="S1616" s="87">
         <v>6.2629999999999999</v>
       </c>
+      <c r="U1616" s="19">
+        <v>0.46069444444444446</v>
+      </c>
+      <c r="V1616">
+        <v>0.9872611</v>
+      </c>
       <c r="W1616" s="1" t="s">
         <v>212</v>
       </c>
@@ -82428,6 +82737,12 @@
       <c r="S1617" s="87">
         <v>5.2160000000000002</v>
       </c>
+      <c r="U1617" s="19">
+        <v>0.46166666666666667</v>
+      </c>
+      <c r="V1617">
+        <v>0.23556270000000001</v>
+      </c>
       <c r="W1617" s="1" t="s">
         <v>212</v>
       </c>
@@ -82467,6 +82782,12 @@
       <c r="S1618" s="87">
         <v>6.9880000000000004</v>
       </c>
+      <c r="U1618" s="19">
+        <v>0.46249999999999997</v>
+      </c>
+      <c r="V1618">
+        <v>0.51297680000000001</v>
+      </c>
       <c r="W1618" s="1" t="s">
         <v>212</v>
       </c>
@@ -82506,6 +82827,12 @@
       <c r="S1619" s="87">
         <v>4.9649999999999999</v>
       </c>
+      <c r="U1619" s="19">
+        <v>0.46340277777777777</v>
+      </c>
+      <c r="V1619" s="20">
+        <v>5.8423179999999998E-2</v>
+      </c>
       <c r="W1619" s="1" t="s">
         <v>212</v>
       </c>
@@ -82545,6 +82872,12 @@
       <c r="S1620" s="87">
         <v>6.9420000000000002</v>
       </c>
+      <c r="U1620" s="19">
+        <v>0.46429398148148149</v>
+      </c>
+      <c r="V1620">
+        <v>9.64671E-2</v>
+      </c>
       <c r="W1620" s="1" t="s">
         <v>212</v>
       </c>
@@ -82584,6 +82917,12 @@
       <c r="S1621" s="87">
         <v>1.736</v>
       </c>
+      <c r="U1621" s="19">
+        <v>0.46504629629629629</v>
+      </c>
+      <c r="V1621" s="20">
+        <v>1.7879260000000001E-2</v>
+      </c>
       <c r="W1621" s="1" t="s">
         <v>212</v>
       </c>
@@ -82623,6 +82962,12 @@
       <c r="S1622" s="87">
         <v>5.0460000000000003</v>
       </c>
+      <c r="U1622" s="19">
+        <v>0.46593749999999995</v>
+      </c>
+      <c r="V1622">
+        <v>0.2520657</v>
+      </c>
       <c r="W1622" s="1" t="s">
         <v>212</v>
       </c>
@@ -82662,6 +83007,12 @@
       <c r="S1623" s="87">
         <v>7.5359999999999996</v>
       </c>
+      <c r="U1623" s="19">
+        <v>0.46684027777777781</v>
+      </c>
+      <c r="V1623">
+        <v>1.203004</v>
+      </c>
       <c r="W1623" s="1" t="s">
         <v>212</v>
       </c>
@@ -82701,6 +83052,12 @@
       <c r="S1624" s="87">
         <v>5.4489999999999998</v>
       </c>
+      <c r="U1624" s="19">
+        <v>0.46784722222222225</v>
+      </c>
+      <c r="V1624">
+        <v>0.84870480000000004</v>
+      </c>
       <c r="W1624" s="1" t="s">
         <v>212</v>
       </c>
@@ -82766,6 +83123,12 @@
       <c r="T1626" s="63">
         <v>0.52152777777777781</v>
       </c>
+      <c r="U1626" s="19">
+        <v>0.46886574074074078</v>
+      </c>
+      <c r="V1626" s="20">
+        <v>1.257168E-2</v>
+      </c>
       <c r="W1626" s="1" t="s">
         <v>212</v>
       </c>
@@ -82798,6 +83161,12 @@
       <c r="T1627" s="63">
         <v>0.51388888888888895</v>
       </c>
+      <c r="U1627" s="19">
+        <v>0.44604166666666667</v>
+      </c>
+      <c r="V1627">
+        <v>0.1174973</v>
+      </c>
       <c r="W1627" s="1" t="s">
         <v>212</v>
       </c>
@@ -82837,6 +83206,12 @@
       <c r="S1628" s="87">
         <v>6.9889999999999999</v>
       </c>
+      <c r="U1628" s="19">
+        <v>0.44687499999999997</v>
+      </c>
+      <c r="V1628" s="20">
+        <v>5.6522969999999999E-2</v>
+      </c>
       <c r="W1628" s="1" t="s">
         <v>212</v>
       </c>
@@ -82876,6 +83251,12 @@
       <c r="S1629" s="87">
         <v>8.3729999999999993</v>
       </c>
+      <c r="U1629" s="19">
+        <v>0.44778935185185187</v>
+      </c>
+      <c r="V1629" s="20">
+        <v>3.9479239999999999E-2</v>
+      </c>
       <c r="W1629" s="1" t="s">
         <v>212</v>
       </c>
@@ -82915,6 +83296,12 @@
       <c r="S1630" s="87">
         <v>3.165</v>
       </c>
+      <c r="U1630" s="19">
+        <v>0.44856481481481486</v>
+      </c>
+      <c r="V1630">
+        <v>1.1658399999999999E-2</v>
+      </c>
       <c r="W1630" s="1" t="s">
         <v>212</v>
       </c>
@@ -82954,6 +83341,12 @@
       <c r="S1631" s="87">
         <v>9.5709999999999997</v>
       </c>
+      <c r="U1631" s="19">
+        <v>0.44930555555555557</v>
+      </c>
+      <c r="V1631">
+        <v>0.81870849999999995</v>
+      </c>
       <c r="W1631" s="1" t="s">
         <v>212</v>
       </c>
@@ -82993,6 +83386,12 @@
       <c r="S1632" s="87">
         <v>2.605</v>
       </c>
+      <c r="U1632" s="19">
+        <v>0.45019675925925928</v>
+      </c>
+      <c r="V1632" s="20">
+        <v>9.0578080000000005E-3</v>
+      </c>
       <c r="W1632" s="1" t="s">
         <v>212</v>
       </c>
@@ -83032,6 +83431,12 @@
       <c r="S1633" s="87">
         <v>6.2060000000000004</v>
       </c>
+      <c r="U1633" s="19">
+        <v>0.45109953703703703</v>
+      </c>
+      <c r="V1633" s="20">
+        <v>8.6133290000000001E-2</v>
+      </c>
       <c r="W1633" s="1" t="s">
         <v>212</v>
       </c>
@@ -83071,6 +83476,12 @@
       <c r="S1634" s="87">
         <v>4.6920000000000002</v>
       </c>
+      <c r="U1634" s="19">
+        <v>0.45181712962962961</v>
+      </c>
+      <c r="V1634" s="20">
+        <v>3.9451279999999998E-2</v>
+      </c>
       <c r="W1634" s="1" t="s">
         <v>212</v>
       </c>
@@ -83110,6 +83521,12 @@
       <c r="S1635" s="87">
         <v>3.1080000000000001</v>
       </c>
+      <c r="U1635" s="19">
+        <v>0.45271990740740736</v>
+      </c>
+      <c r="V1635">
+        <v>0.43016559999999998</v>
+      </c>
       <c r="W1635" s="1" t="s">
         <v>212</v>
       </c>
@@ -83149,6 +83566,12 @@
       <c r="S1636" s="87">
         <v>5.5510000000000002</v>
       </c>
+      <c r="U1636" s="19">
+        <v>0.45363425925925926</v>
+      </c>
+      <c r="V1636" s="20">
+        <v>3.3116010000000001E-2</v>
+      </c>
       <c r="W1636" s="1" t="s">
         <v>212</v>
       </c>
@@ -83188,6 +83611,12 @@
       <c r="S1637" s="87">
         <v>4.4669999999999996</v>
       </c>
+      <c r="U1637" s="19">
+        <v>0.45546296296296296</v>
+      </c>
+      <c r="V1637">
+        <v>0.89781010000000006</v>
+      </c>
       <c r="W1637" s="1" t="s">
         <v>212</v>
       </c>
@@ -83227,6 +83656,12 @@
       <c r="S1638" s="87">
         <v>5.7220000000000004</v>
       </c>
+      <c r="U1638" s="19">
+        <v>0.45636574074074071</v>
+      </c>
+      <c r="V1638" s="20">
+        <v>5.4538589999999998E-2</v>
+      </c>
       <c r="W1638" s="1" t="s">
         <v>212</v>
       </c>
@@ -83266,6 +83701,12 @@
       <c r="S1639" s="87">
         <v>2.702</v>
       </c>
+      <c r="U1639" s="19">
+        <v>0.45710648148148153</v>
+      </c>
+      <c r="V1639" s="20">
+        <v>9.3230889999999997E-3</v>
+      </c>
       <c r="W1639" s="1" t="s">
         <v>212</v>
       </c>
@@ -83305,6 +83746,12 @@
       <c r="S1640" s="87">
         <v>5.98</v>
       </c>
+      <c r="U1640" s="19">
+        <v>0.45788194444444441</v>
+      </c>
+      <c r="V1640" s="20">
+        <v>7.0371829999999996E-2</v>
+      </c>
       <c r="W1640" s="1" t="s">
         <v>212</v>
       </c>
@@ -83344,6 +83791,12 @@
       <c r="S1641" s="87">
         <v>7.1420000000000003</v>
       </c>
+      <c r="U1641" s="19">
+        <v>0.45869212962962963</v>
+      </c>
+      <c r="V1641">
+        <v>0.1145499</v>
+      </c>
       <c r="W1641" s="1" t="s">
         <v>212</v>
       </c>
@@ -83383,6 +83836,12 @@
       <c r="S1642" s="87">
         <v>3.8460000000000001</v>
       </c>
+      <c r="U1642" s="19">
+        <v>0.45973379629629635</v>
+      </c>
+      <c r="V1642" s="20">
+        <v>9.9351670000000003E-2</v>
+      </c>
       <c r="W1642" s="1" t="s">
         <v>212</v>
       </c>
@@ -83422,6 +83881,12 @@
       <c r="S1643" s="87">
         <v>4.28</v>
       </c>
+      <c r="U1643" s="19">
+        <v>0.46069444444444446</v>
+      </c>
+      <c r="V1643">
+        <v>0.39502120000000002</v>
+      </c>
       <c r="W1643" s="1" t="s">
         <v>212</v>
       </c>
@@ -83461,6 +83926,12 @@
       <c r="S1644" s="87">
         <v>7.7489999999999997</v>
       </c>
+      <c r="U1644" s="19">
+        <v>0.46166666666666667</v>
+      </c>
+      <c r="V1644">
+        <v>0.10963820000000001</v>
+      </c>
       <c r="W1644" s="1" t="s">
         <v>212</v>
       </c>
@@ -83500,6 +83971,12 @@
       <c r="S1645" s="87">
         <v>4.476</v>
       </c>
+      <c r="U1645" s="19">
+        <v>0.46249999999999997</v>
+      </c>
+      <c r="V1645" s="20">
+        <v>7.2324630000000001E-2</v>
+      </c>
       <c r="W1645" s="1" t="s">
         <v>212</v>
       </c>
@@ -83539,6 +84016,12 @@
       <c r="S1646" s="87">
         <v>2.1349999999999998</v>
       </c>
+      <c r="U1646" s="19">
+        <v>0.46340277777777777</v>
+      </c>
+      <c r="V1646">
+        <v>0.230986</v>
+      </c>
       <c r="W1646" s="1" t="s">
         <v>212</v>
       </c>
@@ -83578,6 +84061,12 @@
       <c r="S1647" s="87">
         <v>2.8079999999999998</v>
       </c>
+      <c r="U1647" s="19">
+        <v>0.46429398148148149</v>
+      </c>
+      <c r="V1647" s="20">
+        <v>4.6404639999999997E-2</v>
+      </c>
       <c r="W1647" s="1" t="s">
         <v>212</v>
       </c>
@@ -83617,6 +84106,12 @@
       <c r="S1648" s="87">
         <v>4.67</v>
       </c>
+      <c r="U1648" s="19">
+        <v>0.46504629629629629</v>
+      </c>
+      <c r="V1648">
+        <v>0.41907420000000001</v>
+      </c>
       <c r="W1648" s="1" t="s">
         <v>212</v>
       </c>
@@ -83656,6 +84151,12 @@
       <c r="S1649" s="87">
         <v>6.6849999999999996</v>
       </c>
+      <c r="U1649" s="19">
+        <v>0.46593749999999995</v>
+      </c>
+      <c r="V1649">
+        <v>0.67463059999999997</v>
+      </c>
       <c r="W1649" s="1" t="s">
         <v>212</v>
       </c>
@@ -83695,6 +84196,12 @@
       <c r="S1650" s="87">
         <v>7.4770000000000003</v>
       </c>
+      <c r="U1650" s="19">
+        <v>0.46684027777777781</v>
+      </c>
+      <c r="V1650" s="20">
+        <v>7.0690069999999994E-2</v>
+      </c>
       <c r="W1650" s="1" t="s">
         <v>212</v>
       </c>
@@ -83734,6 +84241,12 @@
       <c r="S1651" s="87">
         <v>3.2719999999999998</v>
       </c>
+      <c r="U1651" s="19">
+        <v>0.46784722222222225</v>
+      </c>
+      <c r="V1651" s="20">
+        <v>7.2633810000000002E-3</v>
+      </c>
       <c r="W1651" s="1" t="s">
         <v>212</v>
       </c>
@@ -83798,6 +84311,12 @@
       </c>
       <c r="T1653" s="63">
         <v>0.5180555555555556</v>
+      </c>
+      <c r="U1653" s="19">
+        <v>0.46886574074074078</v>
+      </c>
+      <c r="V1653" s="20">
+        <v>6.2113120000000001E-3</v>
       </c>
       <c r="W1653" s="1" t="s">
         <v>212</v>

</xml_diff>

<commit_message>
entered data for 2018-09-08 cohrot
</commit_message>
<xml_diff>
--- a/Data/2018-08-14_master_datac_2018_collection_year.xlsx
+++ b/Data/2018-08-14_master_datac_2018_collection_year.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andrew.nguyen\Desktop\Circadian_rhythm_runs_seasonal_timing\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE9C68FB-2867-4512-A747-FC1EDD497F93}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B85C67AC-E75E-4537-BDBC-9B421A1D79DC}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3345" yWindow="465" windowWidth="47520" windowHeight="26880" activeTab="1" xr2:uid="{C7477166-8A7C-B04A-9643-C277FEDCDAAB}"/>
   </bookViews>
@@ -16828,9 +16828,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92725FB9-1A17-2546-9DFA-6C0D39437891}">
   <dimension ref="A1:AV1968"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1627" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F1633" sqref="F1633"/>
+    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A1942" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AG1961" sqref="AG1961"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -91572,7 +91572,7 @@
         <v>1</v>
       </c>
       <c r="C1879" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G1879" s="1" t="s">
         <v>675</v>
@@ -91601,7 +91601,7 @@
         <v>2</v>
       </c>
       <c r="C1880" t="s">
-        <v>58</v>
+        <v>201</v>
       </c>
       <c r="G1880" s="1" t="s">
         <v>675</v>
@@ -91630,7 +91630,7 @@
         <v>3</v>
       </c>
       <c r="C1881" t="s">
-        <v>58</v>
+        <v>201</v>
       </c>
       <c r="G1881" s="1" t="s">
         <v>675</v>
@@ -91659,7 +91659,7 @@
         <v>4</v>
       </c>
       <c r="C1882" t="s">
-        <v>58</v>
+        <v>201</v>
       </c>
       <c r="G1882" s="1" t="s">
         <v>675</v>
@@ -91688,7 +91688,7 @@
         <v>5</v>
       </c>
       <c r="C1883" t="s">
-        <v>58</v>
+        <v>201</v>
       </c>
       <c r="G1883" s="1" t="s">
         <v>675</v>
@@ -91717,7 +91717,7 @@
         <v>6</v>
       </c>
       <c r="C1884" t="s">
-        <v>58</v>
+        <v>201</v>
       </c>
       <c r="G1884" s="1" t="s">
         <v>675</v>
@@ -91746,7 +91746,7 @@
         <v>7</v>
       </c>
       <c r="C1885" t="s">
-        <v>58</v>
+        <v>201</v>
       </c>
       <c r="G1885" s="1" t="s">
         <v>675</v>
@@ -92442,7 +92442,7 @@
         <v>1</v>
       </c>
       <c r="C1909" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G1909" s="1" t="s">
         <v>675</v>
@@ -92475,7 +92475,7 @@
         <v>2</v>
       </c>
       <c r="C1910" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G1910" s="1" t="s">
         <v>675</v>
@@ -92508,7 +92508,7 @@
         <v>3</v>
       </c>
       <c r="C1911" t="s">
-        <v>58</v>
+        <v>201</v>
       </c>
       <c r="G1911" s="1" t="s">
         <v>675</v>
@@ -92541,7 +92541,7 @@
         <v>4</v>
       </c>
       <c r="C1912" t="s">
-        <v>58</v>
+        <v>201</v>
       </c>
       <c r="G1912" s="1" t="s">
         <v>675</v>
@@ -92574,7 +92574,7 @@
         <v>5</v>
       </c>
       <c r="C1913" t="s">
-        <v>58</v>
+        <v>201</v>
       </c>
       <c r="G1913" s="1" t="s">
         <v>675</v>
@@ -92607,7 +92607,7 @@
         <v>6</v>
       </c>
       <c r="C1914" t="s">
-        <v>58</v>
+        <v>201</v>
       </c>
       <c r="G1914" s="1" t="s">
         <v>675</v>
@@ -92640,7 +92640,7 @@
         <v>7</v>
       </c>
       <c r="C1915" t="s">
-        <v>58</v>
+        <v>201</v>
       </c>
       <c r="G1915" s="1" t="s">
         <v>675</v>
@@ -93432,7 +93432,7 @@
         <v>1</v>
       </c>
       <c r="C1939" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G1939" s="1" t="s">
         <v>675</v>
@@ -93465,7 +93465,7 @@
         <v>2</v>
       </c>
       <c r="C1940" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G1940" s="1" t="s">
         <v>675</v>
@@ -93498,7 +93498,7 @@
         <v>3</v>
       </c>
       <c r="C1941" t="s">
-        <v>58</v>
+        <v>201</v>
       </c>
       <c r="G1941" s="1" t="s">
         <v>675</v>
@@ -93531,7 +93531,7 @@
         <v>4</v>
       </c>
       <c r="C1942" t="s">
-        <v>58</v>
+        <v>201</v>
       </c>
       <c r="G1942" s="1" t="s">
         <v>675</v>
@@ -93564,7 +93564,7 @@
         <v>5</v>
       </c>
       <c r="C1943" t="s">
-        <v>58</v>
+        <v>201</v>
       </c>
       <c r="G1943" s="1" t="s">
         <v>675</v>
@@ -93597,7 +93597,7 @@
         <v>6</v>
       </c>
       <c r="C1944" t="s">
-        <v>58</v>
+        <v>201</v>
       </c>
       <c r="G1944" s="1" t="s">
         <v>675</v>
@@ -93630,7 +93630,7 @@
         <v>7</v>
       </c>
       <c r="C1945" t="s">
-        <v>58</v>
+        <v>201</v>
       </c>
       <c r="G1945" s="1" t="s">
         <v>675</v>
@@ -93663,7 +93663,7 @@
         <v>8</v>
       </c>
       <c r="C1946" t="s">
-        <v>58</v>
+        <v>201</v>
       </c>
       <c r="G1946" s="1" t="s">
         <v>675</v>

</xml_diff>

<commit_message>
adding data for 2018-09-09 cohort day 10
</commit_message>
<xml_diff>
--- a/Data/2018-08-14_master_datac_2018_collection_year.xlsx
+++ b/Data/2018-08-14_master_datac_2018_collection_year.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hinalkharva\Desktop\Circadian_rhythm_runs_seasonal_timing\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andrew.nguyen\Desktop\Circadian_rhythm_runs_seasonal_timing\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84B6FC81-8E09-4776-A84B-8845B05E533F}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8869C439-C913-4234-94CF-DDC21AB4EC24}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3345" yWindow="465" windowWidth="47520" windowHeight="26880" activeTab="2" xr2:uid="{C7477166-8A7C-B04A-9643-C277FEDCDAAB}"/>
+    <workbookView xWindow="3345" yWindow="465" windowWidth="47520" windowHeight="26880" activeTab="1" xr2:uid="{C7477166-8A7C-B04A-9643-C277FEDCDAAB}"/>
   </bookViews>
   <sheets>
     <sheet name="Maggot_Collections" sheetId="2" r:id="rId1"/>
@@ -21,6 +21,11 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -16823,9 +16828,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92725FB9-1A17-2546-9DFA-6C0D39437891}">
   <dimension ref="A1:AV1968"/>
   <sheetViews>
-    <sheetView topLeftCell="U1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1942" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AG1961" sqref="AG1961"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A1191" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="U1216" sqref="U1216:V1217"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -60538,11 +60543,17 @@
         <v>0.1169152</v>
       </c>
       <c r="T1130" s="63"/>
+      <c r="U1130" s="19">
+        <v>0.28518518518518515</v>
+      </c>
+      <c r="V1130" s="20">
+        <v>8.8259749999999998E-2</v>
+      </c>
       <c r="W1130" s="1" t="s">
         <v>220</v>
       </c>
       <c r="AB1130" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="AC1130" t="s">
         <v>718</v>
@@ -60659,6 +60670,8 @@
       <c r="T1132" s="63">
         <v>0.52777777777777779</v>
       </c>
+      <c r="U1132" s="19"/>
+      <c r="V1132" s="20"/>
       <c r="W1132" s="1" t="s">
         <v>220</v>
       </c>
@@ -60721,6 +60734,12 @@
       <c r="S1133" s="87">
         <v>2.8969999999999998</v>
       </c>
+      <c r="U1133" s="19">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="V1133" s="20">
+        <v>7.064811E-2</v>
+      </c>
       <c r="W1133" s="1" t="s">
         <v>220</v>
       </c>
@@ -60899,6 +60918,12 @@
       <c r="S1136" s="87">
         <v>3.1379999999999999</v>
       </c>
+      <c r="U1136" s="19">
+        <v>0.2908101851851852</v>
+      </c>
+      <c r="V1136">
+        <v>0.2221012</v>
+      </c>
       <c r="W1136" s="1" t="s">
         <v>220</v>
       </c>
@@ -61194,6 +61219,12 @@
       <c r="S1141" s="87">
         <v>2.0470000000000002</v>
       </c>
+      <c r="U1141" s="19">
+        <v>0.29236111111111113</v>
+      </c>
+      <c r="V1141" s="20">
+        <v>7.8658240000000004E-3</v>
+      </c>
       <c r="W1141" s="1" t="s">
         <v>220</v>
       </c>
@@ -61317,6 +61348,12 @@
         <v>8</v>
       </c>
       <c r="T1143" s="20"/>
+      <c r="U1143" s="19">
+        <v>0.29310185185185184</v>
+      </c>
+      <c r="V1143">
+        <v>7.5259199999999998E-2</v>
+      </c>
       <c r="W1143" s="1" t="s">
         <v>220</v>
       </c>
@@ -61605,6 +61642,12 @@
       <c r="S1148" s="87">
         <v>3.88</v>
       </c>
+      <c r="U1148" s="19">
+        <v>0.29390046296296296</v>
+      </c>
+      <c r="V1148" s="20">
+        <v>5.8806270000000001E-2</v>
+      </c>
       <c r="W1148" s="1" t="s">
         <v>220</v>
       </c>
@@ -61728,6 +61771,12 @@
         <v>6.1630000000000003</v>
       </c>
       <c r="T1150" s="20"/>
+      <c r="U1150" s="19">
+        <v>0.29471064814814812</v>
+      </c>
+      <c r="V1150" s="20">
+        <v>8.6631570000000005E-2</v>
+      </c>
       <c r="W1150" s="1" t="s">
         <v>220</v>
       </c>
@@ -61850,6 +61899,12 @@
       <c r="S1152" s="87">
         <v>4.149</v>
       </c>
+      <c r="U1152" s="19">
+        <v>0.29554398148148148</v>
+      </c>
+      <c r="V1152">
+        <v>0.67529479999999997</v>
+      </c>
       <c r="W1152" s="1" t="s">
         <v>220</v>
       </c>
@@ -61912,6 +61967,12 @@
       <c r="S1153" s="87">
         <v>6.3120000000000003</v>
       </c>
+      <c r="U1153" s="19">
+        <v>0.29649305555555555</v>
+      </c>
+      <c r="V1153">
+        <v>0.586511</v>
+      </c>
       <c r="W1153" s="1" t="s">
         <v>220</v>
       </c>
@@ -62087,6 +62148,12 @@
       <c r="S1156" s="87">
         <v>6.3140000000000001</v>
       </c>
+      <c r="U1156" s="19">
+        <v>0.29738425925925926</v>
+      </c>
+      <c r="V1156">
+        <v>0.13185720000000001</v>
+      </c>
       <c r="W1156" s="1" t="s">
         <v>220</v>
       </c>
@@ -62443,6 +62510,12 @@
       <c r="S1162" s="87">
         <v>2.4129999999999998</v>
       </c>
+      <c r="U1162" s="19">
+        <v>0.29810185185185184</v>
+      </c>
+      <c r="V1162" s="20">
+        <v>9.1583540000000005E-2</v>
+      </c>
       <c r="W1162" s="1" t="s">
         <v>220</v>
       </c>
@@ -62506,6 +62579,12 @@
         <v>5.3970000000000002</v>
       </c>
       <c r="T1163" s="20"/>
+      <c r="U1163" s="19">
+        <v>0.29886574074074074</v>
+      </c>
+      <c r="V1163" s="20">
+        <v>3.7529680000000003E-2</v>
+      </c>
       <c r="W1163" s="1" t="s">
         <v>220</v>
       </c>
@@ -62568,6 +62647,12 @@
       <c r="S1164" s="87">
         <v>3.97</v>
       </c>
+      <c r="U1164" s="19">
+        <v>0.2996759259259259</v>
+      </c>
+      <c r="V1164" s="20">
+        <v>3.168812E-2</v>
+      </c>
       <c r="W1164" s="1" t="s">
         <v>220</v>
       </c>
@@ -62860,6 +62945,12 @@
         <v>4.0586750000000003E-3</v>
       </c>
       <c r="T1169" s="20"/>
+      <c r="U1169" s="19">
+        <v>0.30050925925925925</v>
+      </c>
+      <c r="V1169" s="20">
+        <v>5.0249099999999996E-3</v>
+      </c>
       <c r="W1169" s="1" t="s">
         <v>220</v>
       </c>
@@ -62910,7 +63001,15 @@
       <c r="R1170" s="20">
         <v>3.7804010000000001E-3</v>
       </c>
-      <c r="T1170" s="20"/>
+      <c r="T1170" s="63">
+        <v>0.53055555555555556</v>
+      </c>
+      <c r="U1170" s="19">
+        <v>0.30125000000000002</v>
+      </c>
+      <c r="V1170" s="20">
+        <v>4.7582750000000002E-3</v>
+      </c>
       <c r="W1170" s="1" t="s">
         <v>220</v>
       </c>
@@ -62973,6 +63072,12 @@
       <c r="T1171" s="63">
         <v>0.52500000000000002</v>
       </c>
+      <c r="U1171" s="19">
+        <v>0.28518518518518515</v>
+      </c>
+      <c r="V1171">
+        <v>0.1637787</v>
+      </c>
       <c r="W1171" s="1" t="s">
         <v>220</v>
       </c>
@@ -63212,6 +63317,12 @@
         <v>4.12</v>
       </c>
       <c r="T1175" s="20"/>
+      <c r="U1175" s="19">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="V1175">
+        <v>0.15038779999999999</v>
+      </c>
       <c r="W1175" s="1" t="s">
         <v>220</v>
       </c>
@@ -63675,6 +63786,12 @@
       <c r="S1183" s="87">
         <v>9.0749999999999993</v>
       </c>
+      <c r="U1183" s="19">
+        <v>0.2908101851851852</v>
+      </c>
+      <c r="V1183">
+        <v>0.12474150000000001</v>
+      </c>
       <c r="W1183" s="1" t="s">
         <v>220</v>
       </c>
@@ -63797,6 +63914,12 @@
       <c r="S1185" s="87">
         <v>6.5919999999999996</v>
       </c>
+      <c r="U1185" s="19">
+        <v>0.29158564814814814</v>
+      </c>
+      <c r="V1185">
+        <v>0.1101873</v>
+      </c>
       <c r="W1185" s="1" t="s">
         <v>220</v>
       </c>
@@ -64089,6 +64212,12 @@
       <c r="S1190" s="87">
         <v>7.3159999999999998</v>
       </c>
+      <c r="U1190" s="19">
+        <v>0.29236111111111113</v>
+      </c>
+      <c r="V1190" s="20">
+        <v>9.6880910000000001E-2</v>
+      </c>
       <c r="W1190" s="1" t="s">
         <v>220</v>
       </c>
@@ -64151,6 +64280,12 @@
       <c r="S1191" s="87">
         <v>5.6139999999999999</v>
       </c>
+      <c r="U1191" s="19">
+        <v>0.29310185185185184</v>
+      </c>
+      <c r="V1191">
+        <v>0.1355199</v>
+      </c>
       <c r="W1191" s="1" t="s">
         <v>220</v>
       </c>
@@ -64214,6 +64349,12 @@
         <v>2.3079999999999998</v>
       </c>
       <c r="T1192" s="20"/>
+      <c r="U1192" s="19">
+        <v>0.29390046296296296</v>
+      </c>
+      <c r="V1192" s="20">
+        <v>1.9534429999999998E-2</v>
+      </c>
       <c r="W1192" s="1" t="s">
         <v>220</v>
       </c>
@@ -64276,6 +64417,12 @@
       <c r="S1193" s="87">
         <v>5.5309999999999997</v>
       </c>
+      <c r="U1193" s="19">
+        <v>0.29471064814814812</v>
+      </c>
+      <c r="V1193">
+        <v>0.1271833</v>
+      </c>
       <c r="W1193" s="1" t="s">
         <v>220</v>
       </c>
@@ -64395,6 +64542,12 @@
         <v>4.9580000000000002</v>
       </c>
       <c r="T1195" s="20"/>
+      <c r="U1195" s="19">
+        <v>0.29554398148148148</v>
+      </c>
+      <c r="V1195" s="20">
+        <v>8.3964819999999996E-2</v>
+      </c>
       <c r="W1195" s="1" t="s">
         <v>220</v>
       </c>
@@ -64576,6 +64729,12 @@
         <v>7.0359999999999996</v>
       </c>
       <c r="T1198" s="20"/>
+      <c r="U1198" s="19">
+        <v>0.29649305555555555</v>
+      </c>
+      <c r="V1198" s="20">
+        <v>9.8087060000000004E-2</v>
+      </c>
       <c r="W1198" s="1" t="s">
         <v>220</v>
       </c>
@@ -64696,6 +64855,12 @@
         <v>6.3949999999999996</v>
       </c>
       <c r="T1200" s="20"/>
+      <c r="U1200" s="19">
+        <v>0.29738425925925926</v>
+      </c>
+      <c r="V1200" s="20">
+        <v>5.0724940000000003E-2</v>
+      </c>
       <c r="W1200" s="1" t="s">
         <v>220</v>
       </c>
@@ -64931,6 +65096,12 @@
       <c r="S1204" s="87">
         <v>4.54</v>
       </c>
+      <c r="U1204" s="19">
+        <v>0.29810185185185184</v>
+      </c>
+      <c r="V1204">
+        <v>6.1870099999999997E-2</v>
+      </c>
       <c r="W1204" s="1" t="s">
         <v>220</v>
       </c>
@@ -65050,6 +65221,12 @@
       <c r="S1206" s="87">
         <v>5.68</v>
       </c>
+      <c r="U1206" s="19">
+        <v>0.29886574074074074</v>
+      </c>
+      <c r="V1206">
+        <v>0.18514829999999999</v>
+      </c>
       <c r="W1206" s="1" t="s">
         <v>220</v>
       </c>
@@ -65283,6 +65460,12 @@
       <c r="S1210" s="87">
         <v>6.5149999999999997</v>
       </c>
+      <c r="U1210" s="19">
+        <v>0.2996759259259259</v>
+      </c>
+      <c r="V1210">
+        <v>5.1410600000000001E-2</v>
+      </c>
       <c r="W1210" s="1" t="s">
         <v>220</v>
       </c>
@@ -65406,7 +65589,12 @@
         <v>3.9460000000000002</v>
       </c>
       <c r="T1212" s="20"/>
-      <c r="U1212" s="20"/>
+      <c r="U1212" s="19">
+        <v>0.30050925925925925</v>
+      </c>
+      <c r="V1212" s="20">
+        <v>5.1963009999999997E-2</v>
+      </c>
       <c r="W1212" s="1" t="s">
         <v>220</v>
       </c>
@@ -65637,7 +65825,12 @@
         <v>1.033865E-2</v>
       </c>
       <c r="T1216" s="20"/>
-      <c r="U1216" s="20"/>
+      <c r="U1216" s="19">
+        <v>0.30125000000000002</v>
+      </c>
+      <c r="V1216" s="20">
+        <v>1.482967E-2</v>
+      </c>
       <c r="W1216" s="1" t="s">
         <v>220</v>
       </c>
@@ -65691,7 +65884,12 @@
       <c r="T1217" s="63">
         <v>0.53055555555555556</v>
       </c>
-      <c r="U1217" s="20"/>
+      <c r="U1217" s="19">
+        <v>0.30185185185185187</v>
+      </c>
+      <c r="V1217" s="20">
+        <v>1.9692950000000001E-2</v>
+      </c>
       <c r="W1217" s="1" t="s">
         <v>220</v>
       </c>
@@ -81955,6 +82153,9 @@
       </c>
       <c r="K1600" t="s">
         <v>60</v>
+      </c>
+      <c r="L1600">
+        <v>6262</v>
       </c>
       <c r="M1600" s="19"/>
       <c r="N1600" s="20"/>
@@ -82009,6 +82210,9 @@
       <c r="K1601" t="s">
         <v>60</v>
       </c>
+      <c r="L1601">
+        <v>6262</v>
+      </c>
       <c r="S1601" s="87">
         <v>8.673</v>
       </c>
@@ -82054,6 +82258,9 @@
       <c r="K1602" t="s">
         <v>60</v>
       </c>
+      <c r="L1602">
+        <v>6262</v>
+      </c>
       <c r="S1602" s="87">
         <v>6.7759999999999998</v>
       </c>
@@ -82099,6 +82306,9 @@
       <c r="K1603" t="s">
         <v>60</v>
       </c>
+      <c r="L1603">
+        <v>6262</v>
+      </c>
       <c r="S1603" s="87">
         <v>3.77</v>
       </c>
@@ -82144,6 +82354,9 @@
       <c r="K1604" t="s">
         <v>60</v>
       </c>
+      <c r="L1604">
+        <v>6262</v>
+      </c>
       <c r="S1604" s="87">
         <v>6.7839999999999998</v>
       </c>
@@ -82189,6 +82402,9 @@
       <c r="K1605" t="s">
         <v>60</v>
       </c>
+      <c r="L1605">
+        <v>6262</v>
+      </c>
       <c r="S1605" s="87">
         <v>2.6850000000000001</v>
       </c>
@@ -82234,6 +82450,9 @@
       <c r="K1606" t="s">
         <v>60</v>
       </c>
+      <c r="L1606">
+        <v>6262</v>
+      </c>
       <c r="S1606" s="87">
         <v>2.9350000000000001</v>
       </c>
@@ -82279,6 +82498,9 @@
       <c r="K1607" t="s">
         <v>60</v>
       </c>
+      <c r="L1607">
+        <v>6262</v>
+      </c>
       <c r="S1607" s="87">
         <v>5.6710000000000003</v>
       </c>
@@ -82324,6 +82546,9 @@
       <c r="K1608" t="s">
         <v>60</v>
       </c>
+      <c r="L1608">
+        <v>6262</v>
+      </c>
       <c r="S1608" s="87">
         <v>1.998</v>
       </c>
@@ -82369,6 +82594,9 @@
       <c r="K1609" t="s">
         <v>60</v>
       </c>
+      <c r="L1609">
+        <v>6262</v>
+      </c>
       <c r="S1609" s="87">
         <v>8.7219999999999995</v>
       </c>
@@ -82414,6 +82642,9 @@
       <c r="K1610" t="s">
         <v>60</v>
       </c>
+      <c r="L1610">
+        <v>6262</v>
+      </c>
       <c r="S1610" s="87">
         <v>6.1420000000000003</v>
       </c>
@@ -82459,6 +82690,9 @@
       <c r="K1611" t="s">
         <v>60</v>
       </c>
+      <c r="L1611">
+        <v>6262</v>
+      </c>
       <c r="S1611" s="87">
         <v>5.1260000000000003</v>
       </c>
@@ -82504,6 +82738,9 @@
       <c r="K1612" t="s">
         <v>60</v>
       </c>
+      <c r="L1612">
+        <v>6262</v>
+      </c>
       <c r="S1612" s="87">
         <v>7.359</v>
       </c>
@@ -82549,6 +82786,9 @@
       <c r="K1613" t="s">
         <v>60</v>
       </c>
+      <c r="L1613">
+        <v>6262</v>
+      </c>
       <c r="S1613" s="87">
         <v>5.1959999999999997</v>
       </c>
@@ -82594,6 +82834,9 @@
       <c r="K1614" t="s">
         <v>60</v>
       </c>
+      <c r="L1614">
+        <v>6262</v>
+      </c>
       <c r="S1614" s="87">
         <v>5.8280000000000003</v>
       </c>
@@ -82639,6 +82882,9 @@
       <c r="K1615" t="s">
         <v>60</v>
       </c>
+      <c r="L1615">
+        <v>6262</v>
+      </c>
       <c r="S1615" s="87">
         <v>4.093</v>
       </c>
@@ -82684,6 +82930,9 @@
       <c r="K1616" t="s">
         <v>60</v>
       </c>
+      <c r="L1616">
+        <v>6262</v>
+      </c>
       <c r="S1616" s="87">
         <v>6.2629999999999999</v>
       </c>
@@ -82729,6 +82978,9 @@
       <c r="K1617" t="s">
         <v>60</v>
       </c>
+      <c r="L1617">
+        <v>6262</v>
+      </c>
       <c r="S1617" s="87">
         <v>5.2160000000000002</v>
       </c>
@@ -82774,6 +83026,9 @@
       <c r="K1618" t="s">
         <v>60</v>
       </c>
+      <c r="L1618">
+        <v>6262</v>
+      </c>
       <c r="S1618" s="87">
         <v>6.9880000000000004</v>
       </c>
@@ -82819,6 +83074,9 @@
       <c r="K1619" t="s">
         <v>60</v>
       </c>
+      <c r="L1619">
+        <v>6262</v>
+      </c>
       <c r="S1619" s="87">
         <v>4.9649999999999999</v>
       </c>
@@ -82864,6 +83122,9 @@
       <c r="K1620" t="s">
         <v>60</v>
       </c>
+      <c r="L1620">
+        <v>6262</v>
+      </c>
       <c r="S1620" s="87">
         <v>6.9420000000000002</v>
       </c>
@@ -82909,6 +83170,9 @@
       <c r="K1621" t="s">
         <v>60</v>
       </c>
+      <c r="L1621">
+        <v>6262</v>
+      </c>
       <c r="S1621" s="87">
         <v>1.736</v>
       </c>
@@ -82954,6 +83218,9 @@
       <c r="K1622" t="s">
         <v>60</v>
       </c>
+      <c r="L1622">
+        <v>6262</v>
+      </c>
       <c r="S1622" s="87">
         <v>5.0460000000000003</v>
       </c>
@@ -82999,6 +83266,9 @@
       <c r="K1623" t="s">
         <v>60</v>
       </c>
+      <c r="L1623">
+        <v>6262</v>
+      </c>
       <c r="S1623" s="87">
         <v>7.5359999999999996</v>
       </c>
@@ -83044,6 +83314,9 @@
       <c r="K1624" t="s">
         <v>60</v>
       </c>
+      <c r="L1624">
+        <v>6262</v>
+      </c>
       <c r="S1624" s="87">
         <v>5.4489999999999998</v>
       </c>
@@ -83089,6 +83362,9 @@
       <c r="K1625" t="s">
         <v>60</v>
       </c>
+      <c r="L1625">
+        <v>6262</v>
+      </c>
       <c r="W1625" s="1" t="s">
         <v>212</v>
       </c>
@@ -83115,6 +83391,9 @@
       <c r="K1626" t="s">
         <v>60</v>
       </c>
+      <c r="L1626">
+        <v>6262</v>
+      </c>
       <c r="T1626" s="63">
         <v>0.52152777777777781</v>
       </c>
@@ -83150,6 +83429,9 @@
       <c r="K1627" t="s">
         <v>60</v>
       </c>
+      <c r="L1627">
+        <v>7000</v>
+      </c>
       <c r="S1627" s="87">
         <v>7.5780000000000003</v>
       </c>
@@ -83198,6 +83480,9 @@
       <c r="K1628" t="s">
         <v>60</v>
       </c>
+      <c r="L1628">
+        <v>7000</v>
+      </c>
       <c r="S1628" s="87">
         <v>6.9889999999999999</v>
       </c>
@@ -83243,6 +83528,9 @@
       <c r="K1629" t="s">
         <v>60</v>
       </c>
+      <c r="L1629">
+        <v>7000</v>
+      </c>
       <c r="S1629" s="87">
         <v>8.3729999999999993</v>
       </c>
@@ -83288,6 +83576,9 @@
       <c r="K1630" t="s">
         <v>60</v>
       </c>
+      <c r="L1630">
+        <v>7000</v>
+      </c>
       <c r="S1630" s="87">
         <v>3.165</v>
       </c>
@@ -83333,6 +83624,9 @@
       <c r="K1631" t="s">
         <v>60</v>
       </c>
+      <c r="L1631">
+        <v>7000</v>
+      </c>
       <c r="S1631" s="87">
         <v>9.5709999999999997</v>
       </c>
@@ -83378,6 +83672,9 @@
       <c r="K1632" t="s">
         <v>60</v>
       </c>
+      <c r="L1632">
+        <v>7000</v>
+      </c>
       <c r="S1632" s="87">
         <v>2.605</v>
       </c>
@@ -83423,6 +83720,9 @@
       <c r="K1633" t="s">
         <v>60</v>
       </c>
+      <c r="L1633">
+        <v>7000</v>
+      </c>
       <c r="S1633" s="87">
         <v>6.2060000000000004</v>
       </c>
@@ -83468,6 +83768,9 @@
       <c r="K1634" t="s">
         <v>60</v>
       </c>
+      <c r="L1634">
+        <v>7000</v>
+      </c>
       <c r="S1634" s="87">
         <v>4.6920000000000002</v>
       </c>
@@ -83513,6 +83816,9 @@
       <c r="K1635" t="s">
         <v>60</v>
       </c>
+      <c r="L1635">
+        <v>7000</v>
+      </c>
       <c r="S1635" s="87">
         <v>3.1080000000000001</v>
       </c>
@@ -83558,6 +83864,9 @@
       <c r="K1636" t="s">
         <v>60</v>
       </c>
+      <c r="L1636">
+        <v>7000</v>
+      </c>
       <c r="S1636" s="87">
         <v>5.5510000000000002</v>
       </c>
@@ -83603,6 +83912,9 @@
       <c r="K1637" t="s">
         <v>60</v>
       </c>
+      <c r="L1637">
+        <v>7000</v>
+      </c>
       <c r="S1637" s="87">
         <v>4.4669999999999996</v>
       </c>
@@ -83648,6 +83960,9 @@
       <c r="K1638" t="s">
         <v>60</v>
       </c>
+      <c r="L1638">
+        <v>7000</v>
+      </c>
       <c r="S1638" s="87">
         <v>5.7220000000000004</v>
       </c>
@@ -83693,6 +84008,9 @@
       <c r="K1639" t="s">
         <v>60</v>
       </c>
+      <c r="L1639">
+        <v>7000</v>
+      </c>
       <c r="S1639" s="87">
         <v>2.702</v>
       </c>
@@ -83738,6 +84056,9 @@
       <c r="K1640" t="s">
         <v>60</v>
       </c>
+      <c r="L1640">
+        <v>7000</v>
+      </c>
       <c r="S1640" s="87">
         <v>5.98</v>
       </c>
@@ -83783,6 +84104,9 @@
       <c r="K1641" t="s">
         <v>60</v>
       </c>
+      <c r="L1641">
+        <v>7000</v>
+      </c>
       <c r="S1641" s="87">
         <v>7.1420000000000003</v>
       </c>
@@ -83828,6 +84152,9 @@
       <c r="K1642" t="s">
         <v>60</v>
       </c>
+      <c r="L1642">
+        <v>7000</v>
+      </c>
       <c r="S1642" s="87">
         <v>3.8460000000000001</v>
       </c>
@@ -83873,6 +84200,9 @@
       <c r="K1643" t="s">
         <v>60</v>
       </c>
+      <c r="L1643">
+        <v>7000</v>
+      </c>
       <c r="S1643" s="87">
         <v>4.28</v>
       </c>
@@ -83918,6 +84248,9 @@
       <c r="K1644" t="s">
         <v>60</v>
       </c>
+      <c r="L1644">
+        <v>7000</v>
+      </c>
       <c r="S1644" s="87">
         <v>7.7489999999999997</v>
       </c>
@@ -83963,6 +84296,9 @@
       <c r="K1645" t="s">
         <v>60</v>
       </c>
+      <c r="L1645">
+        <v>7000</v>
+      </c>
       <c r="S1645" s="87">
         <v>4.476</v>
       </c>
@@ -84008,6 +84344,9 @@
       <c r="K1646" t="s">
         <v>60</v>
       </c>
+      <c r="L1646">
+        <v>7000</v>
+      </c>
       <c r="S1646" s="87">
         <v>2.1349999999999998</v>
       </c>
@@ -84053,6 +84392,9 @@
       <c r="K1647" t="s">
         <v>60</v>
       </c>
+      <c r="L1647">
+        <v>7000</v>
+      </c>
       <c r="S1647" s="87">
         <v>2.8079999999999998</v>
       </c>
@@ -84098,6 +84440,9 @@
       <c r="K1648" t="s">
         <v>60</v>
       </c>
+      <c r="L1648">
+        <v>7000</v>
+      </c>
       <c r="S1648" s="87">
         <v>4.67</v>
       </c>
@@ -84143,6 +84488,9 @@
       <c r="K1649" t="s">
         <v>60</v>
       </c>
+      <c r="L1649">
+        <v>7000</v>
+      </c>
       <c r="S1649" s="87">
         <v>6.6849999999999996</v>
       </c>
@@ -84188,6 +84536,9 @@
       <c r="K1650" t="s">
         <v>60</v>
       </c>
+      <c r="L1650">
+        <v>7000</v>
+      </c>
       <c r="S1650" s="87">
         <v>7.4770000000000003</v>
       </c>
@@ -84233,6 +84584,9 @@
       <c r="K1651" t="s">
         <v>60</v>
       </c>
+      <c r="L1651">
+        <v>7000</v>
+      </c>
       <c r="S1651" s="87">
         <v>3.2719999999999998</v>
       </c>
@@ -84278,6 +84632,9 @@
       <c r="K1652" t="s">
         <v>60</v>
       </c>
+      <c r="L1652">
+        <v>7000</v>
+      </c>
       <c r="W1652" s="1" t="s">
         <v>212</v>
       </c>
@@ -84304,6 +84661,9 @@
       <c r="K1653" t="s">
         <v>60</v>
       </c>
+      <c r="L1653">
+        <v>7000</v>
+      </c>
       <c r="T1653" s="63">
         <v>0.5180555555555556</v>
       </c>
@@ -84339,11 +84699,20 @@
       <c r="K1654" t="s">
         <v>60</v>
       </c>
+      <c r="L1654">
+        <v>6262</v>
+      </c>
       <c r="S1654" s="87">
         <v>3.0219999999999998</v>
       </c>
       <c r="T1654" s="63">
         <v>0.4861111111111111</v>
+      </c>
+      <c r="U1654" s="19">
+        <v>0.32047453703703704</v>
+      </c>
+      <c r="V1654">
+        <v>0.65574949999999999</v>
       </c>
       <c r="AB1654" t="s">
         <v>86</v>
@@ -84378,8 +84747,17 @@
       <c r="K1655" t="s">
         <v>60</v>
       </c>
+      <c r="L1655">
+        <v>6262</v>
+      </c>
       <c r="S1655" s="87">
         <v>3.5630000000000002</v>
+      </c>
+      <c r="U1655" s="19">
+        <v>0.32142361111111112</v>
+      </c>
+      <c r="V1655">
+        <v>0.5947249</v>
       </c>
       <c r="AB1655" t="s">
         <v>85</v>
@@ -84414,8 +84792,17 @@
       <c r="K1656" t="s">
         <v>60</v>
       </c>
+      <c r="L1656">
+        <v>6262</v>
+      </c>
       <c r="S1656" s="87">
         <v>4.5730000000000004</v>
+      </c>
+      <c r="U1656" s="19">
+        <v>0.3222800925925926</v>
+      </c>
+      <c r="V1656">
+        <v>1.5405660000000001</v>
       </c>
       <c r="AB1656" t="s">
         <v>86</v>
@@ -84450,8 +84837,17 @@
       <c r="K1657" t="s">
         <v>60</v>
       </c>
+      <c r="L1657">
+        <v>6262</v>
+      </c>
       <c r="S1657" s="87">
         <v>7.3789999999999996</v>
+      </c>
+      <c r="U1657" s="19">
+        <v>0.32321759259259258</v>
+      </c>
+      <c r="V1657" s="20">
+        <v>7.6117080000000004E-2</v>
       </c>
       <c r="AB1657" t="s">
         <v>85</v>
@@ -84486,8 +84882,17 @@
       <c r="K1658" t="s">
         <v>60</v>
       </c>
+      <c r="L1658">
+        <v>6262</v>
+      </c>
       <c r="S1658" s="87">
         <v>2.367</v>
+      </c>
+      <c r="U1658" s="19">
+        <v>0.32405092592592594</v>
+      </c>
+      <c r="V1658">
+        <v>0.85802210000000001</v>
       </c>
       <c r="AB1658" t="s">
         <v>86</v>
@@ -84522,8 +84927,17 @@
       <c r="K1659" t="s">
         <v>60</v>
       </c>
+      <c r="L1659">
+        <v>6262</v>
+      </c>
       <c r="S1659" s="87">
         <v>6.0629999999999997</v>
+      </c>
+      <c r="U1659" s="19">
+        <v>0.32502314814814814</v>
+      </c>
+      <c r="V1659">
+        <v>0.21130589999999999</v>
       </c>
       <c r="AB1659" t="s">
         <v>86</v>
@@ -84558,8 +84972,17 @@
       <c r="K1660" t="s">
         <v>60</v>
       </c>
+      <c r="L1660">
+        <v>6262</v>
+      </c>
       <c r="S1660" s="87">
         <v>3.5779999999999998</v>
+      </c>
+      <c r="U1660" s="19">
+        <v>0.32586805555555554</v>
+      </c>
+      <c r="V1660">
+        <v>1.058891</v>
       </c>
       <c r="AB1660" t="s">
         <v>85</v>
@@ -84594,8 +85017,17 @@
       <c r="K1661" t="s">
         <v>60</v>
       </c>
+      <c r="L1661">
+        <v>6262</v>
+      </c>
       <c r="S1661" s="87">
         <v>2.194</v>
+      </c>
+      <c r="U1661" s="19">
+        <v>0.32679398148148148</v>
+      </c>
+      <c r="V1661" s="20">
+        <v>2.9777540000000002E-2</v>
       </c>
       <c r="AB1661" t="s">
         <v>85</v>
@@ -84630,8 +85062,17 @@
       <c r="K1662" t="s">
         <v>60</v>
       </c>
+      <c r="L1662">
+        <v>6262</v>
+      </c>
       <c r="S1662" s="87">
         <v>2.5870000000000002</v>
+      </c>
+      <c r="U1662" s="19">
+        <v>0.3275925925925926</v>
+      </c>
+      <c r="V1662" s="20">
+        <v>2.403307E-2</v>
       </c>
       <c r="AB1662" t="s">
         <v>86</v>
@@ -84666,8 +85107,17 @@
       <c r="K1663" t="s">
         <v>60</v>
       </c>
+      <c r="L1663">
+        <v>6262</v>
+      </c>
       <c r="S1663" s="87">
         <v>3.8879999999999999</v>
+      </c>
+      <c r="U1663" s="19">
+        <v>0.32829861111111108</v>
+      </c>
+      <c r="V1663">
+        <v>0.2507915</v>
       </c>
       <c r="AB1663" t="s">
         <v>85</v>
@@ -84702,8 +85152,17 @@
       <c r="K1664" t="s">
         <v>60</v>
       </c>
+      <c r="L1664">
+        <v>6262</v>
+      </c>
       <c r="S1664" s="87">
         <v>5.8230000000000004</v>
+      </c>
+      <c r="U1664" s="19">
+        <v>0.32931712962962961</v>
+      </c>
+      <c r="V1664" s="20">
+        <v>8.6504880000000006E-2</v>
       </c>
       <c r="AB1664" t="s">
         <v>85</v>
@@ -84738,8 +85197,17 @@
       <c r="K1665" t="s">
         <v>60</v>
       </c>
+      <c r="L1665">
+        <v>6262</v>
+      </c>
       <c r="S1665" s="87">
         <v>5.6379999999999999</v>
+      </c>
+      <c r="U1665" s="19">
+        <v>0.33011574074074074</v>
+      </c>
+      <c r="V1665">
+        <v>0.2042176</v>
       </c>
       <c r="AB1665" t="s">
         <v>86</v>
@@ -84774,8 +85242,17 @@
       <c r="K1666" t="s">
         <v>60</v>
       </c>
+      <c r="L1666">
+        <v>6262</v>
+      </c>
       <c r="S1666" s="87">
         <v>2.504</v>
+      </c>
+      <c r="U1666" s="19">
+        <v>0.33099537037037036</v>
+      </c>
+      <c r="V1666" s="20">
+        <v>2.2886340000000002E-2</v>
       </c>
       <c r="AB1666" t="s">
         <v>85</v>
@@ -84810,8 +85287,17 @@
       <c r="K1667" t="s">
         <v>60</v>
       </c>
+      <c r="L1667">
+        <v>6262</v>
+      </c>
       <c r="S1667" s="87">
         <v>6.1109999999999998</v>
+      </c>
+      <c r="U1667" s="19">
+        <v>0.33172453703703703</v>
+      </c>
+      <c r="V1667">
+        <v>0.1403421</v>
       </c>
       <c r="AB1667" t="s">
         <v>85</v>
@@ -84846,8 +85332,17 @@
       <c r="K1668" t="s">
         <v>60</v>
       </c>
+      <c r="L1668">
+        <v>6262</v>
+      </c>
       <c r="S1668" s="87">
         <v>6.6639999999999997</v>
+      </c>
+      <c r="U1668" s="19">
+        <v>0.33260416666666665</v>
+      </c>
+      <c r="V1668">
+        <v>0.98356949999999999</v>
       </c>
       <c r="AB1668" t="s">
         <v>86</v>
@@ -84882,8 +85377,17 @@
       <c r="K1669" t="s">
         <v>60</v>
       </c>
+      <c r="L1669">
+        <v>6262</v>
+      </c>
       <c r="S1669" s="87">
         <v>5.9770000000000003</v>
+      </c>
+      <c r="U1669" s="19">
+        <v>0.33358796296296295</v>
+      </c>
+      <c r="V1669" s="20">
+        <v>9.4141130000000003E-2</v>
       </c>
       <c r="AB1669" t="s">
         <v>86</v>
@@ -84918,8 +85422,17 @@
       <c r="K1670" t="s">
         <v>60</v>
       </c>
+      <c r="L1670">
+        <v>6262</v>
+      </c>
       <c r="S1670" s="87">
         <v>2.0649999999999999</v>
+      </c>
+      <c r="U1670" s="19">
+        <v>0.33437500000000003</v>
+      </c>
+      <c r="V1670" s="20">
+        <v>2.1459450000000001E-2</v>
       </c>
       <c r="AB1670" t="s">
         <v>86</v>
@@ -84954,15 +85467,24 @@
       <c r="K1671" t="s">
         <v>60</v>
       </c>
+      <c r="L1671">
+        <v>6262</v>
+      </c>
       <c r="S1671" s="87">
         <v>5.3739999999999997</v>
       </c>
+      <c r="U1671" s="19">
+        <v>0.33509259259259255</v>
+      </c>
+      <c r="V1671">
+        <v>0.40442080000000002</v>
+      </c>
       <c r="AB1671" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="AC1671" t="str">
         <f t="shared" si="27"/>
-        <v>A20-10RT-A11</v>
+        <v>A20-10SO-A11</v>
       </c>
       <c r="AF1671" t="s">
         <v>237</v>
@@ -84990,8 +85512,17 @@
       <c r="K1672" t="s">
         <v>60</v>
       </c>
+      <c r="L1672">
+        <v>6262</v>
+      </c>
       <c r="S1672" s="87">
         <v>4.9050000000000002</v>
+      </c>
+      <c r="U1672" s="19">
+        <v>0.33594907407407404</v>
+      </c>
+      <c r="V1672">
+        <v>0.79653220000000002</v>
       </c>
       <c r="AB1672" t="s">
         <v>86</v>
@@ -85026,8 +85557,17 @@
       <c r="K1673" t="s">
         <v>60</v>
       </c>
+      <c r="L1673">
+        <v>6262</v>
+      </c>
       <c r="S1673" s="87">
         <v>3.8660000000000001</v>
+      </c>
+      <c r="U1673" s="19">
+        <v>0.33709490740740744</v>
+      </c>
+      <c r="V1673">
+        <v>0.1230131</v>
       </c>
       <c r="AB1673" t="s">
         <v>85</v>
@@ -85062,8 +85602,17 @@
       <c r="K1674" t="s">
         <v>60</v>
       </c>
+      <c r="L1674">
+        <v>6262</v>
+      </c>
       <c r="S1674" s="87">
         <v>6.6260000000000003</v>
+      </c>
+      <c r="U1674" s="19">
+        <v>0.33788194444444447</v>
+      </c>
+      <c r="V1674">
+        <v>0.1022102</v>
       </c>
       <c r="AB1674" t="s">
         <v>86</v>
@@ -85098,8 +85647,17 @@
       <c r="K1675" t="s">
         <v>60</v>
       </c>
+      <c r="L1675">
+        <v>6262</v>
+      </c>
       <c r="S1675" s="87">
         <v>5.0199999999999996</v>
+      </c>
+      <c r="U1675" s="19">
+        <v>0.33872685185185186</v>
+      </c>
+      <c r="V1675">
+        <v>0.74740309999999999</v>
       </c>
       <c r="AB1675" t="s">
         <v>85</v>
@@ -85134,8 +85692,17 @@
       <c r="K1676" t="s">
         <v>60</v>
       </c>
+      <c r="L1676">
+        <v>6262</v>
+      </c>
       <c r="S1676" s="87">
         <v>4.165</v>
+      </c>
+      <c r="U1676" s="19">
+        <v>0.33969907407407413</v>
+      </c>
+      <c r="V1676">
+        <v>9.7701099999999999E-2</v>
       </c>
       <c r="AB1676" t="s">
         <v>86</v>
@@ -85170,8 +85737,17 @@
       <c r="K1677" t="s">
         <v>60</v>
       </c>
+      <c r="L1677">
+        <v>6262</v>
+      </c>
       <c r="S1677" s="87">
         <v>3.3660000000000001</v>
+      </c>
+      <c r="U1677" s="19">
+        <v>0.34046296296296297</v>
+      </c>
+      <c r="V1677">
+        <v>0.72778390000000004</v>
       </c>
       <c r="AB1677" t="s">
         <v>85</v>
@@ -85206,8 +85782,17 @@
       <c r="K1678" t="s">
         <v>60</v>
       </c>
+      <c r="L1678">
+        <v>6262</v>
+      </c>
       <c r="S1678" s="87">
         <v>5.4</v>
+      </c>
+      <c r="U1678" s="19">
+        <v>0.3414699074074074</v>
+      </c>
+      <c r="V1678">
+        <v>0.15316940000000001</v>
       </c>
       <c r="AB1678" t="s">
         <v>86</v>
@@ -85242,6 +85827,15 @@
       <c r="K1679" t="s">
         <v>60</v>
       </c>
+      <c r="L1679">
+        <v>6262</v>
+      </c>
+      <c r="U1679" s="19">
+        <v>0.34225694444444449</v>
+      </c>
+      <c r="V1679" s="20">
+        <v>1.8956259999999999E-2</v>
+      </c>
     </row>
     <row r="1680" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A1680">
@@ -85265,8 +85859,17 @@
       <c r="K1680" t="s">
         <v>60</v>
       </c>
+      <c r="L1680">
+        <v>6262</v>
+      </c>
       <c r="T1680" s="63">
         <v>0.49027777777777781</v>
+      </c>
+      <c r="U1680" s="19">
+        <v>0.34290509259259255</v>
+      </c>
+      <c r="V1680" s="20">
+        <v>1.6481289999999999E-2</v>
       </c>
     </row>
     <row r="1681" spans="1:32" x14ac:dyDescent="0.25">
@@ -85291,11 +85894,20 @@
       <c r="K1681" t="s">
         <v>60</v>
       </c>
+      <c r="L1681">
+        <v>7000</v>
+      </c>
       <c r="S1681" s="87">
         <v>5.5039999999999996</v>
       </c>
       <c r="T1681" s="63">
         <v>0.49027777777777781</v>
+      </c>
+      <c r="U1681" s="19">
+        <v>0.32047453703703704</v>
+      </c>
+      <c r="V1681" s="20">
+        <v>5.4103459999999999E-2</v>
       </c>
       <c r="AB1681" t="s">
         <v>85</v>
@@ -85330,8 +85942,17 @@
       <c r="K1682" t="s">
         <v>60</v>
       </c>
+      <c r="L1682">
+        <v>7000</v>
+      </c>
       <c r="S1682" s="87">
         <v>8.0180000000000007</v>
+      </c>
+      <c r="U1682" s="19">
+        <v>0.32142361111111112</v>
+      </c>
+      <c r="V1682" s="20">
+        <v>6.256457E-2</v>
       </c>
       <c r="AB1682" t="s">
         <v>86</v>
@@ -85366,18 +85987,27 @@
       <c r="K1683" t="s">
         <v>60</v>
       </c>
+      <c r="L1683">
+        <v>7000</v>
+      </c>
       <c r="S1683" s="87">
         <v>6.2309999999999999</v>
       </c>
+      <c r="U1683" s="19">
+        <v>0.3222800925925926</v>
+      </c>
+      <c r="V1683" s="20">
+        <v>5.094957E-2</v>
+      </c>
       <c r="AB1683" t="s">
         <v>86</v>
       </c>
       <c r="AC1683" t="str">
         <f t="shared" ref="AC1683:AC1705" si="28">"A20-10"&amp;AB1683&amp;"-"&amp;AF1683</f>
-        <v>A20-10SO-E3</v>
+        <v>A20-10SO-E2</v>
       </c>
       <c r="AF1683" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="1684" spans="1:32" x14ac:dyDescent="0.25">
@@ -85402,8 +86032,17 @@
       <c r="K1684" t="s">
         <v>60</v>
       </c>
+      <c r="L1684">
+        <v>7000</v>
+      </c>
       <c r="S1684" s="87">
         <v>4.968</v>
+      </c>
+      <c r="U1684" s="19">
+        <v>0.32321759259259258</v>
+      </c>
+      <c r="V1684" s="20">
+        <v>6.5644380000000002E-2</v>
       </c>
       <c r="AB1684" t="s">
         <v>86</v>
@@ -85438,8 +86077,17 @@
       <c r="K1685" t="s">
         <v>60</v>
       </c>
+      <c r="L1685">
+        <v>7000</v>
+      </c>
       <c r="S1685" s="87">
         <v>6.23</v>
+      </c>
+      <c r="U1685" s="19">
+        <v>0.32405092592592594</v>
+      </c>
+      <c r="V1685">
+        <v>0.90356890000000001</v>
       </c>
       <c r="AB1685" t="s">
         <v>86</v>
@@ -85474,8 +86122,17 @@
       <c r="K1686" t="s">
         <v>60</v>
       </c>
+      <c r="L1686">
+        <v>7000</v>
+      </c>
       <c r="S1686" s="87">
         <v>5.165</v>
+      </c>
+      <c r="U1686" s="19">
+        <v>0.32502314814814814</v>
+      </c>
+      <c r="V1686">
+        <v>0.52412829999999999</v>
       </c>
       <c r="AB1686" t="s">
         <v>86</v>
@@ -85510,8 +86167,17 @@
       <c r="K1687" t="s">
         <v>60</v>
       </c>
+      <c r="L1687">
+        <v>7000</v>
+      </c>
       <c r="S1687" s="87">
         <v>4.7830000000000004</v>
+      </c>
+      <c r="U1687" s="19">
+        <v>0.32586805555555554</v>
+      </c>
+      <c r="V1687" s="20">
+        <v>4.9837630000000001E-2</v>
       </c>
       <c r="AB1687" t="s">
         <v>86</v>
@@ -85546,8 +86212,17 @@
       <c r="K1688" t="s">
         <v>60</v>
       </c>
+      <c r="L1688">
+        <v>7000</v>
+      </c>
       <c r="S1688" s="87">
         <v>8.2319999999999993</v>
+      </c>
+      <c r="U1688" s="19">
+        <v>0.32679398148148148</v>
+      </c>
+      <c r="V1688">
+        <v>0.1172228</v>
       </c>
       <c r="AB1688" t="s">
         <v>85</v>
@@ -85582,8 +86257,17 @@
       <c r="K1689" t="s">
         <v>60</v>
       </c>
+      <c r="L1689">
+        <v>7000</v>
+      </c>
       <c r="S1689" s="87">
         <v>7.585</v>
+      </c>
+      <c r="U1689" s="19">
+        <v>0.3275925925925926</v>
+      </c>
+      <c r="V1689" s="20">
+        <v>3.5956969999999998E-2</v>
       </c>
       <c r="AB1689" t="s">
         <v>86</v>
@@ -85618,8 +86302,17 @@
       <c r="K1690" t="s">
         <v>60</v>
       </c>
+      <c r="L1690">
+        <v>7000</v>
+      </c>
       <c r="S1690" s="87">
         <v>7.2930000000000001</v>
+      </c>
+      <c r="U1690" s="19">
+        <v>0.32829861111111108</v>
+      </c>
+      <c r="V1690">
+        <v>0.6394299</v>
       </c>
       <c r="AB1690" t="s">
         <v>85</v>
@@ -85654,8 +86347,17 @@
       <c r="K1691" t="s">
         <v>60</v>
       </c>
+      <c r="L1691">
+        <v>7000</v>
+      </c>
       <c r="S1691" s="87">
         <v>7.827</v>
+      </c>
+      <c r="U1691" s="19">
+        <v>0.32931712962962961</v>
+      </c>
+      <c r="V1691" s="20">
+        <v>7.5932410000000006E-2</v>
       </c>
       <c r="AB1691" t="s">
         <v>86</v>
@@ -85690,8 +86392,17 @@
       <c r="K1692" t="s">
         <v>60</v>
       </c>
+      <c r="L1692">
+        <v>7000</v>
+      </c>
       <c r="S1692" s="87">
         <v>5.2</v>
+      </c>
+      <c r="U1692" s="19">
+        <v>0.33011574074074074</v>
+      </c>
+      <c r="V1692">
+        <v>0.54177649999999999</v>
       </c>
       <c r="AB1692" t="s">
         <v>86</v>
@@ -85726,8 +86437,17 @@
       <c r="K1693" t="s">
         <v>60</v>
       </c>
+      <c r="L1693">
+        <v>7000</v>
+      </c>
       <c r="S1693" s="87">
         <v>5.2670000000000003</v>
+      </c>
+      <c r="U1693" s="19">
+        <v>0.33099537037037036</v>
+      </c>
+      <c r="V1693">
+        <v>7.3529300000000006E-2</v>
       </c>
       <c r="AB1693" t="s">
         <v>85</v>
@@ -85762,8 +86482,17 @@
       <c r="K1694" t="s">
         <v>60</v>
       </c>
+      <c r="L1694">
+        <v>7000</v>
+      </c>
       <c r="S1694" s="87">
         <v>5.1210000000000004</v>
+      </c>
+      <c r="U1694" s="19">
+        <v>0.33172453703703703</v>
+      </c>
+      <c r="V1694" s="20">
+        <v>8.2771090000000005E-2</v>
       </c>
       <c r="AB1694" t="s">
         <v>85</v>
@@ -85798,8 +86527,17 @@
       <c r="K1695" t="s">
         <v>60</v>
       </c>
+      <c r="L1695">
+        <v>7000</v>
+      </c>
       <c r="S1695" s="87">
         <v>7.718</v>
+      </c>
+      <c r="U1695" s="19">
+        <v>0.33260416666666665</v>
+      </c>
+      <c r="V1695" s="20">
+        <v>6.8984950000000003E-2</v>
       </c>
       <c r="AB1695" t="s">
         <v>85</v>
@@ -85834,8 +86572,17 @@
       <c r="K1696" t="s">
         <v>60</v>
       </c>
+      <c r="L1696">
+        <v>7000</v>
+      </c>
       <c r="S1696" s="87">
         <v>4.2729999999999997</v>
+      </c>
+      <c r="U1696" s="19">
+        <v>0.33358796296296295</v>
+      </c>
+      <c r="V1696" s="20">
+        <v>8.5303820000000002E-2</v>
       </c>
       <c r="AB1696" t="s">
         <v>86</v>
@@ -85870,8 +86617,17 @@
       <c r="K1697" t="s">
         <v>60</v>
       </c>
+      <c r="L1697">
+        <v>7000</v>
+      </c>
       <c r="S1697" s="87">
         <v>5.5949999999999998</v>
+      </c>
+      <c r="U1697" s="19">
+        <v>0.33437500000000003</v>
+      </c>
+      <c r="V1697" s="20">
+        <v>2.9827320000000001E-2</v>
       </c>
       <c r="AB1697" t="s">
         <v>86</v>
@@ -85906,8 +86662,17 @@
       <c r="K1698" t="s">
         <v>60</v>
       </c>
+      <c r="L1698">
+        <v>7000</v>
+      </c>
       <c r="S1698" s="87">
         <v>8.125</v>
+      </c>
+      <c r="U1698" s="19">
+        <v>0.33509259259259255</v>
+      </c>
+      <c r="V1698" s="20">
+        <v>5.555595E-2</v>
       </c>
       <c r="AB1698" t="s">
         <v>85</v>
@@ -85942,18 +86707,27 @@
       <c r="K1699" t="s">
         <v>60</v>
       </c>
+      <c r="L1699">
+        <v>7000</v>
+      </c>
       <c r="S1699" s="87">
         <v>6.8090000000000002</v>
       </c>
+      <c r="U1699" s="19">
+        <v>0.33594907407407404</v>
+      </c>
+      <c r="V1699">
+        <v>0.82179460000000004</v>
+      </c>
       <c r="AB1699" t="s">
         <v>85</v>
       </c>
       <c r="AC1699" t="str">
         <f t="shared" si="28"/>
-        <v>A20-10RT-E9</v>
+        <v>A20-10RT-E8</v>
       </c>
       <c r="AF1699" t="s">
-        <v>167</v>
+        <v>383</v>
       </c>
     </row>
     <row r="1700" spans="1:32" x14ac:dyDescent="0.25">
@@ -85978,18 +86752,27 @@
       <c r="K1700" t="s">
         <v>60</v>
       </c>
+      <c r="L1700">
+        <v>7000</v>
+      </c>
       <c r="S1700" s="87">
         <v>6.2629999999999999</v>
       </c>
+      <c r="U1700" s="19">
+        <v>0.33709490740740744</v>
+      </c>
+      <c r="V1700" s="20">
+        <v>6.6745529999999997E-2</v>
+      </c>
       <c r="AB1700" t="s">
         <v>85</v>
       </c>
       <c r="AC1700" t="str">
         <f t="shared" si="28"/>
-        <v>A20-10RT-C5</v>
+        <v>A20-10RT-E11</v>
       </c>
       <c r="AF1700" t="s">
-        <v>123</v>
+        <v>429</v>
       </c>
     </row>
     <row r="1701" spans="1:32" x14ac:dyDescent="0.25">
@@ -86014,18 +86797,27 @@
       <c r="K1701" t="s">
         <v>60</v>
       </c>
+      <c r="L1701">
+        <v>7000</v>
+      </c>
       <c r="S1701" s="87">
         <v>4.9009999999999998</v>
       </c>
+      <c r="U1701" s="19">
+        <v>0.33788194444444447</v>
+      </c>
+      <c r="V1701" s="20">
+        <v>5.2136710000000003E-2</v>
+      </c>
       <c r="AB1701" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="AC1701" t="str">
         <f t="shared" si="28"/>
-        <v>A20-10RT-E11</v>
+        <v>A20-10SO-A4</v>
       </c>
       <c r="AF1701" t="s">
-        <v>429</v>
+        <v>252</v>
       </c>
     </row>
     <row r="1702" spans="1:32" x14ac:dyDescent="0.25">
@@ -86050,18 +86842,27 @@
       <c r="K1702" t="s">
         <v>60</v>
       </c>
+      <c r="L1702">
+        <v>7000</v>
+      </c>
       <c r="S1702" s="87">
         <v>4.38</v>
       </c>
+      <c r="U1702" s="19">
+        <v>0.33872685185185186</v>
+      </c>
+      <c r="V1702" s="20">
+        <v>5.101841E-2</v>
+      </c>
       <c r="AB1702" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="AC1702" t="str">
         <f t="shared" si="28"/>
-        <v>A20-10SO-A4</v>
+        <v>A20-10RT-C5</v>
       </c>
       <c r="AF1702" t="s">
-        <v>252</v>
+        <v>123</v>
       </c>
     </row>
     <row r="1703" spans="1:32" x14ac:dyDescent="0.25">
@@ -86086,8 +86887,17 @@
       <c r="K1703" t="s">
         <v>60</v>
       </c>
+      <c r="L1703">
+        <v>7000</v>
+      </c>
       <c r="S1703" s="87">
         <v>4.1210000000000004</v>
+      </c>
+      <c r="U1703" s="19">
+        <v>0.33969907407407413</v>
+      </c>
+      <c r="V1703" s="20">
+        <v>5.205854E-2</v>
       </c>
       <c r="AB1703" t="s">
         <v>86</v>
@@ -86122,8 +86932,17 @@
       <c r="K1704" t="s">
         <v>60</v>
       </c>
+      <c r="L1704">
+        <v>7000</v>
+      </c>
       <c r="S1704" s="87">
         <v>4.4320000000000004</v>
+      </c>
+      <c r="U1704" s="19">
+        <v>0.34046296296296297</v>
+      </c>
+      <c r="V1704">
+        <v>0.54911220000000005</v>
       </c>
       <c r="AB1704" t="s">
         <v>85</v>
@@ -86158,8 +86977,17 @@
       <c r="K1705" t="s">
         <v>60</v>
       </c>
+      <c r="L1705">
+        <v>7000</v>
+      </c>
       <c r="S1705" s="87">
         <v>2.2599999999999998</v>
+      </c>
+      <c r="U1705" s="19">
+        <v>0.3414699074074074</v>
+      </c>
+      <c r="V1705" s="20">
+        <v>8.6546319999999996E-2</v>
       </c>
       <c r="AB1705" t="s">
         <v>86</v>
@@ -86194,6 +87022,15 @@
       <c r="K1706" t="s">
         <v>60</v>
       </c>
+      <c r="L1706">
+        <v>7000</v>
+      </c>
+      <c r="U1706" s="19">
+        <v>0.34225694444444449</v>
+      </c>
+      <c r="V1706" s="20">
+        <v>4.8409819999999998E-3</v>
+      </c>
     </row>
     <row r="1707" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A1707">
@@ -86217,8 +87054,17 @@
       <c r="K1707" t="s">
         <v>60</v>
       </c>
+      <c r="L1707">
+        <v>7000</v>
+      </c>
       <c r="T1707" s="63">
         <v>0.49513888888888885</v>
+      </c>
+      <c r="U1707" s="19">
+        <v>0.34290509259259255</v>
+      </c>
+      <c r="V1707" s="20">
+        <v>6.9461269999999999E-3</v>
       </c>
     </row>
     <row r="1708" spans="1:32" x14ac:dyDescent="0.25">
@@ -94422,7 +95268,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD836908-61FC-4C6A-BB55-EB17A2B99FDD}">
   <dimension ref="A1:M90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
+    <sheetView topLeftCell="A68" workbookViewId="0">
       <selection activeCell="G89" sqref="G89"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
updated data for 2018-09-10, day 11 cohort
</commit_message>
<xml_diff>
--- a/Data/2018-08-14_master_datac_2018_collection_year.xlsx
+++ b/Data/2018-08-14_master_datac_2018_collection_year.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tatianagerena\Documents\GitHub\Circadian_rhythm_runs_seasonal_timing\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andrew.nguyen\Desktop\Circadian_rhythm_runs_seasonal_timing\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4B40D4C-8950-4076-972C-671E55776204}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D846974-F9E7-4B56-A103-09B60C80A132}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3345" yWindow="465" windowWidth="47520" windowHeight="26880" activeTab="1" xr2:uid="{C7477166-8A7C-B04A-9643-C277FEDCDAAB}"/>
   </bookViews>
@@ -16834,9 +16834,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92725FB9-1A17-2546-9DFA-6C0D39437891}">
   <dimension ref="A1:AV1970"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AE108" sqref="AE108"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A1283" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="T1292" sqref="T1292"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -68316,6 +68316,12 @@
       <c r="R1291">
         <v>9.0464000000000003E-2</v>
       </c>
+      <c r="S1291" s="87">
+        <v>8.7669999999999995</v>
+      </c>
+      <c r="T1291" s="63">
+        <v>0.43472222222222223</v>
+      </c>
       <c r="W1291" s="1" t="s">
         <v>539</v>
       </c>
@@ -68369,6 +68375,9 @@
       <c r="R1292">
         <v>0.65791719999999998</v>
       </c>
+      <c r="S1292" s="87">
+        <v>3.7879999999999998</v>
+      </c>
       <c r="W1292" s="1" t="s">
         <v>539</v>
       </c>
@@ -68540,6 +68549,9 @@
       <c r="R1295">
         <v>0.66372850000000005</v>
       </c>
+      <c r="S1295" s="87">
+        <v>4.0449999999999999</v>
+      </c>
       <c r="W1295" s="1" t="s">
         <v>539</v>
       </c>
@@ -68823,6 +68835,9 @@
       <c r="R1300" s="20">
         <v>6.3603369999999998E-3</v>
       </c>
+      <c r="S1300" s="87">
+        <v>5.5720000000000001</v>
+      </c>
       <c r="W1300" s="1" t="s">
         <v>539</v>
       </c>
@@ -68879,6 +68894,9 @@
       <c r="R1301">
         <v>0.46428380000000002</v>
       </c>
+      <c r="S1301" s="87">
+        <v>2.2650000000000001</v>
+      </c>
       <c r="W1301" s="1" t="s">
         <v>539</v>
       </c>
@@ -68938,6 +68956,9 @@
       <c r="R1302" s="20">
         <v>2.1573169999999999E-2</v>
       </c>
+      <c r="S1302" s="87">
+        <v>5.9870000000000001</v>
+      </c>
       <c r="W1302" s="1" t="s">
         <v>539</v>
       </c>
@@ -69056,6 +69077,9 @@
       <c r="R1304" s="20">
         <v>4.1845609999999998E-2</v>
       </c>
+      <c r="S1304" s="87">
+        <v>4.1609999999999996</v>
+      </c>
       <c r="W1304" s="1" t="s">
         <v>539</v>
       </c>
@@ -69289,6 +69313,9 @@
       <c r="R1308">
         <v>0.91834090000000002</v>
       </c>
+      <c r="S1308" s="87">
+        <v>6.1449999999999996</v>
+      </c>
       <c r="W1308" s="1" t="s">
         <v>539</v>
       </c>
@@ -69404,6 +69431,9 @@
       <c r="R1310">
         <v>0.1013773</v>
       </c>
+      <c r="S1310" s="87">
+        <v>5.9610000000000003</v>
+      </c>
       <c r="W1310" s="1" t="s">
         <v>539</v>
       </c>
@@ -69867,6 +69897,9 @@
       <c r="R1318" s="20">
         <v>6.9106710000000002E-2</v>
       </c>
+      <c r="S1318" s="87">
+        <v>8.6579999999999995</v>
+      </c>
       <c r="W1318" s="1" t="s">
         <v>539</v>
       </c>
@@ -69926,6 +69959,9 @@
       <c r="R1319">
         <v>0.2077051</v>
       </c>
+      <c r="S1319" s="87">
+        <v>5.4189999999999996</v>
+      </c>
       <c r="W1319" s="1" t="s">
         <v>539</v>
       </c>
@@ -69985,6 +70021,9 @@
       <c r="R1320" s="20">
         <v>1.472506E-2</v>
       </c>
+      <c r="S1320" s="87">
+        <v>3.0859999999999999</v>
+      </c>
       <c r="W1320" s="1" t="s">
         <v>539</v>
       </c>
@@ -70162,6 +70201,9 @@
       <c r="R1323">
         <v>0.65600539999999996</v>
       </c>
+      <c r="S1323" s="87">
+        <v>4.218</v>
+      </c>
       <c r="W1323" s="1" t="s">
         <v>539</v>
       </c>
@@ -70221,6 +70263,9 @@
       <c r="R1324">
         <v>7.3161799999999999E-2</v>
       </c>
+      <c r="S1324" s="87">
+        <v>4.2889999999999997</v>
+      </c>
       <c r="W1324" s="1" t="s">
         <v>539</v>
       </c>
@@ -70457,6 +70502,9 @@
       <c r="R1328">
         <v>0.15078040000000001</v>
       </c>
+      <c r="S1328" s="87">
+        <v>7.4160000000000004</v>
+      </c>
       <c r="W1328" s="1" t="s">
         <v>539</v>
       </c>
@@ -70628,6 +70676,9 @@
       <c r="R1331" s="20">
         <v>7.3853630000000003E-2</v>
       </c>
+      <c r="S1331" s="87">
+        <v>6.1120000000000001</v>
+      </c>
       <c r="W1331" s="1" t="s">
         <v>539</v>
       </c>
@@ -70687,6 +70738,9 @@
       <c r="R1332">
         <v>0.6932545</v>
       </c>
+      <c r="S1332" s="87">
+        <v>2.4649999999999999</v>
+      </c>
       <c r="W1332" s="1" t="s">
         <v>539</v>
       </c>
@@ -70846,6 +70900,9 @@
       <c r="R1335" s="20">
         <v>1.420098E-2</v>
       </c>
+      <c r="T1335" s="63">
+        <v>0.4375</v>
+      </c>
       <c r="W1335" s="1" t="s">
         <v>539</v>
       </c>
@@ -70961,6 +71018,12 @@
       <c r="R1337">
         <v>0.1538959</v>
       </c>
+      <c r="S1337" s="87">
+        <v>5.3719999999999999</v>
+      </c>
+      <c r="T1337" s="63">
+        <v>0.4375</v>
+      </c>
       <c r="W1337" s="1" t="s">
         <v>539</v>
       </c>
@@ -71132,6 +71195,9 @@
       <c r="R1340">
         <v>0.66525190000000001</v>
       </c>
+      <c r="S1340" s="87">
+        <v>7.4640000000000004</v>
+      </c>
       <c r="W1340" s="1" t="s">
         <v>539</v>
       </c>
@@ -71247,6 +71313,9 @@
       <c r="R1342" s="20">
         <v>8.5103559999999995E-2</v>
       </c>
+      <c r="S1342" s="87">
+        <v>6.5579999999999998</v>
+      </c>
       <c r="W1342" s="1" t="s">
         <v>539</v>
       </c>
@@ -71704,6 +71773,9 @@
       <c r="R1350" s="20">
         <v>7.1219669999999999E-2</v>
       </c>
+      <c r="S1350" s="87">
+        <v>6.7910000000000004</v>
+      </c>
       <c r="W1350" s="1" t="s">
         <v>539</v>
       </c>
@@ -72173,6 +72245,9 @@
       <c r="R1358" s="20">
         <v>7.2068149999999997E-2</v>
       </c>
+      <c r="S1358" s="87">
+        <v>6.3739999999999997</v>
+      </c>
       <c r="W1358" s="1" t="s">
         <v>539</v>
       </c>
@@ -72291,6 +72366,9 @@
       <c r="R1360" s="20">
         <v>6.559487E-2</v>
       </c>
+      <c r="S1360" s="87">
+        <v>6.585</v>
+      </c>
       <c r="W1360" s="1" t="s">
         <v>539</v>
       </c>
@@ -72350,6 +72428,9 @@
       <c r="R1361">
         <v>3.5681299999999999E-2</v>
       </c>
+      <c r="S1361" s="87">
+        <v>4.3339999999999996</v>
+      </c>
       <c r="W1361" s="1" t="s">
         <v>539</v>
       </c>
@@ -72465,6 +72546,9 @@
       <c r="R1363" s="20">
         <v>6.5048990000000001E-2</v>
       </c>
+      <c r="S1363" s="87">
+        <v>6.2359999999999998</v>
+      </c>
       <c r="W1363" s="1" t="s">
         <v>539</v>
       </c>
@@ -72754,6 +72838,9 @@
       <c r="R1368" s="20">
         <v>5.0249960000000003E-2</v>
       </c>
+      <c r="S1368" s="87">
+        <v>5.8630000000000004</v>
+      </c>
       <c r="W1368" s="1" t="s">
         <v>539</v>
       </c>
@@ -72869,6 +72956,9 @@
       <c r="R1370" s="20">
         <v>6.8668549999999995E-2</v>
       </c>
+      <c r="S1370" s="87">
+        <v>8.4890000000000008</v>
+      </c>
       <c r="W1370" s="1" t="s">
         <v>539</v>
       </c>
@@ -72987,6 +73077,9 @@
       <c r="R1372" s="20">
         <v>3.8742060000000002E-2</v>
       </c>
+      <c r="S1372" s="87">
+        <v>5.2290000000000001</v>
+      </c>
       <c r="W1372" s="1" t="s">
         <v>539</v>
       </c>
@@ -73161,6 +73254,9 @@
       <c r="R1375">
         <v>1.0704009999999999</v>
       </c>
+      <c r="S1375" s="87">
+        <v>5.7409999999999997</v>
+      </c>
       <c r="W1375" s="1" t="s">
         <v>539</v>
       </c>
@@ -73276,6 +73372,9 @@
       <c r="R1377">
         <v>8.9052099999999995E-2</v>
       </c>
+      <c r="S1377" s="87">
+        <v>7.6689999999999996</v>
+      </c>
       <c r="W1377" s="1" t="s">
         <v>539</v>
       </c>
@@ -73549,6 +73648,9 @@
       </c>
       <c r="R1382" s="20">
         <v>7.8548769999999997E-3</v>
+      </c>
+      <c r="T1382" s="63">
+        <v>0.44027777777777777</v>
       </c>
       <c r="W1382" s="1" t="s">
         <v>539</v>
@@ -87153,6 +87255,12 @@
       <c r="K1710" t="s">
         <v>60</v>
       </c>
+      <c r="S1710" s="87">
+        <v>3.6869999999999998</v>
+      </c>
+      <c r="T1710" s="63">
+        <v>0.44027777777777777</v>
+      </c>
       <c r="AB1710" t="s">
         <v>86</v>
       </c>
@@ -87186,6 +87294,9 @@
       <c r="K1711" t="s">
         <v>60</v>
       </c>
+      <c r="S1711" s="87">
+        <v>7.391</v>
+      </c>
       <c r="AB1711" t="s">
         <v>86</v>
       </c>
@@ -87219,6 +87330,9 @@
       <c r="K1712" t="s">
         <v>60</v>
       </c>
+      <c r="S1712" s="87">
+        <v>5.782</v>
+      </c>
       <c r="AB1712" t="s">
         <v>86</v>
       </c>
@@ -87252,6 +87366,9 @@
       <c r="K1713" t="s">
         <v>60</v>
       </c>
+      <c r="S1713" s="87">
+        <v>3.4780000000000002</v>
+      </c>
       <c r="AB1713" t="s">
         <v>86</v>
       </c>
@@ -87285,6 +87402,9 @@
       <c r="K1714" t="s">
         <v>60</v>
       </c>
+      <c r="S1714" s="87">
+        <v>5.6139999999999999</v>
+      </c>
       <c r="AB1714" t="s">
         <v>85</v>
       </c>
@@ -87318,6 +87438,9 @@
       <c r="K1715" t="s">
         <v>60</v>
       </c>
+      <c r="S1715" s="87">
+        <v>3.641</v>
+      </c>
       <c r="AB1715" t="s">
         <v>85</v>
       </c>
@@ -87351,6 +87474,9 @@
       <c r="K1716" t="s">
         <v>60</v>
       </c>
+      <c r="S1716" s="87">
+        <v>6.48</v>
+      </c>
       <c r="AB1716" t="s">
         <v>85</v>
       </c>
@@ -87384,6 +87510,9 @@
       <c r="K1717" t="s">
         <v>60</v>
       </c>
+      <c r="S1717" s="87">
+        <v>5.72</v>
+      </c>
       <c r="AB1717" t="s">
         <v>85</v>
       </c>
@@ -87417,6 +87546,9 @@
       <c r="K1718" t="s">
         <v>60</v>
       </c>
+      <c r="S1718" s="87">
+        <v>3.8540000000000001</v>
+      </c>
       <c r="AB1718" t="s">
         <v>86</v>
       </c>
@@ -87450,6 +87582,9 @@
       <c r="K1719" t="s">
         <v>60</v>
       </c>
+      <c r="S1719" s="87">
+        <v>4.6539999999999999</v>
+      </c>
       <c r="AB1719" t="s">
         <v>85</v>
       </c>
@@ -87483,6 +87618,9 @@
       <c r="K1720" t="s">
         <v>60</v>
       </c>
+      <c r="S1720" s="87">
+        <v>4.4870000000000001</v>
+      </c>
       <c r="AB1720" t="s">
         <v>85</v>
       </c>
@@ -87516,6 +87654,9 @@
       <c r="K1721" t="s">
         <v>60</v>
       </c>
+      <c r="S1721" s="87">
+        <v>2.8519999999999999</v>
+      </c>
       <c r="AB1721" t="s">
         <v>86</v>
       </c>
@@ -87549,6 +87690,9 @@
       <c r="K1722" t="s">
         <v>60</v>
       </c>
+      <c r="S1722" s="87">
+        <v>4.3029999999999999</v>
+      </c>
       <c r="AB1722" t="s">
         <v>85</v>
       </c>
@@ -87582,6 +87726,9 @@
       <c r="K1723" t="s">
         <v>60</v>
       </c>
+      <c r="S1723" s="87">
+        <v>2.4220000000000002</v>
+      </c>
       <c r="AB1723" t="s">
         <v>85</v>
       </c>
@@ -87615,6 +87762,9 @@
       <c r="K1724" t="s">
         <v>60</v>
       </c>
+      <c r="S1724" s="87">
+        <v>2.9590000000000001</v>
+      </c>
       <c r="AB1724" t="s">
         <v>85</v>
       </c>
@@ -87648,6 +87798,9 @@
       <c r="K1725" t="s">
         <v>60</v>
       </c>
+      <c r="S1725" s="87">
+        <v>3.93</v>
+      </c>
       <c r="AB1725" t="s">
         <v>86</v>
       </c>
@@ -87681,6 +87834,9 @@
       <c r="K1726" t="s">
         <v>60</v>
       </c>
+      <c r="S1726" s="87">
+        <v>4.91</v>
+      </c>
       <c r="AB1726" t="s">
         <v>85</v>
       </c>
@@ -87714,6 +87870,9 @@
       <c r="K1727" t="s">
         <v>60</v>
       </c>
+      <c r="S1727" s="87">
+        <v>5.6879999999999997</v>
+      </c>
       <c r="AB1727" t="s">
         <v>85</v>
       </c>
@@ -87747,6 +87906,9 @@
       <c r="K1728" t="s">
         <v>60</v>
       </c>
+      <c r="S1728" s="87">
+        <v>2.9689999999999999</v>
+      </c>
       <c r="AB1728" t="s">
         <v>86</v>
       </c>
@@ -87780,6 +87942,9 @@
       <c r="K1729" t="s">
         <v>60</v>
       </c>
+      <c r="S1729" s="87">
+        <v>4.7450000000000001</v>
+      </c>
       <c r="AB1729" t="s">
         <v>86</v>
       </c>
@@ -87813,6 +87978,9 @@
       <c r="K1730" t="s">
         <v>60</v>
       </c>
+      <c r="S1730" s="87">
+        <v>3.4580000000000002</v>
+      </c>
       <c r="AB1730" t="s">
         <v>85</v>
       </c>
@@ -87846,6 +88014,9 @@
       <c r="K1731" t="s">
         <v>60</v>
       </c>
+      <c r="S1731" s="87">
+        <v>3.6160000000000001</v>
+      </c>
       <c r="AB1731" t="s">
         <v>85</v>
       </c>
@@ -87879,6 +88050,9 @@
       <c r="K1732" t="s">
         <v>60</v>
       </c>
+      <c r="S1732" s="87">
+        <v>1.208</v>
+      </c>
       <c r="AB1732" t="s">
         <v>85</v>
       </c>
@@ -87912,6 +88086,9 @@
       <c r="K1733" t="s">
         <v>60</v>
       </c>
+      <c r="S1733" s="87">
+        <v>2.7730000000000001</v>
+      </c>
       <c r="AB1733" t="s">
         <v>86</v>
       </c>
@@ -87945,6 +88122,9 @@
       <c r="K1734" t="s">
         <v>60</v>
       </c>
+      <c r="S1734" s="87">
+        <v>3.8759999999999999</v>
+      </c>
       <c r="AB1734" t="s">
         <v>85</v>
       </c>
@@ -88000,6 +88180,9 @@
       </c>
       <c r="K1736" t="s">
         <v>60</v>
+      </c>
+      <c r="T1736" s="63">
+        <v>0.44513888888888892</v>
       </c>
     </row>
     <row r="1737" spans="1:32" x14ac:dyDescent="0.25">

</xml_diff>